<commit_message>
TRIEDA-1543 - Adicionando suporte a exportação para excel com os novos campos de disciplina, "usa sabado?" e "usa domingo?".
</commit_message>
<xml_diff>
--- a/code/client/web/src/main/resources/templateExport.xlsx
+++ b/code/client/web/src/main/resources/templateExport.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="17070" windowHeight="5370" tabRatio="977" activeTab="14"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="17070" windowHeight="5370" tabRatio="622" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Campi" sheetId="3" r:id="rId1"/>
@@ -906,6 +906,38 @@
         </r>
       </text>
     </comment>
+    <comment ref="K5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sim
+Não
+Determina se a disciplina deverá herdar os horários das semanas letivas também no sábado.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sim
+Não
+Determina se a disciplina deverá herdar os horários das semanas letivas também no domingo.</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -1179,7 +1211,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="143">
   <si>
     <t>Planilha de Unidades</t>
   </si>
@@ -1607,6 +1639,12 @@
   </si>
   <si>
     <t>Horário Final</t>
+  </si>
+  <si>
+    <t>Usa Sabado?</t>
+  </si>
+  <si>
+    <t>Usa Domingo?</t>
   </si>
 </sst>
 </file>
@@ -1614,9 +1652,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="&quot;R$&quot;\ #,##0.00"/>
+    <numFmt numFmtId="164" formatCode="&quot;R$&quot;\ #,##0.00"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1632,18 +1670,6 @@
     </font>
     <font>
       <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
@@ -1991,21 +2017,21 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -2020,16 +2046,16 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2111,76 +2137,76 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="27" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="6" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2190,13 +2216,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2208,38 +2234,41 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3036,9 +3065,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O6"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="P42" sqref="P42"/>
-    </sheetView>
+    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3154,7 +3181,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4422,6 +4449,7 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="M5:O5"/>
     <mergeCell ref="P5:Q5"/>
     <mergeCell ref="G5:G6"/>
     <mergeCell ref="F5:F6"/>
@@ -4433,7 +4461,6 @@
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="D5:E5"/>
-    <mergeCell ref="M5:O5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4684,7 +4711,6 @@
     <mergeCell ref="B5:L5"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="C6:C7"/>
-    <mergeCell ref="X6:X7"/>
     <mergeCell ref="J6:L6"/>
     <mergeCell ref="F6:I6"/>
     <mergeCell ref="N6:O6"/>
@@ -4697,6 +4723,7 @@
     <mergeCell ref="V6:V7"/>
     <mergeCell ref="W6:W7"/>
     <mergeCell ref="S6:S7"/>
+    <mergeCell ref="X6:X7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5168,7 +5195,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:N6"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5182,7 +5211,8 @@
     <col min="8" max="8" width="24.7109375" customWidth="1"/>
     <col min="9" max="9" width="25.7109375" customWidth="1"/>
     <col min="10" max="10" width="25.85546875" customWidth="1"/>
-    <col min="11" max="11" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.28515625" customWidth="1"/>
+    <col min="12" max="12" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:14" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
@@ -5250,6 +5280,12 @@
       <c r="J5" s="45" t="s">
         <v>22</v>
       </c>
+      <c r="K5" s="45" t="s">
+        <v>141</v>
+      </c>
+      <c r="L5" s="45" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
@@ -5261,6 +5297,8 @@
       <c r="H6" s="8"/>
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
+      <c r="K6" s="87"/>
+      <c r="L6" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
- TRIEDA-1438: Adaptar os algoritmos e cálculos de modo a suportar que uma mesma demanda tenha mais de uma disciplina substituta ou seja parcialmente atendida por uma ou mais disciplinas substitutas
</commit_message>
<xml_diff>
--- a/code/client/web/src/main/resources/templateExport.xlsx
+++ b/code/client/web/src/main/resources/templateExport.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="17070" windowHeight="5370" tabRatio="622" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="17070" windowHeight="5370" tabRatio="622"/>
   </bookViews>
   <sheets>
     <sheet name="Campi" sheetId="3" r:id="rId1"/>
@@ -41,7 +41,7 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Autor</author>
+    <author>Author</author>
   </authors>
   <commentList>
     <comment ref="B5" authorId="0">
@@ -97,7 +97,7 @@
 <file path=xl/comments10.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Autor</author>
+    <author>Author</author>
   </authors>
   <commentList>
     <comment ref="D5" authorId="0">
@@ -159,7 +159,7 @@
 <file path=xl/comments11.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Autor</author>
+    <author>Author</author>
   </authors>
   <commentList>
     <comment ref="Z1" authorId="0">
@@ -172,7 +172,7 @@
 <file path=xl/comments12.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Autor</author>
+    <author>Author</author>
   </authors>
   <commentList>
     <comment ref="Z1" authorId="0">
@@ -185,7 +185,7 @@
 <file path=xl/comments13.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Autor</author>
+    <author>Author</author>
   </authors>
   <commentList>
     <comment ref="Z1" authorId="0">
@@ -198,7 +198,7 @@
 <file path=xl/comments14.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Autor</author>
+    <author>Author</author>
   </authors>
   <commentList>
     <comment ref="Z1" authorId="0">
@@ -211,7 +211,7 @@
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Autor</author>
+    <author>Author</author>
   </authors>
   <commentList>
     <comment ref="B5" authorId="0">
@@ -268,7 +268,7 @@
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Autor</author>
+    <author>Author</author>
   </authors>
   <commentList>
     <comment ref="B5" authorId="0">
@@ -406,7 +406,7 @@
 <file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Autor</author>
+    <author>Author</author>
   </authors>
   <commentList>
     <comment ref="B5" authorId="0">
@@ -604,7 +604,7 @@
 <file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Autor</author>
+    <author>Author</author>
   </authors>
   <commentList>
     <comment ref="B5" authorId="0">
@@ -945,7 +945,7 @@
 <file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Autor</author>
+    <author>Author</author>
   </authors>
   <commentList>
     <comment ref="B5" authorId="0">
@@ -983,7 +983,7 @@
 <file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Autor</author>
+    <author>Author</author>
   </authors>
   <commentList>
     <comment ref="I5" authorId="0">
@@ -1007,7 +1007,7 @@
 <file path=xl/comments8.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Autor</author>
+    <author>Author</author>
   </authors>
   <commentList>
     <comment ref="D5" authorId="0">
@@ -1173,7 +1173,7 @@
 <file path=xl/comments9.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Autor</author>
+    <author>Author</author>
   </authors>
   <commentList>
     <comment ref="C5" authorId="0">
@@ -1537,9 +1537,6 @@
     <t>Qtd Não Atendida</t>
   </si>
   <si>
-    <t>Código Disciplina Substituta</t>
-  </si>
-  <si>
     <t>Planilha de Atendimentos por Aluno</t>
   </si>
   <si>
@@ -1585,22 +1582,6 @@
     <t>Créd. Práticos</t>
   </si>
   <si>
-    <t>Código
-Campus</t>
-  </si>
-  <si>
-    <t>Código
-Curso</t>
-  </si>
-  <si>
-    <t>Matriz
-Curricular</t>
-  </si>
-  <si>
-    <t>Dia da
-Semana</t>
-  </si>
-  <si>
     <t>Horário</t>
   </si>
   <si>
@@ -1610,10 +1591,6 @@
     <t>Fim</t>
   </si>
   <si>
-    <t>Disciplina
-Substituta</t>
-  </si>
-  <si>
     <t>Planilha de Alunos</t>
   </si>
   <si>
@@ -1645,6 +1622,24 @@
   </si>
   <si>
     <t>Usa Domingo?</t>
+  </si>
+  <si>
+    <t>Código(s) Disciplina(s) Substituta(s)</t>
+  </si>
+  <si>
+    <t>Dia da Semana</t>
+  </si>
+  <si>
+    <t>Disciplina (Aula)</t>
+  </si>
+  <si>
+    <t>Disciplina (Demanda)</t>
+  </si>
+  <si>
+    <t>Dia Semana</t>
+  </si>
+  <si>
+    <t>Disciplina Substituta</t>
   </si>
 </sst>
 </file>
@@ -1744,7 +1739,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="28">
+  <fills count="29">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1907,6 +1902,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC0C0C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="9">
     <border>
@@ -2019,7 +2020,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2194,16 +2195,7 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2216,6 +2208,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2235,48 +2239,62 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Porcentagem" xfId="1" builtinId="5"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFC0C0C0"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -2286,9 +2304,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2326,7 +2344,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -2398,7 +2416,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2574,7 +2592,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:N6"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2597,38 +2615,38 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="70" t="s">
+      <c r="B2" s="71" t="s">
         <v>96</v>
       </c>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
-      <c r="J2" s="70"/>
-      <c r="K2" s="70"/>
-      <c r="L2" s="70"/>
-      <c r="M2" s="70"/>
-      <c r="N2" s="70"/>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
+      <c r="G2" s="71"/>
+      <c r="H2" s="71"/>
+      <c r="I2" s="71"/>
+      <c r="J2" s="71"/>
+      <c r="K2" s="71"/>
+      <c r="L2" s="71"/>
+      <c r="M2" s="71"/>
+      <c r="N2" s="71"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="71" t="s">
+      <c r="B3" s="72" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="71"/>
-      <c r="D3" s="71"/>
-      <c r="E3" s="71"/>
-      <c r="F3" s="71"/>
-      <c r="G3" s="71"/>
-      <c r="H3" s="71"/>
-      <c r="I3" s="71"/>
-      <c r="J3" s="71"/>
-      <c r="K3" s="71"/>
-      <c r="L3" s="71"/>
-      <c r="M3" s="71"/>
-      <c r="N3" s="71"/>
+      <c r="C3" s="72"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="72"/>
+      <c r="F3" s="72"/>
+      <c r="G3" s="72"/>
+      <c r="H3" s="72"/>
+      <c r="I3" s="72"/>
+      <c r="J3" s="72"/>
+      <c r="K3" s="72"/>
+      <c r="L3" s="72"/>
+      <c r="M3" s="72"/>
+      <c r="N3" s="72"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="44" t="s">
@@ -2696,36 +2714,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
-      <c r="J2" s="70"/>
-      <c r="K2" s="70"/>
-      <c r="L2" s="70"/>
-      <c r="M2" s="70"/>
-      <c r="N2" s="70"/>
+      <c r="B2" s="71"/>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
+      <c r="G2" s="71"/>
+      <c r="H2" s="71"/>
+      <c r="I2" s="71"/>
+      <c r="J2" s="71"/>
+      <c r="K2" s="71"/>
+      <c r="L2" s="71"/>
+      <c r="M2" s="71"/>
+      <c r="N2" s="71"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="71" t="s">
+      <c r="B3" s="72" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="71"/>
-      <c r="D3" s="71"/>
-      <c r="E3" s="71"/>
-      <c r="F3" s="71"/>
-      <c r="G3" s="71"/>
-      <c r="H3" s="71"/>
-      <c r="I3" s="71"/>
-      <c r="J3" s="71"/>
-      <c r="K3" s="71"/>
-      <c r="L3" s="71"/>
-      <c r="M3" s="71"/>
-      <c r="N3" s="71"/>
+      <c r="C3" s="72"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="72"/>
+      <c r="F3" s="72"/>
+      <c r="G3" s="72"/>
+      <c r="H3" s="72"/>
+      <c r="I3" s="72"/>
+      <c r="J3" s="72"/>
+      <c r="K3" s="72"/>
+      <c r="L3" s="72"/>
+      <c r="M3" s="72"/>
+      <c r="N3" s="72"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -2794,36 +2812,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
-      <c r="J2" s="70"/>
-      <c r="K2" s="70"/>
-      <c r="L2" s="70"/>
-      <c r="M2" s="70"/>
-      <c r="N2" s="70"/>
+      <c r="B2" s="71"/>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
+      <c r="G2" s="71"/>
+      <c r="H2" s="71"/>
+      <c r="I2" s="71"/>
+      <c r="J2" s="71"/>
+      <c r="K2" s="71"/>
+      <c r="L2" s="71"/>
+      <c r="M2" s="71"/>
+      <c r="N2" s="71"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="71" t="s">
+      <c r="B3" s="72" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="71"/>
-      <c r="D3" s="71"/>
-      <c r="E3" s="71"/>
-      <c r="F3" s="71"/>
-      <c r="G3" s="71"/>
-      <c r="H3" s="71"/>
-      <c r="I3" s="71"/>
-      <c r="J3" s="71"/>
-      <c r="K3" s="71"/>
-      <c r="L3" s="71"/>
-      <c r="M3" s="71"/>
-      <c r="N3" s="71"/>
+      <c r="C3" s="72"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="72"/>
+      <c r="F3" s="72"/>
+      <c r="G3" s="72"/>
+      <c r="H3" s="72"/>
+      <c r="I3" s="72"/>
+      <c r="J3" s="72"/>
+      <c r="K3" s="72"/>
+      <c r="L3" s="72"/>
+      <c r="M3" s="72"/>
+      <c r="N3" s="72"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -2857,10 +2875,10 @@
         <v>107</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>108</v>
+        <v>137</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
@@ -2908,28 +2926,28 @@
       </c>
     </row>
     <row r="2" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
+      <c r="B2" s="71"/>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
     </row>
     <row r="3" spans="2:5" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="71" t="s">
-        <v>132</v>
-      </c>
-      <c r="C3" s="71"/>
-      <c r="D3" s="71"/>
-      <c r="E3" s="71"/>
+      <c r="B3" s="72" t="s">
+        <v>126</v>
+      </c>
+      <c r="C3" s="72"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="72"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="61" t="s">
+      <c r="B5" s="60" t="s">
         <v>101</v>
       </c>
-      <c r="C5" s="60" t="s">
+      <c r="C5" s="59" t="s">
         <v>102</v>
       </c>
-      <c r="D5" s="60" t="s">
-        <v>133</v>
+      <c r="D5" s="59" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
@@ -2972,36 +2990,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
-      <c r="J2" s="70"/>
-      <c r="K2" s="70"/>
-      <c r="L2" s="70"/>
-      <c r="M2" s="70"/>
-      <c r="N2" s="70"/>
+      <c r="B2" s="71"/>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
+      <c r="G2" s="71"/>
+      <c r="H2" s="71"/>
+      <c r="I2" s="71"/>
+      <c r="J2" s="71"/>
+      <c r="K2" s="71"/>
+      <c r="L2" s="71"/>
+      <c r="M2" s="71"/>
+      <c r="N2" s="71"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="71" t="s">
+      <c r="B3" s="72" t="s">
         <v>100</v>
       </c>
-      <c r="C3" s="71"/>
-      <c r="D3" s="71"/>
-      <c r="E3" s="71"/>
-      <c r="F3" s="71"/>
-      <c r="G3" s="71"/>
-      <c r="H3" s="71"/>
-      <c r="I3" s="71"/>
-      <c r="J3" s="71"/>
-      <c r="K3" s="71"/>
-      <c r="L3" s="71"/>
-      <c r="M3" s="71"/>
-      <c r="N3" s="71"/>
+      <c r="C3" s="72"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="72"/>
+      <c r="F3" s="72"/>
+      <c r="G3" s="72"/>
+      <c r="H3" s="72"/>
+      <c r="I3" s="72"/>
+      <c r="J3" s="72"/>
+      <c r="K3" s="72"/>
+      <c r="L3" s="72"/>
+      <c r="M3" s="72"/>
+      <c r="N3" s="72"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -3034,10 +3052,10 @@
       <c r="K5" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="L5" s="72" t="s">
-        <v>111</v>
-      </c>
-      <c r="M5" s="72"/>
+      <c r="L5" s="73" t="s">
+        <v>110</v>
+      </c>
+      <c r="M5" s="73"/>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
@@ -3089,38 +3107,38 @@
       </c>
     </row>
     <row r="2" spans="2:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
-      <c r="J2" s="70"/>
-      <c r="K2" s="70"/>
-      <c r="L2" s="70"/>
-      <c r="M2" s="70"/>
-      <c r="N2" s="70"/>
-      <c r="O2" s="70"/>
+      <c r="B2" s="71"/>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
+      <c r="G2" s="71"/>
+      <c r="H2" s="71"/>
+      <c r="I2" s="71"/>
+      <c r="J2" s="71"/>
+      <c r="K2" s="71"/>
+      <c r="L2" s="71"/>
+      <c r="M2" s="71"/>
+      <c r="N2" s="71"/>
+      <c r="O2" s="71"/>
     </row>
     <row r="3" spans="2:15" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="71" t="s">
+      <c r="B3" s="72" t="s">
         <v>73</v>
       </c>
-      <c r="C3" s="71"/>
-      <c r="D3" s="71"/>
-      <c r="E3" s="71"/>
-      <c r="F3" s="71"/>
-      <c r="G3" s="71"/>
-      <c r="H3" s="71"/>
-      <c r="I3" s="71"/>
-      <c r="J3" s="71"/>
-      <c r="K3" s="71"/>
-      <c r="L3" s="71"/>
-      <c r="M3" s="71"/>
-      <c r="N3" s="71"/>
-      <c r="O3" s="71"/>
+      <c r="C3" s="72"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="72"/>
+      <c r="F3" s="72"/>
+      <c r="G3" s="72"/>
+      <c r="H3" s="72"/>
+      <c r="I3" s="72"/>
+      <c r="J3" s="72"/>
+      <c r="K3" s="72"/>
+      <c r="L3" s="72"/>
+      <c r="M3" s="72"/>
+      <c r="N3" s="72"/>
+      <c r="O3" s="72"/>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -3186,11 +3204,11 @@
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.85546875" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" style="69" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.42578125" style="69" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" style="69" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" style="69" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="11.42578125" style="67"/>
+    <col min="2" max="2" width="16.140625" style="66" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.42578125" style="66" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" style="66" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" style="66" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="11.42578125" style="64"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:5" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
@@ -3199,41 +3217,41 @@
       </c>
     </row>
     <row r="2" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
+      <c r="B2" s="71"/>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
     </row>
     <row r="3" spans="2:5" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="71" t="s">
-        <v>137</v>
-      </c>
-      <c r="C3" s="71"/>
-      <c r="D3" s="71"/>
-      <c r="E3" s="71"/>
+      <c r="B3" s="72" t="s">
+        <v>131</v>
+      </c>
+      <c r="C3" s="72"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="72"/>
     </row>
     <row r="4" spans="2:5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="66"/>
+      <c r="B4" s="63"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="64" t="s">
+      <c r="B5" s="62" t="s">
         <v>45</v>
       </c>
       <c r="C5" s="44" t="s">
-        <v>138</v>
-      </c>
-      <c r="D5" s="63" t="s">
-        <v>139</v>
-      </c>
-      <c r="E5" s="63" t="s">
-        <v>140</v>
+        <v>132</v>
+      </c>
+      <c r="D5" s="61" t="s">
+        <v>133</v>
+      </c>
+      <c r="E5" s="61" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="6" spans="2:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="2"/>
-      <c r="D6" s="68"/>
-      <c r="E6" s="68"/>
+      <c r="D6" s="65"/>
+      <c r="E6" s="65"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -3272,36 +3290,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
-      <c r="J2" s="70"/>
-      <c r="K2" s="70"/>
-      <c r="L2" s="70"/>
-      <c r="M2" s="70"/>
-      <c r="N2" s="70"/>
+      <c r="B2" s="71"/>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
+      <c r="G2" s="71"/>
+      <c r="H2" s="71"/>
+      <c r="I2" s="71"/>
+      <c r="J2" s="71"/>
+      <c r="K2" s="71"/>
+      <c r="L2" s="71"/>
+      <c r="M2" s="71"/>
+      <c r="N2" s="71"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="71" t="s">
+      <c r="B3" s="72" t="s">
         <v>69</v>
       </c>
-      <c r="C3" s="71"/>
-      <c r="D3" s="71"/>
-      <c r="E3" s="71"/>
-      <c r="F3" s="71"/>
-      <c r="G3" s="71"/>
-      <c r="H3" s="71"/>
-      <c r="I3" s="71"/>
-      <c r="J3" s="71"/>
-      <c r="K3" s="71"/>
-      <c r="L3" s="71"/>
-      <c r="M3" s="71"/>
-      <c r="N3" s="71"/>
+      <c r="C3" s="72"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="72"/>
+      <c r="F3" s="72"/>
+      <c r="G3" s="72"/>
+      <c r="H3" s="72"/>
+      <c r="I3" s="72"/>
+      <c r="J3" s="72"/>
+      <c r="K3" s="72"/>
+      <c r="L3" s="72"/>
+      <c r="M3" s="72"/>
+      <c r="N3" s="72"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -3356,36 +3374,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
-      <c r="J2" s="70"/>
-      <c r="K2" s="70"/>
-      <c r="L2" s="70"/>
-      <c r="M2" s="70"/>
-      <c r="N2" s="70"/>
+      <c r="B2" s="71"/>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
+      <c r="G2" s="71"/>
+      <c r="H2" s="71"/>
+      <c r="I2" s="71"/>
+      <c r="J2" s="71"/>
+      <c r="K2" s="71"/>
+      <c r="L2" s="71"/>
+      <c r="M2" s="71"/>
+      <c r="N2" s="71"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="71" t="s">
+      <c r="B3" s="72" t="s">
         <v>74</v>
       </c>
-      <c r="C3" s="71"/>
-      <c r="D3" s="71"/>
-      <c r="E3" s="71"/>
-      <c r="F3" s="71"/>
-      <c r="G3" s="71"/>
-      <c r="H3" s="71"/>
-      <c r="I3" s="71"/>
-      <c r="J3" s="71"/>
-      <c r="K3" s="71"/>
-      <c r="L3" s="71"/>
-      <c r="M3" s="71"/>
-      <c r="N3" s="71"/>
+      <c r="C3" s="72"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="72"/>
+      <c r="F3" s="72"/>
+      <c r="G3" s="72"/>
+      <c r="H3" s="72"/>
+      <c r="I3" s="72"/>
+      <c r="J3" s="72"/>
+      <c r="K3" s="72"/>
+      <c r="L3" s="72"/>
+      <c r="M3" s="72"/>
+      <c r="N3" s="72"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -3452,40 +3470,40 @@
       </c>
     </row>
     <row r="2" spans="2:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
-      <c r="J2" s="70"/>
-      <c r="K2" s="70"/>
-      <c r="L2" s="70"/>
-      <c r="M2" s="70"/>
-      <c r="N2" s="70"/>
-      <c r="O2" s="70"/>
-      <c r="P2" s="70"/>
+      <c r="B2" s="71"/>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
+      <c r="G2" s="71"/>
+      <c r="H2" s="71"/>
+      <c r="I2" s="71"/>
+      <c r="J2" s="71"/>
+      <c r="K2" s="71"/>
+      <c r="L2" s="71"/>
+      <c r="M2" s="71"/>
+      <c r="N2" s="71"/>
+      <c r="O2" s="71"/>
+      <c r="P2" s="71"/>
     </row>
     <row r="3" spans="2:18" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="71" t="s">
+      <c r="B3" s="72" t="s">
         <v>63</v>
       </c>
-      <c r="C3" s="71"/>
-      <c r="D3" s="71"/>
-      <c r="E3" s="71"/>
-      <c r="F3" s="71"/>
-      <c r="G3" s="71"/>
-      <c r="H3" s="71"/>
-      <c r="I3" s="71"/>
-      <c r="J3" s="71"/>
-      <c r="K3" s="71"/>
-      <c r="L3" s="71"/>
-      <c r="M3" s="71"/>
-      <c r="N3" s="71"/>
-      <c r="O3" s="71"/>
-      <c r="P3" s="71"/>
+      <c r="C3" s="72"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="72"/>
+      <c r="F3" s="72"/>
+      <c r="G3" s="72"/>
+      <c r="H3" s="72"/>
+      <c r="I3" s="72"/>
+      <c r="J3" s="72"/>
+      <c r="K3" s="72"/>
+      <c r="L3" s="72"/>
+      <c r="M3" s="72"/>
+      <c r="N3" s="72"/>
+      <c r="O3" s="72"/>
+      <c r="P3" s="72"/>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
@@ -3597,39 +3615,39 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
-      <c r="J2" s="70"/>
-      <c r="K2" s="70"/>
-      <c r="L2" s="70"/>
-      <c r="M2" s="70"/>
-      <c r="N2" s="70"/>
+      <c r="B2" s="71"/>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
+      <c r="G2" s="71"/>
+      <c r="H2" s="71"/>
+      <c r="I2" s="71"/>
+      <c r="J2" s="71"/>
+      <c r="K2" s="71"/>
+      <c r="L2" s="71"/>
+      <c r="M2" s="71"/>
+      <c r="N2" s="71"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="71" t="s">
+      <c r="B3" s="72" t="s">
         <v>64</v>
       </c>
-      <c r="C3" s="71"/>
-      <c r="D3" s="71"/>
-      <c r="E3" s="71"/>
-      <c r="F3" s="71"/>
-      <c r="G3" s="71"/>
-      <c r="H3" s="71"/>
-      <c r="I3" s="71"/>
-      <c r="J3" s="71"/>
-      <c r="K3" s="71"/>
-      <c r="L3" s="71"/>
-      <c r="M3" s="71"/>
-      <c r="N3" s="71"/>
+      <c r="C3" s="72"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="72"/>
+      <c r="F3" s="72"/>
+      <c r="G3" s="72"/>
+      <c r="H3" s="72"/>
+      <c r="I3" s="72"/>
+      <c r="J3" s="72"/>
+      <c r="K3" s="72"/>
+      <c r="L3" s="72"/>
+      <c r="M3" s="72"/>
+      <c r="N3" s="72"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B5" s="59" t="s">
+      <c r="B5" s="58" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="4" t="s">
@@ -3713,38 +3731,38 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="70" t="s">
+      <c r="B2" s="71" t="s">
         <v>97</v>
       </c>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
-      <c r="J2" s="70"/>
-      <c r="K2" s="70"/>
-      <c r="L2" s="70"/>
-      <c r="M2" s="70"/>
-      <c r="N2" s="70"/>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
+      <c r="G2" s="71"/>
+      <c r="H2" s="71"/>
+      <c r="I2" s="71"/>
+      <c r="J2" s="71"/>
+      <c r="K2" s="71"/>
+      <c r="L2" s="71"/>
+      <c r="M2" s="71"/>
+      <c r="N2" s="71"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="71" t="s">
+      <c r="B3" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="71"/>
-      <c r="D3" s="71"/>
-      <c r="E3" s="71"/>
-      <c r="F3" s="71"/>
-      <c r="G3" s="71"/>
-      <c r="H3" s="71"/>
-      <c r="I3" s="71"/>
-      <c r="J3" s="71"/>
-      <c r="K3" s="71"/>
-      <c r="L3" s="71"/>
-      <c r="M3" s="71"/>
-      <c r="N3" s="71"/>
+      <c r="C3" s="72"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="72"/>
+      <c r="F3" s="72"/>
+      <c r="G3" s="72"/>
+      <c r="H3" s="72"/>
+      <c r="I3" s="72"/>
+      <c r="J3" s="72"/>
+      <c r="K3" s="72"/>
+      <c r="L3" s="72"/>
+      <c r="M3" s="72"/>
+      <c r="N3" s="72"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="44" t="s">
@@ -3797,37 +3815,37 @@
       <c r="Z1" s="38"/>
     </row>
     <row r="2" spans="2:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
-      <c r="J2" s="70"/>
-      <c r="K2" s="70"/>
-      <c r="L2" s="70"/>
-      <c r="M2" s="70"/>
-      <c r="N2" s="70"/>
+      <c r="B2" s="71"/>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
+      <c r="G2" s="71"/>
+      <c r="H2" s="71"/>
+      <c r="I2" s="71"/>
+      <c r="J2" s="71"/>
+      <c r="K2" s="71"/>
+      <c r="L2" s="71"/>
+      <c r="M2" s="71"/>
+      <c r="N2" s="71"/>
       <c r="Z2"/>
     </row>
     <row r="3" spans="2:26" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="71" t="s">
+      <c r="B3" s="72" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="71"/>
-      <c r="D3" s="71"/>
-      <c r="E3" s="71"/>
-      <c r="F3" s="71"/>
-      <c r="G3" s="71"/>
-      <c r="H3" s="71"/>
-      <c r="I3" s="71"/>
-      <c r="J3" s="71"/>
-      <c r="K3" s="71"/>
-      <c r="L3" s="71"/>
-      <c r="M3" s="71"/>
-      <c r="N3" s="71"/>
+      <c r="C3" s="72"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="72"/>
+      <c r="F3" s="72"/>
+      <c r="G3" s="72"/>
+      <c r="H3" s="72"/>
+      <c r="I3" s="72"/>
+      <c r="J3" s="72"/>
+      <c r="K3" s="72"/>
+      <c r="L3" s="72"/>
+      <c r="M3" s="72"/>
+      <c r="N3" s="72"/>
       <c r="Z3"/>
     </row>
     <row r="5" spans="2:26" x14ac:dyDescent="0.25">
@@ -3931,37 +3949,37 @@
       <c r="Z1" s="38"/>
     </row>
     <row r="2" spans="2:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
-      <c r="J2" s="70"/>
-      <c r="K2" s="70"/>
-      <c r="L2" s="70"/>
-      <c r="M2" s="70"/>
-      <c r="N2" s="70"/>
+      <c r="B2" s="71"/>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
+      <c r="G2" s="71"/>
+      <c r="H2" s="71"/>
+      <c r="I2" s="71"/>
+      <c r="J2" s="71"/>
+      <c r="K2" s="71"/>
+      <c r="L2" s="71"/>
+      <c r="M2" s="71"/>
+      <c r="N2" s="71"/>
       <c r="Z2"/>
     </row>
     <row r="3" spans="2:26" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="71" t="s">
+      <c r="B3" s="72" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="71"/>
-      <c r="D3" s="71"/>
-      <c r="E3" s="71"/>
-      <c r="F3" s="71"/>
-      <c r="G3" s="71"/>
-      <c r="H3" s="71"/>
-      <c r="I3" s="71"/>
-      <c r="J3" s="71"/>
-      <c r="K3" s="71"/>
-      <c r="L3" s="71"/>
-      <c r="M3" s="71"/>
-      <c r="N3" s="71"/>
+      <c r="C3" s="72"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="72"/>
+      <c r="F3" s="72"/>
+      <c r="G3" s="72"/>
+      <c r="H3" s="72"/>
+      <c r="I3" s="72"/>
+      <c r="J3" s="72"/>
+      <c r="K3" s="72"/>
+      <c r="L3" s="72"/>
+      <c r="M3" s="72"/>
+      <c r="N3" s="72"/>
       <c r="Z3"/>
     </row>
     <row r="5" spans="2:26" x14ac:dyDescent="0.25">
@@ -3978,11 +3996,11 @@
     </row>
     <row r="6" spans="2:26" x14ac:dyDescent="0.25">
       <c r="C6" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="D6" s="73"/>
-      <c r="E6" s="74"/>
-      <c r="F6" s="75"/>
+        <v>109</v>
+      </c>
+      <c r="D6" s="74"/>
+      <c r="E6" s="75"/>
+      <c r="F6" s="76"/>
       <c r="G6" s="50"/>
       <c r="H6" s="50"/>
     </row>
@@ -4060,37 +4078,37 @@
       <c r="Z1" s="38"/>
     </row>
     <row r="2" spans="2:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
-      <c r="J2" s="70"/>
-      <c r="K2" s="70"/>
-      <c r="L2" s="70"/>
-      <c r="M2" s="70"/>
-      <c r="N2" s="70"/>
+      <c r="B2" s="71"/>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
+      <c r="G2" s="71"/>
+      <c r="H2" s="71"/>
+      <c r="I2" s="71"/>
+      <c r="J2" s="71"/>
+      <c r="K2" s="71"/>
+      <c r="L2" s="71"/>
+      <c r="M2" s="71"/>
+      <c r="N2" s="71"/>
       <c r="Z2"/>
     </row>
     <row r="3" spans="2:26" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="71" t="s">
+      <c r="B3" s="72" t="s">
         <v>93</v>
       </c>
-      <c r="C3" s="71"/>
-      <c r="D3" s="71"/>
-      <c r="E3" s="71"/>
-      <c r="F3" s="71"/>
-      <c r="G3" s="71"/>
-      <c r="H3" s="71"/>
-      <c r="I3" s="71"/>
-      <c r="J3" s="71"/>
-      <c r="K3" s="71"/>
-      <c r="L3" s="71"/>
-      <c r="M3" s="71"/>
-      <c r="N3" s="71"/>
+      <c r="C3" s="72"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="72"/>
+      <c r="F3" s="72"/>
+      <c r="G3" s="72"/>
+      <c r="H3" s="72"/>
+      <c r="I3" s="72"/>
+      <c r="J3" s="72"/>
+      <c r="K3" s="72"/>
+      <c r="L3" s="72"/>
+      <c r="M3" s="72"/>
+      <c r="N3" s="72"/>
       <c r="Z3"/>
     </row>
     <row r="5" spans="2:26" x14ac:dyDescent="0.25">
@@ -4185,37 +4203,37 @@
       <c r="Z1" s="38"/>
     </row>
     <row r="2" spans="2:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
-      <c r="J2" s="70"/>
-      <c r="K2" s="70"/>
-      <c r="L2" s="70"/>
-      <c r="M2" s="70"/>
-      <c r="N2" s="70"/>
+      <c r="B2" s="71"/>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
+      <c r="G2" s="71"/>
+      <c r="H2" s="71"/>
+      <c r="I2" s="71"/>
+      <c r="J2" s="71"/>
+      <c r="K2" s="71"/>
+      <c r="L2" s="71"/>
+      <c r="M2" s="71"/>
+      <c r="N2" s="71"/>
       <c r="Z2"/>
     </row>
     <row r="3" spans="2:26" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="71" t="s">
+      <c r="B3" s="72" t="s">
         <v>72</v>
       </c>
-      <c r="C3" s="71"/>
-      <c r="D3" s="71"/>
-      <c r="E3" s="71"/>
-      <c r="F3" s="71"/>
-      <c r="G3" s="71"/>
-      <c r="H3" s="71"/>
-      <c r="I3" s="71"/>
-      <c r="J3" s="71"/>
-      <c r="K3" s="71"/>
-      <c r="L3" s="71"/>
-      <c r="M3" s="71"/>
-      <c r="N3" s="71"/>
+      <c r="C3" s="72"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="72"/>
+      <c r="F3" s="72"/>
+      <c r="G3" s="72"/>
+      <c r="H3" s="72"/>
+      <c r="I3" s="72"/>
+      <c r="J3" s="72"/>
+      <c r="K3" s="72"/>
+      <c r="L3" s="72"/>
+      <c r="M3" s="72"/>
+      <c r="N3" s="72"/>
       <c r="Z3"/>
     </row>
     <row r="5" spans="2:26" x14ac:dyDescent="0.25">
@@ -4303,11 +4321,11 @@
   <cols>
     <col min="1" max="1" width="2.85546875" customWidth="1"/>
     <col min="2" max="2" width="10.5703125" customWidth="1"/>
-    <col min="3" max="3" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="5.140625" bestFit="1" customWidth="1"/>
@@ -4326,106 +4344,104 @@
       </c>
     </row>
     <row r="2" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
-      <c r="J2" s="70"/>
-      <c r="K2" s="70"/>
-      <c r="L2" s="70"/>
+      <c r="B2" s="71"/>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
+      <c r="G2" s="71"/>
+      <c r="H2" s="71"/>
+      <c r="I2" s="71"/>
+      <c r="J2" s="71"/>
+      <c r="K2" s="71"/>
+      <c r="L2" s="71"/>
     </row>
     <row r="3" spans="2:17" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="71" t="s">
-        <v>109</v>
-      </c>
-      <c r="C3" s="71"/>
-      <c r="D3" s="71"/>
-      <c r="E3" s="71"/>
-      <c r="F3" s="71"/>
-      <c r="G3" s="71"/>
-      <c r="H3" s="71"/>
-      <c r="I3" s="71"/>
-      <c r="J3" s="71"/>
-      <c r="K3" s="71"/>
-      <c r="L3" s="71"/>
-    </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B5" s="72" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" s="76" t="s">
-        <v>127</v>
-      </c>
+      <c r="B3" s="72" t="s">
+        <v>108</v>
+      </c>
+      <c r="C3" s="72"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="72"/>
+      <c r="F3" s="72"/>
+      <c r="G3" s="72"/>
+      <c r="H3" s="72"/>
+      <c r="I3" s="72"/>
+      <c r="J3" s="72"/>
+      <c r="K3" s="72"/>
+      <c r="L3" s="72"/>
+    </row>
+    <row r="5" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D5" s="77" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="E5" s="77"/>
-      <c r="F5" s="77" t="s">
-        <v>27</v>
-      </c>
-      <c r="G5" s="76" t="s">
-        <v>131</v>
-      </c>
-      <c r="H5" s="77" t="s">
-        <v>53</v>
-      </c>
-      <c r="I5" s="72" t="s">
-        <v>70</v>
-      </c>
+      <c r="F5" s="78"/>
+      <c r="G5" s="78"/>
+      <c r="H5" s="78"/>
+      <c r="I5" s="78"/>
       <c r="J5" s="77" t="s">
         <v>42</v>
       </c>
       <c r="K5" s="77"/>
       <c r="L5" s="77"/>
       <c r="M5" s="77" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="N5" s="77"/>
       <c r="O5" s="77"/>
-      <c r="P5" s="72" t="s">
-        <v>110</v>
-      </c>
-      <c r="Q5" s="72"/>
+      <c r="P5" s="73" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q5" s="73"/>
     </row>
     <row r="6" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="72"/>
-      <c r="C6" s="76"/>
-      <c r="D6" s="65" t="s">
+      <c r="B6" s="70" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="79" t="s">
+        <v>138</v>
+      </c>
+      <c r="D6" s="69" t="s">
+        <v>124</v>
+      </c>
+      <c r="E6" s="69" t="s">
+        <v>125</v>
+      </c>
+      <c r="F6" s="79" t="s">
+        <v>139</v>
+      </c>
+      <c r="G6" s="79" t="s">
+        <v>140</v>
+      </c>
+      <c r="H6" s="80" t="s">
+        <v>53</v>
+      </c>
+      <c r="I6" s="70" t="s">
+        <v>70</v>
+      </c>
+      <c r="J6" s="69" t="s">
         <v>129</v>
       </c>
-      <c r="E6" s="65" t="s">
-        <v>130</v>
-      </c>
-      <c r="F6" s="77"/>
-      <c r="G6" s="77"/>
-      <c r="H6" s="77"/>
-      <c r="I6" s="72"/>
-      <c r="J6" s="65" t="s">
-        <v>135</v>
-      </c>
-      <c r="K6" s="65" t="s">
-        <v>134</v>
-      </c>
-      <c r="L6" s="62" t="s">
-        <v>117</v>
-      </c>
-      <c r="M6" s="65" t="s">
-        <v>135</v>
-      </c>
-      <c r="N6" s="65" t="s">
-        <v>134</v>
-      </c>
-      <c r="O6" s="62" t="s">
-        <v>117</v>
-      </c>
-      <c r="P6" s="62" t="s">
+      <c r="K6" s="69" t="s">
+        <v>128</v>
+      </c>
+      <c r="L6" s="68" t="s">
+        <v>116</v>
+      </c>
+      <c r="M6" s="69" t="s">
+        <v>129</v>
+      </c>
+      <c r="N6" s="69" t="s">
+        <v>128</v>
+      </c>
+      <c r="O6" s="68" t="s">
+        <v>116</v>
+      </c>
+      <c r="P6" s="68" t="s">
         <v>101</v>
       </c>
-      <c r="Q6" s="62" t="s">
+      <c r="Q6" s="68" t="s">
         <v>103</v>
       </c>
     </row>
@@ -4448,19 +4464,13 @@
       <c r="Q7" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="6">
+    <mergeCell ref="B2:L2"/>
+    <mergeCell ref="B3:L3"/>
+    <mergeCell ref="D5:E5"/>
     <mergeCell ref="M5:O5"/>
     <mergeCell ref="P5:Q5"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="I5:I6"/>
     <mergeCell ref="J5:L5"/>
-    <mergeCell ref="B2:L2"/>
-    <mergeCell ref="B3:L3"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:E5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4470,33 +4480,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:X8"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
-    </sheetView>
+    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.85546875" customWidth="1"/>
     <col min="2" max="2" width="10.5703125" customWidth="1"/>
     <col min="3" max="3" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" customWidth="1"/>
     <col min="6" max="6" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="12" width="6.7109375" customWidth="1"/>
+    <col min="10" max="11" width="7.42578125" customWidth="1"/>
+    <col min="12" max="12" width="5.7109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="6.85546875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="8.28515625" bestFit="1" customWidth="1"/>
     <col min="16" max="17" width="3.5703125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="4.5703125" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="4.7109375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="19.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:24" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
@@ -4505,179 +4514,179 @@
       </c>
     </row>
     <row r="2" spans="2:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
-      <c r="J2" s="70"/>
-      <c r="K2" s="70"/>
-      <c r="L2" s="70"/>
-      <c r="M2" s="70"/>
-      <c r="N2" s="70"/>
-      <c r="O2" s="70"/>
-      <c r="P2" s="70"/>
+      <c r="B2" s="71"/>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
+      <c r="G2" s="71"/>
+      <c r="H2" s="71"/>
+      <c r="I2" s="71"/>
+      <c r="J2" s="71"/>
+      <c r="K2" s="71"/>
+      <c r="L2" s="71"/>
+      <c r="M2" s="71"/>
+      <c r="N2" s="71"/>
+      <c r="O2" s="71"/>
+      <c r="P2" s="71"/>
       <c r="Q2" s="56"/>
       <c r="R2" s="56"/>
     </row>
     <row r="3" spans="2:24" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="71" t="s">
-        <v>112</v>
-      </c>
-      <c r="C3" s="71"/>
-      <c r="D3" s="71"/>
-      <c r="E3" s="71"/>
-      <c r="F3" s="71"/>
-      <c r="G3" s="71"/>
-      <c r="H3" s="71"/>
-      <c r="I3" s="71"/>
-      <c r="J3" s="71"/>
-      <c r="K3" s="71"/>
-      <c r="L3" s="71"/>
-      <c r="M3" s="71"/>
-      <c r="N3" s="71"/>
-      <c r="O3" s="71"/>
-      <c r="P3" s="71"/>
+      <c r="B3" s="72" t="s">
+        <v>111</v>
+      </c>
+      <c r="C3" s="72"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="72"/>
+      <c r="F3" s="72"/>
+      <c r="G3" s="72"/>
+      <c r="H3" s="72"/>
+      <c r="I3" s="72"/>
+      <c r="J3" s="72"/>
+      <c r="K3" s="72"/>
+      <c r="L3" s="72"/>
+      <c r="M3" s="72"/>
+      <c r="N3" s="72"/>
+      <c r="O3" s="72"/>
+      <c r="P3" s="72"/>
       <c r="Q3" s="57"/>
       <c r="R3" s="57"/>
     </row>
     <row r="5" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B5" s="80" t="s">
+      <c r="B5" s="82" t="s">
+        <v>112</v>
+      </c>
+      <c r="C5" s="83"/>
+      <c r="D5" s="83"/>
+      <c r="E5" s="83"/>
+      <c r="F5" s="83"/>
+      <c r="G5" s="83"/>
+      <c r="H5" s="83"/>
+      <c r="I5" s="83"/>
+      <c r="J5" s="83"/>
+      <c r="K5" s="83"/>
+      <c r="L5" s="84"/>
+      <c r="M5" s="82" t="s">
         <v>113</v>
       </c>
-      <c r="C5" s="81"/>
-      <c r="D5" s="81"/>
-      <c r="E5" s="81"/>
-      <c r="F5" s="81"/>
-      <c r="G5" s="81"/>
-      <c r="H5" s="81"/>
-      <c r="I5" s="81"/>
-      <c r="J5" s="81"/>
-      <c r="K5" s="81"/>
-      <c r="L5" s="82"/>
-      <c r="M5" s="80" t="s">
+      <c r="N5" s="83"/>
+      <c r="O5" s="83"/>
+      <c r="P5" s="83"/>
+      <c r="Q5" s="83"/>
+      <c r="R5" s="83"/>
+      <c r="S5" s="83"/>
+      <c r="T5" s="83"/>
+      <c r="U5" s="83"/>
+      <c r="V5" s="83"/>
+      <c r="W5" s="83"/>
+      <c r="X5" s="84"/>
+    </row>
+    <row r="6" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B6" s="85"/>
+      <c r="C6" s="85"/>
+      <c r="D6" s="85"/>
+      <c r="E6" s="85"/>
+      <c r="F6" s="86" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" s="87"/>
+      <c r="H6" s="87"/>
+      <c r="I6" s="88"/>
+      <c r="J6" s="82" t="s">
+        <v>30</v>
+      </c>
+      <c r="K6" s="83"/>
+      <c r="L6" s="84"/>
+      <c r="M6" s="89"/>
+      <c r="N6" s="82" t="s">
+        <v>42</v>
+      </c>
+      <c r="O6" s="84"/>
+      <c r="P6" s="82" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q6" s="83"/>
+      <c r="R6" s="84"/>
+      <c r="S6" s="89"/>
+      <c r="T6" s="82" t="s">
+        <v>123</v>
+      </c>
+      <c r="U6" s="84"/>
+      <c r="V6" s="85"/>
+      <c r="W6" s="85"/>
+      <c r="X6" s="85"/>
+    </row>
+    <row r="7" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B7" s="90" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="91" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="90" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="90" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="81" t="s">
+        <v>117</v>
+      </c>
+      <c r="G7" s="81" t="s">
+        <v>121</v>
+      </c>
+      <c r="H7" s="81" t="s">
+        <v>122</v>
+      </c>
+      <c r="I7" s="81" t="s">
+        <v>118</v>
+      </c>
+      <c r="J7" s="81" t="s">
         <v>114</v>
       </c>
-      <c r="N5" s="81"/>
-      <c r="O5" s="81"/>
-      <c r="P5" s="81"/>
-      <c r="Q5" s="81"/>
-      <c r="R5" s="81"/>
-      <c r="S5" s="81"/>
-      <c r="T5" s="81"/>
-      <c r="U5" s="81"/>
-      <c r="V5" s="81"/>
-      <c r="W5" s="81"/>
-      <c r="X5" s="82"/>
-    </row>
-    <row r="6" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B6" s="78" t="s">
+      <c r="K7" s="81" t="s">
+        <v>115</v>
+      </c>
+      <c r="L7" s="81" t="s">
+        <v>116</v>
+      </c>
+      <c r="M7" s="91" t="s">
+        <v>53</v>
+      </c>
+      <c r="N7" s="81" t="s">
+        <v>119</v>
+      </c>
+      <c r="O7" s="81" t="s">
+        <v>120</v>
+      </c>
+      <c r="P7" s="81" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q7" s="81" t="s">
+        <v>115</v>
+      </c>
+      <c r="R7" s="81" t="s">
+        <v>116</v>
+      </c>
+      <c r="S7" s="90" t="s">
+        <v>141</v>
+      </c>
+      <c r="T7" s="81" t="s">
         <v>124</v>
       </c>
-      <c r="C6" s="83" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" s="78" t="s">
+      <c r="U7" s="81" t="s">
         <v>125</v>
       </c>
-      <c r="E6" s="78" t="s">
-        <v>126</v>
-      </c>
-      <c r="F6" s="84" t="s">
-        <v>27</v>
-      </c>
-      <c r="G6" s="85"/>
-      <c r="H6" s="85"/>
-      <c r="I6" s="86"/>
-      <c r="J6" s="80" t="s">
-        <v>30</v>
-      </c>
-      <c r="K6" s="81"/>
-      <c r="L6" s="82"/>
-      <c r="M6" s="83" t="s">
-        <v>53</v>
-      </c>
-      <c r="N6" s="80" t="s">
-        <v>42</v>
-      </c>
-      <c r="O6" s="82"/>
-      <c r="P6" s="80" t="s">
-        <v>106</v>
-      </c>
-      <c r="Q6" s="81"/>
-      <c r="R6" s="82"/>
-      <c r="S6" s="78" t="s">
-        <v>127</v>
-      </c>
-      <c r="T6" s="80" t="s">
-        <v>128</v>
-      </c>
-      <c r="U6" s="82"/>
-      <c r="V6" s="83" t="s">
+      <c r="V7" s="91" t="s">
         <v>70</v>
       </c>
-      <c r="W6" s="83" t="s">
+      <c r="W7" s="91" t="s">
         <v>32</v>
       </c>
-      <c r="X6" s="78" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="7" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B7" s="79"/>
-      <c r="C7" s="79"/>
-      <c r="D7" s="79"/>
-      <c r="E7" s="79"/>
-      <c r="F7" s="58" t="s">
-        <v>118</v>
-      </c>
-      <c r="G7" s="58" t="s">
-        <v>122</v>
-      </c>
-      <c r="H7" s="58" t="s">
-        <v>123</v>
-      </c>
-      <c r="I7" s="58" t="s">
-        <v>119</v>
-      </c>
-      <c r="J7" s="58" t="s">
-        <v>115</v>
-      </c>
-      <c r="K7" s="58" t="s">
-        <v>116</v>
-      </c>
-      <c r="L7" s="58" t="s">
-        <v>117</v>
-      </c>
-      <c r="M7" s="79"/>
-      <c r="N7" s="58" t="s">
-        <v>120</v>
-      </c>
-      <c r="O7" s="58" t="s">
-        <v>121</v>
-      </c>
-      <c r="P7" s="58" t="s">
-        <v>115</v>
-      </c>
-      <c r="Q7" s="58" t="s">
-        <v>116</v>
-      </c>
-      <c r="R7" s="58" t="s">
-        <v>117</v>
-      </c>
-      <c r="S7" s="79"/>
-      <c r="T7" s="58" t="s">
-        <v>129</v>
-      </c>
-      <c r="U7" s="58" t="s">
-        <v>130</v>
-      </c>
-      <c r="V7" s="79"/>
-      <c r="W7" s="79"/>
-      <c r="X7" s="79"/>
+      <c r="X7" s="90" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="8" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B8" s="2"/>
@@ -4705,25 +4714,18 @@
       <c r="X8" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="18">
+  <mergeCells count="11">
+    <mergeCell ref="T6:U6"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="V6:X6"/>
     <mergeCell ref="B2:P2"/>
     <mergeCell ref="B3:P3"/>
     <mergeCell ref="B5:L5"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
     <mergeCell ref="J6:L6"/>
     <mergeCell ref="F6:I6"/>
     <mergeCell ref="N6:O6"/>
     <mergeCell ref="P6:R6"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
     <mergeCell ref="M5:X5"/>
-    <mergeCell ref="M6:M7"/>
-    <mergeCell ref="T6:U6"/>
-    <mergeCell ref="V6:V7"/>
-    <mergeCell ref="W6:W7"/>
-    <mergeCell ref="S6:S7"/>
-    <mergeCell ref="X6:X7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4844,36 +4846,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
-      <c r="J2" s="70"/>
-      <c r="K2" s="70"/>
-      <c r="L2" s="70"/>
-      <c r="M2" s="70"/>
-      <c r="N2" s="70"/>
+      <c r="B2" s="71"/>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
+      <c r="G2" s="71"/>
+      <c r="H2" s="71"/>
+      <c r="I2" s="71"/>
+      <c r="J2" s="71"/>
+      <c r="K2" s="71"/>
+      <c r="L2" s="71"/>
+      <c r="M2" s="71"/>
+      <c r="N2" s="71"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="71" t="s">
+      <c r="B3" s="72" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="71"/>
-      <c r="D3" s="71"/>
-      <c r="E3" s="71"/>
-      <c r="F3" s="71"/>
-      <c r="G3" s="71"/>
-      <c r="H3" s="71"/>
-      <c r="I3" s="71"/>
-      <c r="J3" s="71"/>
-      <c r="K3" s="71"/>
-      <c r="L3" s="71"/>
-      <c r="M3" s="71"/>
-      <c r="N3" s="71"/>
+      <c r="C3" s="72"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="72"/>
+      <c r="F3" s="72"/>
+      <c r="G3" s="72"/>
+      <c r="H3" s="72"/>
+      <c r="I3" s="72"/>
+      <c r="J3" s="72"/>
+      <c r="K3" s="72"/>
+      <c r="L3" s="72"/>
+      <c r="M3" s="72"/>
+      <c r="N3" s="72"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="44" t="s">
@@ -4940,40 +4942,40 @@
       </c>
     </row>
     <row r="2" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
-      <c r="J2" s="70"/>
-      <c r="K2" s="70"/>
-      <c r="L2" s="70"/>
-      <c r="M2" s="70"/>
-      <c r="N2" s="70"/>
-      <c r="O2" s="70"/>
-      <c r="P2" s="70"/>
+      <c r="B2" s="71"/>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
+      <c r="G2" s="71"/>
+      <c r="H2" s="71"/>
+      <c r="I2" s="71"/>
+      <c r="J2" s="71"/>
+      <c r="K2" s="71"/>
+      <c r="L2" s="71"/>
+      <c r="M2" s="71"/>
+      <c r="N2" s="71"/>
+      <c r="O2" s="71"/>
+      <c r="P2" s="71"/>
     </row>
     <row r="3" spans="2:16" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="71" t="s">
+      <c r="B3" s="72" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="71"/>
-      <c r="D3" s="71"/>
-      <c r="E3" s="71"/>
-      <c r="F3" s="71"/>
-      <c r="G3" s="71"/>
-      <c r="H3" s="71"/>
-      <c r="I3" s="71"/>
-      <c r="J3" s="71"/>
-      <c r="K3" s="71"/>
-      <c r="L3" s="71"/>
-      <c r="M3" s="71"/>
-      <c r="N3" s="71"/>
-      <c r="O3" s="71"/>
-      <c r="P3" s="71"/>
+      <c r="C3" s="72"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="72"/>
+      <c r="F3" s="72"/>
+      <c r="G3" s="72"/>
+      <c r="H3" s="72"/>
+      <c r="I3" s="72"/>
+      <c r="J3" s="72"/>
+      <c r="K3" s="72"/>
+      <c r="L3" s="72"/>
+      <c r="M3" s="72"/>
+      <c r="N3" s="72"/>
+      <c r="O3" s="72"/>
+      <c r="P3" s="72"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="44" t="s">
@@ -5052,40 +5054,40 @@
       </c>
     </row>
     <row r="2" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
-      <c r="J2" s="70"/>
-      <c r="K2" s="70"/>
-      <c r="L2" s="70"/>
-      <c r="M2" s="70"/>
-      <c r="N2" s="70"/>
-      <c r="O2" s="70"/>
-      <c r="P2" s="70"/>
+      <c r="B2" s="71"/>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
+      <c r="G2" s="71"/>
+      <c r="H2" s="71"/>
+      <c r="I2" s="71"/>
+      <c r="J2" s="71"/>
+      <c r="K2" s="71"/>
+      <c r="L2" s="71"/>
+      <c r="M2" s="71"/>
+      <c r="N2" s="71"/>
+      <c r="O2" s="71"/>
+      <c r="P2" s="71"/>
     </row>
     <row r="3" spans="2:16" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="71" t="s">
+      <c r="B3" s="72" t="s">
         <v>68</v>
       </c>
-      <c r="C3" s="71"/>
-      <c r="D3" s="71"/>
-      <c r="E3" s="71"/>
-      <c r="F3" s="71"/>
-      <c r="G3" s="71"/>
-      <c r="H3" s="71"/>
-      <c r="I3" s="71"/>
-      <c r="J3" s="71"/>
-      <c r="K3" s="71"/>
-      <c r="L3" s="71"/>
-      <c r="M3" s="71"/>
-      <c r="N3" s="71"/>
-      <c r="O3" s="71"/>
-      <c r="P3" s="71"/>
+      <c r="C3" s="72"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="72"/>
+      <c r="F3" s="72"/>
+      <c r="G3" s="72"/>
+      <c r="H3" s="72"/>
+      <c r="I3" s="72"/>
+      <c r="J3" s="72"/>
+      <c r="K3" s="72"/>
+      <c r="L3" s="72"/>
+      <c r="M3" s="72"/>
+      <c r="N3" s="72"/>
+      <c r="O3" s="72"/>
+      <c r="P3" s="72"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
@@ -5134,40 +5136,40 @@
       </c>
     </row>
     <row r="2" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
-      <c r="J2" s="70"/>
-      <c r="K2" s="70"/>
-      <c r="L2" s="70"/>
-      <c r="M2" s="70"/>
-      <c r="N2" s="70"/>
-      <c r="O2" s="70"/>
-      <c r="P2" s="70"/>
+      <c r="B2" s="71"/>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
+      <c r="G2" s="71"/>
+      <c r="H2" s="71"/>
+      <c r="I2" s="71"/>
+      <c r="J2" s="71"/>
+      <c r="K2" s="71"/>
+      <c r="L2" s="71"/>
+      <c r="M2" s="71"/>
+      <c r="N2" s="71"/>
+      <c r="O2" s="71"/>
+      <c r="P2" s="71"/>
     </row>
     <row r="3" spans="2:16" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="71" t="s">
+      <c r="B3" s="72" t="s">
         <v>71</v>
       </c>
-      <c r="C3" s="71"/>
-      <c r="D3" s="71"/>
-      <c r="E3" s="71"/>
-      <c r="F3" s="71"/>
-      <c r="G3" s="71"/>
-      <c r="H3" s="71"/>
-      <c r="I3" s="71"/>
-      <c r="J3" s="71"/>
-      <c r="K3" s="71"/>
-      <c r="L3" s="71"/>
-      <c r="M3" s="71"/>
-      <c r="N3" s="71"/>
-      <c r="O3" s="71"/>
-      <c r="P3" s="71"/>
+      <c r="C3" s="72"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="72"/>
+      <c r="F3" s="72"/>
+      <c r="G3" s="72"/>
+      <c r="H3" s="72"/>
+      <c r="I3" s="72"/>
+      <c r="J3" s="72"/>
+      <c r="K3" s="72"/>
+      <c r="L3" s="72"/>
+      <c r="M3" s="72"/>
+      <c r="N3" s="72"/>
+      <c r="O3" s="72"/>
+      <c r="P3" s="72"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
@@ -5195,7 +5197,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:N6"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
@@ -5221,36 +5223,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
-      <c r="J2" s="70"/>
-      <c r="K2" s="70"/>
-      <c r="L2" s="70"/>
-      <c r="M2" s="70"/>
-      <c r="N2" s="70"/>
+      <c r="B2" s="71"/>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
+      <c r="G2" s="71"/>
+      <c r="H2" s="71"/>
+      <c r="I2" s="71"/>
+      <c r="J2" s="71"/>
+      <c r="K2" s="71"/>
+      <c r="L2" s="71"/>
+      <c r="M2" s="71"/>
+      <c r="N2" s="71"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="71" t="s">
+      <c r="B3" s="72" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="71"/>
-      <c r="D3" s="71"/>
-      <c r="E3" s="71"/>
-      <c r="F3" s="71"/>
-      <c r="G3" s="71"/>
-      <c r="H3" s="71"/>
-      <c r="I3" s="71"/>
-      <c r="J3" s="71"/>
-      <c r="K3" s="71"/>
-      <c r="L3" s="71"/>
-      <c r="M3" s="71"/>
-      <c r="N3" s="71"/>
+      <c r="C3" s="72"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="72"/>
+      <c r="F3" s="72"/>
+      <c r="G3" s="72"/>
+      <c r="H3" s="72"/>
+      <c r="I3" s="72"/>
+      <c r="J3" s="72"/>
+      <c r="K3" s="72"/>
+      <c r="L3" s="72"/>
+      <c r="M3" s="72"/>
+      <c r="N3" s="72"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="44" t="s">
@@ -5281,10 +5283,10 @@
         <v>22</v>
       </c>
       <c r="K5" s="45" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="L5" s="45" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
@@ -5297,7 +5299,7 @@
       <c r="H6" s="8"/>
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
-      <c r="K6" s="87"/>
+      <c r="K6" s="67"/>
       <c r="L6" s="6"/>
     </row>
   </sheetData>
@@ -5339,40 +5341,40 @@
       </c>
     </row>
     <row r="2" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
-      <c r="J2" s="70"/>
-      <c r="K2" s="70"/>
-      <c r="L2" s="70"/>
-      <c r="M2" s="70"/>
-      <c r="N2" s="70"/>
-      <c r="O2" s="70"/>
-      <c r="P2" s="70"/>
+      <c r="B2" s="71"/>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
+      <c r="G2" s="71"/>
+      <c r="H2" s="71"/>
+      <c r="I2" s="71"/>
+      <c r="J2" s="71"/>
+      <c r="K2" s="71"/>
+      <c r="L2" s="71"/>
+      <c r="M2" s="71"/>
+      <c r="N2" s="71"/>
+      <c r="O2" s="71"/>
+      <c r="P2" s="71"/>
     </row>
     <row r="3" spans="2:16" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="71" t="s">
+      <c r="B3" s="72" t="s">
         <v>65</v>
       </c>
-      <c r="C3" s="71"/>
-      <c r="D3" s="71"/>
-      <c r="E3" s="71"/>
-      <c r="F3" s="71"/>
-      <c r="G3" s="71"/>
-      <c r="H3" s="71"/>
-      <c r="I3" s="71"/>
-      <c r="J3" s="71"/>
-      <c r="K3" s="71"/>
-      <c r="L3" s="71"/>
-      <c r="M3" s="71"/>
-      <c r="N3" s="71"/>
-      <c r="O3" s="71"/>
-      <c r="P3" s="71"/>
+      <c r="C3" s="72"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="72"/>
+      <c r="F3" s="72"/>
+      <c r="G3" s="72"/>
+      <c r="H3" s="72"/>
+      <c r="I3" s="72"/>
+      <c r="J3" s="72"/>
+      <c r="K3" s="72"/>
+      <c r="L3" s="72"/>
+      <c r="M3" s="72"/>
+      <c r="N3" s="72"/>
+      <c r="O3" s="72"/>
+      <c r="P3" s="72"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="45" t="s">
@@ -5424,36 +5426,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
-      <c r="J2" s="70"/>
-      <c r="K2" s="70"/>
-      <c r="L2" s="70"/>
-      <c r="M2" s="70"/>
-      <c r="N2" s="70"/>
+      <c r="B2" s="71"/>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
+      <c r="G2" s="71"/>
+      <c r="H2" s="71"/>
+      <c r="I2" s="71"/>
+      <c r="J2" s="71"/>
+      <c r="K2" s="71"/>
+      <c r="L2" s="71"/>
+      <c r="M2" s="71"/>
+      <c r="N2" s="71"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="71" t="s">
+      <c r="B3" s="72" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="71"/>
-      <c r="D3" s="71"/>
-      <c r="E3" s="71"/>
-      <c r="F3" s="71"/>
-      <c r="G3" s="71"/>
-      <c r="H3" s="71"/>
-      <c r="I3" s="71"/>
-      <c r="J3" s="71"/>
-      <c r="K3" s="71"/>
-      <c r="L3" s="71"/>
-      <c r="M3" s="71"/>
-      <c r="N3" s="71"/>
+      <c r="C3" s="72"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="72"/>
+      <c r="F3" s="72"/>
+      <c r="G3" s="72"/>
+      <c r="H3" s="72"/>
+      <c r="I3" s="72"/>
+      <c r="J3" s="72"/>
+      <c r="K3" s="72"/>
+      <c r="L3" s="72"/>
+      <c r="M3" s="72"/>
+      <c r="N3" s="72"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">

</xml_diff>

<commit_message>
TRIEDA-1590 - Implementando exportação para excel dos relatórios de Atendimento por Matrícula e por Disciplina. Adicionando Estas duas exportações nas opções "exportar tudo" e "exportar tabelas". Melhorando desempenho da função que faz o cálculo do relatório de atendimento por matrícula e por disciplina.
</commit_message>
<xml_diff>
--- a/code/client/web/src/main/resources/templateExport.xlsx
+++ b/code/client/web/src/main/resources/templateExport.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="17070" windowHeight="5370" tabRatio="622"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="17070" windowHeight="5370" tabRatio="622" firstSheet="16" activeTab="20"/>
   </bookViews>
   <sheets>
     <sheet name="Campi" sheetId="3" r:id="rId1"/>
@@ -26,13 +26,15 @@
     <sheet name="Habilitacao dos Professores" sheetId="13" r:id="rId17"/>
     <sheet name="Resumo por curso" sheetId="14" r:id="rId18"/>
     <sheet name="Resumo por disciplina" sheetId="15" r:id="rId19"/>
-    <sheet name="Relatorio Visao Sala" sheetId="10" r:id="rId20"/>
-    <sheet name="Relatorio Visao Aluno" sheetId="25" r:id="rId21"/>
-    <sheet name="Relatorio Visao Professor" sheetId="21" r:id="rId22"/>
-    <sheet name="Relatorio Visao Curso" sheetId="20" r:id="rId23"/>
-    <sheet name="Atendimentos por Aluno" sheetId="23" r:id="rId24"/>
-    <sheet name="Aulas" sheetId="26" r:id="rId25"/>
-    <sheet name="PaletaCores" sheetId="11" r:id="rId26"/>
+    <sheet name="Atendimentos por Matricula" sheetId="30" r:id="rId20"/>
+    <sheet name="Atendimentos por Disciplina" sheetId="31" r:id="rId21"/>
+    <sheet name="Relatorio Visao Sala" sheetId="10" r:id="rId22"/>
+    <sheet name="Relatorio Visao Aluno" sheetId="25" r:id="rId23"/>
+    <sheet name="Relatorio Visao Professor" sheetId="21" r:id="rId24"/>
+    <sheet name="Relatorio Visao Curso" sheetId="20" r:id="rId25"/>
+    <sheet name="Atendimentos por Aluno" sheetId="23" r:id="rId26"/>
+    <sheet name="Aulas" sheetId="26" r:id="rId27"/>
+    <sheet name="PaletaCores" sheetId="11" r:id="rId28"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
@@ -41,7 +43,7 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Author</author>
+    <author>Autor</author>
   </authors>
   <commentList>
     <comment ref="B5" authorId="0">
@@ -97,7 +99,7 @@
 <file path=xl/comments10.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Author</author>
+    <author>Autor</author>
   </authors>
   <commentList>
     <comment ref="D5" authorId="0">
@@ -159,7 +161,7 @@
 <file path=xl/comments11.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Author</author>
+    <author>Autor</author>
   </authors>
   <commentList>
     <comment ref="Z1" authorId="0">
@@ -172,7 +174,7 @@
 <file path=xl/comments12.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Author</author>
+    <author>Autor</author>
   </authors>
   <commentList>
     <comment ref="Z1" authorId="0">
@@ -185,7 +187,7 @@
 <file path=xl/comments13.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Author</author>
+    <author>Autor</author>
   </authors>
   <commentList>
     <comment ref="Z1" authorId="0">
@@ -198,7 +200,7 @@
 <file path=xl/comments14.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Author</author>
+    <author>Autor</author>
   </authors>
   <commentList>
     <comment ref="Z1" authorId="0">
@@ -211,7 +213,7 @@
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Author</author>
+    <author>Autor</author>
   </authors>
   <commentList>
     <comment ref="B5" authorId="0">
@@ -268,7 +270,7 @@
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Author</author>
+    <author>Autor</author>
   </authors>
   <commentList>
     <comment ref="B5" authorId="0">
@@ -406,7 +408,7 @@
 <file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Author</author>
+    <author>Autor</author>
   </authors>
   <commentList>
     <comment ref="B5" authorId="0">
@@ -604,7 +606,7 @@
 <file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Author</author>
+    <author>Autor</author>
   </authors>
   <commentList>
     <comment ref="B5" authorId="0">
@@ -945,7 +947,7 @@
 <file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Author</author>
+    <author>Autor</author>
   </authors>
   <commentList>
     <comment ref="B5" authorId="0">
@@ -983,7 +985,7 @@
 <file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Author</author>
+    <author>Autor</author>
   </authors>
   <commentList>
     <comment ref="I5" authorId="0">
@@ -1007,7 +1009,7 @@
 <file path=xl/comments8.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Author</author>
+    <author>Autor</author>
   </authors>
   <commentList>
     <comment ref="D5" authorId="0">
@@ -1173,7 +1175,7 @@
 <file path=xl/comments9.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Author</author>
+    <author>Autor</author>
   </authors>
   <commentList>
     <comment ref="C5" authorId="0">
@@ -1211,7 +1213,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="156">
   <si>
     <t>Planilha de Unidades</t>
   </si>
@@ -1640,6 +1642,45 @@
   </si>
   <si>
     <t>Disciplina Substituta</t>
+  </si>
+  <si>
+    <t>Demanda P1</t>
+  </si>
+  <si>
+    <t>Atendidos P1</t>
+  </si>
+  <si>
+    <t>Não Atendidos P1</t>
+  </si>
+  <si>
+    <t>Atendidos P2</t>
+  </si>
+  <si>
+    <t>Demanda P1 (disc)</t>
+  </si>
+  <si>
+    <t>Atendidos P1 (disc)</t>
+  </si>
+  <si>
+    <t>Não Atendidos P1 (disc)</t>
+  </si>
+  <si>
+    <t>Atendidos P2 (disc)</t>
+  </si>
+  <si>
+    <t>Excesso P2</t>
+  </si>
+  <si>
+    <t>Planilha de Atendimentos Por Matrícula</t>
+  </si>
+  <si>
+    <t>Atendidos P1 + P2</t>
+  </si>
+  <si>
+    <t>Demanda P1 - Atendidos</t>
+  </si>
+  <si>
+    <t>Planilha de Atendimentos Por Disciplina</t>
   </si>
 </sst>
 </file>
@@ -1647,9 +1688,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="&quot;R$&quot;\ #,##0.00"/>
+    <numFmt numFmtId="165" formatCode="&quot;R$&quot;\ #,##0.00"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1671,6 +1712,18 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color indexed="8"/>
@@ -1685,16 +1738,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2018,21 +2071,21 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -2047,16 +2100,16 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2138,163 +2191,164 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="27" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="6" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="28" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
+    <cellStyle name="Porcentagem" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <mruColors>
-      <color rgb="FFC0C0C0"/>
-    </mruColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -2304,9 +2358,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Escritório">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2344,7 +2398,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Escritório">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -2416,7 +2470,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Escritório">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2592,7 +2646,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:N6"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2615,38 +2669,38 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="71" t="s">
+      <c r="B2" s="80" t="s">
         <v>96</v>
       </c>
-      <c r="C2" s="71"/>
-      <c r="D2" s="71"/>
-      <c r="E2" s="71"/>
-      <c r="F2" s="71"/>
-      <c r="G2" s="71"/>
-      <c r="H2" s="71"/>
-      <c r="I2" s="71"/>
-      <c r="J2" s="71"/>
-      <c r="K2" s="71"/>
-      <c r="L2" s="71"/>
-      <c r="M2" s="71"/>
-      <c r="N2" s="71"/>
+      <c r="C2" s="80"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="80"/>
+      <c r="F2" s="80"/>
+      <c r="G2" s="80"/>
+      <c r="H2" s="80"/>
+      <c r="I2" s="80"/>
+      <c r="J2" s="80"/>
+      <c r="K2" s="80"/>
+      <c r="L2" s="80"/>
+      <c r="M2" s="80"/>
+      <c r="N2" s="80"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="72" t="s">
+      <c r="B3" s="81" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="72"/>
-      <c r="D3" s="72"/>
-      <c r="E3" s="72"/>
-      <c r="F3" s="72"/>
-      <c r="G3" s="72"/>
-      <c r="H3" s="72"/>
-      <c r="I3" s="72"/>
-      <c r="J3" s="72"/>
-      <c r="K3" s="72"/>
-      <c r="L3" s="72"/>
-      <c r="M3" s="72"/>
-      <c r="N3" s="72"/>
+      <c r="C3" s="81"/>
+      <c r="D3" s="81"/>
+      <c r="E3" s="81"/>
+      <c r="F3" s="81"/>
+      <c r="G3" s="81"/>
+      <c r="H3" s="81"/>
+      <c r="I3" s="81"/>
+      <c r="J3" s="81"/>
+      <c r="K3" s="81"/>
+      <c r="L3" s="81"/>
+      <c r="M3" s="81"/>
+      <c r="N3" s="81"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="44" t="s">
@@ -2714,36 +2768,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="71"/>
-      <c r="C2" s="71"/>
-      <c r="D2" s="71"/>
-      <c r="E2" s="71"/>
-      <c r="F2" s="71"/>
-      <c r="G2" s="71"/>
-      <c r="H2" s="71"/>
-      <c r="I2" s="71"/>
-      <c r="J2" s="71"/>
-      <c r="K2" s="71"/>
-      <c r="L2" s="71"/>
-      <c r="M2" s="71"/>
-      <c r="N2" s="71"/>
+      <c r="B2" s="80"/>
+      <c r="C2" s="80"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="80"/>
+      <c r="F2" s="80"/>
+      <c r="G2" s="80"/>
+      <c r="H2" s="80"/>
+      <c r="I2" s="80"/>
+      <c r="J2" s="80"/>
+      <c r="K2" s="80"/>
+      <c r="L2" s="80"/>
+      <c r="M2" s="80"/>
+      <c r="N2" s="80"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="72" t="s">
+      <c r="B3" s="81" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="72"/>
-      <c r="D3" s="72"/>
-      <c r="E3" s="72"/>
-      <c r="F3" s="72"/>
-      <c r="G3" s="72"/>
-      <c r="H3" s="72"/>
-      <c r="I3" s="72"/>
-      <c r="J3" s="72"/>
-      <c r="K3" s="72"/>
-      <c r="L3" s="72"/>
-      <c r="M3" s="72"/>
-      <c r="N3" s="72"/>
+      <c r="C3" s="81"/>
+      <c r="D3" s="81"/>
+      <c r="E3" s="81"/>
+      <c r="F3" s="81"/>
+      <c r="G3" s="81"/>
+      <c r="H3" s="81"/>
+      <c r="I3" s="81"/>
+      <c r="J3" s="81"/>
+      <c r="K3" s="81"/>
+      <c r="L3" s="81"/>
+      <c r="M3" s="81"/>
+      <c r="N3" s="81"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -2812,36 +2866,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="71"/>
-      <c r="C2" s="71"/>
-      <c r="D2" s="71"/>
-      <c r="E2" s="71"/>
-      <c r="F2" s="71"/>
-      <c r="G2" s="71"/>
-      <c r="H2" s="71"/>
-      <c r="I2" s="71"/>
-      <c r="J2" s="71"/>
-      <c r="K2" s="71"/>
-      <c r="L2" s="71"/>
-      <c r="M2" s="71"/>
-      <c r="N2" s="71"/>
+      <c r="B2" s="80"/>
+      <c r="C2" s="80"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="80"/>
+      <c r="F2" s="80"/>
+      <c r="G2" s="80"/>
+      <c r="H2" s="80"/>
+      <c r="I2" s="80"/>
+      <c r="J2" s="80"/>
+      <c r="K2" s="80"/>
+      <c r="L2" s="80"/>
+      <c r="M2" s="80"/>
+      <c r="N2" s="80"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="72" t="s">
+      <c r="B3" s="81" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="72"/>
-      <c r="D3" s="72"/>
-      <c r="E3" s="72"/>
-      <c r="F3" s="72"/>
-      <c r="G3" s="72"/>
-      <c r="H3" s="72"/>
-      <c r="I3" s="72"/>
-      <c r="J3" s="72"/>
-      <c r="K3" s="72"/>
-      <c r="L3" s="72"/>
-      <c r="M3" s="72"/>
-      <c r="N3" s="72"/>
+      <c r="C3" s="81"/>
+      <c r="D3" s="81"/>
+      <c r="E3" s="81"/>
+      <c r="F3" s="81"/>
+      <c r="G3" s="81"/>
+      <c r="H3" s="81"/>
+      <c r="I3" s="81"/>
+      <c r="J3" s="81"/>
+      <c r="K3" s="81"/>
+      <c r="L3" s="81"/>
+      <c r="M3" s="81"/>
+      <c r="N3" s="81"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -2926,18 +2980,18 @@
       </c>
     </row>
     <row r="2" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="71"/>
-      <c r="C2" s="71"/>
-      <c r="D2" s="71"/>
-      <c r="E2" s="71"/>
+      <c r="B2" s="80"/>
+      <c r="C2" s="80"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="80"/>
     </row>
     <row r="3" spans="2:5" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="72" t="s">
+      <c r="B3" s="81" t="s">
         <v>126</v>
       </c>
-      <c r="C3" s="72"/>
-      <c r="D3" s="72"/>
-      <c r="E3" s="72"/>
+      <c r="C3" s="81"/>
+      <c r="D3" s="81"/>
+      <c r="E3" s="81"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="60" t="s">
@@ -2990,36 +3044,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="71"/>
-      <c r="C2" s="71"/>
-      <c r="D2" s="71"/>
-      <c r="E2" s="71"/>
-      <c r="F2" s="71"/>
-      <c r="G2" s="71"/>
-      <c r="H2" s="71"/>
-      <c r="I2" s="71"/>
-      <c r="J2" s="71"/>
-      <c r="K2" s="71"/>
-      <c r="L2" s="71"/>
-      <c r="M2" s="71"/>
-      <c r="N2" s="71"/>
+      <c r="B2" s="80"/>
+      <c r="C2" s="80"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="80"/>
+      <c r="F2" s="80"/>
+      <c r="G2" s="80"/>
+      <c r="H2" s="80"/>
+      <c r="I2" s="80"/>
+      <c r="J2" s="80"/>
+      <c r="K2" s="80"/>
+      <c r="L2" s="80"/>
+      <c r="M2" s="80"/>
+      <c r="N2" s="80"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="72" t="s">
+      <c r="B3" s="81" t="s">
         <v>100</v>
       </c>
-      <c r="C3" s="72"/>
-      <c r="D3" s="72"/>
-      <c r="E3" s="72"/>
-      <c r="F3" s="72"/>
-      <c r="G3" s="72"/>
-      <c r="H3" s="72"/>
-      <c r="I3" s="72"/>
-      <c r="J3" s="72"/>
-      <c r="K3" s="72"/>
-      <c r="L3" s="72"/>
-      <c r="M3" s="72"/>
-      <c r="N3" s="72"/>
+      <c r="C3" s="81"/>
+      <c r="D3" s="81"/>
+      <c r="E3" s="81"/>
+      <c r="F3" s="81"/>
+      <c r="G3" s="81"/>
+      <c r="H3" s="81"/>
+      <c r="I3" s="81"/>
+      <c r="J3" s="81"/>
+      <c r="K3" s="81"/>
+      <c r="L3" s="81"/>
+      <c r="M3" s="81"/>
+      <c r="N3" s="81"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -3052,10 +3106,10 @@
       <c r="K5" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="L5" s="73" t="s">
+      <c r="L5" s="82" t="s">
         <v>110</v>
       </c>
-      <c r="M5" s="73"/>
+      <c r="M5" s="82"/>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
@@ -3107,38 +3161,38 @@
       </c>
     </row>
     <row r="2" spans="2:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="71"/>
-      <c r="C2" s="71"/>
-      <c r="D2" s="71"/>
-      <c r="E2" s="71"/>
-      <c r="F2" s="71"/>
-      <c r="G2" s="71"/>
-      <c r="H2" s="71"/>
-      <c r="I2" s="71"/>
-      <c r="J2" s="71"/>
-      <c r="K2" s="71"/>
-      <c r="L2" s="71"/>
-      <c r="M2" s="71"/>
-      <c r="N2" s="71"/>
-      <c r="O2" s="71"/>
+      <c r="B2" s="80"/>
+      <c r="C2" s="80"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="80"/>
+      <c r="F2" s="80"/>
+      <c r="G2" s="80"/>
+      <c r="H2" s="80"/>
+      <c r="I2" s="80"/>
+      <c r="J2" s="80"/>
+      <c r="K2" s="80"/>
+      <c r="L2" s="80"/>
+      <c r="M2" s="80"/>
+      <c r="N2" s="80"/>
+      <c r="O2" s="80"/>
     </row>
     <row r="3" spans="2:15" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="72" t="s">
+      <c r="B3" s="81" t="s">
         <v>73</v>
       </c>
-      <c r="C3" s="72"/>
-      <c r="D3" s="72"/>
-      <c r="E3" s="72"/>
-      <c r="F3" s="72"/>
-      <c r="G3" s="72"/>
-      <c r="H3" s="72"/>
-      <c r="I3" s="72"/>
-      <c r="J3" s="72"/>
-      <c r="K3" s="72"/>
-      <c r="L3" s="72"/>
-      <c r="M3" s="72"/>
-      <c r="N3" s="72"/>
-      <c r="O3" s="72"/>
+      <c r="C3" s="81"/>
+      <c r="D3" s="81"/>
+      <c r="E3" s="81"/>
+      <c r="F3" s="81"/>
+      <c r="G3" s="81"/>
+      <c r="H3" s="81"/>
+      <c r="I3" s="81"/>
+      <c r="J3" s="81"/>
+      <c r="K3" s="81"/>
+      <c r="L3" s="81"/>
+      <c r="M3" s="81"/>
+      <c r="N3" s="81"/>
+      <c r="O3" s="81"/>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -3204,11 +3258,11 @@
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.85546875" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" style="66" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.42578125" style="66" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" style="66" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" style="66" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="11.42578125" style="64"/>
+    <col min="2" max="2" width="16.140625" style="67" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.42578125" style="67" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" style="67" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" style="67" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="11.42578125" style="65"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:5" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
@@ -3217,21 +3271,21 @@
       </c>
     </row>
     <row r="2" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="71"/>
-      <c r="C2" s="71"/>
-      <c r="D2" s="71"/>
-      <c r="E2" s="71"/>
+      <c r="B2" s="80"/>
+      <c r="C2" s="80"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="80"/>
     </row>
     <row r="3" spans="2:5" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="72" t="s">
+      <c r="B3" s="81" t="s">
         <v>131</v>
       </c>
-      <c r="C3" s="72"/>
-      <c r="D3" s="72"/>
-      <c r="E3" s="72"/>
+      <c r="C3" s="81"/>
+      <c r="D3" s="81"/>
+      <c r="E3" s="81"/>
     </row>
     <row r="4" spans="2:5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="63"/>
+      <c r="B4" s="64"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="62" t="s">
@@ -3250,8 +3304,8 @@
     <row r="6" spans="2:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="2"/>
-      <c r="D6" s="65"/>
-      <c r="E6" s="65"/>
+      <c r="D6" s="66"/>
+      <c r="E6" s="66"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -3290,36 +3344,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="71"/>
-      <c r="C2" s="71"/>
-      <c r="D2" s="71"/>
-      <c r="E2" s="71"/>
-      <c r="F2" s="71"/>
-      <c r="G2" s="71"/>
-      <c r="H2" s="71"/>
-      <c r="I2" s="71"/>
-      <c r="J2" s="71"/>
-      <c r="K2" s="71"/>
-      <c r="L2" s="71"/>
-      <c r="M2" s="71"/>
-      <c r="N2" s="71"/>
+      <c r="B2" s="80"/>
+      <c r="C2" s="80"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="80"/>
+      <c r="F2" s="80"/>
+      <c r="G2" s="80"/>
+      <c r="H2" s="80"/>
+      <c r="I2" s="80"/>
+      <c r="J2" s="80"/>
+      <c r="K2" s="80"/>
+      <c r="L2" s="80"/>
+      <c r="M2" s="80"/>
+      <c r="N2" s="80"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="72" t="s">
+      <c r="B3" s="81" t="s">
         <v>69</v>
       </c>
-      <c r="C3" s="72"/>
-      <c r="D3" s="72"/>
-      <c r="E3" s="72"/>
-      <c r="F3" s="72"/>
-      <c r="G3" s="72"/>
-      <c r="H3" s="72"/>
-      <c r="I3" s="72"/>
-      <c r="J3" s="72"/>
-      <c r="K3" s="72"/>
-      <c r="L3" s="72"/>
-      <c r="M3" s="72"/>
-      <c r="N3" s="72"/>
+      <c r="C3" s="81"/>
+      <c r="D3" s="81"/>
+      <c r="E3" s="81"/>
+      <c r="F3" s="81"/>
+      <c r="G3" s="81"/>
+      <c r="H3" s="81"/>
+      <c r="I3" s="81"/>
+      <c r="J3" s="81"/>
+      <c r="K3" s="81"/>
+      <c r="L3" s="81"/>
+      <c r="M3" s="81"/>
+      <c r="N3" s="81"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -3374,36 +3428,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="71"/>
-      <c r="C2" s="71"/>
-      <c r="D2" s="71"/>
-      <c r="E2" s="71"/>
-      <c r="F2" s="71"/>
-      <c r="G2" s="71"/>
-      <c r="H2" s="71"/>
-      <c r="I2" s="71"/>
-      <c r="J2" s="71"/>
-      <c r="K2" s="71"/>
-      <c r="L2" s="71"/>
-      <c r="M2" s="71"/>
-      <c r="N2" s="71"/>
+      <c r="B2" s="80"/>
+      <c r="C2" s="80"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="80"/>
+      <c r="F2" s="80"/>
+      <c r="G2" s="80"/>
+      <c r="H2" s="80"/>
+      <c r="I2" s="80"/>
+      <c r="J2" s="80"/>
+      <c r="K2" s="80"/>
+      <c r="L2" s="80"/>
+      <c r="M2" s="80"/>
+      <c r="N2" s="80"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="72" t="s">
+      <c r="B3" s="81" t="s">
         <v>74</v>
       </c>
-      <c r="C3" s="72"/>
-      <c r="D3" s="72"/>
-      <c r="E3" s="72"/>
-      <c r="F3" s="72"/>
-      <c r="G3" s="72"/>
-      <c r="H3" s="72"/>
-      <c r="I3" s="72"/>
-      <c r="J3" s="72"/>
-      <c r="K3" s="72"/>
-      <c r="L3" s="72"/>
-      <c r="M3" s="72"/>
-      <c r="N3" s="72"/>
+      <c r="C3" s="81"/>
+      <c r="D3" s="81"/>
+      <c r="E3" s="81"/>
+      <c r="F3" s="81"/>
+      <c r="G3" s="81"/>
+      <c r="H3" s="81"/>
+      <c r="I3" s="81"/>
+      <c r="J3" s="81"/>
+      <c r="K3" s="81"/>
+      <c r="L3" s="81"/>
+      <c r="M3" s="81"/>
+      <c r="N3" s="81"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -3470,40 +3524,40 @@
       </c>
     </row>
     <row r="2" spans="2:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="71"/>
-      <c r="C2" s="71"/>
-      <c r="D2" s="71"/>
-      <c r="E2" s="71"/>
-      <c r="F2" s="71"/>
-      <c r="G2" s="71"/>
-      <c r="H2" s="71"/>
-      <c r="I2" s="71"/>
-      <c r="J2" s="71"/>
-      <c r="K2" s="71"/>
-      <c r="L2" s="71"/>
-      <c r="M2" s="71"/>
-      <c r="N2" s="71"/>
-      <c r="O2" s="71"/>
-      <c r="P2" s="71"/>
+      <c r="B2" s="80"/>
+      <c r="C2" s="80"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="80"/>
+      <c r="F2" s="80"/>
+      <c r="G2" s="80"/>
+      <c r="H2" s="80"/>
+      <c r="I2" s="80"/>
+      <c r="J2" s="80"/>
+      <c r="K2" s="80"/>
+      <c r="L2" s="80"/>
+      <c r="M2" s="80"/>
+      <c r="N2" s="80"/>
+      <c r="O2" s="80"/>
+      <c r="P2" s="80"/>
     </row>
     <row r="3" spans="2:18" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="72" t="s">
+      <c r="B3" s="81" t="s">
         <v>63</v>
       </c>
-      <c r="C3" s="72"/>
-      <c r="D3" s="72"/>
-      <c r="E3" s="72"/>
-      <c r="F3" s="72"/>
-      <c r="G3" s="72"/>
-      <c r="H3" s="72"/>
-      <c r="I3" s="72"/>
-      <c r="J3" s="72"/>
-      <c r="K3" s="72"/>
-      <c r="L3" s="72"/>
-      <c r="M3" s="72"/>
-      <c r="N3" s="72"/>
-      <c r="O3" s="72"/>
-      <c r="P3" s="72"/>
+      <c r="C3" s="81"/>
+      <c r="D3" s="81"/>
+      <c r="E3" s="81"/>
+      <c r="F3" s="81"/>
+      <c r="G3" s="81"/>
+      <c r="H3" s="81"/>
+      <c r="I3" s="81"/>
+      <c r="J3" s="81"/>
+      <c r="K3" s="81"/>
+      <c r="L3" s="81"/>
+      <c r="M3" s="81"/>
+      <c r="N3" s="81"/>
+      <c r="O3" s="81"/>
+      <c r="P3" s="81"/>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
@@ -3591,7 +3645,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:N6"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection sqref="A1:IV65536"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3615,36 +3671,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="71"/>
-      <c r="C2" s="71"/>
-      <c r="D2" s="71"/>
-      <c r="E2" s="71"/>
-      <c r="F2" s="71"/>
-      <c r="G2" s="71"/>
-      <c r="H2" s="71"/>
-      <c r="I2" s="71"/>
-      <c r="J2" s="71"/>
-      <c r="K2" s="71"/>
-      <c r="L2" s="71"/>
-      <c r="M2" s="71"/>
-      <c r="N2" s="71"/>
+      <c r="B2" s="80"/>
+      <c r="C2" s="80"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="80"/>
+      <c r="F2" s="80"/>
+      <c r="G2" s="80"/>
+      <c r="H2" s="80"/>
+      <c r="I2" s="80"/>
+      <c r="J2" s="80"/>
+      <c r="K2" s="80"/>
+      <c r="L2" s="80"/>
+      <c r="M2" s="80"/>
+      <c r="N2" s="80"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="72" t="s">
+      <c r="B3" s="81" t="s">
         <v>64</v>
       </c>
-      <c r="C3" s="72"/>
-      <c r="D3" s="72"/>
-      <c r="E3" s="72"/>
-      <c r="F3" s="72"/>
-      <c r="G3" s="72"/>
-      <c r="H3" s="72"/>
-      <c r="I3" s="72"/>
-      <c r="J3" s="72"/>
-      <c r="K3" s="72"/>
-      <c r="L3" s="72"/>
-      <c r="M3" s="72"/>
-      <c r="N3" s="72"/>
+      <c r="C3" s="81"/>
+      <c r="D3" s="81"/>
+      <c r="E3" s="81"/>
+      <c r="F3" s="81"/>
+      <c r="G3" s="81"/>
+      <c r="H3" s="81"/>
+      <c r="I3" s="81"/>
+      <c r="J3" s="81"/>
+      <c r="K3" s="81"/>
+      <c r="L3" s="81"/>
+      <c r="M3" s="81"/>
+      <c r="N3" s="81"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="58" t="s">
@@ -3731,38 +3787,38 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="71" t="s">
+      <c r="B2" s="80" t="s">
         <v>97</v>
       </c>
-      <c r="C2" s="71"/>
-      <c r="D2" s="71"/>
-      <c r="E2" s="71"/>
-      <c r="F2" s="71"/>
-      <c r="G2" s="71"/>
-      <c r="H2" s="71"/>
-      <c r="I2" s="71"/>
-      <c r="J2" s="71"/>
-      <c r="K2" s="71"/>
-      <c r="L2" s="71"/>
-      <c r="M2" s="71"/>
-      <c r="N2" s="71"/>
+      <c r="C2" s="80"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="80"/>
+      <c r="F2" s="80"/>
+      <c r="G2" s="80"/>
+      <c r="H2" s="80"/>
+      <c r="I2" s="80"/>
+      <c r="J2" s="80"/>
+      <c r="K2" s="80"/>
+      <c r="L2" s="80"/>
+      <c r="M2" s="80"/>
+      <c r="N2" s="80"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="72" t="s">
+      <c r="B3" s="81" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="72"/>
-      <c r="D3" s="72"/>
-      <c r="E3" s="72"/>
-      <c r="F3" s="72"/>
-      <c r="G3" s="72"/>
-      <c r="H3" s="72"/>
-      <c r="I3" s="72"/>
-      <c r="J3" s="72"/>
-      <c r="K3" s="72"/>
-      <c r="L3" s="72"/>
-      <c r="M3" s="72"/>
-      <c r="N3" s="72"/>
+      <c r="C3" s="81"/>
+      <c r="D3" s="81"/>
+      <c r="E3" s="81"/>
+      <c r="F3" s="81"/>
+      <c r="G3" s="81"/>
+      <c r="H3" s="81"/>
+      <c r="I3" s="81"/>
+      <c r="J3" s="81"/>
+      <c r="K3" s="81"/>
+      <c r="L3" s="81"/>
+      <c r="M3" s="81"/>
+      <c r="N3" s="81"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="44" t="s">
@@ -3792,6 +3848,221 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:N6"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.85546875" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5703125" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" customWidth="1"/>
+    <col min="8" max="8" width="18.28515625" customWidth="1"/>
+    <col min="9" max="9" width="18.7109375" customWidth="1"/>
+    <col min="10" max="10" width="22.140625" customWidth="1"/>
+    <col min="11" max="11" width="18.7109375" customWidth="1"/>
+    <col min="12" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:14" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B1" s="46" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="80"/>
+      <c r="C2" s="80"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="80"/>
+      <c r="F2" s="80"/>
+      <c r="G2" s="80"/>
+      <c r="H2" s="80"/>
+      <c r="I2" s="80"/>
+      <c r="J2" s="80"/>
+      <c r="K2" s="80"/>
+      <c r="L2" s="80"/>
+      <c r="M2" s="80"/>
+      <c r="N2" s="80"/>
+    </row>
+    <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B3" s="81" t="s">
+        <v>152</v>
+      </c>
+      <c r="C3" s="81"/>
+      <c r="D3" s="81"/>
+      <c r="E3" s="81"/>
+      <c r="F3" s="81"/>
+      <c r="G3" s="81"/>
+      <c r="H3" s="81"/>
+      <c r="I3" s="81"/>
+      <c r="J3" s="81"/>
+      <c r="K3" s="81"/>
+      <c r="L3" s="81"/>
+      <c r="M3" s="81"/>
+      <c r="N3" s="81"/>
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B5" s="74" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="74" t="s">
+        <v>101</v>
+      </c>
+      <c r="D5" s="74" t="s">
+        <v>143</v>
+      </c>
+      <c r="E5" s="74" t="s">
+        <v>144</v>
+      </c>
+      <c r="F5" s="74" t="s">
+        <v>145</v>
+      </c>
+      <c r="G5" s="74" t="s">
+        <v>146</v>
+      </c>
+      <c r="H5" s="74" t="s">
+        <v>147</v>
+      </c>
+      <c r="I5" s="74" t="s">
+        <v>148</v>
+      </c>
+      <c r="J5" s="74" t="s">
+        <v>149</v>
+      </c>
+      <c r="K5" s="74" t="s">
+        <v>150</v>
+      </c>
+      <c r="L5" s="74" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B6" s="8"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="79"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:N2"/>
+    <mergeCell ref="B3:N3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:J6"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:J3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.85546875" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" customWidth="1"/>
+    <col min="6" max="6" width="22.140625" customWidth="1"/>
+    <col min="7" max="7" width="18.7109375" customWidth="1"/>
+    <col min="8" max="8" width="18" customWidth="1"/>
+    <col min="9" max="9" width="23.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:10" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B1" s="46" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="80"/>
+      <c r="C2" s="80"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="80"/>
+      <c r="F2" s="80"/>
+      <c r="G2" s="80"/>
+      <c r="H2" s="80"/>
+      <c r="I2" s="80"/>
+      <c r="J2" s="80"/>
+    </row>
+    <row r="3" spans="2:10" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B3" s="81" t="s">
+        <v>155</v>
+      </c>
+      <c r="C3" s="81"/>
+      <c r="D3" s="81"/>
+      <c r="E3" s="81"/>
+      <c r="F3" s="81"/>
+      <c r="G3" s="81"/>
+      <c r="H3" s="81"/>
+      <c r="I3" s="81"/>
+      <c r="J3" s="81"/>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B5" s="74" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="74" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="74" t="s">
+        <v>147</v>
+      </c>
+      <c r="E5" s="74" t="s">
+        <v>148</v>
+      </c>
+      <c r="F5" s="74" t="s">
+        <v>149</v>
+      </c>
+      <c r="G5" s="74" t="s">
+        <v>150</v>
+      </c>
+      <c r="H5" s="74" t="s">
+        <v>153</v>
+      </c>
+      <c r="I5" s="74" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="79"/>
+      <c r="I6" s="79"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="B3:J3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:Z8"/>
   <sheetViews>
@@ -3815,37 +4086,37 @@
       <c r="Z1" s="38"/>
     </row>
     <row r="2" spans="2:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="71"/>
-      <c r="C2" s="71"/>
-      <c r="D2" s="71"/>
-      <c r="E2" s="71"/>
-      <c r="F2" s="71"/>
-      <c r="G2" s="71"/>
-      <c r="H2" s="71"/>
-      <c r="I2" s="71"/>
-      <c r="J2" s="71"/>
-      <c r="K2" s="71"/>
-      <c r="L2" s="71"/>
-      <c r="M2" s="71"/>
-      <c r="N2" s="71"/>
+      <c r="B2" s="80"/>
+      <c r="C2" s="80"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="80"/>
+      <c r="F2" s="80"/>
+      <c r="G2" s="80"/>
+      <c r="H2" s="80"/>
+      <c r="I2" s="80"/>
+      <c r="J2" s="80"/>
+      <c r="K2" s="80"/>
+      <c r="L2" s="80"/>
+      <c r="M2" s="80"/>
+      <c r="N2" s="80"/>
       <c r="Z2"/>
     </row>
     <row r="3" spans="2:26" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="72" t="s">
+      <c r="B3" s="81" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="72"/>
-      <c r="D3" s="72"/>
-      <c r="E3" s="72"/>
-      <c r="F3" s="72"/>
-      <c r="G3" s="72"/>
-      <c r="H3" s="72"/>
-      <c r="I3" s="72"/>
-      <c r="J3" s="72"/>
-      <c r="K3" s="72"/>
-      <c r="L3" s="72"/>
-      <c r="M3" s="72"/>
-      <c r="N3" s="72"/>
+      <c r="C3" s="81"/>
+      <c r="D3" s="81"/>
+      <c r="E3" s="81"/>
+      <c r="F3" s="81"/>
+      <c r="G3" s="81"/>
+      <c r="H3" s="81"/>
+      <c r="I3" s="81"/>
+      <c r="J3" s="81"/>
+      <c r="K3" s="81"/>
+      <c r="L3" s="81"/>
+      <c r="M3" s="81"/>
+      <c r="N3" s="81"/>
       <c r="Z3"/>
     </row>
     <row r="5" spans="2:26" x14ac:dyDescent="0.25">
@@ -3925,7 +4196,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:Z8"/>
   <sheetViews>
@@ -3949,37 +4220,37 @@
       <c r="Z1" s="38"/>
     </row>
     <row r="2" spans="2:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="71"/>
-      <c r="C2" s="71"/>
-      <c r="D2" s="71"/>
-      <c r="E2" s="71"/>
-      <c r="F2" s="71"/>
-      <c r="G2" s="71"/>
-      <c r="H2" s="71"/>
-      <c r="I2" s="71"/>
-      <c r="J2" s="71"/>
-      <c r="K2" s="71"/>
-      <c r="L2" s="71"/>
-      <c r="M2" s="71"/>
-      <c r="N2" s="71"/>
+      <c r="B2" s="80"/>
+      <c r="C2" s="80"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="80"/>
+      <c r="F2" s="80"/>
+      <c r="G2" s="80"/>
+      <c r="H2" s="80"/>
+      <c r="I2" s="80"/>
+      <c r="J2" s="80"/>
+      <c r="K2" s="80"/>
+      <c r="L2" s="80"/>
+      <c r="M2" s="80"/>
+      <c r="N2" s="80"/>
       <c r="Z2"/>
     </row>
     <row r="3" spans="2:26" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="72" t="s">
+      <c r="B3" s="81" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="72"/>
-      <c r="D3" s="72"/>
-      <c r="E3" s="72"/>
-      <c r="F3" s="72"/>
-      <c r="G3" s="72"/>
-      <c r="H3" s="72"/>
-      <c r="I3" s="72"/>
-      <c r="J3" s="72"/>
-      <c r="K3" s="72"/>
-      <c r="L3" s="72"/>
-      <c r="M3" s="72"/>
-      <c r="N3" s="72"/>
+      <c r="C3" s="81"/>
+      <c r="D3" s="81"/>
+      <c r="E3" s="81"/>
+      <c r="F3" s="81"/>
+      <c r="G3" s="81"/>
+      <c r="H3" s="81"/>
+      <c r="I3" s="81"/>
+      <c r="J3" s="81"/>
+      <c r="K3" s="81"/>
+      <c r="L3" s="81"/>
+      <c r="M3" s="81"/>
+      <c r="N3" s="81"/>
       <c r="Z3"/>
     </row>
     <row r="5" spans="2:26" x14ac:dyDescent="0.25">
@@ -3998,9 +4269,9 @@
       <c r="C6" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="D6" s="74"/>
-      <c r="E6" s="75"/>
-      <c r="F6" s="76"/>
+      <c r="D6" s="83"/>
+      <c r="E6" s="84"/>
+      <c r="F6" s="85"/>
       <c r="G6" s="50"/>
       <c r="H6" s="50"/>
     </row>
@@ -4054,7 +4325,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:Z8"/>
   <sheetViews>
@@ -4078,37 +4349,37 @@
       <c r="Z1" s="38"/>
     </row>
     <row r="2" spans="2:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="71"/>
-      <c r="C2" s="71"/>
-      <c r="D2" s="71"/>
-      <c r="E2" s="71"/>
-      <c r="F2" s="71"/>
-      <c r="G2" s="71"/>
-      <c r="H2" s="71"/>
-      <c r="I2" s="71"/>
-      <c r="J2" s="71"/>
-      <c r="K2" s="71"/>
-      <c r="L2" s="71"/>
-      <c r="M2" s="71"/>
-      <c r="N2" s="71"/>
+      <c r="B2" s="80"/>
+      <c r="C2" s="80"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="80"/>
+      <c r="F2" s="80"/>
+      <c r="G2" s="80"/>
+      <c r="H2" s="80"/>
+      <c r="I2" s="80"/>
+      <c r="J2" s="80"/>
+      <c r="K2" s="80"/>
+      <c r="L2" s="80"/>
+      <c r="M2" s="80"/>
+      <c r="N2" s="80"/>
       <c r="Z2"/>
     </row>
     <row r="3" spans="2:26" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="72" t="s">
+      <c r="B3" s="81" t="s">
         <v>93</v>
       </c>
-      <c r="C3" s="72"/>
-      <c r="D3" s="72"/>
-      <c r="E3" s="72"/>
-      <c r="F3" s="72"/>
-      <c r="G3" s="72"/>
-      <c r="H3" s="72"/>
-      <c r="I3" s="72"/>
-      <c r="J3" s="72"/>
-      <c r="K3" s="72"/>
-      <c r="L3" s="72"/>
-      <c r="M3" s="72"/>
-      <c r="N3" s="72"/>
+      <c r="C3" s="81"/>
+      <c r="D3" s="81"/>
+      <c r="E3" s="81"/>
+      <c r="F3" s="81"/>
+      <c r="G3" s="81"/>
+      <c r="H3" s="81"/>
+      <c r="I3" s="81"/>
+      <c r="J3" s="81"/>
+      <c r="K3" s="81"/>
+      <c r="L3" s="81"/>
+      <c r="M3" s="81"/>
+      <c r="N3" s="81"/>
       <c r="Z3"/>
     </row>
     <row r="5" spans="2:26" x14ac:dyDescent="0.25">
@@ -4179,13 +4450,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:Z8"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
-    </sheetView>
+    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4203,37 +4472,37 @@
       <c r="Z1" s="38"/>
     </row>
     <row r="2" spans="2:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="71"/>
-      <c r="C2" s="71"/>
-      <c r="D2" s="71"/>
-      <c r="E2" s="71"/>
-      <c r="F2" s="71"/>
-      <c r="G2" s="71"/>
-      <c r="H2" s="71"/>
-      <c r="I2" s="71"/>
-      <c r="J2" s="71"/>
-      <c r="K2" s="71"/>
-      <c r="L2" s="71"/>
-      <c r="M2" s="71"/>
-      <c r="N2" s="71"/>
+      <c r="B2" s="80"/>
+      <c r="C2" s="80"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="80"/>
+      <c r="F2" s="80"/>
+      <c r="G2" s="80"/>
+      <c r="H2" s="80"/>
+      <c r="I2" s="80"/>
+      <c r="J2" s="80"/>
+      <c r="K2" s="80"/>
+      <c r="L2" s="80"/>
+      <c r="M2" s="80"/>
+      <c r="N2" s="80"/>
       <c r="Z2"/>
     </row>
     <row r="3" spans="2:26" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="72" t="s">
+      <c r="B3" s="81" t="s">
         <v>72</v>
       </c>
-      <c r="C3" s="72"/>
-      <c r="D3" s="72"/>
-      <c r="E3" s="72"/>
-      <c r="F3" s="72"/>
-      <c r="G3" s="72"/>
-      <c r="H3" s="72"/>
-      <c r="I3" s="72"/>
-      <c r="J3" s="72"/>
-      <c r="K3" s="72"/>
-      <c r="L3" s="72"/>
-      <c r="M3" s="72"/>
-      <c r="N3" s="72"/>
+      <c r="C3" s="81"/>
+      <c r="D3" s="81"/>
+      <c r="E3" s="81"/>
+      <c r="F3" s="81"/>
+      <c r="G3" s="81"/>
+      <c r="H3" s="81"/>
+      <c r="I3" s="81"/>
+      <c r="J3" s="81"/>
+      <c r="K3" s="81"/>
+      <c r="L3" s="81"/>
+      <c r="M3" s="81"/>
+      <c r="N3" s="81"/>
       <c r="Z3"/>
     </row>
     <row r="5" spans="2:26" x14ac:dyDescent="0.25">
@@ -4311,23 +4580,25 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:Q7"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="I40" sqref="I40"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.85546875" customWidth="1"/>
     <col min="2" max="2" width="10.5703125" customWidth="1"/>
-    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" customWidth="1"/>
     <col min="4" max="4" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="4.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.42578125" customWidth="1"/>
     <col min="10" max="10" width="5.140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="5.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="5.7109375" bestFit="1" customWidth="1"/>
@@ -4344,104 +4615,104 @@
       </c>
     </row>
     <row r="2" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="71"/>
-      <c r="C2" s="71"/>
-      <c r="D2" s="71"/>
-      <c r="E2" s="71"/>
-      <c r="F2" s="71"/>
-      <c r="G2" s="71"/>
-      <c r="H2" s="71"/>
-      <c r="I2" s="71"/>
-      <c r="J2" s="71"/>
-      <c r="K2" s="71"/>
-      <c r="L2" s="71"/>
+      <c r="B2" s="80"/>
+      <c r="C2" s="80"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="80"/>
+      <c r="F2" s="80"/>
+      <c r="G2" s="80"/>
+      <c r="H2" s="80"/>
+      <c r="I2" s="80"/>
+      <c r="J2" s="80"/>
+      <c r="K2" s="80"/>
+      <c r="L2" s="80"/>
     </row>
     <row r="3" spans="2:17" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="72" t="s">
+      <c r="B3" s="81" t="s">
         <v>108</v>
       </c>
-      <c r="C3" s="72"/>
-      <c r="D3" s="72"/>
-      <c r="E3" s="72"/>
-      <c r="F3" s="72"/>
-      <c r="G3" s="72"/>
-      <c r="H3" s="72"/>
-      <c r="I3" s="72"/>
-      <c r="J3" s="72"/>
-      <c r="K3" s="72"/>
-      <c r="L3" s="72"/>
+      <c r="C3" s="81"/>
+      <c r="D3" s="81"/>
+      <c r="E3" s="81"/>
+      <c r="F3" s="81"/>
+      <c r="G3" s="81"/>
+      <c r="H3" s="81"/>
+      <c r="I3" s="81"/>
+      <c r="J3" s="81"/>
+      <c r="K3" s="81"/>
+      <c r="L3" s="81"/>
     </row>
     <row r="5" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D5" s="77" t="s">
+      <c r="D5" s="86" t="s">
         <v>123</v>
       </c>
-      <c r="E5" s="77"/>
-      <c r="F5" s="78"/>
-      <c r="G5" s="78"/>
-      <c r="H5" s="78"/>
-      <c r="I5" s="78"/>
-      <c r="J5" s="77" t="s">
+      <c r="E5" s="86"/>
+      <c r="F5" s="73"/>
+      <c r="G5" s="73"/>
+      <c r="H5" s="73"/>
+      <c r="I5" s="73"/>
+      <c r="J5" s="86" t="s">
         <v>42</v>
       </c>
-      <c r="K5" s="77"/>
-      <c r="L5" s="77"/>
-      <c r="M5" s="77" t="s">
+      <c r="K5" s="86"/>
+      <c r="L5" s="86"/>
+      <c r="M5" s="86" t="s">
         <v>130</v>
       </c>
-      <c r="N5" s="77"/>
-      <c r="O5" s="77"/>
-      <c r="P5" s="73" t="s">
+      <c r="N5" s="86"/>
+      <c r="O5" s="86"/>
+      <c r="P5" s="82" t="s">
         <v>109</v>
       </c>
-      <c r="Q5" s="73"/>
+      <c r="Q5" s="82"/>
     </row>
     <row r="6" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="70" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="79" t="s">
+      <c r="C6" s="71" t="s">
         <v>138</v>
       </c>
-      <c r="D6" s="69" t="s">
+      <c r="D6" s="63" t="s">
         <v>124</v>
       </c>
-      <c r="E6" s="69" t="s">
+      <c r="E6" s="63" t="s">
         <v>125</v>
       </c>
-      <c r="F6" s="79" t="s">
+      <c r="F6" s="71" t="s">
         <v>139</v>
       </c>
-      <c r="G6" s="79" t="s">
+      <c r="G6" s="71" t="s">
         <v>140</v>
       </c>
-      <c r="H6" s="80" t="s">
+      <c r="H6" s="72" t="s">
         <v>53</v>
       </c>
       <c r="I6" s="70" t="s">
         <v>70</v>
       </c>
-      <c r="J6" s="69" t="s">
+      <c r="J6" s="63" t="s">
         <v>129</v>
       </c>
-      <c r="K6" s="69" t="s">
+      <c r="K6" s="63" t="s">
         <v>128</v>
       </c>
-      <c r="L6" s="68" t="s">
+      <c r="L6" s="69" t="s">
         <v>116</v>
       </c>
-      <c r="M6" s="69" t="s">
+      <c r="M6" s="63" t="s">
         <v>129</v>
       </c>
-      <c r="N6" s="69" t="s">
+      <c r="N6" s="63" t="s">
         <v>128</v>
       </c>
-      <c r="O6" s="68" t="s">
+      <c r="O6" s="69" t="s">
         <v>116</v>
       </c>
-      <c r="P6" s="68" t="s">
+      <c r="P6" s="69" t="s">
         <v>101</v>
       </c>
-      <c r="Q6" s="68" t="s">
+      <c r="Q6" s="69" t="s">
         <v>103</v>
       </c>
     </row>
@@ -4465,18 +4736,18 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="P5:Q5"/>
+    <mergeCell ref="J5:L5"/>
     <mergeCell ref="B2:L2"/>
     <mergeCell ref="B3:L3"/>
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="M5:O5"/>
-    <mergeCell ref="P5:Q5"/>
-    <mergeCell ref="J5:L5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:X8"/>
   <sheetViews>
@@ -4488,12 +4759,12 @@
     <col min="2" max="2" width="10.5703125" customWidth="1"/>
     <col min="3" max="3" width="6.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="7.42578125" customWidth="1"/>
+    <col min="10" max="11" width="6.42578125" customWidth="1"/>
     <col min="12" max="12" width="5.7109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="6.85546875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="8.7109375" bestFit="1" customWidth="1"/>
@@ -4514,177 +4785,177 @@
       </c>
     </row>
     <row r="2" spans="2:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="71"/>
-      <c r="C2" s="71"/>
-      <c r="D2" s="71"/>
-      <c r="E2" s="71"/>
-      <c r="F2" s="71"/>
-      <c r="G2" s="71"/>
-      <c r="H2" s="71"/>
-      <c r="I2" s="71"/>
-      <c r="J2" s="71"/>
-      <c r="K2" s="71"/>
-      <c r="L2" s="71"/>
-      <c r="M2" s="71"/>
-      <c r="N2" s="71"/>
-      <c r="O2" s="71"/>
-      <c r="P2" s="71"/>
+      <c r="B2" s="80"/>
+      <c r="C2" s="80"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="80"/>
+      <c r="F2" s="80"/>
+      <c r="G2" s="80"/>
+      <c r="H2" s="80"/>
+      <c r="I2" s="80"/>
+      <c r="J2" s="80"/>
+      <c r="K2" s="80"/>
+      <c r="L2" s="80"/>
+      <c r="M2" s="80"/>
+      <c r="N2" s="80"/>
+      <c r="O2" s="80"/>
+      <c r="P2" s="80"/>
       <c r="Q2" s="56"/>
       <c r="R2" s="56"/>
     </row>
     <row r="3" spans="2:24" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="72" t="s">
+      <c r="B3" s="81" t="s">
         <v>111</v>
       </c>
-      <c r="C3" s="72"/>
-      <c r="D3" s="72"/>
-      <c r="E3" s="72"/>
-      <c r="F3" s="72"/>
-      <c r="G3" s="72"/>
-      <c r="H3" s="72"/>
-      <c r="I3" s="72"/>
-      <c r="J3" s="72"/>
-      <c r="K3" s="72"/>
-      <c r="L3" s="72"/>
-      <c r="M3" s="72"/>
-      <c r="N3" s="72"/>
-      <c r="O3" s="72"/>
-      <c r="P3" s="72"/>
+      <c r="C3" s="81"/>
+      <c r="D3" s="81"/>
+      <c r="E3" s="81"/>
+      <c r="F3" s="81"/>
+      <c r="G3" s="81"/>
+      <c r="H3" s="81"/>
+      <c r="I3" s="81"/>
+      <c r="J3" s="81"/>
+      <c r="K3" s="81"/>
+      <c r="L3" s="81"/>
+      <c r="M3" s="81"/>
+      <c r="N3" s="81"/>
+      <c r="O3" s="81"/>
+      <c r="P3" s="81"/>
       <c r="Q3" s="57"/>
       <c r="R3" s="57"/>
     </row>
     <row r="5" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B5" s="82" t="s">
+      <c r="B5" s="88" t="s">
         <v>112</v>
       </c>
-      <c r="C5" s="83"/>
-      <c r="D5" s="83"/>
-      <c r="E5" s="83"/>
-      <c r="F5" s="83"/>
-      <c r="G5" s="83"/>
-      <c r="H5" s="83"/>
-      <c r="I5" s="83"/>
-      <c r="J5" s="83"/>
-      <c r="K5" s="83"/>
-      <c r="L5" s="84"/>
-      <c r="M5" s="82" t="s">
+      <c r="C5" s="89"/>
+      <c r="D5" s="89"/>
+      <c r="E5" s="89"/>
+      <c r="F5" s="89"/>
+      <c r="G5" s="89"/>
+      <c r="H5" s="89"/>
+      <c r="I5" s="89"/>
+      <c r="J5" s="89"/>
+      <c r="K5" s="89"/>
+      <c r="L5" s="90"/>
+      <c r="M5" s="88" t="s">
         <v>113</v>
       </c>
-      <c r="N5" s="83"/>
-      <c r="O5" s="83"/>
-      <c r="P5" s="83"/>
-      <c r="Q5" s="83"/>
-      <c r="R5" s="83"/>
-      <c r="S5" s="83"/>
-      <c r="T5" s="83"/>
-      <c r="U5" s="83"/>
-      <c r="V5" s="83"/>
-      <c r="W5" s="83"/>
-      <c r="X5" s="84"/>
+      <c r="N5" s="89"/>
+      <c r="O5" s="89"/>
+      <c r="P5" s="89"/>
+      <c r="Q5" s="89"/>
+      <c r="R5" s="89"/>
+      <c r="S5" s="89"/>
+      <c r="T5" s="89"/>
+      <c r="U5" s="89"/>
+      <c r="V5" s="89"/>
+      <c r="W5" s="89"/>
+      <c r="X5" s="90"/>
     </row>
     <row r="6" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B6" s="85"/>
-      <c r="C6" s="85"/>
-      <c r="D6" s="85"/>
-      <c r="E6" s="85"/>
-      <c r="F6" s="86" t="s">
+      <c r="B6" s="87"/>
+      <c r="C6" s="87"/>
+      <c r="D6" s="87"/>
+      <c r="E6" s="87"/>
+      <c r="F6" s="91" t="s">
         <v>27</v>
       </c>
-      <c r="G6" s="87"/>
-      <c r="H6" s="87"/>
-      <c r="I6" s="88"/>
-      <c r="J6" s="82" t="s">
+      <c r="G6" s="92"/>
+      <c r="H6" s="92"/>
+      <c r="I6" s="93"/>
+      <c r="J6" s="88" t="s">
         <v>30</v>
       </c>
-      <c r="K6" s="83"/>
-      <c r="L6" s="84"/>
-      <c r="M6" s="89"/>
-      <c r="N6" s="82" t="s">
+      <c r="K6" s="89"/>
+      <c r="L6" s="90"/>
+      <c r="M6" s="76"/>
+      <c r="N6" s="88" t="s">
         <v>42</v>
       </c>
-      <c r="O6" s="84"/>
-      <c r="P6" s="82" t="s">
+      <c r="O6" s="90"/>
+      <c r="P6" s="88" t="s">
         <v>106</v>
       </c>
-      <c r="Q6" s="83"/>
-      <c r="R6" s="84"/>
-      <c r="S6" s="89"/>
-      <c r="T6" s="82" t="s">
+      <c r="Q6" s="89"/>
+      <c r="R6" s="90"/>
+      <c r="S6" s="76"/>
+      <c r="T6" s="88" t="s">
         <v>123</v>
       </c>
-      <c r="U6" s="84"/>
-      <c r="V6" s="85"/>
-      <c r="W6" s="85"/>
-      <c r="X6" s="85"/>
+      <c r="U6" s="90"/>
+      <c r="V6" s="87"/>
+      <c r="W6" s="87"/>
+      <c r="X6" s="87"/>
     </row>
     <row r="7" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B7" s="90" t="s">
+      <c r="B7" s="75" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="91" t="s">
+      <c r="C7" s="77" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="90" t="s">
+      <c r="D7" s="75" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="90" t="s">
+      <c r="E7" s="75" t="s">
         <v>29</v>
       </c>
-      <c r="F7" s="81" t="s">
+      <c r="F7" s="78" t="s">
         <v>117</v>
       </c>
-      <c r="G7" s="81" t="s">
+      <c r="G7" s="78" t="s">
         <v>121</v>
       </c>
-      <c r="H7" s="81" t="s">
+      <c r="H7" s="78" t="s">
         <v>122</v>
       </c>
-      <c r="I7" s="81" t="s">
+      <c r="I7" s="78" t="s">
         <v>118</v>
       </c>
-      <c r="J7" s="81" t="s">
+      <c r="J7" s="78" t="s">
         <v>114</v>
       </c>
-      <c r="K7" s="81" t="s">
+      <c r="K7" s="78" t="s">
         <v>115</v>
       </c>
-      <c r="L7" s="81" t="s">
+      <c r="L7" s="78" t="s">
         <v>116</v>
       </c>
-      <c r="M7" s="91" t="s">
+      <c r="M7" s="77" t="s">
         <v>53</v>
       </c>
-      <c r="N7" s="81" t="s">
+      <c r="N7" s="78" t="s">
         <v>119</v>
       </c>
-      <c r="O7" s="81" t="s">
+      <c r="O7" s="78" t="s">
         <v>120</v>
       </c>
-      <c r="P7" s="81" t="s">
+      <c r="P7" s="78" t="s">
         <v>114</v>
       </c>
-      <c r="Q7" s="81" t="s">
+      <c r="Q7" s="78" t="s">
         <v>115</v>
       </c>
-      <c r="R7" s="81" t="s">
+      <c r="R7" s="78" t="s">
         <v>116</v>
       </c>
-      <c r="S7" s="90" t="s">
+      <c r="S7" s="75" t="s">
         <v>141</v>
       </c>
-      <c r="T7" s="81" t="s">
+      <c r="T7" s="78" t="s">
         <v>124</v>
       </c>
-      <c r="U7" s="81" t="s">
+      <c r="U7" s="78" t="s">
         <v>125</v>
       </c>
-      <c r="V7" s="91" t="s">
+      <c r="V7" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="W7" s="91" t="s">
+      <c r="W7" s="77" t="s">
         <v>32</v>
       </c>
-      <c r="X7" s="90" t="s">
+      <c r="X7" s="75" t="s">
         <v>142</v>
       </c>
     </row>
@@ -4715,8 +4986,10 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="P6:R6"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="M5:X5"/>
     <mergeCell ref="T6:U6"/>
-    <mergeCell ref="B6:E6"/>
     <mergeCell ref="V6:X6"/>
     <mergeCell ref="B2:P2"/>
     <mergeCell ref="B3:P3"/>
@@ -4724,14 +4997,12 @@
     <mergeCell ref="J6:L6"/>
     <mergeCell ref="F6:I6"/>
     <mergeCell ref="N6:O6"/>
-    <mergeCell ref="P6:R6"/>
-    <mergeCell ref="M5:X5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A24"/>
   <sheetViews>
@@ -4846,36 +5117,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="71"/>
-      <c r="C2" s="71"/>
-      <c r="D2" s="71"/>
-      <c r="E2" s="71"/>
-      <c r="F2" s="71"/>
-      <c r="G2" s="71"/>
-      <c r="H2" s="71"/>
-      <c r="I2" s="71"/>
-      <c r="J2" s="71"/>
-      <c r="K2" s="71"/>
-      <c r="L2" s="71"/>
-      <c r="M2" s="71"/>
-      <c r="N2" s="71"/>
+      <c r="B2" s="80"/>
+      <c r="C2" s="80"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="80"/>
+      <c r="F2" s="80"/>
+      <c r="G2" s="80"/>
+      <c r="H2" s="80"/>
+      <c r="I2" s="80"/>
+      <c r="J2" s="80"/>
+      <c r="K2" s="80"/>
+      <c r="L2" s="80"/>
+      <c r="M2" s="80"/>
+      <c r="N2" s="80"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="72" t="s">
+      <c r="B3" s="81" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="72"/>
-      <c r="D3" s="72"/>
-      <c r="E3" s="72"/>
-      <c r="F3" s="72"/>
-      <c r="G3" s="72"/>
-      <c r="H3" s="72"/>
-      <c r="I3" s="72"/>
-      <c r="J3" s="72"/>
-      <c r="K3" s="72"/>
-      <c r="L3" s="72"/>
-      <c r="M3" s="72"/>
-      <c r="N3" s="72"/>
+      <c r="C3" s="81"/>
+      <c r="D3" s="81"/>
+      <c r="E3" s="81"/>
+      <c r="F3" s="81"/>
+      <c r="G3" s="81"/>
+      <c r="H3" s="81"/>
+      <c r="I3" s="81"/>
+      <c r="J3" s="81"/>
+      <c r="K3" s="81"/>
+      <c r="L3" s="81"/>
+      <c r="M3" s="81"/>
+      <c r="N3" s="81"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="44" t="s">
@@ -4942,40 +5213,40 @@
       </c>
     </row>
     <row r="2" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="71"/>
-      <c r="C2" s="71"/>
-      <c r="D2" s="71"/>
-      <c r="E2" s="71"/>
-      <c r="F2" s="71"/>
-      <c r="G2" s="71"/>
-      <c r="H2" s="71"/>
-      <c r="I2" s="71"/>
-      <c r="J2" s="71"/>
-      <c r="K2" s="71"/>
-      <c r="L2" s="71"/>
-      <c r="M2" s="71"/>
-      <c r="N2" s="71"/>
-      <c r="O2" s="71"/>
-      <c r="P2" s="71"/>
+      <c r="B2" s="80"/>
+      <c r="C2" s="80"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="80"/>
+      <c r="F2" s="80"/>
+      <c r="G2" s="80"/>
+      <c r="H2" s="80"/>
+      <c r="I2" s="80"/>
+      <c r="J2" s="80"/>
+      <c r="K2" s="80"/>
+      <c r="L2" s="80"/>
+      <c r="M2" s="80"/>
+      <c r="N2" s="80"/>
+      <c r="O2" s="80"/>
+      <c r="P2" s="80"/>
     </row>
     <row r="3" spans="2:16" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="72" t="s">
+      <c r="B3" s="81" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="72"/>
-      <c r="D3" s="72"/>
-      <c r="E3" s="72"/>
-      <c r="F3" s="72"/>
-      <c r="G3" s="72"/>
-      <c r="H3" s="72"/>
-      <c r="I3" s="72"/>
-      <c r="J3" s="72"/>
-      <c r="K3" s="72"/>
-      <c r="L3" s="72"/>
-      <c r="M3" s="72"/>
-      <c r="N3" s="72"/>
-      <c r="O3" s="72"/>
-      <c r="P3" s="72"/>
+      <c r="C3" s="81"/>
+      <c r="D3" s="81"/>
+      <c r="E3" s="81"/>
+      <c r="F3" s="81"/>
+      <c r="G3" s="81"/>
+      <c r="H3" s="81"/>
+      <c r="I3" s="81"/>
+      <c r="J3" s="81"/>
+      <c r="K3" s="81"/>
+      <c r="L3" s="81"/>
+      <c r="M3" s="81"/>
+      <c r="N3" s="81"/>
+      <c r="O3" s="81"/>
+      <c r="P3" s="81"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="44" t="s">
@@ -5054,40 +5325,40 @@
       </c>
     </row>
     <row r="2" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="71"/>
-      <c r="C2" s="71"/>
-      <c r="D2" s="71"/>
-      <c r="E2" s="71"/>
-      <c r="F2" s="71"/>
-      <c r="G2" s="71"/>
-      <c r="H2" s="71"/>
-      <c r="I2" s="71"/>
-      <c r="J2" s="71"/>
-      <c r="K2" s="71"/>
-      <c r="L2" s="71"/>
-      <c r="M2" s="71"/>
-      <c r="N2" s="71"/>
-      <c r="O2" s="71"/>
-      <c r="P2" s="71"/>
+      <c r="B2" s="80"/>
+      <c r="C2" s="80"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="80"/>
+      <c r="F2" s="80"/>
+      <c r="G2" s="80"/>
+      <c r="H2" s="80"/>
+      <c r="I2" s="80"/>
+      <c r="J2" s="80"/>
+      <c r="K2" s="80"/>
+      <c r="L2" s="80"/>
+      <c r="M2" s="80"/>
+      <c r="N2" s="80"/>
+      <c r="O2" s="80"/>
+      <c r="P2" s="80"/>
     </row>
     <row r="3" spans="2:16" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="72" t="s">
+      <c r="B3" s="81" t="s">
         <v>68</v>
       </c>
-      <c r="C3" s="72"/>
-      <c r="D3" s="72"/>
-      <c r="E3" s="72"/>
-      <c r="F3" s="72"/>
-      <c r="G3" s="72"/>
-      <c r="H3" s="72"/>
-      <c r="I3" s="72"/>
-      <c r="J3" s="72"/>
-      <c r="K3" s="72"/>
-      <c r="L3" s="72"/>
-      <c r="M3" s="72"/>
-      <c r="N3" s="72"/>
-      <c r="O3" s="72"/>
-      <c r="P3" s="72"/>
+      <c r="C3" s="81"/>
+      <c r="D3" s="81"/>
+      <c r="E3" s="81"/>
+      <c r="F3" s="81"/>
+      <c r="G3" s="81"/>
+      <c r="H3" s="81"/>
+      <c r="I3" s="81"/>
+      <c r="J3" s="81"/>
+      <c r="K3" s="81"/>
+      <c r="L3" s="81"/>
+      <c r="M3" s="81"/>
+      <c r="N3" s="81"/>
+      <c r="O3" s="81"/>
+      <c r="P3" s="81"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
@@ -5136,40 +5407,40 @@
       </c>
     </row>
     <row r="2" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="71"/>
-      <c r="C2" s="71"/>
-      <c r="D2" s="71"/>
-      <c r="E2" s="71"/>
-      <c r="F2" s="71"/>
-      <c r="G2" s="71"/>
-      <c r="H2" s="71"/>
-      <c r="I2" s="71"/>
-      <c r="J2" s="71"/>
-      <c r="K2" s="71"/>
-      <c r="L2" s="71"/>
-      <c r="M2" s="71"/>
-      <c r="N2" s="71"/>
-      <c r="O2" s="71"/>
-      <c r="P2" s="71"/>
+      <c r="B2" s="80"/>
+      <c r="C2" s="80"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="80"/>
+      <c r="F2" s="80"/>
+      <c r="G2" s="80"/>
+      <c r="H2" s="80"/>
+      <c r="I2" s="80"/>
+      <c r="J2" s="80"/>
+      <c r="K2" s="80"/>
+      <c r="L2" s="80"/>
+      <c r="M2" s="80"/>
+      <c r="N2" s="80"/>
+      <c r="O2" s="80"/>
+      <c r="P2" s="80"/>
     </row>
     <row r="3" spans="2:16" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="72" t="s">
+      <c r="B3" s="81" t="s">
         <v>71</v>
       </c>
-      <c r="C3" s="72"/>
-      <c r="D3" s="72"/>
-      <c r="E3" s="72"/>
-      <c r="F3" s="72"/>
-      <c r="G3" s="72"/>
-      <c r="H3" s="72"/>
-      <c r="I3" s="72"/>
-      <c r="J3" s="72"/>
-      <c r="K3" s="72"/>
-      <c r="L3" s="72"/>
-      <c r="M3" s="72"/>
-      <c r="N3" s="72"/>
-      <c r="O3" s="72"/>
-      <c r="P3" s="72"/>
+      <c r="C3" s="81"/>
+      <c r="D3" s="81"/>
+      <c r="E3" s="81"/>
+      <c r="F3" s="81"/>
+      <c r="G3" s="81"/>
+      <c r="H3" s="81"/>
+      <c r="I3" s="81"/>
+      <c r="J3" s="81"/>
+      <c r="K3" s="81"/>
+      <c r="L3" s="81"/>
+      <c r="M3" s="81"/>
+      <c r="N3" s="81"/>
+      <c r="O3" s="81"/>
+      <c r="P3" s="81"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
@@ -5197,8 +5468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:N6"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView showGridLines="0" topLeftCell="D1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5:L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5223,36 +5494,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="71"/>
-      <c r="C2" s="71"/>
-      <c r="D2" s="71"/>
-      <c r="E2" s="71"/>
-      <c r="F2" s="71"/>
-      <c r="G2" s="71"/>
-      <c r="H2" s="71"/>
-      <c r="I2" s="71"/>
-      <c r="J2" s="71"/>
-      <c r="K2" s="71"/>
-      <c r="L2" s="71"/>
-      <c r="M2" s="71"/>
-      <c r="N2" s="71"/>
+      <c r="B2" s="80"/>
+      <c r="C2" s="80"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="80"/>
+      <c r="F2" s="80"/>
+      <c r="G2" s="80"/>
+      <c r="H2" s="80"/>
+      <c r="I2" s="80"/>
+      <c r="J2" s="80"/>
+      <c r="K2" s="80"/>
+      <c r="L2" s="80"/>
+      <c r="M2" s="80"/>
+      <c r="N2" s="80"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="72" t="s">
+      <c r="B3" s="81" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="72"/>
-      <c r="D3" s="72"/>
-      <c r="E3" s="72"/>
-      <c r="F3" s="72"/>
-      <c r="G3" s="72"/>
-      <c r="H3" s="72"/>
-      <c r="I3" s="72"/>
-      <c r="J3" s="72"/>
-      <c r="K3" s="72"/>
-      <c r="L3" s="72"/>
-      <c r="M3" s="72"/>
-      <c r="N3" s="72"/>
+      <c r="C3" s="81"/>
+      <c r="D3" s="81"/>
+      <c r="E3" s="81"/>
+      <c r="F3" s="81"/>
+      <c r="G3" s="81"/>
+      <c r="H3" s="81"/>
+      <c r="I3" s="81"/>
+      <c r="J3" s="81"/>
+      <c r="K3" s="81"/>
+      <c r="L3" s="81"/>
+      <c r="M3" s="81"/>
+      <c r="N3" s="81"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="44" t="s">
@@ -5299,7 +5570,7 @@
       <c r="H6" s="8"/>
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
-      <c r="K6" s="67"/>
+      <c r="K6" s="68"/>
       <c r="L6" s="6"/>
     </row>
   </sheetData>
@@ -5341,40 +5612,40 @@
       </c>
     </row>
     <row r="2" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="71"/>
-      <c r="C2" s="71"/>
-      <c r="D2" s="71"/>
-      <c r="E2" s="71"/>
-      <c r="F2" s="71"/>
-      <c r="G2" s="71"/>
-      <c r="H2" s="71"/>
-      <c r="I2" s="71"/>
-      <c r="J2" s="71"/>
-      <c r="K2" s="71"/>
-      <c r="L2" s="71"/>
-      <c r="M2" s="71"/>
-      <c r="N2" s="71"/>
-      <c r="O2" s="71"/>
-      <c r="P2" s="71"/>
+      <c r="B2" s="80"/>
+      <c r="C2" s="80"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="80"/>
+      <c r="F2" s="80"/>
+      <c r="G2" s="80"/>
+      <c r="H2" s="80"/>
+      <c r="I2" s="80"/>
+      <c r="J2" s="80"/>
+      <c r="K2" s="80"/>
+      <c r="L2" s="80"/>
+      <c r="M2" s="80"/>
+      <c r="N2" s="80"/>
+      <c r="O2" s="80"/>
+      <c r="P2" s="80"/>
     </row>
     <row r="3" spans="2:16" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="72" t="s">
+      <c r="B3" s="81" t="s">
         <v>65</v>
       </c>
-      <c r="C3" s="72"/>
-      <c r="D3" s="72"/>
-      <c r="E3" s="72"/>
-      <c r="F3" s="72"/>
-      <c r="G3" s="72"/>
-      <c r="H3" s="72"/>
-      <c r="I3" s="72"/>
-      <c r="J3" s="72"/>
-      <c r="K3" s="72"/>
-      <c r="L3" s="72"/>
-      <c r="M3" s="72"/>
-      <c r="N3" s="72"/>
-      <c r="O3" s="72"/>
-      <c r="P3" s="72"/>
+      <c r="C3" s="81"/>
+      <c r="D3" s="81"/>
+      <c r="E3" s="81"/>
+      <c r="F3" s="81"/>
+      <c r="G3" s="81"/>
+      <c r="H3" s="81"/>
+      <c r="I3" s="81"/>
+      <c r="J3" s="81"/>
+      <c r="K3" s="81"/>
+      <c r="L3" s="81"/>
+      <c r="M3" s="81"/>
+      <c r="N3" s="81"/>
+      <c r="O3" s="81"/>
+      <c r="P3" s="81"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="45" t="s">
@@ -5426,36 +5697,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="71"/>
-      <c r="C2" s="71"/>
-      <c r="D2" s="71"/>
-      <c r="E2" s="71"/>
-      <c r="F2" s="71"/>
-      <c r="G2" s="71"/>
-      <c r="H2" s="71"/>
-      <c r="I2" s="71"/>
-      <c r="J2" s="71"/>
-      <c r="K2" s="71"/>
-      <c r="L2" s="71"/>
-      <c r="M2" s="71"/>
-      <c r="N2" s="71"/>
+      <c r="B2" s="80"/>
+      <c r="C2" s="80"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="80"/>
+      <c r="F2" s="80"/>
+      <c r="G2" s="80"/>
+      <c r="H2" s="80"/>
+      <c r="I2" s="80"/>
+      <c r="J2" s="80"/>
+      <c r="K2" s="80"/>
+      <c r="L2" s="80"/>
+      <c r="M2" s="80"/>
+      <c r="N2" s="80"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="72" t="s">
+      <c r="B3" s="81" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="72"/>
-      <c r="D3" s="72"/>
-      <c r="E3" s="72"/>
-      <c r="F3" s="72"/>
-      <c r="G3" s="72"/>
-      <c r="H3" s="72"/>
-      <c r="I3" s="72"/>
-      <c r="J3" s="72"/>
-      <c r="K3" s="72"/>
-      <c r="L3" s="72"/>
-      <c r="M3" s="72"/>
-      <c r="N3" s="72"/>
+      <c r="C3" s="81"/>
+      <c r="D3" s="81"/>
+      <c r="E3" s="81"/>
+      <c r="F3" s="81"/>
+      <c r="G3" s="81"/>
+      <c r="H3" s="81"/>
+      <c r="I3" s="81"/>
+      <c r="J3" s="81"/>
+      <c r="K3" s="81"/>
+      <c r="L3" s="81"/>
+      <c r="M3" s="81"/>
+      <c r="N3" s="81"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">

</xml_diff>

<commit_message>
TRIEDA-1590 - Alterando nome das colunas do relatorio de atendimentos por disciplina.
</commit_message>
<xml_diff>
--- a/code/client/web/src/main/resources/templateExport.xlsx
+++ b/code/client/web/src/main/resources/templateExport.xlsx
@@ -2321,17 +2321,17 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="28" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3971,7 +3971,7 @@
   <dimension ref="B1:J6"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:J3"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3979,10 +3979,10 @@
     <col min="1" max="1" width="2.85546875" customWidth="1"/>
     <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" customWidth="1"/>
-    <col min="6" max="6" width="22.140625" customWidth="1"/>
-    <col min="7" max="7" width="18.7109375" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" customWidth="1"/>
+    <col min="6" max="6" width="18.28515625" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" customWidth="1"/>
     <col min="8" max="8" width="18" customWidth="1"/>
     <col min="9" max="9" width="23.42578125" customWidth="1"/>
   </cols>
@@ -4024,16 +4024,16 @@
         <v>27</v>
       </c>
       <c r="D5" s="74" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E5" s="74" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="F5" s="74" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="G5" s="74" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="H5" s="74" t="s">
         <v>153</v>
@@ -4825,68 +4825,68 @@
       <c r="R3" s="57"/>
     </row>
     <row r="5" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B5" s="88" t="s">
+      <c r="B5" s="87" t="s">
         <v>112</v>
       </c>
-      <c r="C5" s="89"/>
-      <c r="D5" s="89"/>
-      <c r="E5" s="89"/>
-      <c r="F5" s="89"/>
-      <c r="G5" s="89"/>
-      <c r="H5" s="89"/>
-      <c r="I5" s="89"/>
-      <c r="J5" s="89"/>
-      <c r="K5" s="89"/>
-      <c r="L5" s="90"/>
-      <c r="M5" s="88" t="s">
+      <c r="C5" s="88"/>
+      <c r="D5" s="88"/>
+      <c r="E5" s="88"/>
+      <c r="F5" s="88"/>
+      <c r="G5" s="88"/>
+      <c r="H5" s="88"/>
+      <c r="I5" s="88"/>
+      <c r="J5" s="88"/>
+      <c r="K5" s="88"/>
+      <c r="L5" s="89"/>
+      <c r="M5" s="87" t="s">
         <v>113</v>
       </c>
-      <c r="N5" s="89"/>
-      <c r="O5" s="89"/>
-      <c r="P5" s="89"/>
-      <c r="Q5" s="89"/>
-      <c r="R5" s="89"/>
-      <c r="S5" s="89"/>
-      <c r="T5" s="89"/>
-      <c r="U5" s="89"/>
-      <c r="V5" s="89"/>
-      <c r="W5" s="89"/>
-      <c r="X5" s="90"/>
+      <c r="N5" s="88"/>
+      <c r="O5" s="88"/>
+      <c r="P5" s="88"/>
+      <c r="Q5" s="88"/>
+      <c r="R5" s="88"/>
+      <c r="S5" s="88"/>
+      <c r="T5" s="88"/>
+      <c r="U5" s="88"/>
+      <c r="V5" s="88"/>
+      <c r="W5" s="88"/>
+      <c r="X5" s="89"/>
     </row>
     <row r="6" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B6" s="87"/>
-      <c r="C6" s="87"/>
-      <c r="D6" s="87"/>
-      <c r="E6" s="87"/>
+      <c r="B6" s="90"/>
+      <c r="C6" s="90"/>
+      <c r="D6" s="90"/>
+      <c r="E6" s="90"/>
       <c r="F6" s="91" t="s">
         <v>27</v>
       </c>
       <c r="G6" s="92"/>
       <c r="H6" s="92"/>
       <c r="I6" s="93"/>
-      <c r="J6" s="88" t="s">
+      <c r="J6" s="87" t="s">
         <v>30</v>
       </c>
-      <c r="K6" s="89"/>
-      <c r="L6" s="90"/>
+      <c r="K6" s="88"/>
+      <c r="L6" s="89"/>
       <c r="M6" s="76"/>
-      <c r="N6" s="88" t="s">
+      <c r="N6" s="87" t="s">
         <v>42</v>
       </c>
-      <c r="O6" s="90"/>
-      <c r="P6" s="88" t="s">
+      <c r="O6" s="89"/>
+      <c r="P6" s="87" t="s">
         <v>106</v>
       </c>
-      <c r="Q6" s="89"/>
-      <c r="R6" s="90"/>
+      <c r="Q6" s="88"/>
+      <c r="R6" s="89"/>
       <c r="S6" s="76"/>
-      <c r="T6" s="88" t="s">
+      <c r="T6" s="87" t="s">
         <v>123</v>
       </c>
-      <c r="U6" s="90"/>
-      <c r="V6" s="87"/>
-      <c r="W6" s="87"/>
-      <c r="X6" s="87"/>
+      <c r="U6" s="89"/>
+      <c r="V6" s="90"/>
+      <c r="W6" s="90"/>
+      <c r="X6" s="90"/>
     </row>
     <row r="7" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B7" s="75" t="s">
@@ -4986,6 +4986,7 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="N6:O6"/>
     <mergeCell ref="P6:R6"/>
     <mergeCell ref="B6:E6"/>
     <mergeCell ref="M5:X5"/>
@@ -4996,7 +4997,6 @@
     <mergeCell ref="B5:L5"/>
     <mergeCell ref="J6:L6"/>
     <mergeCell ref="F6:I6"/>
-    <mergeCell ref="N6:O6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
TRIEDA-1612 - Adicionando exportação para excel do relatório de atendimentos por faixa de damanda. Adicionando exportação individual e na exportação de "tabelas" e "tudo".
</commit_message>
<xml_diff>
--- a/code/client/web/src/main/resources/templateExport.xlsx
+++ b/code/client/web/src/main/resources/templateExport.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="17070" windowHeight="5370" tabRatio="622" firstSheet="16" activeTab="20"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="17070" windowHeight="5370" tabRatio="622" firstSheet="17" activeTab="21"/>
   </bookViews>
   <sheets>
     <sheet name="Campi" sheetId="3" r:id="rId1"/>
@@ -28,13 +28,14 @@
     <sheet name="Resumo por disciplina" sheetId="15" r:id="rId19"/>
     <sheet name="Atendimentos por Matricula" sheetId="30" r:id="rId20"/>
     <sheet name="Atendimentos por Disciplina" sheetId="31" r:id="rId21"/>
-    <sheet name="Relatorio Visao Sala" sheetId="10" r:id="rId22"/>
-    <sheet name="Relatorio Visao Aluno" sheetId="25" r:id="rId23"/>
-    <sheet name="Relatorio Visao Professor" sheetId="21" r:id="rId24"/>
-    <sheet name="Relatorio Visao Curso" sheetId="20" r:id="rId25"/>
-    <sheet name="Atendimentos por Aluno" sheetId="23" r:id="rId26"/>
-    <sheet name="Aulas" sheetId="26" r:id="rId27"/>
-    <sheet name="PaletaCores" sheetId="11" r:id="rId28"/>
+    <sheet name="Atendimentos Faixa de Demanda" sheetId="32" r:id="rId22"/>
+    <sheet name="Relatorio Visao Sala" sheetId="10" r:id="rId23"/>
+    <sheet name="Relatorio Visao Aluno" sheetId="25" r:id="rId24"/>
+    <sheet name="Relatorio Visao Professor" sheetId="21" r:id="rId25"/>
+    <sheet name="Relatorio Visao Curso" sheetId="20" r:id="rId26"/>
+    <sheet name="Atendimentos por Aluno" sheetId="23" r:id="rId27"/>
+    <sheet name="Aulas" sheetId="26" r:id="rId28"/>
+    <sheet name="PaletaCores" sheetId="11" r:id="rId29"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
@@ -1213,7 +1214,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="168">
   <si>
     <t>Planilha de Unidades</t>
   </si>
@@ -1681,6 +1682,42 @@
   </si>
   <si>
     <t>Planilha de Atendimentos Por Disciplina</t>
+  </si>
+  <si>
+    <t>Planilha de Atendimentos Por Faixa de Demanda</t>
+  </si>
+  <si>
+    <t>Demanda da Diciplina</t>
+  </si>
+  <si>
+    <t>Atendimento P1</t>
+  </si>
+  <si>
+    <t>% Atendimento P1</t>
+  </si>
+  <si>
+    <t>Atendimento P1+P2</t>
+  </si>
+  <si>
+    <t>% Atendimento P1+P2</t>
+  </si>
+  <si>
+    <t>Turmas Abertas</t>
+  </si>
+  <si>
+    <t>Media de Alunos Por Turma</t>
+  </si>
+  <si>
+    <t>Creditos Pagos</t>
+  </si>
+  <si>
+    <t>Demanda P1 Acum</t>
+  </si>
+  <si>
+    <t>Atendimento P1+P2 Acum</t>
+  </si>
+  <si>
+    <t>% Atendimento Acum</t>
   </si>
 </sst>
 </file>
@@ -2073,7 +2110,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2300,6 +2337,18 @@
     <xf numFmtId="1" fontId="6" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2321,6 +2370,9 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2329,9 +2381,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="28" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2669,38 +2718,38 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="80" t="s">
+      <c r="B2" s="84" t="s">
         <v>96</v>
       </c>
-      <c r="C2" s="80"/>
-      <c r="D2" s="80"/>
-      <c r="E2" s="80"/>
-      <c r="F2" s="80"/>
-      <c r="G2" s="80"/>
-      <c r="H2" s="80"/>
-      <c r="I2" s="80"/>
-      <c r="J2" s="80"/>
-      <c r="K2" s="80"/>
-      <c r="L2" s="80"/>
-      <c r="M2" s="80"/>
-      <c r="N2" s="80"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84"/>
+      <c r="H2" s="84"/>
+      <c r="I2" s="84"/>
+      <c r="J2" s="84"/>
+      <c r="K2" s="84"/>
+      <c r="L2" s="84"/>
+      <c r="M2" s="84"/>
+      <c r="N2" s="84"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="81" t="s">
+      <c r="B3" s="85" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="81"/>
-      <c r="D3" s="81"/>
-      <c r="E3" s="81"/>
-      <c r="F3" s="81"/>
-      <c r="G3" s="81"/>
-      <c r="H3" s="81"/>
-      <c r="I3" s="81"/>
-      <c r="J3" s="81"/>
-      <c r="K3" s="81"/>
-      <c r="L3" s="81"/>
-      <c r="M3" s="81"/>
-      <c r="N3" s="81"/>
+      <c r="C3" s="85"/>
+      <c r="D3" s="85"/>
+      <c r="E3" s="85"/>
+      <c r="F3" s="85"/>
+      <c r="G3" s="85"/>
+      <c r="H3" s="85"/>
+      <c r="I3" s="85"/>
+      <c r="J3" s="85"/>
+      <c r="K3" s="85"/>
+      <c r="L3" s="85"/>
+      <c r="M3" s="85"/>
+      <c r="N3" s="85"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="44" t="s">
@@ -2768,36 +2817,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="80"/>
-      <c r="C2" s="80"/>
-      <c r="D2" s="80"/>
-      <c r="E2" s="80"/>
-      <c r="F2" s="80"/>
-      <c r="G2" s="80"/>
-      <c r="H2" s="80"/>
-      <c r="I2" s="80"/>
-      <c r="J2" s="80"/>
-      <c r="K2" s="80"/>
-      <c r="L2" s="80"/>
-      <c r="M2" s="80"/>
-      <c r="N2" s="80"/>
+      <c r="B2" s="84"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84"/>
+      <c r="H2" s="84"/>
+      <c r="I2" s="84"/>
+      <c r="J2" s="84"/>
+      <c r="K2" s="84"/>
+      <c r="L2" s="84"/>
+      <c r="M2" s="84"/>
+      <c r="N2" s="84"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="81" t="s">
+      <c r="B3" s="85" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="81"/>
-      <c r="D3" s="81"/>
-      <c r="E3" s="81"/>
-      <c r="F3" s="81"/>
-      <c r="G3" s="81"/>
-      <c r="H3" s="81"/>
-      <c r="I3" s="81"/>
-      <c r="J3" s="81"/>
-      <c r="K3" s="81"/>
-      <c r="L3" s="81"/>
-      <c r="M3" s="81"/>
-      <c r="N3" s="81"/>
+      <c r="C3" s="85"/>
+      <c r="D3" s="85"/>
+      <c r="E3" s="85"/>
+      <c r="F3" s="85"/>
+      <c r="G3" s="85"/>
+      <c r="H3" s="85"/>
+      <c r="I3" s="85"/>
+      <c r="J3" s="85"/>
+      <c r="K3" s="85"/>
+      <c r="L3" s="85"/>
+      <c r="M3" s="85"/>
+      <c r="N3" s="85"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -2866,36 +2915,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="80"/>
-      <c r="C2" s="80"/>
-      <c r="D2" s="80"/>
-      <c r="E2" s="80"/>
-      <c r="F2" s="80"/>
-      <c r="G2" s="80"/>
-      <c r="H2" s="80"/>
-      <c r="I2" s="80"/>
-      <c r="J2" s="80"/>
-      <c r="K2" s="80"/>
-      <c r="L2" s="80"/>
-      <c r="M2" s="80"/>
-      <c r="N2" s="80"/>
+      <c r="B2" s="84"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84"/>
+      <c r="H2" s="84"/>
+      <c r="I2" s="84"/>
+      <c r="J2" s="84"/>
+      <c r="K2" s="84"/>
+      <c r="L2" s="84"/>
+      <c r="M2" s="84"/>
+      <c r="N2" s="84"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="81" t="s">
+      <c r="B3" s="85" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="81"/>
-      <c r="D3" s="81"/>
-      <c r="E3" s="81"/>
-      <c r="F3" s="81"/>
-      <c r="G3" s="81"/>
-      <c r="H3" s="81"/>
-      <c r="I3" s="81"/>
-      <c r="J3" s="81"/>
-      <c r="K3" s="81"/>
-      <c r="L3" s="81"/>
-      <c r="M3" s="81"/>
-      <c r="N3" s="81"/>
+      <c r="C3" s="85"/>
+      <c r="D3" s="85"/>
+      <c r="E3" s="85"/>
+      <c r="F3" s="85"/>
+      <c r="G3" s="85"/>
+      <c r="H3" s="85"/>
+      <c r="I3" s="85"/>
+      <c r="J3" s="85"/>
+      <c r="K3" s="85"/>
+      <c r="L3" s="85"/>
+      <c r="M3" s="85"/>
+      <c r="N3" s="85"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -2980,18 +3029,18 @@
       </c>
     </row>
     <row r="2" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="80"/>
-      <c r="C2" s="80"/>
-      <c r="D2" s="80"/>
-      <c r="E2" s="80"/>
+      <c r="B2" s="84"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
     </row>
     <row r="3" spans="2:5" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="81" t="s">
+      <c r="B3" s="85" t="s">
         <v>126</v>
       </c>
-      <c r="C3" s="81"/>
-      <c r="D3" s="81"/>
-      <c r="E3" s="81"/>
+      <c r="C3" s="85"/>
+      <c r="D3" s="85"/>
+      <c r="E3" s="85"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="60" t="s">
@@ -3044,36 +3093,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="80"/>
-      <c r="C2" s="80"/>
-      <c r="D2" s="80"/>
-      <c r="E2" s="80"/>
-      <c r="F2" s="80"/>
-      <c r="G2" s="80"/>
-      <c r="H2" s="80"/>
-      <c r="I2" s="80"/>
-      <c r="J2" s="80"/>
-      <c r="K2" s="80"/>
-      <c r="L2" s="80"/>
-      <c r="M2" s="80"/>
-      <c r="N2" s="80"/>
+      <c r="B2" s="84"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84"/>
+      <c r="H2" s="84"/>
+      <c r="I2" s="84"/>
+      <c r="J2" s="84"/>
+      <c r="K2" s="84"/>
+      <c r="L2" s="84"/>
+      <c r="M2" s="84"/>
+      <c r="N2" s="84"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="81" t="s">
+      <c r="B3" s="85" t="s">
         <v>100</v>
       </c>
-      <c r="C3" s="81"/>
-      <c r="D3" s="81"/>
-      <c r="E3" s="81"/>
-      <c r="F3" s="81"/>
-      <c r="G3" s="81"/>
-      <c r="H3" s="81"/>
-      <c r="I3" s="81"/>
-      <c r="J3" s="81"/>
-      <c r="K3" s="81"/>
-      <c r="L3" s="81"/>
-      <c r="M3" s="81"/>
-      <c r="N3" s="81"/>
+      <c r="C3" s="85"/>
+      <c r="D3" s="85"/>
+      <c r="E3" s="85"/>
+      <c r="F3" s="85"/>
+      <c r="G3" s="85"/>
+      <c r="H3" s="85"/>
+      <c r="I3" s="85"/>
+      <c r="J3" s="85"/>
+      <c r="K3" s="85"/>
+      <c r="L3" s="85"/>
+      <c r="M3" s="85"/>
+      <c r="N3" s="85"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -3106,10 +3155,10 @@
       <c r="K5" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="L5" s="82" t="s">
+      <c r="L5" s="86" t="s">
         <v>110</v>
       </c>
-      <c r="M5" s="82"/>
+      <c r="M5" s="86"/>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
@@ -3161,38 +3210,38 @@
       </c>
     </row>
     <row r="2" spans="2:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="80"/>
-      <c r="C2" s="80"/>
-      <c r="D2" s="80"/>
-      <c r="E2" s="80"/>
-      <c r="F2" s="80"/>
-      <c r="G2" s="80"/>
-      <c r="H2" s="80"/>
-      <c r="I2" s="80"/>
-      <c r="J2" s="80"/>
-      <c r="K2" s="80"/>
-      <c r="L2" s="80"/>
-      <c r="M2" s="80"/>
-      <c r="N2" s="80"/>
-      <c r="O2" s="80"/>
+      <c r="B2" s="84"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84"/>
+      <c r="H2" s="84"/>
+      <c r="I2" s="84"/>
+      <c r="J2" s="84"/>
+      <c r="K2" s="84"/>
+      <c r="L2" s="84"/>
+      <c r="M2" s="84"/>
+      <c r="N2" s="84"/>
+      <c r="O2" s="84"/>
     </row>
     <row r="3" spans="2:15" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="81" t="s">
+      <c r="B3" s="85" t="s">
         <v>73</v>
       </c>
-      <c r="C3" s="81"/>
-      <c r="D3" s="81"/>
-      <c r="E3" s="81"/>
-      <c r="F3" s="81"/>
-      <c r="G3" s="81"/>
-      <c r="H3" s="81"/>
-      <c r="I3" s="81"/>
-      <c r="J3" s="81"/>
-      <c r="K3" s="81"/>
-      <c r="L3" s="81"/>
-      <c r="M3" s="81"/>
-      <c r="N3" s="81"/>
-      <c r="O3" s="81"/>
+      <c r="C3" s="85"/>
+      <c r="D3" s="85"/>
+      <c r="E3" s="85"/>
+      <c r="F3" s="85"/>
+      <c r="G3" s="85"/>
+      <c r="H3" s="85"/>
+      <c r="I3" s="85"/>
+      <c r="J3" s="85"/>
+      <c r="K3" s="85"/>
+      <c r="L3" s="85"/>
+      <c r="M3" s="85"/>
+      <c r="N3" s="85"/>
+      <c r="O3" s="85"/>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -3271,18 +3320,18 @@
       </c>
     </row>
     <row r="2" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="80"/>
-      <c r="C2" s="80"/>
-      <c r="D2" s="80"/>
-      <c r="E2" s="80"/>
+      <c r="B2" s="84"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
     </row>
     <row r="3" spans="2:5" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="81" t="s">
+      <c r="B3" s="85" t="s">
         <v>131</v>
       </c>
-      <c r="C3" s="81"/>
-      <c r="D3" s="81"/>
-      <c r="E3" s="81"/>
+      <c r="C3" s="85"/>
+      <c r="D3" s="85"/>
+      <c r="E3" s="85"/>
     </row>
     <row r="4" spans="2:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="64"/>
@@ -3344,36 +3393,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="80"/>
-      <c r="C2" s="80"/>
-      <c r="D2" s="80"/>
-      <c r="E2" s="80"/>
-      <c r="F2" s="80"/>
-      <c r="G2" s="80"/>
-      <c r="H2" s="80"/>
-      <c r="I2" s="80"/>
-      <c r="J2" s="80"/>
-      <c r="K2" s="80"/>
-      <c r="L2" s="80"/>
-      <c r="M2" s="80"/>
-      <c r="N2" s="80"/>
+      <c r="B2" s="84"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84"/>
+      <c r="H2" s="84"/>
+      <c r="I2" s="84"/>
+      <c r="J2" s="84"/>
+      <c r="K2" s="84"/>
+      <c r="L2" s="84"/>
+      <c r="M2" s="84"/>
+      <c r="N2" s="84"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="81" t="s">
+      <c r="B3" s="85" t="s">
         <v>69</v>
       </c>
-      <c r="C3" s="81"/>
-      <c r="D3" s="81"/>
-      <c r="E3" s="81"/>
-      <c r="F3" s="81"/>
-      <c r="G3" s="81"/>
-      <c r="H3" s="81"/>
-      <c r="I3" s="81"/>
-      <c r="J3" s="81"/>
-      <c r="K3" s="81"/>
-      <c r="L3" s="81"/>
-      <c r="M3" s="81"/>
-      <c r="N3" s="81"/>
+      <c r="C3" s="85"/>
+      <c r="D3" s="85"/>
+      <c r="E3" s="85"/>
+      <c r="F3" s="85"/>
+      <c r="G3" s="85"/>
+      <c r="H3" s="85"/>
+      <c r="I3" s="85"/>
+      <c r="J3" s="85"/>
+      <c r="K3" s="85"/>
+      <c r="L3" s="85"/>
+      <c r="M3" s="85"/>
+      <c r="N3" s="85"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -3428,36 +3477,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="80"/>
-      <c r="C2" s="80"/>
-      <c r="D2" s="80"/>
-      <c r="E2" s="80"/>
-      <c r="F2" s="80"/>
-      <c r="G2" s="80"/>
-      <c r="H2" s="80"/>
-      <c r="I2" s="80"/>
-      <c r="J2" s="80"/>
-      <c r="K2" s="80"/>
-      <c r="L2" s="80"/>
-      <c r="M2" s="80"/>
-      <c r="N2" s="80"/>
+      <c r="B2" s="84"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84"/>
+      <c r="H2" s="84"/>
+      <c r="I2" s="84"/>
+      <c r="J2" s="84"/>
+      <c r="K2" s="84"/>
+      <c r="L2" s="84"/>
+      <c r="M2" s="84"/>
+      <c r="N2" s="84"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="81" t="s">
+      <c r="B3" s="85" t="s">
         <v>74</v>
       </c>
-      <c r="C3" s="81"/>
-      <c r="D3" s="81"/>
-      <c r="E3" s="81"/>
-      <c r="F3" s="81"/>
-      <c r="G3" s="81"/>
-      <c r="H3" s="81"/>
-      <c r="I3" s="81"/>
-      <c r="J3" s="81"/>
-      <c r="K3" s="81"/>
-      <c r="L3" s="81"/>
-      <c r="M3" s="81"/>
-      <c r="N3" s="81"/>
+      <c r="C3" s="85"/>
+      <c r="D3" s="85"/>
+      <c r="E3" s="85"/>
+      <c r="F3" s="85"/>
+      <c r="G3" s="85"/>
+      <c r="H3" s="85"/>
+      <c r="I3" s="85"/>
+      <c r="J3" s="85"/>
+      <c r="K3" s="85"/>
+      <c r="L3" s="85"/>
+      <c r="M3" s="85"/>
+      <c r="N3" s="85"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -3524,40 +3573,40 @@
       </c>
     </row>
     <row r="2" spans="2:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="80"/>
-      <c r="C2" s="80"/>
-      <c r="D2" s="80"/>
-      <c r="E2" s="80"/>
-      <c r="F2" s="80"/>
-      <c r="G2" s="80"/>
-      <c r="H2" s="80"/>
-      <c r="I2" s="80"/>
-      <c r="J2" s="80"/>
-      <c r="K2" s="80"/>
-      <c r="L2" s="80"/>
-      <c r="M2" s="80"/>
-      <c r="N2" s="80"/>
-      <c r="O2" s="80"/>
-      <c r="P2" s="80"/>
+      <c r="B2" s="84"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84"/>
+      <c r="H2" s="84"/>
+      <c r="I2" s="84"/>
+      <c r="J2" s="84"/>
+      <c r="K2" s="84"/>
+      <c r="L2" s="84"/>
+      <c r="M2" s="84"/>
+      <c r="N2" s="84"/>
+      <c r="O2" s="84"/>
+      <c r="P2" s="84"/>
     </row>
     <row r="3" spans="2:18" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="81" t="s">
+      <c r="B3" s="85" t="s">
         <v>63</v>
       </c>
-      <c r="C3" s="81"/>
-      <c r="D3" s="81"/>
-      <c r="E3" s="81"/>
-      <c r="F3" s="81"/>
-      <c r="G3" s="81"/>
-      <c r="H3" s="81"/>
-      <c r="I3" s="81"/>
-      <c r="J3" s="81"/>
-      <c r="K3" s="81"/>
-      <c r="L3" s="81"/>
-      <c r="M3" s="81"/>
-      <c r="N3" s="81"/>
-      <c r="O3" s="81"/>
-      <c r="P3" s="81"/>
+      <c r="C3" s="85"/>
+      <c r="D3" s="85"/>
+      <c r="E3" s="85"/>
+      <c r="F3" s="85"/>
+      <c r="G3" s="85"/>
+      <c r="H3" s="85"/>
+      <c r="I3" s="85"/>
+      <c r="J3" s="85"/>
+      <c r="K3" s="85"/>
+      <c r="L3" s="85"/>
+      <c r="M3" s="85"/>
+      <c r="N3" s="85"/>
+      <c r="O3" s="85"/>
+      <c r="P3" s="85"/>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
@@ -3671,36 +3720,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="80"/>
-      <c r="C2" s="80"/>
-      <c r="D2" s="80"/>
-      <c r="E2" s="80"/>
-      <c r="F2" s="80"/>
-      <c r="G2" s="80"/>
-      <c r="H2" s="80"/>
-      <c r="I2" s="80"/>
-      <c r="J2" s="80"/>
-      <c r="K2" s="80"/>
-      <c r="L2" s="80"/>
-      <c r="M2" s="80"/>
-      <c r="N2" s="80"/>
+      <c r="B2" s="84"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84"/>
+      <c r="H2" s="84"/>
+      <c r="I2" s="84"/>
+      <c r="J2" s="84"/>
+      <c r="K2" s="84"/>
+      <c r="L2" s="84"/>
+      <c r="M2" s="84"/>
+      <c r="N2" s="84"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="81" t="s">
+      <c r="B3" s="85" t="s">
         <v>64</v>
       </c>
-      <c r="C3" s="81"/>
-      <c r="D3" s="81"/>
-      <c r="E3" s="81"/>
-      <c r="F3" s="81"/>
-      <c r="G3" s="81"/>
-      <c r="H3" s="81"/>
-      <c r="I3" s="81"/>
-      <c r="J3" s="81"/>
-      <c r="K3" s="81"/>
-      <c r="L3" s="81"/>
-      <c r="M3" s="81"/>
-      <c r="N3" s="81"/>
+      <c r="C3" s="85"/>
+      <c r="D3" s="85"/>
+      <c r="E3" s="85"/>
+      <c r="F3" s="85"/>
+      <c r="G3" s="85"/>
+      <c r="H3" s="85"/>
+      <c r="I3" s="85"/>
+      <c r="J3" s="85"/>
+      <c r="K3" s="85"/>
+      <c r="L3" s="85"/>
+      <c r="M3" s="85"/>
+      <c r="N3" s="85"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="58" t="s">
@@ -3787,38 +3836,38 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="80" t="s">
+      <c r="B2" s="84" t="s">
         <v>97</v>
       </c>
-      <c r="C2" s="80"/>
-      <c r="D2" s="80"/>
-      <c r="E2" s="80"/>
-      <c r="F2" s="80"/>
-      <c r="G2" s="80"/>
-      <c r="H2" s="80"/>
-      <c r="I2" s="80"/>
-      <c r="J2" s="80"/>
-      <c r="K2" s="80"/>
-      <c r="L2" s="80"/>
-      <c r="M2" s="80"/>
-      <c r="N2" s="80"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84"/>
+      <c r="H2" s="84"/>
+      <c r="I2" s="84"/>
+      <c r="J2" s="84"/>
+      <c r="K2" s="84"/>
+      <c r="L2" s="84"/>
+      <c r="M2" s="84"/>
+      <c r="N2" s="84"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="81" t="s">
+      <c r="B3" s="85" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="81"/>
-      <c r="D3" s="81"/>
-      <c r="E3" s="81"/>
-      <c r="F3" s="81"/>
-      <c r="G3" s="81"/>
-      <c r="H3" s="81"/>
-      <c r="I3" s="81"/>
-      <c r="J3" s="81"/>
-      <c r="K3" s="81"/>
-      <c r="L3" s="81"/>
-      <c r="M3" s="81"/>
-      <c r="N3" s="81"/>
+      <c r="C3" s="85"/>
+      <c r="D3" s="85"/>
+      <c r="E3" s="85"/>
+      <c r="F3" s="85"/>
+      <c r="G3" s="85"/>
+      <c r="H3" s="85"/>
+      <c r="I3" s="85"/>
+      <c r="J3" s="85"/>
+      <c r="K3" s="85"/>
+      <c r="L3" s="85"/>
+      <c r="M3" s="85"/>
+      <c r="N3" s="85"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="44" t="s">
@@ -3877,36 +3926,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="80"/>
-      <c r="C2" s="80"/>
-      <c r="D2" s="80"/>
-      <c r="E2" s="80"/>
-      <c r="F2" s="80"/>
-      <c r="G2" s="80"/>
-      <c r="H2" s="80"/>
-      <c r="I2" s="80"/>
-      <c r="J2" s="80"/>
-      <c r="K2" s="80"/>
-      <c r="L2" s="80"/>
-      <c r="M2" s="80"/>
-      <c r="N2" s="80"/>
+      <c r="B2" s="84"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84"/>
+      <c r="H2" s="84"/>
+      <c r="I2" s="84"/>
+      <c r="J2" s="84"/>
+      <c r="K2" s="84"/>
+      <c r="L2" s="84"/>
+      <c r="M2" s="84"/>
+      <c r="N2" s="84"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="81" t="s">
+      <c r="B3" s="85" t="s">
         <v>152</v>
       </c>
-      <c r="C3" s="81"/>
-      <c r="D3" s="81"/>
-      <c r="E3" s="81"/>
-      <c r="F3" s="81"/>
-      <c r="G3" s="81"/>
-      <c r="H3" s="81"/>
-      <c r="I3" s="81"/>
-      <c r="J3" s="81"/>
-      <c r="K3" s="81"/>
-      <c r="L3" s="81"/>
-      <c r="M3" s="81"/>
-      <c r="N3" s="81"/>
+      <c r="C3" s="85"/>
+      <c r="D3" s="85"/>
+      <c r="E3" s="85"/>
+      <c r="F3" s="85"/>
+      <c r="G3" s="85"/>
+      <c r="H3" s="85"/>
+      <c r="I3" s="85"/>
+      <c r="J3" s="85"/>
+      <c r="K3" s="85"/>
+      <c r="L3" s="85"/>
+      <c r="M3" s="85"/>
+      <c r="N3" s="85"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="74" t="s">
@@ -3970,8 +4019,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J6"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3993,28 +4042,28 @@
       </c>
     </row>
     <row r="2" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="80"/>
-      <c r="C2" s="80"/>
-      <c r="D2" s="80"/>
-      <c r="E2" s="80"/>
-      <c r="F2" s="80"/>
-      <c r="G2" s="80"/>
-      <c r="H2" s="80"/>
-      <c r="I2" s="80"/>
-      <c r="J2" s="80"/>
+      <c r="B2" s="84"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84"/>
+      <c r="H2" s="84"/>
+      <c r="I2" s="84"/>
+      <c r="J2" s="84"/>
     </row>
     <row r="3" spans="2:10" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="81" t="s">
+      <c r="B3" s="85" t="s">
         <v>155</v>
       </c>
-      <c r="C3" s="81"/>
-      <c r="D3" s="81"/>
-      <c r="E3" s="81"/>
-      <c r="F3" s="81"/>
-      <c r="G3" s="81"/>
-      <c r="H3" s="81"/>
-      <c r="I3" s="81"/>
-      <c r="J3" s="81"/>
+      <c r="C3" s="85"/>
+      <c r="D3" s="85"/>
+      <c r="E3" s="85"/>
+      <c r="F3" s="85"/>
+      <c r="G3" s="85"/>
+      <c r="H3" s="85"/>
+      <c r="I3" s="85"/>
+      <c r="J3" s="85"/>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" s="74" t="s">
@@ -4063,6 +4112,129 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:N6"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.85546875" customWidth="1"/>
+    <col min="2" max="3" width="20.7109375" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" customWidth="1"/>
+    <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.7109375" customWidth="1"/>
+    <col min="8" max="8" width="21.140625" customWidth="1"/>
+    <col min="9" max="9" width="16.140625" customWidth="1"/>
+    <col min="10" max="10" width="25.85546875" customWidth="1"/>
+    <col min="11" max="11" width="15.7109375" customWidth="1"/>
+    <col min="12" max="12" width="19.140625" customWidth="1"/>
+    <col min="13" max="13" width="25.42578125" customWidth="1"/>
+    <col min="14" max="14" width="21.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:14" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B1" s="46" t="s">
+        <v>95</v>
+      </c>
+      <c r="C1" s="46" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84"/>
+      <c r="H2" s="84"/>
+      <c r="I2" s="84"/>
+      <c r="J2" s="84"/>
+      <c r="K2" s="84"/>
+    </row>
+    <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C3" s="85" t="s">
+        <v>156</v>
+      </c>
+      <c r="D3" s="85"/>
+      <c r="E3" s="85"/>
+      <c r="F3" s="85"/>
+      <c r="G3" s="85"/>
+      <c r="H3" s="85"/>
+      <c r="I3" s="85"/>
+      <c r="J3" s="85"/>
+      <c r="K3" s="85"/>
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B5" s="81" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="80" t="s">
+        <v>157</v>
+      </c>
+      <c r="D5" s="80" t="s">
+        <v>143</v>
+      </c>
+      <c r="E5" s="80" t="s">
+        <v>158</v>
+      </c>
+      <c r="F5" s="80" t="s">
+        <v>159</v>
+      </c>
+      <c r="G5" s="80" t="s">
+        <v>160</v>
+      </c>
+      <c r="H5" s="80" t="s">
+        <v>161</v>
+      </c>
+      <c r="I5" s="80" t="s">
+        <v>162</v>
+      </c>
+      <c r="J5" s="80" t="s">
+        <v>163</v>
+      </c>
+      <c r="K5" s="80" t="s">
+        <v>164</v>
+      </c>
+      <c r="L5" s="80" t="s">
+        <v>165</v>
+      </c>
+      <c r="M5" s="80" t="s">
+        <v>166</v>
+      </c>
+      <c r="N5" s="80" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="79"/>
+      <c r="J6" s="82"/>
+      <c r="K6" s="79"/>
+      <c r="L6" s="79"/>
+      <c r="M6" s="79"/>
+      <c r="N6" s="83"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C2:K2"/>
+    <mergeCell ref="C3:K3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:Z8"/>
   <sheetViews>
@@ -4086,37 +4258,37 @@
       <c r="Z1" s="38"/>
     </row>
     <row r="2" spans="2:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="80"/>
-      <c r="C2" s="80"/>
-      <c r="D2" s="80"/>
-      <c r="E2" s="80"/>
-      <c r="F2" s="80"/>
-      <c r="G2" s="80"/>
-      <c r="H2" s="80"/>
-      <c r="I2" s="80"/>
-      <c r="J2" s="80"/>
-      <c r="K2" s="80"/>
-      <c r="L2" s="80"/>
-      <c r="M2" s="80"/>
-      <c r="N2" s="80"/>
+      <c r="B2" s="84"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84"/>
+      <c r="H2" s="84"/>
+      <c r="I2" s="84"/>
+      <c r="J2" s="84"/>
+      <c r="K2" s="84"/>
+      <c r="L2" s="84"/>
+      <c r="M2" s="84"/>
+      <c r="N2" s="84"/>
       <c r="Z2"/>
     </row>
     <row r="3" spans="2:26" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="81" t="s">
+      <c r="B3" s="85" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="81"/>
-      <c r="D3" s="81"/>
-      <c r="E3" s="81"/>
-      <c r="F3" s="81"/>
-      <c r="G3" s="81"/>
-      <c r="H3" s="81"/>
-      <c r="I3" s="81"/>
-      <c r="J3" s="81"/>
-      <c r="K3" s="81"/>
-      <c r="L3" s="81"/>
-      <c r="M3" s="81"/>
-      <c r="N3" s="81"/>
+      <c r="C3" s="85"/>
+      <c r="D3" s="85"/>
+      <c r="E3" s="85"/>
+      <c r="F3" s="85"/>
+      <c r="G3" s="85"/>
+      <c r="H3" s="85"/>
+      <c r="I3" s="85"/>
+      <c r="J3" s="85"/>
+      <c r="K3" s="85"/>
+      <c r="L3" s="85"/>
+      <c r="M3" s="85"/>
+      <c r="N3" s="85"/>
       <c r="Z3"/>
     </row>
     <row r="5" spans="2:26" x14ac:dyDescent="0.25">
@@ -4196,7 +4368,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:Z8"/>
   <sheetViews>
@@ -4220,37 +4392,37 @@
       <c r="Z1" s="38"/>
     </row>
     <row r="2" spans="2:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="80"/>
-      <c r="C2" s="80"/>
-      <c r="D2" s="80"/>
-      <c r="E2" s="80"/>
-      <c r="F2" s="80"/>
-      <c r="G2" s="80"/>
-      <c r="H2" s="80"/>
-      <c r="I2" s="80"/>
-      <c r="J2" s="80"/>
-      <c r="K2" s="80"/>
-      <c r="L2" s="80"/>
-      <c r="M2" s="80"/>
-      <c r="N2" s="80"/>
+      <c r="B2" s="84"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84"/>
+      <c r="H2" s="84"/>
+      <c r="I2" s="84"/>
+      <c r="J2" s="84"/>
+      <c r="K2" s="84"/>
+      <c r="L2" s="84"/>
+      <c r="M2" s="84"/>
+      <c r="N2" s="84"/>
       <c r="Z2"/>
     </row>
     <row r="3" spans="2:26" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="81" t="s">
+      <c r="B3" s="85" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="81"/>
-      <c r="D3" s="81"/>
-      <c r="E3" s="81"/>
-      <c r="F3" s="81"/>
-      <c r="G3" s="81"/>
-      <c r="H3" s="81"/>
-      <c r="I3" s="81"/>
-      <c r="J3" s="81"/>
-      <c r="K3" s="81"/>
-      <c r="L3" s="81"/>
-      <c r="M3" s="81"/>
-      <c r="N3" s="81"/>
+      <c r="C3" s="85"/>
+      <c r="D3" s="85"/>
+      <c r="E3" s="85"/>
+      <c r="F3" s="85"/>
+      <c r="G3" s="85"/>
+      <c r="H3" s="85"/>
+      <c r="I3" s="85"/>
+      <c r="J3" s="85"/>
+      <c r="K3" s="85"/>
+      <c r="L3" s="85"/>
+      <c r="M3" s="85"/>
+      <c r="N3" s="85"/>
       <c r="Z3"/>
     </row>
     <row r="5" spans="2:26" x14ac:dyDescent="0.25">
@@ -4269,9 +4441,9 @@
       <c r="C6" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="D6" s="83"/>
-      <c r="E6" s="84"/>
-      <c r="F6" s="85"/>
+      <c r="D6" s="87"/>
+      <c r="E6" s="88"/>
+      <c r="F6" s="89"/>
       <c r="G6" s="50"/>
       <c r="H6" s="50"/>
     </row>
@@ -4325,7 +4497,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:Z8"/>
   <sheetViews>
@@ -4349,37 +4521,37 @@
       <c r="Z1" s="38"/>
     </row>
     <row r="2" spans="2:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="80"/>
-      <c r="C2" s="80"/>
-      <c r="D2" s="80"/>
-      <c r="E2" s="80"/>
-      <c r="F2" s="80"/>
-      <c r="G2" s="80"/>
-      <c r="H2" s="80"/>
-      <c r="I2" s="80"/>
-      <c r="J2" s="80"/>
-      <c r="K2" s="80"/>
-      <c r="L2" s="80"/>
-      <c r="M2" s="80"/>
-      <c r="N2" s="80"/>
+      <c r="B2" s="84"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84"/>
+      <c r="H2" s="84"/>
+      <c r="I2" s="84"/>
+      <c r="J2" s="84"/>
+      <c r="K2" s="84"/>
+      <c r="L2" s="84"/>
+      <c r="M2" s="84"/>
+      <c r="N2" s="84"/>
       <c r="Z2"/>
     </row>
     <row r="3" spans="2:26" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="81" t="s">
+      <c r="B3" s="85" t="s">
         <v>93</v>
       </c>
-      <c r="C3" s="81"/>
-      <c r="D3" s="81"/>
-      <c r="E3" s="81"/>
-      <c r="F3" s="81"/>
-      <c r="G3" s="81"/>
-      <c r="H3" s="81"/>
-      <c r="I3" s="81"/>
-      <c r="J3" s="81"/>
-      <c r="K3" s="81"/>
-      <c r="L3" s="81"/>
-      <c r="M3" s="81"/>
-      <c r="N3" s="81"/>
+      <c r="C3" s="85"/>
+      <c r="D3" s="85"/>
+      <c r="E3" s="85"/>
+      <c r="F3" s="85"/>
+      <c r="G3" s="85"/>
+      <c r="H3" s="85"/>
+      <c r="I3" s="85"/>
+      <c r="J3" s="85"/>
+      <c r="K3" s="85"/>
+      <c r="L3" s="85"/>
+      <c r="M3" s="85"/>
+      <c r="N3" s="85"/>
       <c r="Z3"/>
     </row>
     <row r="5" spans="2:26" x14ac:dyDescent="0.25">
@@ -4450,7 +4622,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:Z8"/>
   <sheetViews>
@@ -4472,37 +4644,37 @@
       <c r="Z1" s="38"/>
     </row>
     <row r="2" spans="2:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="80"/>
-      <c r="C2" s="80"/>
-      <c r="D2" s="80"/>
-      <c r="E2" s="80"/>
-      <c r="F2" s="80"/>
-      <c r="G2" s="80"/>
-      <c r="H2" s="80"/>
-      <c r="I2" s="80"/>
-      <c r="J2" s="80"/>
-      <c r="K2" s="80"/>
-      <c r="L2" s="80"/>
-      <c r="M2" s="80"/>
-      <c r="N2" s="80"/>
+      <c r="B2" s="84"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84"/>
+      <c r="H2" s="84"/>
+      <c r="I2" s="84"/>
+      <c r="J2" s="84"/>
+      <c r="K2" s="84"/>
+      <c r="L2" s="84"/>
+      <c r="M2" s="84"/>
+      <c r="N2" s="84"/>
       <c r="Z2"/>
     </row>
     <row r="3" spans="2:26" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="81" t="s">
+      <c r="B3" s="85" t="s">
         <v>72</v>
       </c>
-      <c r="C3" s="81"/>
-      <c r="D3" s="81"/>
-      <c r="E3" s="81"/>
-      <c r="F3" s="81"/>
-      <c r="G3" s="81"/>
-      <c r="H3" s="81"/>
-      <c r="I3" s="81"/>
-      <c r="J3" s="81"/>
-      <c r="K3" s="81"/>
-      <c r="L3" s="81"/>
-      <c r="M3" s="81"/>
-      <c r="N3" s="81"/>
+      <c r="C3" s="85"/>
+      <c r="D3" s="85"/>
+      <c r="E3" s="85"/>
+      <c r="F3" s="85"/>
+      <c r="G3" s="85"/>
+      <c r="H3" s="85"/>
+      <c r="I3" s="85"/>
+      <c r="J3" s="85"/>
+      <c r="K3" s="85"/>
+      <c r="L3" s="85"/>
+      <c r="M3" s="85"/>
+      <c r="N3" s="85"/>
       <c r="Z3"/>
     </row>
     <row r="5" spans="2:26" x14ac:dyDescent="0.25">
@@ -4580,7 +4752,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:Q7"/>
   <sheetViews>
@@ -4615,56 +4787,56 @@
       </c>
     </row>
     <row r="2" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="80"/>
-      <c r="C2" s="80"/>
-      <c r="D2" s="80"/>
-      <c r="E2" s="80"/>
-      <c r="F2" s="80"/>
-      <c r="G2" s="80"/>
-      <c r="H2" s="80"/>
-      <c r="I2" s="80"/>
-      <c r="J2" s="80"/>
-      <c r="K2" s="80"/>
-      <c r="L2" s="80"/>
+      <c r="B2" s="84"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84"/>
+      <c r="H2" s="84"/>
+      <c r="I2" s="84"/>
+      <c r="J2" s="84"/>
+      <c r="K2" s="84"/>
+      <c r="L2" s="84"/>
     </row>
     <row r="3" spans="2:17" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="81" t="s">
+      <c r="B3" s="85" t="s">
         <v>108</v>
       </c>
-      <c r="C3" s="81"/>
-      <c r="D3" s="81"/>
-      <c r="E3" s="81"/>
-      <c r="F3" s="81"/>
-      <c r="G3" s="81"/>
-      <c r="H3" s="81"/>
-      <c r="I3" s="81"/>
-      <c r="J3" s="81"/>
-      <c r="K3" s="81"/>
-      <c r="L3" s="81"/>
+      <c r="C3" s="85"/>
+      <c r="D3" s="85"/>
+      <c r="E3" s="85"/>
+      <c r="F3" s="85"/>
+      <c r="G3" s="85"/>
+      <c r="H3" s="85"/>
+      <c r="I3" s="85"/>
+      <c r="J3" s="85"/>
+      <c r="K3" s="85"/>
+      <c r="L3" s="85"/>
     </row>
     <row r="5" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D5" s="86" t="s">
+      <c r="D5" s="90" t="s">
         <v>123</v>
       </c>
-      <c r="E5" s="86"/>
+      <c r="E5" s="90"/>
       <c r="F5" s="73"/>
       <c r="G5" s="73"/>
       <c r="H5" s="73"/>
       <c r="I5" s="73"/>
-      <c r="J5" s="86" t="s">
+      <c r="J5" s="90" t="s">
         <v>42</v>
       </c>
-      <c r="K5" s="86"/>
-      <c r="L5" s="86"/>
-      <c r="M5" s="86" t="s">
+      <c r="K5" s="90"/>
+      <c r="L5" s="90"/>
+      <c r="M5" s="90" t="s">
         <v>130</v>
       </c>
-      <c r="N5" s="86"/>
-      <c r="O5" s="86"/>
-      <c r="P5" s="82" t="s">
+      <c r="N5" s="90"/>
+      <c r="O5" s="90"/>
+      <c r="P5" s="86" t="s">
         <v>109</v>
       </c>
-      <c r="Q5" s="82"/>
+      <c r="Q5" s="86"/>
     </row>
     <row r="6" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="70" t="s">
@@ -4747,7 +4919,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:X8"/>
   <sheetViews>
@@ -4785,108 +4957,108 @@
       </c>
     </row>
     <row r="2" spans="2:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="80"/>
-      <c r="C2" s="80"/>
-      <c r="D2" s="80"/>
-      <c r="E2" s="80"/>
-      <c r="F2" s="80"/>
-      <c r="G2" s="80"/>
-      <c r="H2" s="80"/>
-      <c r="I2" s="80"/>
-      <c r="J2" s="80"/>
-      <c r="K2" s="80"/>
-      <c r="L2" s="80"/>
-      <c r="M2" s="80"/>
-      <c r="N2" s="80"/>
-      <c r="O2" s="80"/>
-      <c r="P2" s="80"/>
+      <c r="B2" s="84"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84"/>
+      <c r="H2" s="84"/>
+      <c r="I2" s="84"/>
+      <c r="J2" s="84"/>
+      <c r="K2" s="84"/>
+      <c r="L2" s="84"/>
+      <c r="M2" s="84"/>
+      <c r="N2" s="84"/>
+      <c r="O2" s="84"/>
+      <c r="P2" s="84"/>
       <c r="Q2" s="56"/>
       <c r="R2" s="56"/>
     </row>
     <row r="3" spans="2:24" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="81" t="s">
+      <c r="B3" s="85" t="s">
         <v>111</v>
       </c>
-      <c r="C3" s="81"/>
-      <c r="D3" s="81"/>
-      <c r="E3" s="81"/>
-      <c r="F3" s="81"/>
-      <c r="G3" s="81"/>
-      <c r="H3" s="81"/>
-      <c r="I3" s="81"/>
-      <c r="J3" s="81"/>
-      <c r="K3" s="81"/>
-      <c r="L3" s="81"/>
-      <c r="M3" s="81"/>
-      <c r="N3" s="81"/>
-      <c r="O3" s="81"/>
-      <c r="P3" s="81"/>
+      <c r="C3" s="85"/>
+      <c r="D3" s="85"/>
+      <c r="E3" s="85"/>
+      <c r="F3" s="85"/>
+      <c r="G3" s="85"/>
+      <c r="H3" s="85"/>
+      <c r="I3" s="85"/>
+      <c r="J3" s="85"/>
+      <c r="K3" s="85"/>
+      <c r="L3" s="85"/>
+      <c r="M3" s="85"/>
+      <c r="N3" s="85"/>
+      <c r="O3" s="85"/>
+      <c r="P3" s="85"/>
       <c r="Q3" s="57"/>
       <c r="R3" s="57"/>
     </row>
     <row r="5" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B5" s="87" t="s">
+      <c r="B5" s="92" t="s">
         <v>112</v>
       </c>
-      <c r="C5" s="88"/>
-      <c r="D5" s="88"/>
-      <c r="E5" s="88"/>
-      <c r="F5" s="88"/>
-      <c r="G5" s="88"/>
-      <c r="H5" s="88"/>
-      <c r="I5" s="88"/>
-      <c r="J5" s="88"/>
-      <c r="K5" s="88"/>
-      <c r="L5" s="89"/>
-      <c r="M5" s="87" t="s">
+      <c r="C5" s="93"/>
+      <c r="D5" s="93"/>
+      <c r="E5" s="93"/>
+      <c r="F5" s="93"/>
+      <c r="G5" s="93"/>
+      <c r="H5" s="93"/>
+      <c r="I5" s="93"/>
+      <c r="J5" s="93"/>
+      <c r="K5" s="93"/>
+      <c r="L5" s="94"/>
+      <c r="M5" s="92" t="s">
         <v>113</v>
       </c>
-      <c r="N5" s="88"/>
-      <c r="O5" s="88"/>
-      <c r="P5" s="88"/>
-      <c r="Q5" s="88"/>
-      <c r="R5" s="88"/>
-      <c r="S5" s="88"/>
-      <c r="T5" s="88"/>
-      <c r="U5" s="88"/>
-      <c r="V5" s="88"/>
-      <c r="W5" s="88"/>
-      <c r="X5" s="89"/>
+      <c r="N5" s="93"/>
+      <c r="O5" s="93"/>
+      <c r="P5" s="93"/>
+      <c r="Q5" s="93"/>
+      <c r="R5" s="93"/>
+      <c r="S5" s="93"/>
+      <c r="T5" s="93"/>
+      <c r="U5" s="93"/>
+      <c r="V5" s="93"/>
+      <c r="W5" s="93"/>
+      <c r="X5" s="94"/>
     </row>
     <row r="6" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B6" s="90"/>
-      <c r="C6" s="90"/>
-      <c r="D6" s="90"/>
-      <c r="E6" s="90"/>
-      <c r="F6" s="91" t="s">
+      <c r="B6" s="91"/>
+      <c r="C6" s="91"/>
+      <c r="D6" s="91"/>
+      <c r="E6" s="91"/>
+      <c r="F6" s="95" t="s">
         <v>27</v>
       </c>
-      <c r="G6" s="92"/>
-      <c r="H6" s="92"/>
-      <c r="I6" s="93"/>
-      <c r="J6" s="87" t="s">
+      <c r="G6" s="96"/>
+      <c r="H6" s="96"/>
+      <c r="I6" s="97"/>
+      <c r="J6" s="92" t="s">
         <v>30</v>
       </c>
-      <c r="K6" s="88"/>
-      <c r="L6" s="89"/>
+      <c r="K6" s="93"/>
+      <c r="L6" s="94"/>
       <c r="M6" s="76"/>
-      <c r="N6" s="87" t="s">
+      <c r="N6" s="92" t="s">
         <v>42</v>
       </c>
-      <c r="O6" s="89"/>
-      <c r="P6" s="87" t="s">
+      <c r="O6" s="94"/>
+      <c r="P6" s="92" t="s">
         <v>106</v>
       </c>
-      <c r="Q6" s="88"/>
-      <c r="R6" s="89"/>
+      <c r="Q6" s="93"/>
+      <c r="R6" s="94"/>
       <c r="S6" s="76"/>
-      <c r="T6" s="87" t="s">
+      <c r="T6" s="92" t="s">
         <v>123</v>
       </c>
-      <c r="U6" s="89"/>
-      <c r="V6" s="90"/>
-      <c r="W6" s="90"/>
-      <c r="X6" s="90"/>
+      <c r="U6" s="94"/>
+      <c r="V6" s="91"/>
+      <c r="W6" s="91"/>
+      <c r="X6" s="91"/>
     </row>
     <row r="7" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B7" s="75" t="s">
@@ -4986,10 +5158,6 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="N6:O6"/>
-    <mergeCell ref="P6:R6"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="M5:X5"/>
     <mergeCell ref="T6:U6"/>
     <mergeCell ref="V6:X6"/>
     <mergeCell ref="B2:P2"/>
@@ -4997,12 +5165,16 @@
     <mergeCell ref="B5:L5"/>
     <mergeCell ref="J6:L6"/>
     <mergeCell ref="F6:I6"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="P6:R6"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="M5:X5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A24"/>
   <sheetViews>
@@ -5117,36 +5289,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="80"/>
-      <c r="C2" s="80"/>
-      <c r="D2" s="80"/>
-      <c r="E2" s="80"/>
-      <c r="F2" s="80"/>
-      <c r="G2" s="80"/>
-      <c r="H2" s="80"/>
-      <c r="I2" s="80"/>
-      <c r="J2" s="80"/>
-      <c r="K2" s="80"/>
-      <c r="L2" s="80"/>
-      <c r="M2" s="80"/>
-      <c r="N2" s="80"/>
+      <c r="B2" s="84"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84"/>
+      <c r="H2" s="84"/>
+      <c r="I2" s="84"/>
+      <c r="J2" s="84"/>
+      <c r="K2" s="84"/>
+      <c r="L2" s="84"/>
+      <c r="M2" s="84"/>
+      <c r="N2" s="84"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="81" t="s">
+      <c r="B3" s="85" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="81"/>
-      <c r="D3" s="81"/>
-      <c r="E3" s="81"/>
-      <c r="F3" s="81"/>
-      <c r="G3" s="81"/>
-      <c r="H3" s="81"/>
-      <c r="I3" s="81"/>
-      <c r="J3" s="81"/>
-      <c r="K3" s="81"/>
-      <c r="L3" s="81"/>
-      <c r="M3" s="81"/>
-      <c r="N3" s="81"/>
+      <c r="C3" s="85"/>
+      <c r="D3" s="85"/>
+      <c r="E3" s="85"/>
+      <c r="F3" s="85"/>
+      <c r="G3" s="85"/>
+      <c r="H3" s="85"/>
+      <c r="I3" s="85"/>
+      <c r="J3" s="85"/>
+      <c r="K3" s="85"/>
+      <c r="L3" s="85"/>
+      <c r="M3" s="85"/>
+      <c r="N3" s="85"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="44" t="s">
@@ -5213,40 +5385,40 @@
       </c>
     </row>
     <row r="2" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="80"/>
-      <c r="C2" s="80"/>
-      <c r="D2" s="80"/>
-      <c r="E2" s="80"/>
-      <c r="F2" s="80"/>
-      <c r="G2" s="80"/>
-      <c r="H2" s="80"/>
-      <c r="I2" s="80"/>
-      <c r="J2" s="80"/>
-      <c r="K2" s="80"/>
-      <c r="L2" s="80"/>
-      <c r="M2" s="80"/>
-      <c r="N2" s="80"/>
-      <c r="O2" s="80"/>
-      <c r="P2" s="80"/>
+      <c r="B2" s="84"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84"/>
+      <c r="H2" s="84"/>
+      <c r="I2" s="84"/>
+      <c r="J2" s="84"/>
+      <c r="K2" s="84"/>
+      <c r="L2" s="84"/>
+      <c r="M2" s="84"/>
+      <c r="N2" s="84"/>
+      <c r="O2" s="84"/>
+      <c r="P2" s="84"/>
     </row>
     <row r="3" spans="2:16" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="81" t="s">
+      <c r="B3" s="85" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="81"/>
-      <c r="D3" s="81"/>
-      <c r="E3" s="81"/>
-      <c r="F3" s="81"/>
-      <c r="G3" s="81"/>
-      <c r="H3" s="81"/>
-      <c r="I3" s="81"/>
-      <c r="J3" s="81"/>
-      <c r="K3" s="81"/>
-      <c r="L3" s="81"/>
-      <c r="M3" s="81"/>
-      <c r="N3" s="81"/>
-      <c r="O3" s="81"/>
-      <c r="P3" s="81"/>
+      <c r="C3" s="85"/>
+      <c r="D3" s="85"/>
+      <c r="E3" s="85"/>
+      <c r="F3" s="85"/>
+      <c r="G3" s="85"/>
+      <c r="H3" s="85"/>
+      <c r="I3" s="85"/>
+      <c r="J3" s="85"/>
+      <c r="K3" s="85"/>
+      <c r="L3" s="85"/>
+      <c r="M3" s="85"/>
+      <c r="N3" s="85"/>
+      <c r="O3" s="85"/>
+      <c r="P3" s="85"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="44" t="s">
@@ -5325,40 +5497,40 @@
       </c>
     </row>
     <row r="2" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="80"/>
-      <c r="C2" s="80"/>
-      <c r="D2" s="80"/>
-      <c r="E2" s="80"/>
-      <c r="F2" s="80"/>
-      <c r="G2" s="80"/>
-      <c r="H2" s="80"/>
-      <c r="I2" s="80"/>
-      <c r="J2" s="80"/>
-      <c r="K2" s="80"/>
-      <c r="L2" s="80"/>
-      <c r="M2" s="80"/>
-      <c r="N2" s="80"/>
-      <c r="O2" s="80"/>
-      <c r="P2" s="80"/>
+      <c r="B2" s="84"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84"/>
+      <c r="H2" s="84"/>
+      <c r="I2" s="84"/>
+      <c r="J2" s="84"/>
+      <c r="K2" s="84"/>
+      <c r="L2" s="84"/>
+      <c r="M2" s="84"/>
+      <c r="N2" s="84"/>
+      <c r="O2" s="84"/>
+      <c r="P2" s="84"/>
     </row>
     <row r="3" spans="2:16" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="81" t="s">
+      <c r="B3" s="85" t="s">
         <v>68</v>
       </c>
-      <c r="C3" s="81"/>
-      <c r="D3" s="81"/>
-      <c r="E3" s="81"/>
-      <c r="F3" s="81"/>
-      <c r="G3" s="81"/>
-      <c r="H3" s="81"/>
-      <c r="I3" s="81"/>
-      <c r="J3" s="81"/>
-      <c r="K3" s="81"/>
-      <c r="L3" s="81"/>
-      <c r="M3" s="81"/>
-      <c r="N3" s="81"/>
-      <c r="O3" s="81"/>
-      <c r="P3" s="81"/>
+      <c r="C3" s="85"/>
+      <c r="D3" s="85"/>
+      <c r="E3" s="85"/>
+      <c r="F3" s="85"/>
+      <c r="G3" s="85"/>
+      <c r="H3" s="85"/>
+      <c r="I3" s="85"/>
+      <c r="J3" s="85"/>
+      <c r="K3" s="85"/>
+      <c r="L3" s="85"/>
+      <c r="M3" s="85"/>
+      <c r="N3" s="85"/>
+      <c r="O3" s="85"/>
+      <c r="P3" s="85"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
@@ -5407,40 +5579,40 @@
       </c>
     </row>
     <row r="2" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="80"/>
-      <c r="C2" s="80"/>
-      <c r="D2" s="80"/>
-      <c r="E2" s="80"/>
-      <c r="F2" s="80"/>
-      <c r="G2" s="80"/>
-      <c r="H2" s="80"/>
-      <c r="I2" s="80"/>
-      <c r="J2" s="80"/>
-      <c r="K2" s="80"/>
-      <c r="L2" s="80"/>
-      <c r="M2" s="80"/>
-      <c r="N2" s="80"/>
-      <c r="O2" s="80"/>
-      <c r="P2" s="80"/>
+      <c r="B2" s="84"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84"/>
+      <c r="H2" s="84"/>
+      <c r="I2" s="84"/>
+      <c r="J2" s="84"/>
+      <c r="K2" s="84"/>
+      <c r="L2" s="84"/>
+      <c r="M2" s="84"/>
+      <c r="N2" s="84"/>
+      <c r="O2" s="84"/>
+      <c r="P2" s="84"/>
     </row>
     <row r="3" spans="2:16" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="81" t="s">
+      <c r="B3" s="85" t="s">
         <v>71</v>
       </c>
-      <c r="C3" s="81"/>
-      <c r="D3" s="81"/>
-      <c r="E3" s="81"/>
-      <c r="F3" s="81"/>
-      <c r="G3" s="81"/>
-      <c r="H3" s="81"/>
-      <c r="I3" s="81"/>
-      <c r="J3" s="81"/>
-      <c r="K3" s="81"/>
-      <c r="L3" s="81"/>
-      <c r="M3" s="81"/>
-      <c r="N3" s="81"/>
-      <c r="O3" s="81"/>
-      <c r="P3" s="81"/>
+      <c r="C3" s="85"/>
+      <c r="D3" s="85"/>
+      <c r="E3" s="85"/>
+      <c r="F3" s="85"/>
+      <c r="G3" s="85"/>
+      <c r="H3" s="85"/>
+      <c r="I3" s="85"/>
+      <c r="J3" s="85"/>
+      <c r="K3" s="85"/>
+      <c r="L3" s="85"/>
+      <c r="M3" s="85"/>
+      <c r="N3" s="85"/>
+      <c r="O3" s="85"/>
+      <c r="P3" s="85"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
@@ -5494,36 +5666,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="80"/>
-      <c r="C2" s="80"/>
-      <c r="D2" s="80"/>
-      <c r="E2" s="80"/>
-      <c r="F2" s="80"/>
-      <c r="G2" s="80"/>
-      <c r="H2" s="80"/>
-      <c r="I2" s="80"/>
-      <c r="J2" s="80"/>
-      <c r="K2" s="80"/>
-      <c r="L2" s="80"/>
-      <c r="M2" s="80"/>
-      <c r="N2" s="80"/>
+      <c r="B2" s="84"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84"/>
+      <c r="H2" s="84"/>
+      <c r="I2" s="84"/>
+      <c r="J2" s="84"/>
+      <c r="K2" s="84"/>
+      <c r="L2" s="84"/>
+      <c r="M2" s="84"/>
+      <c r="N2" s="84"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="81" t="s">
+      <c r="B3" s="85" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="81"/>
-      <c r="D3" s="81"/>
-      <c r="E3" s="81"/>
-      <c r="F3" s="81"/>
-      <c r="G3" s="81"/>
-      <c r="H3" s="81"/>
-      <c r="I3" s="81"/>
-      <c r="J3" s="81"/>
-      <c r="K3" s="81"/>
-      <c r="L3" s="81"/>
-      <c r="M3" s="81"/>
-      <c r="N3" s="81"/>
+      <c r="C3" s="85"/>
+      <c r="D3" s="85"/>
+      <c r="E3" s="85"/>
+      <c r="F3" s="85"/>
+      <c r="G3" s="85"/>
+      <c r="H3" s="85"/>
+      <c r="I3" s="85"/>
+      <c r="J3" s="85"/>
+      <c r="K3" s="85"/>
+      <c r="L3" s="85"/>
+      <c r="M3" s="85"/>
+      <c r="N3" s="85"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="44" t="s">
@@ -5612,40 +5784,40 @@
       </c>
     </row>
     <row r="2" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="80"/>
-      <c r="C2" s="80"/>
-      <c r="D2" s="80"/>
-      <c r="E2" s="80"/>
-      <c r="F2" s="80"/>
-      <c r="G2" s="80"/>
-      <c r="H2" s="80"/>
-      <c r="I2" s="80"/>
-      <c r="J2" s="80"/>
-      <c r="K2" s="80"/>
-      <c r="L2" s="80"/>
-      <c r="M2" s="80"/>
-      <c r="N2" s="80"/>
-      <c r="O2" s="80"/>
-      <c r="P2" s="80"/>
+      <c r="B2" s="84"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84"/>
+      <c r="H2" s="84"/>
+      <c r="I2" s="84"/>
+      <c r="J2" s="84"/>
+      <c r="K2" s="84"/>
+      <c r="L2" s="84"/>
+      <c r="M2" s="84"/>
+      <c r="N2" s="84"/>
+      <c r="O2" s="84"/>
+      <c r="P2" s="84"/>
     </row>
     <row r="3" spans="2:16" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="81" t="s">
+      <c r="B3" s="85" t="s">
         <v>65</v>
       </c>
-      <c r="C3" s="81"/>
-      <c r="D3" s="81"/>
-      <c r="E3" s="81"/>
-      <c r="F3" s="81"/>
-      <c r="G3" s="81"/>
-      <c r="H3" s="81"/>
-      <c r="I3" s="81"/>
-      <c r="J3" s="81"/>
-      <c r="K3" s="81"/>
-      <c r="L3" s="81"/>
-      <c r="M3" s="81"/>
-      <c r="N3" s="81"/>
-      <c r="O3" s="81"/>
-      <c r="P3" s="81"/>
+      <c r="C3" s="85"/>
+      <c r="D3" s="85"/>
+      <c r="E3" s="85"/>
+      <c r="F3" s="85"/>
+      <c r="G3" s="85"/>
+      <c r="H3" s="85"/>
+      <c r="I3" s="85"/>
+      <c r="J3" s="85"/>
+      <c r="K3" s="85"/>
+      <c r="L3" s="85"/>
+      <c r="M3" s="85"/>
+      <c r="N3" s="85"/>
+      <c r="O3" s="85"/>
+      <c r="P3" s="85"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="45" t="s">
@@ -5697,36 +5869,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="80"/>
-      <c r="C2" s="80"/>
-      <c r="D2" s="80"/>
-      <c r="E2" s="80"/>
-      <c r="F2" s="80"/>
-      <c r="G2" s="80"/>
-      <c r="H2" s="80"/>
-      <c r="I2" s="80"/>
-      <c r="J2" s="80"/>
-      <c r="K2" s="80"/>
-      <c r="L2" s="80"/>
-      <c r="M2" s="80"/>
-      <c r="N2" s="80"/>
+      <c r="B2" s="84"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84"/>
+      <c r="H2" s="84"/>
+      <c r="I2" s="84"/>
+      <c r="J2" s="84"/>
+      <c r="K2" s="84"/>
+      <c r="L2" s="84"/>
+      <c r="M2" s="84"/>
+      <c r="N2" s="84"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="81" t="s">
+      <c r="B3" s="85" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="81"/>
-      <c r="D3" s="81"/>
-      <c r="E3" s="81"/>
-      <c r="F3" s="81"/>
-      <c r="G3" s="81"/>
-      <c r="H3" s="81"/>
-      <c r="I3" s="81"/>
-      <c r="J3" s="81"/>
-      <c r="K3" s="81"/>
-      <c r="L3" s="81"/>
-      <c r="M3" s="81"/>
-      <c r="N3" s="81"/>
+      <c r="C3" s="85"/>
+      <c r="D3" s="85"/>
+      <c r="E3" s="85"/>
+      <c r="F3" s="85"/>
+      <c r="G3" s="85"/>
+      <c r="H3" s="85"/>
+      <c r="I3" s="85"/>
+      <c r="J3" s="85"/>
+      <c r="K3" s="85"/>
+      <c r="L3" s="85"/>
+      <c r="M3" s="85"/>
+      <c r="N3" s="85"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">

</xml_diff>

<commit_message>
TRIEDA-1613 - Criando botao de exportar para excel, ao ser selecionado é aberta uma modal com checkboxes para seleção de quais planilhas deseja exportar. Removendo botões de exportar tabelas, grades, e visao aluno.
</commit_message>
<xml_diff>
--- a/code/client/web/src/main/resources/templateExport.xlsx
+++ b/code/client/web/src/main/resources/templateExport.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="17070" windowHeight="5370" tabRatio="622" firstSheet="17" activeTab="21"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="17070" windowHeight="5370" tabRatio="622" firstSheet="18" activeTab="21"/>
   </bookViews>
   <sheets>
     <sheet name="Campi" sheetId="3" r:id="rId1"/>
@@ -1214,7 +1214,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="168">
   <si>
     <t>Planilha de Unidades</t>
   </si>
@@ -2110,7 +2110,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2370,18 +2370,18 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="28" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="28" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2391,6 +2391,8 @@
     <xf numFmtId="0" fontId="8" fillId="28" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3695,7 +3697,7 @@
   <dimension ref="B1:N6"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection sqref="A1:IV65536"/>
+      <selection activeCell="B2" sqref="B2:N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3901,7 +3903,7 @@
   <dimension ref="B1:N6"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B2" sqref="B2:N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4020,7 +4022,7 @@
   <dimension ref="B1:J6"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:J3"/>
+      <selection activeCell="I40" sqref="I40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4116,7 +4118,7 @@
   <dimension ref="B1:N6"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4140,11 +4142,9 @@
       <c r="B1" s="46" t="s">
         <v>95</v>
       </c>
-      <c r="C1" s="46" t="s">
-        <v>95</v>
-      </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="84"/>
       <c r="C2" s="84"/>
       <c r="D2" s="84"/>
       <c r="E2" s="84"/>
@@ -4153,12 +4153,13 @@
       <c r="H2" s="84"/>
       <c r="I2" s="84"/>
       <c r="J2" s="84"/>
-      <c r="K2" s="84"/>
+      <c r="K2" s="99"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C3" s="85" t="s">
+      <c r="B3" s="85" t="s">
         <v>156</v>
       </c>
+      <c r="C3" s="85"/>
       <c r="D3" s="85"/>
       <c r="E3" s="85"/>
       <c r="F3" s="85"/>
@@ -4166,7 +4167,7 @@
       <c r="H3" s="85"/>
       <c r="I3" s="85"/>
       <c r="J3" s="85"/>
-      <c r="K3" s="85"/>
+      <c r="K3" s="98"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="81" t="s">
@@ -4226,8 +4227,8 @@
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="C2:K2"/>
-    <mergeCell ref="C3:K3"/>
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="B3:J3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -4239,7 +4240,7 @@
   <dimension ref="B1:Z8"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="B2" sqref="B2:N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4997,68 +4998,68 @@
       <c r="R3" s="57"/>
     </row>
     <row r="5" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B5" s="92" t="s">
+      <c r="B5" s="91" t="s">
         <v>112</v>
       </c>
-      <c r="C5" s="93"/>
-      <c r="D5" s="93"/>
-      <c r="E5" s="93"/>
-      <c r="F5" s="93"/>
-      <c r="G5" s="93"/>
-      <c r="H5" s="93"/>
-      <c r="I5" s="93"/>
-      <c r="J5" s="93"/>
-      <c r="K5" s="93"/>
-      <c r="L5" s="94"/>
-      <c r="M5" s="92" t="s">
+      <c r="C5" s="94"/>
+      <c r="D5" s="94"/>
+      <c r="E5" s="94"/>
+      <c r="F5" s="94"/>
+      <c r="G5" s="94"/>
+      <c r="H5" s="94"/>
+      <c r="I5" s="94"/>
+      <c r="J5" s="94"/>
+      <c r="K5" s="94"/>
+      <c r="L5" s="92"/>
+      <c r="M5" s="91" t="s">
         <v>113</v>
       </c>
-      <c r="N5" s="93"/>
-      <c r="O5" s="93"/>
-      <c r="P5" s="93"/>
-      <c r="Q5" s="93"/>
-      <c r="R5" s="93"/>
-      <c r="S5" s="93"/>
-      <c r="T5" s="93"/>
-      <c r="U5" s="93"/>
-      <c r="V5" s="93"/>
-      <c r="W5" s="93"/>
-      <c r="X5" s="94"/>
+      <c r="N5" s="94"/>
+      <c r="O5" s="94"/>
+      <c r="P5" s="94"/>
+      <c r="Q5" s="94"/>
+      <c r="R5" s="94"/>
+      <c r="S5" s="94"/>
+      <c r="T5" s="94"/>
+      <c r="U5" s="94"/>
+      <c r="V5" s="94"/>
+      <c r="W5" s="94"/>
+      <c r="X5" s="92"/>
     </row>
     <row r="6" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B6" s="91"/>
-      <c r="C6" s="91"/>
-      <c r="D6" s="91"/>
-      <c r="E6" s="91"/>
+      <c r="B6" s="93"/>
+      <c r="C6" s="93"/>
+      <c r="D6" s="93"/>
+      <c r="E6" s="93"/>
       <c r="F6" s="95" t="s">
         <v>27</v>
       </c>
       <c r="G6" s="96"/>
       <c r="H6" s="96"/>
       <c r="I6" s="97"/>
-      <c r="J6" s="92" t="s">
+      <c r="J6" s="91" t="s">
         <v>30</v>
       </c>
-      <c r="K6" s="93"/>
-      <c r="L6" s="94"/>
+      <c r="K6" s="94"/>
+      <c r="L6" s="92"/>
       <c r="M6" s="76"/>
-      <c r="N6" s="92" t="s">
+      <c r="N6" s="91" t="s">
         <v>42</v>
       </c>
-      <c r="O6" s="94"/>
-      <c r="P6" s="92" t="s">
+      <c r="O6" s="92"/>
+      <c r="P6" s="91" t="s">
         <v>106</v>
       </c>
-      <c r="Q6" s="93"/>
-      <c r="R6" s="94"/>
+      <c r="Q6" s="94"/>
+      <c r="R6" s="92"/>
       <c r="S6" s="76"/>
-      <c r="T6" s="92" t="s">
+      <c r="T6" s="91" t="s">
         <v>123</v>
       </c>
-      <c r="U6" s="94"/>
-      <c r="V6" s="91"/>
-      <c r="W6" s="91"/>
-      <c r="X6" s="91"/>
+      <c r="U6" s="92"/>
+      <c r="V6" s="93"/>
+      <c r="W6" s="93"/>
+      <c r="X6" s="93"/>
     </row>
     <row r="7" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B7" s="75" t="s">
@@ -5158,6 +5159,7 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="M5:X5"/>
     <mergeCell ref="T6:U6"/>
     <mergeCell ref="V6:X6"/>
     <mergeCell ref="B2:P2"/>
@@ -5168,7 +5170,6 @@
     <mergeCell ref="N6:O6"/>
     <mergeCell ref="P6:R6"/>
     <mergeCell ref="B6:E6"/>
-    <mergeCell ref="M5:X5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
TRIEDA-1620 - Alterando api de exportar XLSX (XSSF) para fazer export por streaming (SXSSF).
</commit_message>
<xml_diff>
--- a/code/client/web/src/main/resources/templateExport.xlsx
+++ b/code/client/web/src/main/resources/templateExport.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="17070" windowHeight="5370" tabRatio="622" firstSheet="18" activeTab="21"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="17070" windowHeight="5370" tabRatio="622" firstSheet="19" activeTab="23"/>
   </bookViews>
   <sheets>
     <sheet name="Campi" sheetId="3" r:id="rId1"/>
@@ -1725,9 +1725,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="&quot;R$&quot;\ #,##0.00"/>
+    <numFmt numFmtId="164" formatCode="&quot;R$&quot;\ #,##0.00"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1743,18 +1743,6 @@
     </font>
     <font>
       <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
@@ -1822,6 +1810,15 @@
     </font>
     <font>
       <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
       <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -2108,21 +2105,21 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -2137,16 +2134,16 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2228,171 +2225,174 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="27" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="6" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2720,38 +2720,38 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="84" t="s">
+      <c r="B2" s="86" t="s">
         <v>96</v>
       </c>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="84"/>
-      <c r="J2" s="84"/>
-      <c r="K2" s="84"/>
-      <c r="L2" s="84"/>
-      <c r="M2" s="84"/>
-      <c r="N2" s="84"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="86"/>
+      <c r="G2" s="86"/>
+      <c r="H2" s="86"/>
+      <c r="I2" s="86"/>
+      <c r="J2" s="86"/>
+      <c r="K2" s="86"/>
+      <c r="L2" s="86"/>
+      <c r="M2" s="86"/>
+      <c r="N2" s="86"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="85" t="s">
+      <c r="B3" s="87" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="85"/>
-      <c r="D3" s="85"/>
-      <c r="E3" s="85"/>
-      <c r="F3" s="85"/>
-      <c r="G3" s="85"/>
-      <c r="H3" s="85"/>
-      <c r="I3" s="85"/>
-      <c r="J3" s="85"/>
-      <c r="K3" s="85"/>
-      <c r="L3" s="85"/>
-      <c r="M3" s="85"/>
-      <c r="N3" s="85"/>
+      <c r="C3" s="87"/>
+      <c r="D3" s="87"/>
+      <c r="E3" s="87"/>
+      <c r="F3" s="87"/>
+      <c r="G3" s="87"/>
+      <c r="H3" s="87"/>
+      <c r="I3" s="87"/>
+      <c r="J3" s="87"/>
+      <c r="K3" s="87"/>
+      <c r="L3" s="87"/>
+      <c r="M3" s="87"/>
+      <c r="N3" s="87"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="44" t="s">
@@ -2819,36 +2819,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="84"/>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="84"/>
-      <c r="J2" s="84"/>
-      <c r="K2" s="84"/>
-      <c r="L2" s="84"/>
-      <c r="M2" s="84"/>
-      <c r="N2" s="84"/>
+      <c r="B2" s="86"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="86"/>
+      <c r="G2" s="86"/>
+      <c r="H2" s="86"/>
+      <c r="I2" s="86"/>
+      <c r="J2" s="86"/>
+      <c r="K2" s="86"/>
+      <c r="L2" s="86"/>
+      <c r="M2" s="86"/>
+      <c r="N2" s="86"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="85" t="s">
+      <c r="B3" s="87" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="85"/>
-      <c r="D3" s="85"/>
-      <c r="E3" s="85"/>
-      <c r="F3" s="85"/>
-      <c r="G3" s="85"/>
-      <c r="H3" s="85"/>
-      <c r="I3" s="85"/>
-      <c r="J3" s="85"/>
-      <c r="K3" s="85"/>
-      <c r="L3" s="85"/>
-      <c r="M3" s="85"/>
-      <c r="N3" s="85"/>
+      <c r="C3" s="87"/>
+      <c r="D3" s="87"/>
+      <c r="E3" s="87"/>
+      <c r="F3" s="87"/>
+      <c r="G3" s="87"/>
+      <c r="H3" s="87"/>
+      <c r="I3" s="87"/>
+      <c r="J3" s="87"/>
+      <c r="K3" s="87"/>
+      <c r="L3" s="87"/>
+      <c r="M3" s="87"/>
+      <c r="N3" s="87"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -2917,36 +2917,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="84"/>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="84"/>
-      <c r="J2" s="84"/>
-      <c r="K2" s="84"/>
-      <c r="L2" s="84"/>
-      <c r="M2" s="84"/>
-      <c r="N2" s="84"/>
+      <c r="B2" s="86"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="86"/>
+      <c r="G2" s="86"/>
+      <c r="H2" s="86"/>
+      <c r="I2" s="86"/>
+      <c r="J2" s="86"/>
+      <c r="K2" s="86"/>
+      <c r="L2" s="86"/>
+      <c r="M2" s="86"/>
+      <c r="N2" s="86"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="85" t="s">
+      <c r="B3" s="87" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="85"/>
-      <c r="D3" s="85"/>
-      <c r="E3" s="85"/>
-      <c r="F3" s="85"/>
-      <c r="G3" s="85"/>
-      <c r="H3" s="85"/>
-      <c r="I3" s="85"/>
-      <c r="J3" s="85"/>
-      <c r="K3" s="85"/>
-      <c r="L3" s="85"/>
-      <c r="M3" s="85"/>
-      <c r="N3" s="85"/>
+      <c r="C3" s="87"/>
+      <c r="D3" s="87"/>
+      <c r="E3" s="87"/>
+      <c r="F3" s="87"/>
+      <c r="G3" s="87"/>
+      <c r="H3" s="87"/>
+      <c r="I3" s="87"/>
+      <c r="J3" s="87"/>
+      <c r="K3" s="87"/>
+      <c r="L3" s="87"/>
+      <c r="M3" s="87"/>
+      <c r="N3" s="87"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -3031,18 +3031,18 @@
       </c>
     </row>
     <row r="2" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="84"/>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
+      <c r="B2" s="86"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="86"/>
     </row>
     <row r="3" spans="2:5" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="85" t="s">
+      <c r="B3" s="87" t="s">
         <v>126</v>
       </c>
-      <c r="C3" s="85"/>
-      <c r="D3" s="85"/>
-      <c r="E3" s="85"/>
+      <c r="C3" s="87"/>
+      <c r="D3" s="87"/>
+      <c r="E3" s="87"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="60" t="s">
@@ -3095,36 +3095,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="84"/>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="84"/>
-      <c r="J2" s="84"/>
-      <c r="K2" s="84"/>
-      <c r="L2" s="84"/>
-      <c r="M2" s="84"/>
-      <c r="N2" s="84"/>
+      <c r="B2" s="86"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="86"/>
+      <c r="G2" s="86"/>
+      <c r="H2" s="86"/>
+      <c r="I2" s="86"/>
+      <c r="J2" s="86"/>
+      <c r="K2" s="86"/>
+      <c r="L2" s="86"/>
+      <c r="M2" s="86"/>
+      <c r="N2" s="86"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="85" t="s">
+      <c r="B3" s="87" t="s">
         <v>100</v>
       </c>
-      <c r="C3" s="85"/>
-      <c r="D3" s="85"/>
-      <c r="E3" s="85"/>
-      <c r="F3" s="85"/>
-      <c r="G3" s="85"/>
-      <c r="H3" s="85"/>
-      <c r="I3" s="85"/>
-      <c r="J3" s="85"/>
-      <c r="K3" s="85"/>
-      <c r="L3" s="85"/>
-      <c r="M3" s="85"/>
-      <c r="N3" s="85"/>
+      <c r="C3" s="87"/>
+      <c r="D3" s="87"/>
+      <c r="E3" s="87"/>
+      <c r="F3" s="87"/>
+      <c r="G3" s="87"/>
+      <c r="H3" s="87"/>
+      <c r="I3" s="87"/>
+      <c r="J3" s="87"/>
+      <c r="K3" s="87"/>
+      <c r="L3" s="87"/>
+      <c r="M3" s="87"/>
+      <c r="N3" s="87"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -3157,10 +3157,10 @@
       <c r="K5" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="L5" s="86" t="s">
+      <c r="L5" s="88" t="s">
         <v>110</v>
       </c>
-      <c r="M5" s="86"/>
+      <c r="M5" s="88"/>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
@@ -3212,38 +3212,38 @@
       </c>
     </row>
     <row r="2" spans="2:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="84"/>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="84"/>
-      <c r="J2" s="84"/>
-      <c r="K2" s="84"/>
-      <c r="L2" s="84"/>
-      <c r="M2" s="84"/>
-      <c r="N2" s="84"/>
-      <c r="O2" s="84"/>
+      <c r="B2" s="86"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="86"/>
+      <c r="G2" s="86"/>
+      <c r="H2" s="86"/>
+      <c r="I2" s="86"/>
+      <c r="J2" s="86"/>
+      <c r="K2" s="86"/>
+      <c r="L2" s="86"/>
+      <c r="M2" s="86"/>
+      <c r="N2" s="86"/>
+      <c r="O2" s="86"/>
     </row>
     <row r="3" spans="2:15" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="85" t="s">
+      <c r="B3" s="87" t="s">
         <v>73</v>
       </c>
-      <c r="C3" s="85"/>
-      <c r="D3" s="85"/>
-      <c r="E3" s="85"/>
-      <c r="F3" s="85"/>
-      <c r="G3" s="85"/>
-      <c r="H3" s="85"/>
-      <c r="I3" s="85"/>
-      <c r="J3" s="85"/>
-      <c r="K3" s="85"/>
-      <c r="L3" s="85"/>
-      <c r="M3" s="85"/>
-      <c r="N3" s="85"/>
-      <c r="O3" s="85"/>
+      <c r="C3" s="87"/>
+      <c r="D3" s="87"/>
+      <c r="E3" s="87"/>
+      <c r="F3" s="87"/>
+      <c r="G3" s="87"/>
+      <c r="H3" s="87"/>
+      <c r="I3" s="87"/>
+      <c r="J3" s="87"/>
+      <c r="K3" s="87"/>
+      <c r="L3" s="87"/>
+      <c r="M3" s="87"/>
+      <c r="N3" s="87"/>
+      <c r="O3" s="87"/>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -3322,18 +3322,18 @@
       </c>
     </row>
     <row r="2" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="84"/>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
+      <c r="B2" s="86"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="86"/>
     </row>
     <row r="3" spans="2:5" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="85" t="s">
+      <c r="B3" s="87" t="s">
         <v>131</v>
       </c>
-      <c r="C3" s="85"/>
-      <c r="D3" s="85"/>
-      <c r="E3" s="85"/>
+      <c r="C3" s="87"/>
+      <c r="D3" s="87"/>
+      <c r="E3" s="87"/>
     </row>
     <row r="4" spans="2:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="64"/>
@@ -3395,36 +3395,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="84"/>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="84"/>
-      <c r="J2" s="84"/>
-      <c r="K2" s="84"/>
-      <c r="L2" s="84"/>
-      <c r="M2" s="84"/>
-      <c r="N2" s="84"/>
+      <c r="B2" s="86"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="86"/>
+      <c r="G2" s="86"/>
+      <c r="H2" s="86"/>
+      <c r="I2" s="86"/>
+      <c r="J2" s="86"/>
+      <c r="K2" s="86"/>
+      <c r="L2" s="86"/>
+      <c r="M2" s="86"/>
+      <c r="N2" s="86"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="85" t="s">
+      <c r="B3" s="87" t="s">
         <v>69</v>
       </c>
-      <c r="C3" s="85"/>
-      <c r="D3" s="85"/>
-      <c r="E3" s="85"/>
-      <c r="F3" s="85"/>
-      <c r="G3" s="85"/>
-      <c r="H3" s="85"/>
-      <c r="I3" s="85"/>
-      <c r="J3" s="85"/>
-      <c r="K3" s="85"/>
-      <c r="L3" s="85"/>
-      <c r="M3" s="85"/>
-      <c r="N3" s="85"/>
+      <c r="C3" s="87"/>
+      <c r="D3" s="87"/>
+      <c r="E3" s="87"/>
+      <c r="F3" s="87"/>
+      <c r="G3" s="87"/>
+      <c r="H3" s="87"/>
+      <c r="I3" s="87"/>
+      <c r="J3" s="87"/>
+      <c r="K3" s="87"/>
+      <c r="L3" s="87"/>
+      <c r="M3" s="87"/>
+      <c r="N3" s="87"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -3479,36 +3479,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="84"/>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="84"/>
-      <c r="J2" s="84"/>
-      <c r="K2" s="84"/>
-      <c r="L2" s="84"/>
-      <c r="M2" s="84"/>
-      <c r="N2" s="84"/>
+      <c r="B2" s="86"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="86"/>
+      <c r="G2" s="86"/>
+      <c r="H2" s="86"/>
+      <c r="I2" s="86"/>
+      <c r="J2" s="86"/>
+      <c r="K2" s="86"/>
+      <c r="L2" s="86"/>
+      <c r="M2" s="86"/>
+      <c r="N2" s="86"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="85" t="s">
+      <c r="B3" s="87" t="s">
         <v>74</v>
       </c>
-      <c r="C3" s="85"/>
-      <c r="D3" s="85"/>
-      <c r="E3" s="85"/>
-      <c r="F3" s="85"/>
-      <c r="G3" s="85"/>
-      <c r="H3" s="85"/>
-      <c r="I3" s="85"/>
-      <c r="J3" s="85"/>
-      <c r="K3" s="85"/>
-      <c r="L3" s="85"/>
-      <c r="M3" s="85"/>
-      <c r="N3" s="85"/>
+      <c r="C3" s="87"/>
+      <c r="D3" s="87"/>
+      <c r="E3" s="87"/>
+      <c r="F3" s="87"/>
+      <c r="G3" s="87"/>
+      <c r="H3" s="87"/>
+      <c r="I3" s="87"/>
+      <c r="J3" s="87"/>
+      <c r="K3" s="87"/>
+      <c r="L3" s="87"/>
+      <c r="M3" s="87"/>
+      <c r="N3" s="87"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -3575,40 +3575,40 @@
       </c>
     </row>
     <row r="2" spans="2:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="84"/>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="84"/>
-      <c r="J2" s="84"/>
-      <c r="K2" s="84"/>
-      <c r="L2" s="84"/>
-      <c r="M2" s="84"/>
-      <c r="N2" s="84"/>
-      <c r="O2" s="84"/>
-      <c r="P2" s="84"/>
+      <c r="B2" s="86"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="86"/>
+      <c r="G2" s="86"/>
+      <c r="H2" s="86"/>
+      <c r="I2" s="86"/>
+      <c r="J2" s="86"/>
+      <c r="K2" s="86"/>
+      <c r="L2" s="86"/>
+      <c r="M2" s="86"/>
+      <c r="N2" s="86"/>
+      <c r="O2" s="86"/>
+      <c r="P2" s="86"/>
     </row>
     <row r="3" spans="2:18" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="85" t="s">
+      <c r="B3" s="87" t="s">
         <v>63</v>
       </c>
-      <c r="C3" s="85"/>
-      <c r="D3" s="85"/>
-      <c r="E3" s="85"/>
-      <c r="F3" s="85"/>
-      <c r="G3" s="85"/>
-      <c r="H3" s="85"/>
-      <c r="I3" s="85"/>
-      <c r="J3" s="85"/>
-      <c r="K3" s="85"/>
-      <c r="L3" s="85"/>
-      <c r="M3" s="85"/>
-      <c r="N3" s="85"/>
-      <c r="O3" s="85"/>
-      <c r="P3" s="85"/>
+      <c r="C3" s="87"/>
+      <c r="D3" s="87"/>
+      <c r="E3" s="87"/>
+      <c r="F3" s="87"/>
+      <c r="G3" s="87"/>
+      <c r="H3" s="87"/>
+      <c r="I3" s="87"/>
+      <c r="J3" s="87"/>
+      <c r="K3" s="87"/>
+      <c r="L3" s="87"/>
+      <c r="M3" s="87"/>
+      <c r="N3" s="87"/>
+      <c r="O3" s="87"/>
+      <c r="P3" s="87"/>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
@@ -3722,36 +3722,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="84"/>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="84"/>
-      <c r="J2" s="84"/>
-      <c r="K2" s="84"/>
-      <c r="L2" s="84"/>
-      <c r="M2" s="84"/>
-      <c r="N2" s="84"/>
+      <c r="B2" s="86"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="86"/>
+      <c r="G2" s="86"/>
+      <c r="H2" s="86"/>
+      <c r="I2" s="86"/>
+      <c r="J2" s="86"/>
+      <c r="K2" s="86"/>
+      <c r="L2" s="86"/>
+      <c r="M2" s="86"/>
+      <c r="N2" s="86"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="85" t="s">
+      <c r="B3" s="87" t="s">
         <v>64</v>
       </c>
-      <c r="C3" s="85"/>
-      <c r="D3" s="85"/>
-      <c r="E3" s="85"/>
-      <c r="F3" s="85"/>
-      <c r="G3" s="85"/>
-      <c r="H3" s="85"/>
-      <c r="I3" s="85"/>
-      <c r="J3" s="85"/>
-      <c r="K3" s="85"/>
-      <c r="L3" s="85"/>
-      <c r="M3" s="85"/>
-      <c r="N3" s="85"/>
+      <c r="C3" s="87"/>
+      <c r="D3" s="87"/>
+      <c r="E3" s="87"/>
+      <c r="F3" s="87"/>
+      <c r="G3" s="87"/>
+      <c r="H3" s="87"/>
+      <c r="I3" s="87"/>
+      <c r="J3" s="87"/>
+      <c r="K3" s="87"/>
+      <c r="L3" s="87"/>
+      <c r="M3" s="87"/>
+      <c r="N3" s="87"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="58" t="s">
@@ -3838,38 +3838,38 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="84" t="s">
+      <c r="B2" s="86" t="s">
         <v>97</v>
       </c>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="84"/>
-      <c r="J2" s="84"/>
-      <c r="K2" s="84"/>
-      <c r="L2" s="84"/>
-      <c r="M2" s="84"/>
-      <c r="N2" s="84"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="86"/>
+      <c r="G2" s="86"/>
+      <c r="H2" s="86"/>
+      <c r="I2" s="86"/>
+      <c r="J2" s="86"/>
+      <c r="K2" s="86"/>
+      <c r="L2" s="86"/>
+      <c r="M2" s="86"/>
+      <c r="N2" s="86"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="85" t="s">
+      <c r="B3" s="87" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="85"/>
-      <c r="D3" s="85"/>
-      <c r="E3" s="85"/>
-      <c r="F3" s="85"/>
-      <c r="G3" s="85"/>
-      <c r="H3" s="85"/>
-      <c r="I3" s="85"/>
-      <c r="J3" s="85"/>
-      <c r="K3" s="85"/>
-      <c r="L3" s="85"/>
-      <c r="M3" s="85"/>
-      <c r="N3" s="85"/>
+      <c r="C3" s="87"/>
+      <c r="D3" s="87"/>
+      <c r="E3" s="87"/>
+      <c r="F3" s="87"/>
+      <c r="G3" s="87"/>
+      <c r="H3" s="87"/>
+      <c r="I3" s="87"/>
+      <c r="J3" s="87"/>
+      <c r="K3" s="87"/>
+      <c r="L3" s="87"/>
+      <c r="M3" s="87"/>
+      <c r="N3" s="87"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="44" t="s">
@@ -3928,36 +3928,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="84"/>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="84"/>
-      <c r="J2" s="84"/>
-      <c r="K2" s="84"/>
-      <c r="L2" s="84"/>
-      <c r="M2" s="84"/>
-      <c r="N2" s="84"/>
+      <c r="B2" s="86"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="86"/>
+      <c r="G2" s="86"/>
+      <c r="H2" s="86"/>
+      <c r="I2" s="86"/>
+      <c r="J2" s="86"/>
+      <c r="K2" s="86"/>
+      <c r="L2" s="86"/>
+      <c r="M2" s="86"/>
+      <c r="N2" s="86"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="85" t="s">
+      <c r="B3" s="87" t="s">
         <v>152</v>
       </c>
-      <c r="C3" s="85"/>
-      <c r="D3" s="85"/>
-      <c r="E3" s="85"/>
-      <c r="F3" s="85"/>
-      <c r="G3" s="85"/>
-      <c r="H3" s="85"/>
-      <c r="I3" s="85"/>
-      <c r="J3" s="85"/>
-      <c r="K3" s="85"/>
-      <c r="L3" s="85"/>
-      <c r="M3" s="85"/>
-      <c r="N3" s="85"/>
+      <c r="C3" s="87"/>
+      <c r="D3" s="87"/>
+      <c r="E3" s="87"/>
+      <c r="F3" s="87"/>
+      <c r="G3" s="87"/>
+      <c r="H3" s="87"/>
+      <c r="I3" s="87"/>
+      <c r="J3" s="87"/>
+      <c r="K3" s="87"/>
+      <c r="L3" s="87"/>
+      <c r="M3" s="87"/>
+      <c r="N3" s="87"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="74" t="s">
@@ -4044,28 +4044,28 @@
       </c>
     </row>
     <row r="2" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="84"/>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="84"/>
-      <c r="J2" s="84"/>
+      <c r="B2" s="86"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="86"/>
+      <c r="G2" s="86"/>
+      <c r="H2" s="86"/>
+      <c r="I2" s="86"/>
+      <c r="J2" s="86"/>
     </row>
     <row r="3" spans="2:10" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="85" t="s">
+      <c r="B3" s="87" t="s">
         <v>155</v>
       </c>
-      <c r="C3" s="85"/>
-      <c r="D3" s="85"/>
-      <c r="E3" s="85"/>
-      <c r="F3" s="85"/>
-      <c r="G3" s="85"/>
-      <c r="H3" s="85"/>
-      <c r="I3" s="85"/>
-      <c r="J3" s="85"/>
+      <c r="C3" s="87"/>
+      <c r="D3" s="87"/>
+      <c r="E3" s="87"/>
+      <c r="F3" s="87"/>
+      <c r="G3" s="87"/>
+      <c r="H3" s="87"/>
+      <c r="I3" s="87"/>
+      <c r="J3" s="87"/>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" s="74" t="s">
@@ -4117,7 +4117,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:N6"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
@@ -4144,30 +4144,30 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="84"/>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="84"/>
-      <c r="J2" s="84"/>
-      <c r="K2" s="99"/>
+      <c r="B2" s="86"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="86"/>
+      <c r="G2" s="86"/>
+      <c r="H2" s="86"/>
+      <c r="I2" s="86"/>
+      <c r="J2" s="86"/>
+      <c r="K2" s="85"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="85" t="s">
+      <c r="B3" s="87" t="s">
         <v>156</v>
       </c>
-      <c r="C3" s="85"/>
-      <c r="D3" s="85"/>
-      <c r="E3" s="85"/>
-      <c r="F3" s="85"/>
-      <c r="G3" s="85"/>
-      <c r="H3" s="85"/>
-      <c r="I3" s="85"/>
-      <c r="J3" s="85"/>
-      <c r="K3" s="98"/>
+      <c r="C3" s="87"/>
+      <c r="D3" s="87"/>
+      <c r="E3" s="87"/>
+      <c r="F3" s="87"/>
+      <c r="G3" s="87"/>
+      <c r="H3" s="87"/>
+      <c r="I3" s="87"/>
+      <c r="J3" s="87"/>
+      <c r="K3" s="84"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="81" t="s">
@@ -4259,37 +4259,37 @@
       <c r="Z1" s="38"/>
     </row>
     <row r="2" spans="2:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="84"/>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="84"/>
-      <c r="J2" s="84"/>
-      <c r="K2" s="84"/>
-      <c r="L2" s="84"/>
-      <c r="M2" s="84"/>
-      <c r="N2" s="84"/>
+      <c r="B2" s="86"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="86"/>
+      <c r="G2" s="86"/>
+      <c r="H2" s="86"/>
+      <c r="I2" s="86"/>
+      <c r="J2" s="86"/>
+      <c r="K2" s="86"/>
+      <c r="L2" s="86"/>
+      <c r="M2" s="86"/>
+      <c r="N2" s="86"/>
       <c r="Z2"/>
     </row>
     <row r="3" spans="2:26" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="85" t="s">
+      <c r="B3" s="87" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="85"/>
-      <c r="D3" s="85"/>
-      <c r="E3" s="85"/>
-      <c r="F3" s="85"/>
-      <c r="G3" s="85"/>
-      <c r="H3" s="85"/>
-      <c r="I3" s="85"/>
-      <c r="J3" s="85"/>
-      <c r="K3" s="85"/>
-      <c r="L3" s="85"/>
-      <c r="M3" s="85"/>
-      <c r="N3" s="85"/>
+      <c r="C3" s="87"/>
+      <c r="D3" s="87"/>
+      <c r="E3" s="87"/>
+      <c r="F3" s="87"/>
+      <c r="G3" s="87"/>
+      <c r="H3" s="87"/>
+      <c r="I3" s="87"/>
+      <c r="J3" s="87"/>
+      <c r="K3" s="87"/>
+      <c r="L3" s="87"/>
+      <c r="M3" s="87"/>
+      <c r="N3" s="87"/>
       <c r="Z3"/>
     </row>
     <row r="5" spans="2:26" x14ac:dyDescent="0.25">
@@ -4373,8 +4373,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:Z8"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4393,37 +4393,37 @@
       <c r="Z1" s="38"/>
     </row>
     <row r="2" spans="2:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="84"/>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="84"/>
-      <c r="J2" s="84"/>
-      <c r="K2" s="84"/>
-      <c r="L2" s="84"/>
-      <c r="M2" s="84"/>
-      <c r="N2" s="84"/>
+      <c r="B2" s="86"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="86"/>
+      <c r="G2" s="86"/>
+      <c r="H2" s="86"/>
+      <c r="I2" s="86"/>
+      <c r="J2" s="86"/>
+      <c r="K2" s="86"/>
+      <c r="L2" s="86"/>
+      <c r="M2" s="86"/>
+      <c r="N2" s="86"/>
       <c r="Z2"/>
     </row>
     <row r="3" spans="2:26" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="85" t="s">
+      <c r="B3" s="100" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="85"/>
-      <c r="D3" s="85"/>
-      <c r="E3" s="85"/>
-      <c r="F3" s="85"/>
-      <c r="G3" s="85"/>
-      <c r="H3" s="85"/>
-      <c r="I3" s="85"/>
-      <c r="J3" s="85"/>
-      <c r="K3" s="85"/>
-      <c r="L3" s="85"/>
-      <c r="M3" s="85"/>
-      <c r="N3" s="85"/>
+      <c r="C3" s="100"/>
+      <c r="D3" s="100"/>
+      <c r="E3" s="100"/>
+      <c r="F3" s="100"/>
+      <c r="G3" s="100"/>
+      <c r="H3" s="100"/>
+      <c r="I3" s="100"/>
+      <c r="J3" s="100"/>
+      <c r="K3" s="100"/>
+      <c r="L3" s="100"/>
+      <c r="M3" s="100"/>
+      <c r="N3" s="100"/>
       <c r="Z3"/>
     </row>
     <row r="5" spans="2:26" x14ac:dyDescent="0.25">
@@ -4442,9 +4442,9 @@
       <c r="C6" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="D6" s="87"/>
-      <c r="E6" s="88"/>
-      <c r="F6" s="89"/>
+      <c r="D6" s="97"/>
+      <c r="E6" s="98"/>
+      <c r="F6" s="99"/>
       <c r="G6" s="50"/>
       <c r="H6" s="50"/>
     </row>
@@ -4487,10 +4487,9 @@
       <c r="I8" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="2">
     <mergeCell ref="B2:N2"/>
     <mergeCell ref="B3:N3"/>
-    <mergeCell ref="D6:F6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -4522,37 +4521,37 @@
       <c r="Z1" s="38"/>
     </row>
     <row r="2" spans="2:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="84"/>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="84"/>
-      <c r="J2" s="84"/>
-      <c r="K2" s="84"/>
-      <c r="L2" s="84"/>
-      <c r="M2" s="84"/>
-      <c r="N2" s="84"/>
+      <c r="B2" s="86"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="86"/>
+      <c r="G2" s="86"/>
+      <c r="H2" s="86"/>
+      <c r="I2" s="86"/>
+      <c r="J2" s="86"/>
+      <c r="K2" s="86"/>
+      <c r="L2" s="86"/>
+      <c r="M2" s="86"/>
+      <c r="N2" s="86"/>
       <c r="Z2"/>
     </row>
     <row r="3" spans="2:26" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="85" t="s">
+      <c r="B3" s="87" t="s">
         <v>93</v>
       </c>
-      <c r="C3" s="85"/>
-      <c r="D3" s="85"/>
-      <c r="E3" s="85"/>
-      <c r="F3" s="85"/>
-      <c r="G3" s="85"/>
-      <c r="H3" s="85"/>
-      <c r="I3" s="85"/>
-      <c r="J3" s="85"/>
-      <c r="K3" s="85"/>
-      <c r="L3" s="85"/>
-      <c r="M3" s="85"/>
-      <c r="N3" s="85"/>
+      <c r="C3" s="87"/>
+      <c r="D3" s="87"/>
+      <c r="E3" s="87"/>
+      <c r="F3" s="87"/>
+      <c r="G3" s="87"/>
+      <c r="H3" s="87"/>
+      <c r="I3" s="87"/>
+      <c r="J3" s="87"/>
+      <c r="K3" s="87"/>
+      <c r="L3" s="87"/>
+      <c r="M3" s="87"/>
+      <c r="N3" s="87"/>
       <c r="Z3"/>
     </row>
     <row r="5" spans="2:26" x14ac:dyDescent="0.25">
@@ -4645,37 +4644,37 @@
       <c r="Z1" s="38"/>
     </row>
     <row r="2" spans="2:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="84"/>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="84"/>
-      <c r="J2" s="84"/>
-      <c r="K2" s="84"/>
-      <c r="L2" s="84"/>
-      <c r="M2" s="84"/>
-      <c r="N2" s="84"/>
+      <c r="B2" s="86"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="86"/>
+      <c r="G2" s="86"/>
+      <c r="H2" s="86"/>
+      <c r="I2" s="86"/>
+      <c r="J2" s="86"/>
+      <c r="K2" s="86"/>
+      <c r="L2" s="86"/>
+      <c r="M2" s="86"/>
+      <c r="N2" s="86"/>
       <c r="Z2"/>
     </row>
     <row r="3" spans="2:26" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="85" t="s">
+      <c r="B3" s="87" t="s">
         <v>72</v>
       </c>
-      <c r="C3" s="85"/>
-      <c r="D3" s="85"/>
-      <c r="E3" s="85"/>
-      <c r="F3" s="85"/>
-      <c r="G3" s="85"/>
-      <c r="H3" s="85"/>
-      <c r="I3" s="85"/>
-      <c r="J3" s="85"/>
-      <c r="K3" s="85"/>
-      <c r="L3" s="85"/>
-      <c r="M3" s="85"/>
-      <c r="N3" s="85"/>
+      <c r="C3" s="87"/>
+      <c r="D3" s="87"/>
+      <c r="E3" s="87"/>
+      <c r="F3" s="87"/>
+      <c r="G3" s="87"/>
+      <c r="H3" s="87"/>
+      <c r="I3" s="87"/>
+      <c r="J3" s="87"/>
+      <c r="K3" s="87"/>
+      <c r="L3" s="87"/>
+      <c r="M3" s="87"/>
+      <c r="N3" s="87"/>
       <c r="Z3"/>
     </row>
     <row r="5" spans="2:26" x14ac:dyDescent="0.25">
@@ -4788,56 +4787,56 @@
       </c>
     </row>
     <row r="2" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="84"/>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="84"/>
-      <c r="J2" s="84"/>
-      <c r="K2" s="84"/>
-      <c r="L2" s="84"/>
+      <c r="B2" s="86"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="86"/>
+      <c r="G2" s="86"/>
+      <c r="H2" s="86"/>
+      <c r="I2" s="86"/>
+      <c r="J2" s="86"/>
+      <c r="K2" s="86"/>
+      <c r="L2" s="86"/>
     </row>
     <row r="3" spans="2:17" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="85" t="s">
+      <c r="B3" s="87" t="s">
         <v>108</v>
       </c>
-      <c r="C3" s="85"/>
-      <c r="D3" s="85"/>
-      <c r="E3" s="85"/>
-      <c r="F3" s="85"/>
-      <c r="G3" s="85"/>
-      <c r="H3" s="85"/>
-      <c r="I3" s="85"/>
-      <c r="J3" s="85"/>
-      <c r="K3" s="85"/>
-      <c r="L3" s="85"/>
+      <c r="C3" s="87"/>
+      <c r="D3" s="87"/>
+      <c r="E3" s="87"/>
+      <c r="F3" s="87"/>
+      <c r="G3" s="87"/>
+      <c r="H3" s="87"/>
+      <c r="I3" s="87"/>
+      <c r="J3" s="87"/>
+      <c r="K3" s="87"/>
+      <c r="L3" s="87"/>
     </row>
     <row r="5" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D5" s="90" t="s">
+      <c r="D5" s="89" t="s">
         <v>123</v>
       </c>
-      <c r="E5" s="90"/>
+      <c r="E5" s="89"/>
       <c r="F5" s="73"/>
       <c r="G5" s="73"/>
       <c r="H5" s="73"/>
       <c r="I5" s="73"/>
-      <c r="J5" s="90" t="s">
+      <c r="J5" s="89" t="s">
         <v>42</v>
       </c>
-      <c r="K5" s="90"/>
-      <c r="L5" s="90"/>
-      <c r="M5" s="90" t="s">
+      <c r="K5" s="89"/>
+      <c r="L5" s="89"/>
+      <c r="M5" s="89" t="s">
         <v>130</v>
       </c>
-      <c r="N5" s="90"/>
-      <c r="O5" s="90"/>
-      <c r="P5" s="86" t="s">
+      <c r="N5" s="89"/>
+      <c r="O5" s="89"/>
+      <c r="P5" s="88" t="s">
         <v>109</v>
       </c>
-      <c r="Q5" s="86"/>
+      <c r="Q5" s="88"/>
     </row>
     <row r="6" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="70" t="s">
@@ -4958,72 +4957,72 @@
       </c>
     </row>
     <row r="2" spans="2:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="84"/>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="84"/>
-      <c r="J2" s="84"/>
-      <c r="K2" s="84"/>
-      <c r="L2" s="84"/>
-      <c r="M2" s="84"/>
-      <c r="N2" s="84"/>
-      <c r="O2" s="84"/>
-      <c r="P2" s="84"/>
+      <c r="B2" s="86"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="86"/>
+      <c r="G2" s="86"/>
+      <c r="H2" s="86"/>
+      <c r="I2" s="86"/>
+      <c r="J2" s="86"/>
+      <c r="K2" s="86"/>
+      <c r="L2" s="86"/>
+      <c r="M2" s="86"/>
+      <c r="N2" s="86"/>
+      <c r="O2" s="86"/>
+      <c r="P2" s="86"/>
       <c r="Q2" s="56"/>
       <c r="R2" s="56"/>
     </row>
     <row r="3" spans="2:24" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="85" t="s">
+      <c r="B3" s="87" t="s">
         <v>111</v>
       </c>
-      <c r="C3" s="85"/>
-      <c r="D3" s="85"/>
-      <c r="E3" s="85"/>
-      <c r="F3" s="85"/>
-      <c r="G3" s="85"/>
-      <c r="H3" s="85"/>
-      <c r="I3" s="85"/>
-      <c r="J3" s="85"/>
-      <c r="K3" s="85"/>
-      <c r="L3" s="85"/>
-      <c r="M3" s="85"/>
-      <c r="N3" s="85"/>
-      <c r="O3" s="85"/>
-      <c r="P3" s="85"/>
+      <c r="C3" s="87"/>
+      <c r="D3" s="87"/>
+      <c r="E3" s="87"/>
+      <c r="F3" s="87"/>
+      <c r="G3" s="87"/>
+      <c r="H3" s="87"/>
+      <c r="I3" s="87"/>
+      <c r="J3" s="87"/>
+      <c r="K3" s="87"/>
+      <c r="L3" s="87"/>
+      <c r="M3" s="87"/>
+      <c r="N3" s="87"/>
+      <c r="O3" s="87"/>
+      <c r="P3" s="87"/>
       <c r="Q3" s="57"/>
       <c r="R3" s="57"/>
     </row>
     <row r="5" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B5" s="91" t="s">
+      <c r="B5" s="90" t="s">
         <v>112</v>
       </c>
-      <c r="C5" s="94"/>
-      <c r="D5" s="94"/>
-      <c r="E5" s="94"/>
-      <c r="F5" s="94"/>
-      <c r="G5" s="94"/>
-      <c r="H5" s="94"/>
-      <c r="I5" s="94"/>
-      <c r="J5" s="94"/>
-      <c r="K5" s="94"/>
+      <c r="C5" s="91"/>
+      <c r="D5" s="91"/>
+      <c r="E5" s="91"/>
+      <c r="F5" s="91"/>
+      <c r="G5" s="91"/>
+      <c r="H5" s="91"/>
+      <c r="I5" s="91"/>
+      <c r="J5" s="91"/>
+      <c r="K5" s="91"/>
       <c r="L5" s="92"/>
-      <c r="M5" s="91" t="s">
+      <c r="M5" s="90" t="s">
         <v>113</v>
       </c>
-      <c r="N5" s="94"/>
-      <c r="O5" s="94"/>
-      <c r="P5" s="94"/>
-      <c r="Q5" s="94"/>
-      <c r="R5" s="94"/>
-      <c r="S5" s="94"/>
-      <c r="T5" s="94"/>
-      <c r="U5" s="94"/>
-      <c r="V5" s="94"/>
-      <c r="W5" s="94"/>
+      <c r="N5" s="91"/>
+      <c r="O5" s="91"/>
+      <c r="P5" s="91"/>
+      <c r="Q5" s="91"/>
+      <c r="R5" s="91"/>
+      <c r="S5" s="91"/>
+      <c r="T5" s="91"/>
+      <c r="U5" s="91"/>
+      <c r="V5" s="91"/>
+      <c r="W5" s="91"/>
       <c r="X5" s="92"/>
     </row>
     <row r="6" spans="2:24" x14ac:dyDescent="0.25">
@@ -5031,29 +5030,29 @@
       <c r="C6" s="93"/>
       <c r="D6" s="93"/>
       <c r="E6" s="93"/>
-      <c r="F6" s="95" t="s">
+      <c r="F6" s="94" t="s">
         <v>27</v>
       </c>
-      <c r="G6" s="96"/>
-      <c r="H6" s="96"/>
-      <c r="I6" s="97"/>
-      <c r="J6" s="91" t="s">
+      <c r="G6" s="95"/>
+      <c r="H6" s="95"/>
+      <c r="I6" s="96"/>
+      <c r="J6" s="90" t="s">
         <v>30</v>
       </c>
-      <c r="K6" s="94"/>
+      <c r="K6" s="91"/>
       <c r="L6" s="92"/>
       <c r="M6" s="76"/>
-      <c r="N6" s="91" t="s">
+      <c r="N6" s="90" t="s">
         <v>42</v>
       </c>
       <c r="O6" s="92"/>
-      <c r="P6" s="91" t="s">
+      <c r="P6" s="90" t="s">
         <v>106</v>
       </c>
-      <c r="Q6" s="94"/>
+      <c r="Q6" s="91"/>
       <c r="R6" s="92"/>
       <c r="S6" s="76"/>
-      <c r="T6" s="91" t="s">
+      <c r="T6" s="90" t="s">
         <v>123</v>
       </c>
       <c r="U6" s="92"/>
@@ -5290,36 +5289,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="84"/>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="84"/>
-      <c r="J2" s="84"/>
-      <c r="K2" s="84"/>
-      <c r="L2" s="84"/>
-      <c r="M2" s="84"/>
-      <c r="N2" s="84"/>
+      <c r="B2" s="86"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="86"/>
+      <c r="G2" s="86"/>
+      <c r="H2" s="86"/>
+      <c r="I2" s="86"/>
+      <c r="J2" s="86"/>
+      <c r="K2" s="86"/>
+      <c r="L2" s="86"/>
+      <c r="M2" s="86"/>
+      <c r="N2" s="86"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="85" t="s">
+      <c r="B3" s="87" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="85"/>
-      <c r="D3" s="85"/>
-      <c r="E3" s="85"/>
-      <c r="F3" s="85"/>
-      <c r="G3" s="85"/>
-      <c r="H3" s="85"/>
-      <c r="I3" s="85"/>
-      <c r="J3" s="85"/>
-      <c r="K3" s="85"/>
-      <c r="L3" s="85"/>
-      <c r="M3" s="85"/>
-      <c r="N3" s="85"/>
+      <c r="C3" s="87"/>
+      <c r="D3" s="87"/>
+      <c r="E3" s="87"/>
+      <c r="F3" s="87"/>
+      <c r="G3" s="87"/>
+      <c r="H3" s="87"/>
+      <c r="I3" s="87"/>
+      <c r="J3" s="87"/>
+      <c r="K3" s="87"/>
+      <c r="L3" s="87"/>
+      <c r="M3" s="87"/>
+      <c r="N3" s="87"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="44" t="s">
@@ -5386,40 +5385,40 @@
       </c>
     </row>
     <row r="2" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="84"/>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="84"/>
-      <c r="J2" s="84"/>
-      <c r="K2" s="84"/>
-      <c r="L2" s="84"/>
-      <c r="M2" s="84"/>
-      <c r="N2" s="84"/>
-      <c r="O2" s="84"/>
-      <c r="P2" s="84"/>
+      <c r="B2" s="86"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="86"/>
+      <c r="G2" s="86"/>
+      <c r="H2" s="86"/>
+      <c r="I2" s="86"/>
+      <c r="J2" s="86"/>
+      <c r="K2" s="86"/>
+      <c r="L2" s="86"/>
+      <c r="M2" s="86"/>
+      <c r="N2" s="86"/>
+      <c r="O2" s="86"/>
+      <c r="P2" s="86"/>
     </row>
     <row r="3" spans="2:16" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="85" t="s">
+      <c r="B3" s="87" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="85"/>
-      <c r="D3" s="85"/>
-      <c r="E3" s="85"/>
-      <c r="F3" s="85"/>
-      <c r="G3" s="85"/>
-      <c r="H3" s="85"/>
-      <c r="I3" s="85"/>
-      <c r="J3" s="85"/>
-      <c r="K3" s="85"/>
-      <c r="L3" s="85"/>
-      <c r="M3" s="85"/>
-      <c r="N3" s="85"/>
-      <c r="O3" s="85"/>
-      <c r="P3" s="85"/>
+      <c r="C3" s="87"/>
+      <c r="D3" s="87"/>
+      <c r="E3" s="87"/>
+      <c r="F3" s="87"/>
+      <c r="G3" s="87"/>
+      <c r="H3" s="87"/>
+      <c r="I3" s="87"/>
+      <c r="J3" s="87"/>
+      <c r="K3" s="87"/>
+      <c r="L3" s="87"/>
+      <c r="M3" s="87"/>
+      <c r="N3" s="87"/>
+      <c r="O3" s="87"/>
+      <c r="P3" s="87"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="44" t="s">
@@ -5498,40 +5497,40 @@
       </c>
     </row>
     <row r="2" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="84"/>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="84"/>
-      <c r="J2" s="84"/>
-      <c r="K2" s="84"/>
-      <c r="L2" s="84"/>
-      <c r="M2" s="84"/>
-      <c r="N2" s="84"/>
-      <c r="O2" s="84"/>
-      <c r="P2" s="84"/>
+      <c r="B2" s="86"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="86"/>
+      <c r="G2" s="86"/>
+      <c r="H2" s="86"/>
+      <c r="I2" s="86"/>
+      <c r="J2" s="86"/>
+      <c r="K2" s="86"/>
+      <c r="L2" s="86"/>
+      <c r="M2" s="86"/>
+      <c r="N2" s="86"/>
+      <c r="O2" s="86"/>
+      <c r="P2" s="86"/>
     </row>
     <row r="3" spans="2:16" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="85" t="s">
+      <c r="B3" s="87" t="s">
         <v>68</v>
       </c>
-      <c r="C3" s="85"/>
-      <c r="D3" s="85"/>
-      <c r="E3" s="85"/>
-      <c r="F3" s="85"/>
-      <c r="G3" s="85"/>
-      <c r="H3" s="85"/>
-      <c r="I3" s="85"/>
-      <c r="J3" s="85"/>
-      <c r="K3" s="85"/>
-      <c r="L3" s="85"/>
-      <c r="M3" s="85"/>
-      <c r="N3" s="85"/>
-      <c r="O3" s="85"/>
-      <c r="P3" s="85"/>
+      <c r="C3" s="87"/>
+      <c r="D3" s="87"/>
+      <c r="E3" s="87"/>
+      <c r="F3" s="87"/>
+      <c r="G3" s="87"/>
+      <c r="H3" s="87"/>
+      <c r="I3" s="87"/>
+      <c r="J3" s="87"/>
+      <c r="K3" s="87"/>
+      <c r="L3" s="87"/>
+      <c r="M3" s="87"/>
+      <c r="N3" s="87"/>
+      <c r="O3" s="87"/>
+      <c r="P3" s="87"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
@@ -5580,40 +5579,40 @@
       </c>
     </row>
     <row r="2" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="84"/>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="84"/>
-      <c r="J2" s="84"/>
-      <c r="K2" s="84"/>
-      <c r="L2" s="84"/>
-      <c r="M2" s="84"/>
-      <c r="N2" s="84"/>
-      <c r="O2" s="84"/>
-      <c r="P2" s="84"/>
+      <c r="B2" s="86"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="86"/>
+      <c r="G2" s="86"/>
+      <c r="H2" s="86"/>
+      <c r="I2" s="86"/>
+      <c r="J2" s="86"/>
+      <c r="K2" s="86"/>
+      <c r="L2" s="86"/>
+      <c r="M2" s="86"/>
+      <c r="N2" s="86"/>
+      <c r="O2" s="86"/>
+      <c r="P2" s="86"/>
     </row>
     <row r="3" spans="2:16" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="85" t="s">
+      <c r="B3" s="87" t="s">
         <v>71</v>
       </c>
-      <c r="C3" s="85"/>
-      <c r="D3" s="85"/>
-      <c r="E3" s="85"/>
-      <c r="F3" s="85"/>
-      <c r="G3" s="85"/>
-      <c r="H3" s="85"/>
-      <c r="I3" s="85"/>
-      <c r="J3" s="85"/>
-      <c r="K3" s="85"/>
-      <c r="L3" s="85"/>
-      <c r="M3" s="85"/>
-      <c r="N3" s="85"/>
-      <c r="O3" s="85"/>
-      <c r="P3" s="85"/>
+      <c r="C3" s="87"/>
+      <c r="D3" s="87"/>
+      <c r="E3" s="87"/>
+      <c r="F3" s="87"/>
+      <c r="G3" s="87"/>
+      <c r="H3" s="87"/>
+      <c r="I3" s="87"/>
+      <c r="J3" s="87"/>
+      <c r="K3" s="87"/>
+      <c r="L3" s="87"/>
+      <c r="M3" s="87"/>
+      <c r="N3" s="87"/>
+      <c r="O3" s="87"/>
+      <c r="P3" s="87"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
@@ -5667,36 +5666,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="84"/>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="84"/>
-      <c r="J2" s="84"/>
-      <c r="K2" s="84"/>
-      <c r="L2" s="84"/>
-      <c r="M2" s="84"/>
-      <c r="N2" s="84"/>
+      <c r="B2" s="86"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="86"/>
+      <c r="G2" s="86"/>
+      <c r="H2" s="86"/>
+      <c r="I2" s="86"/>
+      <c r="J2" s="86"/>
+      <c r="K2" s="86"/>
+      <c r="L2" s="86"/>
+      <c r="M2" s="86"/>
+      <c r="N2" s="86"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="85" t="s">
+      <c r="B3" s="87" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="85"/>
-      <c r="D3" s="85"/>
-      <c r="E3" s="85"/>
-      <c r="F3" s="85"/>
-      <c r="G3" s="85"/>
-      <c r="H3" s="85"/>
-      <c r="I3" s="85"/>
-      <c r="J3" s="85"/>
-      <c r="K3" s="85"/>
-      <c r="L3" s="85"/>
-      <c r="M3" s="85"/>
-      <c r="N3" s="85"/>
+      <c r="C3" s="87"/>
+      <c r="D3" s="87"/>
+      <c r="E3" s="87"/>
+      <c r="F3" s="87"/>
+      <c r="G3" s="87"/>
+      <c r="H3" s="87"/>
+      <c r="I3" s="87"/>
+      <c r="J3" s="87"/>
+      <c r="K3" s="87"/>
+      <c r="L3" s="87"/>
+      <c r="M3" s="87"/>
+      <c r="N3" s="87"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="44" t="s">
@@ -5785,40 +5784,40 @@
       </c>
     </row>
     <row r="2" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="84"/>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="84"/>
-      <c r="J2" s="84"/>
-      <c r="K2" s="84"/>
-      <c r="L2" s="84"/>
-      <c r="M2" s="84"/>
-      <c r="N2" s="84"/>
-      <c r="O2" s="84"/>
-      <c r="P2" s="84"/>
+      <c r="B2" s="86"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="86"/>
+      <c r="G2" s="86"/>
+      <c r="H2" s="86"/>
+      <c r="I2" s="86"/>
+      <c r="J2" s="86"/>
+      <c r="K2" s="86"/>
+      <c r="L2" s="86"/>
+      <c r="M2" s="86"/>
+      <c r="N2" s="86"/>
+      <c r="O2" s="86"/>
+      <c r="P2" s="86"/>
     </row>
     <row r="3" spans="2:16" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="85" t="s">
+      <c r="B3" s="87" t="s">
         <v>65</v>
       </c>
-      <c r="C3" s="85"/>
-      <c r="D3" s="85"/>
-      <c r="E3" s="85"/>
-      <c r="F3" s="85"/>
-      <c r="G3" s="85"/>
-      <c r="H3" s="85"/>
-      <c r="I3" s="85"/>
-      <c r="J3" s="85"/>
-      <c r="K3" s="85"/>
-      <c r="L3" s="85"/>
-      <c r="M3" s="85"/>
-      <c r="N3" s="85"/>
-      <c r="O3" s="85"/>
-      <c r="P3" s="85"/>
+      <c r="C3" s="87"/>
+      <c r="D3" s="87"/>
+      <c r="E3" s="87"/>
+      <c r="F3" s="87"/>
+      <c r="G3" s="87"/>
+      <c r="H3" s="87"/>
+      <c r="I3" s="87"/>
+      <c r="J3" s="87"/>
+      <c r="K3" s="87"/>
+      <c r="L3" s="87"/>
+      <c r="M3" s="87"/>
+      <c r="N3" s="87"/>
+      <c r="O3" s="87"/>
+      <c r="P3" s="87"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="45" t="s">
@@ -5870,36 +5869,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="84"/>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="84"/>
-      <c r="J2" s="84"/>
-      <c r="K2" s="84"/>
-      <c r="L2" s="84"/>
-      <c r="M2" s="84"/>
-      <c r="N2" s="84"/>
+      <c r="B2" s="86"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="86"/>
+      <c r="G2" s="86"/>
+      <c r="H2" s="86"/>
+      <c r="I2" s="86"/>
+      <c r="J2" s="86"/>
+      <c r="K2" s="86"/>
+      <c r="L2" s="86"/>
+      <c r="M2" s="86"/>
+      <c r="N2" s="86"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="85" t="s">
+      <c r="B3" s="87" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="85"/>
-      <c r="D3" s="85"/>
-      <c r="E3" s="85"/>
-      <c r="F3" s="85"/>
-      <c r="G3" s="85"/>
-      <c r="H3" s="85"/>
-      <c r="I3" s="85"/>
-      <c r="J3" s="85"/>
-      <c r="K3" s="85"/>
-      <c r="L3" s="85"/>
-      <c r="M3" s="85"/>
-      <c r="N3" s="85"/>
+      <c r="C3" s="87"/>
+      <c r="D3" s="87"/>
+      <c r="E3" s="87"/>
+      <c r="F3" s="87"/>
+      <c r="G3" s="87"/>
+      <c r="H3" s="87"/>
+      <c r="I3" s="87"/>
+      <c r="J3" s="87"/>
+      <c r="K3" s="87"/>
+      <c r="L3" s="87"/>
+      <c r="M3" s="87"/>
+      <c r="N3" s="87"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">

</xml_diff>

<commit_message>
TRIEDA-1631 - Adicionando exportação para excel do relatório de porcentagem de mestres e doutores.
</commit_message>
<xml_diff>
--- a/code/client/web/src/main/resources/templateExport.xlsx
+++ b/code/client/web/src/main/resources/templateExport.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="17070" windowHeight="5370" tabRatio="622" firstSheet="19" activeTab="23"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="17070" windowHeight="5370" tabRatio="797" firstSheet="21" activeTab="22"/>
   </bookViews>
   <sheets>
     <sheet name="Campi" sheetId="3" r:id="rId1"/>
@@ -29,13 +29,14 @@
     <sheet name="Atendimentos por Matricula" sheetId="30" r:id="rId20"/>
     <sheet name="Atendimentos por Disciplina" sheetId="31" r:id="rId21"/>
     <sheet name="Atendimentos Faixa de Demanda" sheetId="32" r:id="rId22"/>
-    <sheet name="Relatorio Visao Sala" sheetId="10" r:id="rId23"/>
-    <sheet name="Relatorio Visao Aluno" sheetId="25" r:id="rId24"/>
-    <sheet name="Relatorio Visao Professor" sheetId="21" r:id="rId25"/>
-    <sheet name="Relatorio Visao Curso" sheetId="20" r:id="rId26"/>
-    <sheet name="Atendimentos por Aluno" sheetId="23" r:id="rId27"/>
-    <sheet name="Aulas" sheetId="26" r:id="rId28"/>
-    <sheet name="PaletaCores" sheetId="11" r:id="rId29"/>
+    <sheet name="Porcentagem Mestres e Doutores" sheetId="33" r:id="rId23"/>
+    <sheet name="Relatorio Visao Sala" sheetId="10" r:id="rId24"/>
+    <sheet name="Relatorio Visao Aluno" sheetId="25" r:id="rId25"/>
+    <sheet name="Relatorio Visao Professor" sheetId="21" r:id="rId26"/>
+    <sheet name="Relatorio Visao Curso" sheetId="20" r:id="rId27"/>
+    <sheet name="Atendimentos por Aluno" sheetId="23" r:id="rId28"/>
+    <sheet name="Aulas" sheetId="26" r:id="rId29"/>
+    <sheet name="PaletaCores" sheetId="11" r:id="rId30"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
@@ -1214,7 +1215,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="177">
   <si>
     <t>Planilha de Unidades</t>
   </si>
@@ -1718,6 +1719,33 @@
   </si>
   <si>
     <t>% Atendimento Acum</t>
+  </si>
+  <si>
+    <t>Planilha de Porcentagem de Mestres e Doutores</t>
+  </si>
+  <si>
+    <t>Doutores</t>
+  </si>
+  <si>
+    <t>Mestres</t>
+  </si>
+  <si>
+    <t>% Doutores</t>
+  </si>
+  <si>
+    <t>% Mestres e Doutores</t>
+  </si>
+  <si>
+    <t>% Mínimo de Doutores</t>
+  </si>
+  <si>
+    <t>% Mínimo de Mestres e Doutores</t>
+  </si>
+  <si>
+    <t>MÍNIMO MEC</t>
+  </si>
+  <si>
+    <t>ALOCAÇÃO</t>
   </si>
 </sst>
 </file>
@@ -1725,9 +1753,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="&quot;R$&quot;\ #,##0.00"/>
+    <numFmt numFmtId="165" formatCode="&quot;R$&quot;\ #,##0.00"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1743,6 +1771,18 @@
     </font>
     <font>
       <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
@@ -1810,15 +1850,6 @@
     </font>
     <font>
       <b/>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <u/>
       <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -2105,21 +2136,21 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -2134,16 +2165,16 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2225,70 +2256,70 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="27" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="6" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2301,97 +2332,106 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="28" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="28" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2720,38 +2760,38 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="86" t="s">
+      <c r="B2" s="88" t="s">
         <v>96</v>
       </c>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="86"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="86"/>
-      <c r="H2" s="86"/>
-      <c r="I2" s="86"/>
-      <c r="J2" s="86"/>
-      <c r="K2" s="86"/>
-      <c r="L2" s="86"/>
-      <c r="M2" s="86"/>
-      <c r="N2" s="86"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="88"/>
+      <c r="G2" s="88"/>
+      <c r="H2" s="88"/>
+      <c r="I2" s="88"/>
+      <c r="J2" s="88"/>
+      <c r="K2" s="88"/>
+      <c r="L2" s="88"/>
+      <c r="M2" s="88"/>
+      <c r="N2" s="88"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="87" t="s">
+      <c r="B3" s="89" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="87"/>
-      <c r="D3" s="87"/>
-      <c r="E3" s="87"/>
-      <c r="F3" s="87"/>
-      <c r="G3" s="87"/>
-      <c r="H3" s="87"/>
-      <c r="I3" s="87"/>
-      <c r="J3" s="87"/>
-      <c r="K3" s="87"/>
-      <c r="L3" s="87"/>
-      <c r="M3" s="87"/>
-      <c r="N3" s="87"/>
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="89"/>
+      <c r="F3" s="89"/>
+      <c r="G3" s="89"/>
+      <c r="H3" s="89"/>
+      <c r="I3" s="89"/>
+      <c r="J3" s="89"/>
+      <c r="K3" s="89"/>
+      <c r="L3" s="89"/>
+      <c r="M3" s="89"/>
+      <c r="N3" s="89"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="44" t="s">
@@ -2819,36 +2859,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="86"/>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="86"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="86"/>
-      <c r="H2" s="86"/>
-      <c r="I2" s="86"/>
-      <c r="J2" s="86"/>
-      <c r="K2" s="86"/>
-      <c r="L2" s="86"/>
-      <c r="M2" s="86"/>
-      <c r="N2" s="86"/>
+      <c r="B2" s="88"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="88"/>
+      <c r="G2" s="88"/>
+      <c r="H2" s="88"/>
+      <c r="I2" s="88"/>
+      <c r="J2" s="88"/>
+      <c r="K2" s="88"/>
+      <c r="L2" s="88"/>
+      <c r="M2" s="88"/>
+      <c r="N2" s="88"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="87" t="s">
+      <c r="B3" s="89" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="87"/>
-      <c r="D3" s="87"/>
-      <c r="E3" s="87"/>
-      <c r="F3" s="87"/>
-      <c r="G3" s="87"/>
-      <c r="H3" s="87"/>
-      <c r="I3" s="87"/>
-      <c r="J3" s="87"/>
-      <c r="K3" s="87"/>
-      <c r="L3" s="87"/>
-      <c r="M3" s="87"/>
-      <c r="N3" s="87"/>
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="89"/>
+      <c r="F3" s="89"/>
+      <c r="G3" s="89"/>
+      <c r="H3" s="89"/>
+      <c r="I3" s="89"/>
+      <c r="J3" s="89"/>
+      <c r="K3" s="89"/>
+      <c r="L3" s="89"/>
+      <c r="M3" s="89"/>
+      <c r="N3" s="89"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -2917,36 +2957,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="86"/>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="86"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="86"/>
-      <c r="H2" s="86"/>
-      <c r="I2" s="86"/>
-      <c r="J2" s="86"/>
-      <c r="K2" s="86"/>
-      <c r="L2" s="86"/>
-      <c r="M2" s="86"/>
-      <c r="N2" s="86"/>
+      <c r="B2" s="88"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="88"/>
+      <c r="G2" s="88"/>
+      <c r="H2" s="88"/>
+      <c r="I2" s="88"/>
+      <c r="J2" s="88"/>
+      <c r="K2" s="88"/>
+      <c r="L2" s="88"/>
+      <c r="M2" s="88"/>
+      <c r="N2" s="88"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="87" t="s">
+      <c r="B3" s="89" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="87"/>
-      <c r="D3" s="87"/>
-      <c r="E3" s="87"/>
-      <c r="F3" s="87"/>
-      <c r="G3" s="87"/>
-      <c r="H3" s="87"/>
-      <c r="I3" s="87"/>
-      <c r="J3" s="87"/>
-      <c r="K3" s="87"/>
-      <c r="L3" s="87"/>
-      <c r="M3" s="87"/>
-      <c r="N3" s="87"/>
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="89"/>
+      <c r="F3" s="89"/>
+      <c r="G3" s="89"/>
+      <c r="H3" s="89"/>
+      <c r="I3" s="89"/>
+      <c r="J3" s="89"/>
+      <c r="K3" s="89"/>
+      <c r="L3" s="89"/>
+      <c r="M3" s="89"/>
+      <c r="N3" s="89"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -3031,18 +3071,18 @@
       </c>
     </row>
     <row r="2" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="86"/>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="86"/>
+      <c r="B2" s="88"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
     </row>
     <row r="3" spans="2:5" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="87" t="s">
+      <c r="B3" s="89" t="s">
         <v>126</v>
       </c>
-      <c r="C3" s="87"/>
-      <c r="D3" s="87"/>
-      <c r="E3" s="87"/>
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="89"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="60" t="s">
@@ -3095,36 +3135,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="86"/>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="86"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="86"/>
-      <c r="H2" s="86"/>
-      <c r="I2" s="86"/>
-      <c r="J2" s="86"/>
-      <c r="K2" s="86"/>
-      <c r="L2" s="86"/>
-      <c r="M2" s="86"/>
-      <c r="N2" s="86"/>
+      <c r="B2" s="88"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="88"/>
+      <c r="G2" s="88"/>
+      <c r="H2" s="88"/>
+      <c r="I2" s="88"/>
+      <c r="J2" s="88"/>
+      <c r="K2" s="88"/>
+      <c r="L2" s="88"/>
+      <c r="M2" s="88"/>
+      <c r="N2" s="88"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="87" t="s">
+      <c r="B3" s="89" t="s">
         <v>100</v>
       </c>
-      <c r="C3" s="87"/>
-      <c r="D3" s="87"/>
-      <c r="E3" s="87"/>
-      <c r="F3" s="87"/>
-      <c r="G3" s="87"/>
-      <c r="H3" s="87"/>
-      <c r="I3" s="87"/>
-      <c r="J3" s="87"/>
-      <c r="K3" s="87"/>
-      <c r="L3" s="87"/>
-      <c r="M3" s="87"/>
-      <c r="N3" s="87"/>
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="89"/>
+      <c r="F3" s="89"/>
+      <c r="G3" s="89"/>
+      <c r="H3" s="89"/>
+      <c r="I3" s="89"/>
+      <c r="J3" s="89"/>
+      <c r="K3" s="89"/>
+      <c r="L3" s="89"/>
+      <c r="M3" s="89"/>
+      <c r="N3" s="89"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -3157,10 +3197,10 @@
       <c r="K5" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="L5" s="88" t="s">
+      <c r="L5" s="90" t="s">
         <v>110</v>
       </c>
-      <c r="M5" s="88"/>
+      <c r="M5" s="90"/>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
@@ -3212,38 +3252,38 @@
       </c>
     </row>
     <row r="2" spans="2:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="86"/>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="86"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="86"/>
-      <c r="H2" s="86"/>
-      <c r="I2" s="86"/>
-      <c r="J2" s="86"/>
-      <c r="K2" s="86"/>
-      <c r="L2" s="86"/>
-      <c r="M2" s="86"/>
-      <c r="N2" s="86"/>
-      <c r="O2" s="86"/>
+      <c r="B2" s="88"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="88"/>
+      <c r="G2" s="88"/>
+      <c r="H2" s="88"/>
+      <c r="I2" s="88"/>
+      <c r="J2" s="88"/>
+      <c r="K2" s="88"/>
+      <c r="L2" s="88"/>
+      <c r="M2" s="88"/>
+      <c r="N2" s="88"/>
+      <c r="O2" s="88"/>
     </row>
     <row r="3" spans="2:15" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="87" t="s">
+      <c r="B3" s="89" t="s">
         <v>73</v>
       </c>
-      <c r="C3" s="87"/>
-      <c r="D3" s="87"/>
-      <c r="E3" s="87"/>
-      <c r="F3" s="87"/>
-      <c r="G3" s="87"/>
-      <c r="H3" s="87"/>
-      <c r="I3" s="87"/>
-      <c r="J3" s="87"/>
-      <c r="K3" s="87"/>
-      <c r="L3" s="87"/>
-      <c r="M3" s="87"/>
-      <c r="N3" s="87"/>
-      <c r="O3" s="87"/>
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="89"/>
+      <c r="F3" s="89"/>
+      <c r="G3" s="89"/>
+      <c r="H3" s="89"/>
+      <c r="I3" s="89"/>
+      <c r="J3" s="89"/>
+      <c r="K3" s="89"/>
+      <c r="L3" s="89"/>
+      <c r="M3" s="89"/>
+      <c r="N3" s="89"/>
+      <c r="O3" s="89"/>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -3322,18 +3362,18 @@
       </c>
     </row>
     <row r="2" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="86"/>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="86"/>
+      <c r="B2" s="88"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
     </row>
     <row r="3" spans="2:5" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="87" t="s">
+      <c r="B3" s="89" t="s">
         <v>131</v>
       </c>
-      <c r="C3" s="87"/>
-      <c r="D3" s="87"/>
-      <c r="E3" s="87"/>
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="89"/>
     </row>
     <row r="4" spans="2:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="64"/>
@@ -3395,36 +3435,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="86"/>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="86"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="86"/>
-      <c r="H2" s="86"/>
-      <c r="I2" s="86"/>
-      <c r="J2" s="86"/>
-      <c r="K2" s="86"/>
-      <c r="L2" s="86"/>
-      <c r="M2" s="86"/>
-      <c r="N2" s="86"/>
+      <c r="B2" s="88"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="88"/>
+      <c r="G2" s="88"/>
+      <c r="H2" s="88"/>
+      <c r="I2" s="88"/>
+      <c r="J2" s="88"/>
+      <c r="K2" s="88"/>
+      <c r="L2" s="88"/>
+      <c r="M2" s="88"/>
+      <c r="N2" s="88"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="87" t="s">
+      <c r="B3" s="89" t="s">
         <v>69</v>
       </c>
-      <c r="C3" s="87"/>
-      <c r="D3" s="87"/>
-      <c r="E3" s="87"/>
-      <c r="F3" s="87"/>
-      <c r="G3" s="87"/>
-      <c r="H3" s="87"/>
-      <c r="I3" s="87"/>
-      <c r="J3" s="87"/>
-      <c r="K3" s="87"/>
-      <c r="L3" s="87"/>
-      <c r="M3" s="87"/>
-      <c r="N3" s="87"/>
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="89"/>
+      <c r="F3" s="89"/>
+      <c r="G3" s="89"/>
+      <c r="H3" s="89"/>
+      <c r="I3" s="89"/>
+      <c r="J3" s="89"/>
+      <c r="K3" s="89"/>
+      <c r="L3" s="89"/>
+      <c r="M3" s="89"/>
+      <c r="N3" s="89"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -3479,36 +3519,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="86"/>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="86"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="86"/>
-      <c r="H2" s="86"/>
-      <c r="I2" s="86"/>
-      <c r="J2" s="86"/>
-      <c r="K2" s="86"/>
-      <c r="L2" s="86"/>
-      <c r="M2" s="86"/>
-      <c r="N2" s="86"/>
+      <c r="B2" s="88"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="88"/>
+      <c r="G2" s="88"/>
+      <c r="H2" s="88"/>
+      <c r="I2" s="88"/>
+      <c r="J2" s="88"/>
+      <c r="K2" s="88"/>
+      <c r="L2" s="88"/>
+      <c r="M2" s="88"/>
+      <c r="N2" s="88"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="87" t="s">
+      <c r="B3" s="89" t="s">
         <v>74</v>
       </c>
-      <c r="C3" s="87"/>
-      <c r="D3" s="87"/>
-      <c r="E3" s="87"/>
-      <c r="F3" s="87"/>
-      <c r="G3" s="87"/>
-      <c r="H3" s="87"/>
-      <c r="I3" s="87"/>
-      <c r="J3" s="87"/>
-      <c r="K3" s="87"/>
-      <c r="L3" s="87"/>
-      <c r="M3" s="87"/>
-      <c r="N3" s="87"/>
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="89"/>
+      <c r="F3" s="89"/>
+      <c r="G3" s="89"/>
+      <c r="H3" s="89"/>
+      <c r="I3" s="89"/>
+      <c r="J3" s="89"/>
+      <c r="K3" s="89"/>
+      <c r="L3" s="89"/>
+      <c r="M3" s="89"/>
+      <c r="N3" s="89"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -3545,7 +3585,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:R6"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="P6" sqref="P6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3575,40 +3617,40 @@
       </c>
     </row>
     <row r="2" spans="2:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="86"/>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="86"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="86"/>
-      <c r="H2" s="86"/>
-      <c r="I2" s="86"/>
-      <c r="J2" s="86"/>
-      <c r="K2" s="86"/>
-      <c r="L2" s="86"/>
-      <c r="M2" s="86"/>
-      <c r="N2" s="86"/>
-      <c r="O2" s="86"/>
-      <c r="P2" s="86"/>
+      <c r="B2" s="88"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="88"/>
+      <c r="G2" s="88"/>
+      <c r="H2" s="88"/>
+      <c r="I2" s="88"/>
+      <c r="J2" s="88"/>
+      <c r="K2" s="88"/>
+      <c r="L2" s="88"/>
+      <c r="M2" s="88"/>
+      <c r="N2" s="88"/>
+      <c r="O2" s="88"/>
+      <c r="P2" s="88"/>
     </row>
     <row r="3" spans="2:18" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="87" t="s">
+      <c r="B3" s="89" t="s">
         <v>63</v>
       </c>
-      <c r="C3" s="87"/>
-      <c r="D3" s="87"/>
-      <c r="E3" s="87"/>
-      <c r="F3" s="87"/>
-      <c r="G3" s="87"/>
-      <c r="H3" s="87"/>
-      <c r="I3" s="87"/>
-      <c r="J3" s="87"/>
-      <c r="K3" s="87"/>
-      <c r="L3" s="87"/>
-      <c r="M3" s="87"/>
-      <c r="N3" s="87"/>
-      <c r="O3" s="87"/>
-      <c r="P3" s="87"/>
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="89"/>
+      <c r="F3" s="89"/>
+      <c r="G3" s="89"/>
+      <c r="H3" s="89"/>
+      <c r="I3" s="89"/>
+      <c r="J3" s="89"/>
+      <c r="K3" s="89"/>
+      <c r="L3" s="89"/>
+      <c r="M3" s="89"/>
+      <c r="N3" s="89"/>
+      <c r="O3" s="89"/>
+      <c r="P3" s="89"/>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
@@ -3722,36 +3764,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="86"/>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="86"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="86"/>
-      <c r="H2" s="86"/>
-      <c r="I2" s="86"/>
-      <c r="J2" s="86"/>
-      <c r="K2" s="86"/>
-      <c r="L2" s="86"/>
-      <c r="M2" s="86"/>
-      <c r="N2" s="86"/>
+      <c r="B2" s="88"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="88"/>
+      <c r="G2" s="88"/>
+      <c r="H2" s="88"/>
+      <c r="I2" s="88"/>
+      <c r="J2" s="88"/>
+      <c r="K2" s="88"/>
+      <c r="L2" s="88"/>
+      <c r="M2" s="88"/>
+      <c r="N2" s="88"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="87" t="s">
+      <c r="B3" s="89" t="s">
         <v>64</v>
       </c>
-      <c r="C3" s="87"/>
-      <c r="D3" s="87"/>
-      <c r="E3" s="87"/>
-      <c r="F3" s="87"/>
-      <c r="G3" s="87"/>
-      <c r="H3" s="87"/>
-      <c r="I3" s="87"/>
-      <c r="J3" s="87"/>
-      <c r="K3" s="87"/>
-      <c r="L3" s="87"/>
-      <c r="M3" s="87"/>
-      <c r="N3" s="87"/>
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="89"/>
+      <c r="F3" s="89"/>
+      <c r="G3" s="89"/>
+      <c r="H3" s="89"/>
+      <c r="I3" s="89"/>
+      <c r="J3" s="89"/>
+      <c r="K3" s="89"/>
+      <c r="L3" s="89"/>
+      <c r="M3" s="89"/>
+      <c r="N3" s="89"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="58" t="s">
@@ -3838,38 +3880,38 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="86" t="s">
+      <c r="B2" s="88" t="s">
         <v>97</v>
       </c>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="86"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="86"/>
-      <c r="H2" s="86"/>
-      <c r="I2" s="86"/>
-      <c r="J2" s="86"/>
-      <c r="K2" s="86"/>
-      <c r="L2" s="86"/>
-      <c r="M2" s="86"/>
-      <c r="N2" s="86"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="88"/>
+      <c r="G2" s="88"/>
+      <c r="H2" s="88"/>
+      <c r="I2" s="88"/>
+      <c r="J2" s="88"/>
+      <c r="K2" s="88"/>
+      <c r="L2" s="88"/>
+      <c r="M2" s="88"/>
+      <c r="N2" s="88"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="87" t="s">
+      <c r="B3" s="89" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="87"/>
-      <c r="D3" s="87"/>
-      <c r="E3" s="87"/>
-      <c r="F3" s="87"/>
-      <c r="G3" s="87"/>
-      <c r="H3" s="87"/>
-      <c r="I3" s="87"/>
-      <c r="J3" s="87"/>
-      <c r="K3" s="87"/>
-      <c r="L3" s="87"/>
-      <c r="M3" s="87"/>
-      <c r="N3" s="87"/>
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="89"/>
+      <c r="F3" s="89"/>
+      <c r="G3" s="89"/>
+      <c r="H3" s="89"/>
+      <c r="I3" s="89"/>
+      <c r="J3" s="89"/>
+      <c r="K3" s="89"/>
+      <c r="L3" s="89"/>
+      <c r="M3" s="89"/>
+      <c r="N3" s="89"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="44" t="s">
@@ -3928,36 +3970,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="86"/>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="86"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="86"/>
-      <c r="H2" s="86"/>
-      <c r="I2" s="86"/>
-      <c r="J2" s="86"/>
-      <c r="K2" s="86"/>
-      <c r="L2" s="86"/>
-      <c r="M2" s="86"/>
-      <c r="N2" s="86"/>
+      <c r="B2" s="88"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="88"/>
+      <c r="G2" s="88"/>
+      <c r="H2" s="88"/>
+      <c r="I2" s="88"/>
+      <c r="J2" s="88"/>
+      <c r="K2" s="88"/>
+      <c r="L2" s="88"/>
+      <c r="M2" s="88"/>
+      <c r="N2" s="88"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="87" t="s">
+      <c r="B3" s="89" t="s">
         <v>152</v>
       </c>
-      <c r="C3" s="87"/>
-      <c r="D3" s="87"/>
-      <c r="E3" s="87"/>
-      <c r="F3" s="87"/>
-      <c r="G3" s="87"/>
-      <c r="H3" s="87"/>
-      <c r="I3" s="87"/>
-      <c r="J3" s="87"/>
-      <c r="K3" s="87"/>
-      <c r="L3" s="87"/>
-      <c r="M3" s="87"/>
-      <c r="N3" s="87"/>
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="89"/>
+      <c r="F3" s="89"/>
+      <c r="G3" s="89"/>
+      <c r="H3" s="89"/>
+      <c r="I3" s="89"/>
+      <c r="J3" s="89"/>
+      <c r="K3" s="89"/>
+      <c r="L3" s="89"/>
+      <c r="M3" s="89"/>
+      <c r="N3" s="89"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="74" t="s">
@@ -4022,7 +4064,7 @@
   <dimension ref="B1:J6"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="I40" sqref="I40"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4044,28 +4086,28 @@
       </c>
     </row>
     <row r="2" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="86"/>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="86"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="86"/>
-      <c r="H2" s="86"/>
-      <c r="I2" s="86"/>
-      <c r="J2" s="86"/>
+      <c r="B2" s="88"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="88"/>
+      <c r="G2" s="88"/>
+      <c r="H2" s="88"/>
+      <c r="I2" s="88"/>
+      <c r="J2" s="88"/>
     </row>
     <row r="3" spans="2:10" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="87" t="s">
+      <c r="B3" s="89" t="s">
         <v>155</v>
       </c>
-      <c r="C3" s="87"/>
-      <c r="D3" s="87"/>
-      <c r="E3" s="87"/>
-      <c r="F3" s="87"/>
-      <c r="G3" s="87"/>
-      <c r="H3" s="87"/>
-      <c r="I3" s="87"/>
-      <c r="J3" s="87"/>
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="89"/>
+      <c r="F3" s="89"/>
+      <c r="G3" s="89"/>
+      <c r="H3" s="89"/>
+      <c r="I3" s="89"/>
+      <c r="J3" s="89"/>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" s="74" t="s">
@@ -4118,7 +4160,7 @@
   <dimension ref="B1:N6"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4144,29 +4186,29 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="86"/>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="86"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="86"/>
-      <c r="H2" s="86"/>
-      <c r="I2" s="86"/>
-      <c r="J2" s="86"/>
+      <c r="B2" s="88"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="88"/>
+      <c r="G2" s="88"/>
+      <c r="H2" s="88"/>
+      <c r="I2" s="88"/>
+      <c r="J2" s="88"/>
       <c r="K2" s="85"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="87" t="s">
+      <c r="B3" s="89" t="s">
         <v>156</v>
       </c>
-      <c r="C3" s="87"/>
-      <c r="D3" s="87"/>
-      <c r="E3" s="87"/>
-      <c r="F3" s="87"/>
-      <c r="G3" s="87"/>
-      <c r="H3" s="87"/>
-      <c r="I3" s="87"/>
-      <c r="J3" s="87"/>
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="89"/>
+      <c r="F3" s="89"/>
+      <c r="G3" s="89"/>
+      <c r="H3" s="89"/>
+      <c r="I3" s="89"/>
+      <c r="J3" s="89"/>
       <c r="K3" s="84"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
@@ -4236,6 +4278,137 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:K7"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.85546875" customWidth="1"/>
+    <col min="2" max="2" width="23" customWidth="1"/>
+    <col min="3" max="3" width="38.85546875" customWidth="1"/>
+    <col min="4" max="4" width="12" customWidth="1"/>
+    <col min="5" max="6" width="11.5703125" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" customWidth="1"/>
+    <col min="9" max="9" width="22.7109375" customWidth="1"/>
+    <col min="10" max="10" width="25.85546875" customWidth="1"/>
+    <col min="11" max="11" width="32.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:11" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B1" s="46" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="88"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="88"/>
+      <c r="G2" s="88"/>
+      <c r="H2" s="88"/>
+      <c r="I2" s="88"/>
+      <c r="J2" s="88"/>
+      <c r="K2" s="88"/>
+    </row>
+    <row r="3" spans="2:11" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B3" s="89" t="s">
+        <v>168</v>
+      </c>
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="89"/>
+      <c r="F3" s="89"/>
+      <c r="G3" s="89"/>
+      <c r="H3" s="89"/>
+      <c r="I3" s="89"/>
+      <c r="J3" s="89"/>
+      <c r="K3" s="89"/>
+    </row>
+    <row r="4" spans="2:11" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B4" s="86"/>
+      <c r="C4" s="86"/>
+      <c r="D4" s="86"/>
+      <c r="E4" s="86"/>
+      <c r="F4" s="86"/>
+      <c r="G4" s="86"/>
+      <c r="H4" s="86"/>
+      <c r="I4" s="86"/>
+      <c r="J4" s="86"/>
+      <c r="K4" s="86"/>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="H5" s="91" t="s">
+        <v>176</v>
+      </c>
+      <c r="I5" s="92"/>
+      <c r="J5" s="91" t="s">
+        <v>175</v>
+      </c>
+      <c r="K5" s="92"/>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B6" s="87" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="87" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="87" t="s">
+        <v>169</v>
+      </c>
+      <c r="E6" s="87" t="s">
+        <v>170</v>
+      </c>
+      <c r="F6" s="87" t="s">
+        <v>116</v>
+      </c>
+      <c r="G6" s="87" t="s">
+        <v>116</v>
+      </c>
+      <c r="H6" s="87" t="s">
+        <v>171</v>
+      </c>
+      <c r="I6" s="87" t="s">
+        <v>172</v>
+      </c>
+      <c r="J6" s="87" t="s">
+        <v>173</v>
+      </c>
+      <c r="K6" s="87" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="83"/>
+      <c r="J7" s="83"/>
+      <c r="K7" s="83"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B2:K2"/>
+    <mergeCell ref="B3:K3"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="H5:I5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:Z8"/>
   <sheetViews>
@@ -4259,37 +4432,37 @@
       <c r="Z1" s="38"/>
     </row>
     <row r="2" spans="2:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="86"/>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="86"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="86"/>
-      <c r="H2" s="86"/>
-      <c r="I2" s="86"/>
-      <c r="J2" s="86"/>
-      <c r="K2" s="86"/>
-      <c r="L2" s="86"/>
-      <c r="M2" s="86"/>
-      <c r="N2" s="86"/>
+      <c r="B2" s="88"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="88"/>
+      <c r="G2" s="88"/>
+      <c r="H2" s="88"/>
+      <c r="I2" s="88"/>
+      <c r="J2" s="88"/>
+      <c r="K2" s="88"/>
+      <c r="L2" s="88"/>
+      <c r="M2" s="88"/>
+      <c r="N2" s="88"/>
       <c r="Z2"/>
     </row>
     <row r="3" spans="2:26" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="87" t="s">
+      <c r="B3" s="89" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="87"/>
-      <c r="D3" s="87"/>
-      <c r="E3" s="87"/>
-      <c r="F3" s="87"/>
-      <c r="G3" s="87"/>
-      <c r="H3" s="87"/>
-      <c r="I3" s="87"/>
-      <c r="J3" s="87"/>
-      <c r="K3" s="87"/>
-      <c r="L3" s="87"/>
-      <c r="M3" s="87"/>
-      <c r="N3" s="87"/>
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="89"/>
+      <c r="F3" s="89"/>
+      <c r="G3" s="89"/>
+      <c r="H3" s="89"/>
+      <c r="I3" s="89"/>
+      <c r="J3" s="89"/>
+      <c r="K3" s="89"/>
+      <c r="L3" s="89"/>
+      <c r="M3" s="89"/>
+      <c r="N3" s="89"/>
       <c r="Z3"/>
     </row>
     <row r="5" spans="2:26" x14ac:dyDescent="0.25">
@@ -4369,12 +4542,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:Z8"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="L40" sqref="L40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4393,37 +4566,37 @@
       <c r="Z1" s="38"/>
     </row>
     <row r="2" spans="2:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="86"/>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="86"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="86"/>
-      <c r="H2" s="86"/>
-      <c r="I2" s="86"/>
-      <c r="J2" s="86"/>
-      <c r="K2" s="86"/>
-      <c r="L2" s="86"/>
-      <c r="M2" s="86"/>
-      <c r="N2" s="86"/>
+      <c r="B2" s="88"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="88"/>
+      <c r="G2" s="88"/>
+      <c r="H2" s="88"/>
+      <c r="I2" s="88"/>
+      <c r="J2" s="88"/>
+      <c r="K2" s="88"/>
+      <c r="L2" s="88"/>
+      <c r="M2" s="88"/>
+      <c r="N2" s="88"/>
       <c r="Z2"/>
     </row>
     <row r="3" spans="2:26" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="100" t="s">
+      <c r="B3" s="89" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="100"/>
-      <c r="D3" s="100"/>
-      <c r="E3" s="100"/>
-      <c r="F3" s="100"/>
-      <c r="G3" s="100"/>
-      <c r="H3" s="100"/>
-      <c r="I3" s="100"/>
-      <c r="J3" s="100"/>
-      <c r="K3" s="100"/>
-      <c r="L3" s="100"/>
-      <c r="M3" s="100"/>
-      <c r="N3" s="100"/>
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="89"/>
+      <c r="F3" s="89"/>
+      <c r="G3" s="89"/>
+      <c r="H3" s="89"/>
+      <c r="I3" s="89"/>
+      <c r="J3" s="89"/>
+      <c r="K3" s="89"/>
+      <c r="L3" s="89"/>
+      <c r="M3" s="89"/>
+      <c r="N3" s="89"/>
       <c r="Z3"/>
     </row>
     <row r="5" spans="2:26" x14ac:dyDescent="0.25">
@@ -4442,9 +4615,9 @@
       <c r="C6" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="D6" s="97"/>
-      <c r="E6" s="98"/>
-      <c r="F6" s="99"/>
+      <c r="D6" s="93"/>
+      <c r="E6" s="94"/>
+      <c r="F6" s="95"/>
       <c r="G6" s="50"/>
       <c r="H6" s="50"/>
     </row>
@@ -4487,9 +4660,10 @@
       <c r="I8" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="B2:N2"/>
     <mergeCell ref="B3:N3"/>
+    <mergeCell ref="D6:F6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -4497,7 +4671,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:Z8"/>
   <sheetViews>
@@ -4521,37 +4695,37 @@
       <c r="Z1" s="38"/>
     </row>
     <row r="2" spans="2:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="86"/>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="86"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="86"/>
-      <c r="H2" s="86"/>
-      <c r="I2" s="86"/>
-      <c r="J2" s="86"/>
-      <c r="K2" s="86"/>
-      <c r="L2" s="86"/>
-      <c r="M2" s="86"/>
-      <c r="N2" s="86"/>
+      <c r="B2" s="88"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="88"/>
+      <c r="G2" s="88"/>
+      <c r="H2" s="88"/>
+      <c r="I2" s="88"/>
+      <c r="J2" s="88"/>
+      <c r="K2" s="88"/>
+      <c r="L2" s="88"/>
+      <c r="M2" s="88"/>
+      <c r="N2" s="88"/>
       <c r="Z2"/>
     </row>
     <row r="3" spans="2:26" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="87" t="s">
+      <c r="B3" s="89" t="s">
         <v>93</v>
       </c>
-      <c r="C3" s="87"/>
-      <c r="D3" s="87"/>
-      <c r="E3" s="87"/>
-      <c r="F3" s="87"/>
-      <c r="G3" s="87"/>
-      <c r="H3" s="87"/>
-      <c r="I3" s="87"/>
-      <c r="J3" s="87"/>
-      <c r="K3" s="87"/>
-      <c r="L3" s="87"/>
-      <c r="M3" s="87"/>
-      <c r="N3" s="87"/>
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="89"/>
+      <c r="F3" s="89"/>
+      <c r="G3" s="89"/>
+      <c r="H3" s="89"/>
+      <c r="I3" s="89"/>
+      <c r="J3" s="89"/>
+      <c r="K3" s="89"/>
+      <c r="L3" s="89"/>
+      <c r="M3" s="89"/>
+      <c r="N3" s="89"/>
       <c r="Z3"/>
     </row>
     <row r="5" spans="2:26" x14ac:dyDescent="0.25">
@@ -4622,7 +4796,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:Z8"/>
   <sheetViews>
@@ -4644,37 +4818,37 @@
       <c r="Z1" s="38"/>
     </row>
     <row r="2" spans="2:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="86"/>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="86"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="86"/>
-      <c r="H2" s="86"/>
-      <c r="I2" s="86"/>
-      <c r="J2" s="86"/>
-      <c r="K2" s="86"/>
-      <c r="L2" s="86"/>
-      <c r="M2" s="86"/>
-      <c r="N2" s="86"/>
+      <c r="B2" s="88"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="88"/>
+      <c r="G2" s="88"/>
+      <c r="H2" s="88"/>
+      <c r="I2" s="88"/>
+      <c r="J2" s="88"/>
+      <c r="K2" s="88"/>
+      <c r="L2" s="88"/>
+      <c r="M2" s="88"/>
+      <c r="N2" s="88"/>
       <c r="Z2"/>
     </row>
     <row r="3" spans="2:26" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="87" t="s">
+      <c r="B3" s="89" t="s">
         <v>72</v>
       </c>
-      <c r="C3" s="87"/>
-      <c r="D3" s="87"/>
-      <c r="E3" s="87"/>
-      <c r="F3" s="87"/>
-      <c r="G3" s="87"/>
-      <c r="H3" s="87"/>
-      <c r="I3" s="87"/>
-      <c r="J3" s="87"/>
-      <c r="K3" s="87"/>
-      <c r="L3" s="87"/>
-      <c r="M3" s="87"/>
-      <c r="N3" s="87"/>
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="89"/>
+      <c r="F3" s="89"/>
+      <c r="G3" s="89"/>
+      <c r="H3" s="89"/>
+      <c r="I3" s="89"/>
+      <c r="J3" s="89"/>
+      <c r="K3" s="89"/>
+      <c r="L3" s="89"/>
+      <c r="M3" s="89"/>
+      <c r="N3" s="89"/>
       <c r="Z3"/>
     </row>
     <row r="5" spans="2:26" x14ac:dyDescent="0.25">
@@ -4752,12 +4926,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:Q7"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="I40" sqref="I40"/>
+      <selection activeCell="M5" sqref="M5:O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4787,56 +4961,56 @@
       </c>
     </row>
     <row r="2" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="86"/>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="86"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="86"/>
-      <c r="H2" s="86"/>
-      <c r="I2" s="86"/>
-      <c r="J2" s="86"/>
-      <c r="K2" s="86"/>
-      <c r="L2" s="86"/>
+      <c r="B2" s="88"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="88"/>
+      <c r="G2" s="88"/>
+      <c r="H2" s="88"/>
+      <c r="I2" s="88"/>
+      <c r="J2" s="88"/>
+      <c r="K2" s="88"/>
+      <c r="L2" s="88"/>
     </row>
     <row r="3" spans="2:17" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="87" t="s">
+      <c r="B3" s="89" t="s">
         <v>108</v>
       </c>
-      <c r="C3" s="87"/>
-      <c r="D3" s="87"/>
-      <c r="E3" s="87"/>
-      <c r="F3" s="87"/>
-      <c r="G3" s="87"/>
-      <c r="H3" s="87"/>
-      <c r="I3" s="87"/>
-      <c r="J3" s="87"/>
-      <c r="K3" s="87"/>
-      <c r="L3" s="87"/>
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="89"/>
+      <c r="F3" s="89"/>
+      <c r="G3" s="89"/>
+      <c r="H3" s="89"/>
+      <c r="I3" s="89"/>
+      <c r="J3" s="89"/>
+      <c r="K3" s="89"/>
+      <c r="L3" s="89"/>
     </row>
     <row r="5" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D5" s="89" t="s">
+      <c r="D5" s="96" t="s">
         <v>123</v>
       </c>
-      <c r="E5" s="89"/>
+      <c r="E5" s="96"/>
       <c r="F5" s="73"/>
       <c r="G5" s="73"/>
       <c r="H5" s="73"/>
       <c r="I5" s="73"/>
-      <c r="J5" s="89" t="s">
+      <c r="J5" s="96" t="s">
         <v>42</v>
       </c>
-      <c r="K5" s="89"/>
-      <c r="L5" s="89"/>
-      <c r="M5" s="89" t="s">
+      <c r="K5" s="96"/>
+      <c r="L5" s="96"/>
+      <c r="M5" s="96" t="s">
         <v>130</v>
       </c>
-      <c r="N5" s="89"/>
-      <c r="O5" s="89"/>
-      <c r="P5" s="88" t="s">
+      <c r="N5" s="96"/>
+      <c r="O5" s="96"/>
+      <c r="P5" s="90" t="s">
         <v>109</v>
       </c>
-      <c r="Q5" s="88"/>
+      <c r="Q5" s="90"/>
     </row>
     <row r="6" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="70" t="s">
@@ -4919,7 +5093,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:X8"/>
   <sheetViews>
@@ -4957,108 +5131,108 @@
       </c>
     </row>
     <row r="2" spans="2:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="86"/>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="86"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="86"/>
-      <c r="H2" s="86"/>
-      <c r="I2" s="86"/>
-      <c r="J2" s="86"/>
-      <c r="K2" s="86"/>
-      <c r="L2" s="86"/>
-      <c r="M2" s="86"/>
-      <c r="N2" s="86"/>
-      <c r="O2" s="86"/>
-      <c r="P2" s="86"/>
+      <c r="B2" s="88"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="88"/>
+      <c r="G2" s="88"/>
+      <c r="H2" s="88"/>
+      <c r="I2" s="88"/>
+      <c r="J2" s="88"/>
+      <c r="K2" s="88"/>
+      <c r="L2" s="88"/>
+      <c r="M2" s="88"/>
+      <c r="N2" s="88"/>
+      <c r="O2" s="88"/>
+      <c r="P2" s="88"/>
       <c r="Q2" s="56"/>
       <c r="R2" s="56"/>
     </row>
     <row r="3" spans="2:24" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="87" t="s">
+      <c r="B3" s="89" t="s">
         <v>111</v>
       </c>
-      <c r="C3" s="87"/>
-      <c r="D3" s="87"/>
-      <c r="E3" s="87"/>
-      <c r="F3" s="87"/>
-      <c r="G3" s="87"/>
-      <c r="H3" s="87"/>
-      <c r="I3" s="87"/>
-      <c r="J3" s="87"/>
-      <c r="K3" s="87"/>
-      <c r="L3" s="87"/>
-      <c r="M3" s="87"/>
-      <c r="N3" s="87"/>
-      <c r="O3" s="87"/>
-      <c r="P3" s="87"/>
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="89"/>
+      <c r="F3" s="89"/>
+      <c r="G3" s="89"/>
+      <c r="H3" s="89"/>
+      <c r="I3" s="89"/>
+      <c r="J3" s="89"/>
+      <c r="K3" s="89"/>
+      <c r="L3" s="89"/>
+      <c r="M3" s="89"/>
+      <c r="N3" s="89"/>
+      <c r="O3" s="89"/>
+      <c r="P3" s="89"/>
       <c r="Q3" s="57"/>
       <c r="R3" s="57"/>
     </row>
     <row r="5" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B5" s="90" t="s">
+      <c r="B5" s="97" t="s">
         <v>112</v>
       </c>
-      <c r="C5" s="91"/>
-      <c r="D5" s="91"/>
-      <c r="E5" s="91"/>
-      <c r="F5" s="91"/>
-      <c r="G5" s="91"/>
-      <c r="H5" s="91"/>
-      <c r="I5" s="91"/>
-      <c r="J5" s="91"/>
-      <c r="K5" s="91"/>
-      <c r="L5" s="92"/>
-      <c r="M5" s="90" t="s">
+      <c r="C5" s="99"/>
+      <c r="D5" s="99"/>
+      <c r="E5" s="99"/>
+      <c r="F5" s="99"/>
+      <c r="G5" s="99"/>
+      <c r="H5" s="99"/>
+      <c r="I5" s="99"/>
+      <c r="J5" s="99"/>
+      <c r="K5" s="99"/>
+      <c r="L5" s="98"/>
+      <c r="M5" s="97" t="s">
         <v>113</v>
       </c>
-      <c r="N5" s="91"/>
-      <c r="O5" s="91"/>
-      <c r="P5" s="91"/>
-      <c r="Q5" s="91"/>
-      <c r="R5" s="91"/>
-      <c r="S5" s="91"/>
-      <c r="T5" s="91"/>
-      <c r="U5" s="91"/>
-      <c r="V5" s="91"/>
-      <c r="W5" s="91"/>
-      <c r="X5" s="92"/>
+      <c r="N5" s="99"/>
+      <c r="O5" s="99"/>
+      <c r="P5" s="99"/>
+      <c r="Q5" s="99"/>
+      <c r="R5" s="99"/>
+      <c r="S5" s="99"/>
+      <c r="T5" s="99"/>
+      <c r="U5" s="99"/>
+      <c r="V5" s="99"/>
+      <c r="W5" s="99"/>
+      <c r="X5" s="98"/>
     </row>
     <row r="6" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B6" s="93"/>
-      <c r="C6" s="93"/>
-      <c r="D6" s="93"/>
-      <c r="E6" s="93"/>
-      <c r="F6" s="94" t="s">
+      <c r="B6" s="100"/>
+      <c r="C6" s="100"/>
+      <c r="D6" s="100"/>
+      <c r="E6" s="100"/>
+      <c r="F6" s="101" t="s">
         <v>27</v>
       </c>
-      <c r="G6" s="95"/>
-      <c r="H6" s="95"/>
-      <c r="I6" s="96"/>
-      <c r="J6" s="90" t="s">
+      <c r="G6" s="102"/>
+      <c r="H6" s="102"/>
+      <c r="I6" s="103"/>
+      <c r="J6" s="97" t="s">
         <v>30</v>
       </c>
-      <c r="K6" s="91"/>
-      <c r="L6" s="92"/>
+      <c r="K6" s="99"/>
+      <c r="L6" s="98"/>
       <c r="M6" s="76"/>
-      <c r="N6" s="90" t="s">
+      <c r="N6" s="97" t="s">
         <v>42</v>
       </c>
-      <c r="O6" s="92"/>
-      <c r="P6" s="90" t="s">
+      <c r="O6" s="98"/>
+      <c r="P6" s="97" t="s">
         <v>106</v>
       </c>
-      <c r="Q6" s="91"/>
-      <c r="R6" s="92"/>
+      <c r="Q6" s="99"/>
+      <c r="R6" s="98"/>
       <c r="S6" s="76"/>
-      <c r="T6" s="90" t="s">
+      <c r="T6" s="97" t="s">
         <v>123</v>
       </c>
-      <c r="U6" s="92"/>
-      <c r="V6" s="93"/>
-      <c r="W6" s="93"/>
-      <c r="X6" s="93"/>
+      <c r="U6" s="98"/>
+      <c r="V6" s="100"/>
+      <c r="W6" s="100"/>
+      <c r="X6" s="100"/>
     </row>
     <row r="7" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B7" s="75" t="s">
@@ -5158,9 +5332,6 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="M5:X5"/>
-    <mergeCell ref="T6:U6"/>
-    <mergeCell ref="V6:X6"/>
     <mergeCell ref="B2:P2"/>
     <mergeCell ref="B3:P3"/>
     <mergeCell ref="B5:L5"/>
@@ -5169,96 +5340,11 @@
     <mergeCell ref="N6:O6"/>
     <mergeCell ref="P6:R6"/>
     <mergeCell ref="B6:E6"/>
+    <mergeCell ref="M5:X5"/>
+    <mergeCell ref="T6:U6"/>
+    <mergeCell ref="V6:X6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A24"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="14"/>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="15"/>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="16"/>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="17"/>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="18"/>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="19"/>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="20"/>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="21"/>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="22"/>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="23"/>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="24"/>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="25"/>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" s="26"/>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" s="27"/>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" s="28"/>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" s="29"/>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="30"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="31"/>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="32"/>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="33"/>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="34"/>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="35"/>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="36"/>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="37"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5289,36 +5375,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="86"/>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="86"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="86"/>
-      <c r="H2" s="86"/>
-      <c r="I2" s="86"/>
-      <c r="J2" s="86"/>
-      <c r="K2" s="86"/>
-      <c r="L2" s="86"/>
-      <c r="M2" s="86"/>
-      <c r="N2" s="86"/>
+      <c r="B2" s="88"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="88"/>
+      <c r="G2" s="88"/>
+      <c r="H2" s="88"/>
+      <c r="I2" s="88"/>
+      <c r="J2" s="88"/>
+      <c r="K2" s="88"/>
+      <c r="L2" s="88"/>
+      <c r="M2" s="88"/>
+      <c r="N2" s="88"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="87" t="s">
+      <c r="B3" s="89" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="87"/>
-      <c r="D3" s="87"/>
-      <c r="E3" s="87"/>
-      <c r="F3" s="87"/>
-      <c r="G3" s="87"/>
-      <c r="H3" s="87"/>
-      <c r="I3" s="87"/>
-      <c r="J3" s="87"/>
-      <c r="K3" s="87"/>
-      <c r="L3" s="87"/>
-      <c r="M3" s="87"/>
-      <c r="N3" s="87"/>
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="89"/>
+      <c r="F3" s="89"/>
+      <c r="G3" s="89"/>
+      <c r="H3" s="89"/>
+      <c r="I3" s="89"/>
+      <c r="J3" s="89"/>
+      <c r="K3" s="89"/>
+      <c r="L3" s="89"/>
+      <c r="M3" s="89"/>
+      <c r="N3" s="89"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="44" t="s">
@@ -5356,6 +5442,94 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="14"/>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="15"/>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="16"/>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="17"/>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="18"/>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="19"/>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="20"/>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="21"/>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="22"/>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="23"/>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="24"/>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="25"/>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="26"/>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="27"/>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="28"/>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="29"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="30"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="31"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="32"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="33"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="34"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="35"/>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="36"/>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="37"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5385,40 +5559,40 @@
       </c>
     </row>
     <row r="2" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="86"/>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="86"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="86"/>
-      <c r="H2" s="86"/>
-      <c r="I2" s="86"/>
-      <c r="J2" s="86"/>
-      <c r="K2" s="86"/>
-      <c r="L2" s="86"/>
-      <c r="M2" s="86"/>
-      <c r="N2" s="86"/>
-      <c r="O2" s="86"/>
-      <c r="P2" s="86"/>
+      <c r="B2" s="88"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="88"/>
+      <c r="G2" s="88"/>
+      <c r="H2" s="88"/>
+      <c r="I2" s="88"/>
+      <c r="J2" s="88"/>
+      <c r="K2" s="88"/>
+      <c r="L2" s="88"/>
+      <c r="M2" s="88"/>
+      <c r="N2" s="88"/>
+      <c r="O2" s="88"/>
+      <c r="P2" s="88"/>
     </row>
     <row r="3" spans="2:16" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="87" t="s">
+      <c r="B3" s="89" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="87"/>
-      <c r="D3" s="87"/>
-      <c r="E3" s="87"/>
-      <c r="F3" s="87"/>
-      <c r="G3" s="87"/>
-      <c r="H3" s="87"/>
-      <c r="I3" s="87"/>
-      <c r="J3" s="87"/>
-      <c r="K3" s="87"/>
-      <c r="L3" s="87"/>
-      <c r="M3" s="87"/>
-      <c r="N3" s="87"/>
-      <c r="O3" s="87"/>
-      <c r="P3" s="87"/>
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="89"/>
+      <c r="F3" s="89"/>
+      <c r="G3" s="89"/>
+      <c r="H3" s="89"/>
+      <c r="I3" s="89"/>
+      <c r="J3" s="89"/>
+      <c r="K3" s="89"/>
+      <c r="L3" s="89"/>
+      <c r="M3" s="89"/>
+      <c r="N3" s="89"/>
+      <c r="O3" s="89"/>
+      <c r="P3" s="89"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="44" t="s">
@@ -5497,40 +5671,40 @@
       </c>
     </row>
     <row r="2" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="86"/>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="86"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="86"/>
-      <c r="H2" s="86"/>
-      <c r="I2" s="86"/>
-      <c r="J2" s="86"/>
-      <c r="K2" s="86"/>
-      <c r="L2" s="86"/>
-      <c r="M2" s="86"/>
-      <c r="N2" s="86"/>
-      <c r="O2" s="86"/>
-      <c r="P2" s="86"/>
+      <c r="B2" s="88"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="88"/>
+      <c r="G2" s="88"/>
+      <c r="H2" s="88"/>
+      <c r="I2" s="88"/>
+      <c r="J2" s="88"/>
+      <c r="K2" s="88"/>
+      <c r="L2" s="88"/>
+      <c r="M2" s="88"/>
+      <c r="N2" s="88"/>
+      <c r="O2" s="88"/>
+      <c r="P2" s="88"/>
     </row>
     <row r="3" spans="2:16" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="87" t="s">
+      <c r="B3" s="89" t="s">
         <v>68</v>
       </c>
-      <c r="C3" s="87"/>
-      <c r="D3" s="87"/>
-      <c r="E3" s="87"/>
-      <c r="F3" s="87"/>
-      <c r="G3" s="87"/>
-      <c r="H3" s="87"/>
-      <c r="I3" s="87"/>
-      <c r="J3" s="87"/>
-      <c r="K3" s="87"/>
-      <c r="L3" s="87"/>
-      <c r="M3" s="87"/>
-      <c r="N3" s="87"/>
-      <c r="O3" s="87"/>
-      <c r="P3" s="87"/>
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="89"/>
+      <c r="F3" s="89"/>
+      <c r="G3" s="89"/>
+      <c r="H3" s="89"/>
+      <c r="I3" s="89"/>
+      <c r="J3" s="89"/>
+      <c r="K3" s="89"/>
+      <c r="L3" s="89"/>
+      <c r="M3" s="89"/>
+      <c r="N3" s="89"/>
+      <c r="O3" s="89"/>
+      <c r="P3" s="89"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
@@ -5579,40 +5753,40 @@
       </c>
     </row>
     <row r="2" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="86"/>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="86"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="86"/>
-      <c r="H2" s="86"/>
-      <c r="I2" s="86"/>
-      <c r="J2" s="86"/>
-      <c r="K2" s="86"/>
-      <c r="L2" s="86"/>
-      <c r="M2" s="86"/>
-      <c r="N2" s="86"/>
-      <c r="O2" s="86"/>
-      <c r="P2" s="86"/>
+      <c r="B2" s="88"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="88"/>
+      <c r="G2" s="88"/>
+      <c r="H2" s="88"/>
+      <c r="I2" s="88"/>
+      <c r="J2" s="88"/>
+      <c r="K2" s="88"/>
+      <c r="L2" s="88"/>
+      <c r="M2" s="88"/>
+      <c r="N2" s="88"/>
+      <c r="O2" s="88"/>
+      <c r="P2" s="88"/>
     </row>
     <row r="3" spans="2:16" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="87" t="s">
+      <c r="B3" s="89" t="s">
         <v>71</v>
       </c>
-      <c r="C3" s="87"/>
-      <c r="D3" s="87"/>
-      <c r="E3" s="87"/>
-      <c r="F3" s="87"/>
-      <c r="G3" s="87"/>
-      <c r="H3" s="87"/>
-      <c r="I3" s="87"/>
-      <c r="J3" s="87"/>
-      <c r="K3" s="87"/>
-      <c r="L3" s="87"/>
-      <c r="M3" s="87"/>
-      <c r="N3" s="87"/>
-      <c r="O3" s="87"/>
-      <c r="P3" s="87"/>
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="89"/>
+      <c r="F3" s="89"/>
+      <c r="G3" s="89"/>
+      <c r="H3" s="89"/>
+      <c r="I3" s="89"/>
+      <c r="J3" s="89"/>
+      <c r="K3" s="89"/>
+      <c r="L3" s="89"/>
+      <c r="M3" s="89"/>
+      <c r="N3" s="89"/>
+      <c r="O3" s="89"/>
+      <c r="P3" s="89"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
@@ -5666,36 +5840,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="86"/>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="86"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="86"/>
-      <c r="H2" s="86"/>
-      <c r="I2" s="86"/>
-      <c r="J2" s="86"/>
-      <c r="K2" s="86"/>
-      <c r="L2" s="86"/>
-      <c r="M2" s="86"/>
-      <c r="N2" s="86"/>
+      <c r="B2" s="88"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="88"/>
+      <c r="G2" s="88"/>
+      <c r="H2" s="88"/>
+      <c r="I2" s="88"/>
+      <c r="J2" s="88"/>
+      <c r="K2" s="88"/>
+      <c r="L2" s="88"/>
+      <c r="M2" s="88"/>
+      <c r="N2" s="88"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="87" t="s">
+      <c r="B3" s="89" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="87"/>
-      <c r="D3" s="87"/>
-      <c r="E3" s="87"/>
-      <c r="F3" s="87"/>
-      <c r="G3" s="87"/>
-      <c r="H3" s="87"/>
-      <c r="I3" s="87"/>
-      <c r="J3" s="87"/>
-      <c r="K3" s="87"/>
-      <c r="L3" s="87"/>
-      <c r="M3" s="87"/>
-      <c r="N3" s="87"/>
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="89"/>
+      <c r="F3" s="89"/>
+      <c r="G3" s="89"/>
+      <c r="H3" s="89"/>
+      <c r="I3" s="89"/>
+      <c r="J3" s="89"/>
+      <c r="K3" s="89"/>
+      <c r="L3" s="89"/>
+      <c r="M3" s="89"/>
+      <c r="N3" s="89"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="44" t="s">
@@ -5784,40 +5958,40 @@
       </c>
     </row>
     <row r="2" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="86"/>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="86"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="86"/>
-      <c r="H2" s="86"/>
-      <c r="I2" s="86"/>
-      <c r="J2" s="86"/>
-      <c r="K2" s="86"/>
-      <c r="L2" s="86"/>
-      <c r="M2" s="86"/>
-      <c r="N2" s="86"/>
-      <c r="O2" s="86"/>
-      <c r="P2" s="86"/>
+      <c r="B2" s="88"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="88"/>
+      <c r="G2" s="88"/>
+      <c r="H2" s="88"/>
+      <c r="I2" s="88"/>
+      <c r="J2" s="88"/>
+      <c r="K2" s="88"/>
+      <c r="L2" s="88"/>
+      <c r="M2" s="88"/>
+      <c r="N2" s="88"/>
+      <c r="O2" s="88"/>
+      <c r="P2" s="88"/>
     </row>
     <row r="3" spans="2:16" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="87" t="s">
+      <c r="B3" s="89" t="s">
         <v>65</v>
       </c>
-      <c r="C3" s="87"/>
-      <c r="D3" s="87"/>
-      <c r="E3" s="87"/>
-      <c r="F3" s="87"/>
-      <c r="G3" s="87"/>
-      <c r="H3" s="87"/>
-      <c r="I3" s="87"/>
-      <c r="J3" s="87"/>
-      <c r="K3" s="87"/>
-      <c r="L3" s="87"/>
-      <c r="M3" s="87"/>
-      <c r="N3" s="87"/>
-      <c r="O3" s="87"/>
-      <c r="P3" s="87"/>
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="89"/>
+      <c r="F3" s="89"/>
+      <c r="G3" s="89"/>
+      <c r="H3" s="89"/>
+      <c r="I3" s="89"/>
+      <c r="J3" s="89"/>
+      <c r="K3" s="89"/>
+      <c r="L3" s="89"/>
+      <c r="M3" s="89"/>
+      <c r="N3" s="89"/>
+      <c r="O3" s="89"/>
+      <c r="P3" s="89"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="45" t="s">
@@ -5869,36 +6043,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="86"/>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="86"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="86"/>
-      <c r="H2" s="86"/>
-      <c r="I2" s="86"/>
-      <c r="J2" s="86"/>
-      <c r="K2" s="86"/>
-      <c r="L2" s="86"/>
-      <c r="M2" s="86"/>
-      <c r="N2" s="86"/>
+      <c r="B2" s="88"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="88"/>
+      <c r="G2" s="88"/>
+      <c r="H2" s="88"/>
+      <c r="I2" s="88"/>
+      <c r="J2" s="88"/>
+      <c r="K2" s="88"/>
+      <c r="L2" s="88"/>
+      <c r="M2" s="88"/>
+      <c r="N2" s="88"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="87" t="s">
+      <c r="B3" s="89" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="87"/>
-      <c r="D3" s="87"/>
-      <c r="E3" s="87"/>
-      <c r="F3" s="87"/>
-      <c r="G3" s="87"/>
-      <c r="H3" s="87"/>
-      <c r="I3" s="87"/>
-      <c r="J3" s="87"/>
-      <c r="K3" s="87"/>
-      <c r="L3" s="87"/>
-      <c r="M3" s="87"/>
-      <c r="N3" s="87"/>
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="89"/>
+      <c r="F3" s="89"/>
+      <c r="G3" s="89"/>
+      <c r="H3" s="89"/>
+      <c r="I3" s="89"/>
+      <c r="J3" s="89"/>
+      <c r="K3" s="89"/>
+      <c r="L3" s="89"/>
+      <c r="M3" s="89"/>
+      <c r="N3" s="89"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">

</xml_diff>

<commit_message>
TRIEDA-1641 - Adicionando novas colunas no export excel do Atendimentos por Faixa de Demanda. Consertando bug nas colunas de demanda acumulada.
</commit_message>
<xml_diff>
--- a/code/client/web/src/main/resources/templateExport.xlsx
+++ b/code/client/web/src/main/resources/templateExport.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="17070" windowHeight="5370" tabRatio="797" firstSheet="21" activeTab="22"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="17070" windowHeight="5370" tabRatio="797" firstSheet="16" activeTab="21"/>
   </bookViews>
   <sheets>
     <sheet name="Campi" sheetId="3" r:id="rId1"/>
@@ -1215,7 +1215,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="183">
   <si>
     <t>Planilha de Unidades</t>
   </si>
@@ -1746,14 +1746,33 @@
   </si>
   <si>
     <t>ALOCAÇÃO</t>
+  </si>
+  <si>
+    <t>Receita Semanal</t>
+  </si>
+  <si>
+    <t>Custo Docente Semanal</t>
+  </si>
+  <si>
+    <t>Receita Acum</t>
+  </si>
+  <si>
+    <t>Custo Docente Acumulado</t>
+  </si>
+  <si>
+    <t>Custo Docente / Receita Acum %</t>
+  </si>
+  <si>
+    <t>Custo Docente / Receita %</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="165" formatCode="&quot;R$&quot;\ #,##0.00"/>
+    <numFmt numFmtId="173" formatCode="0.0000"/>
   </numFmts>
   <fonts count="14" x14ac:knownFonts="1">
     <font>
@@ -2138,7 +2157,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2385,6 +2404,9 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2415,23 +2437,26 @@
     <xf numFmtId="0" fontId="8" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="28" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="28" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="28" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="173" fontId="6" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2760,38 +2785,38 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="88" t="s">
+      <c r="B2" s="89" t="s">
         <v>96</v>
       </c>
-      <c r="C2" s="88"/>
-      <c r="D2" s="88"/>
-      <c r="E2" s="88"/>
-      <c r="F2" s="88"/>
-      <c r="G2" s="88"/>
-      <c r="H2" s="88"/>
-      <c r="I2" s="88"/>
-      <c r="J2" s="88"/>
-      <c r="K2" s="88"/>
-      <c r="L2" s="88"/>
-      <c r="M2" s="88"/>
-      <c r="N2" s="88"/>
+      <c r="C2" s="89"/>
+      <c r="D2" s="89"/>
+      <c r="E2" s="89"/>
+      <c r="F2" s="89"/>
+      <c r="G2" s="89"/>
+      <c r="H2" s="89"/>
+      <c r="I2" s="89"/>
+      <c r="J2" s="89"/>
+      <c r="K2" s="89"/>
+      <c r="L2" s="89"/>
+      <c r="M2" s="89"/>
+      <c r="N2" s="89"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="89" t="s">
+      <c r="B3" s="90" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="89"/>
-      <c r="D3" s="89"/>
-      <c r="E3" s="89"/>
-      <c r="F3" s="89"/>
-      <c r="G3" s="89"/>
-      <c r="H3" s="89"/>
-      <c r="I3" s="89"/>
-      <c r="J3" s="89"/>
-      <c r="K3" s="89"/>
-      <c r="L3" s="89"/>
-      <c r="M3" s="89"/>
-      <c r="N3" s="89"/>
+      <c r="C3" s="90"/>
+      <c r="D3" s="90"/>
+      <c r="E3" s="90"/>
+      <c r="F3" s="90"/>
+      <c r="G3" s="90"/>
+      <c r="H3" s="90"/>
+      <c r="I3" s="90"/>
+      <c r="J3" s="90"/>
+      <c r="K3" s="90"/>
+      <c r="L3" s="90"/>
+      <c r="M3" s="90"/>
+      <c r="N3" s="90"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="44" t="s">
@@ -2859,36 +2884,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="88"/>
-      <c r="C2" s="88"/>
-      <c r="D2" s="88"/>
-      <c r="E2" s="88"/>
-      <c r="F2" s="88"/>
-      <c r="G2" s="88"/>
-      <c r="H2" s="88"/>
-      <c r="I2" s="88"/>
-      <c r="J2" s="88"/>
-      <c r="K2" s="88"/>
-      <c r="L2" s="88"/>
-      <c r="M2" s="88"/>
-      <c r="N2" s="88"/>
+      <c r="B2" s="89"/>
+      <c r="C2" s="89"/>
+      <c r="D2" s="89"/>
+      <c r="E2" s="89"/>
+      <c r="F2" s="89"/>
+      <c r="G2" s="89"/>
+      <c r="H2" s="89"/>
+      <c r="I2" s="89"/>
+      <c r="J2" s="89"/>
+      <c r="K2" s="89"/>
+      <c r="L2" s="89"/>
+      <c r="M2" s="89"/>
+      <c r="N2" s="89"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="89" t="s">
+      <c r="B3" s="90" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="89"/>
-      <c r="D3" s="89"/>
-      <c r="E3" s="89"/>
-      <c r="F3" s="89"/>
-      <c r="G3" s="89"/>
-      <c r="H3" s="89"/>
-      <c r="I3" s="89"/>
-      <c r="J3" s="89"/>
-      <c r="K3" s="89"/>
-      <c r="L3" s="89"/>
-      <c r="M3" s="89"/>
-      <c r="N3" s="89"/>
+      <c r="C3" s="90"/>
+      <c r="D3" s="90"/>
+      <c r="E3" s="90"/>
+      <c r="F3" s="90"/>
+      <c r="G3" s="90"/>
+      <c r="H3" s="90"/>
+      <c r="I3" s="90"/>
+      <c r="J3" s="90"/>
+      <c r="K3" s="90"/>
+      <c r="L3" s="90"/>
+      <c r="M3" s="90"/>
+      <c r="N3" s="90"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -2957,36 +2982,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="88"/>
-      <c r="C2" s="88"/>
-      <c r="D2" s="88"/>
-      <c r="E2" s="88"/>
-      <c r="F2" s="88"/>
-      <c r="G2" s="88"/>
-      <c r="H2" s="88"/>
-      <c r="I2" s="88"/>
-      <c r="J2" s="88"/>
-      <c r="K2" s="88"/>
-      <c r="L2" s="88"/>
-      <c r="M2" s="88"/>
-      <c r="N2" s="88"/>
+      <c r="B2" s="89"/>
+      <c r="C2" s="89"/>
+      <c r="D2" s="89"/>
+      <c r="E2" s="89"/>
+      <c r="F2" s="89"/>
+      <c r="G2" s="89"/>
+      <c r="H2" s="89"/>
+      <c r="I2" s="89"/>
+      <c r="J2" s="89"/>
+      <c r="K2" s="89"/>
+      <c r="L2" s="89"/>
+      <c r="M2" s="89"/>
+      <c r="N2" s="89"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="89" t="s">
+      <c r="B3" s="90" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="89"/>
-      <c r="D3" s="89"/>
-      <c r="E3" s="89"/>
-      <c r="F3" s="89"/>
-      <c r="G3" s="89"/>
-      <c r="H3" s="89"/>
-      <c r="I3" s="89"/>
-      <c r="J3" s="89"/>
-      <c r="K3" s="89"/>
-      <c r="L3" s="89"/>
-      <c r="M3" s="89"/>
-      <c r="N3" s="89"/>
+      <c r="C3" s="90"/>
+      <c r="D3" s="90"/>
+      <c r="E3" s="90"/>
+      <c r="F3" s="90"/>
+      <c r="G3" s="90"/>
+      <c r="H3" s="90"/>
+      <c r="I3" s="90"/>
+      <c r="J3" s="90"/>
+      <c r="K3" s="90"/>
+      <c r="L3" s="90"/>
+      <c r="M3" s="90"/>
+      <c r="N3" s="90"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -3071,18 +3096,18 @@
       </c>
     </row>
     <row r="2" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="88"/>
-      <c r="C2" s="88"/>
-      <c r="D2" s="88"/>
-      <c r="E2" s="88"/>
+      <c r="B2" s="89"/>
+      <c r="C2" s="89"/>
+      <c r="D2" s="89"/>
+      <c r="E2" s="89"/>
     </row>
     <row r="3" spans="2:5" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="89" t="s">
+      <c r="B3" s="90" t="s">
         <v>126</v>
       </c>
-      <c r="C3" s="89"/>
-      <c r="D3" s="89"/>
-      <c r="E3" s="89"/>
+      <c r="C3" s="90"/>
+      <c r="D3" s="90"/>
+      <c r="E3" s="90"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="60" t="s">
@@ -3135,36 +3160,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="88"/>
-      <c r="C2" s="88"/>
-      <c r="D2" s="88"/>
-      <c r="E2" s="88"/>
-      <c r="F2" s="88"/>
-      <c r="G2" s="88"/>
-      <c r="H2" s="88"/>
-      <c r="I2" s="88"/>
-      <c r="J2" s="88"/>
-      <c r="K2" s="88"/>
-      <c r="L2" s="88"/>
-      <c r="M2" s="88"/>
-      <c r="N2" s="88"/>
+      <c r="B2" s="89"/>
+      <c r="C2" s="89"/>
+      <c r="D2" s="89"/>
+      <c r="E2" s="89"/>
+      <c r="F2" s="89"/>
+      <c r="G2" s="89"/>
+      <c r="H2" s="89"/>
+      <c r="I2" s="89"/>
+      <c r="J2" s="89"/>
+      <c r="K2" s="89"/>
+      <c r="L2" s="89"/>
+      <c r="M2" s="89"/>
+      <c r="N2" s="89"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="89" t="s">
+      <c r="B3" s="90" t="s">
         <v>100</v>
       </c>
-      <c r="C3" s="89"/>
-      <c r="D3" s="89"/>
-      <c r="E3" s="89"/>
-      <c r="F3" s="89"/>
-      <c r="G3" s="89"/>
-      <c r="H3" s="89"/>
-      <c r="I3" s="89"/>
-      <c r="J3" s="89"/>
-      <c r="K3" s="89"/>
-      <c r="L3" s="89"/>
-      <c r="M3" s="89"/>
-      <c r="N3" s="89"/>
+      <c r="C3" s="90"/>
+      <c r="D3" s="90"/>
+      <c r="E3" s="90"/>
+      <c r="F3" s="90"/>
+      <c r="G3" s="90"/>
+      <c r="H3" s="90"/>
+      <c r="I3" s="90"/>
+      <c r="J3" s="90"/>
+      <c r="K3" s="90"/>
+      <c r="L3" s="90"/>
+      <c r="M3" s="90"/>
+      <c r="N3" s="90"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -3197,10 +3222,10 @@
       <c r="K5" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="L5" s="90" t="s">
+      <c r="L5" s="91" t="s">
         <v>110</v>
       </c>
-      <c r="M5" s="90"/>
+      <c r="M5" s="91"/>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
@@ -3252,38 +3277,38 @@
       </c>
     </row>
     <row r="2" spans="2:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="88"/>
-      <c r="C2" s="88"/>
-      <c r="D2" s="88"/>
-      <c r="E2" s="88"/>
-      <c r="F2" s="88"/>
-      <c r="G2" s="88"/>
-      <c r="H2" s="88"/>
-      <c r="I2" s="88"/>
-      <c r="J2" s="88"/>
-      <c r="K2" s="88"/>
-      <c r="L2" s="88"/>
-      <c r="M2" s="88"/>
-      <c r="N2" s="88"/>
-      <c r="O2" s="88"/>
+      <c r="B2" s="89"/>
+      <c r="C2" s="89"/>
+      <c r="D2" s="89"/>
+      <c r="E2" s="89"/>
+      <c r="F2" s="89"/>
+      <c r="G2" s="89"/>
+      <c r="H2" s="89"/>
+      <c r="I2" s="89"/>
+      <c r="J2" s="89"/>
+      <c r="K2" s="89"/>
+      <c r="L2" s="89"/>
+      <c r="M2" s="89"/>
+      <c r="N2" s="89"/>
+      <c r="O2" s="89"/>
     </row>
     <row r="3" spans="2:15" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="89" t="s">
+      <c r="B3" s="90" t="s">
         <v>73</v>
       </c>
-      <c r="C3" s="89"/>
-      <c r="D3" s="89"/>
-      <c r="E3" s="89"/>
-      <c r="F3" s="89"/>
-      <c r="G3" s="89"/>
-      <c r="H3" s="89"/>
-      <c r="I3" s="89"/>
-      <c r="J3" s="89"/>
-      <c r="K3" s="89"/>
-      <c r="L3" s="89"/>
-      <c r="M3" s="89"/>
-      <c r="N3" s="89"/>
-      <c r="O3" s="89"/>
+      <c r="C3" s="90"/>
+      <c r="D3" s="90"/>
+      <c r="E3" s="90"/>
+      <c r="F3" s="90"/>
+      <c r="G3" s="90"/>
+      <c r="H3" s="90"/>
+      <c r="I3" s="90"/>
+      <c r="J3" s="90"/>
+      <c r="K3" s="90"/>
+      <c r="L3" s="90"/>
+      <c r="M3" s="90"/>
+      <c r="N3" s="90"/>
+      <c r="O3" s="90"/>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -3362,18 +3387,18 @@
       </c>
     </row>
     <row r="2" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="88"/>
-      <c r="C2" s="88"/>
-      <c r="D2" s="88"/>
-      <c r="E2" s="88"/>
+      <c r="B2" s="89"/>
+      <c r="C2" s="89"/>
+      <c r="D2" s="89"/>
+      <c r="E2" s="89"/>
     </row>
     <row r="3" spans="2:5" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="89" t="s">
+      <c r="B3" s="90" t="s">
         <v>131</v>
       </c>
-      <c r="C3" s="89"/>
-      <c r="D3" s="89"/>
-      <c r="E3" s="89"/>
+      <c r="C3" s="90"/>
+      <c r="D3" s="90"/>
+      <c r="E3" s="90"/>
     </row>
     <row r="4" spans="2:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="64"/>
@@ -3435,36 +3460,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="88"/>
-      <c r="C2" s="88"/>
-      <c r="D2" s="88"/>
-      <c r="E2" s="88"/>
-      <c r="F2" s="88"/>
-      <c r="G2" s="88"/>
-      <c r="H2" s="88"/>
-      <c r="I2" s="88"/>
-      <c r="J2" s="88"/>
-      <c r="K2" s="88"/>
-      <c r="L2" s="88"/>
-      <c r="M2" s="88"/>
-      <c r="N2" s="88"/>
+      <c r="B2" s="89"/>
+      <c r="C2" s="89"/>
+      <c r="D2" s="89"/>
+      <c r="E2" s="89"/>
+      <c r="F2" s="89"/>
+      <c r="G2" s="89"/>
+      <c r="H2" s="89"/>
+      <c r="I2" s="89"/>
+      <c r="J2" s="89"/>
+      <c r="K2" s="89"/>
+      <c r="L2" s="89"/>
+      <c r="M2" s="89"/>
+      <c r="N2" s="89"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="89" t="s">
+      <c r="B3" s="90" t="s">
         <v>69</v>
       </c>
-      <c r="C3" s="89"/>
-      <c r="D3" s="89"/>
-      <c r="E3" s="89"/>
-      <c r="F3" s="89"/>
-      <c r="G3" s="89"/>
-      <c r="H3" s="89"/>
-      <c r="I3" s="89"/>
-      <c r="J3" s="89"/>
-      <c r="K3" s="89"/>
-      <c r="L3" s="89"/>
-      <c r="M3" s="89"/>
-      <c r="N3" s="89"/>
+      <c r="C3" s="90"/>
+      <c r="D3" s="90"/>
+      <c r="E3" s="90"/>
+      <c r="F3" s="90"/>
+      <c r="G3" s="90"/>
+      <c r="H3" s="90"/>
+      <c r="I3" s="90"/>
+      <c r="J3" s="90"/>
+      <c r="K3" s="90"/>
+      <c r="L3" s="90"/>
+      <c r="M3" s="90"/>
+      <c r="N3" s="90"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -3519,36 +3544,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="88"/>
-      <c r="C2" s="88"/>
-      <c r="D2" s="88"/>
-      <c r="E2" s="88"/>
-      <c r="F2" s="88"/>
-      <c r="G2" s="88"/>
-      <c r="H2" s="88"/>
-      <c r="I2" s="88"/>
-      <c r="J2" s="88"/>
-      <c r="K2" s="88"/>
-      <c r="L2" s="88"/>
-      <c r="M2" s="88"/>
-      <c r="N2" s="88"/>
+      <c r="B2" s="89"/>
+      <c r="C2" s="89"/>
+      <c r="D2" s="89"/>
+      <c r="E2" s="89"/>
+      <c r="F2" s="89"/>
+      <c r="G2" s="89"/>
+      <c r="H2" s="89"/>
+      <c r="I2" s="89"/>
+      <c r="J2" s="89"/>
+      <c r="K2" s="89"/>
+      <c r="L2" s="89"/>
+      <c r="M2" s="89"/>
+      <c r="N2" s="89"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="89" t="s">
+      <c r="B3" s="90" t="s">
         <v>74</v>
       </c>
-      <c r="C3" s="89"/>
-      <c r="D3" s="89"/>
-      <c r="E3" s="89"/>
-      <c r="F3" s="89"/>
-      <c r="G3" s="89"/>
-      <c r="H3" s="89"/>
-      <c r="I3" s="89"/>
-      <c r="J3" s="89"/>
-      <c r="K3" s="89"/>
-      <c r="L3" s="89"/>
-      <c r="M3" s="89"/>
-      <c r="N3" s="89"/>
+      <c r="C3" s="90"/>
+      <c r="D3" s="90"/>
+      <c r="E3" s="90"/>
+      <c r="F3" s="90"/>
+      <c r="G3" s="90"/>
+      <c r="H3" s="90"/>
+      <c r="I3" s="90"/>
+      <c r="J3" s="90"/>
+      <c r="K3" s="90"/>
+      <c r="L3" s="90"/>
+      <c r="M3" s="90"/>
+      <c r="N3" s="90"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -3617,40 +3642,40 @@
       </c>
     </row>
     <row r="2" spans="2:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="88"/>
-      <c r="C2" s="88"/>
-      <c r="D2" s="88"/>
-      <c r="E2" s="88"/>
-      <c r="F2" s="88"/>
-      <c r="G2" s="88"/>
-      <c r="H2" s="88"/>
-      <c r="I2" s="88"/>
-      <c r="J2" s="88"/>
-      <c r="K2" s="88"/>
-      <c r="L2" s="88"/>
-      <c r="M2" s="88"/>
-      <c r="N2" s="88"/>
-      <c r="O2" s="88"/>
-      <c r="P2" s="88"/>
+      <c r="B2" s="89"/>
+      <c r="C2" s="89"/>
+      <c r="D2" s="89"/>
+      <c r="E2" s="89"/>
+      <c r="F2" s="89"/>
+      <c r="G2" s="89"/>
+      <c r="H2" s="89"/>
+      <c r="I2" s="89"/>
+      <c r="J2" s="89"/>
+      <c r="K2" s="89"/>
+      <c r="L2" s="89"/>
+      <c r="M2" s="89"/>
+      <c r="N2" s="89"/>
+      <c r="O2" s="89"/>
+      <c r="P2" s="89"/>
     </row>
     <row r="3" spans="2:18" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="89" t="s">
+      <c r="B3" s="90" t="s">
         <v>63</v>
       </c>
-      <c r="C3" s="89"/>
-      <c r="D3" s="89"/>
-      <c r="E3" s="89"/>
-      <c r="F3" s="89"/>
-      <c r="G3" s="89"/>
-      <c r="H3" s="89"/>
-      <c r="I3" s="89"/>
-      <c r="J3" s="89"/>
-      <c r="K3" s="89"/>
-      <c r="L3" s="89"/>
-      <c r="M3" s="89"/>
-      <c r="N3" s="89"/>
-      <c r="O3" s="89"/>
-      <c r="P3" s="89"/>
+      <c r="C3" s="90"/>
+      <c r="D3" s="90"/>
+      <c r="E3" s="90"/>
+      <c r="F3" s="90"/>
+      <c r="G3" s="90"/>
+      <c r="H3" s="90"/>
+      <c r="I3" s="90"/>
+      <c r="J3" s="90"/>
+      <c r="K3" s="90"/>
+      <c r="L3" s="90"/>
+      <c r="M3" s="90"/>
+      <c r="N3" s="90"/>
+      <c r="O3" s="90"/>
+      <c r="P3" s="90"/>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
@@ -3764,36 +3789,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="88"/>
-      <c r="C2" s="88"/>
-      <c r="D2" s="88"/>
-      <c r="E2" s="88"/>
-      <c r="F2" s="88"/>
-      <c r="G2" s="88"/>
-      <c r="H2" s="88"/>
-      <c r="I2" s="88"/>
-      <c r="J2" s="88"/>
-      <c r="K2" s="88"/>
-      <c r="L2" s="88"/>
-      <c r="M2" s="88"/>
-      <c r="N2" s="88"/>
+      <c r="B2" s="89"/>
+      <c r="C2" s="89"/>
+      <c r="D2" s="89"/>
+      <c r="E2" s="89"/>
+      <c r="F2" s="89"/>
+      <c r="G2" s="89"/>
+      <c r="H2" s="89"/>
+      <c r="I2" s="89"/>
+      <c r="J2" s="89"/>
+      <c r="K2" s="89"/>
+      <c r="L2" s="89"/>
+      <c r="M2" s="89"/>
+      <c r="N2" s="89"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="89" t="s">
+      <c r="B3" s="90" t="s">
         <v>64</v>
       </c>
-      <c r="C3" s="89"/>
-      <c r="D3" s="89"/>
-      <c r="E3" s="89"/>
-      <c r="F3" s="89"/>
-      <c r="G3" s="89"/>
-      <c r="H3" s="89"/>
-      <c r="I3" s="89"/>
-      <c r="J3" s="89"/>
-      <c r="K3" s="89"/>
-      <c r="L3" s="89"/>
-      <c r="M3" s="89"/>
-      <c r="N3" s="89"/>
+      <c r="C3" s="90"/>
+      <c r="D3" s="90"/>
+      <c r="E3" s="90"/>
+      <c r="F3" s="90"/>
+      <c r="G3" s="90"/>
+      <c r="H3" s="90"/>
+      <c r="I3" s="90"/>
+      <c r="J3" s="90"/>
+      <c r="K3" s="90"/>
+      <c r="L3" s="90"/>
+      <c r="M3" s="90"/>
+      <c r="N3" s="90"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="58" t="s">
@@ -3880,38 +3905,38 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="88" t="s">
+      <c r="B2" s="89" t="s">
         <v>97</v>
       </c>
-      <c r="C2" s="88"/>
-      <c r="D2" s="88"/>
-      <c r="E2" s="88"/>
-      <c r="F2" s="88"/>
-      <c r="G2" s="88"/>
-      <c r="H2" s="88"/>
-      <c r="I2" s="88"/>
-      <c r="J2" s="88"/>
-      <c r="K2" s="88"/>
-      <c r="L2" s="88"/>
-      <c r="M2" s="88"/>
-      <c r="N2" s="88"/>
+      <c r="C2" s="89"/>
+      <c r="D2" s="89"/>
+      <c r="E2" s="89"/>
+      <c r="F2" s="89"/>
+      <c r="G2" s="89"/>
+      <c r="H2" s="89"/>
+      <c r="I2" s="89"/>
+      <c r="J2" s="89"/>
+      <c r="K2" s="89"/>
+      <c r="L2" s="89"/>
+      <c r="M2" s="89"/>
+      <c r="N2" s="89"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="89" t="s">
+      <c r="B3" s="90" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="89"/>
-      <c r="D3" s="89"/>
-      <c r="E3" s="89"/>
-      <c r="F3" s="89"/>
-      <c r="G3" s="89"/>
-      <c r="H3" s="89"/>
-      <c r="I3" s="89"/>
-      <c r="J3" s="89"/>
-      <c r="K3" s="89"/>
-      <c r="L3" s="89"/>
-      <c r="M3" s="89"/>
-      <c r="N3" s="89"/>
+      <c r="C3" s="90"/>
+      <c r="D3" s="90"/>
+      <c r="E3" s="90"/>
+      <c r="F3" s="90"/>
+      <c r="G3" s="90"/>
+      <c r="H3" s="90"/>
+      <c r="I3" s="90"/>
+      <c r="J3" s="90"/>
+      <c r="K3" s="90"/>
+      <c r="L3" s="90"/>
+      <c r="M3" s="90"/>
+      <c r="N3" s="90"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="44" t="s">
@@ -3970,36 +3995,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="88"/>
-      <c r="C2" s="88"/>
-      <c r="D2" s="88"/>
-      <c r="E2" s="88"/>
-      <c r="F2" s="88"/>
-      <c r="G2" s="88"/>
-      <c r="H2" s="88"/>
-      <c r="I2" s="88"/>
-      <c r="J2" s="88"/>
-      <c r="K2" s="88"/>
-      <c r="L2" s="88"/>
-      <c r="M2" s="88"/>
-      <c r="N2" s="88"/>
+      <c r="B2" s="89"/>
+      <c r="C2" s="89"/>
+      <c r="D2" s="89"/>
+      <c r="E2" s="89"/>
+      <c r="F2" s="89"/>
+      <c r="G2" s="89"/>
+      <c r="H2" s="89"/>
+      <c r="I2" s="89"/>
+      <c r="J2" s="89"/>
+      <c r="K2" s="89"/>
+      <c r="L2" s="89"/>
+      <c r="M2" s="89"/>
+      <c r="N2" s="89"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="89" t="s">
+      <c r="B3" s="90" t="s">
         <v>152</v>
       </c>
-      <c r="C3" s="89"/>
-      <c r="D3" s="89"/>
-      <c r="E3" s="89"/>
-      <c r="F3" s="89"/>
-      <c r="G3" s="89"/>
-      <c r="H3" s="89"/>
-      <c r="I3" s="89"/>
-      <c r="J3" s="89"/>
-      <c r="K3" s="89"/>
-      <c r="L3" s="89"/>
-      <c r="M3" s="89"/>
-      <c r="N3" s="89"/>
+      <c r="C3" s="90"/>
+      <c r="D3" s="90"/>
+      <c r="E3" s="90"/>
+      <c r="F3" s="90"/>
+      <c r="G3" s="90"/>
+      <c r="H3" s="90"/>
+      <c r="I3" s="90"/>
+      <c r="J3" s="90"/>
+      <c r="K3" s="90"/>
+      <c r="L3" s="90"/>
+      <c r="M3" s="90"/>
+      <c r="N3" s="90"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="74" t="s">
@@ -4086,28 +4111,28 @@
       </c>
     </row>
     <row r="2" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="88"/>
-      <c r="C2" s="88"/>
-      <c r="D2" s="88"/>
-      <c r="E2" s="88"/>
-      <c r="F2" s="88"/>
-      <c r="G2" s="88"/>
-      <c r="H2" s="88"/>
-      <c r="I2" s="88"/>
-      <c r="J2" s="88"/>
+      <c r="B2" s="89"/>
+      <c r="C2" s="89"/>
+      <c r="D2" s="89"/>
+      <c r="E2" s="89"/>
+      <c r="F2" s="89"/>
+      <c r="G2" s="89"/>
+      <c r="H2" s="89"/>
+      <c r="I2" s="89"/>
+      <c r="J2" s="89"/>
     </row>
     <row r="3" spans="2:10" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="89" t="s">
+      <c r="B3" s="90" t="s">
         <v>155</v>
       </c>
-      <c r="C3" s="89"/>
-      <c r="D3" s="89"/>
-      <c r="E3" s="89"/>
-      <c r="F3" s="89"/>
-      <c r="G3" s="89"/>
-      <c r="H3" s="89"/>
-      <c r="I3" s="89"/>
-      <c r="J3" s="89"/>
+      <c r="C3" s="90"/>
+      <c r="D3" s="90"/>
+      <c r="E3" s="90"/>
+      <c r="F3" s="90"/>
+      <c r="G3" s="90"/>
+      <c r="H3" s="90"/>
+      <c r="I3" s="90"/>
+      <c r="J3" s="90"/>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" s="74" t="s">
@@ -4157,10 +4182,10 @@
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:N6"/>
+  <dimension ref="B1:T6"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4178,40 +4203,46 @@
     <col min="12" max="12" width="19.140625" customWidth="1"/>
     <col min="13" max="13" width="25.42578125" customWidth="1"/>
     <col min="14" max="14" width="21.85546875" customWidth="1"/>
+    <col min="15" max="15" width="17" customWidth="1"/>
+    <col min="16" max="16" width="23.7109375" customWidth="1"/>
+    <col min="17" max="17" width="25" customWidth="1"/>
+    <col min="18" max="18" width="14.5703125" customWidth="1"/>
+    <col min="19" max="19" width="24.85546875" customWidth="1"/>
+    <col min="20" max="20" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:20" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="88"/>
-      <c r="C2" s="88"/>
-      <c r="D2" s="88"/>
-      <c r="E2" s="88"/>
-      <c r="F2" s="88"/>
-      <c r="G2" s="88"/>
-      <c r="H2" s="88"/>
-      <c r="I2" s="88"/>
-      <c r="J2" s="88"/>
+    <row r="2" spans="2:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="89"/>
+      <c r="C2" s="89"/>
+      <c r="D2" s="89"/>
+      <c r="E2" s="89"/>
+      <c r="F2" s="89"/>
+      <c r="G2" s="89"/>
+      <c r="H2" s="89"/>
+      <c r="I2" s="89"/>
+      <c r="J2" s="89"/>
       <c r="K2" s="85"/>
     </row>
-    <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="89" t="s">
+    <row r="3" spans="2:20" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B3" s="90" t="s">
         <v>156</v>
       </c>
-      <c r="C3" s="89"/>
-      <c r="D3" s="89"/>
-      <c r="E3" s="89"/>
-      <c r="F3" s="89"/>
-      <c r="G3" s="89"/>
-      <c r="H3" s="89"/>
-      <c r="I3" s="89"/>
-      <c r="J3" s="89"/>
+      <c r="C3" s="90"/>
+      <c r="D3" s="90"/>
+      <c r="E3" s="90"/>
+      <c r="F3" s="90"/>
+      <c r="G3" s="90"/>
+      <c r="H3" s="90"/>
+      <c r="I3" s="90"/>
+      <c r="J3" s="90"/>
       <c r="K3" s="84"/>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B5" s="81" t="s">
         <v>2</v>
       </c>
@@ -4251,8 +4282,26 @@
       <c r="N5" s="80" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="O5" s="88" t="s">
+        <v>177</v>
+      </c>
+      <c r="P5" s="88" t="s">
+        <v>178</v>
+      </c>
+      <c r="Q5" s="88" t="s">
+        <v>182</v>
+      </c>
+      <c r="R5" s="88" t="s">
+        <v>179</v>
+      </c>
+      <c r="S5" s="88" t="s">
+        <v>180</v>
+      </c>
+      <c r="T5" s="88" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="6" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
       <c r="D6" s="9"/>
@@ -4266,6 +4315,12 @@
       <c r="L6" s="79"/>
       <c r="M6" s="79"/>
       <c r="N6" s="83"/>
+      <c r="O6" s="82"/>
+      <c r="P6" s="105"/>
+      <c r="Q6" s="79"/>
+      <c r="R6" s="82"/>
+      <c r="S6" s="82"/>
+      <c r="T6" s="83"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -4281,7 +4336,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K7"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
@@ -4305,30 +4360,30 @@
       </c>
     </row>
     <row r="2" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="88"/>
-      <c r="C2" s="88"/>
-      <c r="D2" s="88"/>
-      <c r="E2" s="88"/>
-      <c r="F2" s="88"/>
-      <c r="G2" s="88"/>
-      <c r="H2" s="88"/>
-      <c r="I2" s="88"/>
-      <c r="J2" s="88"/>
-      <c r="K2" s="88"/>
+      <c r="B2" s="89"/>
+      <c r="C2" s="89"/>
+      <c r="D2" s="89"/>
+      <c r="E2" s="89"/>
+      <c r="F2" s="89"/>
+      <c r="G2" s="89"/>
+      <c r="H2" s="89"/>
+      <c r="I2" s="89"/>
+      <c r="J2" s="89"/>
+      <c r="K2" s="89"/>
     </row>
     <row r="3" spans="2:11" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="89" t="s">
+      <c r="B3" s="90" t="s">
         <v>168</v>
       </c>
-      <c r="C3" s="89"/>
-      <c r="D3" s="89"/>
-      <c r="E3" s="89"/>
-      <c r="F3" s="89"/>
-      <c r="G3" s="89"/>
-      <c r="H3" s="89"/>
-      <c r="I3" s="89"/>
-      <c r="J3" s="89"/>
-      <c r="K3" s="89"/>
+      <c r="C3" s="90"/>
+      <c r="D3" s="90"/>
+      <c r="E3" s="90"/>
+      <c r="F3" s="90"/>
+      <c r="G3" s="90"/>
+      <c r="H3" s="90"/>
+      <c r="I3" s="90"/>
+      <c r="J3" s="90"/>
+      <c r="K3" s="90"/>
     </row>
     <row r="4" spans="2:11" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B4" s="86"/>
@@ -4343,14 +4398,14 @@
       <c r="K4" s="86"/>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="H5" s="91" t="s">
+      <c r="H5" s="92" t="s">
         <v>176</v>
       </c>
-      <c r="I5" s="92"/>
-      <c r="J5" s="91" t="s">
+      <c r="I5" s="93"/>
+      <c r="J5" s="92" t="s">
         <v>175</v>
       </c>
-      <c r="K5" s="92"/>
+      <c r="K5" s="93"/>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" s="87" t="s">
@@ -4432,37 +4487,37 @@
       <c r="Z1" s="38"/>
     </row>
     <row r="2" spans="2:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="88"/>
-      <c r="C2" s="88"/>
-      <c r="D2" s="88"/>
-      <c r="E2" s="88"/>
-      <c r="F2" s="88"/>
-      <c r="G2" s="88"/>
-      <c r="H2" s="88"/>
-      <c r="I2" s="88"/>
-      <c r="J2" s="88"/>
-      <c r="K2" s="88"/>
-      <c r="L2" s="88"/>
-      <c r="M2" s="88"/>
-      <c r="N2" s="88"/>
+      <c r="B2" s="89"/>
+      <c r="C2" s="89"/>
+      <c r="D2" s="89"/>
+      <c r="E2" s="89"/>
+      <c r="F2" s="89"/>
+      <c r="G2" s="89"/>
+      <c r="H2" s="89"/>
+      <c r="I2" s="89"/>
+      <c r="J2" s="89"/>
+      <c r="K2" s="89"/>
+      <c r="L2" s="89"/>
+      <c r="M2" s="89"/>
+      <c r="N2" s="89"/>
       <c r="Z2"/>
     </row>
     <row r="3" spans="2:26" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="89" t="s">
+      <c r="B3" s="90" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="89"/>
-      <c r="D3" s="89"/>
-      <c r="E3" s="89"/>
-      <c r="F3" s="89"/>
-      <c r="G3" s="89"/>
-      <c r="H3" s="89"/>
-      <c r="I3" s="89"/>
-      <c r="J3" s="89"/>
-      <c r="K3" s="89"/>
-      <c r="L3" s="89"/>
-      <c r="M3" s="89"/>
-      <c r="N3" s="89"/>
+      <c r="C3" s="90"/>
+      <c r="D3" s="90"/>
+      <c r="E3" s="90"/>
+      <c r="F3" s="90"/>
+      <c r="G3" s="90"/>
+      <c r="H3" s="90"/>
+      <c r="I3" s="90"/>
+      <c r="J3" s="90"/>
+      <c r="K3" s="90"/>
+      <c r="L3" s="90"/>
+      <c r="M3" s="90"/>
+      <c r="N3" s="90"/>
       <c r="Z3"/>
     </row>
     <row r="5" spans="2:26" x14ac:dyDescent="0.25">
@@ -4566,37 +4621,37 @@
       <c r="Z1" s="38"/>
     </row>
     <row r="2" spans="2:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="88"/>
-      <c r="C2" s="88"/>
-      <c r="D2" s="88"/>
-      <c r="E2" s="88"/>
-      <c r="F2" s="88"/>
-      <c r="G2" s="88"/>
-      <c r="H2" s="88"/>
-      <c r="I2" s="88"/>
-      <c r="J2" s="88"/>
-      <c r="K2" s="88"/>
-      <c r="L2" s="88"/>
-      <c r="M2" s="88"/>
-      <c r="N2" s="88"/>
+      <c r="B2" s="89"/>
+      <c r="C2" s="89"/>
+      <c r="D2" s="89"/>
+      <c r="E2" s="89"/>
+      <c r="F2" s="89"/>
+      <c r="G2" s="89"/>
+      <c r="H2" s="89"/>
+      <c r="I2" s="89"/>
+      <c r="J2" s="89"/>
+      <c r="K2" s="89"/>
+      <c r="L2" s="89"/>
+      <c r="M2" s="89"/>
+      <c r="N2" s="89"/>
       <c r="Z2"/>
     </row>
     <row r="3" spans="2:26" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="89" t="s">
+      <c r="B3" s="90" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="89"/>
-      <c r="D3" s="89"/>
-      <c r="E3" s="89"/>
-      <c r="F3" s="89"/>
-      <c r="G3" s="89"/>
-      <c r="H3" s="89"/>
-      <c r="I3" s="89"/>
-      <c r="J3" s="89"/>
-      <c r="K3" s="89"/>
-      <c r="L3" s="89"/>
-      <c r="M3" s="89"/>
-      <c r="N3" s="89"/>
+      <c r="C3" s="90"/>
+      <c r="D3" s="90"/>
+      <c r="E3" s="90"/>
+      <c r="F3" s="90"/>
+      <c r="G3" s="90"/>
+      <c r="H3" s="90"/>
+      <c r="I3" s="90"/>
+      <c r="J3" s="90"/>
+      <c r="K3" s="90"/>
+      <c r="L3" s="90"/>
+      <c r="M3" s="90"/>
+      <c r="N3" s="90"/>
       <c r="Z3"/>
     </row>
     <row r="5" spans="2:26" x14ac:dyDescent="0.25">
@@ -4615,9 +4670,9 @@
       <c r="C6" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="D6" s="93"/>
-      <c r="E6" s="94"/>
-      <c r="F6" s="95"/>
+      <c r="D6" s="94"/>
+      <c r="E6" s="95"/>
+      <c r="F6" s="96"/>
       <c r="G6" s="50"/>
       <c r="H6" s="50"/>
     </row>
@@ -4695,37 +4750,37 @@
       <c r="Z1" s="38"/>
     </row>
     <row r="2" spans="2:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="88"/>
-      <c r="C2" s="88"/>
-      <c r="D2" s="88"/>
-      <c r="E2" s="88"/>
-      <c r="F2" s="88"/>
-      <c r="G2" s="88"/>
-      <c r="H2" s="88"/>
-      <c r="I2" s="88"/>
-      <c r="J2" s="88"/>
-      <c r="K2" s="88"/>
-      <c r="L2" s="88"/>
-      <c r="M2" s="88"/>
-      <c r="N2" s="88"/>
+      <c r="B2" s="89"/>
+      <c r="C2" s="89"/>
+      <c r="D2" s="89"/>
+      <c r="E2" s="89"/>
+      <c r="F2" s="89"/>
+      <c r="G2" s="89"/>
+      <c r="H2" s="89"/>
+      <c r="I2" s="89"/>
+      <c r="J2" s="89"/>
+      <c r="K2" s="89"/>
+      <c r="L2" s="89"/>
+      <c r="M2" s="89"/>
+      <c r="N2" s="89"/>
       <c r="Z2"/>
     </row>
     <row r="3" spans="2:26" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="89" t="s">
+      <c r="B3" s="90" t="s">
         <v>93</v>
       </c>
-      <c r="C3" s="89"/>
-      <c r="D3" s="89"/>
-      <c r="E3" s="89"/>
-      <c r="F3" s="89"/>
-      <c r="G3" s="89"/>
-      <c r="H3" s="89"/>
-      <c r="I3" s="89"/>
-      <c r="J3" s="89"/>
-      <c r="K3" s="89"/>
-      <c r="L3" s="89"/>
-      <c r="M3" s="89"/>
-      <c r="N3" s="89"/>
+      <c r="C3" s="90"/>
+      <c r="D3" s="90"/>
+      <c r="E3" s="90"/>
+      <c r="F3" s="90"/>
+      <c r="G3" s="90"/>
+      <c r="H3" s="90"/>
+      <c r="I3" s="90"/>
+      <c r="J3" s="90"/>
+      <c r="K3" s="90"/>
+      <c r="L3" s="90"/>
+      <c r="M3" s="90"/>
+      <c r="N3" s="90"/>
       <c r="Z3"/>
     </row>
     <row r="5" spans="2:26" x14ac:dyDescent="0.25">
@@ -4818,37 +4873,37 @@
       <c r="Z1" s="38"/>
     </row>
     <row r="2" spans="2:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="88"/>
-      <c r="C2" s="88"/>
-      <c r="D2" s="88"/>
-      <c r="E2" s="88"/>
-      <c r="F2" s="88"/>
-      <c r="G2" s="88"/>
-      <c r="H2" s="88"/>
-      <c r="I2" s="88"/>
-      <c r="J2" s="88"/>
-      <c r="K2" s="88"/>
-      <c r="L2" s="88"/>
-      <c r="M2" s="88"/>
-      <c r="N2" s="88"/>
+      <c r="B2" s="89"/>
+      <c r="C2" s="89"/>
+      <c r="D2" s="89"/>
+      <c r="E2" s="89"/>
+      <c r="F2" s="89"/>
+      <c r="G2" s="89"/>
+      <c r="H2" s="89"/>
+      <c r="I2" s="89"/>
+      <c r="J2" s="89"/>
+      <c r="K2" s="89"/>
+      <c r="L2" s="89"/>
+      <c r="M2" s="89"/>
+      <c r="N2" s="89"/>
       <c r="Z2"/>
     </row>
     <row r="3" spans="2:26" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="89" t="s">
+      <c r="B3" s="90" t="s">
         <v>72</v>
       </c>
-      <c r="C3" s="89"/>
-      <c r="D3" s="89"/>
-      <c r="E3" s="89"/>
-      <c r="F3" s="89"/>
-      <c r="G3" s="89"/>
-      <c r="H3" s="89"/>
-      <c r="I3" s="89"/>
-      <c r="J3" s="89"/>
-      <c r="K3" s="89"/>
-      <c r="L3" s="89"/>
-      <c r="M3" s="89"/>
-      <c r="N3" s="89"/>
+      <c r="C3" s="90"/>
+      <c r="D3" s="90"/>
+      <c r="E3" s="90"/>
+      <c r="F3" s="90"/>
+      <c r="G3" s="90"/>
+      <c r="H3" s="90"/>
+      <c r="I3" s="90"/>
+      <c r="J3" s="90"/>
+      <c r="K3" s="90"/>
+      <c r="L3" s="90"/>
+      <c r="M3" s="90"/>
+      <c r="N3" s="90"/>
       <c r="Z3"/>
     </row>
     <row r="5" spans="2:26" x14ac:dyDescent="0.25">
@@ -4961,56 +5016,56 @@
       </c>
     </row>
     <row r="2" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="88"/>
-      <c r="C2" s="88"/>
-      <c r="D2" s="88"/>
-      <c r="E2" s="88"/>
-      <c r="F2" s="88"/>
-      <c r="G2" s="88"/>
-      <c r="H2" s="88"/>
-      <c r="I2" s="88"/>
-      <c r="J2" s="88"/>
-      <c r="K2" s="88"/>
-      <c r="L2" s="88"/>
+      <c r="B2" s="89"/>
+      <c r="C2" s="89"/>
+      <c r="D2" s="89"/>
+      <c r="E2" s="89"/>
+      <c r="F2" s="89"/>
+      <c r="G2" s="89"/>
+      <c r="H2" s="89"/>
+      <c r="I2" s="89"/>
+      <c r="J2" s="89"/>
+      <c r="K2" s="89"/>
+      <c r="L2" s="89"/>
     </row>
     <row r="3" spans="2:17" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="89" t="s">
+      <c r="B3" s="90" t="s">
         <v>108</v>
       </c>
-      <c r="C3" s="89"/>
-      <c r="D3" s="89"/>
-      <c r="E3" s="89"/>
-      <c r="F3" s="89"/>
-      <c r="G3" s="89"/>
-      <c r="H3" s="89"/>
-      <c r="I3" s="89"/>
-      <c r="J3" s="89"/>
-      <c r="K3" s="89"/>
-      <c r="L3" s="89"/>
+      <c r="C3" s="90"/>
+      <c r="D3" s="90"/>
+      <c r="E3" s="90"/>
+      <c r="F3" s="90"/>
+      <c r="G3" s="90"/>
+      <c r="H3" s="90"/>
+      <c r="I3" s="90"/>
+      <c r="J3" s="90"/>
+      <c r="K3" s="90"/>
+      <c r="L3" s="90"/>
     </row>
     <row r="5" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D5" s="96" t="s">
+      <c r="D5" s="97" t="s">
         <v>123</v>
       </c>
-      <c r="E5" s="96"/>
+      <c r="E5" s="97"/>
       <c r="F5" s="73"/>
       <c r="G5" s="73"/>
       <c r="H5" s="73"/>
       <c r="I5" s="73"/>
-      <c r="J5" s="96" t="s">
+      <c r="J5" s="97" t="s">
         <v>42</v>
       </c>
-      <c r="K5" s="96"/>
-      <c r="L5" s="96"/>
-      <c r="M5" s="96" t="s">
+      <c r="K5" s="97"/>
+      <c r="L5" s="97"/>
+      <c r="M5" s="97" t="s">
         <v>130</v>
       </c>
-      <c r="N5" s="96"/>
-      <c r="O5" s="96"/>
-      <c r="P5" s="90" t="s">
+      <c r="N5" s="97"/>
+      <c r="O5" s="97"/>
+      <c r="P5" s="91" t="s">
         <v>109</v>
       </c>
-      <c r="Q5" s="90"/>
+      <c r="Q5" s="91"/>
     </row>
     <row r="6" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="70" t="s">
@@ -5097,7 +5152,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:X8"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="Y9" sqref="Y9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5131,47 +5188,47 @@
       </c>
     </row>
     <row r="2" spans="2:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="88"/>
-      <c r="C2" s="88"/>
-      <c r="D2" s="88"/>
-      <c r="E2" s="88"/>
-      <c r="F2" s="88"/>
-      <c r="G2" s="88"/>
-      <c r="H2" s="88"/>
-      <c r="I2" s="88"/>
-      <c r="J2" s="88"/>
-      <c r="K2" s="88"/>
-      <c r="L2" s="88"/>
-      <c r="M2" s="88"/>
-      <c r="N2" s="88"/>
-      <c r="O2" s="88"/>
-      <c r="P2" s="88"/>
+      <c r="B2" s="89"/>
+      <c r="C2" s="89"/>
+      <c r="D2" s="89"/>
+      <c r="E2" s="89"/>
+      <c r="F2" s="89"/>
+      <c r="G2" s="89"/>
+      <c r="H2" s="89"/>
+      <c r="I2" s="89"/>
+      <c r="J2" s="89"/>
+      <c r="K2" s="89"/>
+      <c r="L2" s="89"/>
+      <c r="M2" s="89"/>
+      <c r="N2" s="89"/>
+      <c r="O2" s="89"/>
+      <c r="P2" s="89"/>
       <c r="Q2" s="56"/>
       <c r="R2" s="56"/>
     </row>
     <row r="3" spans="2:24" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="89" t="s">
+      <c r="B3" s="90" t="s">
         <v>111</v>
       </c>
-      <c r="C3" s="89"/>
-      <c r="D3" s="89"/>
-      <c r="E3" s="89"/>
-      <c r="F3" s="89"/>
-      <c r="G3" s="89"/>
-      <c r="H3" s="89"/>
-      <c r="I3" s="89"/>
-      <c r="J3" s="89"/>
-      <c r="K3" s="89"/>
-      <c r="L3" s="89"/>
-      <c r="M3" s="89"/>
-      <c r="N3" s="89"/>
-      <c r="O3" s="89"/>
-      <c r="P3" s="89"/>
+      <c r="C3" s="90"/>
+      <c r="D3" s="90"/>
+      <c r="E3" s="90"/>
+      <c r="F3" s="90"/>
+      <c r="G3" s="90"/>
+      <c r="H3" s="90"/>
+      <c r="I3" s="90"/>
+      <c r="J3" s="90"/>
+      <c r="K3" s="90"/>
+      <c r="L3" s="90"/>
+      <c r="M3" s="90"/>
+      <c r="N3" s="90"/>
+      <c r="O3" s="90"/>
+      <c r="P3" s="90"/>
       <c r="Q3" s="57"/>
       <c r="R3" s="57"/>
     </row>
     <row r="5" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B5" s="97" t="s">
+      <c r="B5" s="98" t="s">
         <v>112</v>
       </c>
       <c r="C5" s="99"/>
@@ -5183,8 +5240,8 @@
       <c r="I5" s="99"/>
       <c r="J5" s="99"/>
       <c r="K5" s="99"/>
-      <c r="L5" s="98"/>
-      <c r="M5" s="97" t="s">
+      <c r="L5" s="100"/>
+      <c r="M5" s="98" t="s">
         <v>113</v>
       </c>
       <c r="N5" s="99"/>
@@ -5197,42 +5254,42 @@
       <c r="U5" s="99"/>
       <c r="V5" s="99"/>
       <c r="W5" s="99"/>
-      <c r="X5" s="98"/>
+      <c r="X5" s="100"/>
     </row>
     <row r="6" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B6" s="100"/>
-      <c r="C6" s="100"/>
-      <c r="D6" s="100"/>
-      <c r="E6" s="100"/>
+      <c r="B6" s="104"/>
+      <c r="C6" s="104"/>
+      <c r="D6" s="104"/>
+      <c r="E6" s="104"/>
       <c r="F6" s="101" t="s">
         <v>27</v>
       </c>
       <c r="G6" s="102"/>
       <c r="H6" s="102"/>
       <c r="I6" s="103"/>
-      <c r="J6" s="97" t="s">
+      <c r="J6" s="98" t="s">
         <v>30</v>
       </c>
       <c r="K6" s="99"/>
-      <c r="L6" s="98"/>
+      <c r="L6" s="100"/>
       <c r="M6" s="76"/>
-      <c r="N6" s="97" t="s">
+      <c r="N6" s="98" t="s">
         <v>42</v>
       </c>
-      <c r="O6" s="98"/>
-      <c r="P6" s="97" t="s">
+      <c r="O6" s="100"/>
+      <c r="P6" s="98" t="s">
         <v>106</v>
       </c>
       <c r="Q6" s="99"/>
-      <c r="R6" s="98"/>
+      <c r="R6" s="100"/>
       <c r="S6" s="76"/>
-      <c r="T6" s="97" t="s">
+      <c r="T6" s="98" t="s">
         <v>123</v>
       </c>
-      <c r="U6" s="98"/>
-      <c r="V6" s="100"/>
-      <c r="W6" s="100"/>
-      <c r="X6" s="100"/>
+      <c r="U6" s="100"/>
+      <c r="V6" s="104"/>
+      <c r="W6" s="104"/>
+      <c r="X6" s="104"/>
     </row>
     <row r="7" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B7" s="75" t="s">
@@ -5332,6 +5389,7 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="V6:X6"/>
     <mergeCell ref="B2:P2"/>
     <mergeCell ref="B3:P3"/>
     <mergeCell ref="B5:L5"/>
@@ -5342,7 +5400,6 @@
     <mergeCell ref="B6:E6"/>
     <mergeCell ref="M5:X5"/>
     <mergeCell ref="T6:U6"/>
-    <mergeCell ref="V6:X6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5375,36 +5432,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="88"/>
-      <c r="C2" s="88"/>
-      <c r="D2" s="88"/>
-      <c r="E2" s="88"/>
-      <c r="F2" s="88"/>
-      <c r="G2" s="88"/>
-      <c r="H2" s="88"/>
-      <c r="I2" s="88"/>
-      <c r="J2" s="88"/>
-      <c r="K2" s="88"/>
-      <c r="L2" s="88"/>
-      <c r="M2" s="88"/>
-      <c r="N2" s="88"/>
+      <c r="B2" s="89"/>
+      <c r="C2" s="89"/>
+      <c r="D2" s="89"/>
+      <c r="E2" s="89"/>
+      <c r="F2" s="89"/>
+      <c r="G2" s="89"/>
+      <c r="H2" s="89"/>
+      <c r="I2" s="89"/>
+      <c r="J2" s="89"/>
+      <c r="K2" s="89"/>
+      <c r="L2" s="89"/>
+      <c r="M2" s="89"/>
+      <c r="N2" s="89"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="89" t="s">
+      <c r="B3" s="90" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="89"/>
-      <c r="D3" s="89"/>
-      <c r="E3" s="89"/>
-      <c r="F3" s="89"/>
-      <c r="G3" s="89"/>
-      <c r="H3" s="89"/>
-      <c r="I3" s="89"/>
-      <c r="J3" s="89"/>
-      <c r="K3" s="89"/>
-      <c r="L3" s="89"/>
-      <c r="M3" s="89"/>
-      <c r="N3" s="89"/>
+      <c r="C3" s="90"/>
+      <c r="D3" s="90"/>
+      <c r="E3" s="90"/>
+      <c r="F3" s="90"/>
+      <c r="G3" s="90"/>
+      <c r="H3" s="90"/>
+      <c r="I3" s="90"/>
+      <c r="J3" s="90"/>
+      <c r="K3" s="90"/>
+      <c r="L3" s="90"/>
+      <c r="M3" s="90"/>
+      <c r="N3" s="90"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="44" t="s">
@@ -5559,40 +5616,40 @@
       </c>
     </row>
     <row r="2" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="88"/>
-      <c r="C2" s="88"/>
-      <c r="D2" s="88"/>
-      <c r="E2" s="88"/>
-      <c r="F2" s="88"/>
-      <c r="G2" s="88"/>
-      <c r="H2" s="88"/>
-      <c r="I2" s="88"/>
-      <c r="J2" s="88"/>
-      <c r="K2" s="88"/>
-      <c r="L2" s="88"/>
-      <c r="M2" s="88"/>
-      <c r="N2" s="88"/>
-      <c r="O2" s="88"/>
-      <c r="P2" s="88"/>
+      <c r="B2" s="89"/>
+      <c r="C2" s="89"/>
+      <c r="D2" s="89"/>
+      <c r="E2" s="89"/>
+      <c r="F2" s="89"/>
+      <c r="G2" s="89"/>
+      <c r="H2" s="89"/>
+      <c r="I2" s="89"/>
+      <c r="J2" s="89"/>
+      <c r="K2" s="89"/>
+      <c r="L2" s="89"/>
+      <c r="M2" s="89"/>
+      <c r="N2" s="89"/>
+      <c r="O2" s="89"/>
+      <c r="P2" s="89"/>
     </row>
     <row r="3" spans="2:16" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="89" t="s">
+      <c r="B3" s="90" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="89"/>
-      <c r="D3" s="89"/>
-      <c r="E3" s="89"/>
-      <c r="F3" s="89"/>
-      <c r="G3" s="89"/>
-      <c r="H3" s="89"/>
-      <c r="I3" s="89"/>
-      <c r="J3" s="89"/>
-      <c r="K3" s="89"/>
-      <c r="L3" s="89"/>
-      <c r="M3" s="89"/>
-      <c r="N3" s="89"/>
-      <c r="O3" s="89"/>
-      <c r="P3" s="89"/>
+      <c r="C3" s="90"/>
+      <c r="D3" s="90"/>
+      <c r="E3" s="90"/>
+      <c r="F3" s="90"/>
+      <c r="G3" s="90"/>
+      <c r="H3" s="90"/>
+      <c r="I3" s="90"/>
+      <c r="J3" s="90"/>
+      <c r="K3" s="90"/>
+      <c r="L3" s="90"/>
+      <c r="M3" s="90"/>
+      <c r="N3" s="90"/>
+      <c r="O3" s="90"/>
+      <c r="P3" s="90"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="44" t="s">
@@ -5671,40 +5728,40 @@
       </c>
     </row>
     <row r="2" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="88"/>
-      <c r="C2" s="88"/>
-      <c r="D2" s="88"/>
-      <c r="E2" s="88"/>
-      <c r="F2" s="88"/>
-      <c r="G2" s="88"/>
-      <c r="H2" s="88"/>
-      <c r="I2" s="88"/>
-      <c r="J2" s="88"/>
-      <c r="K2" s="88"/>
-      <c r="L2" s="88"/>
-      <c r="M2" s="88"/>
-      <c r="N2" s="88"/>
-      <c r="O2" s="88"/>
-      <c r="P2" s="88"/>
+      <c r="B2" s="89"/>
+      <c r="C2" s="89"/>
+      <c r="D2" s="89"/>
+      <c r="E2" s="89"/>
+      <c r="F2" s="89"/>
+      <c r="G2" s="89"/>
+      <c r="H2" s="89"/>
+      <c r="I2" s="89"/>
+      <c r="J2" s="89"/>
+      <c r="K2" s="89"/>
+      <c r="L2" s="89"/>
+      <c r="M2" s="89"/>
+      <c r="N2" s="89"/>
+      <c r="O2" s="89"/>
+      <c r="P2" s="89"/>
     </row>
     <row r="3" spans="2:16" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="89" t="s">
+      <c r="B3" s="90" t="s">
         <v>68</v>
       </c>
-      <c r="C3" s="89"/>
-      <c r="D3" s="89"/>
-      <c r="E3" s="89"/>
-      <c r="F3" s="89"/>
-      <c r="G3" s="89"/>
-      <c r="H3" s="89"/>
-      <c r="I3" s="89"/>
-      <c r="J3" s="89"/>
-      <c r="K3" s="89"/>
-      <c r="L3" s="89"/>
-      <c r="M3" s="89"/>
-      <c r="N3" s="89"/>
-      <c r="O3" s="89"/>
-      <c r="P3" s="89"/>
+      <c r="C3" s="90"/>
+      <c r="D3" s="90"/>
+      <c r="E3" s="90"/>
+      <c r="F3" s="90"/>
+      <c r="G3" s="90"/>
+      <c r="H3" s="90"/>
+      <c r="I3" s="90"/>
+      <c r="J3" s="90"/>
+      <c r="K3" s="90"/>
+      <c r="L3" s="90"/>
+      <c r="M3" s="90"/>
+      <c r="N3" s="90"/>
+      <c r="O3" s="90"/>
+      <c r="P3" s="90"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
@@ -5753,40 +5810,40 @@
       </c>
     </row>
     <row r="2" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="88"/>
-      <c r="C2" s="88"/>
-      <c r="D2" s="88"/>
-      <c r="E2" s="88"/>
-      <c r="F2" s="88"/>
-      <c r="G2" s="88"/>
-      <c r="H2" s="88"/>
-      <c r="I2" s="88"/>
-      <c r="J2" s="88"/>
-      <c r="K2" s="88"/>
-      <c r="L2" s="88"/>
-      <c r="M2" s="88"/>
-      <c r="N2" s="88"/>
-      <c r="O2" s="88"/>
-      <c r="P2" s="88"/>
+      <c r="B2" s="89"/>
+      <c r="C2" s="89"/>
+      <c r="D2" s="89"/>
+      <c r="E2" s="89"/>
+      <c r="F2" s="89"/>
+      <c r="G2" s="89"/>
+      <c r="H2" s="89"/>
+      <c r="I2" s="89"/>
+      <c r="J2" s="89"/>
+      <c r="K2" s="89"/>
+      <c r="L2" s="89"/>
+      <c r="M2" s="89"/>
+      <c r="N2" s="89"/>
+      <c r="O2" s="89"/>
+      <c r="P2" s="89"/>
     </row>
     <row r="3" spans="2:16" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="89" t="s">
+      <c r="B3" s="90" t="s">
         <v>71</v>
       </c>
-      <c r="C3" s="89"/>
-      <c r="D3" s="89"/>
-      <c r="E3" s="89"/>
-      <c r="F3" s="89"/>
-      <c r="G3" s="89"/>
-      <c r="H3" s="89"/>
-      <c r="I3" s="89"/>
-      <c r="J3" s="89"/>
-      <c r="K3" s="89"/>
-      <c r="L3" s="89"/>
-      <c r="M3" s="89"/>
-      <c r="N3" s="89"/>
-      <c r="O3" s="89"/>
-      <c r="P3" s="89"/>
+      <c r="C3" s="90"/>
+      <c r="D3" s="90"/>
+      <c r="E3" s="90"/>
+      <c r="F3" s="90"/>
+      <c r="G3" s="90"/>
+      <c r="H3" s="90"/>
+      <c r="I3" s="90"/>
+      <c r="J3" s="90"/>
+      <c r="K3" s="90"/>
+      <c r="L3" s="90"/>
+      <c r="M3" s="90"/>
+      <c r="N3" s="90"/>
+      <c r="O3" s="90"/>
+      <c r="P3" s="90"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
@@ -5840,36 +5897,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="88"/>
-      <c r="C2" s="88"/>
-      <c r="D2" s="88"/>
-      <c r="E2" s="88"/>
-      <c r="F2" s="88"/>
-      <c r="G2" s="88"/>
-      <c r="H2" s="88"/>
-      <c r="I2" s="88"/>
-      <c r="J2" s="88"/>
-      <c r="K2" s="88"/>
-      <c r="L2" s="88"/>
-      <c r="M2" s="88"/>
-      <c r="N2" s="88"/>
+      <c r="B2" s="89"/>
+      <c r="C2" s="89"/>
+      <c r="D2" s="89"/>
+      <c r="E2" s="89"/>
+      <c r="F2" s="89"/>
+      <c r="G2" s="89"/>
+      <c r="H2" s="89"/>
+      <c r="I2" s="89"/>
+      <c r="J2" s="89"/>
+      <c r="K2" s="89"/>
+      <c r="L2" s="89"/>
+      <c r="M2" s="89"/>
+      <c r="N2" s="89"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="89" t="s">
+      <c r="B3" s="90" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="89"/>
-      <c r="D3" s="89"/>
-      <c r="E3" s="89"/>
-      <c r="F3" s="89"/>
-      <c r="G3" s="89"/>
-      <c r="H3" s="89"/>
-      <c r="I3" s="89"/>
-      <c r="J3" s="89"/>
-      <c r="K3" s="89"/>
-      <c r="L3" s="89"/>
-      <c r="M3" s="89"/>
-      <c r="N3" s="89"/>
+      <c r="C3" s="90"/>
+      <c r="D3" s="90"/>
+      <c r="E3" s="90"/>
+      <c r="F3" s="90"/>
+      <c r="G3" s="90"/>
+      <c r="H3" s="90"/>
+      <c r="I3" s="90"/>
+      <c r="J3" s="90"/>
+      <c r="K3" s="90"/>
+      <c r="L3" s="90"/>
+      <c r="M3" s="90"/>
+      <c r="N3" s="90"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="44" t="s">
@@ -5958,40 +6015,40 @@
       </c>
     </row>
     <row r="2" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="88"/>
-      <c r="C2" s="88"/>
-      <c r="D2" s="88"/>
-      <c r="E2" s="88"/>
-      <c r="F2" s="88"/>
-      <c r="G2" s="88"/>
-      <c r="H2" s="88"/>
-      <c r="I2" s="88"/>
-      <c r="J2" s="88"/>
-      <c r="K2" s="88"/>
-      <c r="L2" s="88"/>
-      <c r="M2" s="88"/>
-      <c r="N2" s="88"/>
-      <c r="O2" s="88"/>
-      <c r="P2" s="88"/>
+      <c r="B2" s="89"/>
+      <c r="C2" s="89"/>
+      <c r="D2" s="89"/>
+      <c r="E2" s="89"/>
+      <c r="F2" s="89"/>
+      <c r="G2" s="89"/>
+      <c r="H2" s="89"/>
+      <c r="I2" s="89"/>
+      <c r="J2" s="89"/>
+      <c r="K2" s="89"/>
+      <c r="L2" s="89"/>
+      <c r="M2" s="89"/>
+      <c r="N2" s="89"/>
+      <c r="O2" s="89"/>
+      <c r="P2" s="89"/>
     </row>
     <row r="3" spans="2:16" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="89" t="s">
+      <c r="B3" s="90" t="s">
         <v>65</v>
       </c>
-      <c r="C3" s="89"/>
-      <c r="D3" s="89"/>
-      <c r="E3" s="89"/>
-      <c r="F3" s="89"/>
-      <c r="G3" s="89"/>
-      <c r="H3" s="89"/>
-      <c r="I3" s="89"/>
-      <c r="J3" s="89"/>
-      <c r="K3" s="89"/>
-      <c r="L3" s="89"/>
-      <c r="M3" s="89"/>
-      <c r="N3" s="89"/>
-      <c r="O3" s="89"/>
-      <c r="P3" s="89"/>
+      <c r="C3" s="90"/>
+      <c r="D3" s="90"/>
+      <c r="E3" s="90"/>
+      <c r="F3" s="90"/>
+      <c r="G3" s="90"/>
+      <c r="H3" s="90"/>
+      <c r="I3" s="90"/>
+      <c r="J3" s="90"/>
+      <c r="K3" s="90"/>
+      <c r="L3" s="90"/>
+      <c r="M3" s="90"/>
+      <c r="N3" s="90"/>
+      <c r="O3" s="90"/>
+      <c r="P3" s="90"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="45" t="s">
@@ -6043,36 +6100,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="88"/>
-      <c r="C2" s="88"/>
-      <c r="D2" s="88"/>
-      <c r="E2" s="88"/>
-      <c r="F2" s="88"/>
-      <c r="G2" s="88"/>
-      <c r="H2" s="88"/>
-      <c r="I2" s="88"/>
-      <c r="J2" s="88"/>
-      <c r="K2" s="88"/>
-      <c r="L2" s="88"/>
-      <c r="M2" s="88"/>
-      <c r="N2" s="88"/>
+      <c r="B2" s="89"/>
+      <c r="C2" s="89"/>
+      <c r="D2" s="89"/>
+      <c r="E2" s="89"/>
+      <c r="F2" s="89"/>
+      <c r="G2" s="89"/>
+      <c r="H2" s="89"/>
+      <c r="I2" s="89"/>
+      <c r="J2" s="89"/>
+      <c r="K2" s="89"/>
+      <c r="L2" s="89"/>
+      <c r="M2" s="89"/>
+      <c r="N2" s="89"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="89" t="s">
+      <c r="B3" s="90" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="89"/>
-      <c r="D3" s="89"/>
-      <c r="E3" s="89"/>
-      <c r="F3" s="89"/>
-      <c r="G3" s="89"/>
-      <c r="H3" s="89"/>
-      <c r="I3" s="89"/>
-      <c r="J3" s="89"/>
-      <c r="K3" s="89"/>
-      <c r="L3" s="89"/>
-      <c r="M3" s="89"/>
-      <c r="N3" s="89"/>
+      <c r="C3" s="90"/>
+      <c r="D3" s="90"/>
+      <c r="E3" s="90"/>
+      <c r="F3" s="90"/>
+      <c r="G3" s="90"/>
+      <c r="H3" s="90"/>
+      <c r="I3" s="90"/>
+      <c r="J3" s="90"/>
+      <c r="K3" s="90"/>
+      <c r="L3" s="90"/>
+      <c r="M3" s="90"/>
+      <c r="N3" s="90"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">

</xml_diff>

<commit_message>
TRIEDA-1639 - Adicionando coluna de Disciplina Aula, que mostra a disciplina de fato lecionada.
</commit_message>
<xml_diff>
--- a/code/client/web/src/main/resources/templateExport.xlsx
+++ b/code/client/web/src/main/resources/templateExport.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="17070" windowHeight="5370" tabRatio="797" firstSheet="16" activeTab="21"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="17070" windowHeight="5370" tabRatio="797" firstSheet="22" activeTab="28"/>
   </bookViews>
   <sheets>
     <sheet name="Campi" sheetId="3" r:id="rId1"/>
@@ -1215,7 +1215,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="184">
   <si>
     <t>Planilha de Unidades</t>
   </si>
@@ -1764,6 +1764,9 @@
   </si>
   <si>
     <t>Custo Docente / Receita %</t>
+  </si>
+  <si>
+    <t>Disciplina Aula</t>
   </si>
 </sst>
 </file>
@@ -2046,7 +2049,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -2152,12 +2155,34 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="112">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2372,9 +2397,6 @@
     <xf numFmtId="0" fontId="8" fillId="28" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="28" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2407,6 +2429,9 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="173" fontId="6" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2434,6 +2459,9 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2452,11 +2480,26 @@
     <xf numFmtId="0" fontId="8" fillId="28" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="173" fontId="6" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4072,7 +4115,7 @@
       <c r="I6" s="9"/>
       <c r="J6" s="9"/>
       <c r="K6" s="9"/>
-      <c r="L6" s="79"/>
+      <c r="L6" s="78"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -4167,8 +4210,8 @@
       <c r="E6" s="9"/>
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
-      <c r="H6" s="79"/>
-      <c r="I6" s="79"/>
+      <c r="H6" s="78"/>
+      <c r="I6" s="78"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -4184,7 +4227,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:T6"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="I1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
@@ -4226,7 +4269,7 @@
       <c r="H2" s="89"/>
       <c r="I2" s="89"/>
       <c r="J2" s="89"/>
-      <c r="K2" s="85"/>
+      <c r="K2" s="84"/>
     </row>
     <row r="3" spans="2:20" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="90" t="s">
@@ -4240,64 +4283,64 @@
       <c r="H3" s="90"/>
       <c r="I3" s="90"/>
       <c r="J3" s="90"/>
-      <c r="K3" s="84"/>
+      <c r="K3" s="83"/>
     </row>
     <row r="5" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B5" s="81" t="s">
+      <c r="B5" s="80" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="80" t="s">
+      <c r="C5" s="79" t="s">
         <v>157</v>
       </c>
-      <c r="D5" s="80" t="s">
+      <c r="D5" s="79" t="s">
         <v>143</v>
       </c>
-      <c r="E5" s="80" t="s">
+      <c r="E5" s="79" t="s">
         <v>158</v>
       </c>
-      <c r="F5" s="80" t="s">
+      <c r="F5" s="79" t="s">
         <v>159</v>
       </c>
-      <c r="G5" s="80" t="s">
+      <c r="G5" s="79" t="s">
         <v>160</v>
       </c>
-      <c r="H5" s="80" t="s">
+      <c r="H5" s="79" t="s">
         <v>161</v>
       </c>
-      <c r="I5" s="80" t="s">
+      <c r="I5" s="79" t="s">
         <v>162</v>
       </c>
-      <c r="J5" s="80" t="s">
+      <c r="J5" s="79" t="s">
         <v>163</v>
       </c>
-      <c r="K5" s="80" t="s">
+      <c r="K5" s="79" t="s">
         <v>164</v>
       </c>
-      <c r="L5" s="80" t="s">
+      <c r="L5" s="79" t="s">
         <v>165</v>
       </c>
-      <c r="M5" s="80" t="s">
+      <c r="M5" s="79" t="s">
         <v>166</v>
       </c>
-      <c r="N5" s="80" t="s">
+      <c r="N5" s="79" t="s">
         <v>167</v>
       </c>
-      <c r="O5" s="88" t="s">
+      <c r="O5" s="87" t="s">
         <v>177</v>
       </c>
-      <c r="P5" s="88" t="s">
+      <c r="P5" s="87" t="s">
         <v>178</v>
       </c>
-      <c r="Q5" s="88" t="s">
+      <c r="Q5" s="87" t="s">
         <v>182</v>
       </c>
-      <c r="R5" s="88" t="s">
+      <c r="R5" s="87" t="s">
         <v>179</v>
       </c>
-      <c r="S5" s="88" t="s">
+      <c r="S5" s="87" t="s">
         <v>180</v>
       </c>
-      <c r="T5" s="88" t="s">
+      <c r="T5" s="87" t="s">
         <v>181</v>
       </c>
     </row>
@@ -4309,18 +4352,18 @@
       <c r="F6" s="8"/>
       <c r="G6" s="9"/>
       <c r="H6" s="8"/>
-      <c r="I6" s="79"/>
-      <c r="J6" s="82"/>
-      <c r="K6" s="79"/>
-      <c r="L6" s="79"/>
-      <c r="M6" s="79"/>
-      <c r="N6" s="83"/>
-      <c r="O6" s="82"/>
-      <c r="P6" s="105"/>
-      <c r="Q6" s="79"/>
-      <c r="R6" s="82"/>
-      <c r="S6" s="82"/>
-      <c r="T6" s="83"/>
+      <c r="I6" s="78"/>
+      <c r="J6" s="81"/>
+      <c r="K6" s="78"/>
+      <c r="L6" s="78"/>
+      <c r="M6" s="78"/>
+      <c r="N6" s="82"/>
+      <c r="O6" s="81"/>
+      <c r="P6" s="88"/>
+      <c r="Q6" s="78"/>
+      <c r="R6" s="81"/>
+      <c r="S6" s="81"/>
+      <c r="T6" s="82"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -4386,16 +4429,16 @@
       <c r="K3" s="90"/>
     </row>
     <row r="4" spans="2:11" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B4" s="86"/>
-      <c r="C4" s="86"/>
-      <c r="D4" s="86"/>
-      <c r="E4" s="86"/>
-      <c r="F4" s="86"/>
-      <c r="G4" s="86"/>
-      <c r="H4" s="86"/>
-      <c r="I4" s="86"/>
-      <c r="J4" s="86"/>
-      <c r="K4" s="86"/>
+      <c r="B4" s="85"/>
+      <c r="C4" s="85"/>
+      <c r="D4" s="85"/>
+      <c r="E4" s="85"/>
+      <c r="F4" s="85"/>
+      <c r="G4" s="85"/>
+      <c r="H4" s="85"/>
+      <c r="I4" s="85"/>
+      <c r="J4" s="85"/>
+      <c r="K4" s="85"/>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="H5" s="92" t="s">
@@ -4408,34 +4451,34 @@
       <c r="K5" s="93"/>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="87" t="s">
+      <c r="B6" s="86" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="87" t="s">
+      <c r="C6" s="86" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="87" t="s">
+      <c r="D6" s="86" t="s">
         <v>169</v>
       </c>
-      <c r="E6" s="87" t="s">
+      <c r="E6" s="86" t="s">
         <v>170</v>
       </c>
-      <c r="F6" s="87" t="s">
+      <c r="F6" s="86" t="s">
         <v>116</v>
       </c>
-      <c r="G6" s="87" t="s">
+      <c r="G6" s="86" t="s">
         <v>116</v>
       </c>
-      <c r="H6" s="87" t="s">
+      <c r="H6" s="86" t="s">
         <v>171</v>
       </c>
-      <c r="I6" s="87" t="s">
+      <c r="I6" s="86" t="s">
         <v>172</v>
       </c>
-      <c r="J6" s="87" t="s">
+      <c r="J6" s="86" t="s">
         <v>173</v>
       </c>
-      <c r="K6" s="87" t="s">
+      <c r="K6" s="86" t="s">
         <v>174</v>
       </c>
     </row>
@@ -4447,9 +4490,9 @@
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
       <c r="H7" s="8"/>
-      <c r="I7" s="83"/>
-      <c r="J7" s="83"/>
-      <c r="K7" s="83"/>
+      <c r="I7" s="82"/>
+      <c r="J7" s="82"/>
+      <c r="K7" s="82"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -5150,10 +5193,10 @@
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:X8"/>
+  <dimension ref="B1:Y8"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="Y9" sqref="Y9"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="Y8" sqref="Y8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5180,14 +5223,15 @@
     <col min="22" max="22" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="4.7109375" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:24" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:25" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="2:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="89"/>
       <c r="C2" s="89"/>
       <c r="D2" s="89"/>
@@ -5206,7 +5250,7 @@
       <c r="Q2" s="56"/>
       <c r="R2" s="56"/>
     </row>
-    <row r="3" spans="2:24" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:25" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="90" t="s">
         <v>111</v>
       </c>
@@ -5227,75 +5271,77 @@
       <c r="Q3" s="57"/>
       <c r="R3" s="57"/>
     </row>
-    <row r="5" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B5" s="98" t="s">
+    <row r="5" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B5" s="99" t="s">
         <v>112</v>
       </c>
-      <c r="C5" s="99"/>
-      <c r="D5" s="99"/>
-      <c r="E5" s="99"/>
-      <c r="F5" s="99"/>
-      <c r="G5" s="99"/>
-      <c r="H5" s="99"/>
-      <c r="I5" s="99"/>
-      <c r="J5" s="99"/>
-      <c r="K5" s="99"/>
-      <c r="L5" s="100"/>
-      <c r="M5" s="98" t="s">
+      <c r="C5" s="100"/>
+      <c r="D5" s="100"/>
+      <c r="E5" s="100"/>
+      <c r="F5" s="100"/>
+      <c r="G5" s="100"/>
+      <c r="H5" s="100"/>
+      <c r="I5" s="100"/>
+      <c r="J5" s="100"/>
+      <c r="K5" s="100"/>
+      <c r="L5" s="101"/>
+      <c r="M5" s="99" t="s">
         <v>113</v>
       </c>
-      <c r="N5" s="99"/>
-      <c r="O5" s="99"/>
-      <c r="P5" s="99"/>
-      <c r="Q5" s="99"/>
-      <c r="R5" s="99"/>
-      <c r="S5" s="99"/>
-      <c r="T5" s="99"/>
-      <c r="U5" s="99"/>
-      <c r="V5" s="99"/>
-      <c r="W5" s="99"/>
+      <c r="N5" s="100"/>
+      <c r="O5" s="100"/>
+      <c r="P5" s="100"/>
+      <c r="Q5" s="100"/>
+      <c r="R5" s="100"/>
+      <c r="S5" s="100"/>
+      <c r="T5" s="100"/>
+      <c r="U5" s="100"/>
+      <c r="V5" s="100"/>
+      <c r="W5" s="100"/>
       <c r="X5" s="100"/>
-    </row>
-    <row r="6" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B6" s="104"/>
-      <c r="C6" s="104"/>
-      <c r="D6" s="104"/>
-      <c r="E6" s="104"/>
-      <c r="F6" s="101" t="s">
+      <c r="Y5" s="101"/>
+    </row>
+    <row r="6" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B6" s="98"/>
+      <c r="C6" s="98"/>
+      <c r="D6" s="98"/>
+      <c r="E6" s="98"/>
+      <c r="F6" s="102" t="s">
         <v>27</v>
       </c>
-      <c r="G6" s="102"/>
-      <c r="H6" s="102"/>
-      <c r="I6" s="103"/>
-      <c r="J6" s="98" t="s">
+      <c r="G6" s="103"/>
+      <c r="H6" s="103"/>
+      <c r="I6" s="104"/>
+      <c r="J6" s="99" t="s">
         <v>30</v>
       </c>
-      <c r="K6" s="99"/>
-      <c r="L6" s="100"/>
-      <c r="M6" s="76"/>
-      <c r="N6" s="98" t="s">
+      <c r="K6" s="100"/>
+      <c r="L6" s="101"/>
+      <c r="M6" s="105"/>
+      <c r="N6" s="106" t="s">
         <v>42</v>
       </c>
-      <c r="O6" s="100"/>
-      <c r="P6" s="98" t="s">
+      <c r="O6" s="107"/>
+      <c r="P6" s="106" t="s">
         <v>106</v>
       </c>
-      <c r="Q6" s="99"/>
-      <c r="R6" s="100"/>
-      <c r="S6" s="76"/>
-      <c r="T6" s="98" t="s">
+      <c r="Q6" s="108"/>
+      <c r="R6" s="107"/>
+      <c r="S6" s="105"/>
+      <c r="T6" s="106" t="s">
         <v>123</v>
       </c>
-      <c r="U6" s="100"/>
-      <c r="V6" s="104"/>
-      <c r="W6" s="104"/>
-      <c r="X6" s="104"/>
-    </row>
-    <row r="7" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="U6" s="107"/>
+      <c r="V6" s="109"/>
+      <c r="W6" s="110"/>
+      <c r="X6" s="110"/>
+      <c r="Y6" s="111"/>
+    </row>
+    <row r="7" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B7" s="75" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="77" t="s">
+      <c r="C7" s="76" t="s">
         <v>28</v>
       </c>
       <c r="D7" s="75" t="s">
@@ -5304,65 +5350,68 @@
       <c r="E7" s="75" t="s">
         <v>29</v>
       </c>
-      <c r="F7" s="78" t="s">
+      <c r="F7" s="77" t="s">
         <v>117</v>
       </c>
-      <c r="G7" s="78" t="s">
+      <c r="G7" s="77" t="s">
         <v>121</v>
       </c>
-      <c r="H7" s="78" t="s">
+      <c r="H7" s="77" t="s">
         <v>122</v>
       </c>
-      <c r="I7" s="78" t="s">
+      <c r="I7" s="77" t="s">
         <v>118</v>
       </c>
-      <c r="J7" s="78" t="s">
+      <c r="J7" s="77" t="s">
         <v>114</v>
       </c>
-      <c r="K7" s="78" t="s">
+      <c r="K7" s="77" t="s">
         <v>115</v>
       </c>
-      <c r="L7" s="78" t="s">
+      <c r="L7" s="77" t="s">
         <v>116</v>
       </c>
-      <c r="M7" s="77" t="s">
+      <c r="M7" s="76" t="s">
         <v>53</v>
       </c>
-      <c r="N7" s="78" t="s">
+      <c r="N7" s="77" t="s">
         <v>119</v>
       </c>
-      <c r="O7" s="78" t="s">
+      <c r="O7" s="77" t="s">
         <v>120</v>
       </c>
-      <c r="P7" s="78" t="s">
+      <c r="P7" s="77" t="s">
         <v>114</v>
       </c>
-      <c r="Q7" s="78" t="s">
+      <c r="Q7" s="77" t="s">
         <v>115</v>
       </c>
-      <c r="R7" s="78" t="s">
+      <c r="R7" s="77" t="s">
         <v>116</v>
       </c>
       <c r="S7" s="75" t="s">
         <v>141</v>
       </c>
-      <c r="T7" s="78" t="s">
+      <c r="T7" s="77" t="s">
         <v>124</v>
       </c>
-      <c r="U7" s="78" t="s">
+      <c r="U7" s="77" t="s">
         <v>125</v>
       </c>
-      <c r="V7" s="77" t="s">
+      <c r="V7" s="76" t="s">
         <v>70</v>
       </c>
-      <c r="W7" s="77" t="s">
+      <c r="W7" s="76" t="s">
         <v>32</v>
       </c>
       <c r="X7" s="75" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="8" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="Y7" s="75" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="8" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -5386,10 +5435,13 @@
       <c r="V8" s="2"/>
       <c r="W8" s="2"/>
       <c r="X8" s="2"/>
+      <c r="Y8" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="V6:X6"/>
+    <mergeCell ref="T6:U6"/>
+    <mergeCell ref="M5:Y5"/>
+    <mergeCell ref="V6:Y6"/>
     <mergeCell ref="B2:P2"/>
     <mergeCell ref="B3:P3"/>
     <mergeCell ref="B5:L5"/>
@@ -5398,10 +5450,9 @@
     <mergeCell ref="N6:O6"/>
     <mergeCell ref="P6:R6"/>
     <mergeCell ref="B6:E6"/>
-    <mergeCell ref="M5:X5"/>
-    <mergeCell ref="T6:U6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
TRIEDA-1617 - Merge do branch EquivalenciaPorCuso com o TRUNK
</commit_message>
<xml_diff>
--- a/code/client/web/src/main/resources/templateExport.xlsx
+++ b/code/client/web/src/main/resources/templateExport.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="17070" windowHeight="5370" tabRatio="797" firstSheet="22" activeTab="28"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="17070" windowHeight="5370" tabRatio="797" firstSheet="5" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Campi" sheetId="3" r:id="rId1"/>
@@ -980,6 +980,20 @@
         </r>
       </text>
     </comment>
+    <comment ref="D5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Código do Curso relacionado a equivalencia, Vazio significa uma equivalencia geral</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -1215,7 +1229,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="184">
   <si>
     <t>Planilha de Unidades</t>
   </si>
@@ -1777,7 +1791,7 @@
     <numFmt numFmtId="165" formatCode="&quot;R$&quot;\ #,##0.00"/>
     <numFmt numFmtId="173" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1877,6 +1891,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="29">
@@ -2182,7 +2203,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="112">
+  <cellXfs count="114">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2432,6 +2453,9 @@
     <xf numFmtId="173" fontId="6" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2459,47 +2483,50 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="28" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2828,38 +2855,38 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="89" t="s">
+      <c r="B2" s="90" t="s">
         <v>96</v>
       </c>
-      <c r="C2" s="89"/>
-      <c r="D2" s="89"/>
-      <c r="E2" s="89"/>
-      <c r="F2" s="89"/>
-      <c r="G2" s="89"/>
-      <c r="H2" s="89"/>
-      <c r="I2" s="89"/>
-      <c r="J2" s="89"/>
-      <c r="K2" s="89"/>
-      <c r="L2" s="89"/>
-      <c r="M2" s="89"/>
-      <c r="N2" s="89"/>
+      <c r="C2" s="90"/>
+      <c r="D2" s="90"/>
+      <c r="E2" s="90"/>
+      <c r="F2" s="90"/>
+      <c r="G2" s="90"/>
+      <c r="H2" s="90"/>
+      <c r="I2" s="90"/>
+      <c r="J2" s="90"/>
+      <c r="K2" s="90"/>
+      <c r="L2" s="90"/>
+      <c r="M2" s="90"/>
+      <c r="N2" s="90"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="90" t="s">
+      <c r="B3" s="91" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="90"/>
-      <c r="D3" s="90"/>
-      <c r="E3" s="90"/>
-      <c r="F3" s="90"/>
-      <c r="G3" s="90"/>
-      <c r="H3" s="90"/>
-      <c r="I3" s="90"/>
-      <c r="J3" s="90"/>
-      <c r="K3" s="90"/>
-      <c r="L3" s="90"/>
-      <c r="M3" s="90"/>
-      <c r="N3" s="90"/>
+      <c r="C3" s="91"/>
+      <c r="D3" s="91"/>
+      <c r="E3" s="91"/>
+      <c r="F3" s="91"/>
+      <c r="G3" s="91"/>
+      <c r="H3" s="91"/>
+      <c r="I3" s="91"/>
+      <c r="J3" s="91"/>
+      <c r="K3" s="91"/>
+      <c r="L3" s="91"/>
+      <c r="M3" s="91"/>
+      <c r="N3" s="91"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="44" t="s">
@@ -2927,36 +2954,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="89"/>
-      <c r="C2" s="89"/>
-      <c r="D2" s="89"/>
-      <c r="E2" s="89"/>
-      <c r="F2" s="89"/>
-      <c r="G2" s="89"/>
-      <c r="H2" s="89"/>
-      <c r="I2" s="89"/>
-      <c r="J2" s="89"/>
-      <c r="K2" s="89"/>
-      <c r="L2" s="89"/>
-      <c r="M2" s="89"/>
-      <c r="N2" s="89"/>
+      <c r="B2" s="90"/>
+      <c r="C2" s="90"/>
+      <c r="D2" s="90"/>
+      <c r="E2" s="90"/>
+      <c r="F2" s="90"/>
+      <c r="G2" s="90"/>
+      <c r="H2" s="90"/>
+      <c r="I2" s="90"/>
+      <c r="J2" s="90"/>
+      <c r="K2" s="90"/>
+      <c r="L2" s="90"/>
+      <c r="M2" s="90"/>
+      <c r="N2" s="90"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="90" t="s">
+      <c r="B3" s="91" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="90"/>
-      <c r="D3" s="90"/>
-      <c r="E3" s="90"/>
-      <c r="F3" s="90"/>
-      <c r="G3" s="90"/>
-      <c r="H3" s="90"/>
-      <c r="I3" s="90"/>
-      <c r="J3" s="90"/>
-      <c r="K3" s="90"/>
-      <c r="L3" s="90"/>
-      <c r="M3" s="90"/>
-      <c r="N3" s="90"/>
+      <c r="C3" s="91"/>
+      <c r="D3" s="91"/>
+      <c r="E3" s="91"/>
+      <c r="F3" s="91"/>
+      <c r="G3" s="91"/>
+      <c r="H3" s="91"/>
+      <c r="I3" s="91"/>
+      <c r="J3" s="91"/>
+      <c r="K3" s="91"/>
+      <c r="L3" s="91"/>
+      <c r="M3" s="91"/>
+      <c r="N3" s="91"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -3025,36 +3052,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="89"/>
-      <c r="C2" s="89"/>
-      <c r="D2" s="89"/>
-      <c r="E2" s="89"/>
-      <c r="F2" s="89"/>
-      <c r="G2" s="89"/>
-      <c r="H2" s="89"/>
-      <c r="I2" s="89"/>
-      <c r="J2" s="89"/>
-      <c r="K2" s="89"/>
-      <c r="L2" s="89"/>
-      <c r="M2" s="89"/>
-      <c r="N2" s="89"/>
+      <c r="B2" s="90"/>
+      <c r="C2" s="90"/>
+      <c r="D2" s="90"/>
+      <c r="E2" s="90"/>
+      <c r="F2" s="90"/>
+      <c r="G2" s="90"/>
+      <c r="H2" s="90"/>
+      <c r="I2" s="90"/>
+      <c r="J2" s="90"/>
+      <c r="K2" s="90"/>
+      <c r="L2" s="90"/>
+      <c r="M2" s="90"/>
+      <c r="N2" s="90"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="90" t="s">
+      <c r="B3" s="91" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="90"/>
-      <c r="D3" s="90"/>
-      <c r="E3" s="90"/>
-      <c r="F3" s="90"/>
-      <c r="G3" s="90"/>
-      <c r="H3" s="90"/>
-      <c r="I3" s="90"/>
-      <c r="J3" s="90"/>
-      <c r="K3" s="90"/>
-      <c r="L3" s="90"/>
-      <c r="M3" s="90"/>
-      <c r="N3" s="90"/>
+      <c r="C3" s="91"/>
+      <c r="D3" s="91"/>
+      <c r="E3" s="91"/>
+      <c r="F3" s="91"/>
+      <c r="G3" s="91"/>
+      <c r="H3" s="91"/>
+      <c r="I3" s="91"/>
+      <c r="J3" s="91"/>
+      <c r="K3" s="91"/>
+      <c r="L3" s="91"/>
+      <c r="M3" s="91"/>
+      <c r="N3" s="91"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -3139,18 +3166,18 @@
       </c>
     </row>
     <row r="2" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="89"/>
-      <c r="C2" s="89"/>
-      <c r="D2" s="89"/>
-      <c r="E2" s="89"/>
+      <c r="B2" s="90"/>
+      <c r="C2" s="90"/>
+      <c r="D2" s="90"/>
+      <c r="E2" s="90"/>
     </row>
     <row r="3" spans="2:5" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="90" t="s">
+      <c r="B3" s="91" t="s">
         <v>126</v>
       </c>
-      <c r="C3" s="90"/>
-      <c r="D3" s="90"/>
-      <c r="E3" s="90"/>
+      <c r="C3" s="91"/>
+      <c r="D3" s="91"/>
+      <c r="E3" s="91"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="60" t="s">
@@ -3203,36 +3230,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="89"/>
-      <c r="C2" s="89"/>
-      <c r="D2" s="89"/>
-      <c r="E2" s="89"/>
-      <c r="F2" s="89"/>
-      <c r="G2" s="89"/>
-      <c r="H2" s="89"/>
-      <c r="I2" s="89"/>
-      <c r="J2" s="89"/>
-      <c r="K2" s="89"/>
-      <c r="L2" s="89"/>
-      <c r="M2" s="89"/>
-      <c r="N2" s="89"/>
+      <c r="B2" s="90"/>
+      <c r="C2" s="90"/>
+      <c r="D2" s="90"/>
+      <c r="E2" s="90"/>
+      <c r="F2" s="90"/>
+      <c r="G2" s="90"/>
+      <c r="H2" s="90"/>
+      <c r="I2" s="90"/>
+      <c r="J2" s="90"/>
+      <c r="K2" s="90"/>
+      <c r="L2" s="90"/>
+      <c r="M2" s="90"/>
+      <c r="N2" s="90"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="90" t="s">
+      <c r="B3" s="91" t="s">
         <v>100</v>
       </c>
-      <c r="C3" s="90"/>
-      <c r="D3" s="90"/>
-      <c r="E3" s="90"/>
-      <c r="F3" s="90"/>
-      <c r="G3" s="90"/>
-      <c r="H3" s="90"/>
-      <c r="I3" s="90"/>
-      <c r="J3" s="90"/>
-      <c r="K3" s="90"/>
-      <c r="L3" s="90"/>
-      <c r="M3" s="90"/>
-      <c r="N3" s="90"/>
+      <c r="C3" s="91"/>
+      <c r="D3" s="91"/>
+      <c r="E3" s="91"/>
+      <c r="F3" s="91"/>
+      <c r="G3" s="91"/>
+      <c r="H3" s="91"/>
+      <c r="I3" s="91"/>
+      <c r="J3" s="91"/>
+      <c r="K3" s="91"/>
+      <c r="L3" s="91"/>
+      <c r="M3" s="91"/>
+      <c r="N3" s="91"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -3265,10 +3292,10 @@
       <c r="K5" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="L5" s="91" t="s">
+      <c r="L5" s="92" t="s">
         <v>110</v>
       </c>
-      <c r="M5" s="91"/>
+      <c r="M5" s="92"/>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
@@ -3320,38 +3347,38 @@
       </c>
     </row>
     <row r="2" spans="2:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="89"/>
-      <c r="C2" s="89"/>
-      <c r="D2" s="89"/>
-      <c r="E2" s="89"/>
-      <c r="F2" s="89"/>
-      <c r="G2" s="89"/>
-      <c r="H2" s="89"/>
-      <c r="I2" s="89"/>
-      <c r="J2" s="89"/>
-      <c r="K2" s="89"/>
-      <c r="L2" s="89"/>
-      <c r="M2" s="89"/>
-      <c r="N2" s="89"/>
-      <c r="O2" s="89"/>
+      <c r="B2" s="90"/>
+      <c r="C2" s="90"/>
+      <c r="D2" s="90"/>
+      <c r="E2" s="90"/>
+      <c r="F2" s="90"/>
+      <c r="G2" s="90"/>
+      <c r="H2" s="90"/>
+      <c r="I2" s="90"/>
+      <c r="J2" s="90"/>
+      <c r="K2" s="90"/>
+      <c r="L2" s="90"/>
+      <c r="M2" s="90"/>
+      <c r="N2" s="90"/>
+      <c r="O2" s="90"/>
     </row>
     <row r="3" spans="2:15" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="90" t="s">
+      <c r="B3" s="91" t="s">
         <v>73</v>
       </c>
-      <c r="C3" s="90"/>
-      <c r="D3" s="90"/>
-      <c r="E3" s="90"/>
-      <c r="F3" s="90"/>
-      <c r="G3" s="90"/>
-      <c r="H3" s="90"/>
-      <c r="I3" s="90"/>
-      <c r="J3" s="90"/>
-      <c r="K3" s="90"/>
-      <c r="L3" s="90"/>
-      <c r="M3" s="90"/>
-      <c r="N3" s="90"/>
-      <c r="O3" s="90"/>
+      <c r="C3" s="91"/>
+      <c r="D3" s="91"/>
+      <c r="E3" s="91"/>
+      <c r="F3" s="91"/>
+      <c r="G3" s="91"/>
+      <c r="H3" s="91"/>
+      <c r="I3" s="91"/>
+      <c r="J3" s="91"/>
+      <c r="K3" s="91"/>
+      <c r="L3" s="91"/>
+      <c r="M3" s="91"/>
+      <c r="N3" s="91"/>
+      <c r="O3" s="91"/>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -3430,18 +3457,18 @@
       </c>
     </row>
     <row r="2" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="89"/>
-      <c r="C2" s="89"/>
-      <c r="D2" s="89"/>
-      <c r="E2" s="89"/>
+      <c r="B2" s="90"/>
+      <c r="C2" s="90"/>
+      <c r="D2" s="90"/>
+      <c r="E2" s="90"/>
     </row>
     <row r="3" spans="2:5" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="90" t="s">
+      <c r="B3" s="91" t="s">
         <v>131</v>
       </c>
-      <c r="C3" s="90"/>
-      <c r="D3" s="90"/>
-      <c r="E3" s="90"/>
+      <c r="C3" s="91"/>
+      <c r="D3" s="91"/>
+      <c r="E3" s="91"/>
     </row>
     <row r="4" spans="2:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="64"/>
@@ -3503,36 +3530,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="89"/>
-      <c r="C2" s="89"/>
-      <c r="D2" s="89"/>
-      <c r="E2" s="89"/>
-      <c r="F2" s="89"/>
-      <c r="G2" s="89"/>
-      <c r="H2" s="89"/>
-      <c r="I2" s="89"/>
-      <c r="J2" s="89"/>
-      <c r="K2" s="89"/>
-      <c r="L2" s="89"/>
-      <c r="M2" s="89"/>
-      <c r="N2" s="89"/>
+      <c r="B2" s="90"/>
+      <c r="C2" s="90"/>
+      <c r="D2" s="90"/>
+      <c r="E2" s="90"/>
+      <c r="F2" s="90"/>
+      <c r="G2" s="90"/>
+      <c r="H2" s="90"/>
+      <c r="I2" s="90"/>
+      <c r="J2" s="90"/>
+      <c r="K2" s="90"/>
+      <c r="L2" s="90"/>
+      <c r="M2" s="90"/>
+      <c r="N2" s="90"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="90" t="s">
+      <c r="B3" s="91" t="s">
         <v>69</v>
       </c>
-      <c r="C3" s="90"/>
-      <c r="D3" s="90"/>
-      <c r="E3" s="90"/>
-      <c r="F3" s="90"/>
-      <c r="G3" s="90"/>
-      <c r="H3" s="90"/>
-      <c r="I3" s="90"/>
-      <c r="J3" s="90"/>
-      <c r="K3" s="90"/>
-      <c r="L3" s="90"/>
-      <c r="M3" s="90"/>
-      <c r="N3" s="90"/>
+      <c r="C3" s="91"/>
+      <c r="D3" s="91"/>
+      <c r="E3" s="91"/>
+      <c r="F3" s="91"/>
+      <c r="G3" s="91"/>
+      <c r="H3" s="91"/>
+      <c r="I3" s="91"/>
+      <c r="J3" s="91"/>
+      <c r="K3" s="91"/>
+      <c r="L3" s="91"/>
+      <c r="M3" s="91"/>
+      <c r="N3" s="91"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -3587,36 +3614,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="89"/>
-      <c r="C2" s="89"/>
-      <c r="D2" s="89"/>
-      <c r="E2" s="89"/>
-      <c r="F2" s="89"/>
-      <c r="G2" s="89"/>
-      <c r="H2" s="89"/>
-      <c r="I2" s="89"/>
-      <c r="J2" s="89"/>
-      <c r="K2" s="89"/>
-      <c r="L2" s="89"/>
-      <c r="M2" s="89"/>
-      <c r="N2" s="89"/>
+      <c r="B2" s="90"/>
+      <c r="C2" s="90"/>
+      <c r="D2" s="90"/>
+      <c r="E2" s="90"/>
+      <c r="F2" s="90"/>
+      <c r="G2" s="90"/>
+      <c r="H2" s="90"/>
+      <c r="I2" s="90"/>
+      <c r="J2" s="90"/>
+      <c r="K2" s="90"/>
+      <c r="L2" s="90"/>
+      <c r="M2" s="90"/>
+      <c r="N2" s="90"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="90" t="s">
+      <c r="B3" s="91" t="s">
         <v>74</v>
       </c>
-      <c r="C3" s="90"/>
-      <c r="D3" s="90"/>
-      <c r="E3" s="90"/>
-      <c r="F3" s="90"/>
-      <c r="G3" s="90"/>
-      <c r="H3" s="90"/>
-      <c r="I3" s="90"/>
-      <c r="J3" s="90"/>
-      <c r="K3" s="90"/>
-      <c r="L3" s="90"/>
-      <c r="M3" s="90"/>
-      <c r="N3" s="90"/>
+      <c r="C3" s="91"/>
+      <c r="D3" s="91"/>
+      <c r="E3" s="91"/>
+      <c r="F3" s="91"/>
+      <c r="G3" s="91"/>
+      <c r="H3" s="91"/>
+      <c r="I3" s="91"/>
+      <c r="J3" s="91"/>
+      <c r="K3" s="91"/>
+      <c r="L3" s="91"/>
+      <c r="M3" s="91"/>
+      <c r="N3" s="91"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -3685,40 +3712,40 @@
       </c>
     </row>
     <row r="2" spans="2:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="89"/>
-      <c r="C2" s="89"/>
-      <c r="D2" s="89"/>
-      <c r="E2" s="89"/>
-      <c r="F2" s="89"/>
-      <c r="G2" s="89"/>
-      <c r="H2" s="89"/>
-      <c r="I2" s="89"/>
-      <c r="J2" s="89"/>
-      <c r="K2" s="89"/>
-      <c r="L2" s="89"/>
-      <c r="M2" s="89"/>
-      <c r="N2" s="89"/>
-      <c r="O2" s="89"/>
-      <c r="P2" s="89"/>
+      <c r="B2" s="90"/>
+      <c r="C2" s="90"/>
+      <c r="D2" s="90"/>
+      <c r="E2" s="90"/>
+      <c r="F2" s="90"/>
+      <c r="G2" s="90"/>
+      <c r="H2" s="90"/>
+      <c r="I2" s="90"/>
+      <c r="J2" s="90"/>
+      <c r="K2" s="90"/>
+      <c r="L2" s="90"/>
+      <c r="M2" s="90"/>
+      <c r="N2" s="90"/>
+      <c r="O2" s="90"/>
+      <c r="P2" s="90"/>
     </row>
     <row r="3" spans="2:18" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="90" t="s">
+      <c r="B3" s="91" t="s">
         <v>63</v>
       </c>
-      <c r="C3" s="90"/>
-      <c r="D3" s="90"/>
-      <c r="E3" s="90"/>
-      <c r="F3" s="90"/>
-      <c r="G3" s="90"/>
-      <c r="H3" s="90"/>
-      <c r="I3" s="90"/>
-      <c r="J3" s="90"/>
-      <c r="K3" s="90"/>
-      <c r="L3" s="90"/>
-      <c r="M3" s="90"/>
-      <c r="N3" s="90"/>
-      <c r="O3" s="90"/>
-      <c r="P3" s="90"/>
+      <c r="C3" s="91"/>
+      <c r="D3" s="91"/>
+      <c r="E3" s="91"/>
+      <c r="F3" s="91"/>
+      <c r="G3" s="91"/>
+      <c r="H3" s="91"/>
+      <c r="I3" s="91"/>
+      <c r="J3" s="91"/>
+      <c r="K3" s="91"/>
+      <c r="L3" s="91"/>
+      <c r="M3" s="91"/>
+      <c r="N3" s="91"/>
+      <c r="O3" s="91"/>
+      <c r="P3" s="91"/>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
@@ -3832,36 +3859,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="89"/>
-      <c r="C2" s="89"/>
-      <c r="D2" s="89"/>
-      <c r="E2" s="89"/>
-      <c r="F2" s="89"/>
-      <c r="G2" s="89"/>
-      <c r="H2" s="89"/>
-      <c r="I2" s="89"/>
-      <c r="J2" s="89"/>
-      <c r="K2" s="89"/>
-      <c r="L2" s="89"/>
-      <c r="M2" s="89"/>
-      <c r="N2" s="89"/>
+      <c r="B2" s="90"/>
+      <c r="C2" s="90"/>
+      <c r="D2" s="90"/>
+      <c r="E2" s="90"/>
+      <c r="F2" s="90"/>
+      <c r="G2" s="90"/>
+      <c r="H2" s="90"/>
+      <c r="I2" s="90"/>
+      <c r="J2" s="90"/>
+      <c r="K2" s="90"/>
+      <c r="L2" s="90"/>
+      <c r="M2" s="90"/>
+      <c r="N2" s="90"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="90" t="s">
+      <c r="B3" s="91" t="s">
         <v>64</v>
       </c>
-      <c r="C3" s="90"/>
-      <c r="D3" s="90"/>
-      <c r="E3" s="90"/>
-      <c r="F3" s="90"/>
-      <c r="G3" s="90"/>
-      <c r="H3" s="90"/>
-      <c r="I3" s="90"/>
-      <c r="J3" s="90"/>
-      <c r="K3" s="90"/>
-      <c r="L3" s="90"/>
-      <c r="M3" s="90"/>
-      <c r="N3" s="90"/>
+      <c r="C3" s="91"/>
+      <c r="D3" s="91"/>
+      <c r="E3" s="91"/>
+      <c r="F3" s="91"/>
+      <c r="G3" s="91"/>
+      <c r="H3" s="91"/>
+      <c r="I3" s="91"/>
+      <c r="J3" s="91"/>
+      <c r="K3" s="91"/>
+      <c r="L3" s="91"/>
+      <c r="M3" s="91"/>
+      <c r="N3" s="91"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="58" t="s">
@@ -3948,38 +3975,38 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="89" t="s">
+      <c r="B2" s="90" t="s">
         <v>97</v>
       </c>
-      <c r="C2" s="89"/>
-      <c r="D2" s="89"/>
-      <c r="E2" s="89"/>
-      <c r="F2" s="89"/>
-      <c r="G2" s="89"/>
-      <c r="H2" s="89"/>
-      <c r="I2" s="89"/>
-      <c r="J2" s="89"/>
-      <c r="K2" s="89"/>
-      <c r="L2" s="89"/>
-      <c r="M2" s="89"/>
-      <c r="N2" s="89"/>
+      <c r="C2" s="90"/>
+      <c r="D2" s="90"/>
+      <c r="E2" s="90"/>
+      <c r="F2" s="90"/>
+      <c r="G2" s="90"/>
+      <c r="H2" s="90"/>
+      <c r="I2" s="90"/>
+      <c r="J2" s="90"/>
+      <c r="K2" s="90"/>
+      <c r="L2" s="90"/>
+      <c r="M2" s="90"/>
+      <c r="N2" s="90"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="90" t="s">
+      <c r="B3" s="91" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="90"/>
-      <c r="D3" s="90"/>
-      <c r="E3" s="90"/>
-      <c r="F3" s="90"/>
-      <c r="G3" s="90"/>
-      <c r="H3" s="90"/>
-      <c r="I3" s="90"/>
-      <c r="J3" s="90"/>
-      <c r="K3" s="90"/>
-      <c r="L3" s="90"/>
-      <c r="M3" s="90"/>
-      <c r="N3" s="90"/>
+      <c r="C3" s="91"/>
+      <c r="D3" s="91"/>
+      <c r="E3" s="91"/>
+      <c r="F3" s="91"/>
+      <c r="G3" s="91"/>
+      <c r="H3" s="91"/>
+      <c r="I3" s="91"/>
+      <c r="J3" s="91"/>
+      <c r="K3" s="91"/>
+      <c r="L3" s="91"/>
+      <c r="M3" s="91"/>
+      <c r="N3" s="91"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="44" t="s">
@@ -4038,36 +4065,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="89"/>
-      <c r="C2" s="89"/>
-      <c r="D2" s="89"/>
-      <c r="E2" s="89"/>
-      <c r="F2" s="89"/>
-      <c r="G2" s="89"/>
-      <c r="H2" s="89"/>
-      <c r="I2" s="89"/>
-      <c r="J2" s="89"/>
-      <c r="K2" s="89"/>
-      <c r="L2" s="89"/>
-      <c r="M2" s="89"/>
-      <c r="N2" s="89"/>
+      <c r="B2" s="90"/>
+      <c r="C2" s="90"/>
+      <c r="D2" s="90"/>
+      <c r="E2" s="90"/>
+      <c r="F2" s="90"/>
+      <c r="G2" s="90"/>
+      <c r="H2" s="90"/>
+      <c r="I2" s="90"/>
+      <c r="J2" s="90"/>
+      <c r="K2" s="90"/>
+      <c r="L2" s="90"/>
+      <c r="M2" s="90"/>
+      <c r="N2" s="90"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="90" t="s">
+      <c r="B3" s="91" t="s">
         <v>152</v>
       </c>
-      <c r="C3" s="90"/>
-      <c r="D3" s="90"/>
-      <c r="E3" s="90"/>
-      <c r="F3" s="90"/>
-      <c r="G3" s="90"/>
-      <c r="H3" s="90"/>
-      <c r="I3" s="90"/>
-      <c r="J3" s="90"/>
-      <c r="K3" s="90"/>
-      <c r="L3" s="90"/>
-      <c r="M3" s="90"/>
-      <c r="N3" s="90"/>
+      <c r="C3" s="91"/>
+      <c r="D3" s="91"/>
+      <c r="E3" s="91"/>
+      <c r="F3" s="91"/>
+      <c r="G3" s="91"/>
+      <c r="H3" s="91"/>
+      <c r="I3" s="91"/>
+      <c r="J3" s="91"/>
+      <c r="K3" s="91"/>
+      <c r="L3" s="91"/>
+      <c r="M3" s="91"/>
+      <c r="N3" s="91"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="74" t="s">
@@ -4154,28 +4181,28 @@
       </c>
     </row>
     <row r="2" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="89"/>
-      <c r="C2" s="89"/>
-      <c r="D2" s="89"/>
-      <c r="E2" s="89"/>
-      <c r="F2" s="89"/>
-      <c r="G2" s="89"/>
-      <c r="H2" s="89"/>
-      <c r="I2" s="89"/>
-      <c r="J2" s="89"/>
+      <c r="B2" s="90"/>
+      <c r="C2" s="90"/>
+      <c r="D2" s="90"/>
+      <c r="E2" s="90"/>
+      <c r="F2" s="90"/>
+      <c r="G2" s="90"/>
+      <c r="H2" s="90"/>
+      <c r="I2" s="90"/>
+      <c r="J2" s="90"/>
     </row>
     <row r="3" spans="2:10" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="90" t="s">
+      <c r="B3" s="91" t="s">
         <v>155</v>
       </c>
-      <c r="C3" s="90"/>
-      <c r="D3" s="90"/>
-      <c r="E3" s="90"/>
-      <c r="F3" s="90"/>
-      <c r="G3" s="90"/>
-      <c r="H3" s="90"/>
-      <c r="I3" s="90"/>
-      <c r="J3" s="90"/>
+      <c r="C3" s="91"/>
+      <c r="D3" s="91"/>
+      <c r="E3" s="91"/>
+      <c r="F3" s="91"/>
+      <c r="G3" s="91"/>
+      <c r="H3" s="91"/>
+      <c r="I3" s="91"/>
+      <c r="J3" s="91"/>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" s="74" t="s">
@@ -4260,29 +4287,29 @@
       </c>
     </row>
     <row r="2" spans="2:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="89"/>
-      <c r="C2" s="89"/>
-      <c r="D2" s="89"/>
-      <c r="E2" s="89"/>
-      <c r="F2" s="89"/>
-      <c r="G2" s="89"/>
-      <c r="H2" s="89"/>
-      <c r="I2" s="89"/>
-      <c r="J2" s="89"/>
+      <c r="B2" s="90"/>
+      <c r="C2" s="90"/>
+      <c r="D2" s="90"/>
+      <c r="E2" s="90"/>
+      <c r="F2" s="90"/>
+      <c r="G2" s="90"/>
+      <c r="H2" s="90"/>
+      <c r="I2" s="90"/>
+      <c r="J2" s="90"/>
       <c r="K2" s="84"/>
     </row>
     <row r="3" spans="2:20" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="90" t="s">
+      <c r="B3" s="91" t="s">
         <v>156</v>
       </c>
-      <c r="C3" s="90"/>
-      <c r="D3" s="90"/>
-      <c r="E3" s="90"/>
-      <c r="F3" s="90"/>
-      <c r="G3" s="90"/>
-      <c r="H3" s="90"/>
-      <c r="I3" s="90"/>
-      <c r="J3" s="90"/>
+      <c r="C3" s="91"/>
+      <c r="D3" s="91"/>
+      <c r="E3" s="91"/>
+      <c r="F3" s="91"/>
+      <c r="G3" s="91"/>
+      <c r="H3" s="91"/>
+      <c r="I3" s="91"/>
+      <c r="J3" s="91"/>
       <c r="K3" s="83"/>
     </row>
     <row r="5" spans="2:20" x14ac:dyDescent="0.25">
@@ -4403,30 +4430,30 @@
       </c>
     </row>
     <row r="2" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="89"/>
-      <c r="C2" s="89"/>
-      <c r="D2" s="89"/>
-      <c r="E2" s="89"/>
-      <c r="F2" s="89"/>
-      <c r="G2" s="89"/>
-      <c r="H2" s="89"/>
-      <c r="I2" s="89"/>
-      <c r="J2" s="89"/>
-      <c r="K2" s="89"/>
+      <c r="B2" s="90"/>
+      <c r="C2" s="90"/>
+      <c r="D2" s="90"/>
+      <c r="E2" s="90"/>
+      <c r="F2" s="90"/>
+      <c r="G2" s="90"/>
+      <c r="H2" s="90"/>
+      <c r="I2" s="90"/>
+      <c r="J2" s="90"/>
+      <c r="K2" s="90"/>
     </row>
     <row r="3" spans="2:11" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="90" t="s">
+      <c r="B3" s="91" t="s">
         <v>168</v>
       </c>
-      <c r="C3" s="90"/>
-      <c r="D3" s="90"/>
-      <c r="E3" s="90"/>
-      <c r="F3" s="90"/>
-      <c r="G3" s="90"/>
-      <c r="H3" s="90"/>
-      <c r="I3" s="90"/>
-      <c r="J3" s="90"/>
-      <c r="K3" s="90"/>
+      <c r="C3" s="91"/>
+      <c r="D3" s="91"/>
+      <c r="E3" s="91"/>
+      <c r="F3" s="91"/>
+      <c r="G3" s="91"/>
+      <c r="H3" s="91"/>
+      <c r="I3" s="91"/>
+      <c r="J3" s="91"/>
+      <c r="K3" s="91"/>
     </row>
     <row r="4" spans="2:11" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B4" s="85"/>
@@ -4441,14 +4468,14 @@
       <c r="K4" s="85"/>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="H5" s="92" t="s">
+      <c r="H5" s="93" t="s">
         <v>176</v>
       </c>
-      <c r="I5" s="93"/>
-      <c r="J5" s="92" t="s">
+      <c r="I5" s="94"/>
+      <c r="J5" s="93" t="s">
         <v>175</v>
       </c>
-      <c r="K5" s="93"/>
+      <c r="K5" s="94"/>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" s="86" t="s">
@@ -4530,37 +4557,37 @@
       <c r="Z1" s="38"/>
     </row>
     <row r="2" spans="2:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="89"/>
-      <c r="C2" s="89"/>
-      <c r="D2" s="89"/>
-      <c r="E2" s="89"/>
-      <c r="F2" s="89"/>
-      <c r="G2" s="89"/>
-      <c r="H2" s="89"/>
-      <c r="I2" s="89"/>
-      <c r="J2" s="89"/>
-      <c r="K2" s="89"/>
-      <c r="L2" s="89"/>
-      <c r="M2" s="89"/>
-      <c r="N2" s="89"/>
+      <c r="B2" s="90"/>
+      <c r="C2" s="90"/>
+      <c r="D2" s="90"/>
+      <c r="E2" s="90"/>
+      <c r="F2" s="90"/>
+      <c r="G2" s="90"/>
+      <c r="H2" s="90"/>
+      <c r="I2" s="90"/>
+      <c r="J2" s="90"/>
+      <c r="K2" s="90"/>
+      <c r="L2" s="90"/>
+      <c r="M2" s="90"/>
+      <c r="N2" s="90"/>
       <c r="Z2"/>
     </row>
     <row r="3" spans="2:26" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="90" t="s">
+      <c r="B3" s="91" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="90"/>
-      <c r="D3" s="90"/>
-      <c r="E3" s="90"/>
-      <c r="F3" s="90"/>
-      <c r="G3" s="90"/>
-      <c r="H3" s="90"/>
-      <c r="I3" s="90"/>
-      <c r="J3" s="90"/>
-      <c r="K3" s="90"/>
-      <c r="L3" s="90"/>
-      <c r="M3" s="90"/>
-      <c r="N3" s="90"/>
+      <c r="C3" s="91"/>
+      <c r="D3" s="91"/>
+      <c r="E3" s="91"/>
+      <c r="F3" s="91"/>
+      <c r="G3" s="91"/>
+      <c r="H3" s="91"/>
+      <c r="I3" s="91"/>
+      <c r="J3" s="91"/>
+      <c r="K3" s="91"/>
+      <c r="L3" s="91"/>
+      <c r="M3" s="91"/>
+      <c r="N3" s="91"/>
       <c r="Z3"/>
     </row>
     <row r="5" spans="2:26" x14ac:dyDescent="0.25">
@@ -4664,37 +4691,37 @@
       <c r="Z1" s="38"/>
     </row>
     <row r="2" spans="2:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="89"/>
-      <c r="C2" s="89"/>
-      <c r="D2" s="89"/>
-      <c r="E2" s="89"/>
-      <c r="F2" s="89"/>
-      <c r="G2" s="89"/>
-      <c r="H2" s="89"/>
-      <c r="I2" s="89"/>
-      <c r="J2" s="89"/>
-      <c r="K2" s="89"/>
-      <c r="L2" s="89"/>
-      <c r="M2" s="89"/>
-      <c r="N2" s="89"/>
+      <c r="B2" s="90"/>
+      <c r="C2" s="90"/>
+      <c r="D2" s="90"/>
+      <c r="E2" s="90"/>
+      <c r="F2" s="90"/>
+      <c r="G2" s="90"/>
+      <c r="H2" s="90"/>
+      <c r="I2" s="90"/>
+      <c r="J2" s="90"/>
+      <c r="K2" s="90"/>
+      <c r="L2" s="90"/>
+      <c r="M2" s="90"/>
+      <c r="N2" s="90"/>
       <c r="Z2"/>
     </row>
     <row r="3" spans="2:26" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="90" t="s">
+      <c r="B3" s="91" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="90"/>
-      <c r="D3" s="90"/>
-      <c r="E3" s="90"/>
-      <c r="F3" s="90"/>
-      <c r="G3" s="90"/>
-      <c r="H3" s="90"/>
-      <c r="I3" s="90"/>
-      <c r="J3" s="90"/>
-      <c r="K3" s="90"/>
-      <c r="L3" s="90"/>
-      <c r="M3" s="90"/>
-      <c r="N3" s="90"/>
+      <c r="C3" s="91"/>
+      <c r="D3" s="91"/>
+      <c r="E3" s="91"/>
+      <c r="F3" s="91"/>
+      <c r="G3" s="91"/>
+      <c r="H3" s="91"/>
+      <c r="I3" s="91"/>
+      <c r="J3" s="91"/>
+      <c r="K3" s="91"/>
+      <c r="L3" s="91"/>
+      <c r="M3" s="91"/>
+      <c r="N3" s="91"/>
       <c r="Z3"/>
     </row>
     <row r="5" spans="2:26" x14ac:dyDescent="0.25">
@@ -4713,9 +4740,9 @@
       <c r="C6" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="D6" s="94"/>
-      <c r="E6" s="95"/>
-      <c r="F6" s="96"/>
+      <c r="D6" s="95"/>
+      <c r="E6" s="96"/>
+      <c r="F6" s="97"/>
       <c r="G6" s="50"/>
       <c r="H6" s="50"/>
     </row>
@@ -4793,37 +4820,37 @@
       <c r="Z1" s="38"/>
     </row>
     <row r="2" spans="2:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="89"/>
-      <c r="C2" s="89"/>
-      <c r="D2" s="89"/>
-      <c r="E2" s="89"/>
-      <c r="F2" s="89"/>
-      <c r="G2" s="89"/>
-      <c r="H2" s="89"/>
-      <c r="I2" s="89"/>
-      <c r="J2" s="89"/>
-      <c r="K2" s="89"/>
-      <c r="L2" s="89"/>
-      <c r="M2" s="89"/>
-      <c r="N2" s="89"/>
+      <c r="B2" s="90"/>
+      <c r="C2" s="90"/>
+      <c r="D2" s="90"/>
+      <c r="E2" s="90"/>
+      <c r="F2" s="90"/>
+      <c r="G2" s="90"/>
+      <c r="H2" s="90"/>
+      <c r="I2" s="90"/>
+      <c r="J2" s="90"/>
+      <c r="K2" s="90"/>
+      <c r="L2" s="90"/>
+      <c r="M2" s="90"/>
+      <c r="N2" s="90"/>
       <c r="Z2"/>
     </row>
     <row r="3" spans="2:26" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="90" t="s">
+      <c r="B3" s="91" t="s">
         <v>93</v>
       </c>
-      <c r="C3" s="90"/>
-      <c r="D3" s="90"/>
-      <c r="E3" s="90"/>
-      <c r="F3" s="90"/>
-      <c r="G3" s="90"/>
-      <c r="H3" s="90"/>
-      <c r="I3" s="90"/>
-      <c r="J3" s="90"/>
-      <c r="K3" s="90"/>
-      <c r="L3" s="90"/>
-      <c r="M3" s="90"/>
-      <c r="N3" s="90"/>
+      <c r="C3" s="91"/>
+      <c r="D3" s="91"/>
+      <c r="E3" s="91"/>
+      <c r="F3" s="91"/>
+      <c r="G3" s="91"/>
+      <c r="H3" s="91"/>
+      <c r="I3" s="91"/>
+      <c r="J3" s="91"/>
+      <c r="K3" s="91"/>
+      <c r="L3" s="91"/>
+      <c r="M3" s="91"/>
+      <c r="N3" s="91"/>
       <c r="Z3"/>
     </row>
     <row r="5" spans="2:26" x14ac:dyDescent="0.25">
@@ -4916,37 +4943,37 @@
       <c r="Z1" s="38"/>
     </row>
     <row r="2" spans="2:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="89"/>
-      <c r="C2" s="89"/>
-      <c r="D2" s="89"/>
-      <c r="E2" s="89"/>
-      <c r="F2" s="89"/>
-      <c r="G2" s="89"/>
-      <c r="H2" s="89"/>
-      <c r="I2" s="89"/>
-      <c r="J2" s="89"/>
-      <c r="K2" s="89"/>
-      <c r="L2" s="89"/>
-      <c r="M2" s="89"/>
-      <c r="N2" s="89"/>
+      <c r="B2" s="90"/>
+      <c r="C2" s="90"/>
+      <c r="D2" s="90"/>
+      <c r="E2" s="90"/>
+      <c r="F2" s="90"/>
+      <c r="G2" s="90"/>
+      <c r="H2" s="90"/>
+      <c r="I2" s="90"/>
+      <c r="J2" s="90"/>
+      <c r="K2" s="90"/>
+      <c r="L2" s="90"/>
+      <c r="M2" s="90"/>
+      <c r="N2" s="90"/>
       <c r="Z2"/>
     </row>
     <row r="3" spans="2:26" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="90" t="s">
+      <c r="B3" s="91" t="s">
         <v>72</v>
       </c>
-      <c r="C3" s="90"/>
-      <c r="D3" s="90"/>
-      <c r="E3" s="90"/>
-      <c r="F3" s="90"/>
-      <c r="G3" s="90"/>
-      <c r="H3" s="90"/>
-      <c r="I3" s="90"/>
-      <c r="J3" s="90"/>
-      <c r="K3" s="90"/>
-      <c r="L3" s="90"/>
-      <c r="M3" s="90"/>
-      <c r="N3" s="90"/>
+      <c r="C3" s="91"/>
+      <c r="D3" s="91"/>
+      <c r="E3" s="91"/>
+      <c r="F3" s="91"/>
+      <c r="G3" s="91"/>
+      <c r="H3" s="91"/>
+      <c r="I3" s="91"/>
+      <c r="J3" s="91"/>
+      <c r="K3" s="91"/>
+      <c r="L3" s="91"/>
+      <c r="M3" s="91"/>
+      <c r="N3" s="91"/>
       <c r="Z3"/>
     </row>
     <row r="5" spans="2:26" x14ac:dyDescent="0.25">
@@ -5059,56 +5086,56 @@
       </c>
     </row>
     <row r="2" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="89"/>
-      <c r="C2" s="89"/>
-      <c r="D2" s="89"/>
-      <c r="E2" s="89"/>
-      <c r="F2" s="89"/>
-      <c r="G2" s="89"/>
-      <c r="H2" s="89"/>
-      <c r="I2" s="89"/>
-      <c r="J2" s="89"/>
-      <c r="K2" s="89"/>
-      <c r="L2" s="89"/>
+      <c r="B2" s="90"/>
+      <c r="C2" s="90"/>
+      <c r="D2" s="90"/>
+      <c r="E2" s="90"/>
+      <c r="F2" s="90"/>
+      <c r="G2" s="90"/>
+      <c r="H2" s="90"/>
+      <c r="I2" s="90"/>
+      <c r="J2" s="90"/>
+      <c r="K2" s="90"/>
+      <c r="L2" s="90"/>
     </row>
     <row r="3" spans="2:17" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="90" t="s">
+      <c r="B3" s="91" t="s">
         <v>108</v>
       </c>
-      <c r="C3" s="90"/>
-      <c r="D3" s="90"/>
-      <c r="E3" s="90"/>
-      <c r="F3" s="90"/>
-      <c r="G3" s="90"/>
-      <c r="H3" s="90"/>
-      <c r="I3" s="90"/>
-      <c r="J3" s="90"/>
-      <c r="K3" s="90"/>
-      <c r="L3" s="90"/>
+      <c r="C3" s="91"/>
+      <c r="D3" s="91"/>
+      <c r="E3" s="91"/>
+      <c r="F3" s="91"/>
+      <c r="G3" s="91"/>
+      <c r="H3" s="91"/>
+      <c r="I3" s="91"/>
+      <c r="J3" s="91"/>
+      <c r="K3" s="91"/>
+      <c r="L3" s="91"/>
     </row>
     <row r="5" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D5" s="97" t="s">
+      <c r="D5" s="98" t="s">
         <v>123</v>
       </c>
-      <c r="E5" s="97"/>
+      <c r="E5" s="98"/>
       <c r="F5" s="73"/>
       <c r="G5" s="73"/>
       <c r="H5" s="73"/>
       <c r="I5" s="73"/>
-      <c r="J5" s="97" t="s">
+      <c r="J5" s="98" t="s">
         <v>42</v>
       </c>
-      <c r="K5" s="97"/>
-      <c r="L5" s="97"/>
-      <c r="M5" s="97" t="s">
+      <c r="K5" s="98"/>
+      <c r="L5" s="98"/>
+      <c r="M5" s="98" t="s">
         <v>130</v>
       </c>
-      <c r="N5" s="97"/>
-      <c r="O5" s="97"/>
-      <c r="P5" s="91" t="s">
+      <c r="N5" s="98"/>
+      <c r="O5" s="98"/>
+      <c r="P5" s="92" t="s">
         <v>109</v>
       </c>
-      <c r="Q5" s="91"/>
+      <c r="Q5" s="92"/>
     </row>
     <row r="6" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="70" t="s">
@@ -5195,7 +5222,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:Y8"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="Y8" sqref="Y8"/>
     </sheetView>
   </sheetViews>
@@ -5232,110 +5259,110 @@
       </c>
     </row>
     <row r="2" spans="2:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="89"/>
-      <c r="C2" s="89"/>
-      <c r="D2" s="89"/>
-      <c r="E2" s="89"/>
-      <c r="F2" s="89"/>
-      <c r="G2" s="89"/>
-      <c r="H2" s="89"/>
-      <c r="I2" s="89"/>
-      <c r="J2" s="89"/>
-      <c r="K2" s="89"/>
-      <c r="L2" s="89"/>
-      <c r="M2" s="89"/>
-      <c r="N2" s="89"/>
-      <c r="O2" s="89"/>
-      <c r="P2" s="89"/>
+      <c r="B2" s="90"/>
+      <c r="C2" s="90"/>
+      <c r="D2" s="90"/>
+      <c r="E2" s="90"/>
+      <c r="F2" s="90"/>
+      <c r="G2" s="90"/>
+      <c r="H2" s="90"/>
+      <c r="I2" s="90"/>
+      <c r="J2" s="90"/>
+      <c r="K2" s="90"/>
+      <c r="L2" s="90"/>
+      <c r="M2" s="90"/>
+      <c r="N2" s="90"/>
+      <c r="O2" s="90"/>
+      <c r="P2" s="90"/>
       <c r="Q2" s="56"/>
       <c r="R2" s="56"/>
     </row>
     <row r="3" spans="2:25" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="90" t="s">
+      <c r="B3" s="91" t="s">
         <v>111</v>
       </c>
-      <c r="C3" s="90"/>
-      <c r="D3" s="90"/>
-      <c r="E3" s="90"/>
-      <c r="F3" s="90"/>
-      <c r="G3" s="90"/>
-      <c r="H3" s="90"/>
-      <c r="I3" s="90"/>
-      <c r="J3" s="90"/>
-      <c r="K3" s="90"/>
-      <c r="L3" s="90"/>
-      <c r="M3" s="90"/>
-      <c r="N3" s="90"/>
-      <c r="O3" s="90"/>
-      <c r="P3" s="90"/>
+      <c r="C3" s="91"/>
+      <c r="D3" s="91"/>
+      <c r="E3" s="91"/>
+      <c r="F3" s="91"/>
+      <c r="G3" s="91"/>
+      <c r="H3" s="91"/>
+      <c r="I3" s="91"/>
+      <c r="J3" s="91"/>
+      <c r="K3" s="91"/>
+      <c r="L3" s="91"/>
+      <c r="M3" s="91"/>
+      <c r="N3" s="91"/>
+      <c r="O3" s="91"/>
+      <c r="P3" s="91"/>
       <c r="Q3" s="57"/>
       <c r="R3" s="57"/>
     </row>
     <row r="5" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B5" s="99" t="s">
+      <c r="B5" s="101" t="s">
         <v>112</v>
       </c>
-      <c r="C5" s="100"/>
-      <c r="D5" s="100"/>
-      <c r="E5" s="100"/>
-      <c r="F5" s="100"/>
-      <c r="G5" s="100"/>
-      <c r="H5" s="100"/>
-      <c r="I5" s="100"/>
-      <c r="J5" s="100"/>
-      <c r="K5" s="100"/>
-      <c r="L5" s="101"/>
-      <c r="M5" s="99" t="s">
+      <c r="C5" s="102"/>
+      <c r="D5" s="102"/>
+      <c r="E5" s="102"/>
+      <c r="F5" s="102"/>
+      <c r="G5" s="102"/>
+      <c r="H5" s="102"/>
+      <c r="I5" s="102"/>
+      <c r="J5" s="102"/>
+      <c r="K5" s="102"/>
+      <c r="L5" s="103"/>
+      <c r="M5" s="101" t="s">
         <v>113</v>
       </c>
-      <c r="N5" s="100"/>
-      <c r="O5" s="100"/>
-      <c r="P5" s="100"/>
-      <c r="Q5" s="100"/>
-      <c r="R5" s="100"/>
-      <c r="S5" s="100"/>
-      <c r="T5" s="100"/>
-      <c r="U5" s="100"/>
-      <c r="V5" s="100"/>
-      <c r="W5" s="100"/>
-      <c r="X5" s="100"/>
-      <c r="Y5" s="101"/>
+      <c r="N5" s="102"/>
+      <c r="O5" s="102"/>
+      <c r="P5" s="102"/>
+      <c r="Q5" s="102"/>
+      <c r="R5" s="102"/>
+      <c r="S5" s="102"/>
+      <c r="T5" s="102"/>
+      <c r="U5" s="102"/>
+      <c r="V5" s="102"/>
+      <c r="W5" s="102"/>
+      <c r="X5" s="102"/>
+      <c r="Y5" s="103"/>
     </row>
     <row r="6" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B6" s="98"/>
-      <c r="C6" s="98"/>
-      <c r="D6" s="98"/>
-      <c r="E6" s="98"/>
-      <c r="F6" s="102" t="s">
+      <c r="B6" s="111"/>
+      <c r="C6" s="111"/>
+      <c r="D6" s="111"/>
+      <c r="E6" s="111"/>
+      <c r="F6" s="107" t="s">
         <v>27</v>
       </c>
-      <c r="G6" s="103"/>
-      <c r="H6" s="103"/>
-      <c r="I6" s="104"/>
-      <c r="J6" s="99" t="s">
+      <c r="G6" s="108"/>
+      <c r="H6" s="108"/>
+      <c r="I6" s="109"/>
+      <c r="J6" s="101" t="s">
         <v>30</v>
       </c>
-      <c r="K6" s="100"/>
-      <c r="L6" s="101"/>
-      <c r="M6" s="105"/>
-      <c r="N6" s="106" t="s">
+      <c r="K6" s="102"/>
+      <c r="L6" s="103"/>
+      <c r="M6" s="89"/>
+      <c r="N6" s="99" t="s">
         <v>42</v>
       </c>
-      <c r="O6" s="107"/>
-      <c r="P6" s="106" t="s">
+      <c r="O6" s="100"/>
+      <c r="P6" s="99" t="s">
         <v>106</v>
       </c>
-      <c r="Q6" s="108"/>
-      <c r="R6" s="107"/>
-      <c r="S6" s="105"/>
-      <c r="T6" s="106" t="s">
+      <c r="Q6" s="110"/>
+      <c r="R6" s="100"/>
+      <c r="S6" s="89"/>
+      <c r="T6" s="99" t="s">
         <v>123</v>
       </c>
-      <c r="U6" s="107"/>
-      <c r="V6" s="109"/>
-      <c r="W6" s="110"/>
-      <c r="X6" s="110"/>
-      <c r="Y6" s="111"/>
+      <c r="U6" s="100"/>
+      <c r="V6" s="104"/>
+      <c r="W6" s="105"/>
+      <c r="X6" s="105"/>
+      <c r="Y6" s="106"/>
     </row>
     <row r="7" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B7" s="75" t="s">
@@ -5439,6 +5466,7 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B6:E6"/>
     <mergeCell ref="T6:U6"/>
     <mergeCell ref="M5:Y5"/>
     <mergeCell ref="V6:Y6"/>
@@ -5449,7 +5477,6 @@
     <mergeCell ref="F6:I6"/>
     <mergeCell ref="N6:O6"/>
     <mergeCell ref="P6:R6"/>
-    <mergeCell ref="B6:E6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -5483,36 +5510,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="89"/>
-      <c r="C2" s="89"/>
-      <c r="D2" s="89"/>
-      <c r="E2" s="89"/>
-      <c r="F2" s="89"/>
-      <c r="G2" s="89"/>
-      <c r="H2" s="89"/>
-      <c r="I2" s="89"/>
-      <c r="J2" s="89"/>
-      <c r="K2" s="89"/>
-      <c r="L2" s="89"/>
-      <c r="M2" s="89"/>
-      <c r="N2" s="89"/>
+      <c r="B2" s="90"/>
+      <c r="C2" s="90"/>
+      <c r="D2" s="90"/>
+      <c r="E2" s="90"/>
+      <c r="F2" s="90"/>
+      <c r="G2" s="90"/>
+      <c r="H2" s="90"/>
+      <c r="I2" s="90"/>
+      <c r="J2" s="90"/>
+      <c r="K2" s="90"/>
+      <c r="L2" s="90"/>
+      <c r="M2" s="90"/>
+      <c r="N2" s="90"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="90" t="s">
+      <c r="B3" s="91" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="90"/>
-      <c r="D3" s="90"/>
-      <c r="E3" s="90"/>
-      <c r="F3" s="90"/>
-      <c r="G3" s="90"/>
-      <c r="H3" s="90"/>
-      <c r="I3" s="90"/>
-      <c r="J3" s="90"/>
-      <c r="K3" s="90"/>
-      <c r="L3" s="90"/>
-      <c r="M3" s="90"/>
-      <c r="N3" s="90"/>
+      <c r="C3" s="91"/>
+      <c r="D3" s="91"/>
+      <c r="E3" s="91"/>
+      <c r="F3" s="91"/>
+      <c r="G3" s="91"/>
+      <c r="H3" s="91"/>
+      <c r="I3" s="91"/>
+      <c r="J3" s="91"/>
+      <c r="K3" s="91"/>
+      <c r="L3" s="91"/>
+      <c r="M3" s="91"/>
+      <c r="N3" s="91"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="44" t="s">
@@ -5667,40 +5694,40 @@
       </c>
     </row>
     <row r="2" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="89"/>
-      <c r="C2" s="89"/>
-      <c r="D2" s="89"/>
-      <c r="E2" s="89"/>
-      <c r="F2" s="89"/>
-      <c r="G2" s="89"/>
-      <c r="H2" s="89"/>
-      <c r="I2" s="89"/>
-      <c r="J2" s="89"/>
-      <c r="K2" s="89"/>
-      <c r="L2" s="89"/>
-      <c r="M2" s="89"/>
-      <c r="N2" s="89"/>
-      <c r="O2" s="89"/>
-      <c r="P2" s="89"/>
+      <c r="B2" s="90"/>
+      <c r="C2" s="90"/>
+      <c r="D2" s="90"/>
+      <c r="E2" s="90"/>
+      <c r="F2" s="90"/>
+      <c r="G2" s="90"/>
+      <c r="H2" s="90"/>
+      <c r="I2" s="90"/>
+      <c r="J2" s="90"/>
+      <c r="K2" s="90"/>
+      <c r="L2" s="90"/>
+      <c r="M2" s="90"/>
+      <c r="N2" s="90"/>
+      <c r="O2" s="90"/>
+      <c r="P2" s="90"/>
     </row>
     <row r="3" spans="2:16" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="90" t="s">
+      <c r="B3" s="91" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="90"/>
-      <c r="D3" s="90"/>
-      <c r="E3" s="90"/>
-      <c r="F3" s="90"/>
-      <c r="G3" s="90"/>
-      <c r="H3" s="90"/>
-      <c r="I3" s="90"/>
-      <c r="J3" s="90"/>
-      <c r="K3" s="90"/>
-      <c r="L3" s="90"/>
-      <c r="M3" s="90"/>
-      <c r="N3" s="90"/>
-      <c r="O3" s="90"/>
-      <c r="P3" s="90"/>
+      <c r="C3" s="91"/>
+      <c r="D3" s="91"/>
+      <c r="E3" s="91"/>
+      <c r="F3" s="91"/>
+      <c r="G3" s="91"/>
+      <c r="H3" s="91"/>
+      <c r="I3" s="91"/>
+      <c r="J3" s="91"/>
+      <c r="K3" s="91"/>
+      <c r="L3" s="91"/>
+      <c r="M3" s="91"/>
+      <c r="N3" s="91"/>
+      <c r="O3" s="91"/>
+      <c r="P3" s="91"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="44" t="s">
@@ -5779,40 +5806,40 @@
       </c>
     </row>
     <row r="2" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="89"/>
-      <c r="C2" s="89"/>
-      <c r="D2" s="89"/>
-      <c r="E2" s="89"/>
-      <c r="F2" s="89"/>
-      <c r="G2" s="89"/>
-      <c r="H2" s="89"/>
-      <c r="I2" s="89"/>
-      <c r="J2" s="89"/>
-      <c r="K2" s="89"/>
-      <c r="L2" s="89"/>
-      <c r="M2" s="89"/>
-      <c r="N2" s="89"/>
-      <c r="O2" s="89"/>
-      <c r="P2" s="89"/>
+      <c r="B2" s="90"/>
+      <c r="C2" s="90"/>
+      <c r="D2" s="90"/>
+      <c r="E2" s="90"/>
+      <c r="F2" s="90"/>
+      <c r="G2" s="90"/>
+      <c r="H2" s="90"/>
+      <c r="I2" s="90"/>
+      <c r="J2" s="90"/>
+      <c r="K2" s="90"/>
+      <c r="L2" s="90"/>
+      <c r="M2" s="90"/>
+      <c r="N2" s="90"/>
+      <c r="O2" s="90"/>
+      <c r="P2" s="90"/>
     </row>
     <row r="3" spans="2:16" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="90" t="s">
+      <c r="B3" s="91" t="s">
         <v>68</v>
       </c>
-      <c r="C3" s="90"/>
-      <c r="D3" s="90"/>
-      <c r="E3" s="90"/>
-      <c r="F3" s="90"/>
-      <c r="G3" s="90"/>
-      <c r="H3" s="90"/>
-      <c r="I3" s="90"/>
-      <c r="J3" s="90"/>
-      <c r="K3" s="90"/>
-      <c r="L3" s="90"/>
-      <c r="M3" s="90"/>
-      <c r="N3" s="90"/>
-      <c r="O3" s="90"/>
-      <c r="P3" s="90"/>
+      <c r="C3" s="91"/>
+      <c r="D3" s="91"/>
+      <c r="E3" s="91"/>
+      <c r="F3" s="91"/>
+      <c r="G3" s="91"/>
+      <c r="H3" s="91"/>
+      <c r="I3" s="91"/>
+      <c r="J3" s="91"/>
+      <c r="K3" s="91"/>
+      <c r="L3" s="91"/>
+      <c r="M3" s="91"/>
+      <c r="N3" s="91"/>
+      <c r="O3" s="91"/>
+      <c r="P3" s="91"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
@@ -5861,40 +5888,40 @@
       </c>
     </row>
     <row r="2" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="89"/>
-      <c r="C2" s="89"/>
-      <c r="D2" s="89"/>
-      <c r="E2" s="89"/>
-      <c r="F2" s="89"/>
-      <c r="G2" s="89"/>
-      <c r="H2" s="89"/>
-      <c r="I2" s="89"/>
-      <c r="J2" s="89"/>
-      <c r="K2" s="89"/>
-      <c r="L2" s="89"/>
-      <c r="M2" s="89"/>
-      <c r="N2" s="89"/>
-      <c r="O2" s="89"/>
-      <c r="P2" s="89"/>
+      <c r="B2" s="90"/>
+      <c r="C2" s="90"/>
+      <c r="D2" s="90"/>
+      <c r="E2" s="90"/>
+      <c r="F2" s="90"/>
+      <c r="G2" s="90"/>
+      <c r="H2" s="90"/>
+      <c r="I2" s="90"/>
+      <c r="J2" s="90"/>
+      <c r="K2" s="90"/>
+      <c r="L2" s="90"/>
+      <c r="M2" s="90"/>
+      <c r="N2" s="90"/>
+      <c r="O2" s="90"/>
+      <c r="P2" s="90"/>
     </row>
     <row r="3" spans="2:16" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="90" t="s">
+      <c r="B3" s="91" t="s">
         <v>71</v>
       </c>
-      <c r="C3" s="90"/>
-      <c r="D3" s="90"/>
-      <c r="E3" s="90"/>
-      <c r="F3" s="90"/>
-      <c r="G3" s="90"/>
-      <c r="H3" s="90"/>
-      <c r="I3" s="90"/>
-      <c r="J3" s="90"/>
-      <c r="K3" s="90"/>
-      <c r="L3" s="90"/>
-      <c r="M3" s="90"/>
-      <c r="N3" s="90"/>
-      <c r="O3" s="90"/>
-      <c r="P3" s="90"/>
+      <c r="C3" s="91"/>
+      <c r="D3" s="91"/>
+      <c r="E3" s="91"/>
+      <c r="F3" s="91"/>
+      <c r="G3" s="91"/>
+      <c r="H3" s="91"/>
+      <c r="I3" s="91"/>
+      <c r="J3" s="91"/>
+      <c r="K3" s="91"/>
+      <c r="L3" s="91"/>
+      <c r="M3" s="91"/>
+      <c r="N3" s="91"/>
+      <c r="O3" s="91"/>
+      <c r="P3" s="91"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
@@ -5948,36 +5975,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="89"/>
-      <c r="C2" s="89"/>
-      <c r="D2" s="89"/>
-      <c r="E2" s="89"/>
-      <c r="F2" s="89"/>
-      <c r="G2" s="89"/>
-      <c r="H2" s="89"/>
-      <c r="I2" s="89"/>
-      <c r="J2" s="89"/>
-      <c r="K2" s="89"/>
-      <c r="L2" s="89"/>
-      <c r="M2" s="89"/>
-      <c r="N2" s="89"/>
+      <c r="B2" s="90"/>
+      <c r="C2" s="90"/>
+      <c r="D2" s="90"/>
+      <c r="E2" s="90"/>
+      <c r="F2" s="90"/>
+      <c r="G2" s="90"/>
+      <c r="H2" s="90"/>
+      <c r="I2" s="90"/>
+      <c r="J2" s="90"/>
+      <c r="K2" s="90"/>
+      <c r="L2" s="90"/>
+      <c r="M2" s="90"/>
+      <c r="N2" s="90"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="90" t="s">
+      <c r="B3" s="91" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="90"/>
-      <c r="D3" s="90"/>
-      <c r="E3" s="90"/>
-      <c r="F3" s="90"/>
-      <c r="G3" s="90"/>
-      <c r="H3" s="90"/>
-      <c r="I3" s="90"/>
-      <c r="J3" s="90"/>
-      <c r="K3" s="90"/>
-      <c r="L3" s="90"/>
-      <c r="M3" s="90"/>
-      <c r="N3" s="90"/>
+      <c r="C3" s="91"/>
+      <c r="D3" s="91"/>
+      <c r="E3" s="91"/>
+      <c r="F3" s="91"/>
+      <c r="G3" s="91"/>
+      <c r="H3" s="91"/>
+      <c r="I3" s="91"/>
+      <c r="J3" s="91"/>
+      <c r="K3" s="91"/>
+      <c r="L3" s="91"/>
+      <c r="M3" s="91"/>
+      <c r="N3" s="91"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="44" t="s">
@@ -6042,8 +6069,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:P6"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6051,7 +6078,7 @@
     <col min="1" max="1" width="2.5703125" customWidth="1"/>
     <col min="2" max="2" width="25.42578125" customWidth="1"/>
     <col min="3" max="3" width="59.140625" customWidth="1"/>
-    <col min="4" max="4" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" customWidth="1"/>
     <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="28.7109375" bestFit="1" customWidth="1"/>
@@ -6066,40 +6093,40 @@
       </c>
     </row>
     <row r="2" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="89"/>
-      <c r="C2" s="89"/>
-      <c r="D2" s="89"/>
-      <c r="E2" s="89"/>
-      <c r="F2" s="89"/>
-      <c r="G2" s="89"/>
-      <c r="H2" s="89"/>
-      <c r="I2" s="89"/>
-      <c r="J2" s="89"/>
-      <c r="K2" s="89"/>
-      <c r="L2" s="89"/>
-      <c r="M2" s="89"/>
-      <c r="N2" s="89"/>
-      <c r="O2" s="89"/>
-      <c r="P2" s="89"/>
+      <c r="B2" s="90"/>
+      <c r="C2" s="90"/>
+      <c r="D2" s="90"/>
+      <c r="E2" s="90"/>
+      <c r="F2" s="90"/>
+      <c r="G2" s="90"/>
+      <c r="H2" s="90"/>
+      <c r="I2" s="90"/>
+      <c r="J2" s="90"/>
+      <c r="K2" s="90"/>
+      <c r="L2" s="90"/>
+      <c r="M2" s="90"/>
+      <c r="N2" s="90"/>
+      <c r="O2" s="90"/>
+      <c r="P2" s="90"/>
     </row>
     <row r="3" spans="2:16" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="90" t="s">
+      <c r="B3" s="91" t="s">
         <v>65</v>
       </c>
-      <c r="C3" s="90"/>
-      <c r="D3" s="90"/>
-      <c r="E3" s="90"/>
-      <c r="F3" s="90"/>
-      <c r="G3" s="90"/>
-      <c r="H3" s="90"/>
-      <c r="I3" s="90"/>
-      <c r="J3" s="90"/>
-      <c r="K3" s="90"/>
-      <c r="L3" s="90"/>
-      <c r="M3" s="90"/>
-      <c r="N3" s="90"/>
-      <c r="O3" s="90"/>
-      <c r="P3" s="90"/>
+      <c r="C3" s="91"/>
+      <c r="D3" s="91"/>
+      <c r="E3" s="91"/>
+      <c r="F3" s="91"/>
+      <c r="G3" s="91"/>
+      <c r="H3" s="91"/>
+      <c r="I3" s="91"/>
+      <c r="J3" s="91"/>
+      <c r="K3" s="91"/>
+      <c r="L3" s="91"/>
+      <c r="M3" s="91"/>
+      <c r="N3" s="91"/>
+      <c r="O3" s="91"/>
+      <c r="P3" s="91"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="45" t="s">
@@ -6108,10 +6135,14 @@
       <c r="C5" s="45" t="s">
         <v>67</v>
       </c>
+      <c r="D5" s="113" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
+      <c r="D6" s="112"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -6151,36 +6182,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="89"/>
-      <c r="C2" s="89"/>
-      <c r="D2" s="89"/>
-      <c r="E2" s="89"/>
-      <c r="F2" s="89"/>
-      <c r="G2" s="89"/>
-      <c r="H2" s="89"/>
-      <c r="I2" s="89"/>
-      <c r="J2" s="89"/>
-      <c r="K2" s="89"/>
-      <c r="L2" s="89"/>
-      <c r="M2" s="89"/>
-      <c r="N2" s="89"/>
+      <c r="B2" s="90"/>
+      <c r="C2" s="90"/>
+      <c r="D2" s="90"/>
+      <c r="E2" s="90"/>
+      <c r="F2" s="90"/>
+      <c r="G2" s="90"/>
+      <c r="H2" s="90"/>
+      <c r="I2" s="90"/>
+      <c r="J2" s="90"/>
+      <c r="K2" s="90"/>
+      <c r="L2" s="90"/>
+      <c r="M2" s="90"/>
+      <c r="N2" s="90"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="90" t="s">
+      <c r="B3" s="91" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="90"/>
-      <c r="D3" s="90"/>
-      <c r="E3" s="90"/>
-      <c r="F3" s="90"/>
-      <c r="G3" s="90"/>
-      <c r="H3" s="90"/>
-      <c r="I3" s="90"/>
-      <c r="J3" s="90"/>
-      <c r="K3" s="90"/>
-      <c r="L3" s="90"/>
-      <c r="M3" s="90"/>
-      <c r="N3" s="90"/>
+      <c r="C3" s="91"/>
+      <c r="D3" s="91"/>
+      <c r="E3" s="91"/>
+      <c r="F3" s="91"/>
+      <c r="G3" s="91"/>
+      <c r="H3" s="91"/>
+      <c r="I3" s="91"/>
+      <c r="J3" s="91"/>
+      <c r="K3" s="91"/>
+      <c r="L3" s="91"/>
+      <c r="M3" s="91"/>
+      <c r="N3" s="91"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">

</xml_diff>

<commit_message>
TRIEDA-1656 - Alterando formatações e posição das colunas do relatório por faixa demanda no excel. TRIEDA-1640 - Criando relatório de Atendimentos por Carga Horaria no excel.
</commit_message>
<xml_diff>
--- a/code/client/web/src/main/resources/templateExport.xlsx
+++ b/code/client/web/src/main/resources/templateExport.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="17070" windowHeight="5370" tabRatio="797" firstSheet="5" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="2505" windowWidth="17070" windowHeight="5310" tabRatio="907" firstSheet="20" activeTab="21"/>
   </bookViews>
   <sheets>
     <sheet name="Campi" sheetId="3" r:id="rId1"/>
@@ -29,14 +29,15 @@
     <sheet name="Atendimentos por Matricula" sheetId="30" r:id="rId20"/>
     <sheet name="Atendimentos por Disciplina" sheetId="31" r:id="rId21"/>
     <sheet name="Atendimentos Faixa de Demanda" sheetId="32" r:id="rId22"/>
-    <sheet name="Porcentagem Mestres e Doutores" sheetId="33" r:id="rId23"/>
-    <sheet name="Relatorio Visao Sala" sheetId="10" r:id="rId24"/>
-    <sheet name="Relatorio Visao Aluno" sheetId="25" r:id="rId25"/>
-    <sheet name="Relatorio Visao Professor" sheetId="21" r:id="rId26"/>
-    <sheet name="Relatorio Visao Curso" sheetId="20" r:id="rId27"/>
-    <sheet name="Atendimentos por Aluno" sheetId="23" r:id="rId28"/>
-    <sheet name="Aulas" sheetId="26" r:id="rId29"/>
-    <sheet name="PaletaCores" sheetId="11" r:id="rId30"/>
+    <sheet name="Atendimentos por Carga Horaria" sheetId="35" r:id="rId23"/>
+    <sheet name="Porcentagem Mestres e Doutores" sheetId="33" r:id="rId24"/>
+    <sheet name="Relatorio Visao Sala" sheetId="10" r:id="rId25"/>
+    <sheet name="Relatorio Visao Aluno" sheetId="25" r:id="rId26"/>
+    <sheet name="Relatorio Visao Professor" sheetId="21" r:id="rId27"/>
+    <sheet name="Relatorio Visao Curso" sheetId="20" r:id="rId28"/>
+    <sheet name="Atendimentos por Aluno" sheetId="23" r:id="rId29"/>
+    <sheet name="Aulas" sheetId="26" r:id="rId30"/>
+    <sheet name="PaletaCores" sheetId="11" r:id="rId31"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
@@ -1229,7 +1230,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="193">
   <si>
     <t>Planilha de Unidades</t>
   </si>
@@ -1781,6 +1782,33 @@
   </si>
   <si>
     <t>Disciplina Aula</t>
+  </si>
+  <si>
+    <t>Matricula</t>
+  </si>
+  <si>
+    <t>Segunda</t>
+  </si>
+  <si>
+    <t>Terça</t>
+  </si>
+  <si>
+    <t>Quarta</t>
+  </si>
+  <si>
+    <t>Quinta</t>
+  </si>
+  <si>
+    <t>Sexta</t>
+  </si>
+  <si>
+    <t>Sábado</t>
+  </si>
+  <si>
+    <t>Domingo</t>
+  </si>
+  <si>
+    <t>Planilha de Atendimentos Por Carga Horária</t>
   </si>
 </sst>
 </file>
@@ -1789,7 +1817,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="165" formatCode="&quot;R$&quot;\ #,##0.00"/>
-    <numFmt numFmtId="173" formatCode="0.0000"/>
+    <numFmt numFmtId="178" formatCode="#,##0.0000"/>
   </numFmts>
   <fonts count="15" x14ac:knownFonts="1">
     <font>
@@ -1830,6 +1858,13 @@
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1891,13 +1926,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="29">
@@ -2201,18 +2229,18 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="114">
+  <cellXfs count="118">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -2230,16 +2258,16 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2321,181 +2349,193 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="7" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="27" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="6" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="173" fontId="6" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="28" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2507,26 +2547,26 @@
     <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="7" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="7" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2855,38 +2895,38 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="90" t="s">
+      <c r="B2" s="92" t="s">
         <v>96</v>
       </c>
-      <c r="C2" s="90"/>
-      <c r="D2" s="90"/>
-      <c r="E2" s="90"/>
-      <c r="F2" s="90"/>
-      <c r="G2" s="90"/>
-      <c r="H2" s="90"/>
-      <c r="I2" s="90"/>
-      <c r="J2" s="90"/>
-      <c r="K2" s="90"/>
-      <c r="L2" s="90"/>
-      <c r="M2" s="90"/>
-      <c r="N2" s="90"/>
+      <c r="C2" s="92"/>
+      <c r="D2" s="92"/>
+      <c r="E2" s="92"/>
+      <c r="F2" s="92"/>
+      <c r="G2" s="92"/>
+      <c r="H2" s="92"/>
+      <c r="I2" s="92"/>
+      <c r="J2" s="92"/>
+      <c r="K2" s="92"/>
+      <c r="L2" s="92"/>
+      <c r="M2" s="92"/>
+      <c r="N2" s="92"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="91" t="s">
+      <c r="B3" s="93" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="91"/>
-      <c r="D3" s="91"/>
-      <c r="E3" s="91"/>
-      <c r="F3" s="91"/>
-      <c r="G3" s="91"/>
-      <c r="H3" s="91"/>
-      <c r="I3" s="91"/>
-      <c r="J3" s="91"/>
-      <c r="K3" s="91"/>
-      <c r="L3" s="91"/>
-      <c r="M3" s="91"/>
-      <c r="N3" s="91"/>
+      <c r="C3" s="93"/>
+      <c r="D3" s="93"/>
+      <c r="E3" s="93"/>
+      <c r="F3" s="93"/>
+      <c r="G3" s="93"/>
+      <c r="H3" s="93"/>
+      <c r="I3" s="93"/>
+      <c r="J3" s="93"/>
+      <c r="K3" s="93"/>
+      <c r="L3" s="93"/>
+      <c r="M3" s="93"/>
+      <c r="N3" s="93"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="44" t="s">
@@ -2954,36 +2994,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="90"/>
-      <c r="C2" s="90"/>
-      <c r="D2" s="90"/>
-      <c r="E2" s="90"/>
-      <c r="F2" s="90"/>
-      <c r="G2" s="90"/>
-      <c r="H2" s="90"/>
-      <c r="I2" s="90"/>
-      <c r="J2" s="90"/>
-      <c r="K2" s="90"/>
-      <c r="L2" s="90"/>
-      <c r="M2" s="90"/>
-      <c r="N2" s="90"/>
+      <c r="B2" s="92"/>
+      <c r="C2" s="92"/>
+      <c r="D2" s="92"/>
+      <c r="E2" s="92"/>
+      <c r="F2" s="92"/>
+      <c r="G2" s="92"/>
+      <c r="H2" s="92"/>
+      <c r="I2" s="92"/>
+      <c r="J2" s="92"/>
+      <c r="K2" s="92"/>
+      <c r="L2" s="92"/>
+      <c r="M2" s="92"/>
+      <c r="N2" s="92"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="91" t="s">
+      <c r="B3" s="93" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="91"/>
-      <c r="D3" s="91"/>
-      <c r="E3" s="91"/>
-      <c r="F3" s="91"/>
-      <c r="G3" s="91"/>
-      <c r="H3" s="91"/>
-      <c r="I3" s="91"/>
-      <c r="J3" s="91"/>
-      <c r="K3" s="91"/>
-      <c r="L3" s="91"/>
-      <c r="M3" s="91"/>
-      <c r="N3" s="91"/>
+      <c r="C3" s="93"/>
+      <c r="D3" s="93"/>
+      <c r="E3" s="93"/>
+      <c r="F3" s="93"/>
+      <c r="G3" s="93"/>
+      <c r="H3" s="93"/>
+      <c r="I3" s="93"/>
+      <c r="J3" s="93"/>
+      <c r="K3" s="93"/>
+      <c r="L3" s="93"/>
+      <c r="M3" s="93"/>
+      <c r="N3" s="93"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -3052,36 +3092,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="90"/>
-      <c r="C2" s="90"/>
-      <c r="D2" s="90"/>
-      <c r="E2" s="90"/>
-      <c r="F2" s="90"/>
-      <c r="G2" s="90"/>
-      <c r="H2" s="90"/>
-      <c r="I2" s="90"/>
-      <c r="J2" s="90"/>
-      <c r="K2" s="90"/>
-      <c r="L2" s="90"/>
-      <c r="M2" s="90"/>
-      <c r="N2" s="90"/>
+      <c r="B2" s="92"/>
+      <c r="C2" s="92"/>
+      <c r="D2" s="92"/>
+      <c r="E2" s="92"/>
+      <c r="F2" s="92"/>
+      <c r="G2" s="92"/>
+      <c r="H2" s="92"/>
+      <c r="I2" s="92"/>
+      <c r="J2" s="92"/>
+      <c r="K2" s="92"/>
+      <c r="L2" s="92"/>
+      <c r="M2" s="92"/>
+      <c r="N2" s="92"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="91" t="s">
+      <c r="B3" s="93" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="91"/>
-      <c r="D3" s="91"/>
-      <c r="E3" s="91"/>
-      <c r="F3" s="91"/>
-      <c r="G3" s="91"/>
-      <c r="H3" s="91"/>
-      <c r="I3" s="91"/>
-      <c r="J3" s="91"/>
-      <c r="K3" s="91"/>
-      <c r="L3" s="91"/>
-      <c r="M3" s="91"/>
-      <c r="N3" s="91"/>
+      <c r="C3" s="93"/>
+      <c r="D3" s="93"/>
+      <c r="E3" s="93"/>
+      <c r="F3" s="93"/>
+      <c r="G3" s="93"/>
+      <c r="H3" s="93"/>
+      <c r="I3" s="93"/>
+      <c r="J3" s="93"/>
+      <c r="K3" s="93"/>
+      <c r="L3" s="93"/>
+      <c r="M3" s="93"/>
+      <c r="N3" s="93"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -3166,18 +3206,18 @@
       </c>
     </row>
     <row r="2" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="90"/>
-      <c r="C2" s="90"/>
-      <c r="D2" s="90"/>
-      <c r="E2" s="90"/>
+      <c r="B2" s="92"/>
+      <c r="C2" s="92"/>
+      <c r="D2" s="92"/>
+      <c r="E2" s="92"/>
     </row>
     <row r="3" spans="2:5" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="91" t="s">
+      <c r="B3" s="93" t="s">
         <v>126</v>
       </c>
-      <c r="C3" s="91"/>
-      <c r="D3" s="91"/>
-      <c r="E3" s="91"/>
+      <c r="C3" s="93"/>
+      <c r="D3" s="93"/>
+      <c r="E3" s="93"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="60" t="s">
@@ -3230,36 +3270,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="90"/>
-      <c r="C2" s="90"/>
-      <c r="D2" s="90"/>
-      <c r="E2" s="90"/>
-      <c r="F2" s="90"/>
-      <c r="G2" s="90"/>
-      <c r="H2" s="90"/>
-      <c r="I2" s="90"/>
-      <c r="J2" s="90"/>
-      <c r="K2" s="90"/>
-      <c r="L2" s="90"/>
-      <c r="M2" s="90"/>
-      <c r="N2" s="90"/>
+      <c r="B2" s="92"/>
+      <c r="C2" s="92"/>
+      <c r="D2" s="92"/>
+      <c r="E2" s="92"/>
+      <c r="F2" s="92"/>
+      <c r="G2" s="92"/>
+      <c r="H2" s="92"/>
+      <c r="I2" s="92"/>
+      <c r="J2" s="92"/>
+      <c r="K2" s="92"/>
+      <c r="L2" s="92"/>
+      <c r="M2" s="92"/>
+      <c r="N2" s="92"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="91" t="s">
+      <c r="B3" s="93" t="s">
         <v>100</v>
       </c>
-      <c r="C3" s="91"/>
-      <c r="D3" s="91"/>
-      <c r="E3" s="91"/>
-      <c r="F3" s="91"/>
-      <c r="G3" s="91"/>
-      <c r="H3" s="91"/>
-      <c r="I3" s="91"/>
-      <c r="J3" s="91"/>
-      <c r="K3" s="91"/>
-      <c r="L3" s="91"/>
-      <c r="M3" s="91"/>
-      <c r="N3" s="91"/>
+      <c r="C3" s="93"/>
+      <c r="D3" s="93"/>
+      <c r="E3" s="93"/>
+      <c r="F3" s="93"/>
+      <c r="G3" s="93"/>
+      <c r="H3" s="93"/>
+      <c r="I3" s="93"/>
+      <c r="J3" s="93"/>
+      <c r="K3" s="93"/>
+      <c r="L3" s="93"/>
+      <c r="M3" s="93"/>
+      <c r="N3" s="93"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -3292,10 +3332,10 @@
       <c r="K5" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="L5" s="92" t="s">
+      <c r="L5" s="94" t="s">
         <v>110</v>
       </c>
-      <c r="M5" s="92"/>
+      <c r="M5" s="94"/>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
@@ -3347,38 +3387,38 @@
       </c>
     </row>
     <row r="2" spans="2:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="90"/>
-      <c r="C2" s="90"/>
-      <c r="D2" s="90"/>
-      <c r="E2" s="90"/>
-      <c r="F2" s="90"/>
-      <c r="G2" s="90"/>
-      <c r="H2" s="90"/>
-      <c r="I2" s="90"/>
-      <c r="J2" s="90"/>
-      <c r="K2" s="90"/>
-      <c r="L2" s="90"/>
-      <c r="M2" s="90"/>
-      <c r="N2" s="90"/>
-      <c r="O2" s="90"/>
+      <c r="B2" s="92"/>
+      <c r="C2" s="92"/>
+      <c r="D2" s="92"/>
+      <c r="E2" s="92"/>
+      <c r="F2" s="92"/>
+      <c r="G2" s="92"/>
+      <c r="H2" s="92"/>
+      <c r="I2" s="92"/>
+      <c r="J2" s="92"/>
+      <c r="K2" s="92"/>
+      <c r="L2" s="92"/>
+      <c r="M2" s="92"/>
+      <c r="N2" s="92"/>
+      <c r="O2" s="92"/>
     </row>
     <row r="3" spans="2:15" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="91" t="s">
+      <c r="B3" s="93" t="s">
         <v>73</v>
       </c>
-      <c r="C3" s="91"/>
-      <c r="D3" s="91"/>
-      <c r="E3" s="91"/>
-      <c r="F3" s="91"/>
-      <c r="G3" s="91"/>
-      <c r="H3" s="91"/>
-      <c r="I3" s="91"/>
-      <c r="J3" s="91"/>
-      <c r="K3" s="91"/>
-      <c r="L3" s="91"/>
-      <c r="M3" s="91"/>
-      <c r="N3" s="91"/>
-      <c r="O3" s="91"/>
+      <c r="C3" s="93"/>
+      <c r="D3" s="93"/>
+      <c r="E3" s="93"/>
+      <c r="F3" s="93"/>
+      <c r="G3" s="93"/>
+      <c r="H3" s="93"/>
+      <c r="I3" s="93"/>
+      <c r="J3" s="93"/>
+      <c r="K3" s="93"/>
+      <c r="L3" s="93"/>
+      <c r="M3" s="93"/>
+      <c r="N3" s="93"/>
+      <c r="O3" s="93"/>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -3457,18 +3497,18 @@
       </c>
     </row>
     <row r="2" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="90"/>
-      <c r="C2" s="90"/>
-      <c r="D2" s="90"/>
-      <c r="E2" s="90"/>
+      <c r="B2" s="92"/>
+      <c r="C2" s="92"/>
+      <c r="D2" s="92"/>
+      <c r="E2" s="92"/>
     </row>
     <row r="3" spans="2:5" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="91" t="s">
+      <c r="B3" s="93" t="s">
         <v>131</v>
       </c>
-      <c r="C3" s="91"/>
-      <c r="D3" s="91"/>
-      <c r="E3" s="91"/>
+      <c r="C3" s="93"/>
+      <c r="D3" s="93"/>
+      <c r="E3" s="93"/>
     </row>
     <row r="4" spans="2:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="64"/>
@@ -3530,36 +3570,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="90"/>
-      <c r="C2" s="90"/>
-      <c r="D2" s="90"/>
-      <c r="E2" s="90"/>
-      <c r="F2" s="90"/>
-      <c r="G2" s="90"/>
-      <c r="H2" s="90"/>
-      <c r="I2" s="90"/>
-      <c r="J2" s="90"/>
-      <c r="K2" s="90"/>
-      <c r="L2" s="90"/>
-      <c r="M2" s="90"/>
-      <c r="N2" s="90"/>
+      <c r="B2" s="92"/>
+      <c r="C2" s="92"/>
+      <c r="D2" s="92"/>
+      <c r="E2" s="92"/>
+      <c r="F2" s="92"/>
+      <c r="G2" s="92"/>
+      <c r="H2" s="92"/>
+      <c r="I2" s="92"/>
+      <c r="J2" s="92"/>
+      <c r="K2" s="92"/>
+      <c r="L2" s="92"/>
+      <c r="M2" s="92"/>
+      <c r="N2" s="92"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="91" t="s">
+      <c r="B3" s="93" t="s">
         <v>69</v>
       </c>
-      <c r="C3" s="91"/>
-      <c r="D3" s="91"/>
-      <c r="E3" s="91"/>
-      <c r="F3" s="91"/>
-      <c r="G3" s="91"/>
-      <c r="H3" s="91"/>
-      <c r="I3" s="91"/>
-      <c r="J3" s="91"/>
-      <c r="K3" s="91"/>
-      <c r="L3" s="91"/>
-      <c r="M3" s="91"/>
-      <c r="N3" s="91"/>
+      <c r="C3" s="93"/>
+      <c r="D3" s="93"/>
+      <c r="E3" s="93"/>
+      <c r="F3" s="93"/>
+      <c r="G3" s="93"/>
+      <c r="H3" s="93"/>
+      <c r="I3" s="93"/>
+      <c r="J3" s="93"/>
+      <c r="K3" s="93"/>
+      <c r="L3" s="93"/>
+      <c r="M3" s="93"/>
+      <c r="N3" s="93"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -3614,36 +3654,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="90"/>
-      <c r="C2" s="90"/>
-      <c r="D2" s="90"/>
-      <c r="E2" s="90"/>
-      <c r="F2" s="90"/>
-      <c r="G2" s="90"/>
-      <c r="H2" s="90"/>
-      <c r="I2" s="90"/>
-      <c r="J2" s="90"/>
-      <c r="K2" s="90"/>
-      <c r="L2" s="90"/>
-      <c r="M2" s="90"/>
-      <c r="N2" s="90"/>
+      <c r="B2" s="92"/>
+      <c r="C2" s="92"/>
+      <c r="D2" s="92"/>
+      <c r="E2" s="92"/>
+      <c r="F2" s="92"/>
+      <c r="G2" s="92"/>
+      <c r="H2" s="92"/>
+      <c r="I2" s="92"/>
+      <c r="J2" s="92"/>
+      <c r="K2" s="92"/>
+      <c r="L2" s="92"/>
+      <c r="M2" s="92"/>
+      <c r="N2" s="92"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="91" t="s">
+      <c r="B3" s="93" t="s">
         <v>74</v>
       </c>
-      <c r="C3" s="91"/>
-      <c r="D3" s="91"/>
-      <c r="E3" s="91"/>
-      <c r="F3" s="91"/>
-      <c r="G3" s="91"/>
-      <c r="H3" s="91"/>
-      <c r="I3" s="91"/>
-      <c r="J3" s="91"/>
-      <c r="K3" s="91"/>
-      <c r="L3" s="91"/>
-      <c r="M3" s="91"/>
-      <c r="N3" s="91"/>
+      <c r="C3" s="93"/>
+      <c r="D3" s="93"/>
+      <c r="E3" s="93"/>
+      <c r="F3" s="93"/>
+      <c r="G3" s="93"/>
+      <c r="H3" s="93"/>
+      <c r="I3" s="93"/>
+      <c r="J3" s="93"/>
+      <c r="K3" s="93"/>
+      <c r="L3" s="93"/>
+      <c r="M3" s="93"/>
+      <c r="N3" s="93"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -3712,40 +3752,40 @@
       </c>
     </row>
     <row r="2" spans="2:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="90"/>
-      <c r="C2" s="90"/>
-      <c r="D2" s="90"/>
-      <c r="E2" s="90"/>
-      <c r="F2" s="90"/>
-      <c r="G2" s="90"/>
-      <c r="H2" s="90"/>
-      <c r="I2" s="90"/>
-      <c r="J2" s="90"/>
-      <c r="K2" s="90"/>
-      <c r="L2" s="90"/>
-      <c r="M2" s="90"/>
-      <c r="N2" s="90"/>
-      <c r="O2" s="90"/>
-      <c r="P2" s="90"/>
+      <c r="B2" s="92"/>
+      <c r="C2" s="92"/>
+      <c r="D2" s="92"/>
+      <c r="E2" s="92"/>
+      <c r="F2" s="92"/>
+      <c r="G2" s="92"/>
+      <c r="H2" s="92"/>
+      <c r="I2" s="92"/>
+      <c r="J2" s="92"/>
+      <c r="K2" s="92"/>
+      <c r="L2" s="92"/>
+      <c r="M2" s="92"/>
+      <c r="N2" s="92"/>
+      <c r="O2" s="92"/>
+      <c r="P2" s="92"/>
     </row>
     <row r="3" spans="2:18" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="91" t="s">
+      <c r="B3" s="93" t="s">
         <v>63</v>
       </c>
-      <c r="C3" s="91"/>
-      <c r="D3" s="91"/>
-      <c r="E3" s="91"/>
-      <c r="F3" s="91"/>
-      <c r="G3" s="91"/>
-      <c r="H3" s="91"/>
-      <c r="I3" s="91"/>
-      <c r="J3" s="91"/>
-      <c r="K3" s="91"/>
-      <c r="L3" s="91"/>
-      <c r="M3" s="91"/>
-      <c r="N3" s="91"/>
-      <c r="O3" s="91"/>
-      <c r="P3" s="91"/>
+      <c r="C3" s="93"/>
+      <c r="D3" s="93"/>
+      <c r="E3" s="93"/>
+      <c r="F3" s="93"/>
+      <c r="G3" s="93"/>
+      <c r="H3" s="93"/>
+      <c r="I3" s="93"/>
+      <c r="J3" s="93"/>
+      <c r="K3" s="93"/>
+      <c r="L3" s="93"/>
+      <c r="M3" s="93"/>
+      <c r="N3" s="93"/>
+      <c r="O3" s="93"/>
+      <c r="P3" s="93"/>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
@@ -3859,36 +3899,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="90"/>
-      <c r="C2" s="90"/>
-      <c r="D2" s="90"/>
-      <c r="E2" s="90"/>
-      <c r="F2" s="90"/>
-      <c r="G2" s="90"/>
-      <c r="H2" s="90"/>
-      <c r="I2" s="90"/>
-      <c r="J2" s="90"/>
-      <c r="K2" s="90"/>
-      <c r="L2" s="90"/>
-      <c r="M2" s="90"/>
-      <c r="N2" s="90"/>
+      <c r="B2" s="92"/>
+      <c r="C2" s="92"/>
+      <c r="D2" s="92"/>
+      <c r="E2" s="92"/>
+      <c r="F2" s="92"/>
+      <c r="G2" s="92"/>
+      <c r="H2" s="92"/>
+      <c r="I2" s="92"/>
+      <c r="J2" s="92"/>
+      <c r="K2" s="92"/>
+      <c r="L2" s="92"/>
+      <c r="M2" s="92"/>
+      <c r="N2" s="92"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="91" t="s">
+      <c r="B3" s="93" t="s">
         <v>64</v>
       </c>
-      <c r="C3" s="91"/>
-      <c r="D3" s="91"/>
-      <c r="E3" s="91"/>
-      <c r="F3" s="91"/>
-      <c r="G3" s="91"/>
-      <c r="H3" s="91"/>
-      <c r="I3" s="91"/>
-      <c r="J3" s="91"/>
-      <c r="K3" s="91"/>
-      <c r="L3" s="91"/>
-      <c r="M3" s="91"/>
-      <c r="N3" s="91"/>
+      <c r="C3" s="93"/>
+      <c r="D3" s="93"/>
+      <c r="E3" s="93"/>
+      <c r="F3" s="93"/>
+      <c r="G3" s="93"/>
+      <c r="H3" s="93"/>
+      <c r="I3" s="93"/>
+      <c r="J3" s="93"/>
+      <c r="K3" s="93"/>
+      <c r="L3" s="93"/>
+      <c r="M3" s="93"/>
+      <c r="N3" s="93"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="58" t="s">
@@ -3975,38 +4015,38 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="90" t="s">
+      <c r="B2" s="92" t="s">
         <v>97</v>
       </c>
-      <c r="C2" s="90"/>
-      <c r="D2" s="90"/>
-      <c r="E2" s="90"/>
-      <c r="F2" s="90"/>
-      <c r="G2" s="90"/>
-      <c r="H2" s="90"/>
-      <c r="I2" s="90"/>
-      <c r="J2" s="90"/>
-      <c r="K2" s="90"/>
-      <c r="L2" s="90"/>
-      <c r="M2" s="90"/>
-      <c r="N2" s="90"/>
+      <c r="C2" s="92"/>
+      <c r="D2" s="92"/>
+      <c r="E2" s="92"/>
+      <c r="F2" s="92"/>
+      <c r="G2" s="92"/>
+      <c r="H2" s="92"/>
+      <c r="I2" s="92"/>
+      <c r="J2" s="92"/>
+      <c r="K2" s="92"/>
+      <c r="L2" s="92"/>
+      <c r="M2" s="92"/>
+      <c r="N2" s="92"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="91" t="s">
+      <c r="B3" s="93" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="91"/>
-      <c r="D3" s="91"/>
-      <c r="E3" s="91"/>
-      <c r="F3" s="91"/>
-      <c r="G3" s="91"/>
-      <c r="H3" s="91"/>
-      <c r="I3" s="91"/>
-      <c r="J3" s="91"/>
-      <c r="K3" s="91"/>
-      <c r="L3" s="91"/>
-      <c r="M3" s="91"/>
-      <c r="N3" s="91"/>
+      <c r="C3" s="93"/>
+      <c r="D3" s="93"/>
+      <c r="E3" s="93"/>
+      <c r="F3" s="93"/>
+      <c r="G3" s="93"/>
+      <c r="H3" s="93"/>
+      <c r="I3" s="93"/>
+      <c r="J3" s="93"/>
+      <c r="K3" s="93"/>
+      <c r="L3" s="93"/>
+      <c r="M3" s="93"/>
+      <c r="N3" s="93"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="44" t="s">
@@ -4065,36 +4105,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="90"/>
-      <c r="C2" s="90"/>
-      <c r="D2" s="90"/>
-      <c r="E2" s="90"/>
-      <c r="F2" s="90"/>
-      <c r="G2" s="90"/>
-      <c r="H2" s="90"/>
-      <c r="I2" s="90"/>
-      <c r="J2" s="90"/>
-      <c r="K2" s="90"/>
-      <c r="L2" s="90"/>
-      <c r="M2" s="90"/>
-      <c r="N2" s="90"/>
+      <c r="B2" s="92"/>
+      <c r="C2" s="92"/>
+      <c r="D2" s="92"/>
+      <c r="E2" s="92"/>
+      <c r="F2" s="92"/>
+      <c r="G2" s="92"/>
+      <c r="H2" s="92"/>
+      <c r="I2" s="92"/>
+      <c r="J2" s="92"/>
+      <c r="K2" s="92"/>
+      <c r="L2" s="92"/>
+      <c r="M2" s="92"/>
+      <c r="N2" s="92"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="91" t="s">
+      <c r="B3" s="93" t="s">
         <v>152</v>
       </c>
-      <c r="C3" s="91"/>
-      <c r="D3" s="91"/>
-      <c r="E3" s="91"/>
-      <c r="F3" s="91"/>
-      <c r="G3" s="91"/>
-      <c r="H3" s="91"/>
-      <c r="I3" s="91"/>
-      <c r="J3" s="91"/>
-      <c r="K3" s="91"/>
-      <c r="L3" s="91"/>
-      <c r="M3" s="91"/>
-      <c r="N3" s="91"/>
+      <c r="C3" s="93"/>
+      <c r="D3" s="93"/>
+      <c r="E3" s="93"/>
+      <c r="F3" s="93"/>
+      <c r="G3" s="93"/>
+      <c r="H3" s="93"/>
+      <c r="I3" s="93"/>
+      <c r="J3" s="93"/>
+      <c r="K3" s="93"/>
+      <c r="L3" s="93"/>
+      <c r="M3" s="93"/>
+      <c r="N3" s="93"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="74" t="s">
@@ -4181,28 +4221,28 @@
       </c>
     </row>
     <row r="2" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="90"/>
-      <c r="C2" s="90"/>
-      <c r="D2" s="90"/>
-      <c r="E2" s="90"/>
-      <c r="F2" s="90"/>
-      <c r="G2" s="90"/>
-      <c r="H2" s="90"/>
-      <c r="I2" s="90"/>
-      <c r="J2" s="90"/>
+      <c r="B2" s="92"/>
+      <c r="C2" s="92"/>
+      <c r="D2" s="92"/>
+      <c r="E2" s="92"/>
+      <c r="F2" s="92"/>
+      <c r="G2" s="92"/>
+      <c r="H2" s="92"/>
+      <c r="I2" s="92"/>
+      <c r="J2" s="92"/>
     </row>
     <row r="3" spans="2:10" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="91" t="s">
+      <c r="B3" s="93" t="s">
         <v>155</v>
       </c>
-      <c r="C3" s="91"/>
-      <c r="D3" s="91"/>
-      <c r="E3" s="91"/>
-      <c r="F3" s="91"/>
-      <c r="G3" s="91"/>
-      <c r="H3" s="91"/>
-      <c r="I3" s="91"/>
-      <c r="J3" s="91"/>
+      <c r="C3" s="93"/>
+      <c r="D3" s="93"/>
+      <c r="E3" s="93"/>
+      <c r="F3" s="93"/>
+      <c r="G3" s="93"/>
+      <c r="H3" s="93"/>
+      <c r="I3" s="93"/>
+      <c r="J3" s="93"/>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" s="74" t="s">
@@ -4254,8 +4294,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:T6"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="I1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="Q14" sqref="Q14"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4267,12 +4307,12 @@
     <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.7109375" customWidth="1"/>
     <col min="8" max="8" width="21.140625" customWidth="1"/>
-    <col min="9" max="9" width="16.140625" customWidth="1"/>
-    <col min="10" max="10" width="25.85546875" customWidth="1"/>
-    <col min="11" max="11" width="15.7109375" customWidth="1"/>
-    <col min="12" max="12" width="19.140625" customWidth="1"/>
-    <col min="13" max="13" width="25.42578125" customWidth="1"/>
-    <col min="14" max="14" width="21.85546875" customWidth="1"/>
+    <col min="9" max="9" width="19.140625" customWidth="1"/>
+    <col min="10" max="10" width="25.42578125" customWidth="1"/>
+    <col min="11" max="11" width="21.85546875" customWidth="1"/>
+    <col min="12" max="12" width="16.140625" customWidth="1"/>
+    <col min="13" max="13" width="25.85546875" customWidth="1"/>
+    <col min="14" max="14" width="15.7109375" customWidth="1"/>
     <col min="15" max="15" width="17" customWidth="1"/>
     <col min="16" max="16" width="23.7109375" customWidth="1"/>
     <col min="17" max="17" width="25" customWidth="1"/>
@@ -4287,30 +4327,32 @@
       </c>
     </row>
     <row r="2" spans="2:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="90"/>
-      <c r="C2" s="90"/>
-      <c r="D2" s="90"/>
-      <c r="E2" s="90"/>
-      <c r="F2" s="90"/>
-      <c r="G2" s="90"/>
-      <c r="H2" s="90"/>
-      <c r="I2" s="90"/>
-      <c r="J2" s="90"/>
-      <c r="K2" s="84"/>
+      <c r="B2" s="117"/>
+      <c r="C2" s="117"/>
+      <c r="D2" s="117"/>
+      <c r="E2" s="117"/>
+      <c r="F2" s="117"/>
+      <c r="G2" s="117"/>
+      <c r="H2" s="117"/>
+      <c r="I2" s="117"/>
+      <c r="L2" s="84"/>
+      <c r="M2" s="84"/>
+      <c r="N2" s="84"/>
     </row>
     <row r="3" spans="2:20" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="91" t="s">
+      <c r="B3" s="93" t="s">
         <v>156</v>
       </c>
-      <c r="C3" s="91"/>
-      <c r="D3" s="91"/>
-      <c r="E3" s="91"/>
-      <c r="F3" s="91"/>
-      <c r="G3" s="91"/>
-      <c r="H3" s="91"/>
-      <c r="I3" s="91"/>
-      <c r="J3" s="91"/>
-      <c r="K3" s="83"/>
+      <c r="C3" s="93"/>
+      <c r="D3" s="93"/>
+      <c r="E3" s="93"/>
+      <c r="F3" s="93"/>
+      <c r="G3" s="93"/>
+      <c r="H3" s="93"/>
+      <c r="I3" s="93"/>
+      <c r="L3" s="83"/>
+      <c r="M3" s="83"/>
+      <c r="N3" s="83"/>
     </row>
     <row r="5" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B5" s="80" t="s">
@@ -4335,22 +4377,22 @@
         <v>161</v>
       </c>
       <c r="I5" s="79" t="s">
+        <v>165</v>
+      </c>
+      <c r="J5" s="79" t="s">
+        <v>166</v>
+      </c>
+      <c r="K5" s="79" t="s">
+        <v>167</v>
+      </c>
+      <c r="L5" s="79" t="s">
         <v>162</v>
       </c>
-      <c r="J5" s="79" t="s">
+      <c r="M5" s="79" t="s">
         <v>163</v>
       </c>
-      <c r="K5" s="79" t="s">
+      <c r="N5" s="79" t="s">
         <v>164</v>
-      </c>
-      <c r="L5" s="79" t="s">
-        <v>165</v>
-      </c>
-      <c r="M5" s="79" t="s">
-        <v>166</v>
-      </c>
-      <c r="N5" s="79" t="s">
-        <v>167</v>
       </c>
       <c r="O5" s="87" t="s">
         <v>177</v>
@@ -4374,28 +4416,28 @@
     <row r="6" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
       <c r="F6" s="8"/>
-      <c r="G6" s="9"/>
+      <c r="G6" s="6"/>
       <c r="H6" s="8"/>
-      <c r="I6" s="78"/>
-      <c r="J6" s="81"/>
-      <c r="K6" s="78"/>
-      <c r="L6" s="78"/>
-      <c r="M6" s="78"/>
-      <c r="N6" s="82"/>
-      <c r="O6" s="81"/>
-      <c r="P6" s="88"/>
+      <c r="I6" s="114"/>
+      <c r="J6" s="114"/>
+      <c r="K6" s="82"/>
+      <c r="L6" s="114"/>
+      <c r="M6" s="115"/>
+      <c r="N6" s="114"/>
+      <c r="O6" s="115"/>
+      <c r="P6" s="116"/>
       <c r="Q6" s="78"/>
-      <c r="R6" s="81"/>
-      <c r="S6" s="81"/>
+      <c r="R6" s="115"/>
+      <c r="S6" s="115"/>
       <c r="T6" s="82"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B2:J2"/>
-    <mergeCell ref="B3:J3"/>
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="B3:I3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -4403,6 +4445,99 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:I6"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.85546875" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" customWidth="1"/>
+    <col min="8" max="9" width="14.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:9" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B1" s="46" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="2:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="92"/>
+      <c r="C2" s="92"/>
+      <c r="D2" s="92"/>
+      <c r="E2" s="92"/>
+      <c r="F2" s="92"/>
+      <c r="G2" s="92"/>
+      <c r="H2" s="92"/>
+      <c r="I2" s="92"/>
+    </row>
+    <row r="3" spans="2:9" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B3" s="93" t="s">
+        <v>192</v>
+      </c>
+      <c r="C3" s="93"/>
+      <c r="D3" s="93"/>
+      <c r="E3" s="93"/>
+      <c r="F3" s="93"/>
+      <c r="G3" s="93"/>
+      <c r="H3" s="93"/>
+      <c r="I3" s="93"/>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B5" s="89" t="s">
+        <v>184</v>
+      </c>
+      <c r="C5" s="89" t="s">
+        <v>185</v>
+      </c>
+      <c r="D5" s="89" t="s">
+        <v>186</v>
+      </c>
+      <c r="E5" s="89" t="s">
+        <v>187</v>
+      </c>
+      <c r="F5" s="89" t="s">
+        <v>188</v>
+      </c>
+      <c r="G5" s="89" t="s">
+        <v>189</v>
+      </c>
+      <c r="H5" s="89" t="s">
+        <v>190</v>
+      </c>
+      <c r="I5" s="89" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B6" s="8"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="81"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="B3:I3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K7"/>
   <sheetViews>
@@ -4430,30 +4565,30 @@
       </c>
     </row>
     <row r="2" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="90"/>
-      <c r="C2" s="90"/>
-      <c r="D2" s="90"/>
-      <c r="E2" s="90"/>
-      <c r="F2" s="90"/>
-      <c r="G2" s="90"/>
-      <c r="H2" s="90"/>
-      <c r="I2" s="90"/>
-      <c r="J2" s="90"/>
-      <c r="K2" s="90"/>
+      <c r="B2" s="92"/>
+      <c r="C2" s="92"/>
+      <c r="D2" s="92"/>
+      <c r="E2" s="92"/>
+      <c r="F2" s="92"/>
+      <c r="G2" s="92"/>
+      <c r="H2" s="92"/>
+      <c r="I2" s="92"/>
+      <c r="J2" s="92"/>
+      <c r="K2" s="92"/>
     </row>
     <row r="3" spans="2:11" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="91" t="s">
+      <c r="B3" s="93" t="s">
         <v>168</v>
       </c>
-      <c r="C3" s="91"/>
-      <c r="D3" s="91"/>
-      <c r="E3" s="91"/>
-      <c r="F3" s="91"/>
-      <c r="G3" s="91"/>
-      <c r="H3" s="91"/>
-      <c r="I3" s="91"/>
-      <c r="J3" s="91"/>
-      <c r="K3" s="91"/>
+      <c r="C3" s="93"/>
+      <c r="D3" s="93"/>
+      <c r="E3" s="93"/>
+      <c r="F3" s="93"/>
+      <c r="G3" s="93"/>
+      <c r="H3" s="93"/>
+      <c r="I3" s="93"/>
+      <c r="J3" s="93"/>
+      <c r="K3" s="93"/>
     </row>
     <row r="4" spans="2:11" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B4" s="85"/>
@@ -4468,14 +4603,14 @@
       <c r="K4" s="85"/>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="H5" s="93" t="s">
+      <c r="H5" s="95" t="s">
         <v>176</v>
       </c>
-      <c r="I5" s="94"/>
-      <c r="J5" s="93" t="s">
+      <c r="I5" s="96"/>
+      <c r="J5" s="95" t="s">
         <v>175</v>
       </c>
-      <c r="K5" s="94"/>
+      <c r="K5" s="96"/>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" s="86" t="s">
@@ -4533,7 +4668,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:Z8"/>
   <sheetViews>
@@ -4557,37 +4692,37 @@
       <c r="Z1" s="38"/>
     </row>
     <row r="2" spans="2:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="90"/>
-      <c r="C2" s="90"/>
-      <c r="D2" s="90"/>
-      <c r="E2" s="90"/>
-      <c r="F2" s="90"/>
-      <c r="G2" s="90"/>
-      <c r="H2" s="90"/>
-      <c r="I2" s="90"/>
-      <c r="J2" s="90"/>
-      <c r="K2" s="90"/>
-      <c r="L2" s="90"/>
-      <c r="M2" s="90"/>
-      <c r="N2" s="90"/>
+      <c r="B2" s="92"/>
+      <c r="C2" s="92"/>
+      <c r="D2" s="92"/>
+      <c r="E2" s="92"/>
+      <c r="F2" s="92"/>
+      <c r="G2" s="92"/>
+      <c r="H2" s="92"/>
+      <c r="I2" s="92"/>
+      <c r="J2" s="92"/>
+      <c r="K2" s="92"/>
+      <c r="L2" s="92"/>
+      <c r="M2" s="92"/>
+      <c r="N2" s="92"/>
       <c r="Z2"/>
     </row>
     <row r="3" spans="2:26" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="91" t="s">
+      <c r="B3" s="93" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="91"/>
-      <c r="D3" s="91"/>
-      <c r="E3" s="91"/>
-      <c r="F3" s="91"/>
-      <c r="G3" s="91"/>
-      <c r="H3" s="91"/>
-      <c r="I3" s="91"/>
-      <c r="J3" s="91"/>
-      <c r="K3" s="91"/>
-      <c r="L3" s="91"/>
-      <c r="M3" s="91"/>
-      <c r="N3" s="91"/>
+      <c r="C3" s="93"/>
+      <c r="D3" s="93"/>
+      <c r="E3" s="93"/>
+      <c r="F3" s="93"/>
+      <c r="G3" s="93"/>
+      <c r="H3" s="93"/>
+      <c r="I3" s="93"/>
+      <c r="J3" s="93"/>
+      <c r="K3" s="93"/>
+      <c r="L3" s="93"/>
+      <c r="M3" s="93"/>
+      <c r="N3" s="93"/>
       <c r="Z3"/>
     </row>
     <row r="5" spans="2:26" x14ac:dyDescent="0.25">
@@ -4667,7 +4802,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:Z8"/>
   <sheetViews>
@@ -4691,37 +4826,37 @@
       <c r="Z1" s="38"/>
     </row>
     <row r="2" spans="2:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="90"/>
-      <c r="C2" s="90"/>
-      <c r="D2" s="90"/>
-      <c r="E2" s="90"/>
-      <c r="F2" s="90"/>
-      <c r="G2" s="90"/>
-      <c r="H2" s="90"/>
-      <c r="I2" s="90"/>
-      <c r="J2" s="90"/>
-      <c r="K2" s="90"/>
-      <c r="L2" s="90"/>
-      <c r="M2" s="90"/>
-      <c r="N2" s="90"/>
+      <c r="B2" s="92"/>
+      <c r="C2" s="92"/>
+      <c r="D2" s="92"/>
+      <c r="E2" s="92"/>
+      <c r="F2" s="92"/>
+      <c r="G2" s="92"/>
+      <c r="H2" s="92"/>
+      <c r="I2" s="92"/>
+      <c r="J2" s="92"/>
+      <c r="K2" s="92"/>
+      <c r="L2" s="92"/>
+      <c r="M2" s="92"/>
+      <c r="N2" s="92"/>
       <c r="Z2"/>
     </row>
     <row r="3" spans="2:26" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="91" t="s">
+      <c r="B3" s="93" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="91"/>
-      <c r="D3" s="91"/>
-      <c r="E3" s="91"/>
-      <c r="F3" s="91"/>
-      <c r="G3" s="91"/>
-      <c r="H3" s="91"/>
-      <c r="I3" s="91"/>
-      <c r="J3" s="91"/>
-      <c r="K3" s="91"/>
-      <c r="L3" s="91"/>
-      <c r="M3" s="91"/>
-      <c r="N3" s="91"/>
+      <c r="C3" s="93"/>
+      <c r="D3" s="93"/>
+      <c r="E3" s="93"/>
+      <c r="F3" s="93"/>
+      <c r="G3" s="93"/>
+      <c r="H3" s="93"/>
+      <c r="I3" s="93"/>
+      <c r="J3" s="93"/>
+      <c r="K3" s="93"/>
+      <c r="L3" s="93"/>
+      <c r="M3" s="93"/>
+      <c r="N3" s="93"/>
       <c r="Z3"/>
     </row>
     <row r="5" spans="2:26" x14ac:dyDescent="0.25">
@@ -4740,9 +4875,9 @@
       <c r="C6" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="D6" s="95"/>
-      <c r="E6" s="96"/>
-      <c r="F6" s="97"/>
+      <c r="D6" s="97"/>
+      <c r="E6" s="98"/>
+      <c r="F6" s="99"/>
       <c r="G6" s="50"/>
       <c r="H6" s="50"/>
     </row>
@@ -4796,7 +4931,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:Z8"/>
   <sheetViews>
@@ -4820,37 +4955,37 @@
       <c r="Z1" s="38"/>
     </row>
     <row r="2" spans="2:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="90"/>
-      <c r="C2" s="90"/>
-      <c r="D2" s="90"/>
-      <c r="E2" s="90"/>
-      <c r="F2" s="90"/>
-      <c r="G2" s="90"/>
-      <c r="H2" s="90"/>
-      <c r="I2" s="90"/>
-      <c r="J2" s="90"/>
-      <c r="K2" s="90"/>
-      <c r="L2" s="90"/>
-      <c r="M2" s="90"/>
-      <c r="N2" s="90"/>
+      <c r="B2" s="92"/>
+      <c r="C2" s="92"/>
+      <c r="D2" s="92"/>
+      <c r="E2" s="92"/>
+      <c r="F2" s="92"/>
+      <c r="G2" s="92"/>
+      <c r="H2" s="92"/>
+      <c r="I2" s="92"/>
+      <c r="J2" s="92"/>
+      <c r="K2" s="92"/>
+      <c r="L2" s="92"/>
+      <c r="M2" s="92"/>
+      <c r="N2" s="92"/>
       <c r="Z2"/>
     </row>
     <row r="3" spans="2:26" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="91" t="s">
+      <c r="B3" s="93" t="s">
         <v>93</v>
       </c>
-      <c r="C3" s="91"/>
-      <c r="D3" s="91"/>
-      <c r="E3" s="91"/>
-      <c r="F3" s="91"/>
-      <c r="G3" s="91"/>
-      <c r="H3" s="91"/>
-      <c r="I3" s="91"/>
-      <c r="J3" s="91"/>
-      <c r="K3" s="91"/>
-      <c r="L3" s="91"/>
-      <c r="M3" s="91"/>
-      <c r="N3" s="91"/>
+      <c r="C3" s="93"/>
+      <c r="D3" s="93"/>
+      <c r="E3" s="93"/>
+      <c r="F3" s="93"/>
+      <c r="G3" s="93"/>
+      <c r="H3" s="93"/>
+      <c r="I3" s="93"/>
+      <c r="J3" s="93"/>
+      <c r="K3" s="93"/>
+      <c r="L3" s="93"/>
+      <c r="M3" s="93"/>
+      <c r="N3" s="93"/>
       <c r="Z3"/>
     </row>
     <row r="5" spans="2:26" x14ac:dyDescent="0.25">
@@ -4921,7 +5056,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:Z8"/>
   <sheetViews>
@@ -4943,37 +5078,37 @@
       <c r="Z1" s="38"/>
     </row>
     <row r="2" spans="2:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="90"/>
-      <c r="C2" s="90"/>
-      <c r="D2" s="90"/>
-      <c r="E2" s="90"/>
-      <c r="F2" s="90"/>
-      <c r="G2" s="90"/>
-      <c r="H2" s="90"/>
-      <c r="I2" s="90"/>
-      <c r="J2" s="90"/>
-      <c r="K2" s="90"/>
-      <c r="L2" s="90"/>
-      <c r="M2" s="90"/>
-      <c r="N2" s="90"/>
+      <c r="B2" s="92"/>
+      <c r="C2" s="92"/>
+      <c r="D2" s="92"/>
+      <c r="E2" s="92"/>
+      <c r="F2" s="92"/>
+      <c r="G2" s="92"/>
+      <c r="H2" s="92"/>
+      <c r="I2" s="92"/>
+      <c r="J2" s="92"/>
+      <c r="K2" s="92"/>
+      <c r="L2" s="92"/>
+      <c r="M2" s="92"/>
+      <c r="N2" s="92"/>
       <c r="Z2"/>
     </row>
     <row r="3" spans="2:26" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="91" t="s">
+      <c r="B3" s="93" t="s">
         <v>72</v>
       </c>
-      <c r="C3" s="91"/>
-      <c r="D3" s="91"/>
-      <c r="E3" s="91"/>
-      <c r="F3" s="91"/>
-      <c r="G3" s="91"/>
-      <c r="H3" s="91"/>
-      <c r="I3" s="91"/>
-      <c r="J3" s="91"/>
-      <c r="K3" s="91"/>
-      <c r="L3" s="91"/>
-      <c r="M3" s="91"/>
-      <c r="N3" s="91"/>
+      <c r="C3" s="93"/>
+      <c r="D3" s="93"/>
+      <c r="E3" s="93"/>
+      <c r="F3" s="93"/>
+      <c r="G3" s="93"/>
+      <c r="H3" s="93"/>
+      <c r="I3" s="93"/>
+      <c r="J3" s="93"/>
+      <c r="K3" s="93"/>
+      <c r="L3" s="93"/>
+      <c r="M3" s="93"/>
+      <c r="N3" s="93"/>
       <c r="Z3"/>
     </row>
     <row r="5" spans="2:26" x14ac:dyDescent="0.25">
@@ -5051,7 +5186,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:Q7"/>
   <sheetViews>
@@ -5086,56 +5221,56 @@
       </c>
     </row>
     <row r="2" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="90"/>
-      <c r="C2" s="90"/>
-      <c r="D2" s="90"/>
-      <c r="E2" s="90"/>
-      <c r="F2" s="90"/>
-      <c r="G2" s="90"/>
-      <c r="H2" s="90"/>
-      <c r="I2" s="90"/>
-      <c r="J2" s="90"/>
-      <c r="K2" s="90"/>
-      <c r="L2" s="90"/>
+      <c r="B2" s="92"/>
+      <c r="C2" s="92"/>
+      <c r="D2" s="92"/>
+      <c r="E2" s="92"/>
+      <c r="F2" s="92"/>
+      <c r="G2" s="92"/>
+      <c r="H2" s="92"/>
+      <c r="I2" s="92"/>
+      <c r="J2" s="92"/>
+      <c r="K2" s="92"/>
+      <c r="L2" s="92"/>
     </row>
     <row r="3" spans="2:17" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="91" t="s">
+      <c r="B3" s="93" t="s">
         <v>108</v>
       </c>
-      <c r="C3" s="91"/>
-      <c r="D3" s="91"/>
-      <c r="E3" s="91"/>
-      <c r="F3" s="91"/>
-      <c r="G3" s="91"/>
-      <c r="H3" s="91"/>
-      <c r="I3" s="91"/>
-      <c r="J3" s="91"/>
-      <c r="K3" s="91"/>
-      <c r="L3" s="91"/>
+      <c r="C3" s="93"/>
+      <c r="D3" s="93"/>
+      <c r="E3" s="93"/>
+      <c r="F3" s="93"/>
+      <c r="G3" s="93"/>
+      <c r="H3" s="93"/>
+      <c r="I3" s="93"/>
+      <c r="J3" s="93"/>
+      <c r="K3" s="93"/>
+      <c r="L3" s="93"/>
     </row>
     <row r="5" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D5" s="98" t="s">
+      <c r="D5" s="100" t="s">
         <v>123</v>
       </c>
-      <c r="E5" s="98"/>
+      <c r="E5" s="100"/>
       <c r="F5" s="73"/>
       <c r="G5" s="73"/>
       <c r="H5" s="73"/>
       <c r="I5" s="73"/>
-      <c r="J5" s="98" t="s">
+      <c r="J5" s="100" t="s">
         <v>42</v>
       </c>
-      <c r="K5" s="98"/>
-      <c r="L5" s="98"/>
-      <c r="M5" s="98" t="s">
+      <c r="K5" s="100"/>
+      <c r="L5" s="100"/>
+      <c r="M5" s="100" t="s">
         <v>130</v>
       </c>
-      <c r="N5" s="98"/>
-      <c r="O5" s="98"/>
-      <c r="P5" s="92" t="s">
+      <c r="N5" s="100"/>
+      <c r="O5" s="100"/>
+      <c r="P5" s="94" t="s">
         <v>109</v>
       </c>
-      <c r="Q5" s="92"/>
+      <c r="Q5" s="94"/>
     </row>
     <row r="6" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="70" t="s">
@@ -5218,7 +5353,104 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:N6"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.85546875" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" customWidth="1"/>
+    <col min="3" max="3" width="30.28515625" customWidth="1"/>
+    <col min="4" max="4" width="33.140625" customWidth="1"/>
+    <col min="5" max="5" width="21.7109375" customWidth="1"/>
+    <col min="6" max="6" width="22.140625" customWidth="1"/>
+    <col min="7" max="7" width="26" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:14" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B1" s="46" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="92"/>
+      <c r="C2" s="92"/>
+      <c r="D2" s="92"/>
+      <c r="E2" s="92"/>
+      <c r="F2" s="92"/>
+      <c r="G2" s="92"/>
+      <c r="H2" s="92"/>
+      <c r="I2" s="92"/>
+      <c r="J2" s="92"/>
+      <c r="K2" s="92"/>
+      <c r="L2" s="92"/>
+      <c r="M2" s="92"/>
+      <c r="N2" s="92"/>
+    </row>
+    <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B3" s="93" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="93"/>
+      <c r="D3" s="93"/>
+      <c r="E3" s="93"/>
+      <c r="F3" s="93"/>
+      <c r="G3" s="93"/>
+      <c r="H3" s="93"/>
+      <c r="I3" s="93"/>
+      <c r="J3" s="93"/>
+      <c r="K3" s="93"/>
+      <c r="L3" s="93"/>
+      <c r="M3" s="93"/>
+      <c r="N3" s="93"/>
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B5" s="44" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5" s="44" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="45" t="s">
+        <v>76</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="6"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:N2"/>
+    <mergeCell ref="B3:N3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:Y8"/>
   <sheetViews>
@@ -5259,110 +5491,110 @@
       </c>
     </row>
     <row r="2" spans="2:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="90"/>
-      <c r="C2" s="90"/>
-      <c r="D2" s="90"/>
-      <c r="E2" s="90"/>
-      <c r="F2" s="90"/>
-      <c r="G2" s="90"/>
-      <c r="H2" s="90"/>
-      <c r="I2" s="90"/>
-      <c r="J2" s="90"/>
-      <c r="K2" s="90"/>
-      <c r="L2" s="90"/>
-      <c r="M2" s="90"/>
-      <c r="N2" s="90"/>
-      <c r="O2" s="90"/>
-      <c r="P2" s="90"/>
+      <c r="B2" s="92"/>
+      <c r="C2" s="92"/>
+      <c r="D2" s="92"/>
+      <c r="E2" s="92"/>
+      <c r="F2" s="92"/>
+      <c r="G2" s="92"/>
+      <c r="H2" s="92"/>
+      <c r="I2" s="92"/>
+      <c r="J2" s="92"/>
+      <c r="K2" s="92"/>
+      <c r="L2" s="92"/>
+      <c r="M2" s="92"/>
+      <c r="N2" s="92"/>
+      <c r="O2" s="92"/>
+      <c r="P2" s="92"/>
       <c r="Q2" s="56"/>
       <c r="R2" s="56"/>
     </row>
     <row r="3" spans="2:25" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="91" t="s">
+      <c r="B3" s="93" t="s">
         <v>111</v>
       </c>
-      <c r="C3" s="91"/>
-      <c r="D3" s="91"/>
-      <c r="E3" s="91"/>
-      <c r="F3" s="91"/>
-      <c r="G3" s="91"/>
-      <c r="H3" s="91"/>
-      <c r="I3" s="91"/>
-      <c r="J3" s="91"/>
-      <c r="K3" s="91"/>
-      <c r="L3" s="91"/>
-      <c r="M3" s="91"/>
-      <c r="N3" s="91"/>
-      <c r="O3" s="91"/>
-      <c r="P3" s="91"/>
+      <c r="C3" s="93"/>
+      <c r="D3" s="93"/>
+      <c r="E3" s="93"/>
+      <c r="F3" s="93"/>
+      <c r="G3" s="93"/>
+      <c r="H3" s="93"/>
+      <c r="I3" s="93"/>
+      <c r="J3" s="93"/>
+      <c r="K3" s="93"/>
+      <c r="L3" s="93"/>
+      <c r="M3" s="93"/>
+      <c r="N3" s="93"/>
+      <c r="O3" s="93"/>
+      <c r="P3" s="93"/>
       <c r="Q3" s="57"/>
       <c r="R3" s="57"/>
     </row>
     <row r="5" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B5" s="101" t="s">
+      <c r="B5" s="105" t="s">
         <v>112</v>
       </c>
-      <c r="C5" s="102"/>
-      <c r="D5" s="102"/>
-      <c r="E5" s="102"/>
-      <c r="F5" s="102"/>
-      <c r="G5" s="102"/>
-      <c r="H5" s="102"/>
-      <c r="I5" s="102"/>
-      <c r="J5" s="102"/>
-      <c r="K5" s="102"/>
-      <c r="L5" s="103"/>
-      <c r="M5" s="101" t="s">
+      <c r="C5" s="106"/>
+      <c r="D5" s="106"/>
+      <c r="E5" s="106"/>
+      <c r="F5" s="106"/>
+      <c r="G5" s="106"/>
+      <c r="H5" s="106"/>
+      <c r="I5" s="106"/>
+      <c r="J5" s="106"/>
+      <c r="K5" s="106"/>
+      <c r="L5" s="107"/>
+      <c r="M5" s="105" t="s">
         <v>113</v>
       </c>
-      <c r="N5" s="102"/>
-      <c r="O5" s="102"/>
-      <c r="P5" s="102"/>
-      <c r="Q5" s="102"/>
-      <c r="R5" s="102"/>
-      <c r="S5" s="102"/>
-      <c r="T5" s="102"/>
-      <c r="U5" s="102"/>
-      <c r="V5" s="102"/>
-      <c r="W5" s="102"/>
-      <c r="X5" s="102"/>
-      <c r="Y5" s="103"/>
+      <c r="N5" s="106"/>
+      <c r="O5" s="106"/>
+      <c r="P5" s="106"/>
+      <c r="Q5" s="106"/>
+      <c r="R5" s="106"/>
+      <c r="S5" s="106"/>
+      <c r="T5" s="106"/>
+      <c r="U5" s="106"/>
+      <c r="V5" s="106"/>
+      <c r="W5" s="106"/>
+      <c r="X5" s="106"/>
+      <c r="Y5" s="107"/>
     </row>
     <row r="6" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B6" s="111"/>
-      <c r="C6" s="111"/>
-      <c r="D6" s="111"/>
-      <c r="E6" s="111"/>
-      <c r="F6" s="107" t="s">
+      <c r="B6" s="104"/>
+      <c r="C6" s="104"/>
+      <c r="D6" s="104"/>
+      <c r="E6" s="104"/>
+      <c r="F6" s="111" t="s">
         <v>27</v>
       </c>
-      <c r="G6" s="108"/>
-      <c r="H6" s="108"/>
-      <c r="I6" s="109"/>
-      <c r="J6" s="101" t="s">
+      <c r="G6" s="112"/>
+      <c r="H6" s="112"/>
+      <c r="I6" s="113"/>
+      <c r="J6" s="105" t="s">
         <v>30</v>
       </c>
-      <c r="K6" s="102"/>
-      <c r="L6" s="103"/>
-      <c r="M6" s="89"/>
-      <c r="N6" s="99" t="s">
+      <c r="K6" s="106"/>
+      <c r="L6" s="107"/>
+      <c r="M6" s="88"/>
+      <c r="N6" s="101" t="s">
         <v>42</v>
       </c>
-      <c r="O6" s="100"/>
-      <c r="P6" s="99" t="s">
+      <c r="O6" s="102"/>
+      <c r="P6" s="101" t="s">
         <v>106</v>
       </c>
-      <c r="Q6" s="110"/>
-      <c r="R6" s="100"/>
-      <c r="S6" s="89"/>
-      <c r="T6" s="99" t="s">
+      <c r="Q6" s="103"/>
+      <c r="R6" s="102"/>
+      <c r="S6" s="88"/>
+      <c r="T6" s="101" t="s">
         <v>123</v>
       </c>
-      <c r="U6" s="100"/>
-      <c r="V6" s="104"/>
-      <c r="W6" s="105"/>
-      <c r="X6" s="105"/>
-      <c r="Y6" s="106"/>
+      <c r="U6" s="102"/>
+      <c r="V6" s="108"/>
+      <c r="W6" s="109"/>
+      <c r="X6" s="109"/>
+      <c r="Y6" s="110"/>
     </row>
     <row r="7" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B7" s="75" t="s">
@@ -5466,10 +5698,6 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="T6:U6"/>
-    <mergeCell ref="M5:Y5"/>
-    <mergeCell ref="V6:Y6"/>
     <mergeCell ref="B2:P2"/>
     <mergeCell ref="B3:P3"/>
     <mergeCell ref="B5:L5"/>
@@ -5477,110 +5705,17 @@
     <mergeCell ref="F6:I6"/>
     <mergeCell ref="N6:O6"/>
     <mergeCell ref="P6:R6"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="T6:U6"/>
+    <mergeCell ref="M5:Y5"/>
+    <mergeCell ref="V6:Y6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:N6"/>
-  <sheetViews>
-    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="2.85546875" customWidth="1"/>
-    <col min="2" max="2" width="22.140625" customWidth="1"/>
-    <col min="3" max="3" width="30.28515625" customWidth="1"/>
-    <col min="4" max="4" width="33.140625" customWidth="1"/>
-    <col min="5" max="5" width="21.7109375" customWidth="1"/>
-    <col min="6" max="6" width="22.140625" customWidth="1"/>
-    <col min="7" max="7" width="26" customWidth="1"/>
-    <col min="8" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:14" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="46" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="90"/>
-      <c r="C2" s="90"/>
-      <c r="D2" s="90"/>
-      <c r="E2" s="90"/>
-      <c r="F2" s="90"/>
-      <c r="G2" s="90"/>
-      <c r="H2" s="90"/>
-      <c r="I2" s="90"/>
-      <c r="J2" s="90"/>
-      <c r="K2" s="90"/>
-      <c r="L2" s="90"/>
-      <c r="M2" s="90"/>
-      <c r="N2" s="90"/>
-    </row>
-    <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="91" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="91"/>
-      <c r="D3" s="91"/>
-      <c r="E3" s="91"/>
-      <c r="F3" s="91"/>
-      <c r="G3" s="91"/>
-      <c r="H3" s="91"/>
-      <c r="I3" s="91"/>
-      <c r="J3" s="91"/>
-      <c r="K3" s="91"/>
-      <c r="L3" s="91"/>
-      <c r="M3" s="91"/>
-      <c r="N3" s="91"/>
-    </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B5" s="44" t="s">
-        <v>77</v>
-      </c>
-      <c r="C5" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="45" t="s">
-        <v>76</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="6"/>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B2:N2"/>
-    <mergeCell ref="B3:N3"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A24"/>
   <sheetViews>
@@ -5694,40 +5829,40 @@
       </c>
     </row>
     <row r="2" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="90"/>
-      <c r="C2" s="90"/>
-      <c r="D2" s="90"/>
-      <c r="E2" s="90"/>
-      <c r="F2" s="90"/>
-      <c r="G2" s="90"/>
-      <c r="H2" s="90"/>
-      <c r="I2" s="90"/>
-      <c r="J2" s="90"/>
-      <c r="K2" s="90"/>
-      <c r="L2" s="90"/>
-      <c r="M2" s="90"/>
-      <c r="N2" s="90"/>
-      <c r="O2" s="90"/>
-      <c r="P2" s="90"/>
+      <c r="B2" s="92"/>
+      <c r="C2" s="92"/>
+      <c r="D2" s="92"/>
+      <c r="E2" s="92"/>
+      <c r="F2" s="92"/>
+      <c r="G2" s="92"/>
+      <c r="H2" s="92"/>
+      <c r="I2" s="92"/>
+      <c r="J2" s="92"/>
+      <c r="K2" s="92"/>
+      <c r="L2" s="92"/>
+      <c r="M2" s="92"/>
+      <c r="N2" s="92"/>
+      <c r="O2" s="92"/>
+      <c r="P2" s="92"/>
     </row>
     <row r="3" spans="2:16" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="91" t="s">
+      <c r="B3" s="93" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="91"/>
-      <c r="D3" s="91"/>
-      <c r="E3" s="91"/>
-      <c r="F3" s="91"/>
-      <c r="G3" s="91"/>
-      <c r="H3" s="91"/>
-      <c r="I3" s="91"/>
-      <c r="J3" s="91"/>
-      <c r="K3" s="91"/>
-      <c r="L3" s="91"/>
-      <c r="M3" s="91"/>
-      <c r="N3" s="91"/>
-      <c r="O3" s="91"/>
-      <c r="P3" s="91"/>
+      <c r="C3" s="93"/>
+      <c r="D3" s="93"/>
+      <c r="E3" s="93"/>
+      <c r="F3" s="93"/>
+      <c r="G3" s="93"/>
+      <c r="H3" s="93"/>
+      <c r="I3" s="93"/>
+      <c r="J3" s="93"/>
+      <c r="K3" s="93"/>
+      <c r="L3" s="93"/>
+      <c r="M3" s="93"/>
+      <c r="N3" s="93"/>
+      <c r="O3" s="93"/>
+      <c r="P3" s="93"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="44" t="s">
@@ -5806,40 +5941,40 @@
       </c>
     </row>
     <row r="2" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="90"/>
-      <c r="C2" s="90"/>
-      <c r="D2" s="90"/>
-      <c r="E2" s="90"/>
-      <c r="F2" s="90"/>
-      <c r="G2" s="90"/>
-      <c r="H2" s="90"/>
-      <c r="I2" s="90"/>
-      <c r="J2" s="90"/>
-      <c r="K2" s="90"/>
-      <c r="L2" s="90"/>
-      <c r="M2" s="90"/>
-      <c r="N2" s="90"/>
-      <c r="O2" s="90"/>
-      <c r="P2" s="90"/>
+      <c r="B2" s="92"/>
+      <c r="C2" s="92"/>
+      <c r="D2" s="92"/>
+      <c r="E2" s="92"/>
+      <c r="F2" s="92"/>
+      <c r="G2" s="92"/>
+      <c r="H2" s="92"/>
+      <c r="I2" s="92"/>
+      <c r="J2" s="92"/>
+      <c r="K2" s="92"/>
+      <c r="L2" s="92"/>
+      <c r="M2" s="92"/>
+      <c r="N2" s="92"/>
+      <c r="O2" s="92"/>
+      <c r="P2" s="92"/>
     </row>
     <row r="3" spans="2:16" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="91" t="s">
+      <c r="B3" s="93" t="s">
         <v>68</v>
       </c>
-      <c r="C3" s="91"/>
-      <c r="D3" s="91"/>
-      <c r="E3" s="91"/>
-      <c r="F3" s="91"/>
-      <c r="G3" s="91"/>
-      <c r="H3" s="91"/>
-      <c r="I3" s="91"/>
-      <c r="J3" s="91"/>
-      <c r="K3" s="91"/>
-      <c r="L3" s="91"/>
-      <c r="M3" s="91"/>
-      <c r="N3" s="91"/>
-      <c r="O3" s="91"/>
-      <c r="P3" s="91"/>
+      <c r="C3" s="93"/>
+      <c r="D3" s="93"/>
+      <c r="E3" s="93"/>
+      <c r="F3" s="93"/>
+      <c r="G3" s="93"/>
+      <c r="H3" s="93"/>
+      <c r="I3" s="93"/>
+      <c r="J3" s="93"/>
+      <c r="K3" s="93"/>
+      <c r="L3" s="93"/>
+      <c r="M3" s="93"/>
+      <c r="N3" s="93"/>
+      <c r="O3" s="93"/>
+      <c r="P3" s="93"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
@@ -5888,40 +6023,40 @@
       </c>
     </row>
     <row r="2" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="90"/>
-      <c r="C2" s="90"/>
-      <c r="D2" s="90"/>
-      <c r="E2" s="90"/>
-      <c r="F2" s="90"/>
-      <c r="G2" s="90"/>
-      <c r="H2" s="90"/>
-      <c r="I2" s="90"/>
-      <c r="J2" s="90"/>
-      <c r="K2" s="90"/>
-      <c r="L2" s="90"/>
-      <c r="M2" s="90"/>
-      <c r="N2" s="90"/>
-      <c r="O2" s="90"/>
-      <c r="P2" s="90"/>
+      <c r="B2" s="92"/>
+      <c r="C2" s="92"/>
+      <c r="D2" s="92"/>
+      <c r="E2" s="92"/>
+      <c r="F2" s="92"/>
+      <c r="G2" s="92"/>
+      <c r="H2" s="92"/>
+      <c r="I2" s="92"/>
+      <c r="J2" s="92"/>
+      <c r="K2" s="92"/>
+      <c r="L2" s="92"/>
+      <c r="M2" s="92"/>
+      <c r="N2" s="92"/>
+      <c r="O2" s="92"/>
+      <c r="P2" s="92"/>
     </row>
     <row r="3" spans="2:16" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="91" t="s">
+      <c r="B3" s="93" t="s">
         <v>71</v>
       </c>
-      <c r="C3" s="91"/>
-      <c r="D3" s="91"/>
-      <c r="E3" s="91"/>
-      <c r="F3" s="91"/>
-      <c r="G3" s="91"/>
-      <c r="H3" s="91"/>
-      <c r="I3" s="91"/>
-      <c r="J3" s="91"/>
-      <c r="K3" s="91"/>
-      <c r="L3" s="91"/>
-      <c r="M3" s="91"/>
-      <c r="N3" s="91"/>
-      <c r="O3" s="91"/>
-      <c r="P3" s="91"/>
+      <c r="C3" s="93"/>
+      <c r="D3" s="93"/>
+      <c r="E3" s="93"/>
+      <c r="F3" s="93"/>
+      <c r="G3" s="93"/>
+      <c r="H3" s="93"/>
+      <c r="I3" s="93"/>
+      <c r="J3" s="93"/>
+      <c r="K3" s="93"/>
+      <c r="L3" s="93"/>
+      <c r="M3" s="93"/>
+      <c r="N3" s="93"/>
+      <c r="O3" s="93"/>
+      <c r="P3" s="93"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
@@ -5975,36 +6110,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="90"/>
-      <c r="C2" s="90"/>
-      <c r="D2" s="90"/>
-      <c r="E2" s="90"/>
-      <c r="F2" s="90"/>
-      <c r="G2" s="90"/>
-      <c r="H2" s="90"/>
-      <c r="I2" s="90"/>
-      <c r="J2" s="90"/>
-      <c r="K2" s="90"/>
-      <c r="L2" s="90"/>
-      <c r="M2" s="90"/>
-      <c r="N2" s="90"/>
+      <c r="B2" s="92"/>
+      <c r="C2" s="92"/>
+      <c r="D2" s="92"/>
+      <c r="E2" s="92"/>
+      <c r="F2" s="92"/>
+      <c r="G2" s="92"/>
+      <c r="H2" s="92"/>
+      <c r="I2" s="92"/>
+      <c r="J2" s="92"/>
+      <c r="K2" s="92"/>
+      <c r="L2" s="92"/>
+      <c r="M2" s="92"/>
+      <c r="N2" s="92"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="91" t="s">
+      <c r="B3" s="93" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="91"/>
-      <c r="D3" s="91"/>
-      <c r="E3" s="91"/>
-      <c r="F3" s="91"/>
-      <c r="G3" s="91"/>
-      <c r="H3" s="91"/>
-      <c r="I3" s="91"/>
-      <c r="J3" s="91"/>
-      <c r="K3" s="91"/>
-      <c r="L3" s="91"/>
-      <c r="M3" s="91"/>
-      <c r="N3" s="91"/>
+      <c r="C3" s="93"/>
+      <c r="D3" s="93"/>
+      <c r="E3" s="93"/>
+      <c r="F3" s="93"/>
+      <c r="G3" s="93"/>
+      <c r="H3" s="93"/>
+      <c r="I3" s="93"/>
+      <c r="J3" s="93"/>
+      <c r="K3" s="93"/>
+      <c r="L3" s="93"/>
+      <c r="M3" s="93"/>
+      <c r="N3" s="93"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="44" t="s">
@@ -6069,7 +6204,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:P6"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="B3" sqref="B3:P3"/>
     </sheetView>
   </sheetViews>
@@ -6093,40 +6228,40 @@
       </c>
     </row>
     <row r="2" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="90"/>
-      <c r="C2" s="90"/>
-      <c r="D2" s="90"/>
-      <c r="E2" s="90"/>
-      <c r="F2" s="90"/>
-      <c r="G2" s="90"/>
-      <c r="H2" s="90"/>
-      <c r="I2" s="90"/>
-      <c r="J2" s="90"/>
-      <c r="K2" s="90"/>
-      <c r="L2" s="90"/>
-      <c r="M2" s="90"/>
-      <c r="N2" s="90"/>
-      <c r="O2" s="90"/>
-      <c r="P2" s="90"/>
+      <c r="B2" s="92"/>
+      <c r="C2" s="92"/>
+      <c r="D2" s="92"/>
+      <c r="E2" s="92"/>
+      <c r="F2" s="92"/>
+      <c r="G2" s="92"/>
+      <c r="H2" s="92"/>
+      <c r="I2" s="92"/>
+      <c r="J2" s="92"/>
+      <c r="K2" s="92"/>
+      <c r="L2" s="92"/>
+      <c r="M2" s="92"/>
+      <c r="N2" s="92"/>
+      <c r="O2" s="92"/>
+      <c r="P2" s="92"/>
     </row>
     <row r="3" spans="2:16" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="91" t="s">
+      <c r="B3" s="93" t="s">
         <v>65</v>
       </c>
-      <c r="C3" s="91"/>
-      <c r="D3" s="91"/>
-      <c r="E3" s="91"/>
-      <c r="F3" s="91"/>
-      <c r="G3" s="91"/>
-      <c r="H3" s="91"/>
-      <c r="I3" s="91"/>
-      <c r="J3" s="91"/>
-      <c r="K3" s="91"/>
-      <c r="L3" s="91"/>
-      <c r="M3" s="91"/>
-      <c r="N3" s="91"/>
-      <c r="O3" s="91"/>
-      <c r="P3" s="91"/>
+      <c r="C3" s="93"/>
+      <c r="D3" s="93"/>
+      <c r="E3" s="93"/>
+      <c r="F3" s="93"/>
+      <c r="G3" s="93"/>
+      <c r="H3" s="93"/>
+      <c r="I3" s="93"/>
+      <c r="J3" s="93"/>
+      <c r="K3" s="93"/>
+      <c r="L3" s="93"/>
+      <c r="M3" s="93"/>
+      <c r="N3" s="93"/>
+      <c r="O3" s="93"/>
+      <c r="P3" s="93"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="45" t="s">
@@ -6135,14 +6270,14 @@
       <c r="C5" s="45" t="s">
         <v>67</v>
       </c>
-      <c r="D5" s="113" t="s">
+      <c r="D5" s="91" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
-      <c r="D6" s="112"/>
+      <c r="D6" s="90"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -6182,36 +6317,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="90"/>
-      <c r="C2" s="90"/>
-      <c r="D2" s="90"/>
-      <c r="E2" s="90"/>
-      <c r="F2" s="90"/>
-      <c r="G2" s="90"/>
-      <c r="H2" s="90"/>
-      <c r="I2" s="90"/>
-      <c r="J2" s="90"/>
-      <c r="K2" s="90"/>
-      <c r="L2" s="90"/>
-      <c r="M2" s="90"/>
-      <c r="N2" s="90"/>
+      <c r="B2" s="92"/>
+      <c r="C2" s="92"/>
+      <c r="D2" s="92"/>
+      <c r="E2" s="92"/>
+      <c r="F2" s="92"/>
+      <c r="G2" s="92"/>
+      <c r="H2" s="92"/>
+      <c r="I2" s="92"/>
+      <c r="J2" s="92"/>
+      <c r="K2" s="92"/>
+      <c r="L2" s="92"/>
+      <c r="M2" s="92"/>
+      <c r="N2" s="92"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="91" t="s">
+      <c r="B3" s="93" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="91"/>
-      <c r="D3" s="91"/>
-      <c r="E3" s="91"/>
-      <c r="F3" s="91"/>
-      <c r="G3" s="91"/>
-      <c r="H3" s="91"/>
-      <c r="I3" s="91"/>
-      <c r="J3" s="91"/>
-      <c r="K3" s="91"/>
-      <c r="L3" s="91"/>
-      <c r="M3" s="91"/>
-      <c r="N3" s="91"/>
+      <c r="C3" s="93"/>
+      <c r="D3" s="93"/>
+      <c r="E3" s="93"/>
+      <c r="F3" s="93"/>
+      <c r="G3" s="93"/>
+      <c r="H3" s="93"/>
+      <c r="I3" s="93"/>
+      <c r="J3" s="93"/>
+      <c r="K3" s="93"/>
+      <c r="L3" s="93"/>
+      <c r="M3" s="93"/>
+      <c r="N3" s="93"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">

</xml_diff>

<commit_message>
TRIEDA-1471 - Alterando associação de curriculoDisciplina-sala para disciplina-sala e curriculoDisciplina-gruposSala para disciplina-gruposSala.
</commit_message>
<xml_diff>
--- a/code/client/web/src/main/resources/templateExport.xlsx
+++ b/code/client/web/src/main/resources/templateExport.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2505" windowWidth="17070" windowHeight="5310" tabRatio="907" firstSheet="20" activeTab="21"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="17070" windowHeight="5370" tabRatio="907" firstSheet="3" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Campi" sheetId="3" r:id="rId1"/>
@@ -989,7 +989,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Código do Curso relacionado a equivalencia, Vazio significa uma equivalencia geral</t>
         </r>
@@ -1230,7 +1230,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="192">
   <si>
     <t>Planilha de Unidades</t>
   </si>
@@ -1494,9 +1494,6 @@
   </si>
   <si>
     <t>Nome Disciplina</t>
-  </si>
-  <si>
-    <t>Código Matriz Curricular</t>
   </si>
   <si>
     <t>Código Currículo</t>
@@ -1864,7 +1861,7 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -2490,6 +2487,15 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="7" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="7" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2499,6 +2505,9 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2523,49 +2532,37 @@
     <xf numFmtId="0" fontId="9" fillId="28" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="28" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="28" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="7" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="7" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2891,42 +2888,42 @@
   <sheetData>
     <row r="1" spans="2:14" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="95" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="92" t="s">
-        <v>96</v>
-      </c>
-      <c r="C2" s="92"/>
-      <c r="D2" s="92"/>
-      <c r="E2" s="92"/>
-      <c r="F2" s="92"/>
-      <c r="G2" s="92"/>
-      <c r="H2" s="92"/>
-      <c r="I2" s="92"/>
-      <c r="J2" s="92"/>
-      <c r="K2" s="92"/>
-      <c r="L2" s="92"/>
-      <c r="M2" s="92"/>
-      <c r="N2" s="92"/>
+      <c r="C2" s="95"/>
+      <c r="D2" s="95"/>
+      <c r="E2" s="95"/>
+      <c r="F2" s="95"/>
+      <c r="G2" s="95"/>
+      <c r="H2" s="95"/>
+      <c r="I2" s="95"/>
+      <c r="J2" s="95"/>
+      <c r="K2" s="95"/>
+      <c r="L2" s="95"/>
+      <c r="M2" s="95"/>
+      <c r="N2" s="95"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="93" t="s">
+      <c r="B3" s="96" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="93"/>
-      <c r="D3" s="93"/>
-      <c r="E3" s="93"/>
-      <c r="F3" s="93"/>
-      <c r="G3" s="93"/>
-      <c r="H3" s="93"/>
-      <c r="I3" s="93"/>
-      <c r="J3" s="93"/>
-      <c r="K3" s="93"/>
-      <c r="L3" s="93"/>
-      <c r="M3" s="93"/>
-      <c r="N3" s="93"/>
+      <c r="C3" s="96"/>
+      <c r="D3" s="96"/>
+      <c r="E3" s="96"/>
+      <c r="F3" s="96"/>
+      <c r="G3" s="96"/>
+      <c r="H3" s="96"/>
+      <c r="I3" s="96"/>
+      <c r="J3" s="96"/>
+      <c r="K3" s="96"/>
+      <c r="L3" s="96"/>
+      <c r="M3" s="96"/>
+      <c r="N3" s="96"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="44" t="s">
@@ -2990,50 +2987,50 @@
   <sheetData>
     <row r="1" spans="2:14" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="92"/>
-      <c r="C2" s="92"/>
-      <c r="D2" s="92"/>
-      <c r="E2" s="92"/>
-      <c r="F2" s="92"/>
-      <c r="G2" s="92"/>
-      <c r="H2" s="92"/>
-      <c r="I2" s="92"/>
-      <c r="J2" s="92"/>
-      <c r="K2" s="92"/>
-      <c r="L2" s="92"/>
-      <c r="M2" s="92"/>
-      <c r="N2" s="92"/>
+      <c r="B2" s="95"/>
+      <c r="C2" s="95"/>
+      <c r="D2" s="95"/>
+      <c r="E2" s="95"/>
+      <c r="F2" s="95"/>
+      <c r="G2" s="95"/>
+      <c r="H2" s="95"/>
+      <c r="I2" s="95"/>
+      <c r="J2" s="95"/>
+      <c r="K2" s="95"/>
+      <c r="L2" s="95"/>
+      <c r="M2" s="95"/>
+      <c r="N2" s="95"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="93" t="s">
+      <c r="B3" s="96" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="93"/>
-      <c r="D3" s="93"/>
-      <c r="E3" s="93"/>
-      <c r="F3" s="93"/>
-      <c r="G3" s="93"/>
-      <c r="H3" s="93"/>
-      <c r="I3" s="93"/>
-      <c r="J3" s="93"/>
-      <c r="K3" s="93"/>
-      <c r="L3" s="93"/>
-      <c r="M3" s="93"/>
-      <c r="N3" s="93"/>
+      <c r="C3" s="96"/>
+      <c r="D3" s="96"/>
+      <c r="E3" s="96"/>
+      <c r="F3" s="96"/>
+      <c r="G3" s="96"/>
+      <c r="H3" s="96"/>
+      <c r="I3" s="96"/>
+      <c r="J3" s="96"/>
+      <c r="K3" s="96"/>
+      <c r="L3" s="96"/>
+      <c r="M3" s="96"/>
+      <c r="N3" s="96"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>79</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>89</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>90</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>26</v>
@@ -3042,7 +3039,7 @@
         <v>27</v>
       </c>
       <c r="G5" s="47" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
@@ -3088,40 +3085,40 @@
   <sheetData>
     <row r="1" spans="2:14" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="92"/>
-      <c r="C2" s="92"/>
-      <c r="D2" s="92"/>
-      <c r="E2" s="92"/>
-      <c r="F2" s="92"/>
-      <c r="G2" s="92"/>
-      <c r="H2" s="92"/>
-      <c r="I2" s="92"/>
-      <c r="J2" s="92"/>
-      <c r="K2" s="92"/>
-      <c r="L2" s="92"/>
-      <c r="M2" s="92"/>
-      <c r="N2" s="92"/>
+      <c r="B2" s="95"/>
+      <c r="C2" s="95"/>
+      <c r="D2" s="95"/>
+      <c r="E2" s="95"/>
+      <c r="F2" s="95"/>
+      <c r="G2" s="95"/>
+      <c r="H2" s="95"/>
+      <c r="I2" s="95"/>
+      <c r="J2" s="95"/>
+      <c r="K2" s="95"/>
+      <c r="L2" s="95"/>
+      <c r="M2" s="95"/>
+      <c r="N2" s="95"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="93" t="s">
+      <c r="B3" s="96" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="93"/>
-      <c r="D3" s="93"/>
-      <c r="E3" s="93"/>
-      <c r="F3" s="93"/>
-      <c r="G3" s="93"/>
-      <c r="H3" s="93"/>
-      <c r="I3" s="93"/>
-      <c r="J3" s="93"/>
-      <c r="K3" s="93"/>
-      <c r="L3" s="93"/>
-      <c r="M3" s="93"/>
-      <c r="N3" s="93"/>
+      <c r="C3" s="96"/>
+      <c r="D3" s="96"/>
+      <c r="E3" s="96"/>
+      <c r="F3" s="96"/>
+      <c r="G3" s="96"/>
+      <c r="H3" s="96"/>
+      <c r="I3" s="96"/>
+      <c r="J3" s="96"/>
+      <c r="K3" s="96"/>
+      <c r="L3" s="96"/>
+      <c r="M3" s="96"/>
+      <c r="N3" s="96"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -3149,16 +3146,16 @@
         <v>58</v>
       </c>
       <c r="J5" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="K5" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="K5" s="4" t="s">
-        <v>107</v>
-      </c>
       <c r="L5" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
@@ -3202,32 +3199,32 @@
   <sheetData>
     <row r="1" spans="2:5" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="92"/>
-      <c r="C2" s="92"/>
-      <c r="D2" s="92"/>
-      <c r="E2" s="92"/>
+      <c r="B2" s="95"/>
+      <c r="C2" s="95"/>
+      <c r="D2" s="95"/>
+      <c r="E2" s="95"/>
     </row>
     <row r="3" spans="2:5" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="93" t="s">
-        <v>126</v>
-      </c>
-      <c r="C3" s="93"/>
-      <c r="D3" s="93"/>
-      <c r="E3" s="93"/>
+      <c r="B3" s="96" t="s">
+        <v>125</v>
+      </c>
+      <c r="C3" s="96"/>
+      <c r="D3" s="96"/>
+      <c r="E3" s="96"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="60" t="s">
+        <v>100</v>
+      </c>
+      <c r="C5" s="59" t="s">
         <v>101</v>
       </c>
-      <c r="C5" s="59" t="s">
-        <v>102</v>
-      </c>
       <c r="D5" s="59" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
@@ -3266,40 +3263,40 @@
   <sheetData>
     <row r="1" spans="2:14" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="92"/>
-      <c r="C2" s="92"/>
-      <c r="D2" s="92"/>
-      <c r="E2" s="92"/>
-      <c r="F2" s="92"/>
-      <c r="G2" s="92"/>
-      <c r="H2" s="92"/>
-      <c r="I2" s="92"/>
-      <c r="J2" s="92"/>
-      <c r="K2" s="92"/>
-      <c r="L2" s="92"/>
-      <c r="M2" s="92"/>
-      <c r="N2" s="92"/>
+      <c r="B2" s="95"/>
+      <c r="C2" s="95"/>
+      <c r="D2" s="95"/>
+      <c r="E2" s="95"/>
+      <c r="F2" s="95"/>
+      <c r="G2" s="95"/>
+      <c r="H2" s="95"/>
+      <c r="I2" s="95"/>
+      <c r="J2" s="95"/>
+      <c r="K2" s="95"/>
+      <c r="L2" s="95"/>
+      <c r="M2" s="95"/>
+      <c r="N2" s="95"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="93" t="s">
-        <v>100</v>
-      </c>
-      <c r="C3" s="93"/>
-      <c r="D3" s="93"/>
-      <c r="E3" s="93"/>
-      <c r="F3" s="93"/>
-      <c r="G3" s="93"/>
-      <c r="H3" s="93"/>
-      <c r="I3" s="93"/>
-      <c r="J3" s="93"/>
-      <c r="K3" s="93"/>
-      <c r="L3" s="93"/>
-      <c r="M3" s="93"/>
-      <c r="N3" s="93"/>
+      <c r="B3" s="96" t="s">
+        <v>99</v>
+      </c>
+      <c r="C3" s="96"/>
+      <c r="D3" s="96"/>
+      <c r="E3" s="96"/>
+      <c r="F3" s="96"/>
+      <c r="G3" s="96"/>
+      <c r="H3" s="96"/>
+      <c r="I3" s="96"/>
+      <c r="J3" s="96"/>
+      <c r="K3" s="96"/>
+      <c r="L3" s="96"/>
+      <c r="M3" s="96"/>
+      <c r="N3" s="96"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -3321,21 +3318,21 @@
         <v>86</v>
       </c>
       <c r="H5" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="I5" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="J5" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="J5" s="4" t="s">
+      <c r="K5" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="K5" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="L5" s="94" t="s">
-        <v>110</v>
-      </c>
-      <c r="M5" s="94"/>
+      <c r="L5" s="97" t="s">
+        <v>109</v>
+      </c>
+      <c r="M5" s="97"/>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
@@ -3383,49 +3380,49 @@
   <sheetData>
     <row r="1" spans="2:15" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="2:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="92"/>
-      <c r="C2" s="92"/>
-      <c r="D2" s="92"/>
-      <c r="E2" s="92"/>
-      <c r="F2" s="92"/>
-      <c r="G2" s="92"/>
-      <c r="H2" s="92"/>
-      <c r="I2" s="92"/>
-      <c r="J2" s="92"/>
-      <c r="K2" s="92"/>
-      <c r="L2" s="92"/>
-      <c r="M2" s="92"/>
-      <c r="N2" s="92"/>
-      <c r="O2" s="92"/>
+      <c r="B2" s="95"/>
+      <c r="C2" s="95"/>
+      <c r="D2" s="95"/>
+      <c r="E2" s="95"/>
+      <c r="F2" s="95"/>
+      <c r="G2" s="95"/>
+      <c r="H2" s="95"/>
+      <c r="I2" s="95"/>
+      <c r="J2" s="95"/>
+      <c r="K2" s="95"/>
+      <c r="L2" s="95"/>
+      <c r="M2" s="95"/>
+      <c r="N2" s="95"/>
+      <c r="O2" s="95"/>
     </row>
     <row r="3" spans="2:15" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="93" t="s">
+      <c r="B3" s="96" t="s">
         <v>73</v>
       </c>
-      <c r="C3" s="93"/>
-      <c r="D3" s="93"/>
-      <c r="E3" s="93"/>
-      <c r="F3" s="93"/>
-      <c r="G3" s="93"/>
-      <c r="H3" s="93"/>
-      <c r="I3" s="93"/>
-      <c r="J3" s="93"/>
-      <c r="K3" s="93"/>
-      <c r="L3" s="93"/>
-      <c r="M3" s="93"/>
-      <c r="N3" s="93"/>
-      <c r="O3" s="93"/>
+      <c r="C3" s="96"/>
+      <c r="D3" s="96"/>
+      <c r="E3" s="96"/>
+      <c r="F3" s="96"/>
+      <c r="G3" s="96"/>
+      <c r="H3" s="96"/>
+      <c r="I3" s="96"/>
+      <c r="J3" s="96"/>
+      <c r="K3" s="96"/>
+      <c r="L3" s="96"/>
+      <c r="M3" s="96"/>
+      <c r="N3" s="96"/>
+      <c r="O3" s="96"/>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>45</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D5" s="45" t="s">
         <v>50</v>
@@ -3446,10 +3443,10 @@
         <v>52</v>
       </c>
       <c r="J5" s="45" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K5" s="45" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.25">
@@ -3493,22 +3490,22 @@
   <sheetData>
     <row r="1" spans="2:5" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="92"/>
-      <c r="C2" s="92"/>
-      <c r="D2" s="92"/>
-      <c r="E2" s="92"/>
+      <c r="B2" s="95"/>
+      <c r="C2" s="95"/>
+      <c r="D2" s="95"/>
+      <c r="E2" s="95"/>
     </row>
     <row r="3" spans="2:5" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="93" t="s">
-        <v>131</v>
-      </c>
-      <c r="C3" s="93"/>
-      <c r="D3" s="93"/>
-      <c r="E3" s="93"/>
+      <c r="B3" s="96" t="s">
+        <v>130</v>
+      </c>
+      <c r="C3" s="96"/>
+      <c r="D3" s="96"/>
+      <c r="E3" s="96"/>
     </row>
     <row r="4" spans="2:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="64"/>
@@ -3518,13 +3515,13 @@
         <v>45</v>
       </c>
       <c r="C5" s="44" t="s">
+        <v>131</v>
+      </c>
+      <c r="D5" s="61" t="s">
         <v>132</v>
       </c>
-      <c r="D5" s="61" t="s">
+      <c r="E5" s="61" t="s">
         <v>133</v>
-      </c>
-      <c r="E5" s="61" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="6" spans="2:5" customFormat="1" x14ac:dyDescent="0.25">
@@ -3566,47 +3563,47 @@
   <sheetData>
     <row r="1" spans="2:14" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="92"/>
-      <c r="C2" s="92"/>
-      <c r="D2" s="92"/>
-      <c r="E2" s="92"/>
-      <c r="F2" s="92"/>
-      <c r="G2" s="92"/>
-      <c r="H2" s="92"/>
-      <c r="I2" s="92"/>
-      <c r="J2" s="92"/>
-      <c r="K2" s="92"/>
-      <c r="L2" s="92"/>
-      <c r="M2" s="92"/>
-      <c r="N2" s="92"/>
+      <c r="B2" s="95"/>
+      <c r="C2" s="95"/>
+      <c r="D2" s="95"/>
+      <c r="E2" s="95"/>
+      <c r="F2" s="95"/>
+      <c r="G2" s="95"/>
+      <c r="H2" s="95"/>
+      <c r="I2" s="95"/>
+      <c r="J2" s="95"/>
+      <c r="K2" s="95"/>
+      <c r="L2" s="95"/>
+      <c r="M2" s="95"/>
+      <c r="N2" s="95"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="93" t="s">
+      <c r="B3" s="96" t="s">
         <v>69</v>
       </c>
-      <c r="C3" s="93"/>
-      <c r="D3" s="93"/>
-      <c r="E3" s="93"/>
-      <c r="F3" s="93"/>
-      <c r="G3" s="93"/>
-      <c r="H3" s="93"/>
-      <c r="I3" s="93"/>
-      <c r="J3" s="93"/>
-      <c r="K3" s="93"/>
-      <c r="L3" s="93"/>
-      <c r="M3" s="93"/>
-      <c r="N3" s="93"/>
+      <c r="C3" s="96"/>
+      <c r="D3" s="96"/>
+      <c r="E3" s="96"/>
+      <c r="F3" s="96"/>
+      <c r="G3" s="96"/>
+      <c r="H3" s="96"/>
+      <c r="I3" s="96"/>
+      <c r="J3" s="96"/>
+      <c r="K3" s="96"/>
+      <c r="L3" s="96"/>
+      <c r="M3" s="96"/>
+      <c r="N3" s="96"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>75</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>70</v>
@@ -3650,44 +3647,44 @@
   <sheetData>
     <row r="1" spans="2:14" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="92"/>
-      <c r="C2" s="92"/>
-      <c r="D2" s="92"/>
-      <c r="E2" s="92"/>
-      <c r="F2" s="92"/>
-      <c r="G2" s="92"/>
-      <c r="H2" s="92"/>
-      <c r="I2" s="92"/>
-      <c r="J2" s="92"/>
-      <c r="K2" s="92"/>
-      <c r="L2" s="92"/>
-      <c r="M2" s="92"/>
-      <c r="N2" s="92"/>
+      <c r="B2" s="95"/>
+      <c r="C2" s="95"/>
+      <c r="D2" s="95"/>
+      <c r="E2" s="95"/>
+      <c r="F2" s="95"/>
+      <c r="G2" s="95"/>
+      <c r="H2" s="95"/>
+      <c r="I2" s="95"/>
+      <c r="J2" s="95"/>
+      <c r="K2" s="95"/>
+      <c r="L2" s="95"/>
+      <c r="M2" s="95"/>
+      <c r="N2" s="95"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="93" t="s">
+      <c r="B3" s="96" t="s">
         <v>74</v>
       </c>
-      <c r="C3" s="93"/>
-      <c r="D3" s="93"/>
-      <c r="E3" s="93"/>
-      <c r="F3" s="93"/>
-      <c r="G3" s="93"/>
-      <c r="H3" s="93"/>
-      <c r="I3" s="93"/>
-      <c r="J3" s="93"/>
-      <c r="K3" s="93"/>
-      <c r="L3" s="93"/>
-      <c r="M3" s="93"/>
-      <c r="N3" s="93"/>
+      <c r="C3" s="96"/>
+      <c r="D3" s="96"/>
+      <c r="E3" s="96"/>
+      <c r="F3" s="96"/>
+      <c r="G3" s="96"/>
+      <c r="H3" s="96"/>
+      <c r="I3" s="96"/>
+      <c r="J3" s="96"/>
+      <c r="K3" s="96"/>
+      <c r="L3" s="96"/>
+      <c r="M3" s="96"/>
+      <c r="N3" s="96"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>86</v>
@@ -3748,44 +3745,44 @@
   <sheetData>
     <row r="1" spans="2:18" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="2:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="92"/>
-      <c r="C2" s="92"/>
-      <c r="D2" s="92"/>
-      <c r="E2" s="92"/>
-      <c r="F2" s="92"/>
-      <c r="G2" s="92"/>
-      <c r="H2" s="92"/>
-      <c r="I2" s="92"/>
-      <c r="J2" s="92"/>
-      <c r="K2" s="92"/>
-      <c r="L2" s="92"/>
-      <c r="M2" s="92"/>
-      <c r="N2" s="92"/>
-      <c r="O2" s="92"/>
-      <c r="P2" s="92"/>
+      <c r="B2" s="95"/>
+      <c r="C2" s="95"/>
+      <c r="D2" s="95"/>
+      <c r="E2" s="95"/>
+      <c r="F2" s="95"/>
+      <c r="G2" s="95"/>
+      <c r="H2" s="95"/>
+      <c r="I2" s="95"/>
+      <c r="J2" s="95"/>
+      <c r="K2" s="95"/>
+      <c r="L2" s="95"/>
+      <c r="M2" s="95"/>
+      <c r="N2" s="95"/>
+      <c r="O2" s="95"/>
+      <c r="P2" s="95"/>
     </row>
     <row r="3" spans="2:18" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="93" t="s">
+      <c r="B3" s="96" t="s">
         <v>63</v>
       </c>
-      <c r="C3" s="93"/>
-      <c r="D3" s="93"/>
-      <c r="E3" s="93"/>
-      <c r="F3" s="93"/>
-      <c r="G3" s="93"/>
-      <c r="H3" s="93"/>
-      <c r="I3" s="93"/>
-      <c r="J3" s="93"/>
-      <c r="K3" s="93"/>
-      <c r="L3" s="93"/>
-      <c r="M3" s="93"/>
-      <c r="N3" s="93"/>
-      <c r="O3" s="93"/>
-      <c r="P3" s="93"/>
+      <c r="C3" s="96"/>
+      <c r="D3" s="96"/>
+      <c r="E3" s="96"/>
+      <c r="F3" s="96"/>
+      <c r="G3" s="96"/>
+      <c r="H3" s="96"/>
+      <c r="I3" s="96"/>
+      <c r="J3" s="96"/>
+      <c r="K3" s="96"/>
+      <c r="L3" s="96"/>
+      <c r="M3" s="96"/>
+      <c r="N3" s="96"/>
+      <c r="O3" s="96"/>
+      <c r="P3" s="96"/>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
@@ -3822,10 +3819,10 @@
         <v>56</v>
       </c>
       <c r="M5" s="53" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="N5" s="53" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="O5" s="4" t="s">
         <v>57</v>
@@ -3895,40 +3892,40 @@
   <sheetData>
     <row r="1" spans="2:14" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="92"/>
-      <c r="C2" s="92"/>
-      <c r="D2" s="92"/>
-      <c r="E2" s="92"/>
-      <c r="F2" s="92"/>
-      <c r="G2" s="92"/>
-      <c r="H2" s="92"/>
-      <c r="I2" s="92"/>
-      <c r="J2" s="92"/>
-      <c r="K2" s="92"/>
-      <c r="L2" s="92"/>
-      <c r="M2" s="92"/>
-      <c r="N2" s="92"/>
+      <c r="B2" s="95"/>
+      <c r="C2" s="95"/>
+      <c r="D2" s="95"/>
+      <c r="E2" s="95"/>
+      <c r="F2" s="95"/>
+      <c r="G2" s="95"/>
+      <c r="H2" s="95"/>
+      <c r="I2" s="95"/>
+      <c r="J2" s="95"/>
+      <c r="K2" s="95"/>
+      <c r="L2" s="95"/>
+      <c r="M2" s="95"/>
+      <c r="N2" s="95"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="93" t="s">
+      <c r="B3" s="96" t="s">
         <v>64</v>
       </c>
-      <c r="C3" s="93"/>
-      <c r="D3" s="93"/>
-      <c r="E3" s="93"/>
-      <c r="F3" s="93"/>
-      <c r="G3" s="93"/>
-      <c r="H3" s="93"/>
-      <c r="I3" s="93"/>
-      <c r="J3" s="93"/>
-      <c r="K3" s="93"/>
-      <c r="L3" s="93"/>
-      <c r="M3" s="93"/>
-      <c r="N3" s="93"/>
+      <c r="C3" s="96"/>
+      <c r="D3" s="96"/>
+      <c r="E3" s="96"/>
+      <c r="F3" s="96"/>
+      <c r="G3" s="96"/>
+      <c r="H3" s="96"/>
+      <c r="I3" s="96"/>
+      <c r="J3" s="96"/>
+      <c r="K3" s="96"/>
+      <c r="L3" s="96"/>
+      <c r="M3" s="96"/>
+      <c r="N3" s="96"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="58" t="s">
@@ -4011,42 +4008,42 @@
   <sheetData>
     <row r="1" spans="2:14" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="92" t="s">
-        <v>97</v>
-      </c>
-      <c r="C2" s="92"/>
-      <c r="D2" s="92"/>
-      <c r="E2" s="92"/>
-      <c r="F2" s="92"/>
-      <c r="G2" s="92"/>
-      <c r="H2" s="92"/>
-      <c r="I2" s="92"/>
-      <c r="J2" s="92"/>
-      <c r="K2" s="92"/>
-      <c r="L2" s="92"/>
-      <c r="M2" s="92"/>
-      <c r="N2" s="92"/>
+      <c r="B2" s="95" t="s">
+        <v>96</v>
+      </c>
+      <c r="C2" s="95"/>
+      <c r="D2" s="95"/>
+      <c r="E2" s="95"/>
+      <c r="F2" s="95"/>
+      <c r="G2" s="95"/>
+      <c r="H2" s="95"/>
+      <c r="I2" s="95"/>
+      <c r="J2" s="95"/>
+      <c r="K2" s="95"/>
+      <c r="L2" s="95"/>
+      <c r="M2" s="95"/>
+      <c r="N2" s="95"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="93" t="s">
+      <c r="B3" s="96" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="93"/>
-      <c r="D3" s="93"/>
-      <c r="E3" s="93"/>
-      <c r="F3" s="93"/>
-      <c r="G3" s="93"/>
-      <c r="H3" s="93"/>
-      <c r="I3" s="93"/>
-      <c r="J3" s="93"/>
-      <c r="K3" s="93"/>
-      <c r="L3" s="93"/>
-      <c r="M3" s="93"/>
-      <c r="N3" s="93"/>
+      <c r="C3" s="96"/>
+      <c r="D3" s="96"/>
+      <c r="E3" s="96"/>
+      <c r="F3" s="96"/>
+      <c r="G3" s="96"/>
+      <c r="H3" s="96"/>
+      <c r="I3" s="96"/>
+      <c r="J3" s="96"/>
+      <c r="K3" s="96"/>
+      <c r="L3" s="96"/>
+      <c r="M3" s="96"/>
+      <c r="N3" s="96"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="44" t="s">
@@ -4101,74 +4098,74 @@
   <sheetData>
     <row r="1" spans="2:14" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="92"/>
-      <c r="C2" s="92"/>
-      <c r="D2" s="92"/>
-      <c r="E2" s="92"/>
-      <c r="F2" s="92"/>
-      <c r="G2" s="92"/>
-      <c r="H2" s="92"/>
-      <c r="I2" s="92"/>
-      <c r="J2" s="92"/>
-      <c r="K2" s="92"/>
-      <c r="L2" s="92"/>
-      <c r="M2" s="92"/>
-      <c r="N2" s="92"/>
+      <c r="B2" s="95"/>
+      <c r="C2" s="95"/>
+      <c r="D2" s="95"/>
+      <c r="E2" s="95"/>
+      <c r="F2" s="95"/>
+      <c r="G2" s="95"/>
+      <c r="H2" s="95"/>
+      <c r="I2" s="95"/>
+      <c r="J2" s="95"/>
+      <c r="K2" s="95"/>
+      <c r="L2" s="95"/>
+      <c r="M2" s="95"/>
+      <c r="N2" s="95"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="93" t="s">
-        <v>152</v>
-      </c>
-      <c r="C3" s="93"/>
-      <c r="D3" s="93"/>
-      <c r="E3" s="93"/>
-      <c r="F3" s="93"/>
-      <c r="G3" s="93"/>
-      <c r="H3" s="93"/>
-      <c r="I3" s="93"/>
-      <c r="J3" s="93"/>
-      <c r="K3" s="93"/>
-      <c r="L3" s="93"/>
-      <c r="M3" s="93"/>
-      <c r="N3" s="93"/>
+      <c r="B3" s="96" t="s">
+        <v>151</v>
+      </c>
+      <c r="C3" s="96"/>
+      <c r="D3" s="96"/>
+      <c r="E3" s="96"/>
+      <c r="F3" s="96"/>
+      <c r="G3" s="96"/>
+      <c r="H3" s="96"/>
+      <c r="I3" s="96"/>
+      <c r="J3" s="96"/>
+      <c r="K3" s="96"/>
+      <c r="L3" s="96"/>
+      <c r="M3" s="96"/>
+      <c r="N3" s="96"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="74" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="74" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D5" s="74" t="s">
+        <v>142</v>
+      </c>
+      <c r="E5" s="74" t="s">
         <v>143</v>
       </c>
-      <c r="E5" s="74" t="s">
+      <c r="F5" s="74" t="s">
         <v>144</v>
       </c>
-      <c r="F5" s="74" t="s">
+      <c r="G5" s="74" t="s">
         <v>145</v>
       </c>
-      <c r="G5" s="74" t="s">
+      <c r="H5" s="74" t="s">
         <v>146</v>
       </c>
-      <c r="H5" s="74" t="s">
+      <c r="I5" s="74" t="s">
         <v>147</v>
       </c>
-      <c r="I5" s="74" t="s">
+      <c r="J5" s="74" t="s">
         <v>148</v>
       </c>
-      <c r="J5" s="74" t="s">
+      <c r="K5" s="74" t="s">
         <v>149</v>
       </c>
-      <c r="K5" s="74" t="s">
+      <c r="L5" s="74" t="s">
         <v>150</v>
-      </c>
-      <c r="L5" s="74" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
@@ -4217,32 +4214,32 @@
   <sheetData>
     <row r="1" spans="2:10" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="92"/>
-      <c r="C2" s="92"/>
-      <c r="D2" s="92"/>
-      <c r="E2" s="92"/>
-      <c r="F2" s="92"/>
-      <c r="G2" s="92"/>
-      <c r="H2" s="92"/>
-      <c r="I2" s="92"/>
-      <c r="J2" s="92"/>
+      <c r="B2" s="95"/>
+      <c r="C2" s="95"/>
+      <c r="D2" s="95"/>
+      <c r="E2" s="95"/>
+      <c r="F2" s="95"/>
+      <c r="G2" s="95"/>
+      <c r="H2" s="95"/>
+      <c r="I2" s="95"/>
+      <c r="J2" s="95"/>
     </row>
     <row r="3" spans="2:10" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="93" t="s">
-        <v>155</v>
-      </c>
-      <c r="C3" s="93"/>
-      <c r="D3" s="93"/>
-      <c r="E3" s="93"/>
-      <c r="F3" s="93"/>
-      <c r="G3" s="93"/>
-      <c r="H3" s="93"/>
-      <c r="I3" s="93"/>
-      <c r="J3" s="93"/>
+      <c r="B3" s="96" t="s">
+        <v>154</v>
+      </c>
+      <c r="C3" s="96"/>
+      <c r="D3" s="96"/>
+      <c r="E3" s="96"/>
+      <c r="F3" s="96"/>
+      <c r="G3" s="96"/>
+      <c r="H3" s="96"/>
+      <c r="I3" s="96"/>
+      <c r="J3" s="96"/>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" s="74" t="s">
@@ -4252,22 +4249,22 @@
         <v>27</v>
       </c>
       <c r="D5" s="74" t="s">
+        <v>142</v>
+      </c>
+      <c r="E5" s="74" t="s">
         <v>143</v>
       </c>
-      <c r="E5" s="74" t="s">
+      <c r="F5" s="74" t="s">
         <v>144</v>
       </c>
-      <c r="F5" s="74" t="s">
+      <c r="G5" s="74" t="s">
         <v>145</v>
       </c>
-      <c r="G5" s="74" t="s">
-        <v>146</v>
-      </c>
       <c r="H5" s="74" t="s">
+        <v>152</v>
+      </c>
+      <c r="I5" s="74" t="s">
         <v>153</v>
-      </c>
-      <c r="I5" s="74" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
@@ -4294,8 +4291,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:T6"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4323,33 +4320,33 @@
   <sheetData>
     <row r="1" spans="2:20" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="2:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="117"/>
-      <c r="C2" s="117"/>
-      <c r="D2" s="117"/>
-      <c r="E2" s="117"/>
-      <c r="F2" s="117"/>
-      <c r="G2" s="117"/>
-      <c r="H2" s="117"/>
-      <c r="I2" s="117"/>
+      <c r="B2" s="98"/>
+      <c r="C2" s="98"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
+      <c r="F2" s="98"/>
+      <c r="G2" s="98"/>
+      <c r="H2" s="98"/>
+      <c r="I2" s="98"/>
       <c r="L2" s="84"/>
       <c r="M2" s="84"/>
       <c r="N2" s="84"/>
     </row>
     <row r="3" spans="2:20" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="93" t="s">
-        <v>156</v>
-      </c>
-      <c r="C3" s="93"/>
-      <c r="D3" s="93"/>
-      <c r="E3" s="93"/>
-      <c r="F3" s="93"/>
-      <c r="G3" s="93"/>
-      <c r="H3" s="93"/>
-      <c r="I3" s="93"/>
+      <c r="B3" s="96" t="s">
+        <v>155</v>
+      </c>
+      <c r="C3" s="96"/>
+      <c r="D3" s="96"/>
+      <c r="E3" s="96"/>
+      <c r="F3" s="96"/>
+      <c r="G3" s="96"/>
+      <c r="H3" s="96"/>
+      <c r="I3" s="96"/>
       <c r="L3" s="83"/>
       <c r="M3" s="83"/>
       <c r="N3" s="83"/>
@@ -4359,58 +4356,58 @@
         <v>2</v>
       </c>
       <c r="C5" s="79" t="s">
+        <v>156</v>
+      </c>
+      <c r="D5" s="79" t="s">
+        <v>142</v>
+      </c>
+      <c r="E5" s="79" t="s">
         <v>157</v>
       </c>
-      <c r="D5" s="79" t="s">
-        <v>143</v>
-      </c>
-      <c r="E5" s="79" t="s">
+      <c r="F5" s="79" t="s">
         <v>158</v>
       </c>
-      <c r="F5" s="79" t="s">
+      <c r="G5" s="79" t="s">
         <v>159</v>
       </c>
-      <c r="G5" s="79" t="s">
+      <c r="H5" s="79" t="s">
         <v>160</v>
       </c>
-      <c r="H5" s="79" t="s">
+      <c r="I5" s="79" t="s">
+        <v>164</v>
+      </c>
+      <c r="J5" s="79" t="s">
+        <v>165</v>
+      </c>
+      <c r="K5" s="79" t="s">
+        <v>166</v>
+      </c>
+      <c r="L5" s="79" t="s">
         <v>161</v>
       </c>
-      <c r="I5" s="79" t="s">
-        <v>165</v>
-      </c>
-      <c r="J5" s="79" t="s">
-        <v>166</v>
-      </c>
-      <c r="K5" s="79" t="s">
-        <v>167</v>
-      </c>
-      <c r="L5" s="79" t="s">
+      <c r="M5" s="79" t="s">
         <v>162</v>
       </c>
-      <c r="M5" s="79" t="s">
+      <c r="N5" s="79" t="s">
         <v>163</v>
       </c>
-      <c r="N5" s="79" t="s">
-        <v>164</v>
-      </c>
       <c r="O5" s="87" t="s">
+        <v>176</v>
+      </c>
+      <c r="P5" s="87" t="s">
         <v>177</v>
       </c>
-      <c r="P5" s="87" t="s">
+      <c r="Q5" s="87" t="s">
+        <v>181</v>
+      </c>
+      <c r="R5" s="87" t="s">
         <v>178</v>
       </c>
-      <c r="Q5" s="87" t="s">
-        <v>182</v>
-      </c>
-      <c r="R5" s="87" t="s">
+      <c r="S5" s="87" t="s">
         <v>179</v>
       </c>
-      <c r="S5" s="87" t="s">
+      <c r="T5" s="87" t="s">
         <v>180</v>
-      </c>
-      <c r="T5" s="87" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.25">
@@ -4421,23 +4418,23 @@
       <c r="F6" s="8"/>
       <c r="G6" s="6"/>
       <c r="H6" s="8"/>
-      <c r="I6" s="114"/>
-      <c r="J6" s="114"/>
+      <c r="I6" s="92"/>
+      <c r="J6" s="92"/>
       <c r="K6" s="82"/>
-      <c r="L6" s="114"/>
-      <c r="M6" s="115"/>
-      <c r="N6" s="114"/>
-      <c r="O6" s="115"/>
-      <c r="P6" s="116"/>
+      <c r="L6" s="92"/>
+      <c r="M6" s="93"/>
+      <c r="N6" s="92"/>
+      <c r="O6" s="93"/>
+      <c r="P6" s="94"/>
       <c r="Q6" s="78"/>
-      <c r="R6" s="115"/>
-      <c r="S6" s="115"/>
+      <c r="R6" s="93"/>
+      <c r="S6" s="93"/>
       <c r="T6" s="82"/>
     </row>
   </sheetData>
   <mergeCells count="2">
+    <mergeCell ref="B3:I3"/>
     <mergeCell ref="B2:I2"/>
-    <mergeCell ref="B3:I3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -4466,55 +4463,55 @@
   <sheetData>
     <row r="1" spans="2:9" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="2:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="92"/>
-      <c r="C2" s="92"/>
-      <c r="D2" s="92"/>
-      <c r="E2" s="92"/>
-      <c r="F2" s="92"/>
-      <c r="G2" s="92"/>
-      <c r="H2" s="92"/>
-      <c r="I2" s="92"/>
+      <c r="B2" s="95"/>
+      <c r="C2" s="95"/>
+      <c r="D2" s="95"/>
+      <c r="E2" s="95"/>
+      <c r="F2" s="95"/>
+      <c r="G2" s="95"/>
+      <c r="H2" s="95"/>
+      <c r="I2" s="95"/>
     </row>
     <row r="3" spans="2:9" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="93" t="s">
-        <v>192</v>
-      </c>
-      <c r="C3" s="93"/>
-      <c r="D3" s="93"/>
-      <c r="E3" s="93"/>
-      <c r="F3" s="93"/>
-      <c r="G3" s="93"/>
-      <c r="H3" s="93"/>
-      <c r="I3" s="93"/>
+      <c r="B3" s="96" t="s">
+        <v>191</v>
+      </c>
+      <c r="C3" s="96"/>
+      <c r="D3" s="96"/>
+      <c r="E3" s="96"/>
+      <c r="F3" s="96"/>
+      <c r="G3" s="96"/>
+      <c r="H3" s="96"/>
+      <c r="I3" s="96"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="89" t="s">
+        <v>183</v>
+      </c>
+      <c r="C5" s="89" t="s">
         <v>184</v>
       </c>
-      <c r="C5" s="89" t="s">
+      <c r="D5" s="89" t="s">
         <v>185</v>
       </c>
-      <c r="D5" s="89" t="s">
+      <c r="E5" s="89" t="s">
         <v>186</v>
       </c>
-      <c r="E5" s="89" t="s">
+      <c r="F5" s="89" t="s">
         <v>187</v>
       </c>
-      <c r="F5" s="89" t="s">
+      <c r="G5" s="89" t="s">
         <v>188</v>
       </c>
-      <c r="G5" s="89" t="s">
+      <c r="H5" s="89" t="s">
         <v>189</v>
       </c>
-      <c r="H5" s="89" t="s">
+      <c r="I5" s="89" t="s">
         <v>190</v>
-      </c>
-      <c r="I5" s="89" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
@@ -4561,34 +4558,34 @@
   <sheetData>
     <row r="1" spans="2:11" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="92"/>
-      <c r="C2" s="92"/>
-      <c r="D2" s="92"/>
-      <c r="E2" s="92"/>
-      <c r="F2" s="92"/>
-      <c r="G2" s="92"/>
-      <c r="H2" s="92"/>
-      <c r="I2" s="92"/>
-      <c r="J2" s="92"/>
-      <c r="K2" s="92"/>
+      <c r="B2" s="95"/>
+      <c r="C2" s="95"/>
+      <c r="D2" s="95"/>
+      <c r="E2" s="95"/>
+      <c r="F2" s="95"/>
+      <c r="G2" s="95"/>
+      <c r="H2" s="95"/>
+      <c r="I2" s="95"/>
+      <c r="J2" s="95"/>
+      <c r="K2" s="95"/>
     </row>
     <row r="3" spans="2:11" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="93" t="s">
-        <v>168</v>
-      </c>
-      <c r="C3" s="93"/>
-      <c r="D3" s="93"/>
-      <c r="E3" s="93"/>
-      <c r="F3" s="93"/>
-      <c r="G3" s="93"/>
-      <c r="H3" s="93"/>
-      <c r="I3" s="93"/>
-      <c r="J3" s="93"/>
-      <c r="K3" s="93"/>
+      <c r="B3" s="96" t="s">
+        <v>167</v>
+      </c>
+      <c r="C3" s="96"/>
+      <c r="D3" s="96"/>
+      <c r="E3" s="96"/>
+      <c r="F3" s="96"/>
+      <c r="G3" s="96"/>
+      <c r="H3" s="96"/>
+      <c r="I3" s="96"/>
+      <c r="J3" s="96"/>
+      <c r="K3" s="96"/>
     </row>
     <row r="4" spans="2:11" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B4" s="85"/>
@@ -4603,14 +4600,14 @@
       <c r="K4" s="85"/>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="H5" s="95" t="s">
-        <v>176</v>
-      </c>
-      <c r="I5" s="96"/>
-      <c r="J5" s="95" t="s">
+      <c r="H5" s="99" t="s">
         <v>175</v>
       </c>
-      <c r="K5" s="96"/>
+      <c r="I5" s="100"/>
+      <c r="J5" s="99" t="s">
+        <v>174</v>
+      </c>
+      <c r="K5" s="100"/>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" s="86" t="s">
@@ -4620,28 +4617,28 @@
         <v>25</v>
       </c>
       <c r="D6" s="86" t="s">
+        <v>168</v>
+      </c>
+      <c r="E6" s="86" t="s">
         <v>169</v>
       </c>
-      <c r="E6" s="86" t="s">
+      <c r="F6" s="86" t="s">
+        <v>115</v>
+      </c>
+      <c r="G6" s="86" t="s">
+        <v>115</v>
+      </c>
+      <c r="H6" s="86" t="s">
         <v>170</v>
       </c>
-      <c r="F6" s="86" t="s">
-        <v>116</v>
-      </c>
-      <c r="G6" s="86" t="s">
-        <v>116</v>
-      </c>
-      <c r="H6" s="86" t="s">
+      <c r="I6" s="86" t="s">
         <v>171</v>
       </c>
-      <c r="I6" s="86" t="s">
+      <c r="J6" s="86" t="s">
         <v>172</v>
       </c>
-      <c r="J6" s="86" t="s">
+      <c r="K6" s="86" t="s">
         <v>173</v>
-      </c>
-      <c r="K6" s="86" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
@@ -4687,42 +4684,42 @@
   <sheetData>
     <row r="1" spans="2:26" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="Z1" s="38"/>
     </row>
     <row r="2" spans="2:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="92"/>
-      <c r="C2" s="92"/>
-      <c r="D2" s="92"/>
-      <c r="E2" s="92"/>
-      <c r="F2" s="92"/>
-      <c r="G2" s="92"/>
-      <c r="H2" s="92"/>
-      <c r="I2" s="92"/>
-      <c r="J2" s="92"/>
-      <c r="K2" s="92"/>
-      <c r="L2" s="92"/>
-      <c r="M2" s="92"/>
-      <c r="N2" s="92"/>
+      <c r="B2" s="95"/>
+      <c r="C2" s="95"/>
+      <c r="D2" s="95"/>
+      <c r="E2" s="95"/>
+      <c r="F2" s="95"/>
+      <c r="G2" s="95"/>
+      <c r="H2" s="95"/>
+      <c r="I2" s="95"/>
+      <c r="J2" s="95"/>
+      <c r="K2" s="95"/>
+      <c r="L2" s="95"/>
+      <c r="M2" s="95"/>
+      <c r="N2" s="95"/>
       <c r="Z2"/>
     </row>
     <row r="3" spans="2:26" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="93" t="s">
+      <c r="B3" s="96" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="93"/>
-      <c r="D3" s="93"/>
-      <c r="E3" s="93"/>
-      <c r="F3" s="93"/>
-      <c r="G3" s="93"/>
-      <c r="H3" s="93"/>
-      <c r="I3" s="93"/>
-      <c r="J3" s="93"/>
-      <c r="K3" s="93"/>
-      <c r="L3" s="93"/>
-      <c r="M3" s="93"/>
-      <c r="N3" s="93"/>
+      <c r="C3" s="96"/>
+      <c r="D3" s="96"/>
+      <c r="E3" s="96"/>
+      <c r="F3" s="96"/>
+      <c r="G3" s="96"/>
+      <c r="H3" s="96"/>
+      <c r="I3" s="96"/>
+      <c r="J3" s="96"/>
+      <c r="K3" s="96"/>
+      <c r="L3" s="96"/>
+      <c r="M3" s="96"/>
+      <c r="N3" s="96"/>
       <c r="Z3"/>
     </row>
     <row r="5" spans="2:26" x14ac:dyDescent="0.25">
@@ -4821,42 +4818,42 @@
   <sheetData>
     <row r="1" spans="2:26" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="Z1" s="38"/>
     </row>
     <row r="2" spans="2:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="92"/>
-      <c r="C2" s="92"/>
-      <c r="D2" s="92"/>
-      <c r="E2" s="92"/>
-      <c r="F2" s="92"/>
-      <c r="G2" s="92"/>
-      <c r="H2" s="92"/>
-      <c r="I2" s="92"/>
-      <c r="J2" s="92"/>
-      <c r="K2" s="92"/>
-      <c r="L2" s="92"/>
-      <c r="M2" s="92"/>
-      <c r="N2" s="92"/>
+      <c r="B2" s="95"/>
+      <c r="C2" s="95"/>
+      <c r="D2" s="95"/>
+      <c r="E2" s="95"/>
+      <c r="F2" s="95"/>
+      <c r="G2" s="95"/>
+      <c r="H2" s="95"/>
+      <c r="I2" s="95"/>
+      <c r="J2" s="95"/>
+      <c r="K2" s="95"/>
+      <c r="L2" s="95"/>
+      <c r="M2" s="95"/>
+      <c r="N2" s="95"/>
       <c r="Z2"/>
     </row>
     <row r="3" spans="2:26" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="93" t="s">
+      <c r="B3" s="96" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="93"/>
-      <c r="D3" s="93"/>
-      <c r="E3" s="93"/>
-      <c r="F3" s="93"/>
-      <c r="G3" s="93"/>
-      <c r="H3" s="93"/>
-      <c r="I3" s="93"/>
-      <c r="J3" s="93"/>
-      <c r="K3" s="93"/>
-      <c r="L3" s="93"/>
-      <c r="M3" s="93"/>
-      <c r="N3" s="93"/>
+      <c r="C3" s="96"/>
+      <c r="D3" s="96"/>
+      <c r="E3" s="96"/>
+      <c r="F3" s="96"/>
+      <c r="G3" s="96"/>
+      <c r="H3" s="96"/>
+      <c r="I3" s="96"/>
+      <c r="J3" s="96"/>
+      <c r="K3" s="96"/>
+      <c r="L3" s="96"/>
+      <c r="M3" s="96"/>
+      <c r="N3" s="96"/>
       <c r="Z3"/>
     </row>
     <row r="5" spans="2:26" x14ac:dyDescent="0.25">
@@ -4873,11 +4870,11 @@
     </row>
     <row r="6" spans="2:26" x14ac:dyDescent="0.25">
       <c r="C6" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="D6" s="97"/>
-      <c r="E6" s="98"/>
-      <c r="F6" s="99"/>
+        <v>108</v>
+      </c>
+      <c r="D6" s="101"/>
+      <c r="E6" s="102"/>
+      <c r="F6" s="103"/>
       <c r="G6" s="50"/>
       <c r="H6" s="50"/>
     </row>
@@ -4950,42 +4947,42 @@
   <sheetData>
     <row r="1" spans="2:26" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="Z1" s="38"/>
     </row>
     <row r="2" spans="2:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="92"/>
-      <c r="C2" s="92"/>
-      <c r="D2" s="92"/>
-      <c r="E2" s="92"/>
-      <c r="F2" s="92"/>
-      <c r="G2" s="92"/>
-      <c r="H2" s="92"/>
-      <c r="I2" s="92"/>
-      <c r="J2" s="92"/>
-      <c r="K2" s="92"/>
-      <c r="L2" s="92"/>
-      <c r="M2" s="92"/>
-      <c r="N2" s="92"/>
+      <c r="B2" s="95"/>
+      <c r="C2" s="95"/>
+      <c r="D2" s="95"/>
+      <c r="E2" s="95"/>
+      <c r="F2" s="95"/>
+      <c r="G2" s="95"/>
+      <c r="H2" s="95"/>
+      <c r="I2" s="95"/>
+      <c r="J2" s="95"/>
+      <c r="K2" s="95"/>
+      <c r="L2" s="95"/>
+      <c r="M2" s="95"/>
+      <c r="N2" s="95"/>
       <c r="Z2"/>
     </row>
     <row r="3" spans="2:26" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="93" t="s">
-        <v>93</v>
-      </c>
-      <c r="C3" s="93"/>
-      <c r="D3" s="93"/>
-      <c r="E3" s="93"/>
-      <c r="F3" s="93"/>
-      <c r="G3" s="93"/>
-      <c r="H3" s="93"/>
-      <c r="I3" s="93"/>
-      <c r="J3" s="93"/>
-      <c r="K3" s="93"/>
-      <c r="L3" s="93"/>
-      <c r="M3" s="93"/>
-      <c r="N3" s="93"/>
+      <c r="B3" s="96" t="s">
+        <v>92</v>
+      </c>
+      <c r="C3" s="96"/>
+      <c r="D3" s="96"/>
+      <c r="E3" s="96"/>
+      <c r="F3" s="96"/>
+      <c r="G3" s="96"/>
+      <c r="H3" s="96"/>
+      <c r="I3" s="96"/>
+      <c r="J3" s="96"/>
+      <c r="K3" s="96"/>
+      <c r="L3" s="96"/>
+      <c r="M3" s="96"/>
+      <c r="N3" s="96"/>
       <c r="Z3"/>
     </row>
     <row r="5" spans="2:26" x14ac:dyDescent="0.25">
@@ -5004,7 +5001,7 @@
       </c>
       <c r="D6" s="12"/>
       <c r="E6" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F6" s="12"/>
     </row>
@@ -5073,42 +5070,42 @@
   <sheetData>
     <row r="1" spans="2:26" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="Z1" s="38"/>
     </row>
     <row r="2" spans="2:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="92"/>
-      <c r="C2" s="92"/>
-      <c r="D2" s="92"/>
-      <c r="E2" s="92"/>
-      <c r="F2" s="92"/>
-      <c r="G2" s="92"/>
-      <c r="H2" s="92"/>
-      <c r="I2" s="92"/>
-      <c r="J2" s="92"/>
-      <c r="K2" s="92"/>
-      <c r="L2" s="92"/>
-      <c r="M2" s="92"/>
-      <c r="N2" s="92"/>
+      <c r="B2" s="95"/>
+      <c r="C2" s="95"/>
+      <c r="D2" s="95"/>
+      <c r="E2" s="95"/>
+      <c r="F2" s="95"/>
+      <c r="G2" s="95"/>
+      <c r="H2" s="95"/>
+      <c r="I2" s="95"/>
+      <c r="J2" s="95"/>
+      <c r="K2" s="95"/>
+      <c r="L2" s="95"/>
+      <c r="M2" s="95"/>
+      <c r="N2" s="95"/>
       <c r="Z2"/>
     </row>
     <row r="3" spans="2:26" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="93" t="s">
+      <c r="B3" s="96" t="s">
         <v>72</v>
       </c>
-      <c r="C3" s="93"/>
-      <c r="D3" s="93"/>
-      <c r="E3" s="93"/>
-      <c r="F3" s="93"/>
-      <c r="G3" s="93"/>
-      <c r="H3" s="93"/>
-      <c r="I3" s="93"/>
-      <c r="J3" s="93"/>
-      <c r="K3" s="93"/>
-      <c r="L3" s="93"/>
-      <c r="M3" s="93"/>
-      <c r="N3" s="93"/>
+      <c r="C3" s="96"/>
+      <c r="D3" s="96"/>
+      <c r="E3" s="96"/>
+      <c r="F3" s="96"/>
+      <c r="G3" s="96"/>
+      <c r="H3" s="96"/>
+      <c r="I3" s="96"/>
+      <c r="J3" s="96"/>
+      <c r="K3" s="96"/>
+      <c r="L3" s="96"/>
+      <c r="M3" s="96"/>
+      <c r="N3" s="96"/>
       <c r="Z3"/>
     </row>
     <row r="5" spans="2:26" x14ac:dyDescent="0.25">
@@ -5217,79 +5214,79 @@
   <sheetData>
     <row r="1" spans="2:17" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="92"/>
-      <c r="C2" s="92"/>
-      <c r="D2" s="92"/>
-      <c r="E2" s="92"/>
-      <c r="F2" s="92"/>
-      <c r="G2" s="92"/>
-      <c r="H2" s="92"/>
-      <c r="I2" s="92"/>
-      <c r="J2" s="92"/>
-      <c r="K2" s="92"/>
-      <c r="L2" s="92"/>
+      <c r="B2" s="95"/>
+      <c r="C2" s="95"/>
+      <c r="D2" s="95"/>
+      <c r="E2" s="95"/>
+      <c r="F2" s="95"/>
+      <c r="G2" s="95"/>
+      <c r="H2" s="95"/>
+      <c r="I2" s="95"/>
+      <c r="J2" s="95"/>
+      <c r="K2" s="95"/>
+      <c r="L2" s="95"/>
     </row>
     <row r="3" spans="2:17" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="93" t="s">
-        <v>108</v>
-      </c>
-      <c r="C3" s="93"/>
-      <c r="D3" s="93"/>
-      <c r="E3" s="93"/>
-      <c r="F3" s="93"/>
-      <c r="G3" s="93"/>
-      <c r="H3" s="93"/>
-      <c r="I3" s="93"/>
-      <c r="J3" s="93"/>
-      <c r="K3" s="93"/>
-      <c r="L3" s="93"/>
+      <c r="B3" s="96" t="s">
+        <v>107</v>
+      </c>
+      <c r="C3" s="96"/>
+      <c r="D3" s="96"/>
+      <c r="E3" s="96"/>
+      <c r="F3" s="96"/>
+      <c r="G3" s="96"/>
+      <c r="H3" s="96"/>
+      <c r="I3" s="96"/>
+      <c r="J3" s="96"/>
+      <c r="K3" s="96"/>
+      <c r="L3" s="96"/>
     </row>
     <row r="5" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D5" s="100" t="s">
-        <v>123</v>
-      </c>
-      <c r="E5" s="100"/>
+      <c r="D5" s="104" t="s">
+        <v>122</v>
+      </c>
+      <c r="E5" s="104"/>
       <c r="F5" s="73"/>
       <c r="G5" s="73"/>
       <c r="H5" s="73"/>
       <c r="I5" s="73"/>
-      <c r="J5" s="100" t="s">
+      <c r="J5" s="104" t="s">
         <v>42</v>
       </c>
-      <c r="K5" s="100"/>
-      <c r="L5" s="100"/>
-      <c r="M5" s="100" t="s">
-        <v>130</v>
-      </c>
-      <c r="N5" s="100"/>
-      <c r="O5" s="100"/>
-      <c r="P5" s="94" t="s">
-        <v>109</v>
-      </c>
-      <c r="Q5" s="94"/>
+      <c r="K5" s="104"/>
+      <c r="L5" s="104"/>
+      <c r="M5" s="104" t="s">
+        <v>129</v>
+      </c>
+      <c r="N5" s="104"/>
+      <c r="O5" s="104"/>
+      <c r="P5" s="97" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q5" s="97"/>
     </row>
     <row r="6" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="70" t="s">
         <v>32</v>
       </c>
       <c r="C6" s="71" t="s">
+        <v>137</v>
+      </c>
+      <c r="D6" s="63" t="s">
+        <v>123</v>
+      </c>
+      <c r="E6" s="63" t="s">
+        <v>124</v>
+      </c>
+      <c r="F6" s="71" t="s">
         <v>138</v>
       </c>
-      <c r="D6" s="63" t="s">
-        <v>124</v>
-      </c>
-      <c r="E6" s="63" t="s">
-        <v>125</v>
-      </c>
-      <c r="F6" s="71" t="s">
+      <c r="G6" s="71" t="s">
         <v>139</v>
-      </c>
-      <c r="G6" s="71" t="s">
-        <v>140</v>
       </c>
       <c r="H6" s="72" t="s">
         <v>53</v>
@@ -5298,28 +5295,28 @@
         <v>70</v>
       </c>
       <c r="J6" s="63" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K6" s="63" t="s">
+        <v>127</v>
+      </c>
+      <c r="L6" s="69" t="s">
+        <v>115</v>
+      </c>
+      <c r="M6" s="63" t="s">
         <v>128</v>
       </c>
-      <c r="L6" s="69" t="s">
-        <v>116</v>
-      </c>
-      <c r="M6" s="63" t="s">
-        <v>129</v>
-      </c>
       <c r="N6" s="63" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="O6" s="69" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="P6" s="69" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="Q6" s="69" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.25">
@@ -5376,40 +5373,40 @@
   <sheetData>
     <row r="1" spans="2:14" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="92"/>
-      <c r="C2" s="92"/>
-      <c r="D2" s="92"/>
-      <c r="E2" s="92"/>
-      <c r="F2" s="92"/>
-      <c r="G2" s="92"/>
-      <c r="H2" s="92"/>
-      <c r="I2" s="92"/>
-      <c r="J2" s="92"/>
-      <c r="K2" s="92"/>
-      <c r="L2" s="92"/>
-      <c r="M2" s="92"/>
-      <c r="N2" s="92"/>
+      <c r="B2" s="95"/>
+      <c r="C2" s="95"/>
+      <c r="D2" s="95"/>
+      <c r="E2" s="95"/>
+      <c r="F2" s="95"/>
+      <c r="G2" s="95"/>
+      <c r="H2" s="95"/>
+      <c r="I2" s="95"/>
+      <c r="J2" s="95"/>
+      <c r="K2" s="95"/>
+      <c r="L2" s="95"/>
+      <c r="M2" s="95"/>
+      <c r="N2" s="95"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="93" t="s">
+      <c r="B3" s="96" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="93"/>
-      <c r="D3" s="93"/>
-      <c r="E3" s="93"/>
-      <c r="F3" s="93"/>
-      <c r="G3" s="93"/>
-      <c r="H3" s="93"/>
-      <c r="I3" s="93"/>
-      <c r="J3" s="93"/>
-      <c r="K3" s="93"/>
-      <c r="L3" s="93"/>
-      <c r="M3" s="93"/>
-      <c r="N3" s="93"/>
+      <c r="C3" s="96"/>
+      <c r="D3" s="96"/>
+      <c r="E3" s="96"/>
+      <c r="F3" s="96"/>
+      <c r="G3" s="96"/>
+      <c r="H3" s="96"/>
+      <c r="I3" s="96"/>
+      <c r="J3" s="96"/>
+      <c r="K3" s="96"/>
+      <c r="L3" s="96"/>
+      <c r="M3" s="96"/>
+      <c r="N3" s="96"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="44" t="s">
@@ -5487,114 +5484,114 @@
   <sheetData>
     <row r="1" spans="2:25" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="2:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="92"/>
-      <c r="C2" s="92"/>
-      <c r="D2" s="92"/>
-      <c r="E2" s="92"/>
-      <c r="F2" s="92"/>
-      <c r="G2" s="92"/>
-      <c r="H2" s="92"/>
-      <c r="I2" s="92"/>
-      <c r="J2" s="92"/>
-      <c r="K2" s="92"/>
-      <c r="L2" s="92"/>
-      <c r="M2" s="92"/>
-      <c r="N2" s="92"/>
-      <c r="O2" s="92"/>
-      <c r="P2" s="92"/>
+      <c r="B2" s="95"/>
+      <c r="C2" s="95"/>
+      <c r="D2" s="95"/>
+      <c r="E2" s="95"/>
+      <c r="F2" s="95"/>
+      <c r="G2" s="95"/>
+      <c r="H2" s="95"/>
+      <c r="I2" s="95"/>
+      <c r="J2" s="95"/>
+      <c r="K2" s="95"/>
+      <c r="L2" s="95"/>
+      <c r="M2" s="95"/>
+      <c r="N2" s="95"/>
+      <c r="O2" s="95"/>
+      <c r="P2" s="95"/>
       <c r="Q2" s="56"/>
       <c r="R2" s="56"/>
     </row>
     <row r="3" spans="2:25" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="93" t="s">
-        <v>111</v>
-      </c>
-      <c r="C3" s="93"/>
-      <c r="D3" s="93"/>
-      <c r="E3" s="93"/>
-      <c r="F3" s="93"/>
-      <c r="G3" s="93"/>
-      <c r="H3" s="93"/>
-      <c r="I3" s="93"/>
-      <c r="J3" s="93"/>
-      <c r="K3" s="93"/>
-      <c r="L3" s="93"/>
-      <c r="M3" s="93"/>
-      <c r="N3" s="93"/>
-      <c r="O3" s="93"/>
-      <c r="P3" s="93"/>
+      <c r="B3" s="96" t="s">
+        <v>110</v>
+      </c>
+      <c r="C3" s="96"/>
+      <c r="D3" s="96"/>
+      <c r="E3" s="96"/>
+      <c r="F3" s="96"/>
+      <c r="G3" s="96"/>
+      <c r="H3" s="96"/>
+      <c r="I3" s="96"/>
+      <c r="J3" s="96"/>
+      <c r="K3" s="96"/>
+      <c r="L3" s="96"/>
+      <c r="M3" s="96"/>
+      <c r="N3" s="96"/>
+      <c r="O3" s="96"/>
+      <c r="P3" s="96"/>
       <c r="Q3" s="57"/>
       <c r="R3" s="57"/>
     </row>
     <row r="5" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B5" s="105" t="s">
+      <c r="B5" s="107" t="s">
+        <v>111</v>
+      </c>
+      <c r="C5" s="108"/>
+      <c r="D5" s="108"/>
+      <c r="E5" s="108"/>
+      <c r="F5" s="108"/>
+      <c r="G5" s="108"/>
+      <c r="H5" s="108"/>
+      <c r="I5" s="108"/>
+      <c r="J5" s="108"/>
+      <c r="K5" s="108"/>
+      <c r="L5" s="109"/>
+      <c r="M5" s="107" t="s">
         <v>112</v>
       </c>
-      <c r="C5" s="106"/>
-      <c r="D5" s="106"/>
-      <c r="E5" s="106"/>
-      <c r="F5" s="106"/>
-      <c r="G5" s="106"/>
-      <c r="H5" s="106"/>
-      <c r="I5" s="106"/>
-      <c r="J5" s="106"/>
-      <c r="K5" s="106"/>
-      <c r="L5" s="107"/>
-      <c r="M5" s="105" t="s">
-        <v>113</v>
-      </c>
-      <c r="N5" s="106"/>
-      <c r="O5" s="106"/>
-      <c r="P5" s="106"/>
-      <c r="Q5" s="106"/>
-      <c r="R5" s="106"/>
-      <c r="S5" s="106"/>
-      <c r="T5" s="106"/>
-      <c r="U5" s="106"/>
-      <c r="V5" s="106"/>
-      <c r="W5" s="106"/>
-      <c r="X5" s="106"/>
-      <c r="Y5" s="107"/>
+      <c r="N5" s="108"/>
+      <c r="O5" s="108"/>
+      <c r="P5" s="108"/>
+      <c r="Q5" s="108"/>
+      <c r="R5" s="108"/>
+      <c r="S5" s="108"/>
+      <c r="T5" s="108"/>
+      <c r="U5" s="108"/>
+      <c r="V5" s="108"/>
+      <c r="W5" s="108"/>
+      <c r="X5" s="108"/>
+      <c r="Y5" s="109"/>
     </row>
     <row r="6" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B6" s="104"/>
-      <c r="C6" s="104"/>
-      <c r="D6" s="104"/>
-      <c r="E6" s="104"/>
-      <c r="F6" s="111" t="s">
+      <c r="B6" s="117"/>
+      <c r="C6" s="117"/>
+      <c r="D6" s="117"/>
+      <c r="E6" s="117"/>
+      <c r="F6" s="113" t="s">
         <v>27</v>
       </c>
-      <c r="G6" s="112"/>
-      <c r="H6" s="112"/>
-      <c r="I6" s="113"/>
-      <c r="J6" s="105" t="s">
+      <c r="G6" s="114"/>
+      <c r="H6" s="114"/>
+      <c r="I6" s="115"/>
+      <c r="J6" s="107" t="s">
         <v>30</v>
       </c>
-      <c r="K6" s="106"/>
-      <c r="L6" s="107"/>
+      <c r="K6" s="108"/>
+      <c r="L6" s="109"/>
       <c r="M6" s="88"/>
-      <c r="N6" s="101" t="s">
+      <c r="N6" s="105" t="s">
         <v>42</v>
       </c>
-      <c r="O6" s="102"/>
-      <c r="P6" s="101" t="s">
-        <v>106</v>
-      </c>
-      <c r="Q6" s="103"/>
-      <c r="R6" s="102"/>
+      <c r="O6" s="106"/>
+      <c r="P6" s="105" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q6" s="116"/>
+      <c r="R6" s="106"/>
       <c r="S6" s="88"/>
-      <c r="T6" s="101" t="s">
-        <v>123</v>
-      </c>
-      <c r="U6" s="102"/>
-      <c r="V6" s="108"/>
-      <c r="W6" s="109"/>
-      <c r="X6" s="109"/>
-      <c r="Y6" s="110"/>
+      <c r="T6" s="105" t="s">
+        <v>122</v>
+      </c>
+      <c r="U6" s="106"/>
+      <c r="V6" s="110"/>
+      <c r="W6" s="111"/>
+      <c r="X6" s="111"/>
+      <c r="Y6" s="112"/>
     </row>
     <row r="7" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B7" s="75" t="s">
@@ -5610,52 +5607,52 @@
         <v>29</v>
       </c>
       <c r="F7" s="77" t="s">
+        <v>116</v>
+      </c>
+      <c r="G7" s="77" t="s">
+        <v>120</v>
+      </c>
+      <c r="H7" s="77" t="s">
+        <v>121</v>
+      </c>
+      <c r="I7" s="77" t="s">
         <v>117</v>
       </c>
-      <c r="G7" s="77" t="s">
-        <v>121</v>
-      </c>
-      <c r="H7" s="77" t="s">
-        <v>122</v>
-      </c>
-      <c r="I7" s="77" t="s">
-        <v>118</v>
-      </c>
       <c r="J7" s="77" t="s">
+        <v>113</v>
+      </c>
+      <c r="K7" s="77" t="s">
         <v>114</v>
       </c>
-      <c r="K7" s="77" t="s">
+      <c r="L7" s="77" t="s">
         <v>115</v>
-      </c>
-      <c r="L7" s="77" t="s">
-        <v>116</v>
       </c>
       <c r="M7" s="76" t="s">
         <v>53</v>
       </c>
       <c r="N7" s="77" t="s">
+        <v>118</v>
+      </c>
+      <c r="O7" s="77" t="s">
         <v>119</v>
       </c>
-      <c r="O7" s="77" t="s">
-        <v>120</v>
-      </c>
       <c r="P7" s="77" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q7" s="77" t="s">
         <v>114</v>
       </c>
-      <c r="Q7" s="77" t="s">
+      <c r="R7" s="77" t="s">
         <v>115</v>
       </c>
-      <c r="R7" s="77" t="s">
-        <v>116</v>
-      </c>
       <c r="S7" s="75" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="T7" s="77" t="s">
+        <v>123</v>
+      </c>
+      <c r="U7" s="77" t="s">
         <v>124</v>
-      </c>
-      <c r="U7" s="77" t="s">
-        <v>125</v>
       </c>
       <c r="V7" s="76" t="s">
         <v>70</v>
@@ -5664,10 +5661,10 @@
         <v>32</v>
       </c>
       <c r="X7" s="75" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="Y7" s="75" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="8" spans="2:25" x14ac:dyDescent="0.25">
@@ -5698,6 +5695,10 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="T6:U6"/>
+    <mergeCell ref="M5:Y5"/>
+    <mergeCell ref="V6:Y6"/>
     <mergeCell ref="B2:P2"/>
     <mergeCell ref="B3:P3"/>
     <mergeCell ref="B5:L5"/>
@@ -5705,10 +5706,6 @@
     <mergeCell ref="F6:I6"/>
     <mergeCell ref="N6:O6"/>
     <mergeCell ref="P6:R6"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="T6:U6"/>
-    <mergeCell ref="M5:Y5"/>
-    <mergeCell ref="V6:Y6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -5825,44 +5822,44 @@
   <sheetData>
     <row r="1" spans="2:16" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="92"/>
-      <c r="C2" s="92"/>
-      <c r="D2" s="92"/>
-      <c r="E2" s="92"/>
-      <c r="F2" s="92"/>
-      <c r="G2" s="92"/>
-      <c r="H2" s="92"/>
-      <c r="I2" s="92"/>
-      <c r="J2" s="92"/>
-      <c r="K2" s="92"/>
-      <c r="L2" s="92"/>
-      <c r="M2" s="92"/>
-      <c r="N2" s="92"/>
-      <c r="O2" s="92"/>
-      <c r="P2" s="92"/>
+      <c r="B2" s="95"/>
+      <c r="C2" s="95"/>
+      <c r="D2" s="95"/>
+      <c r="E2" s="95"/>
+      <c r="F2" s="95"/>
+      <c r="G2" s="95"/>
+      <c r="H2" s="95"/>
+      <c r="I2" s="95"/>
+      <c r="J2" s="95"/>
+      <c r="K2" s="95"/>
+      <c r="L2" s="95"/>
+      <c r="M2" s="95"/>
+      <c r="N2" s="95"/>
+      <c r="O2" s="95"/>
+      <c r="P2" s="95"/>
     </row>
     <row r="3" spans="2:16" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="93" t="s">
+      <c r="B3" s="96" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="93"/>
-      <c r="D3" s="93"/>
-      <c r="E3" s="93"/>
-      <c r="F3" s="93"/>
-      <c r="G3" s="93"/>
-      <c r="H3" s="93"/>
-      <c r="I3" s="93"/>
-      <c r="J3" s="93"/>
-      <c r="K3" s="93"/>
-      <c r="L3" s="93"/>
-      <c r="M3" s="93"/>
-      <c r="N3" s="93"/>
-      <c r="O3" s="93"/>
-      <c r="P3" s="93"/>
+      <c r="C3" s="96"/>
+      <c r="D3" s="96"/>
+      <c r="E3" s="96"/>
+      <c r="F3" s="96"/>
+      <c r="G3" s="96"/>
+      <c r="H3" s="96"/>
+      <c r="I3" s="96"/>
+      <c r="J3" s="96"/>
+      <c r="K3" s="96"/>
+      <c r="L3" s="96"/>
+      <c r="M3" s="96"/>
+      <c r="N3" s="96"/>
+      <c r="O3" s="96"/>
+      <c r="P3" s="96"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="44" t="s">
@@ -5937,44 +5934,44 @@
   <sheetData>
     <row r="1" spans="2:16" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="92"/>
-      <c r="C2" s="92"/>
-      <c r="D2" s="92"/>
-      <c r="E2" s="92"/>
-      <c r="F2" s="92"/>
-      <c r="G2" s="92"/>
-      <c r="H2" s="92"/>
-      <c r="I2" s="92"/>
-      <c r="J2" s="92"/>
-      <c r="K2" s="92"/>
-      <c r="L2" s="92"/>
-      <c r="M2" s="92"/>
-      <c r="N2" s="92"/>
-      <c r="O2" s="92"/>
-      <c r="P2" s="92"/>
+      <c r="B2" s="95"/>
+      <c r="C2" s="95"/>
+      <c r="D2" s="95"/>
+      <c r="E2" s="95"/>
+      <c r="F2" s="95"/>
+      <c r="G2" s="95"/>
+      <c r="H2" s="95"/>
+      <c r="I2" s="95"/>
+      <c r="J2" s="95"/>
+      <c r="K2" s="95"/>
+      <c r="L2" s="95"/>
+      <c r="M2" s="95"/>
+      <c r="N2" s="95"/>
+      <c r="O2" s="95"/>
+      <c r="P2" s="95"/>
     </row>
     <row r="3" spans="2:16" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="93" t="s">
+      <c r="B3" s="96" t="s">
         <v>68</v>
       </c>
-      <c r="C3" s="93"/>
-      <c r="D3" s="93"/>
-      <c r="E3" s="93"/>
-      <c r="F3" s="93"/>
-      <c r="G3" s="93"/>
-      <c r="H3" s="93"/>
-      <c r="I3" s="93"/>
-      <c r="J3" s="93"/>
-      <c r="K3" s="93"/>
-      <c r="L3" s="93"/>
-      <c r="M3" s="93"/>
-      <c r="N3" s="93"/>
-      <c r="O3" s="93"/>
-      <c r="P3" s="93"/>
+      <c r="C3" s="96"/>
+      <c r="D3" s="96"/>
+      <c r="E3" s="96"/>
+      <c r="F3" s="96"/>
+      <c r="G3" s="96"/>
+      <c r="H3" s="96"/>
+      <c r="I3" s="96"/>
+      <c r="J3" s="96"/>
+      <c r="K3" s="96"/>
+      <c r="L3" s="96"/>
+      <c r="M3" s="96"/>
+      <c r="N3" s="96"/>
+      <c r="O3" s="96"/>
+      <c r="P3" s="96"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
@@ -6019,44 +6016,44 @@
   <sheetData>
     <row r="1" spans="2:16" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="92"/>
-      <c r="C2" s="92"/>
-      <c r="D2" s="92"/>
-      <c r="E2" s="92"/>
-      <c r="F2" s="92"/>
-      <c r="G2" s="92"/>
-      <c r="H2" s="92"/>
-      <c r="I2" s="92"/>
-      <c r="J2" s="92"/>
-      <c r="K2" s="92"/>
-      <c r="L2" s="92"/>
-      <c r="M2" s="92"/>
-      <c r="N2" s="92"/>
-      <c r="O2" s="92"/>
-      <c r="P2" s="92"/>
+      <c r="B2" s="95"/>
+      <c r="C2" s="95"/>
+      <c r="D2" s="95"/>
+      <c r="E2" s="95"/>
+      <c r="F2" s="95"/>
+      <c r="G2" s="95"/>
+      <c r="H2" s="95"/>
+      <c r="I2" s="95"/>
+      <c r="J2" s="95"/>
+      <c r="K2" s="95"/>
+      <c r="L2" s="95"/>
+      <c r="M2" s="95"/>
+      <c r="N2" s="95"/>
+      <c r="O2" s="95"/>
+      <c r="P2" s="95"/>
     </row>
     <row r="3" spans="2:16" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="93" t="s">
+      <c r="B3" s="96" t="s">
         <v>71</v>
       </c>
-      <c r="C3" s="93"/>
-      <c r="D3" s="93"/>
-      <c r="E3" s="93"/>
-      <c r="F3" s="93"/>
-      <c r="G3" s="93"/>
-      <c r="H3" s="93"/>
-      <c r="I3" s="93"/>
-      <c r="J3" s="93"/>
-      <c r="K3" s="93"/>
-      <c r="L3" s="93"/>
-      <c r="M3" s="93"/>
-      <c r="N3" s="93"/>
-      <c r="O3" s="93"/>
-      <c r="P3" s="93"/>
+      <c r="C3" s="96"/>
+      <c r="D3" s="96"/>
+      <c r="E3" s="96"/>
+      <c r="F3" s="96"/>
+      <c r="G3" s="96"/>
+      <c r="H3" s="96"/>
+      <c r="I3" s="96"/>
+      <c r="J3" s="96"/>
+      <c r="K3" s="96"/>
+      <c r="L3" s="96"/>
+      <c r="M3" s="96"/>
+      <c r="N3" s="96"/>
+      <c r="O3" s="96"/>
+      <c r="P3" s="96"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
@@ -6106,40 +6103,40 @@
   <sheetData>
     <row r="1" spans="2:14" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="92"/>
-      <c r="C2" s="92"/>
-      <c r="D2" s="92"/>
-      <c r="E2" s="92"/>
-      <c r="F2" s="92"/>
-      <c r="G2" s="92"/>
-      <c r="H2" s="92"/>
-      <c r="I2" s="92"/>
-      <c r="J2" s="92"/>
-      <c r="K2" s="92"/>
-      <c r="L2" s="92"/>
-      <c r="M2" s="92"/>
-      <c r="N2" s="92"/>
+      <c r="B2" s="95"/>
+      <c r="C2" s="95"/>
+      <c r="D2" s="95"/>
+      <c r="E2" s="95"/>
+      <c r="F2" s="95"/>
+      <c r="G2" s="95"/>
+      <c r="H2" s="95"/>
+      <c r="I2" s="95"/>
+      <c r="J2" s="95"/>
+      <c r="K2" s="95"/>
+      <c r="L2" s="95"/>
+      <c r="M2" s="95"/>
+      <c r="N2" s="95"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="93" t="s">
+      <c r="B3" s="96" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="93"/>
-      <c r="D3" s="93"/>
-      <c r="E3" s="93"/>
-      <c r="F3" s="93"/>
-      <c r="G3" s="93"/>
-      <c r="H3" s="93"/>
-      <c r="I3" s="93"/>
-      <c r="J3" s="93"/>
-      <c r="K3" s="93"/>
-      <c r="L3" s="93"/>
-      <c r="M3" s="93"/>
-      <c r="N3" s="93"/>
+      <c r="C3" s="96"/>
+      <c r="D3" s="96"/>
+      <c r="E3" s="96"/>
+      <c r="F3" s="96"/>
+      <c r="G3" s="96"/>
+      <c r="H3" s="96"/>
+      <c r="I3" s="96"/>
+      <c r="J3" s="96"/>
+      <c r="K3" s="96"/>
+      <c r="L3" s="96"/>
+      <c r="M3" s="96"/>
+      <c r="N3" s="96"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="44" t="s">
@@ -6170,10 +6167,10 @@
         <v>22</v>
       </c>
       <c r="K5" s="45" t="s">
+        <v>134</v>
+      </c>
+      <c r="L5" s="45" t="s">
         <v>135</v>
-      </c>
-      <c r="L5" s="45" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
@@ -6224,44 +6221,44 @@
   <sheetData>
     <row r="1" spans="2:16" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="92"/>
-      <c r="C2" s="92"/>
-      <c r="D2" s="92"/>
-      <c r="E2" s="92"/>
-      <c r="F2" s="92"/>
-      <c r="G2" s="92"/>
-      <c r="H2" s="92"/>
-      <c r="I2" s="92"/>
-      <c r="J2" s="92"/>
-      <c r="K2" s="92"/>
-      <c r="L2" s="92"/>
-      <c r="M2" s="92"/>
-      <c r="N2" s="92"/>
-      <c r="O2" s="92"/>
-      <c r="P2" s="92"/>
+      <c r="B2" s="95"/>
+      <c r="C2" s="95"/>
+      <c r="D2" s="95"/>
+      <c r="E2" s="95"/>
+      <c r="F2" s="95"/>
+      <c r="G2" s="95"/>
+      <c r="H2" s="95"/>
+      <c r="I2" s="95"/>
+      <c r="J2" s="95"/>
+      <c r="K2" s="95"/>
+      <c r="L2" s="95"/>
+      <c r="M2" s="95"/>
+      <c r="N2" s="95"/>
+      <c r="O2" s="95"/>
+      <c r="P2" s="95"/>
     </row>
     <row r="3" spans="2:16" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="93" t="s">
+      <c r="B3" s="96" t="s">
         <v>65</v>
       </c>
-      <c r="C3" s="93"/>
-      <c r="D3" s="93"/>
-      <c r="E3" s="93"/>
-      <c r="F3" s="93"/>
-      <c r="G3" s="93"/>
-      <c r="H3" s="93"/>
-      <c r="I3" s="93"/>
-      <c r="J3" s="93"/>
-      <c r="K3" s="93"/>
-      <c r="L3" s="93"/>
-      <c r="M3" s="93"/>
-      <c r="N3" s="93"/>
-      <c r="O3" s="93"/>
-      <c r="P3" s="93"/>
+      <c r="C3" s="96"/>
+      <c r="D3" s="96"/>
+      <c r="E3" s="96"/>
+      <c r="F3" s="96"/>
+      <c r="G3" s="96"/>
+      <c r="H3" s="96"/>
+      <c r="I3" s="96"/>
+      <c r="J3" s="96"/>
+      <c r="K3" s="96"/>
+      <c r="L3" s="96"/>
+      <c r="M3" s="96"/>
+      <c r="N3" s="96"/>
+      <c r="O3" s="96"/>
+      <c r="P3" s="96"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="45" t="s">
@@ -6292,90 +6289,71 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:N6"/>
+  <dimension ref="B1:K6"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.85546875" customWidth="1"/>
     <col min="2" max="2" width="16.7109375" customWidth="1"/>
-    <col min="3" max="3" width="19.140625" customWidth="1"/>
-    <col min="4" max="4" width="28.140625" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" customWidth="1"/>
-    <col min="6" max="6" width="23" customWidth="1"/>
-    <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:11" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="92"/>
-      <c r="C2" s="92"/>
-      <c r="D2" s="92"/>
-      <c r="E2" s="92"/>
-      <c r="F2" s="92"/>
-      <c r="G2" s="92"/>
-      <c r="H2" s="92"/>
-      <c r="I2" s="92"/>
-      <c r="J2" s="92"/>
-      <c r="K2" s="92"/>
-      <c r="L2" s="92"/>
-      <c r="M2" s="92"/>
-      <c r="N2" s="92"/>
-    </row>
-    <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="93" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="98"/>
+      <c r="C2" s="98"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
+      <c r="F2" s="98"/>
+      <c r="G2" s="98"/>
+      <c r="H2" s="98"/>
+      <c r="I2" s="98"/>
+      <c r="J2" s="84"/>
+      <c r="K2" s="84"/>
+    </row>
+    <row r="3" spans="2:11" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B3" s="96" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="93"/>
-      <c r="D3" s="93"/>
-      <c r="E3" s="93"/>
-      <c r="F3" s="93"/>
-      <c r="G3" s="93"/>
-      <c r="H3" s="93"/>
-      <c r="I3" s="93"/>
-      <c r="J3" s="93"/>
-      <c r="K3" s="93"/>
-      <c r="L3" s="93"/>
-      <c r="M3" s="93"/>
-      <c r="N3" s="93"/>
-    </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C3" s="96"/>
+      <c r="D3" s="96"/>
+      <c r="E3" s="96"/>
+      <c r="F3" s="96"/>
+      <c r="G3" s="96"/>
+      <c r="H3" s="96"/>
+      <c r="I3" s="96"/>
+      <c r="J3" s="83"/>
+      <c r="K3" s="83"/>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F5" s="4" t="s">
+      <c r="C5" s="4" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="8"/>
+      <c r="C6" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B2:N2"/>
-    <mergeCell ref="B3:N3"/>
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="B3:I3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
TRIEDA-1674 - Atualizando importação e exportação com os novos campos.
TRIEDA-1675 - Atualizando importação e exportação com os novos campos.
</commit_message>
<xml_diff>
--- a/code/client/web/src/main/resources/templateExport.xlsx
+++ b/code/client/web/src/main/resources/templateExport.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="17070" windowHeight="5370" tabRatio="907" firstSheet="3" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="17070" windowHeight="5370" tabRatio="907" firstSheet="3" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Campi" sheetId="3" r:id="rId1"/>
@@ -919,6 +919,38 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Sim
+Não
+Determina se as aulas teoricas e praticas devem ser lecionadas em sequencia</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Sim
+Não
+Determina se o professor deve ser o mesmo para as aulas teoricas e praticas</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t>Sim
@@ -927,7 +959,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L5" authorId="0">
+    <comment ref="N5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1230,7 +1262,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="194">
   <si>
     <t>Planilha de Unidades</t>
   </si>
@@ -1806,6 +1838,12 @@
   </si>
   <si>
     <t>Planilha de Atendimentos Por Carga Horária</t>
+  </si>
+  <si>
+    <t>Aulas Continuas?</t>
+  </si>
+  <si>
+    <t>Professor Único?</t>
   </si>
 </sst>
 </file>
@@ -1816,7 +1854,7 @@
     <numFmt numFmtId="165" formatCode="&quot;R$&quot;\ #,##0.00"/>
     <numFmt numFmtId="178" formatCode="#,##0.0000"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1923,6 +1961,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="29">
@@ -2502,12 +2547,12 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2526,6 +2571,9 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="28" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2561,9 +2609,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="28" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3329,10 +3374,10 @@
       <c r="K5" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="L5" s="97" t="s">
+      <c r="L5" s="98" t="s">
         <v>109</v>
       </c>
-      <c r="M5" s="97"/>
+      <c r="M5" s="98"/>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
@@ -4324,14 +4369,14 @@
       </c>
     </row>
     <row r="2" spans="2:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="98"/>
-      <c r="C2" s="98"/>
-      <c r="D2" s="98"/>
-      <c r="E2" s="98"/>
-      <c r="F2" s="98"/>
-      <c r="G2" s="98"/>
-      <c r="H2" s="98"/>
-      <c r="I2" s="98"/>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
+      <c r="F2" s="97"/>
+      <c r="G2" s="97"/>
+      <c r="H2" s="97"/>
+      <c r="I2" s="97"/>
       <c r="L2" s="84"/>
       <c r="M2" s="84"/>
       <c r="N2" s="84"/>
@@ -5264,10 +5309,10 @@
       </c>
       <c r="N5" s="104"/>
       <c r="O5" s="104"/>
-      <c r="P5" s="97" t="s">
+      <c r="P5" s="98" t="s">
         <v>108</v>
       </c>
-      <c r="Q5" s="97"/>
+      <c r="Q5" s="98"/>
     </row>
     <row r="6" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="70" t="s">
@@ -5528,70 +5573,70 @@
       <c r="R3" s="57"/>
     </row>
     <row r="5" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B5" s="107" t="s">
+      <c r="B5" s="108" t="s">
         <v>111</v>
       </c>
-      <c r="C5" s="108"/>
-      <c r="D5" s="108"/>
-      <c r="E5" s="108"/>
-      <c r="F5" s="108"/>
-      <c r="G5" s="108"/>
-      <c r="H5" s="108"/>
-      <c r="I5" s="108"/>
-      <c r="J5" s="108"/>
-      <c r="K5" s="108"/>
-      <c r="L5" s="109"/>
-      <c r="M5" s="107" t="s">
+      <c r="C5" s="109"/>
+      <c r="D5" s="109"/>
+      <c r="E5" s="109"/>
+      <c r="F5" s="109"/>
+      <c r="G5" s="109"/>
+      <c r="H5" s="109"/>
+      <c r="I5" s="109"/>
+      <c r="J5" s="109"/>
+      <c r="K5" s="109"/>
+      <c r="L5" s="110"/>
+      <c r="M5" s="108" t="s">
         <v>112</v>
       </c>
-      <c r="N5" s="108"/>
-      <c r="O5" s="108"/>
-      <c r="P5" s="108"/>
-      <c r="Q5" s="108"/>
-      <c r="R5" s="108"/>
-      <c r="S5" s="108"/>
-      <c r="T5" s="108"/>
-      <c r="U5" s="108"/>
-      <c r="V5" s="108"/>
-      <c r="W5" s="108"/>
-      <c r="X5" s="108"/>
-      <c r="Y5" s="109"/>
+      <c r="N5" s="109"/>
+      <c r="O5" s="109"/>
+      <c r="P5" s="109"/>
+      <c r="Q5" s="109"/>
+      <c r="R5" s="109"/>
+      <c r="S5" s="109"/>
+      <c r="T5" s="109"/>
+      <c r="U5" s="109"/>
+      <c r="V5" s="109"/>
+      <c r="W5" s="109"/>
+      <c r="X5" s="109"/>
+      <c r="Y5" s="110"/>
     </row>
     <row r="6" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B6" s="117"/>
-      <c r="C6" s="117"/>
-      <c r="D6" s="117"/>
-      <c r="E6" s="117"/>
-      <c r="F6" s="113" t="s">
+      <c r="B6" s="105"/>
+      <c r="C6" s="105"/>
+      <c r="D6" s="105"/>
+      <c r="E6" s="105"/>
+      <c r="F6" s="114" t="s">
         <v>27</v>
       </c>
-      <c r="G6" s="114"/>
-      <c r="H6" s="114"/>
-      <c r="I6" s="115"/>
-      <c r="J6" s="107" t="s">
+      <c r="G6" s="115"/>
+      <c r="H6" s="115"/>
+      <c r="I6" s="116"/>
+      <c r="J6" s="108" t="s">
         <v>30</v>
       </c>
-      <c r="K6" s="108"/>
-      <c r="L6" s="109"/>
+      <c r="K6" s="109"/>
+      <c r="L6" s="110"/>
       <c r="M6" s="88"/>
-      <c r="N6" s="105" t="s">
+      <c r="N6" s="106" t="s">
         <v>42</v>
       </c>
-      <c r="O6" s="106"/>
-      <c r="P6" s="105" t="s">
+      <c r="O6" s="107"/>
+      <c r="P6" s="106" t="s">
         <v>105</v>
       </c>
-      <c r="Q6" s="116"/>
-      <c r="R6" s="106"/>
+      <c r="Q6" s="117"/>
+      <c r="R6" s="107"/>
       <c r="S6" s="88"/>
-      <c r="T6" s="105" t="s">
+      <c r="T6" s="106" t="s">
         <v>122</v>
       </c>
-      <c r="U6" s="106"/>
-      <c r="V6" s="110"/>
-      <c r="W6" s="111"/>
-      <c r="X6" s="111"/>
-      <c r="Y6" s="112"/>
+      <c r="U6" s="107"/>
+      <c r="V6" s="111"/>
+      <c r="W6" s="112"/>
+      <c r="X6" s="112"/>
+      <c r="Y6" s="113"/>
     </row>
     <row r="7" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B7" s="75" t="s">
@@ -5695,6 +5740,7 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="P6:R6"/>
     <mergeCell ref="B6:E6"/>
     <mergeCell ref="T6:U6"/>
     <mergeCell ref="M5:Y5"/>
@@ -5705,7 +5751,6 @@
     <mergeCell ref="J6:L6"/>
     <mergeCell ref="F6:I6"/>
     <mergeCell ref="N6:O6"/>
-    <mergeCell ref="P6:R6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -6079,10 +6124,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:N6"/>
+  <dimension ref="B1:P6"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="D1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5:L6"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6097,16 +6142,17 @@
     <col min="8" max="8" width="24.7109375" customWidth="1"/>
     <col min="9" max="9" width="25.7109375" customWidth="1"/>
     <col min="10" max="10" width="25.85546875" customWidth="1"/>
-    <col min="11" max="11" width="14.28515625" customWidth="1"/>
-    <col min="12" max="12" width="14.42578125" customWidth="1"/>
+    <col min="11" max="12" width="17.7109375" customWidth="1"/>
+    <col min="13" max="13" width="14.28515625" customWidth="1"/>
+    <col min="14" max="14" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:16" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="95"/>
       <c r="C2" s="95"/>
       <c r="D2" s="95"/>
@@ -6120,8 +6166,10 @@
       <c r="L2" s="95"/>
       <c r="M2" s="95"/>
       <c r="N2" s="95"/>
-    </row>
-    <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="O2" s="95"/>
+      <c r="P2" s="95"/>
+    </row>
+    <row r="3" spans="2:16" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="96" t="s">
         <v>20</v>
       </c>
@@ -6137,8 +6185,10 @@
       <c r="L3" s="96"/>
       <c r="M3" s="96"/>
       <c r="N3" s="96"/>
-    </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="O3" s="96"/>
+      <c r="P3" s="96"/>
+    </row>
+    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="44" t="s">
         <v>86</v>
       </c>
@@ -6166,14 +6216,20 @@
       <c r="J5" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="K5" s="45" t="s">
+      <c r="K5" s="91" t="s">
+        <v>192</v>
+      </c>
+      <c r="L5" s="91" t="s">
+        <v>193</v>
+      </c>
+      <c r="M5" s="45" t="s">
         <v>134</v>
       </c>
-      <c r="L5" s="45" t="s">
+      <c r="N5" s="45" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="6"/>
@@ -6183,13 +6239,15 @@
       <c r="H6" s="8"/>
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
-      <c r="K6" s="68"/>
+      <c r="K6" s="6"/>
       <c r="L6" s="6"/>
+      <c r="M6" s="68"/>
+      <c r="N6" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B2:N2"/>
-    <mergeCell ref="B3:N3"/>
+    <mergeCell ref="B2:P2"/>
+    <mergeCell ref="B3:P3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -6291,7 +6349,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K6"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
@@ -6313,14 +6371,14 @@
       </c>
     </row>
     <row r="2" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="98"/>
-      <c r="C2" s="98"/>
-      <c r="D2" s="98"/>
-      <c r="E2" s="98"/>
-      <c r="F2" s="98"/>
-      <c r="G2" s="98"/>
-      <c r="H2" s="98"/>
-      <c r="I2" s="98"/>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
+      <c r="F2" s="97"/>
+      <c r="G2" s="97"/>
+      <c r="H2" s="97"/>
+      <c r="I2" s="97"/>
       <c r="J2" s="84"/>
       <c r="K2" s="84"/>
     </row>

</xml_diff>

<commit_message>
TRIEDA-1683 - Adicionando parâmetros maximo de dias por semana e mínimo de créditos diários em professores. Atualizando script para criar as tabelas no BD
</commit_message>
<xml_diff>
--- a/code/client/web/src/main/resources/templateExport.xlsx
+++ b/code/client/web/src/main/resources/templateExport.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="17070" windowHeight="5370" tabRatio="907" firstSheet="3" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="17070" windowHeight="5370" tabRatio="907" firstSheet="3" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="Campi" sheetId="3" r:id="rId1"/>
@@ -1262,7 +1262,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="196">
   <si>
     <t>Planilha de Unidades</t>
   </si>
@@ -1844,6 +1844,12 @@
   </si>
   <si>
     <t>Professor Único?</t>
+  </si>
+  <si>
+    <t>Máx. Dias por Semana</t>
+  </si>
+  <si>
+    <t>Min. Creditos Diários</t>
   </si>
 </sst>
 </file>
@@ -1900,6 +1906,13 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1961,13 +1974,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="29">
@@ -2271,18 +2277,18 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="118">
+  <cellXfs count="119">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -2300,16 +2306,16 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2391,202 +2397,208 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="8" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="27" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="7" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="8" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="8" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="8" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="7" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="7" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="28" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="28" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2598,17 +2610,14 @@
     <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2937,38 +2946,38 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="95" t="s">
+      <c r="B2" s="96" t="s">
         <v>95</v>
       </c>
-      <c r="C2" s="95"/>
-      <c r="D2" s="95"/>
-      <c r="E2" s="95"/>
-      <c r="F2" s="95"/>
-      <c r="G2" s="95"/>
-      <c r="H2" s="95"/>
-      <c r="I2" s="95"/>
-      <c r="J2" s="95"/>
-      <c r="K2" s="95"/>
-      <c r="L2" s="95"/>
-      <c r="M2" s="95"/>
-      <c r="N2" s="95"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="96"/>
+      <c r="E2" s="96"/>
+      <c r="F2" s="96"/>
+      <c r="G2" s="96"/>
+      <c r="H2" s="96"/>
+      <c r="I2" s="96"/>
+      <c r="J2" s="96"/>
+      <c r="K2" s="96"/>
+      <c r="L2" s="96"/>
+      <c r="M2" s="96"/>
+      <c r="N2" s="96"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="96" t="s">
+      <c r="B3" s="97" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="96"/>
-      <c r="D3" s="96"/>
-      <c r="E3" s="96"/>
-      <c r="F3" s="96"/>
-      <c r="G3" s="96"/>
-      <c r="H3" s="96"/>
-      <c r="I3" s="96"/>
-      <c r="J3" s="96"/>
-      <c r="K3" s="96"/>
-      <c r="L3" s="96"/>
-      <c r="M3" s="96"/>
-      <c r="N3" s="96"/>
+      <c r="C3" s="97"/>
+      <c r="D3" s="97"/>
+      <c r="E3" s="97"/>
+      <c r="F3" s="97"/>
+      <c r="G3" s="97"/>
+      <c r="H3" s="97"/>
+      <c r="I3" s="97"/>
+      <c r="J3" s="97"/>
+      <c r="K3" s="97"/>
+      <c r="L3" s="97"/>
+      <c r="M3" s="97"/>
+      <c r="N3" s="97"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="44" t="s">
@@ -3036,36 +3045,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="95"/>
-      <c r="C2" s="95"/>
-      <c r="D2" s="95"/>
-      <c r="E2" s="95"/>
-      <c r="F2" s="95"/>
-      <c r="G2" s="95"/>
-      <c r="H2" s="95"/>
-      <c r="I2" s="95"/>
-      <c r="J2" s="95"/>
-      <c r="K2" s="95"/>
-      <c r="L2" s="95"/>
-      <c r="M2" s="95"/>
-      <c r="N2" s="95"/>
+      <c r="B2" s="96"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="96"/>
+      <c r="E2" s="96"/>
+      <c r="F2" s="96"/>
+      <c r="G2" s="96"/>
+      <c r="H2" s="96"/>
+      <c r="I2" s="96"/>
+      <c r="J2" s="96"/>
+      <c r="K2" s="96"/>
+      <c r="L2" s="96"/>
+      <c r="M2" s="96"/>
+      <c r="N2" s="96"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="96" t="s">
+      <c r="B3" s="97" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="96"/>
-      <c r="D3" s="96"/>
-      <c r="E3" s="96"/>
-      <c r="F3" s="96"/>
-      <c r="G3" s="96"/>
-      <c r="H3" s="96"/>
-      <c r="I3" s="96"/>
-      <c r="J3" s="96"/>
-      <c r="K3" s="96"/>
-      <c r="L3" s="96"/>
-      <c r="M3" s="96"/>
-      <c r="N3" s="96"/>
+      <c r="C3" s="97"/>
+      <c r="D3" s="97"/>
+      <c r="E3" s="97"/>
+      <c r="F3" s="97"/>
+      <c r="G3" s="97"/>
+      <c r="H3" s="97"/>
+      <c r="I3" s="97"/>
+      <c r="J3" s="97"/>
+      <c r="K3" s="97"/>
+      <c r="L3" s="97"/>
+      <c r="M3" s="97"/>
+      <c r="N3" s="97"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -3134,36 +3143,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="95"/>
-      <c r="C2" s="95"/>
-      <c r="D2" s="95"/>
-      <c r="E2" s="95"/>
-      <c r="F2" s="95"/>
-      <c r="G2" s="95"/>
-      <c r="H2" s="95"/>
-      <c r="I2" s="95"/>
-      <c r="J2" s="95"/>
-      <c r="K2" s="95"/>
-      <c r="L2" s="95"/>
-      <c r="M2" s="95"/>
-      <c r="N2" s="95"/>
+      <c r="B2" s="96"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="96"/>
+      <c r="E2" s="96"/>
+      <c r="F2" s="96"/>
+      <c r="G2" s="96"/>
+      <c r="H2" s="96"/>
+      <c r="I2" s="96"/>
+      <c r="J2" s="96"/>
+      <c r="K2" s="96"/>
+      <c r="L2" s="96"/>
+      <c r="M2" s="96"/>
+      <c r="N2" s="96"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="96" t="s">
+      <c r="B3" s="97" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="96"/>
-      <c r="D3" s="96"/>
-      <c r="E3" s="96"/>
-      <c r="F3" s="96"/>
-      <c r="G3" s="96"/>
-      <c r="H3" s="96"/>
-      <c r="I3" s="96"/>
-      <c r="J3" s="96"/>
-      <c r="K3" s="96"/>
-      <c r="L3" s="96"/>
-      <c r="M3" s="96"/>
-      <c r="N3" s="96"/>
+      <c r="C3" s="97"/>
+      <c r="D3" s="97"/>
+      <c r="E3" s="97"/>
+      <c r="F3" s="97"/>
+      <c r="G3" s="97"/>
+      <c r="H3" s="97"/>
+      <c r="I3" s="97"/>
+      <c r="J3" s="97"/>
+      <c r="K3" s="97"/>
+      <c r="L3" s="97"/>
+      <c r="M3" s="97"/>
+      <c r="N3" s="97"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -3248,18 +3257,18 @@
       </c>
     </row>
     <row r="2" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="95"/>
-      <c r="C2" s="95"/>
-      <c r="D2" s="95"/>
-      <c r="E2" s="95"/>
+      <c r="B2" s="96"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="96"/>
+      <c r="E2" s="96"/>
     </row>
     <row r="3" spans="2:5" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="96" t="s">
+      <c r="B3" s="97" t="s">
         <v>125</v>
       </c>
-      <c r="C3" s="96"/>
-      <c r="D3" s="96"/>
-      <c r="E3" s="96"/>
+      <c r="C3" s="97"/>
+      <c r="D3" s="97"/>
+      <c r="E3" s="97"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="60" t="s">
@@ -3312,36 +3321,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="95"/>
-      <c r="C2" s="95"/>
-      <c r="D2" s="95"/>
-      <c r="E2" s="95"/>
-      <c r="F2" s="95"/>
-      <c r="G2" s="95"/>
-      <c r="H2" s="95"/>
-      <c r="I2" s="95"/>
-      <c r="J2" s="95"/>
-      <c r="K2" s="95"/>
-      <c r="L2" s="95"/>
-      <c r="M2" s="95"/>
-      <c r="N2" s="95"/>
+      <c r="B2" s="96"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="96"/>
+      <c r="E2" s="96"/>
+      <c r="F2" s="96"/>
+      <c r="G2" s="96"/>
+      <c r="H2" s="96"/>
+      <c r="I2" s="96"/>
+      <c r="J2" s="96"/>
+      <c r="K2" s="96"/>
+      <c r="L2" s="96"/>
+      <c r="M2" s="96"/>
+      <c r="N2" s="96"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="96" t="s">
+      <c r="B3" s="97" t="s">
         <v>99</v>
       </c>
-      <c r="C3" s="96"/>
-      <c r="D3" s="96"/>
-      <c r="E3" s="96"/>
-      <c r="F3" s="96"/>
-      <c r="G3" s="96"/>
-      <c r="H3" s="96"/>
-      <c r="I3" s="96"/>
-      <c r="J3" s="96"/>
-      <c r="K3" s="96"/>
-      <c r="L3" s="96"/>
-      <c r="M3" s="96"/>
-      <c r="N3" s="96"/>
+      <c r="C3" s="97"/>
+      <c r="D3" s="97"/>
+      <c r="E3" s="97"/>
+      <c r="F3" s="97"/>
+      <c r="G3" s="97"/>
+      <c r="H3" s="97"/>
+      <c r="I3" s="97"/>
+      <c r="J3" s="97"/>
+      <c r="K3" s="97"/>
+      <c r="L3" s="97"/>
+      <c r="M3" s="97"/>
+      <c r="N3" s="97"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -3374,10 +3383,10 @@
       <c r="K5" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="L5" s="98" t="s">
+      <c r="L5" s="99" t="s">
         <v>109</v>
       </c>
-      <c r="M5" s="98"/>
+      <c r="M5" s="99"/>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
@@ -3405,7 +3414,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O6"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3420,7 +3431,8 @@
     <col min="9" max="9" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="30.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.140625" customWidth="1"/>
+    <col min="13" max="13" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:15" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
@@ -3429,38 +3441,38 @@
       </c>
     </row>
     <row r="2" spans="2:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="95"/>
-      <c r="C2" s="95"/>
-      <c r="D2" s="95"/>
-      <c r="E2" s="95"/>
-      <c r="F2" s="95"/>
-      <c r="G2" s="95"/>
-      <c r="H2" s="95"/>
-      <c r="I2" s="95"/>
-      <c r="J2" s="95"/>
-      <c r="K2" s="95"/>
-      <c r="L2" s="95"/>
-      <c r="M2" s="95"/>
-      <c r="N2" s="95"/>
-      <c r="O2" s="95"/>
+      <c r="B2" s="96"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="96"/>
+      <c r="E2" s="96"/>
+      <c r="F2" s="96"/>
+      <c r="G2" s="96"/>
+      <c r="H2" s="96"/>
+      <c r="I2" s="96"/>
+      <c r="J2" s="96"/>
+      <c r="K2" s="96"/>
+      <c r="L2" s="96"/>
+      <c r="M2" s="96"/>
+      <c r="N2" s="96"/>
+      <c r="O2" s="96"/>
     </row>
     <row r="3" spans="2:15" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="96" t="s">
+      <c r="B3" s="97" t="s">
         <v>73</v>
       </c>
-      <c r="C3" s="96"/>
-      <c r="D3" s="96"/>
-      <c r="E3" s="96"/>
-      <c r="F3" s="96"/>
-      <c r="G3" s="96"/>
-      <c r="H3" s="96"/>
-      <c r="I3" s="96"/>
-      <c r="J3" s="96"/>
-      <c r="K3" s="96"/>
-      <c r="L3" s="96"/>
-      <c r="M3" s="96"/>
-      <c r="N3" s="96"/>
-      <c r="O3" s="96"/>
+      <c r="C3" s="97"/>
+      <c r="D3" s="97"/>
+      <c r="E3" s="97"/>
+      <c r="F3" s="97"/>
+      <c r="G3" s="97"/>
+      <c r="H3" s="97"/>
+      <c r="I3" s="97"/>
+      <c r="J3" s="97"/>
+      <c r="K3" s="97"/>
+      <c r="L3" s="97"/>
+      <c r="M3" s="97"/>
+      <c r="N3" s="97"/>
+      <c r="O3" s="97"/>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -3492,6 +3504,12 @@
       </c>
       <c r="K5" s="45" t="s">
         <v>98</v>
+      </c>
+      <c r="L5" s="95" t="s">
+        <v>194</v>
+      </c>
+      <c r="M5" s="95" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.25">
@@ -3505,6 +3523,8 @@
       <c r="I6" s="8"/>
       <c r="J6" s="8"/>
       <c r="K6" s="7"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -3539,18 +3559,18 @@
       </c>
     </row>
     <row r="2" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="95"/>
-      <c r="C2" s="95"/>
-      <c r="D2" s="95"/>
-      <c r="E2" s="95"/>
+      <c r="B2" s="96"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="96"/>
+      <c r="E2" s="96"/>
     </row>
     <row r="3" spans="2:5" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="96" t="s">
+      <c r="B3" s="97" t="s">
         <v>130</v>
       </c>
-      <c r="C3" s="96"/>
-      <c r="D3" s="96"/>
-      <c r="E3" s="96"/>
+      <c r="C3" s="97"/>
+      <c r="D3" s="97"/>
+      <c r="E3" s="97"/>
     </row>
     <row r="4" spans="2:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="64"/>
@@ -3612,36 +3632,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="95"/>
-      <c r="C2" s="95"/>
-      <c r="D2" s="95"/>
-      <c r="E2" s="95"/>
-      <c r="F2" s="95"/>
-      <c r="G2" s="95"/>
-      <c r="H2" s="95"/>
-      <c r="I2" s="95"/>
-      <c r="J2" s="95"/>
-      <c r="K2" s="95"/>
-      <c r="L2" s="95"/>
-      <c r="M2" s="95"/>
-      <c r="N2" s="95"/>
+      <c r="B2" s="96"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="96"/>
+      <c r="E2" s="96"/>
+      <c r="F2" s="96"/>
+      <c r="G2" s="96"/>
+      <c r="H2" s="96"/>
+      <c r="I2" s="96"/>
+      <c r="J2" s="96"/>
+      <c r="K2" s="96"/>
+      <c r="L2" s="96"/>
+      <c r="M2" s="96"/>
+      <c r="N2" s="96"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="96" t="s">
+      <c r="B3" s="97" t="s">
         <v>69</v>
       </c>
-      <c r="C3" s="96"/>
-      <c r="D3" s="96"/>
-      <c r="E3" s="96"/>
-      <c r="F3" s="96"/>
-      <c r="G3" s="96"/>
-      <c r="H3" s="96"/>
-      <c r="I3" s="96"/>
-      <c r="J3" s="96"/>
-      <c r="K3" s="96"/>
-      <c r="L3" s="96"/>
-      <c r="M3" s="96"/>
-      <c r="N3" s="96"/>
+      <c r="C3" s="97"/>
+      <c r="D3" s="97"/>
+      <c r="E3" s="97"/>
+      <c r="F3" s="97"/>
+      <c r="G3" s="97"/>
+      <c r="H3" s="97"/>
+      <c r="I3" s="97"/>
+      <c r="J3" s="97"/>
+      <c r="K3" s="97"/>
+      <c r="L3" s="97"/>
+      <c r="M3" s="97"/>
+      <c r="N3" s="97"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -3696,36 +3716,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="95"/>
-      <c r="C2" s="95"/>
-      <c r="D2" s="95"/>
-      <c r="E2" s="95"/>
-      <c r="F2" s="95"/>
-      <c r="G2" s="95"/>
-      <c r="H2" s="95"/>
-      <c r="I2" s="95"/>
-      <c r="J2" s="95"/>
-      <c r="K2" s="95"/>
-      <c r="L2" s="95"/>
-      <c r="M2" s="95"/>
-      <c r="N2" s="95"/>
+      <c r="B2" s="96"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="96"/>
+      <c r="E2" s="96"/>
+      <c r="F2" s="96"/>
+      <c r="G2" s="96"/>
+      <c r="H2" s="96"/>
+      <c r="I2" s="96"/>
+      <c r="J2" s="96"/>
+      <c r="K2" s="96"/>
+      <c r="L2" s="96"/>
+      <c r="M2" s="96"/>
+      <c r="N2" s="96"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="96" t="s">
+      <c r="B3" s="97" t="s">
         <v>74</v>
       </c>
-      <c r="C3" s="96"/>
-      <c r="D3" s="96"/>
-      <c r="E3" s="96"/>
-      <c r="F3" s="96"/>
-      <c r="G3" s="96"/>
-      <c r="H3" s="96"/>
-      <c r="I3" s="96"/>
-      <c r="J3" s="96"/>
-      <c r="K3" s="96"/>
-      <c r="L3" s="96"/>
-      <c r="M3" s="96"/>
-      <c r="N3" s="96"/>
+      <c r="C3" s="97"/>
+      <c r="D3" s="97"/>
+      <c r="E3" s="97"/>
+      <c r="F3" s="97"/>
+      <c r="G3" s="97"/>
+      <c r="H3" s="97"/>
+      <c r="I3" s="97"/>
+      <c r="J3" s="97"/>
+      <c r="K3" s="97"/>
+      <c r="L3" s="97"/>
+      <c r="M3" s="97"/>
+      <c r="N3" s="97"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -3794,40 +3814,40 @@
       </c>
     </row>
     <row r="2" spans="2:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="95"/>
-      <c r="C2" s="95"/>
-      <c r="D2" s="95"/>
-      <c r="E2" s="95"/>
-      <c r="F2" s="95"/>
-      <c r="G2" s="95"/>
-      <c r="H2" s="95"/>
-      <c r="I2" s="95"/>
-      <c r="J2" s="95"/>
-      <c r="K2" s="95"/>
-      <c r="L2" s="95"/>
-      <c r="M2" s="95"/>
-      <c r="N2" s="95"/>
-      <c r="O2" s="95"/>
-      <c r="P2" s="95"/>
+      <c r="B2" s="96"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="96"/>
+      <c r="E2" s="96"/>
+      <c r="F2" s="96"/>
+      <c r="G2" s="96"/>
+      <c r="H2" s="96"/>
+      <c r="I2" s="96"/>
+      <c r="J2" s="96"/>
+      <c r="K2" s="96"/>
+      <c r="L2" s="96"/>
+      <c r="M2" s="96"/>
+      <c r="N2" s="96"/>
+      <c r="O2" s="96"/>
+      <c r="P2" s="96"/>
     </row>
     <row r="3" spans="2:18" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="96" t="s">
+      <c r="B3" s="97" t="s">
         <v>63</v>
       </c>
-      <c r="C3" s="96"/>
-      <c r="D3" s="96"/>
-      <c r="E3" s="96"/>
-      <c r="F3" s="96"/>
-      <c r="G3" s="96"/>
-      <c r="H3" s="96"/>
-      <c r="I3" s="96"/>
-      <c r="J3" s="96"/>
-      <c r="K3" s="96"/>
-      <c r="L3" s="96"/>
-      <c r="M3" s="96"/>
-      <c r="N3" s="96"/>
-      <c r="O3" s="96"/>
-      <c r="P3" s="96"/>
+      <c r="C3" s="97"/>
+      <c r="D3" s="97"/>
+      <c r="E3" s="97"/>
+      <c r="F3" s="97"/>
+      <c r="G3" s="97"/>
+      <c r="H3" s="97"/>
+      <c r="I3" s="97"/>
+      <c r="J3" s="97"/>
+      <c r="K3" s="97"/>
+      <c r="L3" s="97"/>
+      <c r="M3" s="97"/>
+      <c r="N3" s="97"/>
+      <c r="O3" s="97"/>
+      <c r="P3" s="97"/>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
@@ -3941,36 +3961,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="95"/>
-      <c r="C2" s="95"/>
-      <c r="D2" s="95"/>
-      <c r="E2" s="95"/>
-      <c r="F2" s="95"/>
-      <c r="G2" s="95"/>
-      <c r="H2" s="95"/>
-      <c r="I2" s="95"/>
-      <c r="J2" s="95"/>
-      <c r="K2" s="95"/>
-      <c r="L2" s="95"/>
-      <c r="M2" s="95"/>
-      <c r="N2" s="95"/>
+      <c r="B2" s="96"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="96"/>
+      <c r="E2" s="96"/>
+      <c r="F2" s="96"/>
+      <c r="G2" s="96"/>
+      <c r="H2" s="96"/>
+      <c r="I2" s="96"/>
+      <c r="J2" s="96"/>
+      <c r="K2" s="96"/>
+      <c r="L2" s="96"/>
+      <c r="M2" s="96"/>
+      <c r="N2" s="96"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="96" t="s">
+      <c r="B3" s="97" t="s">
         <v>64</v>
       </c>
-      <c r="C3" s="96"/>
-      <c r="D3" s="96"/>
-      <c r="E3" s="96"/>
-      <c r="F3" s="96"/>
-      <c r="G3" s="96"/>
-      <c r="H3" s="96"/>
-      <c r="I3" s="96"/>
-      <c r="J3" s="96"/>
-      <c r="K3" s="96"/>
-      <c r="L3" s="96"/>
-      <c r="M3" s="96"/>
-      <c r="N3" s="96"/>
+      <c r="C3" s="97"/>
+      <c r="D3" s="97"/>
+      <c r="E3" s="97"/>
+      <c r="F3" s="97"/>
+      <c r="G3" s="97"/>
+      <c r="H3" s="97"/>
+      <c r="I3" s="97"/>
+      <c r="J3" s="97"/>
+      <c r="K3" s="97"/>
+      <c r="L3" s="97"/>
+      <c r="M3" s="97"/>
+      <c r="N3" s="97"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="58" t="s">
@@ -4057,38 +4077,38 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="95" t="s">
+      <c r="B2" s="96" t="s">
         <v>96</v>
       </c>
-      <c r="C2" s="95"/>
-      <c r="D2" s="95"/>
-      <c r="E2" s="95"/>
-      <c r="F2" s="95"/>
-      <c r="G2" s="95"/>
-      <c r="H2" s="95"/>
-      <c r="I2" s="95"/>
-      <c r="J2" s="95"/>
-      <c r="K2" s="95"/>
-      <c r="L2" s="95"/>
-      <c r="M2" s="95"/>
-      <c r="N2" s="95"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="96"/>
+      <c r="E2" s="96"/>
+      <c r="F2" s="96"/>
+      <c r="G2" s="96"/>
+      <c r="H2" s="96"/>
+      <c r="I2" s="96"/>
+      <c r="J2" s="96"/>
+      <c r="K2" s="96"/>
+      <c r="L2" s="96"/>
+      <c r="M2" s="96"/>
+      <c r="N2" s="96"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="96" t="s">
+      <c r="B3" s="97" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="96"/>
-      <c r="D3" s="96"/>
-      <c r="E3" s="96"/>
-      <c r="F3" s="96"/>
-      <c r="G3" s="96"/>
-      <c r="H3" s="96"/>
-      <c r="I3" s="96"/>
-      <c r="J3" s="96"/>
-      <c r="K3" s="96"/>
-      <c r="L3" s="96"/>
-      <c r="M3" s="96"/>
-      <c r="N3" s="96"/>
+      <c r="C3" s="97"/>
+      <c r="D3" s="97"/>
+      <c r="E3" s="97"/>
+      <c r="F3" s="97"/>
+      <c r="G3" s="97"/>
+      <c r="H3" s="97"/>
+      <c r="I3" s="97"/>
+      <c r="J3" s="97"/>
+      <c r="K3" s="97"/>
+      <c r="L3" s="97"/>
+      <c r="M3" s="97"/>
+      <c r="N3" s="97"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="44" t="s">
@@ -4147,36 +4167,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="95"/>
-      <c r="C2" s="95"/>
-      <c r="D2" s="95"/>
-      <c r="E2" s="95"/>
-      <c r="F2" s="95"/>
-      <c r="G2" s="95"/>
-      <c r="H2" s="95"/>
-      <c r="I2" s="95"/>
-      <c r="J2" s="95"/>
-      <c r="K2" s="95"/>
-      <c r="L2" s="95"/>
-      <c r="M2" s="95"/>
-      <c r="N2" s="95"/>
+      <c r="B2" s="96"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="96"/>
+      <c r="E2" s="96"/>
+      <c r="F2" s="96"/>
+      <c r="G2" s="96"/>
+      <c r="H2" s="96"/>
+      <c r="I2" s="96"/>
+      <c r="J2" s="96"/>
+      <c r="K2" s="96"/>
+      <c r="L2" s="96"/>
+      <c r="M2" s="96"/>
+      <c r="N2" s="96"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="96" t="s">
+      <c r="B3" s="97" t="s">
         <v>151</v>
       </c>
-      <c r="C3" s="96"/>
-      <c r="D3" s="96"/>
-      <c r="E3" s="96"/>
-      <c r="F3" s="96"/>
-      <c r="G3" s="96"/>
-      <c r="H3" s="96"/>
-      <c r="I3" s="96"/>
-      <c r="J3" s="96"/>
-      <c r="K3" s="96"/>
-      <c r="L3" s="96"/>
-      <c r="M3" s="96"/>
-      <c r="N3" s="96"/>
+      <c r="C3" s="97"/>
+      <c r="D3" s="97"/>
+      <c r="E3" s="97"/>
+      <c r="F3" s="97"/>
+      <c r="G3" s="97"/>
+      <c r="H3" s="97"/>
+      <c r="I3" s="97"/>
+      <c r="J3" s="97"/>
+      <c r="K3" s="97"/>
+      <c r="L3" s="97"/>
+      <c r="M3" s="97"/>
+      <c r="N3" s="97"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="74" t="s">
@@ -4263,28 +4283,28 @@
       </c>
     </row>
     <row r="2" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="95"/>
-      <c r="C2" s="95"/>
-      <c r="D2" s="95"/>
-      <c r="E2" s="95"/>
-      <c r="F2" s="95"/>
-      <c r="G2" s="95"/>
-      <c r="H2" s="95"/>
-      <c r="I2" s="95"/>
-      <c r="J2" s="95"/>
+      <c r="B2" s="96"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="96"/>
+      <c r="E2" s="96"/>
+      <c r="F2" s="96"/>
+      <c r="G2" s="96"/>
+      <c r="H2" s="96"/>
+      <c r="I2" s="96"/>
+      <c r="J2" s="96"/>
     </row>
     <row r="3" spans="2:10" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="96" t="s">
+      <c r="B3" s="97" t="s">
         <v>154</v>
       </c>
-      <c r="C3" s="96"/>
-      <c r="D3" s="96"/>
-      <c r="E3" s="96"/>
-      <c r="F3" s="96"/>
-      <c r="G3" s="96"/>
-      <c r="H3" s="96"/>
-      <c r="I3" s="96"/>
-      <c r="J3" s="96"/>
+      <c r="C3" s="97"/>
+      <c r="D3" s="97"/>
+      <c r="E3" s="97"/>
+      <c r="F3" s="97"/>
+      <c r="G3" s="97"/>
+      <c r="H3" s="97"/>
+      <c r="I3" s="97"/>
+      <c r="J3" s="97"/>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" s="74" t="s">
@@ -4369,29 +4389,29 @@
       </c>
     </row>
     <row r="2" spans="2:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="97"/>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="97"/>
+      <c r="B2" s="98"/>
+      <c r="C2" s="98"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
+      <c r="F2" s="98"/>
+      <c r="G2" s="98"/>
+      <c r="H2" s="98"/>
+      <c r="I2" s="98"/>
       <c r="L2" s="84"/>
       <c r="M2" s="84"/>
       <c r="N2" s="84"/>
     </row>
     <row r="3" spans="2:20" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="96" t="s">
+      <c r="B3" s="97" t="s">
         <v>155</v>
       </c>
-      <c r="C3" s="96"/>
-      <c r="D3" s="96"/>
-      <c r="E3" s="96"/>
-      <c r="F3" s="96"/>
-      <c r="G3" s="96"/>
-      <c r="H3" s="96"/>
-      <c r="I3" s="96"/>
+      <c r="C3" s="97"/>
+      <c r="D3" s="97"/>
+      <c r="E3" s="97"/>
+      <c r="F3" s="97"/>
+      <c r="G3" s="97"/>
+      <c r="H3" s="97"/>
+      <c r="I3" s="97"/>
       <c r="L3" s="83"/>
       <c r="M3" s="83"/>
       <c r="N3" s="83"/>
@@ -4512,26 +4532,26 @@
       </c>
     </row>
     <row r="2" spans="2:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="95"/>
-      <c r="C2" s="95"/>
-      <c r="D2" s="95"/>
-      <c r="E2" s="95"/>
-      <c r="F2" s="95"/>
-      <c r="G2" s="95"/>
-      <c r="H2" s="95"/>
-      <c r="I2" s="95"/>
+      <c r="B2" s="96"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="96"/>
+      <c r="E2" s="96"/>
+      <c r="F2" s="96"/>
+      <c r="G2" s="96"/>
+      <c r="H2" s="96"/>
+      <c r="I2" s="96"/>
     </row>
     <row r="3" spans="2:9" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="96" t="s">
+      <c r="B3" s="97" t="s">
         <v>191</v>
       </c>
-      <c r="C3" s="96"/>
-      <c r="D3" s="96"/>
-      <c r="E3" s="96"/>
-      <c r="F3" s="96"/>
-      <c r="G3" s="96"/>
-      <c r="H3" s="96"/>
-      <c r="I3" s="96"/>
+      <c r="C3" s="97"/>
+      <c r="D3" s="97"/>
+      <c r="E3" s="97"/>
+      <c r="F3" s="97"/>
+      <c r="G3" s="97"/>
+      <c r="H3" s="97"/>
+      <c r="I3" s="97"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="89" t="s">
@@ -4607,30 +4627,30 @@
       </c>
     </row>
     <row r="2" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="95"/>
-      <c r="C2" s="95"/>
-      <c r="D2" s="95"/>
-      <c r="E2" s="95"/>
-      <c r="F2" s="95"/>
-      <c r="G2" s="95"/>
-      <c r="H2" s="95"/>
-      <c r="I2" s="95"/>
-      <c r="J2" s="95"/>
-      <c r="K2" s="95"/>
+      <c r="B2" s="96"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="96"/>
+      <c r="E2" s="96"/>
+      <c r="F2" s="96"/>
+      <c r="G2" s="96"/>
+      <c r="H2" s="96"/>
+      <c r="I2" s="96"/>
+      <c r="J2" s="96"/>
+      <c r="K2" s="96"/>
     </row>
     <row r="3" spans="2:11" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="96" t="s">
+      <c r="B3" s="97" t="s">
         <v>167</v>
       </c>
-      <c r="C3" s="96"/>
-      <c r="D3" s="96"/>
-      <c r="E3" s="96"/>
-      <c r="F3" s="96"/>
-      <c r="G3" s="96"/>
-      <c r="H3" s="96"/>
-      <c r="I3" s="96"/>
-      <c r="J3" s="96"/>
-      <c r="K3" s="96"/>
+      <c r="C3" s="97"/>
+      <c r="D3" s="97"/>
+      <c r="E3" s="97"/>
+      <c r="F3" s="97"/>
+      <c r="G3" s="97"/>
+      <c r="H3" s="97"/>
+      <c r="I3" s="97"/>
+      <c r="J3" s="97"/>
+      <c r="K3" s="97"/>
     </row>
     <row r="4" spans="2:11" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B4" s="85"/>
@@ -4645,14 +4665,14 @@
       <c r="K4" s="85"/>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="H5" s="99" t="s">
+      <c r="H5" s="100" t="s">
         <v>175</v>
       </c>
-      <c r="I5" s="100"/>
-      <c r="J5" s="99" t="s">
+      <c r="I5" s="101"/>
+      <c r="J5" s="100" t="s">
         <v>174</v>
       </c>
-      <c r="K5" s="100"/>
+      <c r="K5" s="101"/>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" s="86" t="s">
@@ -4734,37 +4754,37 @@
       <c r="Z1" s="38"/>
     </row>
     <row r="2" spans="2:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="95"/>
-      <c r="C2" s="95"/>
-      <c r="D2" s="95"/>
-      <c r="E2" s="95"/>
-      <c r="F2" s="95"/>
-      <c r="G2" s="95"/>
-      <c r="H2" s="95"/>
-      <c r="I2" s="95"/>
-      <c r="J2" s="95"/>
-      <c r="K2" s="95"/>
-      <c r="L2" s="95"/>
-      <c r="M2" s="95"/>
-      <c r="N2" s="95"/>
+      <c r="B2" s="96"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="96"/>
+      <c r="E2" s="96"/>
+      <c r="F2" s="96"/>
+      <c r="G2" s="96"/>
+      <c r="H2" s="96"/>
+      <c r="I2" s="96"/>
+      <c r="J2" s="96"/>
+      <c r="K2" s="96"/>
+      <c r="L2" s="96"/>
+      <c r="M2" s="96"/>
+      <c r="N2" s="96"/>
       <c r="Z2"/>
     </row>
     <row r="3" spans="2:26" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="96" t="s">
+      <c r="B3" s="97" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="96"/>
-      <c r="D3" s="96"/>
-      <c r="E3" s="96"/>
-      <c r="F3" s="96"/>
-      <c r="G3" s="96"/>
-      <c r="H3" s="96"/>
-      <c r="I3" s="96"/>
-      <c r="J3" s="96"/>
-      <c r="K3" s="96"/>
-      <c r="L3" s="96"/>
-      <c r="M3" s="96"/>
-      <c r="N3" s="96"/>
+      <c r="C3" s="97"/>
+      <c r="D3" s="97"/>
+      <c r="E3" s="97"/>
+      <c r="F3" s="97"/>
+      <c r="G3" s="97"/>
+      <c r="H3" s="97"/>
+      <c r="I3" s="97"/>
+      <c r="J3" s="97"/>
+      <c r="K3" s="97"/>
+      <c r="L3" s="97"/>
+      <c r="M3" s="97"/>
+      <c r="N3" s="97"/>
       <c r="Z3"/>
     </row>
     <row r="5" spans="2:26" x14ac:dyDescent="0.25">
@@ -4868,37 +4888,37 @@
       <c r="Z1" s="38"/>
     </row>
     <row r="2" spans="2:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="95"/>
-      <c r="C2" s="95"/>
-      <c r="D2" s="95"/>
-      <c r="E2" s="95"/>
-      <c r="F2" s="95"/>
-      <c r="G2" s="95"/>
-      <c r="H2" s="95"/>
-      <c r="I2" s="95"/>
-      <c r="J2" s="95"/>
-      <c r="K2" s="95"/>
-      <c r="L2" s="95"/>
-      <c r="M2" s="95"/>
-      <c r="N2" s="95"/>
+      <c r="B2" s="96"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="96"/>
+      <c r="E2" s="96"/>
+      <c r="F2" s="96"/>
+      <c r="G2" s="96"/>
+      <c r="H2" s="96"/>
+      <c r="I2" s="96"/>
+      <c r="J2" s="96"/>
+      <c r="K2" s="96"/>
+      <c r="L2" s="96"/>
+      <c r="M2" s="96"/>
+      <c r="N2" s="96"/>
       <c r="Z2"/>
     </row>
     <row r="3" spans="2:26" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="96" t="s">
+      <c r="B3" s="97" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="96"/>
-      <c r="D3" s="96"/>
-      <c r="E3" s="96"/>
-      <c r="F3" s="96"/>
-      <c r="G3" s="96"/>
-      <c r="H3" s="96"/>
-      <c r="I3" s="96"/>
-      <c r="J3" s="96"/>
-      <c r="K3" s="96"/>
-      <c r="L3" s="96"/>
-      <c r="M3" s="96"/>
-      <c r="N3" s="96"/>
+      <c r="C3" s="97"/>
+      <c r="D3" s="97"/>
+      <c r="E3" s="97"/>
+      <c r="F3" s="97"/>
+      <c r="G3" s="97"/>
+      <c r="H3" s="97"/>
+      <c r="I3" s="97"/>
+      <c r="J3" s="97"/>
+      <c r="K3" s="97"/>
+      <c r="L3" s="97"/>
+      <c r="M3" s="97"/>
+      <c r="N3" s="97"/>
       <c r="Z3"/>
     </row>
     <row r="5" spans="2:26" x14ac:dyDescent="0.25">
@@ -4917,9 +4937,9 @@
       <c r="C6" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="D6" s="101"/>
-      <c r="E6" s="102"/>
-      <c r="F6" s="103"/>
+      <c r="D6" s="102"/>
+      <c r="E6" s="103"/>
+      <c r="F6" s="104"/>
       <c r="G6" s="50"/>
       <c r="H6" s="50"/>
     </row>
@@ -4997,37 +5017,37 @@
       <c r="Z1" s="38"/>
     </row>
     <row r="2" spans="2:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="95"/>
-      <c r="C2" s="95"/>
-      <c r="D2" s="95"/>
-      <c r="E2" s="95"/>
-      <c r="F2" s="95"/>
-      <c r="G2" s="95"/>
-      <c r="H2" s="95"/>
-      <c r="I2" s="95"/>
-      <c r="J2" s="95"/>
-      <c r="K2" s="95"/>
-      <c r="L2" s="95"/>
-      <c r="M2" s="95"/>
-      <c r="N2" s="95"/>
+      <c r="B2" s="96"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="96"/>
+      <c r="E2" s="96"/>
+      <c r="F2" s="96"/>
+      <c r="G2" s="96"/>
+      <c r="H2" s="96"/>
+      <c r="I2" s="96"/>
+      <c r="J2" s="96"/>
+      <c r="K2" s="96"/>
+      <c r="L2" s="96"/>
+      <c r="M2" s="96"/>
+      <c r="N2" s="96"/>
       <c r="Z2"/>
     </row>
     <row r="3" spans="2:26" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="96" t="s">
+      <c r="B3" s="97" t="s">
         <v>92</v>
       </c>
-      <c r="C3" s="96"/>
-      <c r="D3" s="96"/>
-      <c r="E3" s="96"/>
-      <c r="F3" s="96"/>
-      <c r="G3" s="96"/>
-      <c r="H3" s="96"/>
-      <c r="I3" s="96"/>
-      <c r="J3" s="96"/>
-      <c r="K3" s="96"/>
-      <c r="L3" s="96"/>
-      <c r="M3" s="96"/>
-      <c r="N3" s="96"/>
+      <c r="C3" s="97"/>
+      <c r="D3" s="97"/>
+      <c r="E3" s="97"/>
+      <c r="F3" s="97"/>
+      <c r="G3" s="97"/>
+      <c r="H3" s="97"/>
+      <c r="I3" s="97"/>
+      <c r="J3" s="97"/>
+      <c r="K3" s="97"/>
+      <c r="L3" s="97"/>
+      <c r="M3" s="97"/>
+      <c r="N3" s="97"/>
       <c r="Z3"/>
     </row>
     <row r="5" spans="2:26" x14ac:dyDescent="0.25">
@@ -5120,37 +5140,37 @@
       <c r="Z1" s="38"/>
     </row>
     <row r="2" spans="2:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="95"/>
-      <c r="C2" s="95"/>
-      <c r="D2" s="95"/>
-      <c r="E2" s="95"/>
-      <c r="F2" s="95"/>
-      <c r="G2" s="95"/>
-      <c r="H2" s="95"/>
-      <c r="I2" s="95"/>
-      <c r="J2" s="95"/>
-      <c r="K2" s="95"/>
-      <c r="L2" s="95"/>
-      <c r="M2" s="95"/>
-      <c r="N2" s="95"/>
+      <c r="B2" s="96"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="96"/>
+      <c r="E2" s="96"/>
+      <c r="F2" s="96"/>
+      <c r="G2" s="96"/>
+      <c r="H2" s="96"/>
+      <c r="I2" s="96"/>
+      <c r="J2" s="96"/>
+      <c r="K2" s="96"/>
+      <c r="L2" s="96"/>
+      <c r="M2" s="96"/>
+      <c r="N2" s="96"/>
       <c r="Z2"/>
     </row>
     <row r="3" spans="2:26" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="96" t="s">
+      <c r="B3" s="97" t="s">
         <v>72</v>
       </c>
-      <c r="C3" s="96"/>
-      <c r="D3" s="96"/>
-      <c r="E3" s="96"/>
-      <c r="F3" s="96"/>
-      <c r="G3" s="96"/>
-      <c r="H3" s="96"/>
-      <c r="I3" s="96"/>
-      <c r="J3" s="96"/>
-      <c r="K3" s="96"/>
-      <c r="L3" s="96"/>
-      <c r="M3" s="96"/>
-      <c r="N3" s="96"/>
+      <c r="C3" s="97"/>
+      <c r="D3" s="97"/>
+      <c r="E3" s="97"/>
+      <c r="F3" s="97"/>
+      <c r="G3" s="97"/>
+      <c r="H3" s="97"/>
+      <c r="I3" s="97"/>
+      <c r="J3" s="97"/>
+      <c r="K3" s="97"/>
+      <c r="L3" s="97"/>
+      <c r="M3" s="97"/>
+      <c r="N3" s="97"/>
       <c r="Z3"/>
     </row>
     <row r="5" spans="2:26" x14ac:dyDescent="0.25">
@@ -5263,56 +5283,56 @@
       </c>
     </row>
     <row r="2" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="95"/>
-      <c r="C2" s="95"/>
-      <c r="D2" s="95"/>
-      <c r="E2" s="95"/>
-      <c r="F2" s="95"/>
-      <c r="G2" s="95"/>
-      <c r="H2" s="95"/>
-      <c r="I2" s="95"/>
-      <c r="J2" s="95"/>
-      <c r="K2" s="95"/>
-      <c r="L2" s="95"/>
+      <c r="B2" s="96"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="96"/>
+      <c r="E2" s="96"/>
+      <c r="F2" s="96"/>
+      <c r="G2" s="96"/>
+      <c r="H2" s="96"/>
+      <c r="I2" s="96"/>
+      <c r="J2" s="96"/>
+      <c r="K2" s="96"/>
+      <c r="L2" s="96"/>
     </row>
     <row r="3" spans="2:17" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="96" t="s">
+      <c r="B3" s="97" t="s">
         <v>107</v>
       </c>
-      <c r="C3" s="96"/>
-      <c r="D3" s="96"/>
-      <c r="E3" s="96"/>
-      <c r="F3" s="96"/>
-      <c r="G3" s="96"/>
-      <c r="H3" s="96"/>
-      <c r="I3" s="96"/>
-      <c r="J3" s="96"/>
-      <c r="K3" s="96"/>
-      <c r="L3" s="96"/>
+      <c r="C3" s="97"/>
+      <c r="D3" s="97"/>
+      <c r="E3" s="97"/>
+      <c r="F3" s="97"/>
+      <c r="G3" s="97"/>
+      <c r="H3" s="97"/>
+      <c r="I3" s="97"/>
+      <c r="J3" s="97"/>
+      <c r="K3" s="97"/>
+      <c r="L3" s="97"/>
     </row>
     <row r="5" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D5" s="104" t="s">
+      <c r="D5" s="105" t="s">
         <v>122</v>
       </c>
-      <c r="E5" s="104"/>
+      <c r="E5" s="105"/>
       <c r="F5" s="73"/>
       <c r="G5" s="73"/>
       <c r="H5" s="73"/>
       <c r="I5" s="73"/>
-      <c r="J5" s="104" t="s">
+      <c r="J5" s="105" t="s">
         <v>42</v>
       </c>
-      <c r="K5" s="104"/>
-      <c r="L5" s="104"/>
-      <c r="M5" s="104" t="s">
+      <c r="K5" s="105"/>
+      <c r="L5" s="105"/>
+      <c r="M5" s="105" t="s">
         <v>129</v>
       </c>
-      <c r="N5" s="104"/>
-      <c r="O5" s="104"/>
-      <c r="P5" s="98" t="s">
+      <c r="N5" s="105"/>
+      <c r="O5" s="105"/>
+      <c r="P5" s="99" t="s">
         <v>108</v>
       </c>
-      <c r="Q5" s="98"/>
+      <c r="Q5" s="99"/>
     </row>
     <row r="6" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="70" t="s">
@@ -5422,36 +5442,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="95"/>
-      <c r="C2" s="95"/>
-      <c r="D2" s="95"/>
-      <c r="E2" s="95"/>
-      <c r="F2" s="95"/>
-      <c r="G2" s="95"/>
-      <c r="H2" s="95"/>
-      <c r="I2" s="95"/>
-      <c r="J2" s="95"/>
-      <c r="K2" s="95"/>
-      <c r="L2" s="95"/>
-      <c r="M2" s="95"/>
-      <c r="N2" s="95"/>
+      <c r="B2" s="96"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="96"/>
+      <c r="E2" s="96"/>
+      <c r="F2" s="96"/>
+      <c r="G2" s="96"/>
+      <c r="H2" s="96"/>
+      <c r="I2" s="96"/>
+      <c r="J2" s="96"/>
+      <c r="K2" s="96"/>
+      <c r="L2" s="96"/>
+      <c r="M2" s="96"/>
+      <c r="N2" s="96"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="96" t="s">
+      <c r="B3" s="97" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="96"/>
-      <c r="D3" s="96"/>
-      <c r="E3" s="96"/>
-      <c r="F3" s="96"/>
-      <c r="G3" s="96"/>
-      <c r="H3" s="96"/>
-      <c r="I3" s="96"/>
-      <c r="J3" s="96"/>
-      <c r="K3" s="96"/>
-      <c r="L3" s="96"/>
-      <c r="M3" s="96"/>
-      <c r="N3" s="96"/>
+      <c r="C3" s="97"/>
+      <c r="D3" s="97"/>
+      <c r="E3" s="97"/>
+      <c r="F3" s="97"/>
+      <c r="G3" s="97"/>
+      <c r="H3" s="97"/>
+      <c r="I3" s="97"/>
+      <c r="J3" s="97"/>
+      <c r="K3" s="97"/>
+      <c r="L3" s="97"/>
+      <c r="M3" s="97"/>
+      <c r="N3" s="97"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="44" t="s">
@@ -5533,110 +5553,110 @@
       </c>
     </row>
     <row r="2" spans="2:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="95"/>
-      <c r="C2" s="95"/>
-      <c r="D2" s="95"/>
-      <c r="E2" s="95"/>
-      <c r="F2" s="95"/>
-      <c r="G2" s="95"/>
-      <c r="H2" s="95"/>
-      <c r="I2" s="95"/>
-      <c r="J2" s="95"/>
-      <c r="K2" s="95"/>
-      <c r="L2" s="95"/>
-      <c r="M2" s="95"/>
-      <c r="N2" s="95"/>
-      <c r="O2" s="95"/>
-      <c r="P2" s="95"/>
+      <c r="B2" s="96"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="96"/>
+      <c r="E2" s="96"/>
+      <c r="F2" s="96"/>
+      <c r="G2" s="96"/>
+      <c r="H2" s="96"/>
+      <c r="I2" s="96"/>
+      <c r="J2" s="96"/>
+      <c r="K2" s="96"/>
+      <c r="L2" s="96"/>
+      <c r="M2" s="96"/>
+      <c r="N2" s="96"/>
+      <c r="O2" s="96"/>
+      <c r="P2" s="96"/>
       <c r="Q2" s="56"/>
       <c r="R2" s="56"/>
     </row>
     <row r="3" spans="2:25" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="96" t="s">
+      <c r="B3" s="97" t="s">
         <v>110</v>
       </c>
-      <c r="C3" s="96"/>
-      <c r="D3" s="96"/>
-      <c r="E3" s="96"/>
-      <c r="F3" s="96"/>
-      <c r="G3" s="96"/>
-      <c r="H3" s="96"/>
-      <c r="I3" s="96"/>
-      <c r="J3" s="96"/>
-      <c r="K3" s="96"/>
-      <c r="L3" s="96"/>
-      <c r="M3" s="96"/>
-      <c r="N3" s="96"/>
-      <c r="O3" s="96"/>
-      <c r="P3" s="96"/>
+      <c r="C3" s="97"/>
+      <c r="D3" s="97"/>
+      <c r="E3" s="97"/>
+      <c r="F3" s="97"/>
+      <c r="G3" s="97"/>
+      <c r="H3" s="97"/>
+      <c r="I3" s="97"/>
+      <c r="J3" s="97"/>
+      <c r="K3" s="97"/>
+      <c r="L3" s="97"/>
+      <c r="M3" s="97"/>
+      <c r="N3" s="97"/>
+      <c r="O3" s="97"/>
+      <c r="P3" s="97"/>
       <c r="Q3" s="57"/>
       <c r="R3" s="57"/>
     </row>
     <row r="5" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B5" s="108" t="s">
+      <c r="B5" s="110" t="s">
         <v>111</v>
       </c>
-      <c r="C5" s="109"/>
-      <c r="D5" s="109"/>
-      <c r="E5" s="109"/>
-      <c r="F5" s="109"/>
-      <c r="G5" s="109"/>
-      <c r="H5" s="109"/>
-      <c r="I5" s="109"/>
-      <c r="J5" s="109"/>
-      <c r="K5" s="109"/>
-      <c r="L5" s="110"/>
-      <c r="M5" s="108" t="s">
+      <c r="C5" s="111"/>
+      <c r="D5" s="111"/>
+      <c r="E5" s="111"/>
+      <c r="F5" s="111"/>
+      <c r="G5" s="111"/>
+      <c r="H5" s="111"/>
+      <c r="I5" s="111"/>
+      <c r="J5" s="111"/>
+      <c r="K5" s="111"/>
+      <c r="L5" s="112"/>
+      <c r="M5" s="110" t="s">
         <v>112</v>
       </c>
-      <c r="N5" s="109"/>
-      <c r="O5" s="109"/>
-      <c r="P5" s="109"/>
-      <c r="Q5" s="109"/>
-      <c r="R5" s="109"/>
-      <c r="S5" s="109"/>
-      <c r="T5" s="109"/>
-      <c r="U5" s="109"/>
-      <c r="V5" s="109"/>
-      <c r="W5" s="109"/>
-      <c r="X5" s="109"/>
-      <c r="Y5" s="110"/>
+      <c r="N5" s="111"/>
+      <c r="O5" s="111"/>
+      <c r="P5" s="111"/>
+      <c r="Q5" s="111"/>
+      <c r="R5" s="111"/>
+      <c r="S5" s="111"/>
+      <c r="T5" s="111"/>
+      <c r="U5" s="111"/>
+      <c r="V5" s="111"/>
+      <c r="W5" s="111"/>
+      <c r="X5" s="111"/>
+      <c r="Y5" s="112"/>
     </row>
     <row r="6" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B6" s="105"/>
-      <c r="C6" s="105"/>
-      <c r="D6" s="105"/>
-      <c r="E6" s="105"/>
-      <c r="F6" s="114" t="s">
+      <c r="B6" s="109"/>
+      <c r="C6" s="109"/>
+      <c r="D6" s="109"/>
+      <c r="E6" s="109"/>
+      <c r="F6" s="116" t="s">
         <v>27</v>
       </c>
-      <c r="G6" s="115"/>
-      <c r="H6" s="115"/>
-      <c r="I6" s="116"/>
-      <c r="J6" s="108" t="s">
+      <c r="G6" s="117"/>
+      <c r="H6" s="117"/>
+      <c r="I6" s="118"/>
+      <c r="J6" s="110" t="s">
         <v>30</v>
       </c>
-      <c r="K6" s="109"/>
-      <c r="L6" s="110"/>
+      <c r="K6" s="111"/>
+      <c r="L6" s="112"/>
       <c r="M6" s="88"/>
       <c r="N6" s="106" t="s">
         <v>42</v>
       </c>
-      <c r="O6" s="107"/>
+      <c r="O6" s="108"/>
       <c r="P6" s="106" t="s">
         <v>105</v>
       </c>
-      <c r="Q6" s="117"/>
-      <c r="R6" s="107"/>
+      <c r="Q6" s="107"/>
+      <c r="R6" s="108"/>
       <c r="S6" s="88"/>
       <c r="T6" s="106" t="s">
         <v>122</v>
       </c>
-      <c r="U6" s="107"/>
-      <c r="V6" s="111"/>
-      <c r="W6" s="112"/>
-      <c r="X6" s="112"/>
-      <c r="Y6" s="113"/>
+      <c r="U6" s="108"/>
+      <c r="V6" s="113"/>
+      <c r="W6" s="114"/>
+      <c r="X6" s="114"/>
+      <c r="Y6" s="115"/>
     </row>
     <row r="7" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B7" s="75" t="s">
@@ -5740,6 +5760,7 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="N6:O6"/>
     <mergeCell ref="P6:R6"/>
     <mergeCell ref="B6:E6"/>
     <mergeCell ref="T6:U6"/>
@@ -5750,7 +5771,6 @@
     <mergeCell ref="B5:L5"/>
     <mergeCell ref="J6:L6"/>
     <mergeCell ref="F6:I6"/>
-    <mergeCell ref="N6:O6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -5871,40 +5891,40 @@
       </c>
     </row>
     <row r="2" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="95"/>
-      <c r="C2" s="95"/>
-      <c r="D2" s="95"/>
-      <c r="E2" s="95"/>
-      <c r="F2" s="95"/>
-      <c r="G2" s="95"/>
-      <c r="H2" s="95"/>
-      <c r="I2" s="95"/>
-      <c r="J2" s="95"/>
-      <c r="K2" s="95"/>
-      <c r="L2" s="95"/>
-      <c r="M2" s="95"/>
-      <c r="N2" s="95"/>
-      <c r="O2" s="95"/>
-      <c r="P2" s="95"/>
+      <c r="B2" s="96"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="96"/>
+      <c r="E2" s="96"/>
+      <c r="F2" s="96"/>
+      <c r="G2" s="96"/>
+      <c r="H2" s="96"/>
+      <c r="I2" s="96"/>
+      <c r="J2" s="96"/>
+      <c r="K2" s="96"/>
+      <c r="L2" s="96"/>
+      <c r="M2" s="96"/>
+      <c r="N2" s="96"/>
+      <c r="O2" s="96"/>
+      <c r="P2" s="96"/>
     </row>
     <row r="3" spans="2:16" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="96" t="s">
+      <c r="B3" s="97" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="96"/>
-      <c r="D3" s="96"/>
-      <c r="E3" s="96"/>
-      <c r="F3" s="96"/>
-      <c r="G3" s="96"/>
-      <c r="H3" s="96"/>
-      <c r="I3" s="96"/>
-      <c r="J3" s="96"/>
-      <c r="K3" s="96"/>
-      <c r="L3" s="96"/>
-      <c r="M3" s="96"/>
-      <c r="N3" s="96"/>
-      <c r="O3" s="96"/>
-      <c r="P3" s="96"/>
+      <c r="C3" s="97"/>
+      <c r="D3" s="97"/>
+      <c r="E3" s="97"/>
+      <c r="F3" s="97"/>
+      <c r="G3" s="97"/>
+      <c r="H3" s="97"/>
+      <c r="I3" s="97"/>
+      <c r="J3" s="97"/>
+      <c r="K3" s="97"/>
+      <c r="L3" s="97"/>
+      <c r="M3" s="97"/>
+      <c r="N3" s="97"/>
+      <c r="O3" s="97"/>
+      <c r="P3" s="97"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="44" t="s">
@@ -5983,40 +6003,40 @@
       </c>
     </row>
     <row r="2" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="95"/>
-      <c r="C2" s="95"/>
-      <c r="D2" s="95"/>
-      <c r="E2" s="95"/>
-      <c r="F2" s="95"/>
-      <c r="G2" s="95"/>
-      <c r="H2" s="95"/>
-      <c r="I2" s="95"/>
-      <c r="J2" s="95"/>
-      <c r="K2" s="95"/>
-      <c r="L2" s="95"/>
-      <c r="M2" s="95"/>
-      <c r="N2" s="95"/>
-      <c r="O2" s="95"/>
-      <c r="P2" s="95"/>
+      <c r="B2" s="96"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="96"/>
+      <c r="E2" s="96"/>
+      <c r="F2" s="96"/>
+      <c r="G2" s="96"/>
+      <c r="H2" s="96"/>
+      <c r="I2" s="96"/>
+      <c r="J2" s="96"/>
+      <c r="K2" s="96"/>
+      <c r="L2" s="96"/>
+      <c r="M2" s="96"/>
+      <c r="N2" s="96"/>
+      <c r="O2" s="96"/>
+      <c r="P2" s="96"/>
     </row>
     <row r="3" spans="2:16" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="96" t="s">
+      <c r="B3" s="97" t="s">
         <v>68</v>
       </c>
-      <c r="C3" s="96"/>
-      <c r="D3" s="96"/>
-      <c r="E3" s="96"/>
-      <c r="F3" s="96"/>
-      <c r="G3" s="96"/>
-      <c r="H3" s="96"/>
-      <c r="I3" s="96"/>
-      <c r="J3" s="96"/>
-      <c r="K3" s="96"/>
-      <c r="L3" s="96"/>
-      <c r="M3" s="96"/>
-      <c r="N3" s="96"/>
-      <c r="O3" s="96"/>
-      <c r="P3" s="96"/>
+      <c r="C3" s="97"/>
+      <c r="D3" s="97"/>
+      <c r="E3" s="97"/>
+      <c r="F3" s="97"/>
+      <c r="G3" s="97"/>
+      <c r="H3" s="97"/>
+      <c r="I3" s="97"/>
+      <c r="J3" s="97"/>
+      <c r="K3" s="97"/>
+      <c r="L3" s="97"/>
+      <c r="M3" s="97"/>
+      <c r="N3" s="97"/>
+      <c r="O3" s="97"/>
+      <c r="P3" s="97"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
@@ -6065,40 +6085,40 @@
       </c>
     </row>
     <row r="2" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="95"/>
-      <c r="C2" s="95"/>
-      <c r="D2" s="95"/>
-      <c r="E2" s="95"/>
-      <c r="F2" s="95"/>
-      <c r="G2" s="95"/>
-      <c r="H2" s="95"/>
-      <c r="I2" s="95"/>
-      <c r="J2" s="95"/>
-      <c r="K2" s="95"/>
-      <c r="L2" s="95"/>
-      <c r="M2" s="95"/>
-      <c r="N2" s="95"/>
-      <c r="O2" s="95"/>
-      <c r="P2" s="95"/>
+      <c r="B2" s="96"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="96"/>
+      <c r="E2" s="96"/>
+      <c r="F2" s="96"/>
+      <c r="G2" s="96"/>
+      <c r="H2" s="96"/>
+      <c r="I2" s="96"/>
+      <c r="J2" s="96"/>
+      <c r="K2" s="96"/>
+      <c r="L2" s="96"/>
+      <c r="M2" s="96"/>
+      <c r="N2" s="96"/>
+      <c r="O2" s="96"/>
+      <c r="P2" s="96"/>
     </row>
     <row r="3" spans="2:16" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="96" t="s">
+      <c r="B3" s="97" t="s">
         <v>71</v>
       </c>
-      <c r="C3" s="96"/>
-      <c r="D3" s="96"/>
-      <c r="E3" s="96"/>
-      <c r="F3" s="96"/>
-      <c r="G3" s="96"/>
-      <c r="H3" s="96"/>
-      <c r="I3" s="96"/>
-      <c r="J3" s="96"/>
-      <c r="K3" s="96"/>
-      <c r="L3" s="96"/>
-      <c r="M3" s="96"/>
-      <c r="N3" s="96"/>
-      <c r="O3" s="96"/>
-      <c r="P3" s="96"/>
+      <c r="C3" s="97"/>
+      <c r="D3" s="97"/>
+      <c r="E3" s="97"/>
+      <c r="F3" s="97"/>
+      <c r="G3" s="97"/>
+      <c r="H3" s="97"/>
+      <c r="I3" s="97"/>
+      <c r="J3" s="97"/>
+      <c r="K3" s="97"/>
+      <c r="L3" s="97"/>
+      <c r="M3" s="97"/>
+      <c r="N3" s="97"/>
+      <c r="O3" s="97"/>
+      <c r="P3" s="97"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
@@ -6126,7 +6146,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:P6"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
@@ -6153,40 +6173,40 @@
       </c>
     </row>
     <row r="2" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="95"/>
-      <c r="C2" s="95"/>
-      <c r="D2" s="95"/>
-      <c r="E2" s="95"/>
-      <c r="F2" s="95"/>
-      <c r="G2" s="95"/>
-      <c r="H2" s="95"/>
-      <c r="I2" s="95"/>
-      <c r="J2" s="95"/>
-      <c r="K2" s="95"/>
-      <c r="L2" s="95"/>
-      <c r="M2" s="95"/>
-      <c r="N2" s="95"/>
-      <c r="O2" s="95"/>
-      <c r="P2" s="95"/>
+      <c r="B2" s="96"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="96"/>
+      <c r="E2" s="96"/>
+      <c r="F2" s="96"/>
+      <c r="G2" s="96"/>
+      <c r="H2" s="96"/>
+      <c r="I2" s="96"/>
+      <c r="J2" s="96"/>
+      <c r="K2" s="96"/>
+      <c r="L2" s="96"/>
+      <c r="M2" s="96"/>
+      <c r="N2" s="96"/>
+      <c r="O2" s="96"/>
+      <c r="P2" s="96"/>
     </row>
     <row r="3" spans="2:16" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="96" t="s">
+      <c r="B3" s="97" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="96"/>
-      <c r="D3" s="96"/>
-      <c r="E3" s="96"/>
-      <c r="F3" s="96"/>
-      <c r="G3" s="96"/>
-      <c r="H3" s="96"/>
-      <c r="I3" s="96"/>
-      <c r="J3" s="96"/>
-      <c r="K3" s="96"/>
-      <c r="L3" s="96"/>
-      <c r="M3" s="96"/>
-      <c r="N3" s="96"/>
-      <c r="O3" s="96"/>
-      <c r="P3" s="96"/>
+      <c r="C3" s="97"/>
+      <c r="D3" s="97"/>
+      <c r="E3" s="97"/>
+      <c r="F3" s="97"/>
+      <c r="G3" s="97"/>
+      <c r="H3" s="97"/>
+      <c r="I3" s="97"/>
+      <c r="J3" s="97"/>
+      <c r="K3" s="97"/>
+      <c r="L3" s="97"/>
+      <c r="M3" s="97"/>
+      <c r="N3" s="97"/>
+      <c r="O3" s="97"/>
+      <c r="P3" s="97"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="44" t="s">
@@ -6283,40 +6303,40 @@
       </c>
     </row>
     <row r="2" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="95"/>
-      <c r="C2" s="95"/>
-      <c r="D2" s="95"/>
-      <c r="E2" s="95"/>
-      <c r="F2" s="95"/>
-      <c r="G2" s="95"/>
-      <c r="H2" s="95"/>
-      <c r="I2" s="95"/>
-      <c r="J2" s="95"/>
-      <c r="K2" s="95"/>
-      <c r="L2" s="95"/>
-      <c r="M2" s="95"/>
-      <c r="N2" s="95"/>
-      <c r="O2" s="95"/>
-      <c r="P2" s="95"/>
+      <c r="B2" s="96"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="96"/>
+      <c r="E2" s="96"/>
+      <c r="F2" s="96"/>
+      <c r="G2" s="96"/>
+      <c r="H2" s="96"/>
+      <c r="I2" s="96"/>
+      <c r="J2" s="96"/>
+      <c r="K2" s="96"/>
+      <c r="L2" s="96"/>
+      <c r="M2" s="96"/>
+      <c r="N2" s="96"/>
+      <c r="O2" s="96"/>
+      <c r="P2" s="96"/>
     </row>
     <row r="3" spans="2:16" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="96" t="s">
+      <c r="B3" s="97" t="s">
         <v>65</v>
       </c>
-      <c r="C3" s="96"/>
-      <c r="D3" s="96"/>
-      <c r="E3" s="96"/>
-      <c r="F3" s="96"/>
-      <c r="G3" s="96"/>
-      <c r="H3" s="96"/>
-      <c r="I3" s="96"/>
-      <c r="J3" s="96"/>
-      <c r="K3" s="96"/>
-      <c r="L3" s="96"/>
-      <c r="M3" s="96"/>
-      <c r="N3" s="96"/>
-      <c r="O3" s="96"/>
-      <c r="P3" s="96"/>
+      <c r="C3" s="97"/>
+      <c r="D3" s="97"/>
+      <c r="E3" s="97"/>
+      <c r="F3" s="97"/>
+      <c r="G3" s="97"/>
+      <c r="H3" s="97"/>
+      <c r="I3" s="97"/>
+      <c r="J3" s="97"/>
+      <c r="K3" s="97"/>
+      <c r="L3" s="97"/>
+      <c r="M3" s="97"/>
+      <c r="N3" s="97"/>
+      <c r="O3" s="97"/>
+      <c r="P3" s="97"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="45" t="s">
@@ -6371,28 +6391,28 @@
       </c>
     </row>
     <row r="2" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="97"/>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="97"/>
+      <c r="B2" s="98"/>
+      <c r="C2" s="98"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
+      <c r="F2" s="98"/>
+      <c r="G2" s="98"/>
+      <c r="H2" s="98"/>
+      <c r="I2" s="98"/>
       <c r="J2" s="84"/>
       <c r="K2" s="84"/>
     </row>
     <row r="3" spans="2:11" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="96" t="s">
+      <c r="B3" s="97" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="96"/>
-      <c r="D3" s="96"/>
-      <c r="E3" s="96"/>
-      <c r="F3" s="96"/>
-      <c r="G3" s="96"/>
-      <c r="H3" s="96"/>
-      <c r="I3" s="96"/>
+      <c r="C3" s="97"/>
+      <c r="D3" s="97"/>
+      <c r="E3" s="97"/>
+      <c r="F3" s="97"/>
+      <c r="G3" s="97"/>
+      <c r="H3" s="97"/>
+      <c r="I3" s="97"/>
       <c r="J3" s="83"/>
       <c r="K3" s="83"/>
     </row>

</xml_diff>

<commit_message>
Trieda-1701 - Adicionando campos Capacidade maxima e custo de operação por credito em salas. Alterando campo Capacidade para Capacidade Instalada. Adicionando parametro de considerar capacidade maxima das salas. Criando script para atualizaro BD.
</commit_message>
<xml_diff>
--- a/code/client/web/src/main/resources/templateExport.xlsx
+++ b/code/client/web/src/main/resources/templateExport.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="17070" windowHeight="5370" tabRatio="907" firstSheet="3" activeTab="13"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="17070" windowHeight="5370" tabRatio="907" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Campi" sheetId="3" r:id="rId1"/>
@@ -1262,7 +1262,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="198">
   <si>
     <t>Planilha de Unidades</t>
   </si>
@@ -1498,9 +1498,6 @@
     <t>Código Sala</t>
   </si>
   <si>
-    <t>Capacidade (alunos)</t>
-  </si>
-  <si>
     <t>Código Curso</t>
   </si>
   <si>
@@ -1850,6 +1847,15 @@
   </si>
   <si>
     <t>Min. Creditos Diários</t>
+  </si>
+  <si>
+    <t>Capacidade Instalada (alunos)</t>
+  </si>
+  <si>
+    <t>Capacidade Máxima (alunos)</t>
+  </si>
+  <si>
+    <t>Custo de Operação por Crédito (R$)</t>
   </si>
 </sst>
 </file>
@@ -2279,7 +2285,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="119">
+  <cellXfs count="120">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2550,6 +2556,9 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2583,10 +2592,10 @@
     <xf numFmtId="0" fontId="10" fillId="28" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="28" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="28" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2942,42 +2951,42 @@
   <sheetData>
     <row r="1" spans="2:14" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="97" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="96" t="s">
-        <v>95</v>
-      </c>
-      <c r="C2" s="96"/>
-      <c r="D2" s="96"/>
-      <c r="E2" s="96"/>
-      <c r="F2" s="96"/>
-      <c r="G2" s="96"/>
-      <c r="H2" s="96"/>
-      <c r="I2" s="96"/>
-      <c r="J2" s="96"/>
-      <c r="K2" s="96"/>
-      <c r="L2" s="96"/>
-      <c r="M2" s="96"/>
-      <c r="N2" s="96"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
+      <c r="F2" s="97"/>
+      <c r="G2" s="97"/>
+      <c r="H2" s="97"/>
+      <c r="I2" s="97"/>
+      <c r="J2" s="97"/>
+      <c r="K2" s="97"/>
+      <c r="L2" s="97"/>
+      <c r="M2" s="97"/>
+      <c r="N2" s="97"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="97" t="s">
+      <c r="B3" s="98" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="97"/>
-      <c r="D3" s="97"/>
-      <c r="E3" s="97"/>
-      <c r="F3" s="97"/>
-      <c r="G3" s="97"/>
-      <c r="H3" s="97"/>
-      <c r="I3" s="97"/>
-      <c r="J3" s="97"/>
-      <c r="K3" s="97"/>
-      <c r="L3" s="97"/>
-      <c r="M3" s="97"/>
-      <c r="N3" s="97"/>
+      <c r="C3" s="98"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="98"/>
+      <c r="F3" s="98"/>
+      <c r="G3" s="98"/>
+      <c r="H3" s="98"/>
+      <c r="I3" s="98"/>
+      <c r="J3" s="98"/>
+      <c r="K3" s="98"/>
+      <c r="L3" s="98"/>
+      <c r="M3" s="98"/>
+      <c r="N3" s="98"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="44" t="s">
@@ -3041,50 +3050,50 @@
   <sheetData>
     <row r="1" spans="2:14" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="96"/>
-      <c r="C2" s="96"/>
-      <c r="D2" s="96"/>
-      <c r="E2" s="96"/>
-      <c r="F2" s="96"/>
-      <c r="G2" s="96"/>
-      <c r="H2" s="96"/>
-      <c r="I2" s="96"/>
-      <c r="J2" s="96"/>
-      <c r="K2" s="96"/>
-      <c r="L2" s="96"/>
-      <c r="M2" s="96"/>
-      <c r="N2" s="96"/>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
+      <c r="F2" s="97"/>
+      <c r="G2" s="97"/>
+      <c r="H2" s="97"/>
+      <c r="I2" s="97"/>
+      <c r="J2" s="97"/>
+      <c r="K2" s="97"/>
+      <c r="L2" s="97"/>
+      <c r="M2" s="97"/>
+      <c r="N2" s="97"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="97" t="s">
+      <c r="B3" s="98" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="97"/>
-      <c r="D3" s="97"/>
-      <c r="E3" s="97"/>
-      <c r="F3" s="97"/>
-      <c r="G3" s="97"/>
-      <c r="H3" s="97"/>
-      <c r="I3" s="97"/>
-      <c r="J3" s="97"/>
-      <c r="K3" s="97"/>
-      <c r="L3" s="97"/>
-      <c r="M3" s="97"/>
-      <c r="N3" s="97"/>
+      <c r="C3" s="98"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="98"/>
+      <c r="F3" s="98"/>
+      <c r="G3" s="98"/>
+      <c r="H3" s="98"/>
+      <c r="I3" s="98"/>
+      <c r="J3" s="98"/>
+      <c r="K3" s="98"/>
+      <c r="L3" s="98"/>
+      <c r="M3" s="98"/>
+      <c r="N3" s="98"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>88</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>89</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>26</v>
@@ -3093,7 +3102,7 @@
         <v>27</v>
       </c>
       <c r="G5" s="47" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
@@ -3139,40 +3148,40 @@
   <sheetData>
     <row r="1" spans="2:14" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="96"/>
-      <c r="C2" s="96"/>
-      <c r="D2" s="96"/>
-      <c r="E2" s="96"/>
-      <c r="F2" s="96"/>
-      <c r="G2" s="96"/>
-      <c r="H2" s="96"/>
-      <c r="I2" s="96"/>
-      <c r="J2" s="96"/>
-      <c r="K2" s="96"/>
-      <c r="L2" s="96"/>
-      <c r="M2" s="96"/>
-      <c r="N2" s="96"/>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
+      <c r="F2" s="97"/>
+      <c r="G2" s="97"/>
+      <c r="H2" s="97"/>
+      <c r="I2" s="97"/>
+      <c r="J2" s="97"/>
+      <c r="K2" s="97"/>
+      <c r="L2" s="97"/>
+      <c r="M2" s="97"/>
+      <c r="N2" s="97"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="97" t="s">
+      <c r="B3" s="98" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="97"/>
-      <c r="D3" s="97"/>
-      <c r="E3" s="97"/>
-      <c r="F3" s="97"/>
-      <c r="G3" s="97"/>
-      <c r="H3" s="97"/>
-      <c r="I3" s="97"/>
-      <c r="J3" s="97"/>
-      <c r="K3" s="97"/>
-      <c r="L3" s="97"/>
-      <c r="M3" s="97"/>
-      <c r="N3" s="97"/>
+      <c r="C3" s="98"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="98"/>
+      <c r="F3" s="98"/>
+      <c r="G3" s="98"/>
+      <c r="H3" s="98"/>
+      <c r="I3" s="98"/>
+      <c r="J3" s="98"/>
+      <c r="K3" s="98"/>
+      <c r="L3" s="98"/>
+      <c r="M3" s="98"/>
+      <c r="N3" s="98"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -3182,7 +3191,7 @@
         <v>28</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>29</v>
@@ -3191,7 +3200,7 @@
         <v>26</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H5" s="4" t="s">
         <v>30</v>
@@ -3200,16 +3209,16 @@
         <v>58</v>
       </c>
       <c r="J5" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="K5" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="K5" s="4" t="s">
-        <v>106</v>
-      </c>
       <c r="L5" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
@@ -3253,32 +3262,32 @@
   <sheetData>
     <row r="1" spans="2:5" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="96"/>
-      <c r="C2" s="96"/>
-      <c r="D2" s="96"/>
-      <c r="E2" s="96"/>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
     </row>
     <row r="3" spans="2:5" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="97" t="s">
-        <v>125</v>
-      </c>
-      <c r="C3" s="97"/>
-      <c r="D3" s="97"/>
-      <c r="E3" s="97"/>
+      <c r="B3" s="98" t="s">
+        <v>124</v>
+      </c>
+      <c r="C3" s="98"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="98"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="60" t="s">
+        <v>99</v>
+      </c>
+      <c r="C5" s="59" t="s">
         <v>100</v>
       </c>
-      <c r="C5" s="59" t="s">
-        <v>101</v>
-      </c>
       <c r="D5" s="59" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
@@ -3317,40 +3326,40 @@
   <sheetData>
     <row r="1" spans="2:14" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="96"/>
-      <c r="C2" s="96"/>
-      <c r="D2" s="96"/>
-      <c r="E2" s="96"/>
-      <c r="F2" s="96"/>
-      <c r="G2" s="96"/>
-      <c r="H2" s="96"/>
-      <c r="I2" s="96"/>
-      <c r="J2" s="96"/>
-      <c r="K2" s="96"/>
-      <c r="L2" s="96"/>
-      <c r="M2" s="96"/>
-      <c r="N2" s="96"/>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
+      <c r="F2" s="97"/>
+      <c r="G2" s="97"/>
+      <c r="H2" s="97"/>
+      <c r="I2" s="97"/>
+      <c r="J2" s="97"/>
+      <c r="K2" s="97"/>
+      <c r="L2" s="97"/>
+      <c r="M2" s="97"/>
+      <c r="N2" s="97"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="97" t="s">
-        <v>99</v>
-      </c>
-      <c r="C3" s="97"/>
-      <c r="D3" s="97"/>
-      <c r="E3" s="97"/>
-      <c r="F3" s="97"/>
-      <c r="G3" s="97"/>
-      <c r="H3" s="97"/>
-      <c r="I3" s="97"/>
-      <c r="J3" s="97"/>
-      <c r="K3" s="97"/>
-      <c r="L3" s="97"/>
-      <c r="M3" s="97"/>
-      <c r="N3" s="97"/>
+      <c r="B3" s="98" t="s">
+        <v>98</v>
+      </c>
+      <c r="C3" s="98"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="98"/>
+      <c r="F3" s="98"/>
+      <c r="G3" s="98"/>
+      <c r="H3" s="98"/>
+      <c r="I3" s="98"/>
+      <c r="J3" s="98"/>
+      <c r="K3" s="98"/>
+      <c r="L3" s="98"/>
+      <c r="M3" s="98"/>
+      <c r="N3" s="98"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -3360,7 +3369,7 @@
         <v>28</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>29</v>
@@ -3369,24 +3378,24 @@
         <v>26</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H5" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="I5" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="J5" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="J5" s="4" t="s">
+      <c r="K5" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="K5" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="L5" s="99" t="s">
-        <v>109</v>
-      </c>
-      <c r="M5" s="99"/>
+      <c r="L5" s="100" t="s">
+        <v>108</v>
+      </c>
+      <c r="M5" s="100"/>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
@@ -3414,8 +3423,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O6"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3437,49 +3446,49 @@
   <sheetData>
     <row r="1" spans="2:15" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="2:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="96"/>
-      <c r="C2" s="96"/>
-      <c r="D2" s="96"/>
-      <c r="E2" s="96"/>
-      <c r="F2" s="96"/>
-      <c r="G2" s="96"/>
-      <c r="H2" s="96"/>
-      <c r="I2" s="96"/>
-      <c r="J2" s="96"/>
-      <c r="K2" s="96"/>
-      <c r="L2" s="96"/>
-      <c r="M2" s="96"/>
-      <c r="N2" s="96"/>
-      <c r="O2" s="96"/>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
+      <c r="F2" s="97"/>
+      <c r="G2" s="97"/>
+      <c r="H2" s="97"/>
+      <c r="I2" s="97"/>
+      <c r="J2" s="97"/>
+      <c r="K2" s="97"/>
+      <c r="L2" s="97"/>
+      <c r="M2" s="97"/>
+      <c r="N2" s="97"/>
+      <c r="O2" s="97"/>
     </row>
     <row r="3" spans="2:15" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="97" t="s">
+      <c r="B3" s="98" t="s">
         <v>73</v>
       </c>
-      <c r="C3" s="97"/>
-      <c r="D3" s="97"/>
-      <c r="E3" s="97"/>
-      <c r="F3" s="97"/>
-      <c r="G3" s="97"/>
-      <c r="H3" s="97"/>
-      <c r="I3" s="97"/>
-      <c r="J3" s="97"/>
-      <c r="K3" s="97"/>
-      <c r="L3" s="97"/>
-      <c r="M3" s="97"/>
-      <c r="N3" s="97"/>
-      <c r="O3" s="97"/>
+      <c r="C3" s="98"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="98"/>
+      <c r="F3" s="98"/>
+      <c r="G3" s="98"/>
+      <c r="H3" s="98"/>
+      <c r="I3" s="98"/>
+      <c r="J3" s="98"/>
+      <c r="K3" s="98"/>
+      <c r="L3" s="98"/>
+      <c r="M3" s="98"/>
+      <c r="N3" s="98"/>
+      <c r="O3" s="98"/>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>45</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D5" s="45" t="s">
         <v>50</v>
@@ -3500,16 +3509,16 @@
         <v>52</v>
       </c>
       <c r="J5" s="45" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="K5" s="45" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L5" s="95" t="s">
+        <v>193</v>
+      </c>
+      <c r="M5" s="95" t="s">
         <v>194</v>
-      </c>
-      <c r="M5" s="95" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.25">
@@ -3555,22 +3564,22 @@
   <sheetData>
     <row r="1" spans="2:5" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="96"/>
-      <c r="C2" s="96"/>
-      <c r="D2" s="96"/>
-      <c r="E2" s="96"/>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
     </row>
     <row r="3" spans="2:5" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="97" t="s">
-        <v>130</v>
-      </c>
-      <c r="C3" s="97"/>
-      <c r="D3" s="97"/>
-      <c r="E3" s="97"/>
+      <c r="B3" s="98" t="s">
+        <v>129</v>
+      </c>
+      <c r="C3" s="98"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="98"/>
     </row>
     <row r="4" spans="2:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="64"/>
@@ -3580,13 +3589,13 @@
         <v>45</v>
       </c>
       <c r="C5" s="44" t="s">
+        <v>130</v>
+      </c>
+      <c r="D5" s="61" t="s">
         <v>131</v>
       </c>
-      <c r="D5" s="61" t="s">
+      <c r="E5" s="61" t="s">
         <v>132</v>
-      </c>
-      <c r="E5" s="61" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="6" spans="2:5" customFormat="1" x14ac:dyDescent="0.25">
@@ -3628,47 +3637,47 @@
   <sheetData>
     <row r="1" spans="2:14" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="96"/>
-      <c r="C2" s="96"/>
-      <c r="D2" s="96"/>
-      <c r="E2" s="96"/>
-      <c r="F2" s="96"/>
-      <c r="G2" s="96"/>
-      <c r="H2" s="96"/>
-      <c r="I2" s="96"/>
-      <c r="J2" s="96"/>
-      <c r="K2" s="96"/>
-      <c r="L2" s="96"/>
-      <c r="M2" s="96"/>
-      <c r="N2" s="96"/>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
+      <c r="F2" s="97"/>
+      <c r="G2" s="97"/>
+      <c r="H2" s="97"/>
+      <c r="I2" s="97"/>
+      <c r="J2" s="97"/>
+      <c r="K2" s="97"/>
+      <c r="L2" s="97"/>
+      <c r="M2" s="97"/>
+      <c r="N2" s="97"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="97" t="s">
+      <c r="B3" s="98" t="s">
         <v>69</v>
       </c>
-      <c r="C3" s="97"/>
-      <c r="D3" s="97"/>
-      <c r="E3" s="97"/>
-      <c r="F3" s="97"/>
-      <c r="G3" s="97"/>
-      <c r="H3" s="97"/>
-      <c r="I3" s="97"/>
-      <c r="J3" s="97"/>
-      <c r="K3" s="97"/>
-      <c r="L3" s="97"/>
-      <c r="M3" s="97"/>
-      <c r="N3" s="97"/>
+      <c r="C3" s="98"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="98"/>
+      <c r="F3" s="98"/>
+      <c r="G3" s="98"/>
+      <c r="H3" s="98"/>
+      <c r="I3" s="98"/>
+      <c r="J3" s="98"/>
+      <c r="K3" s="98"/>
+      <c r="L3" s="98"/>
+      <c r="M3" s="98"/>
+      <c r="N3" s="98"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>75</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>70</v>
@@ -3712,47 +3721,47 @@
   <sheetData>
     <row r="1" spans="2:14" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="96"/>
-      <c r="C2" s="96"/>
-      <c r="D2" s="96"/>
-      <c r="E2" s="96"/>
-      <c r="F2" s="96"/>
-      <c r="G2" s="96"/>
-      <c r="H2" s="96"/>
-      <c r="I2" s="96"/>
-      <c r="J2" s="96"/>
-      <c r="K2" s="96"/>
-      <c r="L2" s="96"/>
-      <c r="M2" s="96"/>
-      <c r="N2" s="96"/>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
+      <c r="F2" s="97"/>
+      <c r="G2" s="97"/>
+      <c r="H2" s="97"/>
+      <c r="I2" s="97"/>
+      <c r="J2" s="97"/>
+      <c r="K2" s="97"/>
+      <c r="L2" s="97"/>
+      <c r="M2" s="97"/>
+      <c r="N2" s="97"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="97" t="s">
+      <c r="B3" s="98" t="s">
         <v>74</v>
       </c>
-      <c r="C3" s="97"/>
-      <c r="D3" s="97"/>
-      <c r="E3" s="97"/>
-      <c r="F3" s="97"/>
-      <c r="G3" s="97"/>
-      <c r="H3" s="97"/>
-      <c r="I3" s="97"/>
-      <c r="J3" s="97"/>
-      <c r="K3" s="97"/>
-      <c r="L3" s="97"/>
-      <c r="M3" s="97"/>
-      <c r="N3" s="97"/>
+      <c r="C3" s="98"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="98"/>
+      <c r="F3" s="98"/>
+      <c r="G3" s="98"/>
+      <c r="H3" s="98"/>
+      <c r="I3" s="98"/>
+      <c r="J3" s="98"/>
+      <c r="K3" s="98"/>
+      <c r="L3" s="98"/>
+      <c r="M3" s="98"/>
+      <c r="N3" s="98"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D5" s="45" t="s">
         <v>51</v>
@@ -3810,44 +3819,44 @@
   <sheetData>
     <row r="1" spans="2:18" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="2:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="96"/>
-      <c r="C2" s="96"/>
-      <c r="D2" s="96"/>
-      <c r="E2" s="96"/>
-      <c r="F2" s="96"/>
-      <c r="G2" s="96"/>
-      <c r="H2" s="96"/>
-      <c r="I2" s="96"/>
-      <c r="J2" s="96"/>
-      <c r="K2" s="96"/>
-      <c r="L2" s="96"/>
-      <c r="M2" s="96"/>
-      <c r="N2" s="96"/>
-      <c r="O2" s="96"/>
-      <c r="P2" s="96"/>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
+      <c r="F2" s="97"/>
+      <c r="G2" s="97"/>
+      <c r="H2" s="97"/>
+      <c r="I2" s="97"/>
+      <c r="J2" s="97"/>
+      <c r="K2" s="97"/>
+      <c r="L2" s="97"/>
+      <c r="M2" s="97"/>
+      <c r="N2" s="97"/>
+      <c r="O2" s="97"/>
+      <c r="P2" s="97"/>
     </row>
     <row r="3" spans="2:18" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="97" t="s">
+      <c r="B3" s="98" t="s">
         <v>63</v>
       </c>
-      <c r="C3" s="97"/>
-      <c r="D3" s="97"/>
-      <c r="E3" s="97"/>
-      <c r="F3" s="97"/>
-      <c r="G3" s="97"/>
-      <c r="H3" s="97"/>
-      <c r="I3" s="97"/>
-      <c r="J3" s="97"/>
-      <c r="K3" s="97"/>
-      <c r="L3" s="97"/>
-      <c r="M3" s="97"/>
-      <c r="N3" s="97"/>
-      <c r="O3" s="97"/>
-      <c r="P3" s="97"/>
+      <c r="C3" s="98"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="98"/>
+      <c r="F3" s="98"/>
+      <c r="G3" s="98"/>
+      <c r="H3" s="98"/>
+      <c r="I3" s="98"/>
+      <c r="J3" s="98"/>
+      <c r="K3" s="98"/>
+      <c r="L3" s="98"/>
+      <c r="M3" s="98"/>
+      <c r="N3" s="98"/>
+      <c r="O3" s="98"/>
+      <c r="P3" s="98"/>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
@@ -3884,10 +3893,10 @@
         <v>56</v>
       </c>
       <c r="M5" s="53" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="N5" s="53" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="O5" s="4" t="s">
         <v>57</v>
@@ -3957,40 +3966,40 @@
   <sheetData>
     <row r="1" spans="2:14" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="96"/>
-      <c r="C2" s="96"/>
-      <c r="D2" s="96"/>
-      <c r="E2" s="96"/>
-      <c r="F2" s="96"/>
-      <c r="G2" s="96"/>
-      <c r="H2" s="96"/>
-      <c r="I2" s="96"/>
-      <c r="J2" s="96"/>
-      <c r="K2" s="96"/>
-      <c r="L2" s="96"/>
-      <c r="M2" s="96"/>
-      <c r="N2" s="96"/>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
+      <c r="F2" s="97"/>
+      <c r="G2" s="97"/>
+      <c r="H2" s="97"/>
+      <c r="I2" s="97"/>
+      <c r="J2" s="97"/>
+      <c r="K2" s="97"/>
+      <c r="L2" s="97"/>
+      <c r="M2" s="97"/>
+      <c r="N2" s="97"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="97" t="s">
+      <c r="B3" s="98" t="s">
         <v>64</v>
       </c>
-      <c r="C3" s="97"/>
-      <c r="D3" s="97"/>
-      <c r="E3" s="97"/>
-      <c r="F3" s="97"/>
-      <c r="G3" s="97"/>
-      <c r="H3" s="97"/>
-      <c r="I3" s="97"/>
-      <c r="J3" s="97"/>
-      <c r="K3" s="97"/>
-      <c r="L3" s="97"/>
-      <c r="M3" s="97"/>
-      <c r="N3" s="97"/>
+      <c r="C3" s="98"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="98"/>
+      <c r="F3" s="98"/>
+      <c r="G3" s="98"/>
+      <c r="H3" s="98"/>
+      <c r="I3" s="98"/>
+      <c r="J3" s="98"/>
+      <c r="K3" s="98"/>
+      <c r="L3" s="98"/>
+      <c r="M3" s="98"/>
+      <c r="N3" s="98"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="58" t="s">
@@ -4073,42 +4082,42 @@
   <sheetData>
     <row r="1" spans="2:14" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="96" t="s">
-        <v>96</v>
-      </c>
-      <c r="C2" s="96"/>
-      <c r="D2" s="96"/>
-      <c r="E2" s="96"/>
-      <c r="F2" s="96"/>
-      <c r="G2" s="96"/>
-      <c r="H2" s="96"/>
-      <c r="I2" s="96"/>
-      <c r="J2" s="96"/>
-      <c r="K2" s="96"/>
-      <c r="L2" s="96"/>
-      <c r="M2" s="96"/>
-      <c r="N2" s="96"/>
+      <c r="B2" s="97" t="s">
+        <v>95</v>
+      </c>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
+      <c r="F2" s="97"/>
+      <c r="G2" s="97"/>
+      <c r="H2" s="97"/>
+      <c r="I2" s="97"/>
+      <c r="J2" s="97"/>
+      <c r="K2" s="97"/>
+      <c r="L2" s="97"/>
+      <c r="M2" s="97"/>
+      <c r="N2" s="97"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="97" t="s">
+      <c r="B3" s="98" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="97"/>
-      <c r="D3" s="97"/>
-      <c r="E3" s="97"/>
-      <c r="F3" s="97"/>
-      <c r="G3" s="97"/>
-      <c r="H3" s="97"/>
-      <c r="I3" s="97"/>
-      <c r="J3" s="97"/>
-      <c r="K3" s="97"/>
-      <c r="L3" s="97"/>
-      <c r="M3" s="97"/>
-      <c r="N3" s="97"/>
+      <c r="C3" s="98"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="98"/>
+      <c r="F3" s="98"/>
+      <c r="G3" s="98"/>
+      <c r="H3" s="98"/>
+      <c r="I3" s="98"/>
+      <c r="J3" s="98"/>
+      <c r="K3" s="98"/>
+      <c r="L3" s="98"/>
+      <c r="M3" s="98"/>
+      <c r="N3" s="98"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="44" t="s">
@@ -4163,74 +4172,74 @@
   <sheetData>
     <row r="1" spans="2:14" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="96"/>
-      <c r="C2" s="96"/>
-      <c r="D2" s="96"/>
-      <c r="E2" s="96"/>
-      <c r="F2" s="96"/>
-      <c r="G2" s="96"/>
-      <c r="H2" s="96"/>
-      <c r="I2" s="96"/>
-      <c r="J2" s="96"/>
-      <c r="K2" s="96"/>
-      <c r="L2" s="96"/>
-      <c r="M2" s="96"/>
-      <c r="N2" s="96"/>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
+      <c r="F2" s="97"/>
+      <c r="G2" s="97"/>
+      <c r="H2" s="97"/>
+      <c r="I2" s="97"/>
+      <c r="J2" s="97"/>
+      <c r="K2" s="97"/>
+      <c r="L2" s="97"/>
+      <c r="M2" s="97"/>
+      <c r="N2" s="97"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="97" t="s">
-        <v>151</v>
-      </c>
-      <c r="C3" s="97"/>
-      <c r="D3" s="97"/>
-      <c r="E3" s="97"/>
-      <c r="F3" s="97"/>
-      <c r="G3" s="97"/>
-      <c r="H3" s="97"/>
-      <c r="I3" s="97"/>
-      <c r="J3" s="97"/>
-      <c r="K3" s="97"/>
-      <c r="L3" s="97"/>
-      <c r="M3" s="97"/>
-      <c r="N3" s="97"/>
+      <c r="B3" s="98" t="s">
+        <v>150</v>
+      </c>
+      <c r="C3" s="98"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="98"/>
+      <c r="F3" s="98"/>
+      <c r="G3" s="98"/>
+      <c r="H3" s="98"/>
+      <c r="I3" s="98"/>
+      <c r="J3" s="98"/>
+      <c r="K3" s="98"/>
+      <c r="L3" s="98"/>
+      <c r="M3" s="98"/>
+      <c r="N3" s="98"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="74" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="74" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D5" s="74" t="s">
+        <v>141</v>
+      </c>
+      <c r="E5" s="74" t="s">
         <v>142</v>
       </c>
-      <c r="E5" s="74" t="s">
+      <c r="F5" s="74" t="s">
         <v>143</v>
       </c>
-      <c r="F5" s="74" t="s">
+      <c r="G5" s="74" t="s">
         <v>144</v>
       </c>
-      <c r="G5" s="74" t="s">
+      <c r="H5" s="74" t="s">
         <v>145</v>
       </c>
-      <c r="H5" s="74" t="s">
+      <c r="I5" s="74" t="s">
         <v>146</v>
       </c>
-      <c r="I5" s="74" t="s">
+      <c r="J5" s="74" t="s">
         <v>147</v>
       </c>
-      <c r="J5" s="74" t="s">
+      <c r="K5" s="74" t="s">
         <v>148</v>
       </c>
-      <c r="K5" s="74" t="s">
+      <c r="L5" s="74" t="s">
         <v>149</v>
-      </c>
-      <c r="L5" s="74" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
@@ -4279,32 +4288,32 @@
   <sheetData>
     <row r="1" spans="2:10" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="96"/>
-      <c r="C2" s="96"/>
-      <c r="D2" s="96"/>
-      <c r="E2" s="96"/>
-      <c r="F2" s="96"/>
-      <c r="G2" s="96"/>
-      <c r="H2" s="96"/>
-      <c r="I2" s="96"/>
-      <c r="J2" s="96"/>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
+      <c r="F2" s="97"/>
+      <c r="G2" s="97"/>
+      <c r="H2" s="97"/>
+      <c r="I2" s="97"/>
+      <c r="J2" s="97"/>
     </row>
     <row r="3" spans="2:10" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="97" t="s">
-        <v>154</v>
-      </c>
-      <c r="C3" s="97"/>
-      <c r="D3" s="97"/>
-      <c r="E3" s="97"/>
-      <c r="F3" s="97"/>
-      <c r="G3" s="97"/>
-      <c r="H3" s="97"/>
-      <c r="I3" s="97"/>
-      <c r="J3" s="97"/>
+      <c r="B3" s="98" t="s">
+        <v>153</v>
+      </c>
+      <c r="C3" s="98"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="98"/>
+      <c r="F3" s="98"/>
+      <c r="G3" s="98"/>
+      <c r="H3" s="98"/>
+      <c r="I3" s="98"/>
+      <c r="J3" s="98"/>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" s="74" t="s">
@@ -4314,22 +4323,22 @@
         <v>27</v>
       </c>
       <c r="D5" s="74" t="s">
+        <v>141</v>
+      </c>
+      <c r="E5" s="74" t="s">
         <v>142</v>
       </c>
-      <c r="E5" s="74" t="s">
+      <c r="F5" s="74" t="s">
         <v>143</v>
       </c>
-      <c r="F5" s="74" t="s">
+      <c r="G5" s="74" t="s">
         <v>144</v>
       </c>
-      <c r="G5" s="74" t="s">
-        <v>145</v>
-      </c>
       <c r="H5" s="74" t="s">
+        <v>151</v>
+      </c>
+      <c r="I5" s="74" t="s">
         <v>152</v>
-      </c>
-      <c r="I5" s="74" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
@@ -4385,33 +4394,33 @@
   <sheetData>
     <row r="1" spans="2:20" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="2:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="98"/>
-      <c r="C2" s="98"/>
-      <c r="D2" s="98"/>
-      <c r="E2" s="98"/>
-      <c r="F2" s="98"/>
-      <c r="G2" s="98"/>
-      <c r="H2" s="98"/>
-      <c r="I2" s="98"/>
+      <c r="B2" s="99"/>
+      <c r="C2" s="99"/>
+      <c r="D2" s="99"/>
+      <c r="E2" s="99"/>
+      <c r="F2" s="99"/>
+      <c r="G2" s="99"/>
+      <c r="H2" s="99"/>
+      <c r="I2" s="99"/>
       <c r="L2" s="84"/>
       <c r="M2" s="84"/>
       <c r="N2" s="84"/>
     </row>
     <row r="3" spans="2:20" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="97" t="s">
-        <v>155</v>
-      </c>
-      <c r="C3" s="97"/>
-      <c r="D3" s="97"/>
-      <c r="E3" s="97"/>
-      <c r="F3" s="97"/>
-      <c r="G3" s="97"/>
-      <c r="H3" s="97"/>
-      <c r="I3" s="97"/>
+      <c r="B3" s="98" t="s">
+        <v>154</v>
+      </c>
+      <c r="C3" s="98"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="98"/>
+      <c r="F3" s="98"/>
+      <c r="G3" s="98"/>
+      <c r="H3" s="98"/>
+      <c r="I3" s="98"/>
       <c r="L3" s="83"/>
       <c r="M3" s="83"/>
       <c r="N3" s="83"/>
@@ -4421,58 +4430,58 @@
         <v>2</v>
       </c>
       <c r="C5" s="79" t="s">
+        <v>155</v>
+      </c>
+      <c r="D5" s="79" t="s">
+        <v>141</v>
+      </c>
+      <c r="E5" s="79" t="s">
         <v>156</v>
       </c>
-      <c r="D5" s="79" t="s">
-        <v>142</v>
-      </c>
-      <c r="E5" s="79" t="s">
+      <c r="F5" s="79" t="s">
         <v>157</v>
       </c>
-      <c r="F5" s="79" t="s">
+      <c r="G5" s="79" t="s">
         <v>158</v>
       </c>
-      <c r="G5" s="79" t="s">
+      <c r="H5" s="79" t="s">
         <v>159</v>
       </c>
-      <c r="H5" s="79" t="s">
+      <c r="I5" s="79" t="s">
+        <v>163</v>
+      </c>
+      <c r="J5" s="79" t="s">
+        <v>164</v>
+      </c>
+      <c r="K5" s="79" t="s">
+        <v>165</v>
+      </c>
+      <c r="L5" s="79" t="s">
         <v>160</v>
       </c>
-      <c r="I5" s="79" t="s">
-        <v>164</v>
-      </c>
-      <c r="J5" s="79" t="s">
-        <v>165</v>
-      </c>
-      <c r="K5" s="79" t="s">
-        <v>166</v>
-      </c>
-      <c r="L5" s="79" t="s">
+      <c r="M5" s="79" t="s">
         <v>161</v>
       </c>
-      <c r="M5" s="79" t="s">
+      <c r="N5" s="79" t="s">
         <v>162</v>
       </c>
-      <c r="N5" s="79" t="s">
-        <v>163</v>
-      </c>
       <c r="O5" s="87" t="s">
+        <v>175</v>
+      </c>
+      <c r="P5" s="87" t="s">
         <v>176</v>
       </c>
-      <c r="P5" s="87" t="s">
+      <c r="Q5" s="87" t="s">
+        <v>180</v>
+      </c>
+      <c r="R5" s="87" t="s">
         <v>177</v>
       </c>
-      <c r="Q5" s="87" t="s">
-        <v>181</v>
-      </c>
-      <c r="R5" s="87" t="s">
+      <c r="S5" s="87" t="s">
         <v>178</v>
       </c>
-      <c r="S5" s="87" t="s">
+      <c r="T5" s="87" t="s">
         <v>179</v>
-      </c>
-      <c r="T5" s="87" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.25">
@@ -4528,55 +4537,55 @@
   <sheetData>
     <row r="1" spans="2:9" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="2:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="96"/>
-      <c r="C2" s="96"/>
-      <c r="D2" s="96"/>
-      <c r="E2" s="96"/>
-      <c r="F2" s="96"/>
-      <c r="G2" s="96"/>
-      <c r="H2" s="96"/>
-      <c r="I2" s="96"/>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
+      <c r="F2" s="97"/>
+      <c r="G2" s="97"/>
+      <c r="H2" s="97"/>
+      <c r="I2" s="97"/>
     </row>
     <row r="3" spans="2:9" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="97" t="s">
-        <v>191</v>
-      </c>
-      <c r="C3" s="97"/>
-      <c r="D3" s="97"/>
-      <c r="E3" s="97"/>
-      <c r="F3" s="97"/>
-      <c r="G3" s="97"/>
-      <c r="H3" s="97"/>
-      <c r="I3" s="97"/>
+      <c r="B3" s="98" t="s">
+        <v>190</v>
+      </c>
+      <c r="C3" s="98"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="98"/>
+      <c r="F3" s="98"/>
+      <c r="G3" s="98"/>
+      <c r="H3" s="98"/>
+      <c r="I3" s="98"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="89" t="s">
+        <v>182</v>
+      </c>
+      <c r="C5" s="89" t="s">
         <v>183</v>
       </c>
-      <c r="C5" s="89" t="s">
+      <c r="D5" s="89" t="s">
         <v>184</v>
       </c>
-      <c r="D5" s="89" t="s">
+      <c r="E5" s="89" t="s">
         <v>185</v>
       </c>
-      <c r="E5" s="89" t="s">
+      <c r="F5" s="89" t="s">
         <v>186</v>
       </c>
-      <c r="F5" s="89" t="s">
+      <c r="G5" s="89" t="s">
         <v>187</v>
       </c>
-      <c r="G5" s="89" t="s">
+      <c r="H5" s="89" t="s">
         <v>188</v>
       </c>
-      <c r="H5" s="89" t="s">
+      <c r="I5" s="89" t="s">
         <v>189</v>
-      </c>
-      <c r="I5" s="89" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
@@ -4623,34 +4632,34 @@
   <sheetData>
     <row r="1" spans="2:11" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="96"/>
-      <c r="C2" s="96"/>
-      <c r="D2" s="96"/>
-      <c r="E2" s="96"/>
-      <c r="F2" s="96"/>
-      <c r="G2" s="96"/>
-      <c r="H2" s="96"/>
-      <c r="I2" s="96"/>
-      <c r="J2" s="96"/>
-      <c r="K2" s="96"/>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
+      <c r="F2" s="97"/>
+      <c r="G2" s="97"/>
+      <c r="H2" s="97"/>
+      <c r="I2" s="97"/>
+      <c r="J2" s="97"/>
+      <c r="K2" s="97"/>
     </row>
     <row r="3" spans="2:11" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="97" t="s">
-        <v>167</v>
-      </c>
-      <c r="C3" s="97"/>
-      <c r="D3" s="97"/>
-      <c r="E3" s="97"/>
-      <c r="F3" s="97"/>
-      <c r="G3" s="97"/>
-      <c r="H3" s="97"/>
-      <c r="I3" s="97"/>
-      <c r="J3" s="97"/>
-      <c r="K3" s="97"/>
+      <c r="B3" s="98" t="s">
+        <v>166</v>
+      </c>
+      <c r="C3" s="98"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="98"/>
+      <c r="F3" s="98"/>
+      <c r="G3" s="98"/>
+      <c r="H3" s="98"/>
+      <c r="I3" s="98"/>
+      <c r="J3" s="98"/>
+      <c r="K3" s="98"/>
     </row>
     <row r="4" spans="2:11" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B4" s="85"/>
@@ -4665,14 +4674,14 @@
       <c r="K4" s="85"/>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="H5" s="100" t="s">
-        <v>175</v>
-      </c>
-      <c r="I5" s="101"/>
-      <c r="J5" s="100" t="s">
+      <c r="H5" s="101" t="s">
         <v>174</v>
       </c>
-      <c r="K5" s="101"/>
+      <c r="I5" s="102"/>
+      <c r="J5" s="101" t="s">
+        <v>173</v>
+      </c>
+      <c r="K5" s="102"/>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" s="86" t="s">
@@ -4682,28 +4691,28 @@
         <v>25</v>
       </c>
       <c r="D6" s="86" t="s">
+        <v>167</v>
+      </c>
+      <c r="E6" s="86" t="s">
         <v>168</v>
       </c>
-      <c r="E6" s="86" t="s">
+      <c r="F6" s="86" t="s">
+        <v>114</v>
+      </c>
+      <c r="G6" s="86" t="s">
+        <v>114</v>
+      </c>
+      <c r="H6" s="86" t="s">
         <v>169</v>
       </c>
-      <c r="F6" s="86" t="s">
-        <v>115</v>
-      </c>
-      <c r="G6" s="86" t="s">
-        <v>115</v>
-      </c>
-      <c r="H6" s="86" t="s">
+      <c r="I6" s="86" t="s">
         <v>170</v>
       </c>
-      <c r="I6" s="86" t="s">
+      <c r="J6" s="86" t="s">
         <v>171</v>
       </c>
-      <c r="J6" s="86" t="s">
+      <c r="K6" s="86" t="s">
         <v>172</v>
-      </c>
-      <c r="K6" s="86" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
@@ -4749,42 +4758,42 @@
   <sheetData>
     <row r="1" spans="2:26" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="Z1" s="38"/>
     </row>
     <row r="2" spans="2:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="96"/>
-      <c r="C2" s="96"/>
-      <c r="D2" s="96"/>
-      <c r="E2" s="96"/>
-      <c r="F2" s="96"/>
-      <c r="G2" s="96"/>
-      <c r="H2" s="96"/>
-      <c r="I2" s="96"/>
-      <c r="J2" s="96"/>
-      <c r="K2" s="96"/>
-      <c r="L2" s="96"/>
-      <c r="M2" s="96"/>
-      <c r="N2" s="96"/>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
+      <c r="F2" s="97"/>
+      <c r="G2" s="97"/>
+      <c r="H2" s="97"/>
+      <c r="I2" s="97"/>
+      <c r="J2" s="97"/>
+      <c r="K2" s="97"/>
+      <c r="L2" s="97"/>
+      <c r="M2" s="97"/>
+      <c r="N2" s="97"/>
       <c r="Z2"/>
     </row>
     <row r="3" spans="2:26" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="97" t="s">
+      <c r="B3" s="98" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="97"/>
-      <c r="D3" s="97"/>
-      <c r="E3" s="97"/>
-      <c r="F3" s="97"/>
-      <c r="G3" s="97"/>
-      <c r="H3" s="97"/>
-      <c r="I3" s="97"/>
-      <c r="J3" s="97"/>
-      <c r="K3" s="97"/>
-      <c r="L3" s="97"/>
-      <c r="M3" s="97"/>
-      <c r="N3" s="97"/>
+      <c r="C3" s="98"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="98"/>
+      <c r="F3" s="98"/>
+      <c r="G3" s="98"/>
+      <c r="H3" s="98"/>
+      <c r="I3" s="98"/>
+      <c r="J3" s="98"/>
+      <c r="K3" s="98"/>
+      <c r="L3" s="98"/>
+      <c r="M3" s="98"/>
+      <c r="N3" s="98"/>
       <c r="Z3"/>
     </row>
     <row r="5" spans="2:26" x14ac:dyDescent="0.25">
@@ -4883,42 +4892,42 @@
   <sheetData>
     <row r="1" spans="2:26" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="Z1" s="38"/>
     </row>
     <row r="2" spans="2:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="96"/>
-      <c r="C2" s="96"/>
-      <c r="D2" s="96"/>
-      <c r="E2" s="96"/>
-      <c r="F2" s="96"/>
-      <c r="G2" s="96"/>
-      <c r="H2" s="96"/>
-      <c r="I2" s="96"/>
-      <c r="J2" s="96"/>
-      <c r="K2" s="96"/>
-      <c r="L2" s="96"/>
-      <c r="M2" s="96"/>
-      <c r="N2" s="96"/>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
+      <c r="F2" s="97"/>
+      <c r="G2" s="97"/>
+      <c r="H2" s="97"/>
+      <c r="I2" s="97"/>
+      <c r="J2" s="97"/>
+      <c r="K2" s="97"/>
+      <c r="L2" s="97"/>
+      <c r="M2" s="97"/>
+      <c r="N2" s="97"/>
       <c r="Z2"/>
     </row>
     <row r="3" spans="2:26" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="97" t="s">
+      <c r="B3" s="98" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="97"/>
-      <c r="D3" s="97"/>
-      <c r="E3" s="97"/>
-      <c r="F3" s="97"/>
-      <c r="G3" s="97"/>
-      <c r="H3" s="97"/>
-      <c r="I3" s="97"/>
-      <c r="J3" s="97"/>
-      <c r="K3" s="97"/>
-      <c r="L3" s="97"/>
-      <c r="M3" s="97"/>
-      <c r="N3" s="97"/>
+      <c r="C3" s="98"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="98"/>
+      <c r="F3" s="98"/>
+      <c r="G3" s="98"/>
+      <c r="H3" s="98"/>
+      <c r="I3" s="98"/>
+      <c r="J3" s="98"/>
+      <c r="K3" s="98"/>
+      <c r="L3" s="98"/>
+      <c r="M3" s="98"/>
+      <c r="N3" s="98"/>
       <c r="Z3"/>
     </row>
     <row r="5" spans="2:26" x14ac:dyDescent="0.25">
@@ -4935,11 +4944,11 @@
     </row>
     <row r="6" spans="2:26" x14ac:dyDescent="0.25">
       <c r="C6" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="D6" s="102"/>
-      <c r="E6" s="103"/>
-      <c r="F6" s="104"/>
+        <v>107</v>
+      </c>
+      <c r="D6" s="103"/>
+      <c r="E6" s="104"/>
+      <c r="F6" s="105"/>
       <c r="G6" s="50"/>
       <c r="H6" s="50"/>
     </row>
@@ -5012,42 +5021,42 @@
   <sheetData>
     <row r="1" spans="2:26" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="Z1" s="38"/>
     </row>
     <row r="2" spans="2:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="96"/>
-      <c r="C2" s="96"/>
-      <c r="D2" s="96"/>
-      <c r="E2" s="96"/>
-      <c r="F2" s="96"/>
-      <c r="G2" s="96"/>
-      <c r="H2" s="96"/>
-      <c r="I2" s="96"/>
-      <c r="J2" s="96"/>
-      <c r="K2" s="96"/>
-      <c r="L2" s="96"/>
-      <c r="M2" s="96"/>
-      <c r="N2" s="96"/>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
+      <c r="F2" s="97"/>
+      <c r="G2" s="97"/>
+      <c r="H2" s="97"/>
+      <c r="I2" s="97"/>
+      <c r="J2" s="97"/>
+      <c r="K2" s="97"/>
+      <c r="L2" s="97"/>
+      <c r="M2" s="97"/>
+      <c r="N2" s="97"/>
       <c r="Z2"/>
     </row>
     <row r="3" spans="2:26" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="97" t="s">
-        <v>92</v>
-      </c>
-      <c r="C3" s="97"/>
-      <c r="D3" s="97"/>
-      <c r="E3" s="97"/>
-      <c r="F3" s="97"/>
-      <c r="G3" s="97"/>
-      <c r="H3" s="97"/>
-      <c r="I3" s="97"/>
-      <c r="J3" s="97"/>
-      <c r="K3" s="97"/>
-      <c r="L3" s="97"/>
-      <c r="M3" s="97"/>
-      <c r="N3" s="97"/>
+      <c r="B3" s="98" t="s">
+        <v>91</v>
+      </c>
+      <c r="C3" s="98"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="98"/>
+      <c r="F3" s="98"/>
+      <c r="G3" s="98"/>
+      <c r="H3" s="98"/>
+      <c r="I3" s="98"/>
+      <c r="J3" s="98"/>
+      <c r="K3" s="98"/>
+      <c r="L3" s="98"/>
+      <c r="M3" s="98"/>
+      <c r="N3" s="98"/>
       <c r="Z3"/>
     </row>
     <row r="5" spans="2:26" x14ac:dyDescent="0.25">
@@ -5066,7 +5075,7 @@
       </c>
       <c r="D6" s="12"/>
       <c r="E6" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F6" s="12"/>
     </row>
@@ -5135,42 +5144,42 @@
   <sheetData>
     <row r="1" spans="2:26" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="Z1" s="38"/>
     </row>
     <row r="2" spans="2:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="96"/>
-      <c r="C2" s="96"/>
-      <c r="D2" s="96"/>
-      <c r="E2" s="96"/>
-      <c r="F2" s="96"/>
-      <c r="G2" s="96"/>
-      <c r="H2" s="96"/>
-      <c r="I2" s="96"/>
-      <c r="J2" s="96"/>
-      <c r="K2" s="96"/>
-      <c r="L2" s="96"/>
-      <c r="M2" s="96"/>
-      <c r="N2" s="96"/>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
+      <c r="F2" s="97"/>
+      <c r="G2" s="97"/>
+      <c r="H2" s="97"/>
+      <c r="I2" s="97"/>
+      <c r="J2" s="97"/>
+      <c r="K2" s="97"/>
+      <c r="L2" s="97"/>
+      <c r="M2" s="97"/>
+      <c r="N2" s="97"/>
       <c r="Z2"/>
     </row>
     <row r="3" spans="2:26" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="97" t="s">
+      <c r="B3" s="98" t="s">
         <v>72</v>
       </c>
-      <c r="C3" s="97"/>
-      <c r="D3" s="97"/>
-      <c r="E3" s="97"/>
-      <c r="F3" s="97"/>
-      <c r="G3" s="97"/>
-      <c r="H3" s="97"/>
-      <c r="I3" s="97"/>
-      <c r="J3" s="97"/>
-      <c r="K3" s="97"/>
-      <c r="L3" s="97"/>
-      <c r="M3" s="97"/>
-      <c r="N3" s="97"/>
+      <c r="C3" s="98"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="98"/>
+      <c r="F3" s="98"/>
+      <c r="G3" s="98"/>
+      <c r="H3" s="98"/>
+      <c r="I3" s="98"/>
+      <c r="J3" s="98"/>
+      <c r="K3" s="98"/>
+      <c r="L3" s="98"/>
+      <c r="M3" s="98"/>
+      <c r="N3" s="98"/>
       <c r="Z3"/>
     </row>
     <row r="5" spans="2:26" x14ac:dyDescent="0.25">
@@ -5279,79 +5288,79 @@
   <sheetData>
     <row r="1" spans="2:17" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="96"/>
-      <c r="C2" s="96"/>
-      <c r="D2" s="96"/>
-      <c r="E2" s="96"/>
-      <c r="F2" s="96"/>
-      <c r="G2" s="96"/>
-      <c r="H2" s="96"/>
-      <c r="I2" s="96"/>
-      <c r="J2" s="96"/>
-      <c r="K2" s="96"/>
-      <c r="L2" s="96"/>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
+      <c r="F2" s="97"/>
+      <c r="G2" s="97"/>
+      <c r="H2" s="97"/>
+      <c r="I2" s="97"/>
+      <c r="J2" s="97"/>
+      <c r="K2" s="97"/>
+      <c r="L2" s="97"/>
     </row>
     <row r="3" spans="2:17" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="97" t="s">
-        <v>107</v>
-      </c>
-      <c r="C3" s="97"/>
-      <c r="D3" s="97"/>
-      <c r="E3" s="97"/>
-      <c r="F3" s="97"/>
-      <c r="G3" s="97"/>
-      <c r="H3" s="97"/>
-      <c r="I3" s="97"/>
-      <c r="J3" s="97"/>
-      <c r="K3" s="97"/>
-      <c r="L3" s="97"/>
+      <c r="B3" s="98" t="s">
+        <v>106</v>
+      </c>
+      <c r="C3" s="98"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="98"/>
+      <c r="F3" s="98"/>
+      <c r="G3" s="98"/>
+      <c r="H3" s="98"/>
+      <c r="I3" s="98"/>
+      <c r="J3" s="98"/>
+      <c r="K3" s="98"/>
+      <c r="L3" s="98"/>
     </row>
     <row r="5" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D5" s="105" t="s">
-        <v>122</v>
-      </c>
-      <c r="E5" s="105"/>
+      <c r="D5" s="106" t="s">
+        <v>121</v>
+      </c>
+      <c r="E5" s="106"/>
       <c r="F5" s="73"/>
       <c r="G5" s="73"/>
       <c r="H5" s="73"/>
       <c r="I5" s="73"/>
-      <c r="J5" s="105" t="s">
+      <c r="J5" s="106" t="s">
         <v>42</v>
       </c>
-      <c r="K5" s="105"/>
-      <c r="L5" s="105"/>
-      <c r="M5" s="105" t="s">
-        <v>129</v>
-      </c>
-      <c r="N5" s="105"/>
-      <c r="O5" s="105"/>
-      <c r="P5" s="99" t="s">
-        <v>108</v>
-      </c>
-      <c r="Q5" s="99"/>
+      <c r="K5" s="106"/>
+      <c r="L5" s="106"/>
+      <c r="M5" s="106" t="s">
+        <v>128</v>
+      </c>
+      <c r="N5" s="106"/>
+      <c r="O5" s="106"/>
+      <c r="P5" s="100" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q5" s="100"/>
     </row>
     <row r="6" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="70" t="s">
         <v>32</v>
       </c>
       <c r="C6" s="71" t="s">
+        <v>136</v>
+      </c>
+      <c r="D6" s="63" t="s">
+        <v>122</v>
+      </c>
+      <c r="E6" s="63" t="s">
+        <v>123</v>
+      </c>
+      <c r="F6" s="71" t="s">
         <v>137</v>
       </c>
-      <c r="D6" s="63" t="s">
-        <v>123</v>
-      </c>
-      <c r="E6" s="63" t="s">
-        <v>124</v>
-      </c>
-      <c r="F6" s="71" t="s">
+      <c r="G6" s="71" t="s">
         <v>138</v>
-      </c>
-      <c r="G6" s="71" t="s">
-        <v>139</v>
       </c>
       <c r="H6" s="72" t="s">
         <v>53</v>
@@ -5360,28 +5369,28 @@
         <v>70</v>
       </c>
       <c r="J6" s="63" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K6" s="63" t="s">
+        <v>126</v>
+      </c>
+      <c r="L6" s="69" t="s">
+        <v>114</v>
+      </c>
+      <c r="M6" s="63" t="s">
         <v>127</v>
       </c>
-      <c r="L6" s="69" t="s">
-        <v>115</v>
-      </c>
-      <c r="M6" s="63" t="s">
-        <v>128</v>
-      </c>
       <c r="N6" s="63" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="O6" s="69" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="P6" s="69" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="Q6" s="69" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.25">
@@ -5419,7 +5428,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:N6"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5429,49 +5440,48 @@
     <col min="4" max="4" width="33.140625" customWidth="1"/>
     <col min="5" max="5" width="21.7109375" customWidth="1"/>
     <col min="6" max="6" width="22.140625" customWidth="1"/>
-    <col min="7" max="7" width="26" customWidth="1"/>
-    <col min="8" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="29.5703125" customWidth="1"/>
+    <col min="9" max="9" width="33.140625" customWidth="1"/>
     <col min="10" max="10" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="7.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:14" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="96"/>
-      <c r="C2" s="96"/>
-      <c r="D2" s="96"/>
-      <c r="E2" s="96"/>
-      <c r="F2" s="96"/>
-      <c r="G2" s="96"/>
-      <c r="H2" s="96"/>
-      <c r="I2" s="96"/>
-      <c r="J2" s="96"/>
-      <c r="K2" s="96"/>
-      <c r="L2" s="96"/>
-      <c r="M2" s="96"/>
-      <c r="N2" s="96"/>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
+      <c r="F2" s="97"/>
+      <c r="G2" s="97"/>
+      <c r="H2" s="97"/>
+      <c r="I2" s="97"/>
+      <c r="J2" s="97"/>
+      <c r="K2" s="97"/>
+      <c r="L2" s="97"/>
+      <c r="M2" s="97"/>
+      <c r="N2" s="97"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="97" t="s">
+      <c r="B3" s="98" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="97"/>
-      <c r="D3" s="97"/>
-      <c r="E3" s="97"/>
-      <c r="F3" s="97"/>
-      <c r="G3" s="97"/>
-      <c r="H3" s="97"/>
-      <c r="I3" s="97"/>
-      <c r="J3" s="97"/>
-      <c r="K3" s="97"/>
-      <c r="L3" s="97"/>
-      <c r="M3" s="97"/>
-      <c r="N3" s="97"/>
+      <c r="C3" s="98"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="98"/>
+      <c r="F3" s="98"/>
+      <c r="G3" s="98"/>
+      <c r="H3" s="98"/>
+      <c r="I3" s="98"/>
+      <c r="J3" s="98"/>
+      <c r="K3" s="98"/>
+      <c r="L3" s="98"/>
+      <c r="M3" s="98"/>
+      <c r="N3" s="98"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="44" t="s">
@@ -5490,7 +5500,13 @@
         <v>11</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>78</v>
+        <v>195</v>
+      </c>
+      <c r="H5" s="96" t="s">
+        <v>196</v>
+      </c>
+      <c r="I5" s="96" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
@@ -5500,6 +5516,8 @@
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -5549,114 +5567,114 @@
   <sheetData>
     <row r="1" spans="2:25" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="2:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="96"/>
-      <c r="C2" s="96"/>
-      <c r="D2" s="96"/>
-      <c r="E2" s="96"/>
-      <c r="F2" s="96"/>
-      <c r="G2" s="96"/>
-      <c r="H2" s="96"/>
-      <c r="I2" s="96"/>
-      <c r="J2" s="96"/>
-      <c r="K2" s="96"/>
-      <c r="L2" s="96"/>
-      <c r="M2" s="96"/>
-      <c r="N2" s="96"/>
-      <c r="O2" s="96"/>
-      <c r="P2" s="96"/>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
+      <c r="F2" s="97"/>
+      <c r="G2" s="97"/>
+      <c r="H2" s="97"/>
+      <c r="I2" s="97"/>
+      <c r="J2" s="97"/>
+      <c r="K2" s="97"/>
+      <c r="L2" s="97"/>
+      <c r="M2" s="97"/>
+      <c r="N2" s="97"/>
+      <c r="O2" s="97"/>
+      <c r="P2" s="97"/>
       <c r="Q2" s="56"/>
       <c r="R2" s="56"/>
     </row>
     <row r="3" spans="2:25" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="97" t="s">
-        <v>110</v>
-      </c>
-      <c r="C3" s="97"/>
-      <c r="D3" s="97"/>
-      <c r="E3" s="97"/>
-      <c r="F3" s="97"/>
-      <c r="G3" s="97"/>
-      <c r="H3" s="97"/>
-      <c r="I3" s="97"/>
-      <c r="J3" s="97"/>
-      <c r="K3" s="97"/>
-      <c r="L3" s="97"/>
-      <c r="M3" s="97"/>
-      <c r="N3" s="97"/>
-      <c r="O3" s="97"/>
-      <c r="P3" s="97"/>
+      <c r="B3" s="98" t="s">
+        <v>109</v>
+      </c>
+      <c r="C3" s="98"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="98"/>
+      <c r="F3" s="98"/>
+      <c r="G3" s="98"/>
+      <c r="H3" s="98"/>
+      <c r="I3" s="98"/>
+      <c r="J3" s="98"/>
+      <c r="K3" s="98"/>
+      <c r="L3" s="98"/>
+      <c r="M3" s="98"/>
+      <c r="N3" s="98"/>
+      <c r="O3" s="98"/>
+      <c r="P3" s="98"/>
       <c r="Q3" s="57"/>
       <c r="R3" s="57"/>
     </row>
     <row r="5" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B5" s="110" t="s">
+      <c r="B5" s="111" t="s">
+        <v>110</v>
+      </c>
+      <c r="C5" s="112"/>
+      <c r="D5" s="112"/>
+      <c r="E5" s="112"/>
+      <c r="F5" s="112"/>
+      <c r="G5" s="112"/>
+      <c r="H5" s="112"/>
+      <c r="I5" s="112"/>
+      <c r="J5" s="112"/>
+      <c r="K5" s="112"/>
+      <c r="L5" s="113"/>
+      <c r="M5" s="111" t="s">
         <v>111</v>
       </c>
-      <c r="C5" s="111"/>
-      <c r="D5" s="111"/>
-      <c r="E5" s="111"/>
-      <c r="F5" s="111"/>
-      <c r="G5" s="111"/>
-      <c r="H5" s="111"/>
-      <c r="I5" s="111"/>
-      <c r="J5" s="111"/>
-      <c r="K5" s="111"/>
-      <c r="L5" s="112"/>
-      <c r="M5" s="110" t="s">
-        <v>112</v>
-      </c>
-      <c r="N5" s="111"/>
-      <c r="O5" s="111"/>
-      <c r="P5" s="111"/>
-      <c r="Q5" s="111"/>
-      <c r="R5" s="111"/>
-      <c r="S5" s="111"/>
-      <c r="T5" s="111"/>
-      <c r="U5" s="111"/>
-      <c r="V5" s="111"/>
-      <c r="W5" s="111"/>
-      <c r="X5" s="111"/>
-      <c r="Y5" s="112"/>
+      <c r="N5" s="112"/>
+      <c r="O5" s="112"/>
+      <c r="P5" s="112"/>
+      <c r="Q5" s="112"/>
+      <c r="R5" s="112"/>
+      <c r="S5" s="112"/>
+      <c r="T5" s="112"/>
+      <c r="U5" s="112"/>
+      <c r="V5" s="112"/>
+      <c r="W5" s="112"/>
+      <c r="X5" s="112"/>
+      <c r="Y5" s="113"/>
     </row>
     <row r="6" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B6" s="109"/>
-      <c r="C6" s="109"/>
-      <c r="D6" s="109"/>
-      <c r="E6" s="109"/>
-      <c r="F6" s="116" t="s">
+      <c r="B6" s="110"/>
+      <c r="C6" s="110"/>
+      <c r="D6" s="110"/>
+      <c r="E6" s="110"/>
+      <c r="F6" s="117" t="s">
         <v>27</v>
       </c>
-      <c r="G6" s="117"/>
-      <c r="H6" s="117"/>
-      <c r="I6" s="118"/>
-      <c r="J6" s="110" t="s">
+      <c r="G6" s="118"/>
+      <c r="H6" s="118"/>
+      <c r="I6" s="119"/>
+      <c r="J6" s="111" t="s">
         <v>30</v>
       </c>
-      <c r="K6" s="111"/>
-      <c r="L6" s="112"/>
+      <c r="K6" s="112"/>
+      <c r="L6" s="113"/>
       <c r="M6" s="88"/>
-      <c r="N6" s="106" t="s">
+      <c r="N6" s="107" t="s">
         <v>42</v>
       </c>
       <c r="O6" s="108"/>
-      <c r="P6" s="106" t="s">
-        <v>105</v>
-      </c>
-      <c r="Q6" s="107"/>
+      <c r="P6" s="107" t="s">
+        <v>104</v>
+      </c>
+      <c r="Q6" s="109"/>
       <c r="R6" s="108"/>
       <c r="S6" s="88"/>
-      <c r="T6" s="106" t="s">
-        <v>122</v>
+      <c r="T6" s="107" t="s">
+        <v>121</v>
       </c>
       <c r="U6" s="108"/>
-      <c r="V6" s="113"/>
-      <c r="W6" s="114"/>
-      <c r="X6" s="114"/>
-      <c r="Y6" s="115"/>
+      <c r="V6" s="114"/>
+      <c r="W6" s="115"/>
+      <c r="X6" s="115"/>
+      <c r="Y6" s="116"/>
     </row>
     <row r="7" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B7" s="75" t="s">
@@ -5672,52 +5690,52 @@
         <v>29</v>
       </c>
       <c r="F7" s="77" t="s">
+        <v>115</v>
+      </c>
+      <c r="G7" s="77" t="s">
+        <v>119</v>
+      </c>
+      <c r="H7" s="77" t="s">
+        <v>120</v>
+      </c>
+      <c r="I7" s="77" t="s">
         <v>116</v>
       </c>
-      <c r="G7" s="77" t="s">
-        <v>120</v>
-      </c>
-      <c r="H7" s="77" t="s">
-        <v>121</v>
-      </c>
-      <c r="I7" s="77" t="s">
-        <v>117</v>
-      </c>
       <c r="J7" s="77" t="s">
+        <v>112</v>
+      </c>
+      <c r="K7" s="77" t="s">
         <v>113</v>
       </c>
-      <c r="K7" s="77" t="s">
+      <c r="L7" s="77" t="s">
         <v>114</v>
-      </c>
-      <c r="L7" s="77" t="s">
-        <v>115</v>
       </c>
       <c r="M7" s="76" t="s">
         <v>53</v>
       </c>
       <c r="N7" s="77" t="s">
+        <v>117</v>
+      </c>
+      <c r="O7" s="77" t="s">
         <v>118</v>
       </c>
-      <c r="O7" s="77" t="s">
-        <v>119</v>
-      </c>
       <c r="P7" s="77" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q7" s="77" t="s">
         <v>113</v>
       </c>
-      <c r="Q7" s="77" t="s">
+      <c r="R7" s="77" t="s">
         <v>114</v>
       </c>
-      <c r="R7" s="77" t="s">
-        <v>115</v>
-      </c>
       <c r="S7" s="75" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="T7" s="77" t="s">
+        <v>122</v>
+      </c>
+      <c r="U7" s="77" t="s">
         <v>123</v>
-      </c>
-      <c r="U7" s="77" t="s">
-        <v>124</v>
       </c>
       <c r="V7" s="76" t="s">
         <v>70</v>
@@ -5726,10 +5744,10 @@
         <v>32</v>
       </c>
       <c r="X7" s="75" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="Y7" s="75" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="8" spans="2:25" x14ac:dyDescent="0.25">
@@ -5760,17 +5778,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B2:P2"/>
+    <mergeCell ref="B3:P3"/>
+    <mergeCell ref="B5:L5"/>
+    <mergeCell ref="J6:L6"/>
+    <mergeCell ref="F6:I6"/>
     <mergeCell ref="N6:O6"/>
     <mergeCell ref="P6:R6"/>
     <mergeCell ref="B6:E6"/>
     <mergeCell ref="T6:U6"/>
     <mergeCell ref="M5:Y5"/>
     <mergeCell ref="V6:Y6"/>
-    <mergeCell ref="B2:P2"/>
-    <mergeCell ref="B3:P3"/>
-    <mergeCell ref="B5:L5"/>
-    <mergeCell ref="J6:L6"/>
-    <mergeCell ref="F6:I6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -5887,60 +5905,60 @@
   <sheetData>
     <row r="1" spans="2:16" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="96"/>
-      <c r="C2" s="96"/>
-      <c r="D2" s="96"/>
-      <c r="E2" s="96"/>
-      <c r="F2" s="96"/>
-      <c r="G2" s="96"/>
-      <c r="H2" s="96"/>
-      <c r="I2" s="96"/>
-      <c r="J2" s="96"/>
-      <c r="K2" s="96"/>
-      <c r="L2" s="96"/>
-      <c r="M2" s="96"/>
-      <c r="N2" s="96"/>
-      <c r="O2" s="96"/>
-      <c r="P2" s="96"/>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
+      <c r="F2" s="97"/>
+      <c r="G2" s="97"/>
+      <c r="H2" s="97"/>
+      <c r="I2" s="97"/>
+      <c r="J2" s="97"/>
+      <c r="K2" s="97"/>
+      <c r="L2" s="97"/>
+      <c r="M2" s="97"/>
+      <c r="N2" s="97"/>
+      <c r="O2" s="97"/>
+      <c r="P2" s="97"/>
     </row>
     <row r="3" spans="2:16" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="97" t="s">
+      <c r="B3" s="98" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="97"/>
-      <c r="D3" s="97"/>
-      <c r="E3" s="97"/>
-      <c r="F3" s="97"/>
-      <c r="G3" s="97"/>
-      <c r="H3" s="97"/>
-      <c r="I3" s="97"/>
-      <c r="J3" s="97"/>
-      <c r="K3" s="97"/>
-      <c r="L3" s="97"/>
-      <c r="M3" s="97"/>
-      <c r="N3" s="97"/>
-      <c r="O3" s="97"/>
-      <c r="P3" s="97"/>
+      <c r="C3" s="98"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="98"/>
+      <c r="F3" s="98"/>
+      <c r="G3" s="98"/>
+      <c r="H3" s="98"/>
+      <c r="I3" s="98"/>
+      <c r="J3" s="98"/>
+      <c r="K3" s="98"/>
+      <c r="L3" s="98"/>
+      <c r="M3" s="98"/>
+      <c r="N3" s="98"/>
+      <c r="O3" s="98"/>
+      <c r="P3" s="98"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="44" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="D5" s="44" t="s">
         <v>80</v>
       </c>
-      <c r="D5" s="44" t="s">
+      <c r="E5" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="F5" s="4" t="s">
         <v>82</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>83</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>44</v>
@@ -5952,7 +5970,7 @@
         <v>15</v>
       </c>
       <c r="J5" s="45" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
@@ -5999,48 +6017,48 @@
   <sheetData>
     <row r="1" spans="2:16" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="96"/>
-      <c r="C2" s="96"/>
-      <c r="D2" s="96"/>
-      <c r="E2" s="96"/>
-      <c r="F2" s="96"/>
-      <c r="G2" s="96"/>
-      <c r="H2" s="96"/>
-      <c r="I2" s="96"/>
-      <c r="J2" s="96"/>
-      <c r="K2" s="96"/>
-      <c r="L2" s="96"/>
-      <c r="M2" s="96"/>
-      <c r="N2" s="96"/>
-      <c r="O2" s="96"/>
-      <c r="P2" s="96"/>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
+      <c r="F2" s="97"/>
+      <c r="G2" s="97"/>
+      <c r="H2" s="97"/>
+      <c r="I2" s="97"/>
+      <c r="J2" s="97"/>
+      <c r="K2" s="97"/>
+      <c r="L2" s="97"/>
+      <c r="M2" s="97"/>
+      <c r="N2" s="97"/>
+      <c r="O2" s="97"/>
+      <c r="P2" s="97"/>
     </row>
     <row r="3" spans="2:16" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="97" t="s">
+      <c r="B3" s="98" t="s">
         <v>68</v>
       </c>
-      <c r="C3" s="97"/>
-      <c r="D3" s="97"/>
-      <c r="E3" s="97"/>
-      <c r="F3" s="97"/>
-      <c r="G3" s="97"/>
-      <c r="H3" s="97"/>
-      <c r="I3" s="97"/>
-      <c r="J3" s="97"/>
-      <c r="K3" s="97"/>
-      <c r="L3" s="97"/>
-      <c r="M3" s="97"/>
-      <c r="N3" s="97"/>
-      <c r="O3" s="97"/>
-      <c r="P3" s="97"/>
+      <c r="C3" s="98"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="98"/>
+      <c r="F3" s="98"/>
+      <c r="G3" s="98"/>
+      <c r="H3" s="98"/>
+      <c r="I3" s="98"/>
+      <c r="J3" s="98"/>
+      <c r="K3" s="98"/>
+      <c r="L3" s="98"/>
+      <c r="M3" s="98"/>
+      <c r="N3" s="98"/>
+      <c r="O3" s="98"/>
+      <c r="P3" s="98"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>24</v>
@@ -6081,44 +6099,44 @@
   <sheetData>
     <row r="1" spans="2:16" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="96"/>
-      <c r="C2" s="96"/>
-      <c r="D2" s="96"/>
-      <c r="E2" s="96"/>
-      <c r="F2" s="96"/>
-      <c r="G2" s="96"/>
-      <c r="H2" s="96"/>
-      <c r="I2" s="96"/>
-      <c r="J2" s="96"/>
-      <c r="K2" s="96"/>
-      <c r="L2" s="96"/>
-      <c r="M2" s="96"/>
-      <c r="N2" s="96"/>
-      <c r="O2" s="96"/>
-      <c r="P2" s="96"/>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
+      <c r="F2" s="97"/>
+      <c r="G2" s="97"/>
+      <c r="H2" s="97"/>
+      <c r="I2" s="97"/>
+      <c r="J2" s="97"/>
+      <c r="K2" s="97"/>
+      <c r="L2" s="97"/>
+      <c r="M2" s="97"/>
+      <c r="N2" s="97"/>
+      <c r="O2" s="97"/>
+      <c r="P2" s="97"/>
     </row>
     <row r="3" spans="2:16" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="97" t="s">
+      <c r="B3" s="98" t="s">
         <v>71</v>
       </c>
-      <c r="C3" s="97"/>
-      <c r="D3" s="97"/>
-      <c r="E3" s="97"/>
-      <c r="F3" s="97"/>
-      <c r="G3" s="97"/>
-      <c r="H3" s="97"/>
-      <c r="I3" s="97"/>
-      <c r="J3" s="97"/>
-      <c r="K3" s="97"/>
-      <c r="L3" s="97"/>
-      <c r="M3" s="97"/>
-      <c r="N3" s="97"/>
-      <c r="O3" s="97"/>
-      <c r="P3" s="97"/>
+      <c r="C3" s="98"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="98"/>
+      <c r="F3" s="98"/>
+      <c r="G3" s="98"/>
+      <c r="H3" s="98"/>
+      <c r="I3" s="98"/>
+      <c r="J3" s="98"/>
+      <c r="K3" s="98"/>
+      <c r="L3" s="98"/>
+      <c r="M3" s="98"/>
+      <c r="N3" s="98"/>
+      <c r="O3" s="98"/>
+      <c r="P3" s="98"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
@@ -6169,51 +6187,51 @@
   <sheetData>
     <row r="1" spans="2:16" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="96"/>
-      <c r="C2" s="96"/>
-      <c r="D2" s="96"/>
-      <c r="E2" s="96"/>
-      <c r="F2" s="96"/>
-      <c r="G2" s="96"/>
-      <c r="H2" s="96"/>
-      <c r="I2" s="96"/>
-      <c r="J2" s="96"/>
-      <c r="K2" s="96"/>
-      <c r="L2" s="96"/>
-      <c r="M2" s="96"/>
-      <c r="N2" s="96"/>
-      <c r="O2" s="96"/>
-      <c r="P2" s="96"/>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
+      <c r="F2" s="97"/>
+      <c r="G2" s="97"/>
+      <c r="H2" s="97"/>
+      <c r="I2" s="97"/>
+      <c r="J2" s="97"/>
+      <c r="K2" s="97"/>
+      <c r="L2" s="97"/>
+      <c r="M2" s="97"/>
+      <c r="N2" s="97"/>
+      <c r="O2" s="97"/>
+      <c r="P2" s="97"/>
     </row>
     <row r="3" spans="2:16" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="97" t="s">
+      <c r="B3" s="98" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="97"/>
-      <c r="D3" s="97"/>
-      <c r="E3" s="97"/>
-      <c r="F3" s="97"/>
-      <c r="G3" s="97"/>
-      <c r="H3" s="97"/>
-      <c r="I3" s="97"/>
-      <c r="J3" s="97"/>
-      <c r="K3" s="97"/>
-      <c r="L3" s="97"/>
-      <c r="M3" s="97"/>
-      <c r="N3" s="97"/>
-      <c r="O3" s="97"/>
-      <c r="P3" s="97"/>
+      <c r="C3" s="98"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="98"/>
+      <c r="F3" s="98"/>
+      <c r="G3" s="98"/>
+      <c r="H3" s="98"/>
+      <c r="I3" s="98"/>
+      <c r="J3" s="98"/>
+      <c r="K3" s="98"/>
+      <c r="L3" s="98"/>
+      <c r="M3" s="98"/>
+      <c r="N3" s="98"/>
+      <c r="O3" s="98"/>
+      <c r="P3" s="98"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="44" t="s">
+        <v>85</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>86</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>87</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>16</v>
@@ -6237,16 +6255,16 @@
         <v>22</v>
       </c>
       <c r="K5" s="91" t="s">
+        <v>191</v>
+      </c>
+      <c r="L5" s="91" t="s">
         <v>192</v>
       </c>
-      <c r="L5" s="91" t="s">
-        <v>193</v>
-      </c>
       <c r="M5" s="45" t="s">
+        <v>133</v>
+      </c>
+      <c r="N5" s="45" t="s">
         <v>134</v>
-      </c>
-      <c r="N5" s="45" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
@@ -6299,44 +6317,44 @@
   <sheetData>
     <row r="1" spans="2:16" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="96"/>
-      <c r="C2" s="96"/>
-      <c r="D2" s="96"/>
-      <c r="E2" s="96"/>
-      <c r="F2" s="96"/>
-      <c r="G2" s="96"/>
-      <c r="H2" s="96"/>
-      <c r="I2" s="96"/>
-      <c r="J2" s="96"/>
-      <c r="K2" s="96"/>
-      <c r="L2" s="96"/>
-      <c r="M2" s="96"/>
-      <c r="N2" s="96"/>
-      <c r="O2" s="96"/>
-      <c r="P2" s="96"/>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
+      <c r="F2" s="97"/>
+      <c r="G2" s="97"/>
+      <c r="H2" s="97"/>
+      <c r="I2" s="97"/>
+      <c r="J2" s="97"/>
+      <c r="K2" s="97"/>
+      <c r="L2" s="97"/>
+      <c r="M2" s="97"/>
+      <c r="N2" s="97"/>
+      <c r="O2" s="97"/>
+      <c r="P2" s="97"/>
     </row>
     <row r="3" spans="2:16" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="97" t="s">
+      <c r="B3" s="98" t="s">
         <v>65</v>
       </c>
-      <c r="C3" s="97"/>
-      <c r="D3" s="97"/>
-      <c r="E3" s="97"/>
-      <c r="F3" s="97"/>
-      <c r="G3" s="97"/>
-      <c r="H3" s="97"/>
-      <c r="I3" s="97"/>
-      <c r="J3" s="97"/>
-      <c r="K3" s="97"/>
-      <c r="L3" s="97"/>
-      <c r="M3" s="97"/>
-      <c r="N3" s="97"/>
-      <c r="O3" s="97"/>
-      <c r="P3" s="97"/>
+      <c r="C3" s="98"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="98"/>
+      <c r="F3" s="98"/>
+      <c r="G3" s="98"/>
+      <c r="H3" s="98"/>
+      <c r="I3" s="98"/>
+      <c r="J3" s="98"/>
+      <c r="K3" s="98"/>
+      <c r="L3" s="98"/>
+      <c r="M3" s="98"/>
+      <c r="N3" s="98"/>
+      <c r="O3" s="98"/>
+      <c r="P3" s="98"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="45" t="s">
@@ -6387,32 +6405,32 @@
   <sheetData>
     <row r="1" spans="2:11" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="98"/>
-      <c r="C2" s="98"/>
-      <c r="D2" s="98"/>
-      <c r="E2" s="98"/>
-      <c r="F2" s="98"/>
-      <c r="G2" s="98"/>
-      <c r="H2" s="98"/>
-      <c r="I2" s="98"/>
+      <c r="B2" s="99"/>
+      <c r="C2" s="99"/>
+      <c r="D2" s="99"/>
+      <c r="E2" s="99"/>
+      <c r="F2" s="99"/>
+      <c r="G2" s="99"/>
+      <c r="H2" s="99"/>
+      <c r="I2" s="99"/>
       <c r="J2" s="84"/>
       <c r="K2" s="84"/>
     </row>
     <row r="3" spans="2:11" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="97" t="s">
+      <c r="B3" s="98" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="97"/>
-      <c r="D3" s="97"/>
-      <c r="E3" s="97"/>
-      <c r="F3" s="97"/>
-      <c r="G3" s="97"/>
-      <c r="H3" s="97"/>
-      <c r="I3" s="97"/>
+      <c r="C3" s="98"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="98"/>
+      <c r="F3" s="98"/>
+      <c r="G3" s="98"/>
+      <c r="H3" s="98"/>
+      <c r="I3" s="98"/>
       <c r="J3" s="83"/>
       <c r="K3" s="83"/>
     </row>
@@ -6421,7 +6439,7 @@
         <v>77</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
TRIEDA-1702 - Criando importação e exportação das disponibilidades das salas.
</commit_message>
<xml_diff>
--- a/code/client/web/src/main/resources/templateExport.xlsx
+++ b/code/client/web/src/main/resources/templateExport.xlsx
@@ -4,40 +4,41 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="17070" windowHeight="5370" tabRatio="907" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="17070" windowHeight="5370" tabRatio="954" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Campi" sheetId="3" r:id="rId1"/>
     <sheet name="Unidades" sheetId="1" r:id="rId2"/>
     <sheet name="Salas" sheetId="4" r:id="rId3"/>
-    <sheet name="Cursos" sheetId="5" r:id="rId4"/>
-    <sheet name="Areas de Titulacao" sheetId="16" r:id="rId5"/>
-    <sheet name="Curso - Area de Titulacao" sheetId="19" r:id="rId6"/>
-    <sheet name="Disciplinas" sheetId="6" r:id="rId7"/>
-    <sheet name="Equivalencias" sheetId="17" r:id="rId8"/>
-    <sheet name="Disciplinas-Salas" sheetId="9" r:id="rId9"/>
-    <sheet name="Curriculos" sheetId="7" r:id="rId10"/>
-    <sheet name="Ofertas e Demandas" sheetId="8" r:id="rId11"/>
-    <sheet name="Alunos" sheetId="27" r:id="rId12"/>
-    <sheet name="Demanda por Aluno" sheetId="22" r:id="rId13"/>
-    <sheet name="Professores" sheetId="12" r:id="rId14"/>
-    <sheet name="Disponibilidades Professores" sheetId="28" r:id="rId15"/>
-    <sheet name="Campi de Trabalho" sheetId="18" r:id="rId16"/>
-    <sheet name="Habilitacao dos Professores" sheetId="13" r:id="rId17"/>
-    <sheet name="Resumo por curso" sheetId="14" r:id="rId18"/>
-    <sheet name="Resumo por disciplina" sheetId="15" r:id="rId19"/>
-    <sheet name="Atendimentos por Matricula" sheetId="30" r:id="rId20"/>
-    <sheet name="Atendimentos por Disciplina" sheetId="31" r:id="rId21"/>
-    <sheet name="Atendimentos Faixa de Demanda" sheetId="32" r:id="rId22"/>
-    <sheet name="Atendimentos por Carga Horaria" sheetId="35" r:id="rId23"/>
-    <sheet name="Porcentagem Mestres e Doutores" sheetId="33" r:id="rId24"/>
-    <sheet name="Relatorio Visao Sala" sheetId="10" r:id="rId25"/>
-    <sheet name="Relatorio Visao Aluno" sheetId="25" r:id="rId26"/>
-    <sheet name="Relatorio Visao Professor" sheetId="21" r:id="rId27"/>
-    <sheet name="Relatorio Visao Curso" sheetId="20" r:id="rId28"/>
-    <sheet name="Atendimentos por Aluno" sheetId="23" r:id="rId29"/>
-    <sheet name="Aulas" sheetId="26" r:id="rId30"/>
-    <sheet name="PaletaCores" sheetId="11" r:id="rId31"/>
+    <sheet name="Disponibilidades Salas" sheetId="36" r:id="rId4"/>
+    <sheet name="Cursos" sheetId="5" r:id="rId5"/>
+    <sheet name="Areas de Titulacao" sheetId="16" r:id="rId6"/>
+    <sheet name="Curso - Area de Titulacao" sheetId="19" r:id="rId7"/>
+    <sheet name="Disciplinas" sheetId="6" r:id="rId8"/>
+    <sheet name="Equivalencias" sheetId="17" r:id="rId9"/>
+    <sheet name="Disciplinas-Salas" sheetId="9" r:id="rId10"/>
+    <sheet name="Curriculos" sheetId="7" r:id="rId11"/>
+    <sheet name="Ofertas e Demandas" sheetId="8" r:id="rId12"/>
+    <sheet name="Alunos" sheetId="27" r:id="rId13"/>
+    <sheet name="Demanda por Aluno" sheetId="22" r:id="rId14"/>
+    <sheet name="Professores" sheetId="12" r:id="rId15"/>
+    <sheet name="Disponibilidades Professores" sheetId="28" r:id="rId16"/>
+    <sheet name="Campi de Trabalho" sheetId="18" r:id="rId17"/>
+    <sheet name="Habilitacao dos Professores" sheetId="13" r:id="rId18"/>
+    <sheet name="Resumo por curso" sheetId="14" r:id="rId19"/>
+    <sheet name="Resumo por disciplina" sheetId="15" r:id="rId20"/>
+    <sheet name="Atendimentos por Matricula" sheetId="30" r:id="rId21"/>
+    <sheet name="Atendimentos por Disciplina" sheetId="31" r:id="rId22"/>
+    <sheet name="Atendimentos Faixa de Demanda" sheetId="32" r:id="rId23"/>
+    <sheet name="Atendimentos por Carga Horaria" sheetId="35" r:id="rId24"/>
+    <sheet name="Porcentagem Mestres e Doutores" sheetId="33" r:id="rId25"/>
+    <sheet name="Relatorio Visao Sala" sheetId="10" r:id="rId26"/>
+    <sheet name="Relatorio Visao Aluno" sheetId="25" r:id="rId27"/>
+    <sheet name="Relatorio Visao Professor" sheetId="21" r:id="rId28"/>
+    <sheet name="Relatorio Visao Curso" sheetId="20" r:id="rId29"/>
+    <sheet name="Atendimentos por Aluno" sheetId="23" r:id="rId30"/>
+    <sheet name="Aulas" sheetId="26" r:id="rId31"/>
+    <sheet name="PaletaCores" sheetId="11" r:id="rId32"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
@@ -105,7 +106,7 @@
     <author>Autor</author>
   </authors>
   <commentList>
-    <comment ref="D5" authorId="0">
+    <comment ref="C5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -115,45 +116,23 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">OPCIONAL:
+          <t>1 = DOMINGO
+2 = SEGUNDA
+3 = TERÇA
+4 = QUARTA
+5 = QUINTA
+6 = SEXTA
+7 = SÁBADO</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
 </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Preferência do professor em ministrar a disciplina.
-Maior Preferência = 10
-Menor preferência = 1
-Para desconsiderar este critério, manter todas as preferências iguais a 1.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E5" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">OPCIONAL:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Nota da avaliação de desempenho do professor na disciplina, em períodos passados.
-Para desconsiderar este critério, manter todas as notas iguais a 1.</t>
         </r>
       </text>
     </comment>
@@ -167,8 +146,57 @@
     <author>Autor</author>
   </authors>
   <commentList>
-    <comment ref="Z1" authorId="0">
-      <text/>
+    <comment ref="D5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">OPCIONAL:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Preferência do professor em ministrar a disciplina.
+Maior Preferência = 10
+Menor preferência = 1
+Para desconsiderar este critério, manter todas as preferências iguais a 1.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">OPCIONAL:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Nota da avaliação de desempenho do professor na disciplina, em períodos passados.
+Para desconsiderar este critério, manter todas as notas iguais a 1.</t>
+        </r>
+      </text>
     </comment>
   </commentList>
 </comments>
@@ -213,6 +241,19 @@
 </comments>
 </file>
 
+<file path=xl/comments15.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Autor</author>
+  </authors>
+  <commentList>
+    <comment ref="Z1" authorId="0">
+      <text/>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
@@ -414,7 +455,7 @@
     <author>Autor</author>
   </authors>
   <commentList>
-    <comment ref="B5" authorId="0">
+    <comment ref="C5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -424,181 +465,23 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">Código único do curso </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>no sistema legado da instituição de ensino.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D5" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Neste campo é necessário inserir o </t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Código do Tipo de Curso</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">.
-Os valores permitidos são aqueles que já foram cadastrados pelo usuário na base de dados do Trieda. Para consultá-los, basta acessar a opção </t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Tipos de Curso</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> da aba </t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Cursos</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> do menu </t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Master Data</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> do </t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Trieda Web</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>.
-obs: qualquer valor diferente dos valores permitidos impossibiltará a importação dos dados pelo Trieda Web e disponibilizará uma mensagem de erro para o usuário.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I5" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Máximo de disciplinas</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> que um mesmo professor pode ministrar para o mesmo curso.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="J5" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Permitir que um professor ministre </t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>mais de 1 disciplina para um curso, no mesmo período</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>.</t>
+          <t>1 = DOMINGO
+2 = SEGUNDA
+3 = TERÇA
+4 = QUARTA
+5 = QUINTA
+6 = SEXTA
+7 = SÁBADO</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
         </r>
       </text>
     </comment>
@@ -622,45 +505,49 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Código único da disciplina</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> no sistema legado da instituição de ensino.</t>
+          <t xml:space="preserve">Código único do curso </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>no sistema legado da instituição de ensino.</t>
         </r>
       </text>
     </comment>
-    <comment ref="F5" authorId="0">
+    <comment ref="D5" authorId="0">
       <text>
         <r>
           <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Neste campo é necessário inserir o </t>
+        </r>
+        <r>
+          <rPr>
             <b/>
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">Sim
-Não
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Aplicado somente aos créditos práticos.
-Os créditos teóricos serão sempre alocados em Salas de Aula.
-Disciplinas que possuem créditos práticos, com a opção "Não" neste campo, terão seus créditos práticos tratados como teóricos.
-</t>
+          <t>Código do Tipo de Curso</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">.
+Os valores permitidos são aqueles que já foram cadastrados pelo usuário na base de dados do Trieda. Para consultá-los, basta acessar a opção </t>
         </r>
         <r>
           <rPr>
@@ -670,20 +557,16 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Disciplinas com a opção "Sim" neste campo deverão possuir Laboratório associado, na aba "Disciplinas-Salas".</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G5" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Neste campo é necessário inserir o </t>
+          <t>Tipos de Curso</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> da aba </t>
         </r>
         <r>
           <rPr>
@@ -693,17 +576,16 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Tipo da Disciplina</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">. Os valores permitidos são: 
-- </t>
+          <t>Cursos</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> do menu </t>
         </r>
         <r>
           <rPr>
@@ -713,17 +595,16 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Presencial</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-- </t>
+          <t>Master Data</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> do </t>
         </r>
         <r>
           <rPr>
@@ -733,148 +614,16 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Online</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-- </t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Telepresencial</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-obs: qualquer valor diferente dos valores permitidos impossibiltará a importação dos dados pelo Trieda Web e disponibilizará uma mensagem de erro para o usuário.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H5" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Trata-se de um </t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>campo Opcional</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">. Este campo representa o </t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Nível de Dificuldade da Disciplina</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">. Os valores permitidos são: 
-- </t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>BAIXO</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-- </t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>MEDIO</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-- </t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>ALTO</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
+          <t>Trieda Web</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>.
 obs: qualquer valor diferente dos valores permitidos impossibiltará a importação dos dados pelo Trieda Web e disponibilizará uma mensagem de erro para o usuário.</t>
         </r>
       </text>
@@ -889,9 +638,16 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>OPCIONAL:
-Restrição pedagógica do número máximo de alunos em sala de aula para uma disciplina específica. 
-Quanto omitido, o TRIEDA assume a capacidade da sala alocada.</t>
+          <t>Máximo de disciplinas</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> que um mesmo professor pode ministrar para o mesmo curso.</t>
         </r>
       </text>
     </comment>
@@ -899,79 +655,31 @@
       <text>
         <r>
           <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Permitir que um professor ministre </t>
+        </r>
+        <r>
+          <rPr>
             <b/>
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>OPCIONAL:
-Restrição pedagógica do número máximo de alunos em sala de aula para uma disciplina específica. 
-Quanto omitido, o TRIEDA assume a capacidade do laboratório alocado.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="K5" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Sim
-Não
-Determina se as aulas teoricas e praticas devem ser lecionadas em sequencia</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="L5" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Sim
-Não
-Determina se o professor deve ser o mesmo para as aulas teoricas e praticas</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="M5" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Sim
-Não
-Determina se a disciplina deverá herdar os horários das semanas letivas também no sábado.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="N5" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Sim
-Não
-Determina se a disciplina deverá herdar os horários das semanas letivas também no domingo.</t>
+          <t>mais de 1 disciplina para um curso, no mesmo período</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>.</t>
         </r>
       </text>
     </comment>
@@ -995,11 +703,20 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Código da disciplina cursada</t>
+          <t>Código único da disciplina</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> no sistema legado da instituição de ensino.</t>
         </r>
       </text>
     </comment>
-    <comment ref="C5" authorId="0">
+    <comment ref="F5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1009,21 +726,333 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Código da disciplina eliminada</t>
+          <t xml:space="preserve">Sim
+Não
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Aplicado somente aos créditos práticos.
+Os créditos teóricos serão sempre alocados em Salas de Aula.
+Disciplinas que possuem créditos práticos, com a opção "Não" neste campo, terão seus créditos práticos tratados como teóricos.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Disciplinas com a opção "Sim" neste campo deverão possuir Laboratório associado, na aba "Disciplinas-Salas".</t>
         </r>
       </text>
     </comment>
-    <comment ref="D5" authorId="0">
+    <comment ref="G5" authorId="0">
       <text>
         <r>
           <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Neste campo é necessário inserir o </t>
+        </r>
+        <r>
+          <rPr>
             <b/>
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Código do Curso relacionado a equivalencia, Vazio significa uma equivalencia geral</t>
+          <t>Tipo da Disciplina</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">. Os valores permitidos são: 
+- </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Presencial</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+- </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Online</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+- </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Telepresencial</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+obs: qualquer valor diferente dos valores permitidos impossibiltará a importação dos dados pelo Trieda Web e disponibilizará uma mensagem de erro para o usuário.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Trata-se de um </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>campo Opcional</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">. Este campo representa o </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Nível de Dificuldade da Disciplina</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">. Os valores permitidos são: 
+- </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>BAIXO</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+- </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>MEDIO</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+- </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>ALTO</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+obs: qualquer valor diferente dos valores permitidos impossibiltará a importação dos dados pelo Trieda Web e disponibilizará uma mensagem de erro para o usuário.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>OPCIONAL:
+Restrição pedagógica do número máximo de alunos em sala de aula para uma disciplina específica. 
+Quanto omitido, o TRIEDA assume a capacidade da sala alocada.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>OPCIONAL:
+Restrição pedagógica do número máximo de alunos em sala de aula para uma disciplina específica. 
+Quanto omitido, o TRIEDA assume a capacidade do laboratório alocado.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Sim
+Não
+Determina se as aulas teoricas e praticas devem ser lecionadas em sequencia</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Sim
+Não
+Determina se o professor deve ser o mesmo para as aulas teoricas e praticas</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sim
+Não
+Determina se a disciplina deverá herdar os horários das semanas letivas também no sábado.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sim
+Não
+Determina se a disciplina deverá herdar os horários das semanas letivas também no domingo.</t>
         </r>
       </text>
     </comment>
@@ -1037,17 +1066,45 @@
     <author>Autor</author>
   </authors>
   <commentList>
-    <comment ref="I5" authorId="0">
+    <comment ref="B5" authorId="0">
       <text>
         <r>
           <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Receita Semanal por Crédito e Aluno (em Reais)
-</t>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Código da disciplina cursada</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Código da disciplina eliminada</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Código do Curso relacionado a equivalencia, Vazio significa uma equivalencia geral</t>
         </r>
       </text>
     </comment>
@@ -1061,159 +1118,17 @@
     <author>Autor</author>
   </authors>
   <commentList>
-    <comment ref="D5" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Neste campo é necessário inserir o </t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Tipo de Contrato do Professor</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">. Os valores permitidos são: 
-- </t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Horista</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-- </t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Integral</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-obs: qualquer valor diferente dos valores permitidos impossibiltará a importação dos dados pelo Trieda Web e disponibilizará uma mensagem de erro para o usuário.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E5" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Em créditos semanais</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F5" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Em créditos semanais</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="I5" authorId="0">
       <text>
         <r>
           <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">OPCIONAL:
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Receita Semanal por Crédito e Aluno (em Reais)
 </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Nota consolidada da avaliação de desempenho do professor.
-Melhor desempenho = 10
-Pior desempenho = 1
-Para desconsiderar este critério, manter todas as notas iguais a 1.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="J5" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Em créditos semanais</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="K5" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Apenas custo do professor em sala de aula.</t>
         </r>
       </text>
     </comment>
@@ -1227,23 +1142,46 @@
     <author>Autor</author>
   </authors>
   <commentList>
-    <comment ref="C5" authorId="0">
+    <comment ref="D5" authorId="0">
       <text>
         <r>
           <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Neste campo é necessário inserir o </t>
+        </r>
+        <r>
+          <rPr>
             <b/>
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>1 = DOMINGO
-2 = SEGUNDA
-3 = TERÇA
-4 = QUARTA
-5 = QUINTA
-6 = SEXTA
-7 = SÁBADO</t>
+          <t>Tipo de Contrato do Professor</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">. Os valores permitidos são: 
+- </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Horista</t>
         </r>
         <r>
           <rPr>
@@ -1253,7 +1191,110 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
+- </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Integral</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+obs: qualquer valor diferente dos valores permitidos impossibiltará a importação dos dados pelo Trieda Web e disponibilizará uma mensagem de erro para o usuário.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Em créditos semanais</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Em créditos semanais</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">OPCIONAL:
 </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Nota consolidada da avaliação de desempenho do professor.
+Melhor desempenho = 10
+Pior desempenho = 1
+Para desconsiderar este critério, manter todas as notas iguais a 1.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Em créditos semanais</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Apenas custo do professor em sala de aula.</t>
         </r>
       </text>
     </comment>
@@ -1262,7 +1303,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="198">
   <si>
     <t>Planilha de Unidades</t>
   </si>
@@ -2285,7 +2326,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="120">
+  <cellXfs count="121">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2559,6 +2600,9 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2589,6 +2633,24 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="28" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2601,15 +2663,6 @@
     <xf numFmtId="0" fontId="0" fillId="28" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="28" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2617,15 +2670,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2955,38 +2999,38 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="97" t="s">
+      <c r="B2" s="98" t="s">
         <v>94</v>
       </c>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="97"/>
-      <c r="J2" s="97"/>
-      <c r="K2" s="97"/>
-      <c r="L2" s="97"/>
-      <c r="M2" s="97"/>
-      <c r="N2" s="97"/>
+      <c r="C2" s="98"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
+      <c r="F2" s="98"/>
+      <c r="G2" s="98"/>
+      <c r="H2" s="98"/>
+      <c r="I2" s="98"/>
+      <c r="J2" s="98"/>
+      <c r="K2" s="98"/>
+      <c r="L2" s="98"/>
+      <c r="M2" s="98"/>
+      <c r="N2" s="98"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="98" t="s">
+      <c r="B3" s="99" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="98"/>
-      <c r="F3" s="98"/>
-      <c r="G3" s="98"/>
-      <c r="H3" s="98"/>
-      <c r="I3" s="98"/>
-      <c r="J3" s="98"/>
-      <c r="K3" s="98"/>
-      <c r="L3" s="98"/>
-      <c r="M3" s="98"/>
-      <c r="N3" s="98"/>
+      <c r="C3" s="99"/>
+      <c r="D3" s="99"/>
+      <c r="E3" s="99"/>
+      <c r="F3" s="99"/>
+      <c r="G3" s="99"/>
+      <c r="H3" s="99"/>
+      <c r="I3" s="99"/>
+      <c r="J3" s="99"/>
+      <c r="K3" s="99"/>
+      <c r="L3" s="99"/>
+      <c r="M3" s="99"/>
+      <c r="N3" s="99"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="44" t="s">
@@ -3028,6 +3072,79 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:K6"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.85546875" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" customWidth="1"/>
+    <col min="3" max="3" width="23" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:11" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B1" s="46" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="100"/>
+      <c r="C2" s="100"/>
+      <c r="D2" s="100"/>
+      <c r="E2" s="100"/>
+      <c r="F2" s="100"/>
+      <c r="G2" s="100"/>
+      <c r="H2" s="100"/>
+      <c r="I2" s="100"/>
+      <c r="J2" s="84"/>
+      <c r="K2" s="84"/>
+    </row>
+    <row r="3" spans="2:11" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B3" s="99" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="99"/>
+      <c r="D3" s="99"/>
+      <c r="E3" s="99"/>
+      <c r="F3" s="99"/>
+      <c r="G3" s="99"/>
+      <c r="H3" s="99"/>
+      <c r="I3" s="99"/>
+      <c r="J3" s="83"/>
+      <c r="K3" s="83"/>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B5" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B6" s="2"/>
+      <c r="C6" s="8"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="B3:I3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:N6"/>
   <sheetViews>
@@ -3054,36 +3171,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="97"/>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="97"/>
-      <c r="J2" s="97"/>
-      <c r="K2" s="97"/>
-      <c r="L2" s="97"/>
-      <c r="M2" s="97"/>
-      <c r="N2" s="97"/>
+      <c r="B2" s="98"/>
+      <c r="C2" s="98"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
+      <c r="F2" s="98"/>
+      <c r="G2" s="98"/>
+      <c r="H2" s="98"/>
+      <c r="I2" s="98"/>
+      <c r="J2" s="98"/>
+      <c r="K2" s="98"/>
+      <c r="L2" s="98"/>
+      <c r="M2" s="98"/>
+      <c r="N2" s="98"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="98" t="s">
+      <c r="B3" s="99" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="98"/>
-      <c r="F3" s="98"/>
-      <c r="G3" s="98"/>
-      <c r="H3" s="98"/>
-      <c r="I3" s="98"/>
-      <c r="J3" s="98"/>
-      <c r="K3" s="98"/>
-      <c r="L3" s="98"/>
-      <c r="M3" s="98"/>
-      <c r="N3" s="98"/>
+      <c r="C3" s="99"/>
+      <c r="D3" s="99"/>
+      <c r="E3" s="99"/>
+      <c r="F3" s="99"/>
+      <c r="G3" s="99"/>
+      <c r="H3" s="99"/>
+      <c r="I3" s="99"/>
+      <c r="J3" s="99"/>
+      <c r="K3" s="99"/>
+      <c r="L3" s="99"/>
+      <c r="M3" s="99"/>
+      <c r="N3" s="99"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -3123,7 +3240,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:N6"/>
   <sheetViews>
@@ -3152,36 +3269,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="97"/>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="97"/>
-      <c r="J2" s="97"/>
-      <c r="K2" s="97"/>
-      <c r="L2" s="97"/>
-      <c r="M2" s="97"/>
-      <c r="N2" s="97"/>
+      <c r="B2" s="98"/>
+      <c r="C2" s="98"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
+      <c r="F2" s="98"/>
+      <c r="G2" s="98"/>
+      <c r="H2" s="98"/>
+      <c r="I2" s="98"/>
+      <c r="J2" s="98"/>
+      <c r="K2" s="98"/>
+      <c r="L2" s="98"/>
+      <c r="M2" s="98"/>
+      <c r="N2" s="98"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="98" t="s">
+      <c r="B3" s="99" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="98"/>
-      <c r="F3" s="98"/>
-      <c r="G3" s="98"/>
-      <c r="H3" s="98"/>
-      <c r="I3" s="98"/>
-      <c r="J3" s="98"/>
-      <c r="K3" s="98"/>
-      <c r="L3" s="98"/>
-      <c r="M3" s="98"/>
-      <c r="N3" s="98"/>
+      <c r="C3" s="99"/>
+      <c r="D3" s="99"/>
+      <c r="E3" s="99"/>
+      <c r="F3" s="99"/>
+      <c r="G3" s="99"/>
+      <c r="H3" s="99"/>
+      <c r="I3" s="99"/>
+      <c r="J3" s="99"/>
+      <c r="K3" s="99"/>
+      <c r="L3" s="99"/>
+      <c r="M3" s="99"/>
+      <c r="N3" s="99"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -3246,7 +3363,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E6"/>
   <sheetViews>
@@ -3266,18 +3383,18 @@
       </c>
     </row>
     <row r="2" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="97"/>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
+      <c r="B2" s="98"/>
+      <c r="C2" s="98"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
     </row>
     <row r="3" spans="2:5" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="98" t="s">
+      <c r="B3" s="99" t="s">
         <v>124</v>
       </c>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="98"/>
+      <c r="C3" s="99"/>
+      <c r="D3" s="99"/>
+      <c r="E3" s="99"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="60" t="s">
@@ -3304,7 +3421,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:N6"/>
   <sheetViews>
@@ -3330,36 +3447,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="97"/>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="97"/>
-      <c r="J2" s="97"/>
-      <c r="K2" s="97"/>
-      <c r="L2" s="97"/>
-      <c r="M2" s="97"/>
-      <c r="N2" s="97"/>
+      <c r="B2" s="98"/>
+      <c r="C2" s="98"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
+      <c r="F2" s="98"/>
+      <c r="G2" s="98"/>
+      <c r="H2" s="98"/>
+      <c r="I2" s="98"/>
+      <c r="J2" s="98"/>
+      <c r="K2" s="98"/>
+      <c r="L2" s="98"/>
+      <c r="M2" s="98"/>
+      <c r="N2" s="98"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="98" t="s">
+      <c r="B3" s="99" t="s">
         <v>98</v>
       </c>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="98"/>
-      <c r="F3" s="98"/>
-      <c r="G3" s="98"/>
-      <c r="H3" s="98"/>
-      <c r="I3" s="98"/>
-      <c r="J3" s="98"/>
-      <c r="K3" s="98"/>
-      <c r="L3" s="98"/>
-      <c r="M3" s="98"/>
-      <c r="N3" s="98"/>
+      <c r="C3" s="99"/>
+      <c r="D3" s="99"/>
+      <c r="E3" s="99"/>
+      <c r="F3" s="99"/>
+      <c r="G3" s="99"/>
+      <c r="H3" s="99"/>
+      <c r="I3" s="99"/>
+      <c r="J3" s="99"/>
+      <c r="K3" s="99"/>
+      <c r="L3" s="99"/>
+      <c r="M3" s="99"/>
+      <c r="N3" s="99"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -3392,10 +3509,10 @@
       <c r="K5" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="L5" s="100" t="s">
+      <c r="L5" s="101" t="s">
         <v>108</v>
       </c>
-      <c r="M5" s="100"/>
+      <c r="M5" s="101"/>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
@@ -3419,7 +3536,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O6"/>
   <sheetViews>
@@ -3450,38 +3567,38 @@
       </c>
     </row>
     <row r="2" spans="2:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="97"/>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="97"/>
-      <c r="J2" s="97"/>
-      <c r="K2" s="97"/>
-      <c r="L2" s="97"/>
-      <c r="M2" s="97"/>
-      <c r="N2" s="97"/>
-      <c r="O2" s="97"/>
+      <c r="B2" s="98"/>
+      <c r="C2" s="98"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
+      <c r="F2" s="98"/>
+      <c r="G2" s="98"/>
+      <c r="H2" s="98"/>
+      <c r="I2" s="98"/>
+      <c r="J2" s="98"/>
+      <c r="K2" s="98"/>
+      <c r="L2" s="98"/>
+      <c r="M2" s="98"/>
+      <c r="N2" s="98"/>
+      <c r="O2" s="98"/>
     </row>
     <row r="3" spans="2:15" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="98" t="s">
+      <c r="B3" s="99" t="s">
         <v>73</v>
       </c>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="98"/>
-      <c r="F3" s="98"/>
-      <c r="G3" s="98"/>
-      <c r="H3" s="98"/>
-      <c r="I3" s="98"/>
-      <c r="J3" s="98"/>
-      <c r="K3" s="98"/>
-      <c r="L3" s="98"/>
-      <c r="M3" s="98"/>
-      <c r="N3" s="98"/>
-      <c r="O3" s="98"/>
+      <c r="C3" s="99"/>
+      <c r="D3" s="99"/>
+      <c r="E3" s="99"/>
+      <c r="F3" s="99"/>
+      <c r="G3" s="99"/>
+      <c r="H3" s="99"/>
+      <c r="I3" s="99"/>
+      <c r="J3" s="99"/>
+      <c r="K3" s="99"/>
+      <c r="L3" s="99"/>
+      <c r="M3" s="99"/>
+      <c r="N3" s="99"/>
+      <c r="O3" s="99"/>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -3546,7 +3663,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
@@ -3568,18 +3685,18 @@
       </c>
     </row>
     <row r="2" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="97"/>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
+      <c r="B2" s="98"/>
+      <c r="C2" s="98"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
     </row>
     <row r="3" spans="2:5" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="98" t="s">
+      <c r="B3" s="99" t="s">
         <v>129</v>
       </c>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="98"/>
+      <c r="C3" s="99"/>
+      <c r="D3" s="99"/>
+      <c r="E3" s="99"/>
     </row>
     <row r="4" spans="2:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="64"/>
@@ -3614,7 +3731,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:N6"/>
   <sheetViews>
@@ -3641,36 +3758,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="97"/>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="97"/>
-      <c r="J2" s="97"/>
-      <c r="K2" s="97"/>
-      <c r="L2" s="97"/>
-      <c r="M2" s="97"/>
-      <c r="N2" s="97"/>
+      <c r="B2" s="98"/>
+      <c r="C2" s="98"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
+      <c r="F2" s="98"/>
+      <c r="G2" s="98"/>
+      <c r="H2" s="98"/>
+      <c r="I2" s="98"/>
+      <c r="J2" s="98"/>
+      <c r="K2" s="98"/>
+      <c r="L2" s="98"/>
+      <c r="M2" s="98"/>
+      <c r="N2" s="98"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="98" t="s">
+      <c r="B3" s="99" t="s">
         <v>69</v>
       </c>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="98"/>
-      <c r="F3" s="98"/>
-      <c r="G3" s="98"/>
-      <c r="H3" s="98"/>
-      <c r="I3" s="98"/>
-      <c r="J3" s="98"/>
-      <c r="K3" s="98"/>
-      <c r="L3" s="98"/>
-      <c r="M3" s="98"/>
-      <c r="N3" s="98"/>
+      <c r="C3" s="99"/>
+      <c r="D3" s="99"/>
+      <c r="E3" s="99"/>
+      <c r="F3" s="99"/>
+      <c r="G3" s="99"/>
+      <c r="H3" s="99"/>
+      <c r="I3" s="99"/>
+      <c r="J3" s="99"/>
+      <c r="K3" s="99"/>
+      <c r="L3" s="99"/>
+      <c r="M3" s="99"/>
+      <c r="N3" s="99"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -3698,7 +3815,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:N6"/>
   <sheetViews>
@@ -3725,36 +3842,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="97"/>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="97"/>
-      <c r="J2" s="97"/>
-      <c r="K2" s="97"/>
-      <c r="L2" s="97"/>
-      <c r="M2" s="97"/>
-      <c r="N2" s="97"/>
+      <c r="B2" s="98"/>
+      <c r="C2" s="98"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
+      <c r="F2" s="98"/>
+      <c r="G2" s="98"/>
+      <c r="H2" s="98"/>
+      <c r="I2" s="98"/>
+      <c r="J2" s="98"/>
+      <c r="K2" s="98"/>
+      <c r="L2" s="98"/>
+      <c r="M2" s="98"/>
+      <c r="N2" s="98"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="98" t="s">
+      <c r="B3" s="99" t="s">
         <v>74</v>
       </c>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="98"/>
-      <c r="F3" s="98"/>
-      <c r="G3" s="98"/>
-      <c r="H3" s="98"/>
-      <c r="I3" s="98"/>
-      <c r="J3" s="98"/>
-      <c r="K3" s="98"/>
-      <c r="L3" s="98"/>
-      <c r="M3" s="98"/>
-      <c r="N3" s="98"/>
+      <c r="C3" s="99"/>
+      <c r="D3" s="99"/>
+      <c r="E3" s="99"/>
+      <c r="F3" s="99"/>
+      <c r="G3" s="99"/>
+      <c r="H3" s="99"/>
+      <c r="I3" s="99"/>
+      <c r="J3" s="99"/>
+      <c r="K3" s="99"/>
+      <c r="L3" s="99"/>
+      <c r="M3" s="99"/>
+      <c r="N3" s="99"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -3787,7 +3904,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:R6"/>
   <sheetViews>
@@ -3823,40 +3940,40 @@
       </c>
     </row>
     <row r="2" spans="2:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="97"/>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="97"/>
-      <c r="J2" s="97"/>
-      <c r="K2" s="97"/>
-      <c r="L2" s="97"/>
-      <c r="M2" s="97"/>
-      <c r="N2" s="97"/>
-      <c r="O2" s="97"/>
-      <c r="P2" s="97"/>
+      <c r="B2" s="98"/>
+      <c r="C2" s="98"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
+      <c r="F2" s="98"/>
+      <c r="G2" s="98"/>
+      <c r="H2" s="98"/>
+      <c r="I2" s="98"/>
+      <c r="J2" s="98"/>
+      <c r="K2" s="98"/>
+      <c r="L2" s="98"/>
+      <c r="M2" s="98"/>
+      <c r="N2" s="98"/>
+      <c r="O2" s="98"/>
+      <c r="P2" s="98"/>
     </row>
     <row r="3" spans="2:18" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="98" t="s">
+      <c r="B3" s="99" t="s">
         <v>63</v>
       </c>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="98"/>
-      <c r="F3" s="98"/>
-      <c r="G3" s="98"/>
-      <c r="H3" s="98"/>
-      <c r="I3" s="98"/>
-      <c r="J3" s="98"/>
-      <c r="K3" s="98"/>
-      <c r="L3" s="98"/>
-      <c r="M3" s="98"/>
-      <c r="N3" s="98"/>
-      <c r="O3" s="98"/>
-      <c r="P3" s="98"/>
+      <c r="C3" s="99"/>
+      <c r="D3" s="99"/>
+      <c r="E3" s="99"/>
+      <c r="F3" s="99"/>
+      <c r="G3" s="99"/>
+      <c r="H3" s="99"/>
+      <c r="I3" s="99"/>
+      <c r="J3" s="99"/>
+      <c r="K3" s="99"/>
+      <c r="L3" s="99"/>
+      <c r="M3" s="99"/>
+      <c r="N3" s="99"/>
+      <c r="O3" s="99"/>
+      <c r="P3" s="99"/>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
@@ -3934,125 +4051,6 @@
   <mergeCells count="2">
     <mergeCell ref="B2:P2"/>
     <mergeCell ref="B3:P3"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:N6"/>
-  <sheetViews>
-    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:N2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="2.85546875" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:14" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="46" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="97"/>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="97"/>
-      <c r="J2" s="97"/>
-      <c r="K2" s="97"/>
-      <c r="L2" s="97"/>
-      <c r="M2" s="97"/>
-      <c r="N2" s="97"/>
-    </row>
-    <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="98" t="s">
-        <v>64</v>
-      </c>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="98"/>
-      <c r="F3" s="98"/>
-      <c r="G3" s="98"/>
-      <c r="H3" s="98"/>
-      <c r="I3" s="98"/>
-      <c r="J3" s="98"/>
-      <c r="K3" s="98"/>
-      <c r="L3" s="98"/>
-      <c r="M3" s="98"/>
-      <c r="N3" s="98"/>
-    </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B5" s="58" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="K5" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="L5" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="39"/>
-      <c r="I6" s="54"/>
-      <c r="J6" s="54"/>
-      <c r="K6" s="54"/>
-      <c r="L6" s="55"/>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B2:N2"/>
-    <mergeCell ref="B3:N3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -4086,38 +4084,38 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="97" t="s">
+      <c r="B2" s="98" t="s">
         <v>95</v>
       </c>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="97"/>
-      <c r="J2" s="97"/>
-      <c r="K2" s="97"/>
-      <c r="L2" s="97"/>
-      <c r="M2" s="97"/>
-      <c r="N2" s="97"/>
+      <c r="C2" s="98"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
+      <c r="F2" s="98"/>
+      <c r="G2" s="98"/>
+      <c r="H2" s="98"/>
+      <c r="I2" s="98"/>
+      <c r="J2" s="98"/>
+      <c r="K2" s="98"/>
+      <c r="L2" s="98"/>
+      <c r="M2" s="98"/>
+      <c r="N2" s="98"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="98" t="s">
+      <c r="B3" s="99" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="98"/>
-      <c r="F3" s="98"/>
-      <c r="G3" s="98"/>
-      <c r="H3" s="98"/>
-      <c r="I3" s="98"/>
-      <c r="J3" s="98"/>
-      <c r="K3" s="98"/>
-      <c r="L3" s="98"/>
-      <c r="M3" s="98"/>
-      <c r="N3" s="98"/>
+      <c r="C3" s="99"/>
+      <c r="D3" s="99"/>
+      <c r="E3" s="99"/>
+      <c r="F3" s="99"/>
+      <c r="G3" s="99"/>
+      <c r="H3" s="99"/>
+      <c r="I3" s="99"/>
+      <c r="J3" s="99"/>
+      <c r="K3" s="99"/>
+      <c r="L3" s="99"/>
+      <c r="M3" s="99"/>
+      <c r="N3" s="99"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="44" t="s">
@@ -4147,6 +4145,125 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:N6"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:N2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.85546875" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:14" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B1" s="46" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="98"/>
+      <c r="C2" s="98"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
+      <c r="F2" s="98"/>
+      <c r="G2" s="98"/>
+      <c r="H2" s="98"/>
+      <c r="I2" s="98"/>
+      <c r="J2" s="98"/>
+      <c r="K2" s="98"/>
+      <c r="L2" s="98"/>
+      <c r="M2" s="98"/>
+      <c r="N2" s="98"/>
+    </row>
+    <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B3" s="99" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" s="99"/>
+      <c r="D3" s="99"/>
+      <c r="E3" s="99"/>
+      <c r="F3" s="99"/>
+      <c r="G3" s="99"/>
+      <c r="H3" s="99"/>
+      <c r="I3" s="99"/>
+      <c r="J3" s="99"/>
+      <c r="K3" s="99"/>
+      <c r="L3" s="99"/>
+      <c r="M3" s="99"/>
+      <c r="N3" s="99"/>
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B5" s="58" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="39"/>
+      <c r="I6" s="54"/>
+      <c r="J6" s="54"/>
+      <c r="K6" s="54"/>
+      <c r="L6" s="55"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:N2"/>
+    <mergeCell ref="B3:N3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:N6"/>
   <sheetViews>
@@ -4176,36 +4293,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="97"/>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="97"/>
-      <c r="J2" s="97"/>
-      <c r="K2" s="97"/>
-      <c r="L2" s="97"/>
-      <c r="M2" s="97"/>
-      <c r="N2" s="97"/>
+      <c r="B2" s="98"/>
+      <c r="C2" s="98"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
+      <c r="F2" s="98"/>
+      <c r="G2" s="98"/>
+      <c r="H2" s="98"/>
+      <c r="I2" s="98"/>
+      <c r="J2" s="98"/>
+      <c r="K2" s="98"/>
+      <c r="L2" s="98"/>
+      <c r="M2" s="98"/>
+      <c r="N2" s="98"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="98" t="s">
+      <c r="B3" s="99" t="s">
         <v>150</v>
       </c>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="98"/>
-      <c r="F3" s="98"/>
-      <c r="G3" s="98"/>
-      <c r="H3" s="98"/>
-      <c r="I3" s="98"/>
-      <c r="J3" s="98"/>
-      <c r="K3" s="98"/>
-      <c r="L3" s="98"/>
-      <c r="M3" s="98"/>
-      <c r="N3" s="98"/>
+      <c r="C3" s="99"/>
+      <c r="D3" s="99"/>
+      <c r="E3" s="99"/>
+      <c r="F3" s="99"/>
+      <c r="G3" s="99"/>
+      <c r="H3" s="99"/>
+      <c r="I3" s="99"/>
+      <c r="J3" s="99"/>
+      <c r="K3" s="99"/>
+      <c r="L3" s="99"/>
+      <c r="M3" s="99"/>
+      <c r="N3" s="99"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="74" t="s">
@@ -4265,7 +4382,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J6"/>
   <sheetViews>
@@ -4292,28 +4409,28 @@
       </c>
     </row>
     <row r="2" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="97"/>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="97"/>
-      <c r="J2" s="97"/>
+      <c r="B2" s="98"/>
+      <c r="C2" s="98"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
+      <c r="F2" s="98"/>
+      <c r="G2" s="98"/>
+      <c r="H2" s="98"/>
+      <c r="I2" s="98"/>
+      <c r="J2" s="98"/>
     </row>
     <row r="3" spans="2:10" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="98" t="s">
+      <c r="B3" s="99" t="s">
         <v>153</v>
       </c>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="98"/>
-      <c r="F3" s="98"/>
-      <c r="G3" s="98"/>
-      <c r="H3" s="98"/>
-      <c r="I3" s="98"/>
-      <c r="J3" s="98"/>
+      <c r="C3" s="99"/>
+      <c r="D3" s="99"/>
+      <c r="E3" s="99"/>
+      <c r="F3" s="99"/>
+      <c r="G3" s="99"/>
+      <c r="H3" s="99"/>
+      <c r="I3" s="99"/>
+      <c r="J3" s="99"/>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" s="74" t="s">
@@ -4361,7 +4478,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:T6"/>
   <sheetViews>
@@ -4398,29 +4515,29 @@
       </c>
     </row>
     <row r="2" spans="2:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="99"/>
-      <c r="C2" s="99"/>
-      <c r="D2" s="99"/>
-      <c r="E2" s="99"/>
-      <c r="F2" s="99"/>
-      <c r="G2" s="99"/>
-      <c r="H2" s="99"/>
-      <c r="I2" s="99"/>
+      <c r="B2" s="100"/>
+      <c r="C2" s="100"/>
+      <c r="D2" s="100"/>
+      <c r="E2" s="100"/>
+      <c r="F2" s="100"/>
+      <c r="G2" s="100"/>
+      <c r="H2" s="100"/>
+      <c r="I2" s="100"/>
       <c r="L2" s="84"/>
       <c r="M2" s="84"/>
       <c r="N2" s="84"/>
     </row>
     <row r="3" spans="2:20" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="98" t="s">
+      <c r="B3" s="99" t="s">
         <v>154</v>
       </c>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="98"/>
-      <c r="F3" s="98"/>
-      <c r="G3" s="98"/>
-      <c r="H3" s="98"/>
-      <c r="I3" s="98"/>
+      <c r="C3" s="99"/>
+      <c r="D3" s="99"/>
+      <c r="E3" s="99"/>
+      <c r="F3" s="99"/>
+      <c r="G3" s="99"/>
+      <c r="H3" s="99"/>
+      <c r="I3" s="99"/>
       <c r="L3" s="83"/>
       <c r="M3" s="83"/>
       <c r="N3" s="83"/>
@@ -4515,7 +4632,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:I6"/>
   <sheetViews>
@@ -4541,26 +4658,26 @@
       </c>
     </row>
     <row r="2" spans="2:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="97"/>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="97"/>
+      <c r="B2" s="98"/>
+      <c r="C2" s="98"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
+      <c r="F2" s="98"/>
+      <c r="G2" s="98"/>
+      <c r="H2" s="98"/>
+      <c r="I2" s="98"/>
     </row>
     <row r="3" spans="2:9" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="98" t="s">
+      <c r="B3" s="99" t="s">
         <v>190</v>
       </c>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="98"/>
-      <c r="F3" s="98"/>
-      <c r="G3" s="98"/>
-      <c r="H3" s="98"/>
-      <c r="I3" s="98"/>
+      <c r="C3" s="99"/>
+      <c r="D3" s="99"/>
+      <c r="E3" s="99"/>
+      <c r="F3" s="99"/>
+      <c r="G3" s="99"/>
+      <c r="H3" s="99"/>
+      <c r="I3" s="99"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="89" t="s">
@@ -4608,7 +4725,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K7"/>
   <sheetViews>
@@ -4636,30 +4753,30 @@
       </c>
     </row>
     <row r="2" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="97"/>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="97"/>
-      <c r="J2" s="97"/>
-      <c r="K2" s="97"/>
+      <c r="B2" s="98"/>
+      <c r="C2" s="98"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
+      <c r="F2" s="98"/>
+      <c r="G2" s="98"/>
+      <c r="H2" s="98"/>
+      <c r="I2" s="98"/>
+      <c r="J2" s="98"/>
+      <c r="K2" s="98"/>
     </row>
     <row r="3" spans="2:11" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="98" t="s">
+      <c r="B3" s="99" t="s">
         <v>166</v>
       </c>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="98"/>
-      <c r="F3" s="98"/>
-      <c r="G3" s="98"/>
-      <c r="H3" s="98"/>
-      <c r="I3" s="98"/>
-      <c r="J3" s="98"/>
-      <c r="K3" s="98"/>
+      <c r="C3" s="99"/>
+      <c r="D3" s="99"/>
+      <c r="E3" s="99"/>
+      <c r="F3" s="99"/>
+      <c r="G3" s="99"/>
+      <c r="H3" s="99"/>
+      <c r="I3" s="99"/>
+      <c r="J3" s="99"/>
+      <c r="K3" s="99"/>
     </row>
     <row r="4" spans="2:11" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B4" s="85"/>
@@ -4674,14 +4791,14 @@
       <c r="K4" s="85"/>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="H5" s="101" t="s">
+      <c r="H5" s="102" t="s">
         <v>174</v>
       </c>
-      <c r="I5" s="102"/>
-      <c r="J5" s="101" t="s">
+      <c r="I5" s="103"/>
+      <c r="J5" s="102" t="s">
         <v>173</v>
       </c>
-      <c r="K5" s="102"/>
+      <c r="K5" s="103"/>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" s="86" t="s">
@@ -4739,7 +4856,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:Z8"/>
   <sheetViews>
@@ -4763,37 +4880,37 @@
       <c r="Z1" s="38"/>
     </row>
     <row r="2" spans="2:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="97"/>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="97"/>
-      <c r="J2" s="97"/>
-      <c r="K2" s="97"/>
-      <c r="L2" s="97"/>
-      <c r="M2" s="97"/>
-      <c r="N2" s="97"/>
+      <c r="B2" s="98"/>
+      <c r="C2" s="98"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
+      <c r="F2" s="98"/>
+      <c r="G2" s="98"/>
+      <c r="H2" s="98"/>
+      <c r="I2" s="98"/>
+      <c r="J2" s="98"/>
+      <c r="K2" s="98"/>
+      <c r="L2" s="98"/>
+      <c r="M2" s="98"/>
+      <c r="N2" s="98"/>
       <c r="Z2"/>
     </row>
     <row r="3" spans="2:26" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="98" t="s">
+      <c r="B3" s="99" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="98"/>
-      <c r="F3" s="98"/>
-      <c r="G3" s="98"/>
-      <c r="H3" s="98"/>
-      <c r="I3" s="98"/>
-      <c r="J3" s="98"/>
-      <c r="K3" s="98"/>
-      <c r="L3" s="98"/>
-      <c r="M3" s="98"/>
-      <c r="N3" s="98"/>
+      <c r="C3" s="99"/>
+      <c r="D3" s="99"/>
+      <c r="E3" s="99"/>
+      <c r="F3" s="99"/>
+      <c r="G3" s="99"/>
+      <c r="H3" s="99"/>
+      <c r="I3" s="99"/>
+      <c r="J3" s="99"/>
+      <c r="K3" s="99"/>
+      <c r="L3" s="99"/>
+      <c r="M3" s="99"/>
+      <c r="N3" s="99"/>
       <c r="Z3"/>
     </row>
     <row r="5" spans="2:26" x14ac:dyDescent="0.25">
@@ -4873,7 +4990,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:Z8"/>
   <sheetViews>
@@ -4897,37 +5014,37 @@
       <c r="Z1" s="38"/>
     </row>
     <row r="2" spans="2:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="97"/>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="97"/>
-      <c r="J2" s="97"/>
-      <c r="K2" s="97"/>
-      <c r="L2" s="97"/>
-      <c r="M2" s="97"/>
-      <c r="N2" s="97"/>
+      <c r="B2" s="98"/>
+      <c r="C2" s="98"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
+      <c r="F2" s="98"/>
+      <c r="G2" s="98"/>
+      <c r="H2" s="98"/>
+      <c r="I2" s="98"/>
+      <c r="J2" s="98"/>
+      <c r="K2" s="98"/>
+      <c r="L2" s="98"/>
+      <c r="M2" s="98"/>
+      <c r="N2" s="98"/>
       <c r="Z2"/>
     </row>
     <row r="3" spans="2:26" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="98" t="s">
+      <c r="B3" s="99" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="98"/>
-      <c r="F3" s="98"/>
-      <c r="G3" s="98"/>
-      <c r="H3" s="98"/>
-      <c r="I3" s="98"/>
-      <c r="J3" s="98"/>
-      <c r="K3" s="98"/>
-      <c r="L3" s="98"/>
-      <c r="M3" s="98"/>
-      <c r="N3" s="98"/>
+      <c r="C3" s="99"/>
+      <c r="D3" s="99"/>
+      <c r="E3" s="99"/>
+      <c r="F3" s="99"/>
+      <c r="G3" s="99"/>
+      <c r="H3" s="99"/>
+      <c r="I3" s="99"/>
+      <c r="J3" s="99"/>
+      <c r="K3" s="99"/>
+      <c r="L3" s="99"/>
+      <c r="M3" s="99"/>
+      <c r="N3" s="99"/>
       <c r="Z3"/>
     </row>
     <row r="5" spans="2:26" x14ac:dyDescent="0.25">
@@ -4946,9 +5063,9 @@
       <c r="C6" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="D6" s="103"/>
-      <c r="E6" s="104"/>
-      <c r="F6" s="105"/>
+      <c r="D6" s="104"/>
+      <c r="E6" s="105"/>
+      <c r="F6" s="106"/>
       <c r="G6" s="50"/>
       <c r="H6" s="50"/>
     </row>
@@ -5002,7 +5119,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:Z8"/>
   <sheetViews>
@@ -5026,37 +5143,37 @@
       <c r="Z1" s="38"/>
     </row>
     <row r="2" spans="2:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="97"/>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="97"/>
-      <c r="J2" s="97"/>
-      <c r="K2" s="97"/>
-      <c r="L2" s="97"/>
-      <c r="M2" s="97"/>
-      <c r="N2" s="97"/>
+      <c r="B2" s="98"/>
+      <c r="C2" s="98"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
+      <c r="F2" s="98"/>
+      <c r="G2" s="98"/>
+      <c r="H2" s="98"/>
+      <c r="I2" s="98"/>
+      <c r="J2" s="98"/>
+      <c r="K2" s="98"/>
+      <c r="L2" s="98"/>
+      <c r="M2" s="98"/>
+      <c r="N2" s="98"/>
       <c r="Z2"/>
     </row>
     <row r="3" spans="2:26" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="98" t="s">
+      <c r="B3" s="99" t="s">
         <v>91</v>
       </c>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="98"/>
-      <c r="F3" s="98"/>
-      <c r="G3" s="98"/>
-      <c r="H3" s="98"/>
-      <c r="I3" s="98"/>
-      <c r="J3" s="98"/>
-      <c r="K3" s="98"/>
-      <c r="L3" s="98"/>
-      <c r="M3" s="98"/>
-      <c r="N3" s="98"/>
+      <c r="C3" s="99"/>
+      <c r="D3" s="99"/>
+      <c r="E3" s="99"/>
+      <c r="F3" s="99"/>
+      <c r="G3" s="99"/>
+      <c r="H3" s="99"/>
+      <c r="I3" s="99"/>
+      <c r="J3" s="99"/>
+      <c r="K3" s="99"/>
+      <c r="L3" s="99"/>
+      <c r="M3" s="99"/>
+      <c r="N3" s="99"/>
       <c r="Z3"/>
     </row>
     <row r="5" spans="2:26" x14ac:dyDescent="0.25">
@@ -5127,7 +5244,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:Z8"/>
   <sheetViews>
@@ -5149,37 +5266,37 @@
       <c r="Z1" s="38"/>
     </row>
     <row r="2" spans="2:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="97"/>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="97"/>
-      <c r="J2" s="97"/>
-      <c r="K2" s="97"/>
-      <c r="L2" s="97"/>
-      <c r="M2" s="97"/>
-      <c r="N2" s="97"/>
+      <c r="B2" s="98"/>
+      <c r="C2" s="98"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
+      <c r="F2" s="98"/>
+      <c r="G2" s="98"/>
+      <c r="H2" s="98"/>
+      <c r="I2" s="98"/>
+      <c r="J2" s="98"/>
+      <c r="K2" s="98"/>
+      <c r="L2" s="98"/>
+      <c r="M2" s="98"/>
+      <c r="N2" s="98"/>
       <c r="Z2"/>
     </row>
     <row r="3" spans="2:26" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="98" t="s">
+      <c r="B3" s="99" t="s">
         <v>72</v>
       </c>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="98"/>
-      <c r="F3" s="98"/>
-      <c r="G3" s="98"/>
-      <c r="H3" s="98"/>
-      <c r="I3" s="98"/>
-      <c r="J3" s="98"/>
-      <c r="K3" s="98"/>
-      <c r="L3" s="98"/>
-      <c r="M3" s="98"/>
-      <c r="N3" s="98"/>
+      <c r="C3" s="99"/>
+      <c r="D3" s="99"/>
+      <c r="E3" s="99"/>
+      <c r="F3" s="99"/>
+      <c r="G3" s="99"/>
+      <c r="H3" s="99"/>
+      <c r="I3" s="99"/>
+      <c r="J3" s="99"/>
+      <c r="K3" s="99"/>
+      <c r="L3" s="99"/>
+      <c r="M3" s="99"/>
+      <c r="N3" s="99"/>
       <c r="Z3"/>
     </row>
     <row r="5" spans="2:26" x14ac:dyDescent="0.25">
@@ -5257,7 +5374,113 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:N6"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.85546875" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" customWidth="1"/>
+    <col min="3" max="3" width="30.28515625" customWidth="1"/>
+    <col min="4" max="4" width="33.140625" customWidth="1"/>
+    <col min="5" max="5" width="21.7109375" customWidth="1"/>
+    <col min="6" max="6" width="22.140625" customWidth="1"/>
+    <col min="7" max="8" width="29.5703125" customWidth="1"/>
+    <col min="9" max="9" width="33.140625" customWidth="1"/>
+    <col min="10" max="10" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:14" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B1" s="46" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="98"/>
+      <c r="C2" s="98"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
+      <c r="F2" s="98"/>
+      <c r="G2" s="98"/>
+      <c r="H2" s="98"/>
+      <c r="I2" s="98"/>
+      <c r="J2" s="98"/>
+      <c r="K2" s="98"/>
+      <c r="L2" s="98"/>
+      <c r="M2" s="98"/>
+      <c r="N2" s="98"/>
+    </row>
+    <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B3" s="99" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="99"/>
+      <c r="D3" s="99"/>
+      <c r="E3" s="99"/>
+      <c r="F3" s="99"/>
+      <c r="G3" s="99"/>
+      <c r="H3" s="99"/>
+      <c r="I3" s="99"/>
+      <c r="J3" s="99"/>
+      <c r="K3" s="99"/>
+      <c r="L3" s="99"/>
+      <c r="M3" s="99"/>
+      <c r="N3" s="99"/>
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B5" s="44" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5" s="44" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="45" t="s">
+        <v>76</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="H5" s="96" t="s">
+        <v>196</v>
+      </c>
+      <c r="I5" s="96" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:N2"/>
+    <mergeCell ref="B3:N3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:Q7"/>
   <sheetViews>
@@ -5292,56 +5515,56 @@
       </c>
     </row>
     <row r="2" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="97"/>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="97"/>
-      <c r="J2" s="97"/>
-      <c r="K2" s="97"/>
-      <c r="L2" s="97"/>
+      <c r="B2" s="98"/>
+      <c r="C2" s="98"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
+      <c r="F2" s="98"/>
+      <c r="G2" s="98"/>
+      <c r="H2" s="98"/>
+      <c r="I2" s="98"/>
+      <c r="J2" s="98"/>
+      <c r="K2" s="98"/>
+      <c r="L2" s="98"/>
     </row>
     <row r="3" spans="2:17" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="98" t="s">
+      <c r="B3" s="99" t="s">
         <v>106</v>
       </c>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="98"/>
-      <c r="F3" s="98"/>
-      <c r="G3" s="98"/>
-      <c r="H3" s="98"/>
-      <c r="I3" s="98"/>
-      <c r="J3" s="98"/>
-      <c r="K3" s="98"/>
-      <c r="L3" s="98"/>
+      <c r="C3" s="99"/>
+      <c r="D3" s="99"/>
+      <c r="E3" s="99"/>
+      <c r="F3" s="99"/>
+      <c r="G3" s="99"/>
+      <c r="H3" s="99"/>
+      <c r="I3" s="99"/>
+      <c r="J3" s="99"/>
+      <c r="K3" s="99"/>
+      <c r="L3" s="99"/>
     </row>
     <row r="5" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D5" s="106" t="s">
+      <c r="D5" s="107" t="s">
         <v>121</v>
       </c>
-      <c r="E5" s="106"/>
+      <c r="E5" s="107"/>
       <c r="F5" s="73"/>
       <c r="G5" s="73"/>
       <c r="H5" s="73"/>
       <c r="I5" s="73"/>
-      <c r="J5" s="106" t="s">
+      <c r="J5" s="107" t="s">
         <v>42</v>
       </c>
-      <c r="K5" s="106"/>
-      <c r="L5" s="106"/>
-      <c r="M5" s="106" t="s">
+      <c r="K5" s="107"/>
+      <c r="L5" s="107"/>
+      <c r="M5" s="107" t="s">
         <v>128</v>
       </c>
-      <c r="N5" s="106"/>
-      <c r="O5" s="106"/>
-      <c r="P5" s="100" t="s">
+      <c r="N5" s="107"/>
+      <c r="O5" s="107"/>
+      <c r="P5" s="101" t="s">
         <v>107</v>
       </c>
-      <c r="Q5" s="100"/>
+      <c r="Q5" s="101"/>
     </row>
     <row r="6" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="70" t="s">
@@ -5424,113 +5647,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:N6"/>
-  <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="2.85546875" customWidth="1"/>
-    <col min="2" max="2" width="22.140625" customWidth="1"/>
-    <col min="3" max="3" width="30.28515625" customWidth="1"/>
-    <col min="4" max="4" width="33.140625" customWidth="1"/>
-    <col min="5" max="5" width="21.7109375" customWidth="1"/>
-    <col min="6" max="6" width="22.140625" customWidth="1"/>
-    <col min="7" max="8" width="29.5703125" customWidth="1"/>
-    <col min="9" max="9" width="33.140625" customWidth="1"/>
-    <col min="10" max="10" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:14" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="46" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="97"/>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="97"/>
-      <c r="J2" s="97"/>
-      <c r="K2" s="97"/>
-      <c r="L2" s="97"/>
-      <c r="M2" s="97"/>
-      <c r="N2" s="97"/>
-    </row>
-    <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="98" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="98"/>
-      <c r="F3" s="98"/>
-      <c r="G3" s="98"/>
-      <c r="H3" s="98"/>
-      <c r="I3" s="98"/>
-      <c r="J3" s="98"/>
-      <c r="K3" s="98"/>
-      <c r="L3" s="98"/>
-      <c r="M3" s="98"/>
-      <c r="N3" s="98"/>
-    </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B5" s="44" t="s">
-        <v>77</v>
-      </c>
-      <c r="C5" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="45" t="s">
-        <v>76</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="H5" s="96" t="s">
-        <v>196</v>
-      </c>
-      <c r="I5" s="96" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="7"/>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B2:N2"/>
-    <mergeCell ref="B3:N3"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:Y8"/>
   <sheetViews>
@@ -5571,110 +5688,110 @@
       </c>
     </row>
     <row r="2" spans="2:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="97"/>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="97"/>
-      <c r="J2" s="97"/>
-      <c r="K2" s="97"/>
-      <c r="L2" s="97"/>
-      <c r="M2" s="97"/>
-      <c r="N2" s="97"/>
-      <c r="O2" s="97"/>
-      <c r="P2" s="97"/>
+      <c r="B2" s="98"/>
+      <c r="C2" s="98"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
+      <c r="F2" s="98"/>
+      <c r="G2" s="98"/>
+      <c r="H2" s="98"/>
+      <c r="I2" s="98"/>
+      <c r="J2" s="98"/>
+      <c r="K2" s="98"/>
+      <c r="L2" s="98"/>
+      <c r="M2" s="98"/>
+      <c r="N2" s="98"/>
+      <c r="O2" s="98"/>
+      <c r="P2" s="98"/>
       <c r="Q2" s="56"/>
       <c r="R2" s="56"/>
     </row>
     <row r="3" spans="2:25" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="98" t="s">
+      <c r="B3" s="99" t="s">
         <v>109</v>
       </c>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="98"/>
-      <c r="F3" s="98"/>
-      <c r="G3" s="98"/>
-      <c r="H3" s="98"/>
-      <c r="I3" s="98"/>
-      <c r="J3" s="98"/>
-      <c r="K3" s="98"/>
-      <c r="L3" s="98"/>
-      <c r="M3" s="98"/>
-      <c r="N3" s="98"/>
-      <c r="O3" s="98"/>
-      <c r="P3" s="98"/>
+      <c r="C3" s="99"/>
+      <c r="D3" s="99"/>
+      <c r="E3" s="99"/>
+      <c r="F3" s="99"/>
+      <c r="G3" s="99"/>
+      <c r="H3" s="99"/>
+      <c r="I3" s="99"/>
+      <c r="J3" s="99"/>
+      <c r="K3" s="99"/>
+      <c r="L3" s="99"/>
+      <c r="M3" s="99"/>
+      <c r="N3" s="99"/>
+      <c r="O3" s="99"/>
+      <c r="P3" s="99"/>
       <c r="Q3" s="57"/>
       <c r="R3" s="57"/>
     </row>
     <row r="5" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B5" s="111" t="s">
+      <c r="B5" s="108" t="s">
         <v>110</v>
       </c>
-      <c r="C5" s="112"/>
-      <c r="D5" s="112"/>
-      <c r="E5" s="112"/>
-      <c r="F5" s="112"/>
-      <c r="G5" s="112"/>
-      <c r="H5" s="112"/>
-      <c r="I5" s="112"/>
-      <c r="J5" s="112"/>
-      <c r="K5" s="112"/>
-      <c r="L5" s="113"/>
-      <c r="M5" s="111" t="s">
+      <c r="C5" s="109"/>
+      <c r="D5" s="109"/>
+      <c r="E5" s="109"/>
+      <c r="F5" s="109"/>
+      <c r="G5" s="109"/>
+      <c r="H5" s="109"/>
+      <c r="I5" s="109"/>
+      <c r="J5" s="109"/>
+      <c r="K5" s="109"/>
+      <c r="L5" s="110"/>
+      <c r="M5" s="108" t="s">
         <v>111</v>
       </c>
-      <c r="N5" s="112"/>
-      <c r="O5" s="112"/>
-      <c r="P5" s="112"/>
-      <c r="Q5" s="112"/>
-      <c r="R5" s="112"/>
-      <c r="S5" s="112"/>
-      <c r="T5" s="112"/>
-      <c r="U5" s="112"/>
-      <c r="V5" s="112"/>
-      <c r="W5" s="112"/>
-      <c r="X5" s="112"/>
-      <c r="Y5" s="113"/>
+      <c r="N5" s="109"/>
+      <c r="O5" s="109"/>
+      <c r="P5" s="109"/>
+      <c r="Q5" s="109"/>
+      <c r="R5" s="109"/>
+      <c r="S5" s="109"/>
+      <c r="T5" s="109"/>
+      <c r="U5" s="109"/>
+      <c r="V5" s="109"/>
+      <c r="W5" s="109"/>
+      <c r="X5" s="109"/>
+      <c r="Y5" s="110"/>
     </row>
     <row r="6" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B6" s="110"/>
-      <c r="C6" s="110"/>
-      <c r="D6" s="110"/>
-      <c r="E6" s="110"/>
-      <c r="F6" s="117" t="s">
+      <c r="B6" s="117"/>
+      <c r="C6" s="117"/>
+      <c r="D6" s="117"/>
+      <c r="E6" s="117"/>
+      <c r="F6" s="111" t="s">
         <v>27</v>
       </c>
-      <c r="G6" s="118"/>
-      <c r="H6" s="118"/>
-      <c r="I6" s="119"/>
-      <c r="J6" s="111" t="s">
+      <c r="G6" s="112"/>
+      <c r="H6" s="112"/>
+      <c r="I6" s="113"/>
+      <c r="J6" s="108" t="s">
         <v>30</v>
       </c>
-      <c r="K6" s="112"/>
-      <c r="L6" s="113"/>
+      <c r="K6" s="109"/>
+      <c r="L6" s="110"/>
       <c r="M6" s="88"/>
-      <c r="N6" s="107" t="s">
+      <c r="N6" s="114" t="s">
         <v>42</v>
       </c>
-      <c r="O6" s="108"/>
-      <c r="P6" s="107" t="s">
+      <c r="O6" s="115"/>
+      <c r="P6" s="114" t="s">
         <v>104</v>
       </c>
-      <c r="Q6" s="109"/>
-      <c r="R6" s="108"/>
+      <c r="Q6" s="116"/>
+      <c r="R6" s="115"/>
       <c r="S6" s="88"/>
-      <c r="T6" s="107" t="s">
+      <c r="T6" s="114" t="s">
         <v>121</v>
       </c>
-      <c r="U6" s="108"/>
-      <c r="V6" s="114"/>
-      <c r="W6" s="115"/>
-      <c r="X6" s="115"/>
-      <c r="Y6" s="116"/>
+      <c r="U6" s="115"/>
+      <c r="V6" s="118"/>
+      <c r="W6" s="119"/>
+      <c r="X6" s="119"/>
+      <c r="Y6" s="120"/>
     </row>
     <row r="7" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B7" s="75" t="s">
@@ -5778,6 +5895,9 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="T6:U6"/>
+    <mergeCell ref="M5:Y5"/>
+    <mergeCell ref="V6:Y6"/>
     <mergeCell ref="B2:P2"/>
     <mergeCell ref="B3:P3"/>
     <mergeCell ref="B5:L5"/>
@@ -5786,16 +5906,13 @@
     <mergeCell ref="N6:O6"/>
     <mergeCell ref="P6:R6"/>
     <mergeCell ref="B6:E6"/>
-    <mergeCell ref="T6:U6"/>
-    <mergeCell ref="M5:Y5"/>
-    <mergeCell ref="V6:Y6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A24"/>
   <sheetViews>
@@ -5884,6 +6001,76 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.85546875" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" style="67" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.42578125" style="67" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" style="67" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" style="67" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="11.42578125" style="65"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:5" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B1" s="46" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="98"/>
+      <c r="C2" s="98"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
+    </row>
+    <row r="3" spans="2:5" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B3" s="99" t="s">
+        <v>129</v>
+      </c>
+      <c r="C3" s="99"/>
+      <c r="D3" s="99"/>
+      <c r="E3" s="99"/>
+    </row>
+    <row r="4" spans="2:5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="64"/>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="70" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5" s="44" t="s">
+        <v>130</v>
+      </c>
+      <c r="D5" s="97" t="s">
+        <v>131</v>
+      </c>
+      <c r="E5" s="97" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="8"/>
+      <c r="C6" s="90"/>
+      <c r="D6" s="66"/>
+      <c r="E6" s="66"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B3:E3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:P6"/>
   <sheetViews>
@@ -5909,40 +6096,40 @@
       </c>
     </row>
     <row r="2" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="97"/>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="97"/>
-      <c r="J2" s="97"/>
-      <c r="K2" s="97"/>
-      <c r="L2" s="97"/>
-      <c r="M2" s="97"/>
-      <c r="N2" s="97"/>
-      <c r="O2" s="97"/>
-      <c r="P2" s="97"/>
+      <c r="B2" s="98"/>
+      <c r="C2" s="98"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
+      <c r="F2" s="98"/>
+      <c r="G2" s="98"/>
+      <c r="H2" s="98"/>
+      <c r="I2" s="98"/>
+      <c r="J2" s="98"/>
+      <c r="K2" s="98"/>
+      <c r="L2" s="98"/>
+      <c r="M2" s="98"/>
+      <c r="N2" s="98"/>
+      <c r="O2" s="98"/>
+      <c r="P2" s="98"/>
     </row>
     <row r="3" spans="2:16" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="98" t="s">
+      <c r="B3" s="99" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="98"/>
-      <c r="F3" s="98"/>
-      <c r="G3" s="98"/>
-      <c r="H3" s="98"/>
-      <c r="I3" s="98"/>
-      <c r="J3" s="98"/>
-      <c r="K3" s="98"/>
-      <c r="L3" s="98"/>
-      <c r="M3" s="98"/>
-      <c r="N3" s="98"/>
-      <c r="O3" s="98"/>
-      <c r="P3" s="98"/>
+      <c r="C3" s="99"/>
+      <c r="D3" s="99"/>
+      <c r="E3" s="99"/>
+      <c r="F3" s="99"/>
+      <c r="G3" s="99"/>
+      <c r="H3" s="99"/>
+      <c r="I3" s="99"/>
+      <c r="J3" s="99"/>
+      <c r="K3" s="99"/>
+      <c r="L3" s="99"/>
+      <c r="M3" s="99"/>
+      <c r="N3" s="99"/>
+      <c r="O3" s="99"/>
+      <c r="P3" s="99"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="44" t="s">
@@ -5995,7 +6182,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:P6"/>
   <sheetViews>
@@ -6021,40 +6208,40 @@
       </c>
     </row>
     <row r="2" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="97"/>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="97"/>
-      <c r="J2" s="97"/>
-      <c r="K2" s="97"/>
-      <c r="L2" s="97"/>
-      <c r="M2" s="97"/>
-      <c r="N2" s="97"/>
-      <c r="O2" s="97"/>
-      <c r="P2" s="97"/>
+      <c r="B2" s="98"/>
+      <c r="C2" s="98"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
+      <c r="F2" s="98"/>
+      <c r="G2" s="98"/>
+      <c r="H2" s="98"/>
+      <c r="I2" s="98"/>
+      <c r="J2" s="98"/>
+      <c r="K2" s="98"/>
+      <c r="L2" s="98"/>
+      <c r="M2" s="98"/>
+      <c r="N2" s="98"/>
+      <c r="O2" s="98"/>
+      <c r="P2" s="98"/>
     </row>
     <row r="3" spans="2:16" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="98" t="s">
+      <c r="B3" s="99" t="s">
         <v>68</v>
       </c>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="98"/>
-      <c r="F3" s="98"/>
-      <c r="G3" s="98"/>
-      <c r="H3" s="98"/>
-      <c r="I3" s="98"/>
-      <c r="J3" s="98"/>
-      <c r="K3" s="98"/>
-      <c r="L3" s="98"/>
-      <c r="M3" s="98"/>
-      <c r="N3" s="98"/>
-      <c r="O3" s="98"/>
-      <c r="P3" s="98"/>
+      <c r="C3" s="99"/>
+      <c r="D3" s="99"/>
+      <c r="E3" s="99"/>
+      <c r="F3" s="99"/>
+      <c r="G3" s="99"/>
+      <c r="H3" s="99"/>
+      <c r="I3" s="99"/>
+      <c r="J3" s="99"/>
+      <c r="K3" s="99"/>
+      <c r="L3" s="99"/>
+      <c r="M3" s="99"/>
+      <c r="N3" s="99"/>
+      <c r="O3" s="99"/>
+      <c r="P3" s="99"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
@@ -6078,7 +6265,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:P6"/>
   <sheetViews>
@@ -6103,40 +6290,40 @@
       </c>
     </row>
     <row r="2" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="97"/>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="97"/>
-      <c r="J2" s="97"/>
-      <c r="K2" s="97"/>
-      <c r="L2" s="97"/>
-      <c r="M2" s="97"/>
-      <c r="N2" s="97"/>
-      <c r="O2" s="97"/>
-      <c r="P2" s="97"/>
+      <c r="B2" s="98"/>
+      <c r="C2" s="98"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
+      <c r="F2" s="98"/>
+      <c r="G2" s="98"/>
+      <c r="H2" s="98"/>
+      <c r="I2" s="98"/>
+      <c r="J2" s="98"/>
+      <c r="K2" s="98"/>
+      <c r="L2" s="98"/>
+      <c r="M2" s="98"/>
+      <c r="N2" s="98"/>
+      <c r="O2" s="98"/>
+      <c r="P2" s="98"/>
     </row>
     <row r="3" spans="2:16" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="98" t="s">
+      <c r="B3" s="99" t="s">
         <v>71</v>
       </c>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="98"/>
-      <c r="F3" s="98"/>
-      <c r="G3" s="98"/>
-      <c r="H3" s="98"/>
-      <c r="I3" s="98"/>
-      <c r="J3" s="98"/>
-      <c r="K3" s="98"/>
-      <c r="L3" s="98"/>
-      <c r="M3" s="98"/>
-      <c r="N3" s="98"/>
-      <c r="O3" s="98"/>
-      <c r="P3" s="98"/>
+      <c r="C3" s="99"/>
+      <c r="D3" s="99"/>
+      <c r="E3" s="99"/>
+      <c r="F3" s="99"/>
+      <c r="G3" s="99"/>
+      <c r="H3" s="99"/>
+      <c r="I3" s="99"/>
+      <c r="J3" s="99"/>
+      <c r="K3" s="99"/>
+      <c r="L3" s="99"/>
+      <c r="M3" s="99"/>
+      <c r="N3" s="99"/>
+      <c r="O3" s="99"/>
+      <c r="P3" s="99"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
@@ -6160,7 +6347,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:P6"/>
   <sheetViews>
@@ -6191,40 +6378,40 @@
       </c>
     </row>
     <row r="2" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="97"/>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="97"/>
-      <c r="J2" s="97"/>
-      <c r="K2" s="97"/>
-      <c r="L2" s="97"/>
-      <c r="M2" s="97"/>
-      <c r="N2" s="97"/>
-      <c r="O2" s="97"/>
-      <c r="P2" s="97"/>
+      <c r="B2" s="98"/>
+      <c r="C2" s="98"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
+      <c r="F2" s="98"/>
+      <c r="G2" s="98"/>
+      <c r="H2" s="98"/>
+      <c r="I2" s="98"/>
+      <c r="J2" s="98"/>
+      <c r="K2" s="98"/>
+      <c r="L2" s="98"/>
+      <c r="M2" s="98"/>
+      <c r="N2" s="98"/>
+      <c r="O2" s="98"/>
+      <c r="P2" s="98"/>
     </row>
     <row r="3" spans="2:16" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="98" t="s">
+      <c r="B3" s="99" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="98"/>
-      <c r="F3" s="98"/>
-      <c r="G3" s="98"/>
-      <c r="H3" s="98"/>
-      <c r="I3" s="98"/>
-      <c r="J3" s="98"/>
-      <c r="K3" s="98"/>
-      <c r="L3" s="98"/>
-      <c r="M3" s="98"/>
-      <c r="N3" s="98"/>
-      <c r="O3" s="98"/>
-      <c r="P3" s="98"/>
+      <c r="C3" s="99"/>
+      <c r="D3" s="99"/>
+      <c r="E3" s="99"/>
+      <c r="F3" s="99"/>
+      <c r="G3" s="99"/>
+      <c r="H3" s="99"/>
+      <c r="I3" s="99"/>
+      <c r="J3" s="99"/>
+      <c r="K3" s="99"/>
+      <c r="L3" s="99"/>
+      <c r="M3" s="99"/>
+      <c r="N3" s="99"/>
+      <c r="O3" s="99"/>
+      <c r="P3" s="99"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="44" t="s">
@@ -6293,7 +6480,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:P6"/>
   <sheetViews>
@@ -6321,40 +6508,40 @@
       </c>
     </row>
     <row r="2" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="97"/>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="97"/>
-      <c r="J2" s="97"/>
-      <c r="K2" s="97"/>
-      <c r="L2" s="97"/>
-      <c r="M2" s="97"/>
-      <c r="N2" s="97"/>
-      <c r="O2" s="97"/>
-      <c r="P2" s="97"/>
+      <c r="B2" s="98"/>
+      <c r="C2" s="98"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
+      <c r="F2" s="98"/>
+      <c r="G2" s="98"/>
+      <c r="H2" s="98"/>
+      <c r="I2" s="98"/>
+      <c r="J2" s="98"/>
+      <c r="K2" s="98"/>
+      <c r="L2" s="98"/>
+      <c r="M2" s="98"/>
+      <c r="N2" s="98"/>
+      <c r="O2" s="98"/>
+      <c r="P2" s="98"/>
     </row>
     <row r="3" spans="2:16" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="98" t="s">
+      <c r="B3" s="99" t="s">
         <v>65</v>
       </c>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="98"/>
-      <c r="F3" s="98"/>
-      <c r="G3" s="98"/>
-      <c r="H3" s="98"/>
-      <c r="I3" s="98"/>
-      <c r="J3" s="98"/>
-      <c r="K3" s="98"/>
-      <c r="L3" s="98"/>
-      <c r="M3" s="98"/>
-      <c r="N3" s="98"/>
-      <c r="O3" s="98"/>
-      <c r="P3" s="98"/>
+      <c r="C3" s="99"/>
+      <c r="D3" s="99"/>
+      <c r="E3" s="99"/>
+      <c r="F3" s="99"/>
+      <c r="G3" s="99"/>
+      <c r="H3" s="99"/>
+      <c r="I3" s="99"/>
+      <c r="J3" s="99"/>
+      <c r="K3" s="99"/>
+      <c r="L3" s="99"/>
+      <c r="M3" s="99"/>
+      <c r="N3" s="99"/>
+      <c r="O3" s="99"/>
+      <c r="P3" s="99"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="45" t="s">
@@ -6381,77 +6568,4 @@
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:K6"/>
-  <sheetViews>
-    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="2.85546875" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" customWidth="1"/>
-    <col min="3" max="3" width="23" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:11" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="46" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="2" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="99"/>
-      <c r="C2" s="99"/>
-      <c r="D2" s="99"/>
-      <c r="E2" s="99"/>
-      <c r="F2" s="99"/>
-      <c r="G2" s="99"/>
-      <c r="H2" s="99"/>
-      <c r="I2" s="99"/>
-      <c r="J2" s="84"/>
-      <c r="K2" s="84"/>
-    </row>
-    <row r="3" spans="2:11" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="98" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="98"/>
-      <c r="F3" s="98"/>
-      <c r="G3" s="98"/>
-      <c r="H3" s="98"/>
-      <c r="I3" s="98"/>
-      <c r="J3" s="83"/>
-      <c r="K3" s="83"/>
-    </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="2"/>
-      <c r="C6" s="8"/>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B2:I2"/>
-    <mergeCell ref="B3:I3"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
TRIEDA-1640 - Alterando exportação para mostrar minutos ao invés de créditos. Tirando casas decimais do template excel.
</commit_message>
<xml_diff>
--- a/code/client/web/src/main/resources/templateExport.xlsx
+++ b/code/client/web/src/main/resources/templateExport.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="17070" windowHeight="5370" tabRatio="954" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="17070" windowHeight="5370" tabRatio="954" firstSheet="23" activeTab="23"/>
   </bookViews>
   <sheets>
     <sheet name="Campi" sheetId="3" r:id="rId1"/>
@@ -47,7 +47,7 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Autor</author>
+    <author>Author</author>
   </authors>
   <commentList>
     <comment ref="B5" authorId="0">
@@ -103,7 +103,7 @@
 <file path=xl/comments10.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Autor</author>
+    <author>Author</author>
   </authors>
   <commentList>
     <comment ref="C5" authorId="0">
@@ -143,7 +143,7 @@
 <file path=xl/comments11.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Autor</author>
+    <author>Author</author>
   </authors>
   <commentList>
     <comment ref="D5" authorId="0">
@@ -205,7 +205,7 @@
 <file path=xl/comments12.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Autor</author>
+    <author>Author</author>
   </authors>
   <commentList>
     <comment ref="Z1" authorId="0">
@@ -218,7 +218,7 @@
 <file path=xl/comments13.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Autor</author>
+    <author>Author</author>
   </authors>
   <commentList>
     <comment ref="Z1" authorId="0">
@@ -231,7 +231,7 @@
 <file path=xl/comments14.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Autor</author>
+    <author>Author</author>
   </authors>
   <commentList>
     <comment ref="Z1" authorId="0">
@@ -244,7 +244,7 @@
 <file path=xl/comments15.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Autor</author>
+    <author>Author</author>
   </authors>
   <commentList>
     <comment ref="Z1" authorId="0">
@@ -257,7 +257,7 @@
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Autor</author>
+    <author>Author</author>
   </authors>
   <commentList>
     <comment ref="B5" authorId="0">
@@ -314,7 +314,7 @@
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Autor</author>
+    <author>Author</author>
   </authors>
   <commentList>
     <comment ref="B5" authorId="0">
@@ -452,7 +452,7 @@
 <file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Autor</author>
+    <author>Author</author>
   </authors>
   <commentList>
     <comment ref="C5" authorId="0">
@@ -492,7 +492,7 @@
 <file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Autor</author>
+    <author>Author</author>
   </authors>
   <commentList>
     <comment ref="B5" authorId="0">
@@ -690,7 +690,7 @@
 <file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Autor</author>
+    <author>Author</author>
   </authors>
   <commentList>
     <comment ref="B5" authorId="0">
@@ -1063,7 +1063,7 @@
 <file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Autor</author>
+    <author>Author</author>
   </authors>
   <commentList>
     <comment ref="B5" authorId="0">
@@ -1115,7 +1115,7 @@
 <file path=xl/comments8.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Autor</author>
+    <author>Author</author>
   </authors>
   <commentList>
     <comment ref="I5" authorId="0">
@@ -1139,7 +1139,7 @@
 <file path=xl/comments9.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Autor</author>
+    <author>Author</author>
   </authors>
   <commentList>
     <comment ref="D5" authorId="0">
@@ -2326,7 +2326,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="121">
+  <cellXfs count="120">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2556,9 +2556,6 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2633,6 +2630,12 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2642,6 +2645,15 @@
     <xf numFmtId="0" fontId="10" fillId="28" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2651,31 +2663,16 @@
     <xf numFmtId="0" fontId="10" fillId="28" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="28" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="28" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Porcentagem" xfId="1" builtinId="5"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -2688,9 +2685,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2728,7 +2725,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -2800,7 +2797,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2999,38 +2996,38 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="98" t="s">
+      <c r="B2" s="97" t="s">
         <v>94</v>
       </c>
-      <c r="C2" s="98"/>
-      <c r="D2" s="98"/>
-      <c r="E2" s="98"/>
-      <c r="F2" s="98"/>
-      <c r="G2" s="98"/>
-      <c r="H2" s="98"/>
-      <c r="I2" s="98"/>
-      <c r="J2" s="98"/>
-      <c r="K2" s="98"/>
-      <c r="L2" s="98"/>
-      <c r="M2" s="98"/>
-      <c r="N2" s="98"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
+      <c r="F2" s="97"/>
+      <c r="G2" s="97"/>
+      <c r="H2" s="97"/>
+      <c r="I2" s="97"/>
+      <c r="J2" s="97"/>
+      <c r="K2" s="97"/>
+      <c r="L2" s="97"/>
+      <c r="M2" s="97"/>
+      <c r="N2" s="97"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="99" t="s">
+      <c r="B3" s="98" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="99"/>
-      <c r="D3" s="99"/>
-      <c r="E3" s="99"/>
-      <c r="F3" s="99"/>
-      <c r="G3" s="99"/>
-      <c r="H3" s="99"/>
-      <c r="I3" s="99"/>
-      <c r="J3" s="99"/>
-      <c r="K3" s="99"/>
-      <c r="L3" s="99"/>
-      <c r="M3" s="99"/>
-      <c r="N3" s="99"/>
+      <c r="C3" s="98"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="98"/>
+      <c r="F3" s="98"/>
+      <c r="G3" s="98"/>
+      <c r="H3" s="98"/>
+      <c r="I3" s="98"/>
+      <c r="J3" s="98"/>
+      <c r="K3" s="98"/>
+      <c r="L3" s="98"/>
+      <c r="M3" s="98"/>
+      <c r="N3" s="98"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="44" t="s">
@@ -3097,30 +3094,30 @@
       </c>
     </row>
     <row r="2" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="100"/>
-      <c r="C2" s="100"/>
-      <c r="D2" s="100"/>
-      <c r="E2" s="100"/>
-      <c r="F2" s="100"/>
-      <c r="G2" s="100"/>
-      <c r="H2" s="100"/>
-      <c r="I2" s="100"/>
-      <c r="J2" s="84"/>
-      <c r="K2" s="84"/>
+      <c r="B2" s="99"/>
+      <c r="C2" s="99"/>
+      <c r="D2" s="99"/>
+      <c r="E2" s="99"/>
+      <c r="F2" s="99"/>
+      <c r="G2" s="99"/>
+      <c r="H2" s="99"/>
+      <c r="I2" s="99"/>
+      <c r="J2" s="83"/>
+      <c r="K2" s="83"/>
     </row>
     <row r="3" spans="2:11" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="99" t="s">
+      <c r="B3" s="98" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="99"/>
-      <c r="D3" s="99"/>
-      <c r="E3" s="99"/>
-      <c r="F3" s="99"/>
-      <c r="G3" s="99"/>
-      <c r="H3" s="99"/>
-      <c r="I3" s="99"/>
-      <c r="J3" s="83"/>
-      <c r="K3" s="83"/>
+      <c r="C3" s="98"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="98"/>
+      <c r="F3" s="98"/>
+      <c r="G3" s="98"/>
+      <c r="H3" s="98"/>
+      <c r="I3" s="98"/>
+      <c r="J3" s="82"/>
+      <c r="K3" s="82"/>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -3171,36 +3168,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="98"/>
-      <c r="C2" s="98"/>
-      <c r="D2" s="98"/>
-      <c r="E2" s="98"/>
-      <c r="F2" s="98"/>
-      <c r="G2" s="98"/>
-      <c r="H2" s="98"/>
-      <c r="I2" s="98"/>
-      <c r="J2" s="98"/>
-      <c r="K2" s="98"/>
-      <c r="L2" s="98"/>
-      <c r="M2" s="98"/>
-      <c r="N2" s="98"/>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
+      <c r="F2" s="97"/>
+      <c r="G2" s="97"/>
+      <c r="H2" s="97"/>
+      <c r="I2" s="97"/>
+      <c r="J2" s="97"/>
+      <c r="K2" s="97"/>
+      <c r="L2" s="97"/>
+      <c r="M2" s="97"/>
+      <c r="N2" s="97"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="99" t="s">
+      <c r="B3" s="98" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="99"/>
-      <c r="D3" s="99"/>
-      <c r="E3" s="99"/>
-      <c r="F3" s="99"/>
-      <c r="G3" s="99"/>
-      <c r="H3" s="99"/>
-      <c r="I3" s="99"/>
-      <c r="J3" s="99"/>
-      <c r="K3" s="99"/>
-      <c r="L3" s="99"/>
-      <c r="M3" s="99"/>
-      <c r="N3" s="99"/>
+      <c r="C3" s="98"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="98"/>
+      <c r="F3" s="98"/>
+      <c r="G3" s="98"/>
+      <c r="H3" s="98"/>
+      <c r="I3" s="98"/>
+      <c r="J3" s="98"/>
+      <c r="K3" s="98"/>
+      <c r="L3" s="98"/>
+      <c r="M3" s="98"/>
+      <c r="N3" s="98"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -3269,36 +3266,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="98"/>
-      <c r="C2" s="98"/>
-      <c r="D2" s="98"/>
-      <c r="E2" s="98"/>
-      <c r="F2" s="98"/>
-      <c r="G2" s="98"/>
-      <c r="H2" s="98"/>
-      <c r="I2" s="98"/>
-      <c r="J2" s="98"/>
-      <c r="K2" s="98"/>
-      <c r="L2" s="98"/>
-      <c r="M2" s="98"/>
-      <c r="N2" s="98"/>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
+      <c r="F2" s="97"/>
+      <c r="G2" s="97"/>
+      <c r="H2" s="97"/>
+      <c r="I2" s="97"/>
+      <c r="J2" s="97"/>
+      <c r="K2" s="97"/>
+      <c r="L2" s="97"/>
+      <c r="M2" s="97"/>
+      <c r="N2" s="97"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="99" t="s">
+      <c r="B3" s="98" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="99"/>
-      <c r="D3" s="99"/>
-      <c r="E3" s="99"/>
-      <c r="F3" s="99"/>
-      <c r="G3" s="99"/>
-      <c r="H3" s="99"/>
-      <c r="I3" s="99"/>
-      <c r="J3" s="99"/>
-      <c r="K3" s="99"/>
-      <c r="L3" s="99"/>
-      <c r="M3" s="99"/>
-      <c r="N3" s="99"/>
+      <c r="C3" s="98"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="98"/>
+      <c r="F3" s="98"/>
+      <c r="G3" s="98"/>
+      <c r="H3" s="98"/>
+      <c r="I3" s="98"/>
+      <c r="J3" s="98"/>
+      <c r="K3" s="98"/>
+      <c r="L3" s="98"/>
+      <c r="M3" s="98"/>
+      <c r="N3" s="98"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -3383,18 +3380,18 @@
       </c>
     </row>
     <row r="2" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="98"/>
-      <c r="C2" s="98"/>
-      <c r="D2" s="98"/>
-      <c r="E2" s="98"/>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
     </row>
     <row r="3" spans="2:5" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="99" t="s">
+      <c r="B3" s="98" t="s">
         <v>124</v>
       </c>
-      <c r="C3" s="99"/>
-      <c r="D3" s="99"/>
-      <c r="E3" s="99"/>
+      <c r="C3" s="98"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="98"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="60" t="s">
@@ -3447,36 +3444,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="98"/>
-      <c r="C2" s="98"/>
-      <c r="D2" s="98"/>
-      <c r="E2" s="98"/>
-      <c r="F2" s="98"/>
-      <c r="G2" s="98"/>
-      <c r="H2" s="98"/>
-      <c r="I2" s="98"/>
-      <c r="J2" s="98"/>
-      <c r="K2" s="98"/>
-      <c r="L2" s="98"/>
-      <c r="M2" s="98"/>
-      <c r="N2" s="98"/>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
+      <c r="F2" s="97"/>
+      <c r="G2" s="97"/>
+      <c r="H2" s="97"/>
+      <c r="I2" s="97"/>
+      <c r="J2" s="97"/>
+      <c r="K2" s="97"/>
+      <c r="L2" s="97"/>
+      <c r="M2" s="97"/>
+      <c r="N2" s="97"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="99" t="s">
+      <c r="B3" s="98" t="s">
         <v>98</v>
       </c>
-      <c r="C3" s="99"/>
-      <c r="D3" s="99"/>
-      <c r="E3" s="99"/>
-      <c r="F3" s="99"/>
-      <c r="G3" s="99"/>
-      <c r="H3" s="99"/>
-      <c r="I3" s="99"/>
-      <c r="J3" s="99"/>
-      <c r="K3" s="99"/>
-      <c r="L3" s="99"/>
-      <c r="M3" s="99"/>
-      <c r="N3" s="99"/>
+      <c r="C3" s="98"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="98"/>
+      <c r="F3" s="98"/>
+      <c r="G3" s="98"/>
+      <c r="H3" s="98"/>
+      <c r="I3" s="98"/>
+      <c r="J3" s="98"/>
+      <c r="K3" s="98"/>
+      <c r="L3" s="98"/>
+      <c r="M3" s="98"/>
+      <c r="N3" s="98"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -3509,10 +3506,10 @@
       <c r="K5" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="L5" s="101" t="s">
+      <c r="L5" s="100" t="s">
         <v>108</v>
       </c>
-      <c r="M5" s="101"/>
+      <c r="M5" s="100"/>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
@@ -3567,38 +3564,38 @@
       </c>
     </row>
     <row r="2" spans="2:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="98"/>
-      <c r="C2" s="98"/>
-      <c r="D2" s="98"/>
-      <c r="E2" s="98"/>
-      <c r="F2" s="98"/>
-      <c r="G2" s="98"/>
-      <c r="H2" s="98"/>
-      <c r="I2" s="98"/>
-      <c r="J2" s="98"/>
-      <c r="K2" s="98"/>
-      <c r="L2" s="98"/>
-      <c r="M2" s="98"/>
-      <c r="N2" s="98"/>
-      <c r="O2" s="98"/>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
+      <c r="F2" s="97"/>
+      <c r="G2" s="97"/>
+      <c r="H2" s="97"/>
+      <c r="I2" s="97"/>
+      <c r="J2" s="97"/>
+      <c r="K2" s="97"/>
+      <c r="L2" s="97"/>
+      <c r="M2" s="97"/>
+      <c r="N2" s="97"/>
+      <c r="O2" s="97"/>
     </row>
     <row r="3" spans="2:15" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="99" t="s">
+      <c r="B3" s="98" t="s">
         <v>73</v>
       </c>
-      <c r="C3" s="99"/>
-      <c r="D3" s="99"/>
-      <c r="E3" s="99"/>
-      <c r="F3" s="99"/>
-      <c r="G3" s="99"/>
-      <c r="H3" s="99"/>
-      <c r="I3" s="99"/>
-      <c r="J3" s="99"/>
-      <c r="K3" s="99"/>
-      <c r="L3" s="99"/>
-      <c r="M3" s="99"/>
-      <c r="N3" s="99"/>
-      <c r="O3" s="99"/>
+      <c r="C3" s="98"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="98"/>
+      <c r="F3" s="98"/>
+      <c r="G3" s="98"/>
+      <c r="H3" s="98"/>
+      <c r="I3" s="98"/>
+      <c r="J3" s="98"/>
+      <c r="K3" s="98"/>
+      <c r="L3" s="98"/>
+      <c r="M3" s="98"/>
+      <c r="N3" s="98"/>
+      <c r="O3" s="98"/>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -3631,10 +3628,10 @@
       <c r="K5" s="45" t="s">
         <v>97</v>
       </c>
-      <c r="L5" s="95" t="s">
+      <c r="L5" s="94" t="s">
         <v>193</v>
       </c>
-      <c r="M5" s="95" t="s">
+      <c r="M5" s="94" t="s">
         <v>194</v>
       </c>
     </row>
@@ -3685,18 +3682,18 @@
       </c>
     </row>
     <row r="2" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="98"/>
-      <c r="C2" s="98"/>
-      <c r="D2" s="98"/>
-      <c r="E2" s="98"/>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
     </row>
     <row r="3" spans="2:5" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="99" t="s">
+      <c r="B3" s="98" t="s">
         <v>129</v>
       </c>
-      <c r="C3" s="99"/>
-      <c r="D3" s="99"/>
-      <c r="E3" s="99"/>
+      <c r="C3" s="98"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="98"/>
     </row>
     <row r="4" spans="2:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="64"/>
@@ -3758,36 +3755,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="98"/>
-      <c r="C2" s="98"/>
-      <c r="D2" s="98"/>
-      <c r="E2" s="98"/>
-      <c r="F2" s="98"/>
-      <c r="G2" s="98"/>
-      <c r="H2" s="98"/>
-      <c r="I2" s="98"/>
-      <c r="J2" s="98"/>
-      <c r="K2" s="98"/>
-      <c r="L2" s="98"/>
-      <c r="M2" s="98"/>
-      <c r="N2" s="98"/>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
+      <c r="F2" s="97"/>
+      <c r="G2" s="97"/>
+      <c r="H2" s="97"/>
+      <c r="I2" s="97"/>
+      <c r="J2" s="97"/>
+      <c r="K2" s="97"/>
+      <c r="L2" s="97"/>
+      <c r="M2" s="97"/>
+      <c r="N2" s="97"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="99" t="s">
+      <c r="B3" s="98" t="s">
         <v>69</v>
       </c>
-      <c r="C3" s="99"/>
-      <c r="D3" s="99"/>
-      <c r="E3" s="99"/>
-      <c r="F3" s="99"/>
-      <c r="G3" s="99"/>
-      <c r="H3" s="99"/>
-      <c r="I3" s="99"/>
-      <c r="J3" s="99"/>
-      <c r="K3" s="99"/>
-      <c r="L3" s="99"/>
-      <c r="M3" s="99"/>
-      <c r="N3" s="99"/>
+      <c r="C3" s="98"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="98"/>
+      <c r="F3" s="98"/>
+      <c r="G3" s="98"/>
+      <c r="H3" s="98"/>
+      <c r="I3" s="98"/>
+      <c r="J3" s="98"/>
+      <c r="K3" s="98"/>
+      <c r="L3" s="98"/>
+      <c r="M3" s="98"/>
+      <c r="N3" s="98"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -3842,36 +3839,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="98"/>
-      <c r="C2" s="98"/>
-      <c r="D2" s="98"/>
-      <c r="E2" s="98"/>
-      <c r="F2" s="98"/>
-      <c r="G2" s="98"/>
-      <c r="H2" s="98"/>
-      <c r="I2" s="98"/>
-      <c r="J2" s="98"/>
-      <c r="K2" s="98"/>
-      <c r="L2" s="98"/>
-      <c r="M2" s="98"/>
-      <c r="N2" s="98"/>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
+      <c r="F2" s="97"/>
+      <c r="G2" s="97"/>
+      <c r="H2" s="97"/>
+      <c r="I2" s="97"/>
+      <c r="J2" s="97"/>
+      <c r="K2" s="97"/>
+      <c r="L2" s="97"/>
+      <c r="M2" s="97"/>
+      <c r="N2" s="97"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="99" t="s">
+      <c r="B3" s="98" t="s">
         <v>74</v>
       </c>
-      <c r="C3" s="99"/>
-      <c r="D3" s="99"/>
-      <c r="E3" s="99"/>
-      <c r="F3" s="99"/>
-      <c r="G3" s="99"/>
-      <c r="H3" s="99"/>
-      <c r="I3" s="99"/>
-      <c r="J3" s="99"/>
-      <c r="K3" s="99"/>
-      <c r="L3" s="99"/>
-      <c r="M3" s="99"/>
-      <c r="N3" s="99"/>
+      <c r="C3" s="98"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="98"/>
+      <c r="F3" s="98"/>
+      <c r="G3" s="98"/>
+      <c r="H3" s="98"/>
+      <c r="I3" s="98"/>
+      <c r="J3" s="98"/>
+      <c r="K3" s="98"/>
+      <c r="L3" s="98"/>
+      <c r="M3" s="98"/>
+      <c r="N3" s="98"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -3940,40 +3937,40 @@
       </c>
     </row>
     <row r="2" spans="2:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="98"/>
-      <c r="C2" s="98"/>
-      <c r="D2" s="98"/>
-      <c r="E2" s="98"/>
-      <c r="F2" s="98"/>
-      <c r="G2" s="98"/>
-      <c r="H2" s="98"/>
-      <c r="I2" s="98"/>
-      <c r="J2" s="98"/>
-      <c r="K2" s="98"/>
-      <c r="L2" s="98"/>
-      <c r="M2" s="98"/>
-      <c r="N2" s="98"/>
-      <c r="O2" s="98"/>
-      <c r="P2" s="98"/>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
+      <c r="F2" s="97"/>
+      <c r="G2" s="97"/>
+      <c r="H2" s="97"/>
+      <c r="I2" s="97"/>
+      <c r="J2" s="97"/>
+      <c r="K2" s="97"/>
+      <c r="L2" s="97"/>
+      <c r="M2" s="97"/>
+      <c r="N2" s="97"/>
+      <c r="O2" s="97"/>
+      <c r="P2" s="97"/>
     </row>
     <row r="3" spans="2:18" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="99" t="s">
+      <c r="B3" s="98" t="s">
         <v>63</v>
       </c>
-      <c r="C3" s="99"/>
-      <c r="D3" s="99"/>
-      <c r="E3" s="99"/>
-      <c r="F3" s="99"/>
-      <c r="G3" s="99"/>
-      <c r="H3" s="99"/>
-      <c r="I3" s="99"/>
-      <c r="J3" s="99"/>
-      <c r="K3" s="99"/>
-      <c r="L3" s="99"/>
-      <c r="M3" s="99"/>
-      <c r="N3" s="99"/>
-      <c r="O3" s="99"/>
-      <c r="P3" s="99"/>
+      <c r="C3" s="98"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="98"/>
+      <c r="F3" s="98"/>
+      <c r="G3" s="98"/>
+      <c r="H3" s="98"/>
+      <c r="I3" s="98"/>
+      <c r="J3" s="98"/>
+      <c r="K3" s="98"/>
+      <c r="L3" s="98"/>
+      <c r="M3" s="98"/>
+      <c r="N3" s="98"/>
+      <c r="O3" s="98"/>
+      <c r="P3" s="98"/>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
@@ -4084,38 +4081,38 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="98" t="s">
+      <c r="B2" s="97" t="s">
         <v>95</v>
       </c>
-      <c r="C2" s="98"/>
-      <c r="D2" s="98"/>
-      <c r="E2" s="98"/>
-      <c r="F2" s="98"/>
-      <c r="G2" s="98"/>
-      <c r="H2" s="98"/>
-      <c r="I2" s="98"/>
-      <c r="J2" s="98"/>
-      <c r="K2" s="98"/>
-      <c r="L2" s="98"/>
-      <c r="M2" s="98"/>
-      <c r="N2" s="98"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
+      <c r="F2" s="97"/>
+      <c r="G2" s="97"/>
+      <c r="H2" s="97"/>
+      <c r="I2" s="97"/>
+      <c r="J2" s="97"/>
+      <c r="K2" s="97"/>
+      <c r="L2" s="97"/>
+      <c r="M2" s="97"/>
+      <c r="N2" s="97"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="99" t="s">
+      <c r="B3" s="98" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="99"/>
-      <c r="D3" s="99"/>
-      <c r="E3" s="99"/>
-      <c r="F3" s="99"/>
-      <c r="G3" s="99"/>
-      <c r="H3" s="99"/>
-      <c r="I3" s="99"/>
-      <c r="J3" s="99"/>
-      <c r="K3" s="99"/>
-      <c r="L3" s="99"/>
-      <c r="M3" s="99"/>
-      <c r="N3" s="99"/>
+      <c r="C3" s="98"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="98"/>
+      <c r="F3" s="98"/>
+      <c r="G3" s="98"/>
+      <c r="H3" s="98"/>
+      <c r="I3" s="98"/>
+      <c r="J3" s="98"/>
+      <c r="K3" s="98"/>
+      <c r="L3" s="98"/>
+      <c r="M3" s="98"/>
+      <c r="N3" s="98"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="44" t="s">
@@ -4174,36 +4171,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="98"/>
-      <c r="C2" s="98"/>
-      <c r="D2" s="98"/>
-      <c r="E2" s="98"/>
-      <c r="F2" s="98"/>
-      <c r="G2" s="98"/>
-      <c r="H2" s="98"/>
-      <c r="I2" s="98"/>
-      <c r="J2" s="98"/>
-      <c r="K2" s="98"/>
-      <c r="L2" s="98"/>
-      <c r="M2" s="98"/>
-      <c r="N2" s="98"/>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
+      <c r="F2" s="97"/>
+      <c r="G2" s="97"/>
+      <c r="H2" s="97"/>
+      <c r="I2" s="97"/>
+      <c r="J2" s="97"/>
+      <c r="K2" s="97"/>
+      <c r="L2" s="97"/>
+      <c r="M2" s="97"/>
+      <c r="N2" s="97"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="99" t="s">
+      <c r="B3" s="98" t="s">
         <v>64</v>
       </c>
-      <c r="C3" s="99"/>
-      <c r="D3" s="99"/>
-      <c r="E3" s="99"/>
-      <c r="F3" s="99"/>
-      <c r="G3" s="99"/>
-      <c r="H3" s="99"/>
-      <c r="I3" s="99"/>
-      <c r="J3" s="99"/>
-      <c r="K3" s="99"/>
-      <c r="L3" s="99"/>
-      <c r="M3" s="99"/>
-      <c r="N3" s="99"/>
+      <c r="C3" s="98"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="98"/>
+      <c r="F3" s="98"/>
+      <c r="G3" s="98"/>
+      <c r="H3" s="98"/>
+      <c r="I3" s="98"/>
+      <c r="J3" s="98"/>
+      <c r="K3" s="98"/>
+      <c r="L3" s="98"/>
+      <c r="M3" s="98"/>
+      <c r="N3" s="98"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="58" t="s">
@@ -4293,36 +4290,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="98"/>
-      <c r="C2" s="98"/>
-      <c r="D2" s="98"/>
-      <c r="E2" s="98"/>
-      <c r="F2" s="98"/>
-      <c r="G2" s="98"/>
-      <c r="H2" s="98"/>
-      <c r="I2" s="98"/>
-      <c r="J2" s="98"/>
-      <c r="K2" s="98"/>
-      <c r="L2" s="98"/>
-      <c r="M2" s="98"/>
-      <c r="N2" s="98"/>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
+      <c r="F2" s="97"/>
+      <c r="G2" s="97"/>
+      <c r="H2" s="97"/>
+      <c r="I2" s="97"/>
+      <c r="J2" s="97"/>
+      <c r="K2" s="97"/>
+      <c r="L2" s="97"/>
+      <c r="M2" s="97"/>
+      <c r="N2" s="97"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="99" t="s">
+      <c r="B3" s="98" t="s">
         <v>150</v>
       </c>
-      <c r="C3" s="99"/>
-      <c r="D3" s="99"/>
-      <c r="E3" s="99"/>
-      <c r="F3" s="99"/>
-      <c r="G3" s="99"/>
-      <c r="H3" s="99"/>
-      <c r="I3" s="99"/>
-      <c r="J3" s="99"/>
-      <c r="K3" s="99"/>
-      <c r="L3" s="99"/>
-      <c r="M3" s="99"/>
-      <c r="N3" s="99"/>
+      <c r="C3" s="98"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="98"/>
+      <c r="F3" s="98"/>
+      <c r="G3" s="98"/>
+      <c r="H3" s="98"/>
+      <c r="I3" s="98"/>
+      <c r="J3" s="98"/>
+      <c r="K3" s="98"/>
+      <c r="L3" s="98"/>
+      <c r="M3" s="98"/>
+      <c r="N3" s="98"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="74" t="s">
@@ -4409,28 +4406,28 @@
       </c>
     </row>
     <row r="2" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="98"/>
-      <c r="C2" s="98"/>
-      <c r="D2" s="98"/>
-      <c r="E2" s="98"/>
-      <c r="F2" s="98"/>
-      <c r="G2" s="98"/>
-      <c r="H2" s="98"/>
-      <c r="I2" s="98"/>
-      <c r="J2" s="98"/>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
+      <c r="F2" s="97"/>
+      <c r="G2" s="97"/>
+      <c r="H2" s="97"/>
+      <c r="I2" s="97"/>
+      <c r="J2" s="97"/>
     </row>
     <row r="3" spans="2:10" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="99" t="s">
+      <c r="B3" s="98" t="s">
         <v>153</v>
       </c>
-      <c r="C3" s="99"/>
-      <c r="D3" s="99"/>
-      <c r="E3" s="99"/>
-      <c r="F3" s="99"/>
-      <c r="G3" s="99"/>
-      <c r="H3" s="99"/>
-      <c r="I3" s="99"/>
-      <c r="J3" s="99"/>
+      <c r="C3" s="98"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="98"/>
+      <c r="F3" s="98"/>
+      <c r="G3" s="98"/>
+      <c r="H3" s="98"/>
+      <c r="I3" s="98"/>
+      <c r="J3" s="98"/>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" s="74" t="s">
@@ -4515,32 +4512,32 @@
       </c>
     </row>
     <row r="2" spans="2:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="100"/>
-      <c r="C2" s="100"/>
-      <c r="D2" s="100"/>
-      <c r="E2" s="100"/>
-      <c r="F2" s="100"/>
-      <c r="G2" s="100"/>
-      <c r="H2" s="100"/>
-      <c r="I2" s="100"/>
-      <c r="L2" s="84"/>
-      <c r="M2" s="84"/>
-      <c r="N2" s="84"/>
+      <c r="B2" s="99"/>
+      <c r="C2" s="99"/>
+      <c r="D2" s="99"/>
+      <c r="E2" s="99"/>
+      <c r="F2" s="99"/>
+      <c r="G2" s="99"/>
+      <c r="H2" s="99"/>
+      <c r="I2" s="99"/>
+      <c r="L2" s="83"/>
+      <c r="M2" s="83"/>
+      <c r="N2" s="83"/>
     </row>
     <row r="3" spans="2:20" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="99" t="s">
+      <c r="B3" s="98" t="s">
         <v>154</v>
       </c>
-      <c r="C3" s="99"/>
-      <c r="D3" s="99"/>
-      <c r="E3" s="99"/>
-      <c r="F3" s="99"/>
-      <c r="G3" s="99"/>
-      <c r="H3" s="99"/>
-      <c r="I3" s="99"/>
-      <c r="L3" s="83"/>
-      <c r="M3" s="83"/>
-      <c r="N3" s="83"/>
+      <c r="C3" s="98"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="98"/>
+      <c r="F3" s="98"/>
+      <c r="G3" s="98"/>
+      <c r="H3" s="98"/>
+      <c r="I3" s="98"/>
+      <c r="L3" s="82"/>
+      <c r="M3" s="82"/>
+      <c r="N3" s="82"/>
     </row>
     <row r="5" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B5" s="80" t="s">
@@ -4582,22 +4579,22 @@
       <c r="N5" s="79" t="s">
         <v>162</v>
       </c>
-      <c r="O5" s="87" t="s">
+      <c r="O5" s="86" t="s">
         <v>175</v>
       </c>
-      <c r="P5" s="87" t="s">
+      <c r="P5" s="86" t="s">
         <v>176</v>
       </c>
-      <c r="Q5" s="87" t="s">
+      <c r="Q5" s="86" t="s">
         <v>180</v>
       </c>
-      <c r="R5" s="87" t="s">
+      <c r="R5" s="86" t="s">
         <v>177</v>
       </c>
-      <c r="S5" s="87" t="s">
+      <c r="S5" s="86" t="s">
         <v>178</v>
       </c>
-      <c r="T5" s="87" t="s">
+      <c r="T5" s="86" t="s">
         <v>179</v>
       </c>
     </row>
@@ -4609,18 +4606,18 @@
       <c r="F6" s="8"/>
       <c r="G6" s="6"/>
       <c r="H6" s="8"/>
-      <c r="I6" s="92"/>
-      <c r="J6" s="92"/>
-      <c r="K6" s="82"/>
-      <c r="L6" s="92"/>
-      <c r="M6" s="93"/>
-      <c r="N6" s="92"/>
-      <c r="O6" s="93"/>
-      <c r="P6" s="94"/>
+      <c r="I6" s="91"/>
+      <c r="J6" s="91"/>
+      <c r="K6" s="81"/>
+      <c r="L6" s="91"/>
+      <c r="M6" s="92"/>
+      <c r="N6" s="91"/>
+      <c r="O6" s="92"/>
+      <c r="P6" s="93"/>
       <c r="Q6" s="78"/>
-      <c r="R6" s="93"/>
-      <c r="S6" s="93"/>
-      <c r="T6" s="82"/>
+      <c r="R6" s="92"/>
+      <c r="S6" s="92"/>
+      <c r="T6" s="81"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -4636,8 +4633,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:I6"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4658,62 +4655,62 @@
       </c>
     </row>
     <row r="2" spans="2:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="98"/>
-      <c r="C2" s="98"/>
-      <c r="D2" s="98"/>
-      <c r="E2" s="98"/>
-      <c r="F2" s="98"/>
-      <c r="G2" s="98"/>
-      <c r="H2" s="98"/>
-      <c r="I2" s="98"/>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
+      <c r="F2" s="97"/>
+      <c r="G2" s="97"/>
+      <c r="H2" s="97"/>
+      <c r="I2" s="97"/>
     </row>
     <row r="3" spans="2:9" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="99" t="s">
+      <c r="B3" s="98" t="s">
         <v>190</v>
       </c>
-      <c r="C3" s="99"/>
-      <c r="D3" s="99"/>
-      <c r="E3" s="99"/>
-      <c r="F3" s="99"/>
-      <c r="G3" s="99"/>
-      <c r="H3" s="99"/>
-      <c r="I3" s="99"/>
+      <c r="C3" s="98"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="98"/>
+      <c r="F3" s="98"/>
+      <c r="G3" s="98"/>
+      <c r="H3" s="98"/>
+      <c r="I3" s="98"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="89" t="s">
+      <c r="B5" s="88" t="s">
         <v>182</v>
       </c>
-      <c r="C5" s="89" t="s">
+      <c r="C5" s="88" t="s">
         <v>183</v>
       </c>
-      <c r="D5" s="89" t="s">
+      <c r="D5" s="88" t="s">
         <v>184</v>
       </c>
-      <c r="E5" s="89" t="s">
+      <c r="E5" s="88" t="s">
         <v>185</v>
       </c>
-      <c r="F5" s="89" t="s">
+      <c r="F5" s="88" t="s">
         <v>186</v>
       </c>
-      <c r="G5" s="89" t="s">
+      <c r="G5" s="88" t="s">
         <v>187</v>
       </c>
-      <c r="H5" s="89" t="s">
+      <c r="H5" s="88" t="s">
         <v>188</v>
       </c>
-      <c r="I5" s="89" t="s">
+      <c r="I5" s="88" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="81"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="78"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -4753,82 +4750,82 @@
       </c>
     </row>
     <row r="2" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="98"/>
-      <c r="C2" s="98"/>
-      <c r="D2" s="98"/>
-      <c r="E2" s="98"/>
-      <c r="F2" s="98"/>
-      <c r="G2" s="98"/>
-      <c r="H2" s="98"/>
-      <c r="I2" s="98"/>
-      <c r="J2" s="98"/>
-      <c r="K2" s="98"/>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
+      <c r="F2" s="97"/>
+      <c r="G2" s="97"/>
+      <c r="H2" s="97"/>
+      <c r="I2" s="97"/>
+      <c r="J2" s="97"/>
+      <c r="K2" s="97"/>
     </row>
     <row r="3" spans="2:11" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="99" t="s">
+      <c r="B3" s="98" t="s">
         <v>166</v>
       </c>
-      <c r="C3" s="99"/>
-      <c r="D3" s="99"/>
-      <c r="E3" s="99"/>
-      <c r="F3" s="99"/>
-      <c r="G3" s="99"/>
-      <c r="H3" s="99"/>
-      <c r="I3" s="99"/>
-      <c r="J3" s="99"/>
-      <c r="K3" s="99"/>
+      <c r="C3" s="98"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="98"/>
+      <c r="F3" s="98"/>
+      <c r="G3" s="98"/>
+      <c r="H3" s="98"/>
+      <c r="I3" s="98"/>
+      <c r="J3" s="98"/>
+      <c r="K3" s="98"/>
     </row>
     <row r="4" spans="2:11" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B4" s="85"/>
-      <c r="C4" s="85"/>
-      <c r="D4" s="85"/>
-      <c r="E4" s="85"/>
-      <c r="F4" s="85"/>
-      <c r="G4" s="85"/>
-      <c r="H4" s="85"/>
-      <c r="I4" s="85"/>
-      <c r="J4" s="85"/>
-      <c r="K4" s="85"/>
+      <c r="B4" s="84"/>
+      <c r="C4" s="84"/>
+      <c r="D4" s="84"/>
+      <c r="E4" s="84"/>
+      <c r="F4" s="84"/>
+      <c r="G4" s="84"/>
+      <c r="H4" s="84"/>
+      <c r="I4" s="84"/>
+      <c r="J4" s="84"/>
+      <c r="K4" s="84"/>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="H5" s="102" t="s">
+      <c r="H5" s="101" t="s">
         <v>174</v>
       </c>
-      <c r="I5" s="103"/>
-      <c r="J5" s="102" t="s">
+      <c r="I5" s="102"/>
+      <c r="J5" s="101" t="s">
         <v>173</v>
       </c>
-      <c r="K5" s="103"/>
+      <c r="K5" s="102"/>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="86" t="s">
+      <c r="B6" s="85" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="86" t="s">
+      <c r="C6" s="85" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="86" t="s">
+      <c r="D6" s="85" t="s">
         <v>167</v>
       </c>
-      <c r="E6" s="86" t="s">
+      <c r="E6" s="85" t="s">
         <v>168</v>
       </c>
-      <c r="F6" s="86" t="s">
+      <c r="F6" s="85" t="s">
         <v>114</v>
       </c>
-      <c r="G6" s="86" t="s">
+      <c r="G6" s="85" t="s">
         <v>114</v>
       </c>
-      <c r="H6" s="86" t="s">
+      <c r="H6" s="85" t="s">
         <v>169</v>
       </c>
-      <c r="I6" s="86" t="s">
+      <c r="I6" s="85" t="s">
         <v>170</v>
       </c>
-      <c r="J6" s="86" t="s">
+      <c r="J6" s="85" t="s">
         <v>171</v>
       </c>
-      <c r="K6" s="86" t="s">
+      <c r="K6" s="85" t="s">
         <v>172</v>
       </c>
     </row>
@@ -4840,9 +4837,9 @@
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
       <c r="H7" s="8"/>
-      <c r="I7" s="82"/>
-      <c r="J7" s="82"/>
-      <c r="K7" s="82"/>
+      <c r="I7" s="81"/>
+      <c r="J7" s="81"/>
+      <c r="K7" s="81"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -4880,37 +4877,37 @@
       <c r="Z1" s="38"/>
     </row>
     <row r="2" spans="2:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="98"/>
-      <c r="C2" s="98"/>
-      <c r="D2" s="98"/>
-      <c r="E2" s="98"/>
-      <c r="F2" s="98"/>
-      <c r="G2" s="98"/>
-      <c r="H2" s="98"/>
-      <c r="I2" s="98"/>
-      <c r="J2" s="98"/>
-      <c r="K2" s="98"/>
-      <c r="L2" s="98"/>
-      <c r="M2" s="98"/>
-      <c r="N2" s="98"/>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
+      <c r="F2" s="97"/>
+      <c r="G2" s="97"/>
+      <c r="H2" s="97"/>
+      <c r="I2" s="97"/>
+      <c r="J2" s="97"/>
+      <c r="K2" s="97"/>
+      <c r="L2" s="97"/>
+      <c r="M2" s="97"/>
+      <c r="N2" s="97"/>
       <c r="Z2"/>
     </row>
     <row r="3" spans="2:26" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="99" t="s">
+      <c r="B3" s="98" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="99"/>
-      <c r="D3" s="99"/>
-      <c r="E3" s="99"/>
-      <c r="F3" s="99"/>
-      <c r="G3" s="99"/>
-      <c r="H3" s="99"/>
-      <c r="I3" s="99"/>
-      <c r="J3" s="99"/>
-      <c r="K3" s="99"/>
-      <c r="L3" s="99"/>
-      <c r="M3" s="99"/>
-      <c r="N3" s="99"/>
+      <c r="C3" s="98"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="98"/>
+      <c r="F3" s="98"/>
+      <c r="G3" s="98"/>
+      <c r="H3" s="98"/>
+      <c r="I3" s="98"/>
+      <c r="J3" s="98"/>
+      <c r="K3" s="98"/>
+      <c r="L3" s="98"/>
+      <c r="M3" s="98"/>
+      <c r="N3" s="98"/>
       <c r="Z3"/>
     </row>
     <row r="5" spans="2:26" x14ac:dyDescent="0.25">
@@ -5014,37 +5011,37 @@
       <c r="Z1" s="38"/>
     </row>
     <row r="2" spans="2:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="98"/>
-      <c r="C2" s="98"/>
-      <c r="D2" s="98"/>
-      <c r="E2" s="98"/>
-      <c r="F2" s="98"/>
-      <c r="G2" s="98"/>
-      <c r="H2" s="98"/>
-      <c r="I2" s="98"/>
-      <c r="J2" s="98"/>
-      <c r="K2" s="98"/>
-      <c r="L2" s="98"/>
-      <c r="M2" s="98"/>
-      <c r="N2" s="98"/>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
+      <c r="F2" s="97"/>
+      <c r="G2" s="97"/>
+      <c r="H2" s="97"/>
+      <c r="I2" s="97"/>
+      <c r="J2" s="97"/>
+      <c r="K2" s="97"/>
+      <c r="L2" s="97"/>
+      <c r="M2" s="97"/>
+      <c r="N2" s="97"/>
       <c r="Z2"/>
     </row>
     <row r="3" spans="2:26" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="99" t="s">
+      <c r="B3" s="98" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="99"/>
-      <c r="D3" s="99"/>
-      <c r="E3" s="99"/>
-      <c r="F3" s="99"/>
-      <c r="G3" s="99"/>
-      <c r="H3" s="99"/>
-      <c r="I3" s="99"/>
-      <c r="J3" s="99"/>
-      <c r="K3" s="99"/>
-      <c r="L3" s="99"/>
-      <c r="M3" s="99"/>
-      <c r="N3" s="99"/>
+      <c r="C3" s="98"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="98"/>
+      <c r="F3" s="98"/>
+      <c r="G3" s="98"/>
+      <c r="H3" s="98"/>
+      <c r="I3" s="98"/>
+      <c r="J3" s="98"/>
+      <c r="K3" s="98"/>
+      <c r="L3" s="98"/>
+      <c r="M3" s="98"/>
+      <c r="N3" s="98"/>
       <c r="Z3"/>
     </row>
     <row r="5" spans="2:26" x14ac:dyDescent="0.25">
@@ -5063,9 +5060,9 @@
       <c r="C6" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="D6" s="104"/>
-      <c r="E6" s="105"/>
-      <c r="F6" s="106"/>
+      <c r="D6" s="103"/>
+      <c r="E6" s="104"/>
+      <c r="F6" s="105"/>
       <c r="G6" s="50"/>
       <c r="H6" s="50"/>
     </row>
@@ -5143,37 +5140,37 @@
       <c r="Z1" s="38"/>
     </row>
     <row r="2" spans="2:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="98"/>
-      <c r="C2" s="98"/>
-      <c r="D2" s="98"/>
-      <c r="E2" s="98"/>
-      <c r="F2" s="98"/>
-      <c r="G2" s="98"/>
-      <c r="H2" s="98"/>
-      <c r="I2" s="98"/>
-      <c r="J2" s="98"/>
-      <c r="K2" s="98"/>
-      <c r="L2" s="98"/>
-      <c r="M2" s="98"/>
-      <c r="N2" s="98"/>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
+      <c r="F2" s="97"/>
+      <c r="G2" s="97"/>
+      <c r="H2" s="97"/>
+      <c r="I2" s="97"/>
+      <c r="J2" s="97"/>
+      <c r="K2" s="97"/>
+      <c r="L2" s="97"/>
+      <c r="M2" s="97"/>
+      <c r="N2" s="97"/>
       <c r="Z2"/>
     </row>
     <row r="3" spans="2:26" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="99" t="s">
+      <c r="B3" s="98" t="s">
         <v>91</v>
       </c>
-      <c r="C3" s="99"/>
-      <c r="D3" s="99"/>
-      <c r="E3" s="99"/>
-      <c r="F3" s="99"/>
-      <c r="G3" s="99"/>
-      <c r="H3" s="99"/>
-      <c r="I3" s="99"/>
-      <c r="J3" s="99"/>
-      <c r="K3" s="99"/>
-      <c r="L3" s="99"/>
-      <c r="M3" s="99"/>
-      <c r="N3" s="99"/>
+      <c r="C3" s="98"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="98"/>
+      <c r="F3" s="98"/>
+      <c r="G3" s="98"/>
+      <c r="H3" s="98"/>
+      <c r="I3" s="98"/>
+      <c r="J3" s="98"/>
+      <c r="K3" s="98"/>
+      <c r="L3" s="98"/>
+      <c r="M3" s="98"/>
+      <c r="N3" s="98"/>
       <c r="Z3"/>
     </row>
     <row r="5" spans="2:26" x14ac:dyDescent="0.25">
@@ -5266,37 +5263,37 @@
       <c r="Z1" s="38"/>
     </row>
     <row r="2" spans="2:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="98"/>
-      <c r="C2" s="98"/>
-      <c r="D2" s="98"/>
-      <c r="E2" s="98"/>
-      <c r="F2" s="98"/>
-      <c r="G2" s="98"/>
-      <c r="H2" s="98"/>
-      <c r="I2" s="98"/>
-      <c r="J2" s="98"/>
-      <c r="K2" s="98"/>
-      <c r="L2" s="98"/>
-      <c r="M2" s="98"/>
-      <c r="N2" s="98"/>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
+      <c r="F2" s="97"/>
+      <c r="G2" s="97"/>
+      <c r="H2" s="97"/>
+      <c r="I2" s="97"/>
+      <c r="J2" s="97"/>
+      <c r="K2" s="97"/>
+      <c r="L2" s="97"/>
+      <c r="M2" s="97"/>
+      <c r="N2" s="97"/>
       <c r="Z2"/>
     </row>
     <row r="3" spans="2:26" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="99" t="s">
+      <c r="B3" s="98" t="s">
         <v>72</v>
       </c>
-      <c r="C3" s="99"/>
-      <c r="D3" s="99"/>
-      <c r="E3" s="99"/>
-      <c r="F3" s="99"/>
-      <c r="G3" s="99"/>
-      <c r="H3" s="99"/>
-      <c r="I3" s="99"/>
-      <c r="J3" s="99"/>
-      <c r="K3" s="99"/>
-      <c r="L3" s="99"/>
-      <c r="M3" s="99"/>
-      <c r="N3" s="99"/>
+      <c r="C3" s="98"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="98"/>
+      <c r="F3" s="98"/>
+      <c r="G3" s="98"/>
+      <c r="H3" s="98"/>
+      <c r="I3" s="98"/>
+      <c r="J3" s="98"/>
+      <c r="K3" s="98"/>
+      <c r="L3" s="98"/>
+      <c r="M3" s="98"/>
+      <c r="N3" s="98"/>
       <c r="Z3"/>
     </row>
     <row r="5" spans="2:26" x14ac:dyDescent="0.25">
@@ -5402,36 +5399,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="98"/>
-      <c r="C2" s="98"/>
-      <c r="D2" s="98"/>
-      <c r="E2" s="98"/>
-      <c r="F2" s="98"/>
-      <c r="G2" s="98"/>
-      <c r="H2" s="98"/>
-      <c r="I2" s="98"/>
-      <c r="J2" s="98"/>
-      <c r="K2" s="98"/>
-      <c r="L2" s="98"/>
-      <c r="M2" s="98"/>
-      <c r="N2" s="98"/>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
+      <c r="F2" s="97"/>
+      <c r="G2" s="97"/>
+      <c r="H2" s="97"/>
+      <c r="I2" s="97"/>
+      <c r="J2" s="97"/>
+      <c r="K2" s="97"/>
+      <c r="L2" s="97"/>
+      <c r="M2" s="97"/>
+      <c r="N2" s="97"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="99" t="s">
+      <c r="B3" s="98" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="99"/>
-      <c r="D3" s="99"/>
-      <c r="E3" s="99"/>
-      <c r="F3" s="99"/>
-      <c r="G3" s="99"/>
-      <c r="H3" s="99"/>
-      <c r="I3" s="99"/>
-      <c r="J3" s="99"/>
-      <c r="K3" s="99"/>
-      <c r="L3" s="99"/>
-      <c r="M3" s="99"/>
-      <c r="N3" s="99"/>
+      <c r="C3" s="98"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="98"/>
+      <c r="F3" s="98"/>
+      <c r="G3" s="98"/>
+      <c r="H3" s="98"/>
+      <c r="I3" s="98"/>
+      <c r="J3" s="98"/>
+      <c r="K3" s="98"/>
+      <c r="L3" s="98"/>
+      <c r="M3" s="98"/>
+      <c r="N3" s="98"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="44" t="s">
@@ -5452,10 +5449,10 @@
       <c r="G5" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="H5" s="96" t="s">
+      <c r="H5" s="95" t="s">
         <v>196</v>
       </c>
-      <c r="I5" s="96" t="s">
+      <c r="I5" s="95" t="s">
         <v>197</v>
       </c>
     </row>
@@ -5515,56 +5512,56 @@
       </c>
     </row>
     <row r="2" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="98"/>
-      <c r="C2" s="98"/>
-      <c r="D2" s="98"/>
-      <c r="E2" s="98"/>
-      <c r="F2" s="98"/>
-      <c r="G2" s="98"/>
-      <c r="H2" s="98"/>
-      <c r="I2" s="98"/>
-      <c r="J2" s="98"/>
-      <c r="K2" s="98"/>
-      <c r="L2" s="98"/>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
+      <c r="F2" s="97"/>
+      <c r="G2" s="97"/>
+      <c r="H2" s="97"/>
+      <c r="I2" s="97"/>
+      <c r="J2" s="97"/>
+      <c r="K2" s="97"/>
+      <c r="L2" s="97"/>
     </row>
     <row r="3" spans="2:17" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="99" t="s">
+      <c r="B3" s="98" t="s">
         <v>106</v>
       </c>
-      <c r="C3" s="99"/>
-      <c r="D3" s="99"/>
-      <c r="E3" s="99"/>
-      <c r="F3" s="99"/>
-      <c r="G3" s="99"/>
-      <c r="H3" s="99"/>
-      <c r="I3" s="99"/>
-      <c r="J3" s="99"/>
-      <c r="K3" s="99"/>
-      <c r="L3" s="99"/>
+      <c r="C3" s="98"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="98"/>
+      <c r="F3" s="98"/>
+      <c r="G3" s="98"/>
+      <c r="H3" s="98"/>
+      <c r="I3" s="98"/>
+      <c r="J3" s="98"/>
+      <c r="K3" s="98"/>
+      <c r="L3" s="98"/>
     </row>
     <row r="5" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D5" s="107" t="s">
+      <c r="D5" s="106" t="s">
         <v>121</v>
       </c>
-      <c r="E5" s="107"/>
+      <c r="E5" s="106"/>
       <c r="F5" s="73"/>
       <c r="G5" s="73"/>
       <c r="H5" s="73"/>
       <c r="I5" s="73"/>
-      <c r="J5" s="107" t="s">
+      <c r="J5" s="106" t="s">
         <v>42</v>
       </c>
-      <c r="K5" s="107"/>
-      <c r="L5" s="107"/>
-      <c r="M5" s="107" t="s">
+      <c r="K5" s="106"/>
+      <c r="L5" s="106"/>
+      <c r="M5" s="106" t="s">
         <v>128</v>
       </c>
-      <c r="N5" s="107"/>
-      <c r="O5" s="107"/>
-      <c r="P5" s="101" t="s">
+      <c r="N5" s="106"/>
+      <c r="O5" s="106"/>
+      <c r="P5" s="100" t="s">
         <v>107</v>
       </c>
-      <c r="Q5" s="101"/>
+      <c r="Q5" s="100"/>
     </row>
     <row r="6" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="70" t="s">
@@ -5688,110 +5685,110 @@
       </c>
     </row>
     <row r="2" spans="2:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="98"/>
-      <c r="C2" s="98"/>
-      <c r="D2" s="98"/>
-      <c r="E2" s="98"/>
-      <c r="F2" s="98"/>
-      <c r="G2" s="98"/>
-      <c r="H2" s="98"/>
-      <c r="I2" s="98"/>
-      <c r="J2" s="98"/>
-      <c r="K2" s="98"/>
-      <c r="L2" s="98"/>
-      <c r="M2" s="98"/>
-      <c r="N2" s="98"/>
-      <c r="O2" s="98"/>
-      <c r="P2" s="98"/>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
+      <c r="F2" s="97"/>
+      <c r="G2" s="97"/>
+      <c r="H2" s="97"/>
+      <c r="I2" s="97"/>
+      <c r="J2" s="97"/>
+      <c r="K2" s="97"/>
+      <c r="L2" s="97"/>
+      <c r="M2" s="97"/>
+      <c r="N2" s="97"/>
+      <c r="O2" s="97"/>
+      <c r="P2" s="97"/>
       <c r="Q2" s="56"/>
       <c r="R2" s="56"/>
     </row>
     <row r="3" spans="2:25" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="99" t="s">
+      <c r="B3" s="98" t="s">
         <v>109</v>
       </c>
-      <c r="C3" s="99"/>
-      <c r="D3" s="99"/>
-      <c r="E3" s="99"/>
-      <c r="F3" s="99"/>
-      <c r="G3" s="99"/>
-      <c r="H3" s="99"/>
-      <c r="I3" s="99"/>
-      <c r="J3" s="99"/>
-      <c r="K3" s="99"/>
-      <c r="L3" s="99"/>
-      <c r="M3" s="99"/>
-      <c r="N3" s="99"/>
-      <c r="O3" s="99"/>
-      <c r="P3" s="99"/>
+      <c r="C3" s="98"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="98"/>
+      <c r="F3" s="98"/>
+      <c r="G3" s="98"/>
+      <c r="H3" s="98"/>
+      <c r="I3" s="98"/>
+      <c r="J3" s="98"/>
+      <c r="K3" s="98"/>
+      <c r="L3" s="98"/>
+      <c r="M3" s="98"/>
+      <c r="N3" s="98"/>
+      <c r="O3" s="98"/>
+      <c r="P3" s="98"/>
       <c r="Q3" s="57"/>
       <c r="R3" s="57"/>
     </row>
     <row r="5" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B5" s="108" t="s">
+      <c r="B5" s="109" t="s">
         <v>110</v>
       </c>
-      <c r="C5" s="109"/>
-      <c r="D5" s="109"/>
-      <c r="E5" s="109"/>
-      <c r="F5" s="109"/>
-      <c r="G5" s="109"/>
-      <c r="H5" s="109"/>
-      <c r="I5" s="109"/>
-      <c r="J5" s="109"/>
-      <c r="K5" s="109"/>
-      <c r="L5" s="110"/>
-      <c r="M5" s="108" t="s">
+      <c r="C5" s="110"/>
+      <c r="D5" s="110"/>
+      <c r="E5" s="110"/>
+      <c r="F5" s="110"/>
+      <c r="G5" s="110"/>
+      <c r="H5" s="110"/>
+      <c r="I5" s="110"/>
+      <c r="J5" s="110"/>
+      <c r="K5" s="110"/>
+      <c r="L5" s="111"/>
+      <c r="M5" s="109" t="s">
         <v>111</v>
       </c>
-      <c r="N5" s="109"/>
-      <c r="O5" s="109"/>
-      <c r="P5" s="109"/>
-      <c r="Q5" s="109"/>
-      <c r="R5" s="109"/>
-      <c r="S5" s="109"/>
-      <c r="T5" s="109"/>
-      <c r="U5" s="109"/>
-      <c r="V5" s="109"/>
-      <c r="W5" s="109"/>
-      <c r="X5" s="109"/>
-      <c r="Y5" s="110"/>
+      <c r="N5" s="110"/>
+      <c r="O5" s="110"/>
+      <c r="P5" s="110"/>
+      <c r="Q5" s="110"/>
+      <c r="R5" s="110"/>
+      <c r="S5" s="110"/>
+      <c r="T5" s="110"/>
+      <c r="U5" s="110"/>
+      <c r="V5" s="110"/>
+      <c r="W5" s="110"/>
+      <c r="X5" s="110"/>
+      <c r="Y5" s="111"/>
     </row>
     <row r="6" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B6" s="117"/>
-      <c r="C6" s="117"/>
-      <c r="D6" s="117"/>
-      <c r="E6" s="117"/>
-      <c r="F6" s="111" t="s">
+      <c r="B6" s="119"/>
+      <c r="C6" s="119"/>
+      <c r="D6" s="119"/>
+      <c r="E6" s="119"/>
+      <c r="F6" s="115" t="s">
         <v>27</v>
       </c>
-      <c r="G6" s="112"/>
-      <c r="H6" s="112"/>
-      <c r="I6" s="113"/>
-      <c r="J6" s="108" t="s">
+      <c r="G6" s="116"/>
+      <c r="H6" s="116"/>
+      <c r="I6" s="117"/>
+      <c r="J6" s="109" t="s">
         <v>30</v>
       </c>
-      <c r="K6" s="109"/>
-      <c r="L6" s="110"/>
-      <c r="M6" s="88"/>
-      <c r="N6" s="114" t="s">
+      <c r="K6" s="110"/>
+      <c r="L6" s="111"/>
+      <c r="M6" s="87"/>
+      <c r="N6" s="107" t="s">
         <v>42</v>
       </c>
-      <c r="O6" s="115"/>
-      <c r="P6" s="114" t="s">
+      <c r="O6" s="108"/>
+      <c r="P6" s="107" t="s">
         <v>104</v>
       </c>
-      <c r="Q6" s="116"/>
-      <c r="R6" s="115"/>
-      <c r="S6" s="88"/>
-      <c r="T6" s="114" t="s">
+      <c r="Q6" s="118"/>
+      <c r="R6" s="108"/>
+      <c r="S6" s="87"/>
+      <c r="T6" s="107" t="s">
         <v>121</v>
       </c>
-      <c r="U6" s="115"/>
-      <c r="V6" s="118"/>
-      <c r="W6" s="119"/>
-      <c r="X6" s="119"/>
-      <c r="Y6" s="120"/>
+      <c r="U6" s="108"/>
+      <c r="V6" s="112"/>
+      <c r="W6" s="113"/>
+      <c r="X6" s="113"/>
+      <c r="Y6" s="114"/>
     </row>
     <row r="7" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B7" s="75" t="s">
@@ -5895,6 +5892,7 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B6:E6"/>
     <mergeCell ref="T6:U6"/>
     <mergeCell ref="M5:Y5"/>
     <mergeCell ref="V6:Y6"/>
@@ -5905,7 +5903,6 @@
     <mergeCell ref="F6:I6"/>
     <mergeCell ref="N6:O6"/>
     <mergeCell ref="P6:R6"/>
-    <mergeCell ref="B6:E6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -6004,7 +6001,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
@@ -6024,18 +6021,18 @@
       </c>
     </row>
     <row r="2" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="98"/>
-      <c r="C2" s="98"/>
-      <c r="D2" s="98"/>
-      <c r="E2" s="98"/>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
     </row>
     <row r="3" spans="2:5" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="99" t="s">
+      <c r="B3" s="98" t="s">
         <v>129</v>
       </c>
-      <c r="C3" s="99"/>
-      <c r="D3" s="99"/>
-      <c r="E3" s="99"/>
+      <c r="C3" s="98"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="98"/>
     </row>
     <row r="4" spans="2:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="64"/>
@@ -6047,16 +6044,16 @@
       <c r="C5" s="44" t="s">
         <v>130</v>
       </c>
-      <c r="D5" s="97" t="s">
+      <c r="D5" s="96" t="s">
         <v>131</v>
       </c>
-      <c r="E5" s="97" t="s">
+      <c r="E5" s="96" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="6" spans="2:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
-      <c r="C6" s="90"/>
+      <c r="C6" s="89"/>
       <c r="D6" s="66"/>
       <c r="E6" s="66"/>
     </row>
@@ -6096,40 +6093,40 @@
       </c>
     </row>
     <row r="2" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="98"/>
-      <c r="C2" s="98"/>
-      <c r="D2" s="98"/>
-      <c r="E2" s="98"/>
-      <c r="F2" s="98"/>
-      <c r="G2" s="98"/>
-      <c r="H2" s="98"/>
-      <c r="I2" s="98"/>
-      <c r="J2" s="98"/>
-      <c r="K2" s="98"/>
-      <c r="L2" s="98"/>
-      <c r="M2" s="98"/>
-      <c r="N2" s="98"/>
-      <c r="O2" s="98"/>
-      <c r="P2" s="98"/>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
+      <c r="F2" s="97"/>
+      <c r="G2" s="97"/>
+      <c r="H2" s="97"/>
+      <c r="I2" s="97"/>
+      <c r="J2" s="97"/>
+      <c r="K2" s="97"/>
+      <c r="L2" s="97"/>
+      <c r="M2" s="97"/>
+      <c r="N2" s="97"/>
+      <c r="O2" s="97"/>
+      <c r="P2" s="97"/>
     </row>
     <row r="3" spans="2:16" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="99" t="s">
+      <c r="B3" s="98" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="99"/>
-      <c r="D3" s="99"/>
-      <c r="E3" s="99"/>
-      <c r="F3" s="99"/>
-      <c r="G3" s="99"/>
-      <c r="H3" s="99"/>
-      <c r="I3" s="99"/>
-      <c r="J3" s="99"/>
-      <c r="K3" s="99"/>
-      <c r="L3" s="99"/>
-      <c r="M3" s="99"/>
-      <c r="N3" s="99"/>
-      <c r="O3" s="99"/>
-      <c r="P3" s="99"/>
+      <c r="C3" s="98"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="98"/>
+      <c r="F3" s="98"/>
+      <c r="G3" s="98"/>
+      <c r="H3" s="98"/>
+      <c r="I3" s="98"/>
+      <c r="J3" s="98"/>
+      <c r="K3" s="98"/>
+      <c r="L3" s="98"/>
+      <c r="M3" s="98"/>
+      <c r="N3" s="98"/>
+      <c r="O3" s="98"/>
+      <c r="P3" s="98"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="44" t="s">
@@ -6208,40 +6205,40 @@
       </c>
     </row>
     <row r="2" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="98"/>
-      <c r="C2" s="98"/>
-      <c r="D2" s="98"/>
-      <c r="E2" s="98"/>
-      <c r="F2" s="98"/>
-      <c r="G2" s="98"/>
-      <c r="H2" s="98"/>
-      <c r="I2" s="98"/>
-      <c r="J2" s="98"/>
-      <c r="K2" s="98"/>
-      <c r="L2" s="98"/>
-      <c r="M2" s="98"/>
-      <c r="N2" s="98"/>
-      <c r="O2" s="98"/>
-      <c r="P2" s="98"/>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
+      <c r="F2" s="97"/>
+      <c r="G2" s="97"/>
+      <c r="H2" s="97"/>
+      <c r="I2" s="97"/>
+      <c r="J2" s="97"/>
+      <c r="K2" s="97"/>
+      <c r="L2" s="97"/>
+      <c r="M2" s="97"/>
+      <c r="N2" s="97"/>
+      <c r="O2" s="97"/>
+      <c r="P2" s="97"/>
     </row>
     <row r="3" spans="2:16" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="99" t="s">
+      <c r="B3" s="98" t="s">
         <v>68</v>
       </c>
-      <c r="C3" s="99"/>
-      <c r="D3" s="99"/>
-      <c r="E3" s="99"/>
-      <c r="F3" s="99"/>
-      <c r="G3" s="99"/>
-      <c r="H3" s="99"/>
-      <c r="I3" s="99"/>
-      <c r="J3" s="99"/>
-      <c r="K3" s="99"/>
-      <c r="L3" s="99"/>
-      <c r="M3" s="99"/>
-      <c r="N3" s="99"/>
-      <c r="O3" s="99"/>
-      <c r="P3" s="99"/>
+      <c r="C3" s="98"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="98"/>
+      <c r="F3" s="98"/>
+      <c r="G3" s="98"/>
+      <c r="H3" s="98"/>
+      <c r="I3" s="98"/>
+      <c r="J3" s="98"/>
+      <c r="K3" s="98"/>
+      <c r="L3" s="98"/>
+      <c r="M3" s="98"/>
+      <c r="N3" s="98"/>
+      <c r="O3" s="98"/>
+      <c r="P3" s="98"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
@@ -6290,40 +6287,40 @@
       </c>
     </row>
     <row r="2" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="98"/>
-      <c r="C2" s="98"/>
-      <c r="D2" s="98"/>
-      <c r="E2" s="98"/>
-      <c r="F2" s="98"/>
-      <c r="G2" s="98"/>
-      <c r="H2" s="98"/>
-      <c r="I2" s="98"/>
-      <c r="J2" s="98"/>
-      <c r="K2" s="98"/>
-      <c r="L2" s="98"/>
-      <c r="M2" s="98"/>
-      <c r="N2" s="98"/>
-      <c r="O2" s="98"/>
-      <c r="P2" s="98"/>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
+      <c r="F2" s="97"/>
+      <c r="G2" s="97"/>
+      <c r="H2" s="97"/>
+      <c r="I2" s="97"/>
+      <c r="J2" s="97"/>
+      <c r="K2" s="97"/>
+      <c r="L2" s="97"/>
+      <c r="M2" s="97"/>
+      <c r="N2" s="97"/>
+      <c r="O2" s="97"/>
+      <c r="P2" s="97"/>
     </row>
     <row r="3" spans="2:16" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="99" t="s">
+      <c r="B3" s="98" t="s">
         <v>71</v>
       </c>
-      <c r="C3" s="99"/>
-      <c r="D3" s="99"/>
-      <c r="E3" s="99"/>
-      <c r="F3" s="99"/>
-      <c r="G3" s="99"/>
-      <c r="H3" s="99"/>
-      <c r="I3" s="99"/>
-      <c r="J3" s="99"/>
-      <c r="K3" s="99"/>
-      <c r="L3" s="99"/>
-      <c r="M3" s="99"/>
-      <c r="N3" s="99"/>
-      <c r="O3" s="99"/>
-      <c r="P3" s="99"/>
+      <c r="C3" s="98"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="98"/>
+      <c r="F3" s="98"/>
+      <c r="G3" s="98"/>
+      <c r="H3" s="98"/>
+      <c r="I3" s="98"/>
+      <c r="J3" s="98"/>
+      <c r="K3" s="98"/>
+      <c r="L3" s="98"/>
+      <c r="M3" s="98"/>
+      <c r="N3" s="98"/>
+      <c r="O3" s="98"/>
+      <c r="P3" s="98"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
@@ -6378,40 +6375,40 @@
       </c>
     </row>
     <row r="2" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="98"/>
-      <c r="C2" s="98"/>
-      <c r="D2" s="98"/>
-      <c r="E2" s="98"/>
-      <c r="F2" s="98"/>
-      <c r="G2" s="98"/>
-      <c r="H2" s="98"/>
-      <c r="I2" s="98"/>
-      <c r="J2" s="98"/>
-      <c r="K2" s="98"/>
-      <c r="L2" s="98"/>
-      <c r="M2" s="98"/>
-      <c r="N2" s="98"/>
-      <c r="O2" s="98"/>
-      <c r="P2" s="98"/>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
+      <c r="F2" s="97"/>
+      <c r="G2" s="97"/>
+      <c r="H2" s="97"/>
+      <c r="I2" s="97"/>
+      <c r="J2" s="97"/>
+      <c r="K2" s="97"/>
+      <c r="L2" s="97"/>
+      <c r="M2" s="97"/>
+      <c r="N2" s="97"/>
+      <c r="O2" s="97"/>
+      <c r="P2" s="97"/>
     </row>
     <row r="3" spans="2:16" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="99" t="s">
+      <c r="B3" s="98" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="99"/>
-      <c r="D3" s="99"/>
-      <c r="E3" s="99"/>
-      <c r="F3" s="99"/>
-      <c r="G3" s="99"/>
-      <c r="H3" s="99"/>
-      <c r="I3" s="99"/>
-      <c r="J3" s="99"/>
-      <c r="K3" s="99"/>
-      <c r="L3" s="99"/>
-      <c r="M3" s="99"/>
-      <c r="N3" s="99"/>
-      <c r="O3" s="99"/>
-      <c r="P3" s="99"/>
+      <c r="C3" s="98"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="98"/>
+      <c r="F3" s="98"/>
+      <c r="G3" s="98"/>
+      <c r="H3" s="98"/>
+      <c r="I3" s="98"/>
+      <c r="J3" s="98"/>
+      <c r="K3" s="98"/>
+      <c r="L3" s="98"/>
+      <c r="M3" s="98"/>
+      <c r="N3" s="98"/>
+      <c r="O3" s="98"/>
+      <c r="P3" s="98"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="44" t="s">
@@ -6441,10 +6438,10 @@
       <c r="J5" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="K5" s="91" t="s">
+      <c r="K5" s="90" t="s">
         <v>191</v>
       </c>
-      <c r="L5" s="91" t="s">
+      <c r="L5" s="90" t="s">
         <v>192</v>
       </c>
       <c r="M5" s="45" t="s">
@@ -6508,40 +6505,40 @@
       </c>
     </row>
     <row r="2" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="98"/>
-      <c r="C2" s="98"/>
-      <c r="D2" s="98"/>
-      <c r="E2" s="98"/>
-      <c r="F2" s="98"/>
-      <c r="G2" s="98"/>
-      <c r="H2" s="98"/>
-      <c r="I2" s="98"/>
-      <c r="J2" s="98"/>
-      <c r="K2" s="98"/>
-      <c r="L2" s="98"/>
-      <c r="M2" s="98"/>
-      <c r="N2" s="98"/>
-      <c r="O2" s="98"/>
-      <c r="P2" s="98"/>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
+      <c r="F2" s="97"/>
+      <c r="G2" s="97"/>
+      <c r="H2" s="97"/>
+      <c r="I2" s="97"/>
+      <c r="J2" s="97"/>
+      <c r="K2" s="97"/>
+      <c r="L2" s="97"/>
+      <c r="M2" s="97"/>
+      <c r="N2" s="97"/>
+      <c r="O2" s="97"/>
+      <c r="P2" s="97"/>
     </row>
     <row r="3" spans="2:16" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="99" t="s">
+      <c r="B3" s="98" t="s">
         <v>65</v>
       </c>
-      <c r="C3" s="99"/>
-      <c r="D3" s="99"/>
-      <c r="E3" s="99"/>
-      <c r="F3" s="99"/>
-      <c r="G3" s="99"/>
-      <c r="H3" s="99"/>
-      <c r="I3" s="99"/>
-      <c r="J3" s="99"/>
-      <c r="K3" s="99"/>
-      <c r="L3" s="99"/>
-      <c r="M3" s="99"/>
-      <c r="N3" s="99"/>
-      <c r="O3" s="99"/>
-      <c r="P3" s="99"/>
+      <c r="C3" s="98"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="98"/>
+      <c r="F3" s="98"/>
+      <c r="G3" s="98"/>
+      <c r="H3" s="98"/>
+      <c r="I3" s="98"/>
+      <c r="J3" s="98"/>
+      <c r="K3" s="98"/>
+      <c r="L3" s="98"/>
+      <c r="M3" s="98"/>
+      <c r="N3" s="98"/>
+      <c r="O3" s="98"/>
+      <c r="P3" s="98"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="45" t="s">
@@ -6550,14 +6547,14 @@
       <c r="C5" s="45" t="s">
         <v>67</v>
       </c>
-      <c r="D5" s="91" t="s">
+      <c r="D5" s="90" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
-      <c r="D6" s="90"/>
+      <c r="D6" s="89"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
TRIEDA-1708 - Alterando texto "Usa Laboratório?" para "Exige Laboratório?" em disciplinas.
</commit_message>
<xml_diff>
--- a/code/client/web/src/main/resources/templateExport.xlsx
+++ b/code/client/web/src/main/resources/templateExport.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="17070" windowHeight="5370" tabRatio="954" firstSheet="23" activeTab="23"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="17070" windowHeight="5370" tabRatio="954" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Campi" sheetId="3" r:id="rId1"/>
@@ -1359,9 +1359,6 @@
     <t>Créditos Práticos</t>
   </si>
   <si>
-    <t>Usa Laboratório?</t>
-  </si>
-  <si>
     <t>Nível de Dificuldade</t>
   </si>
   <si>
@@ -1897,6 +1894,9 @@
   </si>
   <si>
     <t>Custo de Operação por Crédito (R$)</t>
+  </si>
+  <si>
+    <t>Exige Laboratório?</t>
   </si>
 </sst>
 </file>
@@ -2630,6 +2630,9 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="28" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2665,9 +2668,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="28" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2992,12 +2992,12 @@
   <sheetData>
     <row r="1" spans="2:14" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="97" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C2" s="97"/>
       <c r="D2" s="97"/>
@@ -3031,7 +3031,7 @@
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="44" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>1</v>
@@ -3090,7 +3090,7 @@
   <sheetData>
     <row r="1" spans="2:11" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3107,7 +3107,7 @@
     </row>
     <row r="3" spans="2:11" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="98" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C3" s="98"/>
       <c r="D3" s="98"/>
@@ -3121,10 +3121,10 @@
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
@@ -3164,7 +3164,7 @@
   <sheetData>
     <row r="1" spans="2:14" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3184,7 +3184,7 @@
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="98" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C3" s="98"/>
       <c r="D3" s="98"/>
@@ -3201,22 +3201,22 @@
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>88</v>
-      </c>
       <c r="E5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>27</v>
-      </c>
       <c r="G5" s="47" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
@@ -3262,7 +3262,7 @@
   <sheetData>
     <row r="1" spans="2:14" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3282,7 +3282,7 @@
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="98" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C3" s="98"/>
       <c r="D3" s="98"/>
@@ -3299,40 +3299,40 @@
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="E5" s="4" t="s">
+      <c r="F5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="H5" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>30</v>
-      </c>
       <c r="I5" s="45" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J5" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="K5" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="K5" s="4" t="s">
-        <v>105</v>
-      </c>
       <c r="L5" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
@@ -3376,7 +3376,7 @@
   <sheetData>
     <row r="1" spans="2:5" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3387,7 +3387,7 @@
     </row>
     <row r="3" spans="2:5" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="98" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C3" s="98"/>
       <c r="D3" s="98"/>
@@ -3395,13 +3395,13 @@
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="60" t="s">
+        <v>98</v>
+      </c>
+      <c r="C5" s="59" t="s">
         <v>99</v>
       </c>
-      <c r="C5" s="59" t="s">
-        <v>100</v>
-      </c>
       <c r="D5" s="59" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
@@ -3440,7 +3440,7 @@
   <sheetData>
     <row r="1" spans="2:14" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3460,7 +3460,7 @@
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="98" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C3" s="98"/>
       <c r="D3" s="98"/>
@@ -3477,37 +3477,37 @@
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>29</v>
-      </c>
       <c r="F5" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H5" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="I5" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="J5" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="J5" s="4" t="s">
+      <c r="K5" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="K5" s="4" t="s">
-        <v>102</v>
-      </c>
       <c r="L5" s="100" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="M5" s="100"/>
     </row>
@@ -3560,7 +3560,7 @@
   <sheetData>
     <row r="1" spans="2:15" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="2:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3581,7 +3581,7 @@
     </row>
     <row r="3" spans="2:15" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="98" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C3" s="98"/>
       <c r="D3" s="98"/>
@@ -3599,40 +3599,40 @@
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D5" s="45" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" s="45" t="s">
         <v>45</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="F5" s="45" t="s">
+        <v>46</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I5" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="J5" s="45" t="s">
         <v>89</v>
       </c>
-      <c r="D5" s="45" t="s">
-        <v>50</v>
-      </c>
-      <c r="E5" s="45" t="s">
-        <v>46</v>
-      </c>
-      <c r="F5" s="45" t="s">
-        <v>47</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="I5" s="45" t="s">
-        <v>52</v>
-      </c>
-      <c r="J5" s="45" t="s">
-        <v>90</v>
-      </c>
       <c r="K5" s="45" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="L5" s="94" t="s">
+        <v>192</v>
+      </c>
+      <c r="M5" s="94" t="s">
         <v>193</v>
-      </c>
-      <c r="M5" s="94" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.25">
@@ -3678,7 +3678,7 @@
   <sheetData>
     <row r="1" spans="2:5" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3689,7 +3689,7 @@
     </row>
     <row r="3" spans="2:5" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="98" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C3" s="98"/>
       <c r="D3" s="98"/>
@@ -3700,16 +3700,16 @@
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="62" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C5" s="44" t="s">
+        <v>129</v>
+      </c>
+      <c r="D5" s="61" t="s">
         <v>130</v>
       </c>
-      <c r="D5" s="61" t="s">
+      <c r="E5" s="61" t="s">
         <v>131</v>
-      </c>
-      <c r="E5" s="61" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="6" spans="2:5" customFormat="1" x14ac:dyDescent="0.25">
@@ -3751,7 +3751,7 @@
   <sheetData>
     <row r="1" spans="2:14" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3771,7 +3771,7 @@
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="98" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C3" s="98"/>
       <c r="D3" s="98"/>
@@ -3788,13 +3788,13 @@
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
@@ -3835,7 +3835,7 @@
   <sheetData>
     <row r="1" spans="2:14" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3855,7 +3855,7 @@
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="98" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C3" s="98"/>
       <c r="D3" s="98"/>
@@ -3872,16 +3872,16 @@
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D5" s="45" t="s">
+        <v>50</v>
+      </c>
+      <c r="E5" s="45" t="s">
         <v>51</v>
-      </c>
-      <c r="E5" s="45" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
@@ -3933,7 +3933,7 @@
   <sheetData>
     <row r="1" spans="2:18" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="2:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3955,7 +3955,7 @@
     </row>
     <row r="3" spans="2:18" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="98" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C3" s="98"/>
       <c r="D3" s="98"/>
@@ -3977,52 +3977,52 @@
         <v>2</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="F5" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F5" s="4" t="s">
+      <c r="G5" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="4" t="s">
-        <v>27</v>
-      </c>
       <c r="H5" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="I5" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="J5" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="K5" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="J5" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="K5" s="4" t="s">
+      <c r="L5" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="L5" s="4" t="s">
+      <c r="M5" s="53" t="s">
+        <v>95</v>
+      </c>
+      <c r="N5" s="53" t="s">
+        <v>88</v>
+      </c>
+      <c r="O5" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="M5" s="53" t="s">
-        <v>96</v>
-      </c>
-      <c r="N5" s="53" t="s">
-        <v>89</v>
-      </c>
-      <c r="O5" s="4" t="s">
+      <c r="P5" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="P5" s="4" t="s">
+      <c r="Q5" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="Q5" s="4" t="s">
+      <c r="R5" s="4" t="s">
         <v>59</v>
-      </c>
-      <c r="R5" s="4" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.25">
@@ -4077,12 +4077,12 @@
   <sheetData>
     <row r="1" spans="2:14" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="97" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C2" s="97"/>
       <c r="D2" s="97"/>
@@ -4116,13 +4116,13 @@
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="44" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
@@ -4167,7 +4167,7 @@
   <sheetData>
     <row r="1" spans="2:14" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -4187,7 +4187,7 @@
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="98" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C3" s="98"/>
       <c r="D3" s="98"/>
@@ -4207,34 +4207,34 @@
         <v>2</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E5" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G5" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>62</v>
-      </c>
       <c r="H5" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I5" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="J5" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="J5" s="4" t="s">
+      <c r="K5" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="K5" s="4" t="s">
+      <c r="L5" s="4" t="s">
         <v>59</v>
-      </c>
-      <c r="L5" s="4" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
@@ -4286,7 +4286,7 @@
   <sheetData>
     <row r="1" spans="2:14" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -4306,7 +4306,7 @@
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="98" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C3" s="98"/>
       <c r="D3" s="98"/>
@@ -4326,34 +4326,34 @@
         <v>2</v>
       </c>
       <c r="C5" s="74" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D5" s="74" t="s">
+        <v>140</v>
+      </c>
+      <c r="E5" s="74" t="s">
         <v>141</v>
       </c>
-      <c r="E5" s="74" t="s">
+      <c r="F5" s="74" t="s">
         <v>142</v>
       </c>
-      <c r="F5" s="74" t="s">
+      <c r="G5" s="74" t="s">
         <v>143</v>
       </c>
-      <c r="G5" s="74" t="s">
+      <c r="H5" s="74" t="s">
         <v>144</v>
       </c>
-      <c r="H5" s="74" t="s">
+      <c r="I5" s="74" t="s">
         <v>145</v>
       </c>
-      <c r="I5" s="74" t="s">
+      <c r="J5" s="74" t="s">
         <v>146</v>
       </c>
-      <c r="J5" s="74" t="s">
+      <c r="K5" s="74" t="s">
         <v>147</v>
       </c>
-      <c r="K5" s="74" t="s">
+      <c r="L5" s="74" t="s">
         <v>148</v>
-      </c>
-      <c r="L5" s="74" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
@@ -4402,7 +4402,7 @@
   <sheetData>
     <row r="1" spans="2:10" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -4418,7 +4418,7 @@
     </row>
     <row r="3" spans="2:10" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="98" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C3" s="98"/>
       <c r="D3" s="98"/>
@@ -4434,25 +4434,25 @@
         <v>2</v>
       </c>
       <c r="C5" s="74" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D5" s="74" t="s">
+        <v>140</v>
+      </c>
+      <c r="E5" s="74" t="s">
         <v>141</v>
       </c>
-      <c r="E5" s="74" t="s">
+      <c r="F5" s="74" t="s">
         <v>142</v>
       </c>
-      <c r="F5" s="74" t="s">
+      <c r="G5" s="74" t="s">
         <v>143</v>
       </c>
-      <c r="G5" s="74" t="s">
-        <v>144</v>
-      </c>
       <c r="H5" s="74" t="s">
+        <v>150</v>
+      </c>
+      <c r="I5" s="74" t="s">
         <v>151</v>
-      </c>
-      <c r="I5" s="74" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
@@ -4508,7 +4508,7 @@
   <sheetData>
     <row r="1" spans="2:20" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="2:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -4526,7 +4526,7 @@
     </row>
     <row r="3" spans="2:20" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="98" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C3" s="98"/>
       <c r="D3" s="98"/>
@@ -4544,58 +4544,58 @@
         <v>2</v>
       </c>
       <c r="C5" s="79" t="s">
+        <v>154</v>
+      </c>
+      <c r="D5" s="79" t="s">
+        <v>140</v>
+      </c>
+      <c r="E5" s="79" t="s">
         <v>155</v>
       </c>
-      <c r="D5" s="79" t="s">
-        <v>141</v>
-      </c>
-      <c r="E5" s="79" t="s">
+      <c r="F5" s="79" t="s">
         <v>156</v>
       </c>
-      <c r="F5" s="79" t="s">
+      <c r="G5" s="79" t="s">
         <v>157</v>
       </c>
-      <c r="G5" s="79" t="s">
+      <c r="H5" s="79" t="s">
         <v>158</v>
       </c>
-      <c r="H5" s="79" t="s">
+      <c r="I5" s="79" t="s">
+        <v>162</v>
+      </c>
+      <c r="J5" s="79" t="s">
+        <v>163</v>
+      </c>
+      <c r="K5" s="79" t="s">
+        <v>164</v>
+      </c>
+      <c r="L5" s="79" t="s">
         <v>159</v>
       </c>
-      <c r="I5" s="79" t="s">
-        <v>163</v>
-      </c>
-      <c r="J5" s="79" t="s">
-        <v>164</v>
-      </c>
-      <c r="K5" s="79" t="s">
-        <v>165</v>
-      </c>
-      <c r="L5" s="79" t="s">
+      <c r="M5" s="79" t="s">
         <v>160</v>
       </c>
-      <c r="M5" s="79" t="s">
+      <c r="N5" s="79" t="s">
         <v>161</v>
       </c>
-      <c r="N5" s="79" t="s">
-        <v>162</v>
-      </c>
       <c r="O5" s="86" t="s">
+        <v>174</v>
+      </c>
+      <c r="P5" s="86" t="s">
         <v>175</v>
       </c>
-      <c r="P5" s="86" t="s">
+      <c r="Q5" s="86" t="s">
+        <v>179</v>
+      </c>
+      <c r="R5" s="86" t="s">
         <v>176</v>
       </c>
-      <c r="Q5" s="86" t="s">
-        <v>180</v>
-      </c>
-      <c r="R5" s="86" t="s">
+      <c r="S5" s="86" t="s">
         <v>177</v>
       </c>
-      <c r="S5" s="86" t="s">
+      <c r="T5" s="86" t="s">
         <v>178</v>
-      </c>
-      <c r="T5" s="86" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.25">
@@ -4633,7 +4633,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:I6"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
@@ -4651,7 +4651,7 @@
   <sheetData>
     <row r="1" spans="2:9" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="2:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -4666,7 +4666,7 @@
     </row>
     <row r="3" spans="2:9" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="98" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C3" s="98"/>
       <c r="D3" s="98"/>
@@ -4678,28 +4678,28 @@
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="88" t="s">
+        <v>181</v>
+      </c>
+      <c r="C5" s="88" t="s">
         <v>182</v>
       </c>
-      <c r="C5" s="88" t="s">
+      <c r="D5" s="88" t="s">
         <v>183</v>
       </c>
-      <c r="D5" s="88" t="s">
+      <c r="E5" s="88" t="s">
         <v>184</v>
       </c>
-      <c r="E5" s="88" t="s">
+      <c r="F5" s="88" t="s">
         <v>185</v>
       </c>
-      <c r="F5" s="88" t="s">
+      <c r="G5" s="88" t="s">
         <v>186</v>
       </c>
-      <c r="G5" s="88" t="s">
+      <c r="H5" s="88" t="s">
         <v>187</v>
       </c>
-      <c r="H5" s="88" t="s">
+      <c r="I5" s="88" t="s">
         <v>188</v>
-      </c>
-      <c r="I5" s="88" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
@@ -4746,7 +4746,7 @@
   <sheetData>
     <row r="1" spans="2:11" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -4763,7 +4763,7 @@
     </row>
     <row r="3" spans="2:11" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="98" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C3" s="98"/>
       <c r="D3" s="98"/>
@@ -4789,11 +4789,11 @@
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="H5" s="101" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="I5" s="102"/>
       <c r="J5" s="101" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="K5" s="102"/>
     </row>
@@ -4802,31 +4802,31 @@
         <v>2</v>
       </c>
       <c r="C6" s="85" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D6" s="85" t="s">
+        <v>166</v>
+      </c>
+      <c r="E6" s="85" t="s">
         <v>167</v>
       </c>
-      <c r="E6" s="85" t="s">
+      <c r="F6" s="85" t="s">
+        <v>113</v>
+      </c>
+      <c r="G6" s="85" t="s">
+        <v>113</v>
+      </c>
+      <c r="H6" s="85" t="s">
         <v>168</v>
       </c>
-      <c r="F6" s="85" t="s">
-        <v>114</v>
-      </c>
-      <c r="G6" s="85" t="s">
-        <v>114</v>
-      </c>
-      <c r="H6" s="85" t="s">
+      <c r="I6" s="85" t="s">
         <v>169</v>
       </c>
-      <c r="I6" s="85" t="s">
+      <c r="J6" s="85" t="s">
         <v>170</v>
       </c>
-      <c r="J6" s="85" t="s">
+      <c r="K6" s="85" t="s">
         <v>171</v>
-      </c>
-      <c r="K6" s="85" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
@@ -4872,7 +4872,7 @@
   <sheetData>
     <row r="1" spans="2:26" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="Z1" s="38"/>
     </row>
@@ -4894,7 +4894,7 @@
     </row>
     <row r="3" spans="2:26" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="98" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C3" s="98"/>
       <c r="D3" s="98"/>
@@ -4916,7 +4916,7 @@
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F5" s="13"/>
       <c r="G5" s="11" t="s">
@@ -4930,7 +4930,7 @@
       </c>
       <c r="D6" s="12"/>
       <c r="E6" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F6" s="12"/>
       <c r="G6" s="10" t="s">
@@ -4940,28 +4940,28 @@
     </row>
     <row r="7" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C7" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="E7" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="F7" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="G7" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="H7" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="I7" s="4" t="s">
         <v>40</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="8" spans="2:26" x14ac:dyDescent="0.25">
@@ -5006,7 +5006,7 @@
   <sheetData>
     <row r="1" spans="2:26" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="Z1" s="38"/>
     </row>
@@ -5028,7 +5028,7 @@
     </row>
     <row r="3" spans="2:26" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="98" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C3" s="98"/>
       <c r="D3" s="98"/>
@@ -5050,7 +5050,7 @@
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="51" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F5" s="13"/>
       <c r="G5" s="48"/>
@@ -5058,7 +5058,7 @@
     </row>
     <row r="6" spans="2:26" x14ac:dyDescent="0.25">
       <c r="C6" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D6" s="103"/>
       <c r="E6" s="104"/>
@@ -5068,28 +5068,28 @@
     </row>
     <row r="7" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C7" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="E7" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="F7" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="G7" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="H7" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="H7" s="41" t="s">
+      <c r="I7" s="4" t="s">
         <v>40</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="8" spans="2:26" x14ac:dyDescent="0.25">
@@ -5135,7 +5135,7 @@
   <sheetData>
     <row r="1" spans="2:26" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="Z1" s="38"/>
     </row>
@@ -5157,7 +5157,7 @@
     </row>
     <row r="3" spans="2:26" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="98" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C3" s="98"/>
       <c r="D3" s="98"/>
@@ -5179,44 +5179,44 @@
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F5" s="13"/>
     </row>
     <row r="6" spans="2:26" x14ac:dyDescent="0.25">
       <c r="C6" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D6" s="12"/>
       <c r="E6" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F6" s="12"/>
     </row>
     <row r="7" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C7" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="E7" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="F7" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="G7" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="H7" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="I7" s="4" t="s">
         <v>40</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="8" spans="2:26" x14ac:dyDescent="0.25">
@@ -5258,7 +5258,7 @@
   <sheetData>
     <row r="1" spans="2:26" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="Z1" s="38"/>
     </row>
@@ -5280,7 +5280,7 @@
     </row>
     <row r="3" spans="2:26" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="98" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C3" s="98"/>
       <c r="D3" s="98"/>
@@ -5298,7 +5298,7 @@
     </row>
     <row r="5" spans="2:26" x14ac:dyDescent="0.25">
       <c r="C5" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="11" t="s">
@@ -5306,17 +5306,17 @@
       </c>
       <c r="F5" s="13"/>
       <c r="G5" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H5" s="12"/>
     </row>
     <row r="6" spans="2:26" x14ac:dyDescent="0.25">
       <c r="C6" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D6" s="12"/>
       <c r="E6" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F6" s="40"/>
       <c r="G6" s="42"/>
@@ -5324,28 +5324,28 @@
     </row>
     <row r="7" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C7" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="E7" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="F7" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="G7" s="41" t="s">
         <v>38</v>
       </c>
-      <c r="G7" s="41" t="s">
+      <c r="H7" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="H7" s="41" t="s">
+      <c r="I7" s="4" t="s">
         <v>40</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="8" spans="2:26" x14ac:dyDescent="0.25">
@@ -5395,7 +5395,7 @@
   <sheetData>
     <row r="1" spans="2:14" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -5432,13 +5432,13 @@
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="44" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C5" s="44" t="s">
         <v>8</v>
       </c>
       <c r="D5" s="45" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>10</v>
@@ -5447,13 +5447,13 @@
         <v>11</v>
       </c>
       <c r="G5" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="H5" s="95" t="s">
         <v>195</v>
       </c>
-      <c r="H5" s="95" t="s">
+      <c r="I5" s="95" t="s">
         <v>196</v>
-      </c>
-      <c r="I5" s="95" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
@@ -5508,7 +5508,7 @@
   <sheetData>
     <row r="1" spans="2:17" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -5526,7 +5526,7 @@
     </row>
     <row r="3" spans="2:17" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="98" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C3" s="98"/>
       <c r="D3" s="98"/>
@@ -5541,7 +5541,7 @@
     </row>
     <row r="5" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D5" s="106" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E5" s="106"/>
       <c r="F5" s="73"/>
@@ -5549,68 +5549,68 @@
       <c r="H5" s="73"/>
       <c r="I5" s="73"/>
       <c r="J5" s="106" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K5" s="106"/>
       <c r="L5" s="106"/>
       <c r="M5" s="106" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N5" s="106"/>
       <c r="O5" s="106"/>
       <c r="P5" s="100" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="Q5" s="100"/>
     </row>
     <row r="6" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="70" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C6" s="71" t="s">
+        <v>135</v>
+      </c>
+      <c r="D6" s="63" t="s">
+        <v>121</v>
+      </c>
+      <c r="E6" s="63" t="s">
+        <v>122</v>
+      </c>
+      <c r="F6" s="71" t="s">
         <v>136</v>
       </c>
-      <c r="D6" s="63" t="s">
-        <v>122</v>
-      </c>
-      <c r="E6" s="63" t="s">
-        <v>123</v>
-      </c>
-      <c r="F6" s="71" t="s">
+      <c r="G6" s="71" t="s">
         <v>137</v>
       </c>
-      <c r="G6" s="71" t="s">
-        <v>138</v>
-      </c>
       <c r="H6" s="72" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I6" s="70" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J6" s="63" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K6" s="63" t="s">
+        <v>125</v>
+      </c>
+      <c r="L6" s="69" t="s">
+        <v>113</v>
+      </c>
+      <c r="M6" s="63" t="s">
         <v>126</v>
       </c>
-      <c r="L6" s="69" t="s">
-        <v>114</v>
-      </c>
-      <c r="M6" s="63" t="s">
-        <v>127</v>
-      </c>
       <c r="N6" s="63" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="O6" s="69" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="P6" s="69" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Q6" s="69" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.25">
@@ -5681,7 +5681,7 @@
   <sheetData>
     <row r="1" spans="2:25" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="2:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -5705,7 +5705,7 @@
     </row>
     <row r="3" spans="2:25" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="98" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C3" s="98"/>
       <c r="D3" s="98"/>
@@ -5725,143 +5725,143 @@
       <c r="R3" s="57"/>
     </row>
     <row r="5" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B5" s="109" t="s">
+      <c r="B5" s="110" t="s">
+        <v>109</v>
+      </c>
+      <c r="C5" s="111"/>
+      <c r="D5" s="111"/>
+      <c r="E5" s="111"/>
+      <c r="F5" s="111"/>
+      <c r="G5" s="111"/>
+      <c r="H5" s="111"/>
+      <c r="I5" s="111"/>
+      <c r="J5" s="111"/>
+      <c r="K5" s="111"/>
+      <c r="L5" s="112"/>
+      <c r="M5" s="110" t="s">
         <v>110</v>
       </c>
-      <c r="C5" s="110"/>
-      <c r="D5" s="110"/>
-      <c r="E5" s="110"/>
-      <c r="F5" s="110"/>
-      <c r="G5" s="110"/>
-      <c r="H5" s="110"/>
-      <c r="I5" s="110"/>
-      <c r="J5" s="110"/>
-      <c r="K5" s="110"/>
-      <c r="L5" s="111"/>
-      <c r="M5" s="109" t="s">
-        <v>111</v>
-      </c>
-      <c r="N5" s="110"/>
-      <c r="O5" s="110"/>
-      <c r="P5" s="110"/>
-      <c r="Q5" s="110"/>
-      <c r="R5" s="110"/>
-      <c r="S5" s="110"/>
-      <c r="T5" s="110"/>
-      <c r="U5" s="110"/>
-      <c r="V5" s="110"/>
-      <c r="W5" s="110"/>
-      <c r="X5" s="110"/>
-      <c r="Y5" s="111"/>
+      <c r="N5" s="111"/>
+      <c r="O5" s="111"/>
+      <c r="P5" s="111"/>
+      <c r="Q5" s="111"/>
+      <c r="R5" s="111"/>
+      <c r="S5" s="111"/>
+      <c r="T5" s="111"/>
+      <c r="U5" s="111"/>
+      <c r="V5" s="111"/>
+      <c r="W5" s="111"/>
+      <c r="X5" s="111"/>
+      <c r="Y5" s="112"/>
     </row>
     <row r="6" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B6" s="119"/>
-      <c r="C6" s="119"/>
-      <c r="D6" s="119"/>
-      <c r="E6" s="119"/>
-      <c r="F6" s="115" t="s">
-        <v>27</v>
-      </c>
-      <c r="G6" s="116"/>
-      <c r="H6" s="116"/>
-      <c r="I6" s="117"/>
-      <c r="J6" s="109" t="s">
-        <v>30</v>
-      </c>
-      <c r="K6" s="110"/>
-      <c r="L6" s="111"/>
+      <c r="B6" s="107"/>
+      <c r="C6" s="107"/>
+      <c r="D6" s="107"/>
+      <c r="E6" s="107"/>
+      <c r="F6" s="116" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" s="117"/>
+      <c r="H6" s="117"/>
+      <c r="I6" s="118"/>
+      <c r="J6" s="110" t="s">
+        <v>29</v>
+      </c>
+      <c r="K6" s="111"/>
+      <c r="L6" s="112"/>
       <c r="M6" s="87"/>
-      <c r="N6" s="107" t="s">
-        <v>42</v>
-      </c>
-      <c r="O6" s="108"/>
-      <c r="P6" s="107" t="s">
-        <v>104</v>
-      </c>
-      <c r="Q6" s="118"/>
-      <c r="R6" s="108"/>
+      <c r="N6" s="108" t="s">
+        <v>41</v>
+      </c>
+      <c r="O6" s="109"/>
+      <c r="P6" s="108" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q6" s="119"/>
+      <c r="R6" s="109"/>
       <c r="S6" s="87"/>
-      <c r="T6" s="107" t="s">
-        <v>121</v>
-      </c>
-      <c r="U6" s="108"/>
-      <c r="V6" s="112"/>
-      <c r="W6" s="113"/>
-      <c r="X6" s="113"/>
-      <c r="Y6" s="114"/>
+      <c r="T6" s="108" t="s">
+        <v>120</v>
+      </c>
+      <c r="U6" s="109"/>
+      <c r="V6" s="113"/>
+      <c r="W6" s="114"/>
+      <c r="X6" s="114"/>
+      <c r="Y6" s="115"/>
     </row>
     <row r="7" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B7" s="75" t="s">
         <v>2</v>
       </c>
       <c r="C7" s="76" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="75" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="75" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="75" t="s">
-        <v>25</v>
-      </c>
-      <c r="E7" s="75" t="s">
-        <v>29</v>
-      </c>
       <c r="F7" s="77" t="s">
+        <v>114</v>
+      </c>
+      <c r="G7" s="77" t="s">
+        <v>118</v>
+      </c>
+      <c r="H7" s="77" t="s">
+        <v>119</v>
+      </c>
+      <c r="I7" s="77" t="s">
         <v>115</v>
       </c>
-      <c r="G7" s="77" t="s">
-        <v>119</v>
-      </c>
-      <c r="H7" s="77" t="s">
-        <v>120</v>
-      </c>
-      <c r="I7" s="77" t="s">
+      <c r="J7" s="77" t="s">
+        <v>111</v>
+      </c>
+      <c r="K7" s="77" t="s">
+        <v>112</v>
+      </c>
+      <c r="L7" s="77" t="s">
+        <v>113</v>
+      </c>
+      <c r="M7" s="76" t="s">
+        <v>52</v>
+      </c>
+      <c r="N7" s="77" t="s">
         <v>116</v>
       </c>
-      <c r="J7" s="77" t="s">
+      <c r="O7" s="77" t="s">
+        <v>117</v>
+      </c>
+      <c r="P7" s="77" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q7" s="77" t="s">
         <v>112</v>
       </c>
-      <c r="K7" s="77" t="s">
+      <c r="R7" s="77" t="s">
         <v>113</v>
       </c>
-      <c r="L7" s="77" t="s">
-        <v>114</v>
-      </c>
-      <c r="M7" s="76" t="s">
-        <v>53</v>
-      </c>
-      <c r="N7" s="77" t="s">
-        <v>117</v>
-      </c>
-      <c r="O7" s="77" t="s">
-        <v>118</v>
-      </c>
-      <c r="P7" s="77" t="s">
-        <v>112</v>
-      </c>
-      <c r="Q7" s="77" t="s">
-        <v>113</v>
-      </c>
-      <c r="R7" s="77" t="s">
-        <v>114</v>
-      </c>
       <c r="S7" s="75" t="s">
+        <v>138</v>
+      </c>
+      <c r="T7" s="77" t="s">
+        <v>121</v>
+      </c>
+      <c r="U7" s="77" t="s">
+        <v>122</v>
+      </c>
+      <c r="V7" s="76" t="s">
+        <v>69</v>
+      </c>
+      <c r="W7" s="76" t="s">
+        <v>31</v>
+      </c>
+      <c r="X7" s="75" t="s">
         <v>139</v>
       </c>
-      <c r="T7" s="77" t="s">
-        <v>122</v>
-      </c>
-      <c r="U7" s="77" t="s">
-        <v>123</v>
-      </c>
-      <c r="V7" s="76" t="s">
-        <v>70</v>
-      </c>
-      <c r="W7" s="76" t="s">
-        <v>32</v>
-      </c>
-      <c r="X7" s="75" t="s">
-        <v>140</v>
-      </c>
       <c r="Y7" s="75" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="8" spans="2:25" x14ac:dyDescent="0.25">
@@ -5892,6 +5892,7 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="P6:R6"/>
     <mergeCell ref="B6:E6"/>
     <mergeCell ref="T6:U6"/>
     <mergeCell ref="M5:Y5"/>
@@ -5902,7 +5903,6 @@
     <mergeCell ref="J6:L6"/>
     <mergeCell ref="F6:I6"/>
     <mergeCell ref="N6:O6"/>
-    <mergeCell ref="P6:R6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -6017,7 +6017,7 @@
   <sheetData>
     <row r="1" spans="2:5" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -6028,7 +6028,7 @@
     </row>
     <row r="3" spans="2:5" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="98" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C3" s="98"/>
       <c r="D3" s="98"/>
@@ -6039,16 +6039,16 @@
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="70" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C5" s="44" t="s">
+        <v>129</v>
+      </c>
+      <c r="D5" s="96" t="s">
         <v>130</v>
       </c>
-      <c r="D5" s="96" t="s">
+      <c r="E5" s="96" t="s">
         <v>131</v>
-      </c>
-      <c r="E5" s="96" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="6" spans="2:5" customFormat="1" x14ac:dyDescent="0.25">
@@ -6089,7 +6089,7 @@
   <sheetData>
     <row r="1" spans="2:16" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -6130,31 +6130,31 @@
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="44" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="D5" s="44" t="s">
         <v>79</v>
       </c>
-      <c r="D5" s="44" t="s">
+      <c r="E5" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="F5" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>82</v>
-      </c>
       <c r="G5" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I5" s="45" t="s">
         <v>15</v>
       </c>
       <c r="J5" s="45" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
@@ -6201,7 +6201,7 @@
   <sheetData>
     <row r="1" spans="2:16" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -6223,7 +6223,7 @@
     </row>
     <row r="3" spans="2:16" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="98" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C3" s="98"/>
       <c r="D3" s="98"/>
@@ -6242,10 +6242,10 @@
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
@@ -6283,7 +6283,7 @@
   <sheetData>
     <row r="1" spans="2:16" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -6305,7 +6305,7 @@
     </row>
     <row r="3" spans="2:16" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="98" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C3" s="98"/>
       <c r="D3" s="98"/>
@@ -6324,10 +6324,10 @@
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
@@ -6348,8 +6348,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:P6"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6359,7 +6359,7 @@
     <col min="3" max="3" width="58.28515625" customWidth="1"/>
     <col min="4" max="4" width="17.7109375" customWidth="1"/>
     <col min="5" max="5" width="17" customWidth="1"/>
-    <col min="6" max="6" width="16.7109375" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" customWidth="1"/>
     <col min="7" max="7" width="19.5703125" customWidth="1"/>
     <col min="8" max="8" width="24.7109375" customWidth="1"/>
     <col min="9" max="9" width="25.7109375" customWidth="1"/>
@@ -6371,7 +6371,7 @@
   <sheetData>
     <row r="1" spans="2:16" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -6393,7 +6393,7 @@
     </row>
     <row r="3" spans="2:16" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="98" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C3" s="98"/>
       <c r="D3" s="98"/>
@@ -6412,10 +6412,10 @@
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="44" t="s">
+        <v>84</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>85</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>86</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>16</v>
@@ -6424,31 +6424,31 @@
         <v>17</v>
       </c>
       <c r="F5" s="45" t="s">
-        <v>18</v>
+        <v>197</v>
       </c>
       <c r="G5" s="45" t="s">
         <v>8</v>
       </c>
       <c r="H5" s="45" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I5" s="45" t="s">
+        <v>20</v>
+      </c>
+      <c r="J5" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="J5" s="45" t="s">
-        <v>22</v>
-      </c>
       <c r="K5" s="90" t="s">
+        <v>190</v>
+      </c>
+      <c r="L5" s="90" t="s">
         <v>191</v>
       </c>
-      <c r="L5" s="90" t="s">
-        <v>192</v>
-      </c>
       <c r="M5" s="45" t="s">
+        <v>132</v>
+      </c>
+      <c r="N5" s="45" t="s">
         <v>133</v>
-      </c>
-      <c r="N5" s="45" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
@@ -6501,7 +6501,7 @@
   <sheetData>
     <row r="1" spans="2:16" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -6523,7 +6523,7 @@
     </row>
     <row r="3" spans="2:16" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="98" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C3" s="98"/>
       <c r="D3" s="98"/>
@@ -6542,13 +6542,13 @@
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="45" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" s="45" t="s">
         <v>66</v>
       </c>
-      <c r="C5" s="45" t="s">
-        <v>67</v>
-      </c>
       <c r="D5" s="90" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
TRIEDA-1713 - Criando funcionalidade de geracao de demanda (telas e informações no banco necessárias). Alterando disciplinaComboBox para disciplinaAutoCompleteBox e criando disciplinaComboBox padrão.
</commit_message>
<xml_diff>
--- a/code/client/web/src/main/resources/templateExport.xlsx
+++ b/code/client/web/src/main/resources/templateExport.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="17070" windowHeight="5370" tabRatio="954" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="17070" windowHeight="5370" tabRatio="986" firstSheet="2" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="Campi" sheetId="3" r:id="rId1"/>
@@ -18,27 +18,30 @@
     <sheet name="Equivalencias" sheetId="17" r:id="rId9"/>
     <sheet name="Disciplinas-Salas" sheetId="9" r:id="rId10"/>
     <sheet name="Curriculos" sheetId="7" r:id="rId11"/>
-    <sheet name="Ofertas e Demandas" sheetId="8" r:id="rId12"/>
-    <sheet name="Alunos" sheetId="27" r:id="rId13"/>
-    <sheet name="Demanda por Aluno" sheetId="22" r:id="rId14"/>
-    <sheet name="Professores" sheetId="12" r:id="rId15"/>
-    <sheet name="Disponibilidades Professores" sheetId="28" r:id="rId16"/>
-    <sheet name="Campi de Trabalho" sheetId="18" r:id="rId17"/>
-    <sheet name="Habilitacao dos Professores" sheetId="13" r:id="rId18"/>
-    <sheet name="Resumo por curso" sheetId="14" r:id="rId19"/>
-    <sheet name="Resumo por disciplina" sheetId="15" r:id="rId20"/>
-    <sheet name="Atendimentos por Matricula" sheetId="30" r:id="rId21"/>
-    <sheet name="Atendimentos por Disciplina" sheetId="31" r:id="rId22"/>
-    <sheet name="Atendimentos Faixa de Demanda" sheetId="32" r:id="rId23"/>
-    <sheet name="Atendimentos por Carga Horaria" sheetId="35" r:id="rId24"/>
-    <sheet name="Porcentagem Mestres e Doutores" sheetId="33" r:id="rId25"/>
-    <sheet name="Relatorio Visao Sala" sheetId="10" r:id="rId26"/>
-    <sheet name="Relatorio Visao Aluno" sheetId="25" r:id="rId27"/>
-    <sheet name="Relatorio Visao Professor" sheetId="21" r:id="rId28"/>
-    <sheet name="Relatorio Visao Curso" sheetId="20" r:id="rId29"/>
-    <sheet name="Atendimentos por Aluno" sheetId="23" r:id="rId30"/>
-    <sheet name="Aulas" sheetId="26" r:id="rId31"/>
-    <sheet name="PaletaCores" sheetId="11" r:id="rId32"/>
+    <sheet name="Disciplinas Pre-Requisitos" sheetId="37" r:id="rId12"/>
+    <sheet name="Disciplinas Co-Requisitos" sheetId="38" r:id="rId13"/>
+    <sheet name="Disciplinas Cursadas por Aluno" sheetId="39" r:id="rId14"/>
+    <sheet name="Ofertas e Demandas" sheetId="8" r:id="rId15"/>
+    <sheet name="Alunos" sheetId="27" r:id="rId16"/>
+    <sheet name="Demanda por Aluno" sheetId="22" r:id="rId17"/>
+    <sheet name="Professores" sheetId="12" r:id="rId18"/>
+    <sheet name="Disponibilidades Professores" sheetId="28" r:id="rId19"/>
+    <sheet name="Campi de Trabalho" sheetId="18" r:id="rId20"/>
+    <sheet name="Habilitacao dos Professores" sheetId="13" r:id="rId21"/>
+    <sheet name="Resumo por curso" sheetId="14" r:id="rId22"/>
+    <sheet name="Resumo por disciplina" sheetId="15" r:id="rId23"/>
+    <sheet name="Atendimentos por Matricula" sheetId="30" r:id="rId24"/>
+    <sheet name="Atendimentos por Disciplina" sheetId="31" r:id="rId25"/>
+    <sheet name="Atendimentos Faixa de Demanda" sheetId="32" r:id="rId26"/>
+    <sheet name="Atendimentos por Carga Horaria" sheetId="35" r:id="rId27"/>
+    <sheet name="Porcentagem Mestres e Doutores" sheetId="33" r:id="rId28"/>
+    <sheet name="Relatorio Visao Sala" sheetId="10" r:id="rId29"/>
+    <sheet name="Relatorio Visao Aluno" sheetId="25" r:id="rId30"/>
+    <sheet name="Relatorio Visao Professor" sheetId="21" r:id="rId31"/>
+    <sheet name="Relatorio Visao Curso" sheetId="20" r:id="rId32"/>
+    <sheet name="Atendimentos por Aluno" sheetId="23" r:id="rId33"/>
+    <sheet name="Aulas" sheetId="26" r:id="rId34"/>
+    <sheet name="PaletaCores" sheetId="11" r:id="rId35"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
@@ -1303,7 +1306,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="203">
   <si>
     <t>Planilha de Unidades</t>
   </si>
@@ -1897,6 +1900,21 @@
   </si>
   <si>
     <t>Exige Laboratório?</t>
+  </si>
+  <si>
+    <t>Planilha de Disciplinas Pre-Requisitos</t>
+  </si>
+  <si>
+    <t>Código Disciplina Pré-Requisito</t>
+  </si>
+  <si>
+    <t>Código Disciplina Co-Requisito</t>
+  </si>
+  <si>
+    <t>Planilha de Disciplinas Co-Requisitos</t>
+  </si>
+  <si>
+    <t>Planilha de Disciplinas Cursadas por Aluno</t>
   </si>
 </sst>
 </file>
@@ -1969,16 +1987,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2326,16 +2344,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="120">
+  <cellXfs count="122">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -2353,16 +2371,16 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2444,10 +2462,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2463,22 +2481,22 @@
     <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="27" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -2489,25 +2507,25 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2520,10 +2538,10 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2535,25 +2553,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="8" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2564,16 +2582,16 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="28" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2591,13 +2609,19 @@
     <xf numFmtId="178" fontId="8" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2609,13 +2633,13 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2630,24 +2654,36 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="28" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="28" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2656,18 +2692,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2996,38 +3020,38 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="97" t="s">
+      <c r="B2" s="99" t="s">
         <v>93</v>
       </c>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="97"/>
-      <c r="J2" s="97"/>
-      <c r="K2" s="97"/>
-      <c r="L2" s="97"/>
-      <c r="M2" s="97"/>
-      <c r="N2" s="97"/>
+      <c r="C2" s="99"/>
+      <c r="D2" s="99"/>
+      <c r="E2" s="99"/>
+      <c r="F2" s="99"/>
+      <c r="G2" s="99"/>
+      <c r="H2" s="99"/>
+      <c r="I2" s="99"/>
+      <c r="J2" s="99"/>
+      <c r="K2" s="99"/>
+      <c r="L2" s="99"/>
+      <c r="M2" s="99"/>
+      <c r="N2" s="99"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="98" t="s">
+      <c r="B3" s="100" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="98"/>
-      <c r="F3" s="98"/>
-      <c r="G3" s="98"/>
-      <c r="H3" s="98"/>
-      <c r="I3" s="98"/>
-      <c r="J3" s="98"/>
-      <c r="K3" s="98"/>
-      <c r="L3" s="98"/>
-      <c r="M3" s="98"/>
-      <c r="N3" s="98"/>
+      <c r="C3" s="100"/>
+      <c r="D3" s="100"/>
+      <c r="E3" s="100"/>
+      <c r="F3" s="100"/>
+      <c r="G3" s="100"/>
+      <c r="H3" s="100"/>
+      <c r="I3" s="100"/>
+      <c r="J3" s="100"/>
+      <c r="K3" s="100"/>
+      <c r="L3" s="100"/>
+      <c r="M3" s="100"/>
+      <c r="N3" s="100"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="44" t="s">
@@ -3094,28 +3118,28 @@
       </c>
     </row>
     <row r="2" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="99"/>
-      <c r="C2" s="99"/>
-      <c r="D2" s="99"/>
-      <c r="E2" s="99"/>
-      <c r="F2" s="99"/>
-      <c r="G2" s="99"/>
-      <c r="H2" s="99"/>
-      <c r="I2" s="99"/>
+      <c r="B2" s="101"/>
+      <c r="C2" s="101"/>
+      <c r="D2" s="101"/>
+      <c r="E2" s="101"/>
+      <c r="F2" s="101"/>
+      <c r="G2" s="101"/>
+      <c r="H2" s="101"/>
+      <c r="I2" s="101"/>
       <c r="J2" s="83"/>
       <c r="K2" s="83"/>
     </row>
     <row r="3" spans="2:11" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="98" t="s">
+      <c r="B3" s="100" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="98"/>
-      <c r="F3" s="98"/>
-      <c r="G3" s="98"/>
-      <c r="H3" s="98"/>
-      <c r="I3" s="98"/>
+      <c r="C3" s="100"/>
+      <c r="D3" s="100"/>
+      <c r="E3" s="100"/>
+      <c r="F3" s="100"/>
+      <c r="G3" s="100"/>
+      <c r="H3" s="100"/>
+      <c r="I3" s="100"/>
       <c r="J3" s="82"/>
       <c r="K3" s="82"/>
     </row>
@@ -3145,7 +3169,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:N6"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3168,36 +3194,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="97"/>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="97"/>
-      <c r="J2" s="97"/>
-      <c r="K2" s="97"/>
-      <c r="L2" s="97"/>
-      <c r="M2" s="97"/>
-      <c r="N2" s="97"/>
+      <c r="B2" s="99"/>
+      <c r="C2" s="99"/>
+      <c r="D2" s="99"/>
+      <c r="E2" s="99"/>
+      <c r="F2" s="99"/>
+      <c r="G2" s="99"/>
+      <c r="H2" s="99"/>
+      <c r="I2" s="99"/>
+      <c r="J2" s="99"/>
+      <c r="K2" s="99"/>
+      <c r="L2" s="99"/>
+      <c r="M2" s="99"/>
+      <c r="N2" s="99"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="98" t="s">
+      <c r="B3" s="100" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="98"/>
-      <c r="F3" s="98"/>
-      <c r="G3" s="98"/>
-      <c r="H3" s="98"/>
-      <c r="I3" s="98"/>
-      <c r="J3" s="98"/>
-      <c r="K3" s="98"/>
-      <c r="L3" s="98"/>
-      <c r="M3" s="98"/>
-      <c r="N3" s="98"/>
+      <c r="C3" s="100"/>
+      <c r="D3" s="100"/>
+      <c r="E3" s="100"/>
+      <c r="F3" s="100"/>
+      <c r="G3" s="100"/>
+      <c r="H3" s="100"/>
+      <c r="I3" s="100"/>
+      <c r="J3" s="100"/>
+      <c r="K3" s="100"/>
+      <c r="L3" s="100"/>
+      <c r="M3" s="100"/>
+      <c r="N3" s="100"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -3238,6 +3264,262 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:L6"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.85546875" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" customWidth="1"/>
+    <col min="3" max="3" width="21.28515625" customWidth="1"/>
+    <col min="4" max="4" width="24.28515625" customWidth="1"/>
+    <col min="5" max="5" width="32.28515625" customWidth="1"/>
+    <col min="6" max="6" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:12" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B1" s="46" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="99"/>
+      <c r="C2" s="99"/>
+      <c r="D2" s="99"/>
+      <c r="E2" s="99"/>
+      <c r="F2" s="99"/>
+      <c r="G2" s="99"/>
+      <c r="H2" s="99"/>
+      <c r="I2" s="99"/>
+      <c r="J2" s="99"/>
+      <c r="K2" s="99"/>
+      <c r="L2" s="99"/>
+    </row>
+    <row r="3" spans="2:12" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B3" s="100" t="s">
+        <v>198</v>
+      </c>
+      <c r="C3" s="100"/>
+      <c r="D3" s="100"/>
+      <c r="E3" s="100"/>
+      <c r="F3" s="100"/>
+      <c r="G3" s="100"/>
+      <c r="H3" s="100"/>
+      <c r="I3" s="100"/>
+      <c r="J3" s="100"/>
+      <c r="K3" s="100"/>
+      <c r="L3" s="100"/>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B5" s="70" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="70" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="97" t="s">
+        <v>84</v>
+      </c>
+      <c r="E5" s="97" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B6" s="89"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:L2"/>
+    <mergeCell ref="B3:L3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:L6"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:L3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.85546875" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" customWidth="1"/>
+    <col min="3" max="3" width="21.28515625" customWidth="1"/>
+    <col min="4" max="4" width="24.28515625" customWidth="1"/>
+    <col min="5" max="5" width="32.28515625" customWidth="1"/>
+    <col min="6" max="6" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:12" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B1" s="46" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="99"/>
+      <c r="C2" s="99"/>
+      <c r="D2" s="99"/>
+      <c r="E2" s="99"/>
+      <c r="F2" s="99"/>
+      <c r="G2" s="99"/>
+      <c r="H2" s="99"/>
+      <c r="I2" s="99"/>
+      <c r="J2" s="99"/>
+      <c r="K2" s="99"/>
+      <c r="L2" s="99"/>
+    </row>
+    <row r="3" spans="2:12" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B3" s="100" t="s">
+        <v>201</v>
+      </c>
+      <c r="C3" s="100"/>
+      <c r="D3" s="100"/>
+      <c r="E3" s="100"/>
+      <c r="F3" s="100"/>
+      <c r="G3" s="100"/>
+      <c r="H3" s="100"/>
+      <c r="I3" s="100"/>
+      <c r="J3" s="100"/>
+      <c r="K3" s="100"/>
+      <c r="L3" s="100"/>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B5" s="70" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="70" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="97" t="s">
+        <v>84</v>
+      </c>
+      <c r="E5" s="97" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B6" s="89"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:L2"/>
+    <mergeCell ref="B3:L3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:L6"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.85546875" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" customWidth="1"/>
+    <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" customWidth="1"/>
+    <col min="6" max="6" width="21.85546875" customWidth="1"/>
+    <col min="7" max="7" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:12" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B1" s="46" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="99"/>
+      <c r="C2" s="99"/>
+      <c r="D2" s="99"/>
+      <c r="E2" s="99"/>
+      <c r="F2" s="99"/>
+      <c r="G2" s="99"/>
+      <c r="H2" s="99"/>
+      <c r="I2" s="99"/>
+      <c r="J2" s="99"/>
+      <c r="K2" s="99"/>
+      <c r="L2" s="99"/>
+    </row>
+    <row r="3" spans="2:12" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B3" s="100" t="s">
+        <v>202</v>
+      </c>
+      <c r="C3" s="100"/>
+      <c r="D3" s="100"/>
+      <c r="E3" s="100"/>
+      <c r="F3" s="100"/>
+      <c r="G3" s="100"/>
+      <c r="H3" s="100"/>
+      <c r="I3" s="100"/>
+      <c r="J3" s="100"/>
+      <c r="K3" s="100"/>
+      <c r="L3" s="100"/>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B5" s="70" t="s">
+        <v>98</v>
+      </c>
+      <c r="C5" s="70" t="s">
+        <v>77</v>
+      </c>
+      <c r="D5" s="70" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="98" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="98" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B6" s="89"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="8"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:L2"/>
+    <mergeCell ref="B3:L3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:N6"/>
   <sheetViews>
@@ -3266,36 +3548,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="97"/>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="97"/>
-      <c r="J2" s="97"/>
-      <c r="K2" s="97"/>
-      <c r="L2" s="97"/>
-      <c r="M2" s="97"/>
-      <c r="N2" s="97"/>
+      <c r="B2" s="99"/>
+      <c r="C2" s="99"/>
+      <c r="D2" s="99"/>
+      <c r="E2" s="99"/>
+      <c r="F2" s="99"/>
+      <c r="G2" s="99"/>
+      <c r="H2" s="99"/>
+      <c r="I2" s="99"/>
+      <c r="J2" s="99"/>
+      <c r="K2" s="99"/>
+      <c r="L2" s="99"/>
+      <c r="M2" s="99"/>
+      <c r="N2" s="99"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="98" t="s">
+      <c r="B3" s="100" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="98"/>
-      <c r="F3" s="98"/>
-      <c r="G3" s="98"/>
-      <c r="H3" s="98"/>
-      <c r="I3" s="98"/>
-      <c r="J3" s="98"/>
-      <c r="K3" s="98"/>
-      <c r="L3" s="98"/>
-      <c r="M3" s="98"/>
-      <c r="N3" s="98"/>
+      <c r="C3" s="100"/>
+      <c r="D3" s="100"/>
+      <c r="E3" s="100"/>
+      <c r="F3" s="100"/>
+      <c r="G3" s="100"/>
+      <c r="H3" s="100"/>
+      <c r="I3" s="100"/>
+      <c r="J3" s="100"/>
+      <c r="K3" s="100"/>
+      <c r="L3" s="100"/>
+      <c r="M3" s="100"/>
+      <c r="N3" s="100"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -3360,7 +3642,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E6"/>
   <sheetViews>
@@ -3380,18 +3662,18 @@
       </c>
     </row>
     <row r="2" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="97"/>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
+      <c r="B2" s="99"/>
+      <c r="C2" s="99"/>
+      <c r="D2" s="99"/>
+      <c r="E2" s="99"/>
     </row>
     <row r="3" spans="2:5" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="98" t="s">
+      <c r="B3" s="100" t="s">
         <v>123</v>
       </c>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="98"/>
+      <c r="C3" s="100"/>
+      <c r="D3" s="100"/>
+      <c r="E3" s="100"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="60" t="s">
@@ -3418,7 +3700,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:N6"/>
   <sheetViews>
@@ -3444,36 +3726,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="97"/>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="97"/>
-      <c r="J2" s="97"/>
-      <c r="K2" s="97"/>
-      <c r="L2" s="97"/>
-      <c r="M2" s="97"/>
-      <c r="N2" s="97"/>
+      <c r="B2" s="99"/>
+      <c r="C2" s="99"/>
+      <c r="D2" s="99"/>
+      <c r="E2" s="99"/>
+      <c r="F2" s="99"/>
+      <c r="G2" s="99"/>
+      <c r="H2" s="99"/>
+      <c r="I2" s="99"/>
+      <c r="J2" s="99"/>
+      <c r="K2" s="99"/>
+      <c r="L2" s="99"/>
+      <c r="M2" s="99"/>
+      <c r="N2" s="99"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="98" t="s">
+      <c r="B3" s="100" t="s">
         <v>97</v>
       </c>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="98"/>
-      <c r="F3" s="98"/>
-      <c r="G3" s="98"/>
-      <c r="H3" s="98"/>
-      <c r="I3" s="98"/>
-      <c r="J3" s="98"/>
-      <c r="K3" s="98"/>
-      <c r="L3" s="98"/>
-      <c r="M3" s="98"/>
-      <c r="N3" s="98"/>
+      <c r="C3" s="100"/>
+      <c r="D3" s="100"/>
+      <c r="E3" s="100"/>
+      <c r="F3" s="100"/>
+      <c r="G3" s="100"/>
+      <c r="H3" s="100"/>
+      <c r="I3" s="100"/>
+      <c r="J3" s="100"/>
+      <c r="K3" s="100"/>
+      <c r="L3" s="100"/>
+      <c r="M3" s="100"/>
+      <c r="N3" s="100"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -3506,10 +3788,10 @@
       <c r="K5" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="L5" s="100" t="s">
+      <c r="L5" s="102" t="s">
         <v>107</v>
       </c>
-      <c r="M5" s="100"/>
+      <c r="M5" s="102"/>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
@@ -3533,7 +3815,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O6"/>
   <sheetViews>
@@ -3564,38 +3846,38 @@
       </c>
     </row>
     <row r="2" spans="2:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="97"/>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="97"/>
-      <c r="J2" s="97"/>
-      <c r="K2" s="97"/>
-      <c r="L2" s="97"/>
-      <c r="M2" s="97"/>
-      <c r="N2" s="97"/>
-      <c r="O2" s="97"/>
+      <c r="B2" s="99"/>
+      <c r="C2" s="99"/>
+      <c r="D2" s="99"/>
+      <c r="E2" s="99"/>
+      <c r="F2" s="99"/>
+      <c r="G2" s="99"/>
+      <c r="H2" s="99"/>
+      <c r="I2" s="99"/>
+      <c r="J2" s="99"/>
+      <c r="K2" s="99"/>
+      <c r="L2" s="99"/>
+      <c r="M2" s="99"/>
+      <c r="N2" s="99"/>
+      <c r="O2" s="99"/>
     </row>
     <row r="3" spans="2:15" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="98" t="s">
+      <c r="B3" s="100" t="s">
         <v>72</v>
       </c>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="98"/>
-      <c r="F3" s="98"/>
-      <c r="G3" s="98"/>
-      <c r="H3" s="98"/>
-      <c r="I3" s="98"/>
-      <c r="J3" s="98"/>
-      <c r="K3" s="98"/>
-      <c r="L3" s="98"/>
-      <c r="M3" s="98"/>
-      <c r="N3" s="98"/>
-      <c r="O3" s="98"/>
+      <c r="C3" s="100"/>
+      <c r="D3" s="100"/>
+      <c r="E3" s="100"/>
+      <c r="F3" s="100"/>
+      <c r="G3" s="100"/>
+      <c r="H3" s="100"/>
+      <c r="I3" s="100"/>
+      <c r="J3" s="100"/>
+      <c r="K3" s="100"/>
+      <c r="L3" s="100"/>
+      <c r="M3" s="100"/>
+      <c r="N3" s="100"/>
+      <c r="O3" s="100"/>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -3660,7 +3942,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
@@ -3682,18 +3964,18 @@
       </c>
     </row>
     <row r="2" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="97"/>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
+      <c r="B2" s="99"/>
+      <c r="C2" s="99"/>
+      <c r="D2" s="99"/>
+      <c r="E2" s="99"/>
     </row>
     <row r="3" spans="2:5" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="98" t="s">
+      <c r="B3" s="100" t="s">
         <v>128</v>
       </c>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="98"/>
+      <c r="C3" s="100"/>
+      <c r="D3" s="100"/>
+      <c r="E3" s="100"/>
     </row>
     <row r="4" spans="2:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="64"/>
@@ -3728,7 +4010,94 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:N6"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.85546875" customWidth="1"/>
+    <col min="2" max="2" width="27" customWidth="1"/>
+    <col min="3" max="3" width="29.7109375" customWidth="1"/>
+    <col min="4" max="4" width="42.7109375" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:14" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B1" s="46" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="99" t="s">
+        <v>94</v>
+      </c>
+      <c r="C2" s="99"/>
+      <c r="D2" s="99"/>
+      <c r="E2" s="99"/>
+      <c r="F2" s="99"/>
+      <c r="G2" s="99"/>
+      <c r="H2" s="99"/>
+      <c r="I2" s="99"/>
+      <c r="J2" s="99"/>
+      <c r="K2" s="99"/>
+      <c r="L2" s="99"/>
+      <c r="M2" s="99"/>
+      <c r="N2" s="99"/>
+    </row>
+    <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B3" s="100" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="100"/>
+      <c r="D3" s="100"/>
+      <c r="E3" s="100"/>
+      <c r="F3" s="100"/>
+      <c r="G3" s="100"/>
+      <c r="H3" s="100"/>
+      <c r="I3" s="100"/>
+      <c r="J3" s="100"/>
+      <c r="K3" s="100"/>
+      <c r="L3" s="100"/>
+      <c r="M3" s="100"/>
+      <c r="N3" s="100"/>
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B5" s="44" t="s">
+        <v>75</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:N2"/>
+    <mergeCell ref="B3:N3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:N6"/>
   <sheetViews>
@@ -3755,36 +4124,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="97"/>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="97"/>
-      <c r="J2" s="97"/>
-      <c r="K2" s="97"/>
-      <c r="L2" s="97"/>
-      <c r="M2" s="97"/>
-      <c r="N2" s="97"/>
+      <c r="B2" s="99"/>
+      <c r="C2" s="99"/>
+      <c r="D2" s="99"/>
+      <c r="E2" s="99"/>
+      <c r="F2" s="99"/>
+      <c r="G2" s="99"/>
+      <c r="H2" s="99"/>
+      <c r="I2" s="99"/>
+      <c r="J2" s="99"/>
+      <c r="K2" s="99"/>
+      <c r="L2" s="99"/>
+      <c r="M2" s="99"/>
+      <c r="N2" s="99"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="98" t="s">
+      <c r="B3" s="100" t="s">
         <v>68</v>
       </c>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="98"/>
-      <c r="F3" s="98"/>
-      <c r="G3" s="98"/>
-      <c r="H3" s="98"/>
-      <c r="I3" s="98"/>
-      <c r="J3" s="98"/>
-      <c r="K3" s="98"/>
-      <c r="L3" s="98"/>
-      <c r="M3" s="98"/>
-      <c r="N3" s="98"/>
+      <c r="C3" s="100"/>
+      <c r="D3" s="100"/>
+      <c r="E3" s="100"/>
+      <c r="F3" s="100"/>
+      <c r="G3" s="100"/>
+      <c r="H3" s="100"/>
+      <c r="I3" s="100"/>
+      <c r="J3" s="100"/>
+      <c r="K3" s="100"/>
+      <c r="L3" s="100"/>
+      <c r="M3" s="100"/>
+      <c r="N3" s="100"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -3812,7 +4181,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:N6"/>
   <sheetViews>
@@ -3839,36 +4208,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="97"/>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="97"/>
-      <c r="J2" s="97"/>
-      <c r="K2" s="97"/>
-      <c r="L2" s="97"/>
-      <c r="M2" s="97"/>
-      <c r="N2" s="97"/>
+      <c r="B2" s="99"/>
+      <c r="C2" s="99"/>
+      <c r="D2" s="99"/>
+      <c r="E2" s="99"/>
+      <c r="F2" s="99"/>
+      <c r="G2" s="99"/>
+      <c r="H2" s="99"/>
+      <c r="I2" s="99"/>
+      <c r="J2" s="99"/>
+      <c r="K2" s="99"/>
+      <c r="L2" s="99"/>
+      <c r="M2" s="99"/>
+      <c r="N2" s="99"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="98" t="s">
+      <c r="B3" s="100" t="s">
         <v>73</v>
       </c>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="98"/>
-      <c r="F3" s="98"/>
-      <c r="G3" s="98"/>
-      <c r="H3" s="98"/>
-      <c r="I3" s="98"/>
-      <c r="J3" s="98"/>
-      <c r="K3" s="98"/>
-      <c r="L3" s="98"/>
-      <c r="M3" s="98"/>
-      <c r="N3" s="98"/>
+      <c r="C3" s="100"/>
+      <c r="D3" s="100"/>
+      <c r="E3" s="100"/>
+      <c r="F3" s="100"/>
+      <c r="G3" s="100"/>
+      <c r="H3" s="100"/>
+      <c r="I3" s="100"/>
+      <c r="J3" s="100"/>
+      <c r="K3" s="100"/>
+      <c r="L3" s="100"/>
+      <c r="M3" s="100"/>
+      <c r="N3" s="100"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -3901,7 +4270,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:R6"/>
   <sheetViews>
@@ -3937,40 +4306,40 @@
       </c>
     </row>
     <row r="2" spans="2:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="97"/>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="97"/>
-      <c r="J2" s="97"/>
-      <c r="K2" s="97"/>
-      <c r="L2" s="97"/>
-      <c r="M2" s="97"/>
-      <c r="N2" s="97"/>
-      <c r="O2" s="97"/>
-      <c r="P2" s="97"/>
+      <c r="B2" s="99"/>
+      <c r="C2" s="99"/>
+      <c r="D2" s="99"/>
+      <c r="E2" s="99"/>
+      <c r="F2" s="99"/>
+      <c r="G2" s="99"/>
+      <c r="H2" s="99"/>
+      <c r="I2" s="99"/>
+      <c r="J2" s="99"/>
+      <c r="K2" s="99"/>
+      <c r="L2" s="99"/>
+      <c r="M2" s="99"/>
+      <c r="N2" s="99"/>
+      <c r="O2" s="99"/>
+      <c r="P2" s="99"/>
     </row>
     <row r="3" spans="2:18" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="98" t="s">
+      <c r="B3" s="100" t="s">
         <v>62</v>
       </c>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="98"/>
-      <c r="F3" s="98"/>
-      <c r="G3" s="98"/>
-      <c r="H3" s="98"/>
-      <c r="I3" s="98"/>
-      <c r="J3" s="98"/>
-      <c r="K3" s="98"/>
-      <c r="L3" s="98"/>
-      <c r="M3" s="98"/>
-      <c r="N3" s="98"/>
-      <c r="O3" s="98"/>
-      <c r="P3" s="98"/>
+      <c r="C3" s="100"/>
+      <c r="D3" s="100"/>
+      <c r="E3" s="100"/>
+      <c r="F3" s="100"/>
+      <c r="G3" s="100"/>
+      <c r="H3" s="100"/>
+      <c r="I3" s="100"/>
+      <c r="J3" s="100"/>
+      <c r="K3" s="100"/>
+      <c r="L3" s="100"/>
+      <c r="M3" s="100"/>
+      <c r="N3" s="100"/>
+      <c r="O3" s="100"/>
+      <c r="P3" s="100"/>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
@@ -4054,94 +4423,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:N6"/>
-  <sheetViews>
-    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="2.85546875" customWidth="1"/>
-    <col min="2" max="2" width="27" customWidth="1"/>
-    <col min="3" max="3" width="29.7109375" customWidth="1"/>
-    <col min="4" max="4" width="42.7109375" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:14" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="46" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="97" t="s">
-        <v>94</v>
-      </c>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="97"/>
-      <c r="J2" s="97"/>
-      <c r="K2" s="97"/>
-      <c r="L2" s="97"/>
-      <c r="M2" s="97"/>
-      <c r="N2" s="97"/>
-    </row>
-    <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="98" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="98"/>
-      <c r="F3" s="98"/>
-      <c r="G3" s="98"/>
-      <c r="H3" s="98"/>
-      <c r="I3" s="98"/>
-      <c r="J3" s="98"/>
-      <c r="K3" s="98"/>
-      <c r="L3" s="98"/>
-      <c r="M3" s="98"/>
-      <c r="N3" s="98"/>
-    </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B5" s="44" t="s">
-        <v>75</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B2:N2"/>
-    <mergeCell ref="B3:N3"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:N6"/>
   <sheetViews>
@@ -4171,36 +4453,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="97"/>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="97"/>
-      <c r="J2" s="97"/>
-      <c r="K2" s="97"/>
-      <c r="L2" s="97"/>
-      <c r="M2" s="97"/>
-      <c r="N2" s="97"/>
+      <c r="B2" s="99"/>
+      <c r="C2" s="99"/>
+      <c r="D2" s="99"/>
+      <c r="E2" s="99"/>
+      <c r="F2" s="99"/>
+      <c r="G2" s="99"/>
+      <c r="H2" s="99"/>
+      <c r="I2" s="99"/>
+      <c r="J2" s="99"/>
+      <c r="K2" s="99"/>
+      <c r="L2" s="99"/>
+      <c r="M2" s="99"/>
+      <c r="N2" s="99"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="98" t="s">
+      <c r="B3" s="100" t="s">
         <v>63</v>
       </c>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="98"/>
-      <c r="F3" s="98"/>
-      <c r="G3" s="98"/>
-      <c r="H3" s="98"/>
-      <c r="I3" s="98"/>
-      <c r="J3" s="98"/>
-      <c r="K3" s="98"/>
-      <c r="L3" s="98"/>
-      <c r="M3" s="98"/>
-      <c r="N3" s="98"/>
+      <c r="C3" s="100"/>
+      <c r="D3" s="100"/>
+      <c r="E3" s="100"/>
+      <c r="F3" s="100"/>
+      <c r="G3" s="100"/>
+      <c r="H3" s="100"/>
+      <c r="I3" s="100"/>
+      <c r="J3" s="100"/>
+      <c r="K3" s="100"/>
+      <c r="L3" s="100"/>
+      <c r="M3" s="100"/>
+      <c r="N3" s="100"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="58" t="s">
@@ -4260,7 +4542,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:N6"/>
   <sheetViews>
@@ -4290,36 +4572,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="97"/>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="97"/>
-      <c r="J2" s="97"/>
-      <c r="K2" s="97"/>
-      <c r="L2" s="97"/>
-      <c r="M2" s="97"/>
-      <c r="N2" s="97"/>
+      <c r="B2" s="99"/>
+      <c r="C2" s="99"/>
+      <c r="D2" s="99"/>
+      <c r="E2" s="99"/>
+      <c r="F2" s="99"/>
+      <c r="G2" s="99"/>
+      <c r="H2" s="99"/>
+      <c r="I2" s="99"/>
+      <c r="J2" s="99"/>
+      <c r="K2" s="99"/>
+      <c r="L2" s="99"/>
+      <c r="M2" s="99"/>
+      <c r="N2" s="99"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="98" t="s">
+      <c r="B3" s="100" t="s">
         <v>149</v>
       </c>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="98"/>
-      <c r="F3" s="98"/>
-      <c r="G3" s="98"/>
-      <c r="H3" s="98"/>
-      <c r="I3" s="98"/>
-      <c r="J3" s="98"/>
-      <c r="K3" s="98"/>
-      <c r="L3" s="98"/>
-      <c r="M3" s="98"/>
-      <c r="N3" s="98"/>
+      <c r="C3" s="100"/>
+      <c r="D3" s="100"/>
+      <c r="E3" s="100"/>
+      <c r="F3" s="100"/>
+      <c r="G3" s="100"/>
+      <c r="H3" s="100"/>
+      <c r="I3" s="100"/>
+      <c r="J3" s="100"/>
+      <c r="K3" s="100"/>
+      <c r="L3" s="100"/>
+      <c r="M3" s="100"/>
+      <c r="N3" s="100"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="74" t="s">
@@ -4379,7 +4661,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J6"/>
   <sheetViews>
@@ -4406,28 +4688,28 @@
       </c>
     </row>
     <row r="2" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="97"/>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="97"/>
-      <c r="J2" s="97"/>
+      <c r="B2" s="99"/>
+      <c r="C2" s="99"/>
+      <c r="D2" s="99"/>
+      <c r="E2" s="99"/>
+      <c r="F2" s="99"/>
+      <c r="G2" s="99"/>
+      <c r="H2" s="99"/>
+      <c r="I2" s="99"/>
+      <c r="J2" s="99"/>
     </row>
     <row r="3" spans="2:10" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="98" t="s">
+      <c r="B3" s="100" t="s">
         <v>152</v>
       </c>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="98"/>
-      <c r="F3" s="98"/>
-      <c r="G3" s="98"/>
-      <c r="H3" s="98"/>
-      <c r="I3" s="98"/>
-      <c r="J3" s="98"/>
+      <c r="C3" s="100"/>
+      <c r="D3" s="100"/>
+      <c r="E3" s="100"/>
+      <c r="F3" s="100"/>
+      <c r="G3" s="100"/>
+      <c r="H3" s="100"/>
+      <c r="I3" s="100"/>
+      <c r="J3" s="100"/>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" s="74" t="s">
@@ -4475,7 +4757,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:T6"/>
   <sheetViews>
@@ -4512,29 +4794,29 @@
       </c>
     </row>
     <row r="2" spans="2:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="99"/>
-      <c r="C2" s="99"/>
-      <c r="D2" s="99"/>
-      <c r="E2" s="99"/>
-      <c r="F2" s="99"/>
-      <c r="G2" s="99"/>
-      <c r="H2" s="99"/>
-      <c r="I2" s="99"/>
+      <c r="B2" s="101"/>
+      <c r="C2" s="101"/>
+      <c r="D2" s="101"/>
+      <c r="E2" s="101"/>
+      <c r="F2" s="101"/>
+      <c r="G2" s="101"/>
+      <c r="H2" s="101"/>
+      <c r="I2" s="101"/>
       <c r="L2" s="83"/>
       <c r="M2" s="83"/>
       <c r="N2" s="83"/>
     </row>
     <row r="3" spans="2:20" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="98" t="s">
+      <c r="B3" s="100" t="s">
         <v>153</v>
       </c>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="98"/>
-      <c r="F3" s="98"/>
-      <c r="G3" s="98"/>
-      <c r="H3" s="98"/>
-      <c r="I3" s="98"/>
+      <c r="C3" s="100"/>
+      <c r="D3" s="100"/>
+      <c r="E3" s="100"/>
+      <c r="F3" s="100"/>
+      <c r="G3" s="100"/>
+      <c r="H3" s="100"/>
+      <c r="I3" s="100"/>
       <c r="L3" s="82"/>
       <c r="M3" s="82"/>
       <c r="N3" s="82"/>
@@ -4629,7 +4911,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:I6"/>
   <sheetViews>
@@ -4655,26 +4937,26 @@
       </c>
     </row>
     <row r="2" spans="2:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="97"/>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="97"/>
+      <c r="B2" s="99"/>
+      <c r="C2" s="99"/>
+      <c r="D2" s="99"/>
+      <c r="E2" s="99"/>
+      <c r="F2" s="99"/>
+      <c r="G2" s="99"/>
+      <c r="H2" s="99"/>
+      <c r="I2" s="99"/>
     </row>
     <row r="3" spans="2:9" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="98" t="s">
+      <c r="B3" s="100" t="s">
         <v>189</v>
       </c>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="98"/>
-      <c r="F3" s="98"/>
-      <c r="G3" s="98"/>
-      <c r="H3" s="98"/>
-      <c r="I3" s="98"/>
+      <c r="C3" s="100"/>
+      <c r="D3" s="100"/>
+      <c r="E3" s="100"/>
+      <c r="F3" s="100"/>
+      <c r="G3" s="100"/>
+      <c r="H3" s="100"/>
+      <c r="I3" s="100"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="88" t="s">
@@ -4722,7 +5004,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K7"/>
   <sheetViews>
@@ -4750,30 +5032,30 @@
       </c>
     </row>
     <row r="2" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="97"/>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="97"/>
-      <c r="J2" s="97"/>
-      <c r="K2" s="97"/>
+      <c r="B2" s="99"/>
+      <c r="C2" s="99"/>
+      <c r="D2" s="99"/>
+      <c r="E2" s="99"/>
+      <c r="F2" s="99"/>
+      <c r="G2" s="99"/>
+      <c r="H2" s="99"/>
+      <c r="I2" s="99"/>
+      <c r="J2" s="99"/>
+      <c r="K2" s="99"/>
     </row>
     <row r="3" spans="2:11" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="98" t="s">
+      <c r="B3" s="100" t="s">
         <v>165</v>
       </c>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="98"/>
-      <c r="F3" s="98"/>
-      <c r="G3" s="98"/>
-      <c r="H3" s="98"/>
-      <c r="I3" s="98"/>
-      <c r="J3" s="98"/>
-      <c r="K3" s="98"/>
+      <c r="C3" s="100"/>
+      <c r="D3" s="100"/>
+      <c r="E3" s="100"/>
+      <c r="F3" s="100"/>
+      <c r="G3" s="100"/>
+      <c r="H3" s="100"/>
+      <c r="I3" s="100"/>
+      <c r="J3" s="100"/>
+      <c r="K3" s="100"/>
     </row>
     <row r="4" spans="2:11" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B4" s="84"/>
@@ -4788,14 +5070,14 @@
       <c r="K4" s="84"/>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="H5" s="101" t="s">
+      <c r="H5" s="103" t="s">
         <v>173</v>
       </c>
-      <c r="I5" s="102"/>
-      <c r="J5" s="101" t="s">
+      <c r="I5" s="104"/>
+      <c r="J5" s="103" t="s">
         <v>172</v>
       </c>
-      <c r="K5" s="102"/>
+      <c r="K5" s="104"/>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" s="85" t="s">
@@ -4853,7 +5135,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:Z8"/>
   <sheetViews>
@@ -4877,37 +5159,37 @@
       <c r="Z1" s="38"/>
     </row>
     <row r="2" spans="2:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="97"/>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="97"/>
-      <c r="J2" s="97"/>
-      <c r="K2" s="97"/>
-      <c r="L2" s="97"/>
-      <c r="M2" s="97"/>
-      <c r="N2" s="97"/>
+      <c r="B2" s="99"/>
+      <c r="C2" s="99"/>
+      <c r="D2" s="99"/>
+      <c r="E2" s="99"/>
+      <c r="F2" s="99"/>
+      <c r="G2" s="99"/>
+      <c r="H2" s="99"/>
+      <c r="I2" s="99"/>
+      <c r="J2" s="99"/>
+      <c r="K2" s="99"/>
+      <c r="L2" s="99"/>
+      <c r="M2" s="99"/>
+      <c r="N2" s="99"/>
       <c r="Z2"/>
     </row>
     <row r="3" spans="2:26" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="98" t="s">
+      <c r="B3" s="100" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="98"/>
-      <c r="F3" s="98"/>
-      <c r="G3" s="98"/>
-      <c r="H3" s="98"/>
-      <c r="I3" s="98"/>
-      <c r="J3" s="98"/>
-      <c r="K3" s="98"/>
-      <c r="L3" s="98"/>
-      <c r="M3" s="98"/>
-      <c r="N3" s="98"/>
+      <c r="C3" s="100"/>
+      <c r="D3" s="100"/>
+      <c r="E3" s="100"/>
+      <c r="F3" s="100"/>
+      <c r="G3" s="100"/>
+      <c r="H3" s="100"/>
+      <c r="I3" s="100"/>
+      <c r="J3" s="100"/>
+      <c r="K3" s="100"/>
+      <c r="L3" s="100"/>
+      <c r="M3" s="100"/>
+      <c r="N3" s="100"/>
       <c r="Z3"/>
     </row>
     <row r="5" spans="2:26" x14ac:dyDescent="0.25">
@@ -4958,390 +5240,6 @@
         <v>38</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B8" s="2">
-        <v>1</v>
-      </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B2:N2"/>
-    <mergeCell ref="B3:N3"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:Z8"/>
-  <sheetViews>
-    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="L40" sqref="L40"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="2.85546875" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" customWidth="1"/>
-    <col min="3" max="9" width="22.7109375" customWidth="1"/>
-    <col min="10" max="10" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:26" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="46" t="s">
-        <v>92</v>
-      </c>
-      <c r="Z1" s="38"/>
-    </row>
-    <row r="2" spans="2:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="97"/>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="97"/>
-      <c r="J2" s="97"/>
-      <c r="K2" s="97"/>
-      <c r="L2" s="97"/>
-      <c r="M2" s="97"/>
-      <c r="N2" s="97"/>
-      <c r="Z2"/>
-    </row>
-    <row r="3" spans="2:26" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="98" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="98"/>
-      <c r="F3" s="98"/>
-      <c r="G3" s="98"/>
-      <c r="H3" s="98"/>
-      <c r="I3" s="98"/>
-      <c r="J3" s="98"/>
-      <c r="K3" s="98"/>
-      <c r="L3" s="98"/>
-      <c r="M3" s="98"/>
-      <c r="N3" s="98"/>
-      <c r="Z3"/>
-    </row>
-    <row r="5" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="C5" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="51" t="s">
-        <v>27</v>
-      </c>
-      <c r="F5" s="13"/>
-      <c r="G5" s="48"/>
-      <c r="H5" s="49"/>
-    </row>
-    <row r="6" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="C6" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="D6" s="103"/>
-      <c r="E6" s="104"/>
-      <c r="F6" s="105"/>
-      <c r="G6" s="50"/>
-      <c r="H6" s="50"/>
-    </row>
-    <row r="7" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B7" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="H7" s="41" t="s">
-        <v>39</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B8" s="2">
-        <v>1</v>
-      </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-    </row>
-  </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="B2:N2"/>
-    <mergeCell ref="B3:N3"/>
-    <mergeCell ref="D6:F6"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:Z8"/>
-  <sheetViews>
-    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="2.85546875" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" customWidth="1"/>
-    <col min="3" max="9" width="22.7109375" customWidth="1"/>
-    <col min="10" max="10" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:26" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="46" t="s">
-        <v>92</v>
-      </c>
-      <c r="Z1" s="38"/>
-    </row>
-    <row r="2" spans="2:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="97"/>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="97"/>
-      <c r="J2" s="97"/>
-      <c r="K2" s="97"/>
-      <c r="L2" s="97"/>
-      <c r="M2" s="97"/>
-      <c r="N2" s="97"/>
-      <c r="Z2"/>
-    </row>
-    <row r="3" spans="2:26" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="98" t="s">
-        <v>90</v>
-      </c>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="98"/>
-      <c r="F3" s="98"/>
-      <c r="G3" s="98"/>
-      <c r="H3" s="98"/>
-      <c r="I3" s="98"/>
-      <c r="J3" s="98"/>
-      <c r="K3" s="98"/>
-      <c r="L3" s="98"/>
-      <c r="M3" s="98"/>
-      <c r="N3" s="98"/>
-      <c r="Z3"/>
-    </row>
-    <row r="5" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="C5" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="F5" s="13"/>
-    </row>
-    <row r="6" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="C6" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" s="12"/>
-      <c r="E6" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="F6" s="12"/>
-    </row>
-    <row r="7" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B7" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B8" s="2">
-        <v>1</v>
-      </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B2:N2"/>
-    <mergeCell ref="B3:N3"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:Z8"/>
-  <sheetViews>
-    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="2.85546875" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" customWidth="1"/>
-    <col min="3" max="9" width="22.7109375" customWidth="1"/>
-    <col min="10" max="10" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:26" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="46" t="s">
-        <v>92</v>
-      </c>
-      <c r="Z1" s="38"/>
-    </row>
-    <row r="2" spans="2:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="97"/>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="97"/>
-      <c r="J2" s="97"/>
-      <c r="K2" s="97"/>
-      <c r="L2" s="97"/>
-      <c r="M2" s="97"/>
-      <c r="N2" s="97"/>
-      <c r="Z2"/>
-    </row>
-    <row r="3" spans="2:26" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="98" t="s">
-        <v>71</v>
-      </c>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="98"/>
-      <c r="F3" s="98"/>
-      <c r="G3" s="98"/>
-      <c r="H3" s="98"/>
-      <c r="I3" s="98"/>
-      <c r="J3" s="98"/>
-      <c r="K3" s="98"/>
-      <c r="L3" s="98"/>
-      <c r="M3" s="98"/>
-      <c r="N3" s="98"/>
-      <c r="Z3"/>
-    </row>
-    <row r="5" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="C5" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="F5" s="13"/>
-      <c r="G5" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="H5" s="12"/>
-    </row>
-    <row r="6" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="C6" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" s="12"/>
-      <c r="E6" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="F6" s="40"/>
-      <c r="G6" s="42"/>
-      <c r="H6" s="43"/>
-    </row>
-    <row r="7" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B7" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="G7" s="41" t="s">
-        <v>38</v>
-      </c>
-      <c r="H7" s="41" t="s">
         <v>39</v>
       </c>
       <c r="I7" s="4" t="s">
@@ -5399,36 +5297,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="97"/>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="97"/>
-      <c r="J2" s="97"/>
-      <c r="K2" s="97"/>
-      <c r="L2" s="97"/>
-      <c r="M2" s="97"/>
-      <c r="N2" s="97"/>
+      <c r="B2" s="99"/>
+      <c r="C2" s="99"/>
+      <c r="D2" s="99"/>
+      <c r="E2" s="99"/>
+      <c r="F2" s="99"/>
+      <c r="G2" s="99"/>
+      <c r="H2" s="99"/>
+      <c r="I2" s="99"/>
+      <c r="J2" s="99"/>
+      <c r="K2" s="99"/>
+      <c r="L2" s="99"/>
+      <c r="M2" s="99"/>
+      <c r="N2" s="99"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="98" t="s">
+      <c r="B3" s="100" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="98"/>
-      <c r="F3" s="98"/>
-      <c r="G3" s="98"/>
-      <c r="H3" s="98"/>
-      <c r="I3" s="98"/>
-      <c r="J3" s="98"/>
-      <c r="K3" s="98"/>
-      <c r="L3" s="98"/>
-      <c r="M3" s="98"/>
-      <c r="N3" s="98"/>
+      <c r="C3" s="100"/>
+      <c r="D3" s="100"/>
+      <c r="E3" s="100"/>
+      <c r="F3" s="100"/>
+      <c r="G3" s="100"/>
+      <c r="H3" s="100"/>
+      <c r="I3" s="100"/>
+      <c r="J3" s="100"/>
+      <c r="K3" s="100"/>
+      <c r="L3" s="100"/>
+      <c r="M3" s="100"/>
+      <c r="N3" s="100"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="44" t="s">
@@ -5478,6 +5376,390 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:Z8"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="L40" sqref="L40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.85546875" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" customWidth="1"/>
+    <col min="3" max="9" width="22.7109375" customWidth="1"/>
+    <col min="10" max="10" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:26" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B1" s="46" t="s">
+        <v>92</v>
+      </c>
+      <c r="Z1" s="38"/>
+    </row>
+    <row r="2" spans="2:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="99"/>
+      <c r="C2" s="99"/>
+      <c r="D2" s="99"/>
+      <c r="E2" s="99"/>
+      <c r="F2" s="99"/>
+      <c r="G2" s="99"/>
+      <c r="H2" s="99"/>
+      <c r="I2" s="99"/>
+      <c r="J2" s="99"/>
+      <c r="K2" s="99"/>
+      <c r="L2" s="99"/>
+      <c r="M2" s="99"/>
+      <c r="N2" s="99"/>
+      <c r="Z2"/>
+    </row>
+    <row r="3" spans="2:26" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B3" s="100" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="100"/>
+      <c r="D3" s="100"/>
+      <c r="E3" s="100"/>
+      <c r="F3" s="100"/>
+      <c r="G3" s="100"/>
+      <c r="H3" s="100"/>
+      <c r="I3" s="100"/>
+      <c r="J3" s="100"/>
+      <c r="K3" s="100"/>
+      <c r="L3" s="100"/>
+      <c r="M3" s="100"/>
+      <c r="N3" s="100"/>
+      <c r="Z3"/>
+    </row>
+    <row r="5" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="C5" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="51" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="13"/>
+      <c r="G5" s="48"/>
+      <c r="H5" s="49"/>
+    </row>
+    <row r="6" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="C6" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="D6" s="105"/>
+      <c r="E6" s="106"/>
+      <c r="F6" s="107"/>
+      <c r="G6" s="50"/>
+      <c r="H6" s="50"/>
+    </row>
+    <row r="7" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B7" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H7" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B8" s="2">
+        <v>1</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B2:N2"/>
+    <mergeCell ref="B3:N3"/>
+    <mergeCell ref="D6:F6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:Z8"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.85546875" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" customWidth="1"/>
+    <col min="3" max="9" width="22.7109375" customWidth="1"/>
+    <col min="10" max="10" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:26" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B1" s="46" t="s">
+        <v>92</v>
+      </c>
+      <c r="Z1" s="38"/>
+    </row>
+    <row r="2" spans="2:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="99"/>
+      <c r="C2" s="99"/>
+      <c r="D2" s="99"/>
+      <c r="E2" s="99"/>
+      <c r="F2" s="99"/>
+      <c r="G2" s="99"/>
+      <c r="H2" s="99"/>
+      <c r="I2" s="99"/>
+      <c r="J2" s="99"/>
+      <c r="K2" s="99"/>
+      <c r="L2" s="99"/>
+      <c r="M2" s="99"/>
+      <c r="N2" s="99"/>
+      <c r="Z2"/>
+    </row>
+    <row r="3" spans="2:26" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B3" s="100" t="s">
+        <v>90</v>
+      </c>
+      <c r="C3" s="100"/>
+      <c r="D3" s="100"/>
+      <c r="E3" s="100"/>
+      <c r="F3" s="100"/>
+      <c r="G3" s="100"/>
+      <c r="H3" s="100"/>
+      <c r="I3" s="100"/>
+      <c r="J3" s="100"/>
+      <c r="K3" s="100"/>
+      <c r="L3" s="100"/>
+      <c r="M3" s="100"/>
+      <c r="N3" s="100"/>
+      <c r="Z3"/>
+    </row>
+    <row r="5" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="C5" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="F5" s="13"/>
+    </row>
+    <row r="6" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="C6" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="12"/>
+      <c r="E6" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="F6" s="12"/>
+    </row>
+    <row r="7" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B7" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B8" s="2">
+        <v>1</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:N2"/>
+    <mergeCell ref="B3:N3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:Z8"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.85546875" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" customWidth="1"/>
+    <col min="3" max="9" width="22.7109375" customWidth="1"/>
+    <col min="10" max="10" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:26" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B1" s="46" t="s">
+        <v>92</v>
+      </c>
+      <c r="Z1" s="38"/>
+    </row>
+    <row r="2" spans="2:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="99"/>
+      <c r="C2" s="99"/>
+      <c r="D2" s="99"/>
+      <c r="E2" s="99"/>
+      <c r="F2" s="99"/>
+      <c r="G2" s="99"/>
+      <c r="H2" s="99"/>
+      <c r="I2" s="99"/>
+      <c r="J2" s="99"/>
+      <c r="K2" s="99"/>
+      <c r="L2" s="99"/>
+      <c r="M2" s="99"/>
+      <c r="N2" s="99"/>
+      <c r="Z2"/>
+    </row>
+    <row r="3" spans="2:26" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B3" s="100" t="s">
+        <v>71</v>
+      </c>
+      <c r="C3" s="100"/>
+      <c r="D3" s="100"/>
+      <c r="E3" s="100"/>
+      <c r="F3" s="100"/>
+      <c r="G3" s="100"/>
+      <c r="H3" s="100"/>
+      <c r="I3" s="100"/>
+      <c r="J3" s="100"/>
+      <c r="K3" s="100"/>
+      <c r="L3" s="100"/>
+      <c r="M3" s="100"/>
+      <c r="N3" s="100"/>
+      <c r="Z3"/>
+    </row>
+    <row r="5" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="C5" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="13"/>
+      <c r="G5" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" s="12"/>
+    </row>
+    <row r="6" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="C6" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="12"/>
+      <c r="E6" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="40"/>
+      <c r="G6" s="42"/>
+      <c r="H6" s="43"/>
+    </row>
+    <row r="7" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B7" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G7" s="41" t="s">
+        <v>38</v>
+      </c>
+      <c r="H7" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B8" s="2">
+        <v>1</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:N2"/>
+    <mergeCell ref="B3:N3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:Q7"/>
   <sheetViews>
@@ -5512,56 +5794,56 @@
       </c>
     </row>
     <row r="2" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="97"/>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="97"/>
-      <c r="J2" s="97"/>
-      <c r="K2" s="97"/>
-      <c r="L2" s="97"/>
+      <c r="B2" s="99"/>
+      <c r="C2" s="99"/>
+      <c r="D2" s="99"/>
+      <c r="E2" s="99"/>
+      <c r="F2" s="99"/>
+      <c r="G2" s="99"/>
+      <c r="H2" s="99"/>
+      <c r="I2" s="99"/>
+      <c r="J2" s="99"/>
+      <c r="K2" s="99"/>
+      <c r="L2" s="99"/>
     </row>
     <row r="3" spans="2:17" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="98" t="s">
+      <c r="B3" s="100" t="s">
         <v>105</v>
       </c>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="98"/>
-      <c r="F3" s="98"/>
-      <c r="G3" s="98"/>
-      <c r="H3" s="98"/>
-      <c r="I3" s="98"/>
-      <c r="J3" s="98"/>
-      <c r="K3" s="98"/>
-      <c r="L3" s="98"/>
+      <c r="C3" s="100"/>
+      <c r="D3" s="100"/>
+      <c r="E3" s="100"/>
+      <c r="F3" s="100"/>
+      <c r="G3" s="100"/>
+      <c r="H3" s="100"/>
+      <c r="I3" s="100"/>
+      <c r="J3" s="100"/>
+      <c r="K3" s="100"/>
+      <c r="L3" s="100"/>
     </row>
     <row r="5" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D5" s="106" t="s">
+      <c r="D5" s="108" t="s">
         <v>120</v>
       </c>
-      <c r="E5" s="106"/>
+      <c r="E5" s="108"/>
       <c r="F5" s="73"/>
       <c r="G5" s="73"/>
       <c r="H5" s="73"/>
       <c r="I5" s="73"/>
-      <c r="J5" s="106" t="s">
+      <c r="J5" s="108" t="s">
         <v>41</v>
       </c>
-      <c r="K5" s="106"/>
-      <c r="L5" s="106"/>
-      <c r="M5" s="106" t="s">
+      <c r="K5" s="108"/>
+      <c r="L5" s="108"/>
+      <c r="M5" s="108" t="s">
         <v>127</v>
       </c>
-      <c r="N5" s="106"/>
-      <c r="O5" s="106"/>
-      <c r="P5" s="100" t="s">
+      <c r="N5" s="108"/>
+      <c r="O5" s="108"/>
+      <c r="P5" s="102" t="s">
         <v>106</v>
       </c>
-      <c r="Q5" s="100"/>
+      <c r="Q5" s="102"/>
     </row>
     <row r="6" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="70" t="s">
@@ -5644,7 +5926,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:Y8"/>
   <sheetViews>
@@ -5685,110 +5967,110 @@
       </c>
     </row>
     <row r="2" spans="2:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="97"/>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="97"/>
-      <c r="J2" s="97"/>
-      <c r="K2" s="97"/>
-      <c r="L2" s="97"/>
-      <c r="M2" s="97"/>
-      <c r="N2" s="97"/>
-      <c r="O2" s="97"/>
-      <c r="P2" s="97"/>
+      <c r="B2" s="99"/>
+      <c r="C2" s="99"/>
+      <c r="D2" s="99"/>
+      <c r="E2" s="99"/>
+      <c r="F2" s="99"/>
+      <c r="G2" s="99"/>
+      <c r="H2" s="99"/>
+      <c r="I2" s="99"/>
+      <c r="J2" s="99"/>
+      <c r="K2" s="99"/>
+      <c r="L2" s="99"/>
+      <c r="M2" s="99"/>
+      <c r="N2" s="99"/>
+      <c r="O2" s="99"/>
+      <c r="P2" s="99"/>
       <c r="Q2" s="56"/>
       <c r="R2" s="56"/>
     </row>
     <row r="3" spans="2:25" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="98" t="s">
+      <c r="B3" s="100" t="s">
         <v>108</v>
       </c>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="98"/>
-      <c r="F3" s="98"/>
-      <c r="G3" s="98"/>
-      <c r="H3" s="98"/>
-      <c r="I3" s="98"/>
-      <c r="J3" s="98"/>
-      <c r="K3" s="98"/>
-      <c r="L3" s="98"/>
-      <c r="M3" s="98"/>
-      <c r="N3" s="98"/>
-      <c r="O3" s="98"/>
-      <c r="P3" s="98"/>
+      <c r="C3" s="100"/>
+      <c r="D3" s="100"/>
+      <c r="E3" s="100"/>
+      <c r="F3" s="100"/>
+      <c r="G3" s="100"/>
+      <c r="H3" s="100"/>
+      <c r="I3" s="100"/>
+      <c r="J3" s="100"/>
+      <c r="K3" s="100"/>
+      <c r="L3" s="100"/>
+      <c r="M3" s="100"/>
+      <c r="N3" s="100"/>
+      <c r="O3" s="100"/>
+      <c r="P3" s="100"/>
       <c r="Q3" s="57"/>
       <c r="R3" s="57"/>
     </row>
     <row r="5" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B5" s="110" t="s">
+      <c r="B5" s="109" t="s">
         <v>109</v>
       </c>
-      <c r="C5" s="111"/>
-      <c r="D5" s="111"/>
-      <c r="E5" s="111"/>
-      <c r="F5" s="111"/>
-      <c r="G5" s="111"/>
-      <c r="H5" s="111"/>
-      <c r="I5" s="111"/>
-      <c r="J5" s="111"/>
-      <c r="K5" s="111"/>
-      <c r="L5" s="112"/>
-      <c r="M5" s="110" t="s">
+      <c r="C5" s="110"/>
+      <c r="D5" s="110"/>
+      <c r="E5" s="110"/>
+      <c r="F5" s="110"/>
+      <c r="G5" s="110"/>
+      <c r="H5" s="110"/>
+      <c r="I5" s="110"/>
+      <c r="J5" s="110"/>
+      <c r="K5" s="110"/>
+      <c r="L5" s="111"/>
+      <c r="M5" s="109" t="s">
         <v>110</v>
       </c>
-      <c r="N5" s="111"/>
-      <c r="O5" s="111"/>
-      <c r="P5" s="111"/>
-      <c r="Q5" s="111"/>
-      <c r="R5" s="111"/>
-      <c r="S5" s="111"/>
-      <c r="T5" s="111"/>
-      <c r="U5" s="111"/>
-      <c r="V5" s="111"/>
-      <c r="W5" s="111"/>
-      <c r="X5" s="111"/>
-      <c r="Y5" s="112"/>
+      <c r="N5" s="110"/>
+      <c r="O5" s="110"/>
+      <c r="P5" s="110"/>
+      <c r="Q5" s="110"/>
+      <c r="R5" s="110"/>
+      <c r="S5" s="110"/>
+      <c r="T5" s="110"/>
+      <c r="U5" s="110"/>
+      <c r="V5" s="110"/>
+      <c r="W5" s="110"/>
+      <c r="X5" s="110"/>
+      <c r="Y5" s="111"/>
     </row>
     <row r="6" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B6" s="107"/>
-      <c r="C6" s="107"/>
-      <c r="D6" s="107"/>
-      <c r="E6" s="107"/>
-      <c r="F6" s="116" t="s">
+      <c r="B6" s="118"/>
+      <c r="C6" s="118"/>
+      <c r="D6" s="118"/>
+      <c r="E6" s="118"/>
+      <c r="F6" s="112" t="s">
         <v>26</v>
       </c>
-      <c r="G6" s="117"/>
-      <c r="H6" s="117"/>
-      <c r="I6" s="118"/>
-      <c r="J6" s="110" t="s">
+      <c r="G6" s="113"/>
+      <c r="H6" s="113"/>
+      <c r="I6" s="114"/>
+      <c r="J6" s="109" t="s">
         <v>29</v>
       </c>
-      <c r="K6" s="111"/>
-      <c r="L6" s="112"/>
+      <c r="K6" s="110"/>
+      <c r="L6" s="111"/>
       <c r="M6" s="87"/>
-      <c r="N6" s="108" t="s">
+      <c r="N6" s="115" t="s">
         <v>41</v>
       </c>
-      <c r="O6" s="109"/>
-      <c r="P6" s="108" t="s">
+      <c r="O6" s="116"/>
+      <c r="P6" s="115" t="s">
         <v>103</v>
       </c>
-      <c r="Q6" s="119"/>
-      <c r="R6" s="109"/>
+      <c r="Q6" s="117"/>
+      <c r="R6" s="116"/>
       <c r="S6" s="87"/>
-      <c r="T6" s="108" t="s">
+      <c r="T6" s="115" t="s">
         <v>120</v>
       </c>
-      <c r="U6" s="109"/>
-      <c r="V6" s="113"/>
-      <c r="W6" s="114"/>
-      <c r="X6" s="114"/>
-      <c r="Y6" s="115"/>
+      <c r="U6" s="116"/>
+      <c r="V6" s="119"/>
+      <c r="W6" s="120"/>
+      <c r="X6" s="120"/>
+      <c r="Y6" s="121"/>
     </row>
     <row r="7" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B7" s="75" t="s">
@@ -5892,8 +6174,6 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="P6:R6"/>
-    <mergeCell ref="B6:E6"/>
     <mergeCell ref="T6:U6"/>
     <mergeCell ref="M5:Y5"/>
     <mergeCell ref="V6:Y6"/>
@@ -5903,13 +6183,15 @@
     <mergeCell ref="J6:L6"/>
     <mergeCell ref="F6:I6"/>
     <mergeCell ref="N6:O6"/>
+    <mergeCell ref="P6:R6"/>
+    <mergeCell ref="B6:E6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A24"/>
   <sheetViews>
@@ -6021,18 +6303,18 @@
       </c>
     </row>
     <row r="2" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="97"/>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
+      <c r="B2" s="99"/>
+      <c r="C2" s="99"/>
+      <c r="D2" s="99"/>
+      <c r="E2" s="99"/>
     </row>
     <row r="3" spans="2:5" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="98" t="s">
+      <c r="B3" s="100" t="s">
         <v>128</v>
       </c>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="98"/>
+      <c r="C3" s="100"/>
+      <c r="D3" s="100"/>
+      <c r="E3" s="100"/>
     </row>
     <row r="4" spans="2:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="64"/>
@@ -6093,40 +6375,40 @@
       </c>
     </row>
     <row r="2" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="97"/>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="97"/>
-      <c r="J2" s="97"/>
-      <c r="K2" s="97"/>
-      <c r="L2" s="97"/>
-      <c r="M2" s="97"/>
-      <c r="N2" s="97"/>
-      <c r="O2" s="97"/>
-      <c r="P2" s="97"/>
+      <c r="B2" s="99"/>
+      <c r="C2" s="99"/>
+      <c r="D2" s="99"/>
+      <c r="E2" s="99"/>
+      <c r="F2" s="99"/>
+      <c r="G2" s="99"/>
+      <c r="H2" s="99"/>
+      <c r="I2" s="99"/>
+      <c r="J2" s="99"/>
+      <c r="K2" s="99"/>
+      <c r="L2" s="99"/>
+      <c r="M2" s="99"/>
+      <c r="N2" s="99"/>
+      <c r="O2" s="99"/>
+      <c r="P2" s="99"/>
     </row>
     <row r="3" spans="2:16" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="98" t="s">
+      <c r="B3" s="100" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="98"/>
-      <c r="F3" s="98"/>
-      <c r="G3" s="98"/>
-      <c r="H3" s="98"/>
-      <c r="I3" s="98"/>
-      <c r="J3" s="98"/>
-      <c r="K3" s="98"/>
-      <c r="L3" s="98"/>
-      <c r="M3" s="98"/>
-      <c r="N3" s="98"/>
-      <c r="O3" s="98"/>
-      <c r="P3" s="98"/>
+      <c r="C3" s="100"/>
+      <c r="D3" s="100"/>
+      <c r="E3" s="100"/>
+      <c r="F3" s="100"/>
+      <c r="G3" s="100"/>
+      <c r="H3" s="100"/>
+      <c r="I3" s="100"/>
+      <c r="J3" s="100"/>
+      <c r="K3" s="100"/>
+      <c r="L3" s="100"/>
+      <c r="M3" s="100"/>
+      <c r="N3" s="100"/>
+      <c r="O3" s="100"/>
+      <c r="P3" s="100"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="44" t="s">
@@ -6205,40 +6487,40 @@
       </c>
     </row>
     <row r="2" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="97"/>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="97"/>
-      <c r="J2" s="97"/>
-      <c r="K2" s="97"/>
-      <c r="L2" s="97"/>
-      <c r="M2" s="97"/>
-      <c r="N2" s="97"/>
-      <c r="O2" s="97"/>
-      <c r="P2" s="97"/>
+      <c r="B2" s="99"/>
+      <c r="C2" s="99"/>
+      <c r="D2" s="99"/>
+      <c r="E2" s="99"/>
+      <c r="F2" s="99"/>
+      <c r="G2" s="99"/>
+      <c r="H2" s="99"/>
+      <c r="I2" s="99"/>
+      <c r="J2" s="99"/>
+      <c r="K2" s="99"/>
+      <c r="L2" s="99"/>
+      <c r="M2" s="99"/>
+      <c r="N2" s="99"/>
+      <c r="O2" s="99"/>
+      <c r="P2" s="99"/>
     </row>
     <row r="3" spans="2:16" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="98" t="s">
+      <c r="B3" s="100" t="s">
         <v>67</v>
       </c>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="98"/>
-      <c r="F3" s="98"/>
-      <c r="G3" s="98"/>
-      <c r="H3" s="98"/>
-      <c r="I3" s="98"/>
-      <c r="J3" s="98"/>
-      <c r="K3" s="98"/>
-      <c r="L3" s="98"/>
-      <c r="M3" s="98"/>
-      <c r="N3" s="98"/>
-      <c r="O3" s="98"/>
-      <c r="P3" s="98"/>
+      <c r="C3" s="100"/>
+      <c r="D3" s="100"/>
+      <c r="E3" s="100"/>
+      <c r="F3" s="100"/>
+      <c r="G3" s="100"/>
+      <c r="H3" s="100"/>
+      <c r="I3" s="100"/>
+      <c r="J3" s="100"/>
+      <c r="K3" s="100"/>
+      <c r="L3" s="100"/>
+      <c r="M3" s="100"/>
+      <c r="N3" s="100"/>
+      <c r="O3" s="100"/>
+      <c r="P3" s="100"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
@@ -6287,40 +6569,40 @@
       </c>
     </row>
     <row r="2" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="97"/>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="97"/>
-      <c r="J2" s="97"/>
-      <c r="K2" s="97"/>
-      <c r="L2" s="97"/>
-      <c r="M2" s="97"/>
-      <c r="N2" s="97"/>
-      <c r="O2" s="97"/>
-      <c r="P2" s="97"/>
+      <c r="B2" s="99"/>
+      <c r="C2" s="99"/>
+      <c r="D2" s="99"/>
+      <c r="E2" s="99"/>
+      <c r="F2" s="99"/>
+      <c r="G2" s="99"/>
+      <c r="H2" s="99"/>
+      <c r="I2" s="99"/>
+      <c r="J2" s="99"/>
+      <c r="K2" s="99"/>
+      <c r="L2" s="99"/>
+      <c r="M2" s="99"/>
+      <c r="N2" s="99"/>
+      <c r="O2" s="99"/>
+      <c r="P2" s="99"/>
     </row>
     <row r="3" spans="2:16" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="98" t="s">
+      <c r="B3" s="100" t="s">
         <v>70</v>
       </c>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="98"/>
-      <c r="F3" s="98"/>
-      <c r="G3" s="98"/>
-      <c r="H3" s="98"/>
-      <c r="I3" s="98"/>
-      <c r="J3" s="98"/>
-      <c r="K3" s="98"/>
-      <c r="L3" s="98"/>
-      <c r="M3" s="98"/>
-      <c r="N3" s="98"/>
-      <c r="O3" s="98"/>
-      <c r="P3" s="98"/>
+      <c r="C3" s="100"/>
+      <c r="D3" s="100"/>
+      <c r="E3" s="100"/>
+      <c r="F3" s="100"/>
+      <c r="G3" s="100"/>
+      <c r="H3" s="100"/>
+      <c r="I3" s="100"/>
+      <c r="J3" s="100"/>
+      <c r="K3" s="100"/>
+      <c r="L3" s="100"/>
+      <c r="M3" s="100"/>
+      <c r="N3" s="100"/>
+      <c r="O3" s="100"/>
+      <c r="P3" s="100"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
@@ -6348,8 +6630,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:P6"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView showGridLines="0" topLeftCell="C1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="J43" sqref="J43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6375,40 +6657,40 @@
       </c>
     </row>
     <row r="2" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="97"/>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="97"/>
-      <c r="J2" s="97"/>
-      <c r="K2" s="97"/>
-      <c r="L2" s="97"/>
-      <c r="M2" s="97"/>
-      <c r="N2" s="97"/>
-      <c r="O2" s="97"/>
-      <c r="P2" s="97"/>
+      <c r="B2" s="99"/>
+      <c r="C2" s="99"/>
+      <c r="D2" s="99"/>
+      <c r="E2" s="99"/>
+      <c r="F2" s="99"/>
+      <c r="G2" s="99"/>
+      <c r="H2" s="99"/>
+      <c r="I2" s="99"/>
+      <c r="J2" s="99"/>
+      <c r="K2" s="99"/>
+      <c r="L2" s="99"/>
+      <c r="M2" s="99"/>
+      <c r="N2" s="99"/>
+      <c r="O2" s="99"/>
+      <c r="P2" s="99"/>
     </row>
     <row r="3" spans="2:16" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="98" t="s">
+      <c r="B3" s="100" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="98"/>
-      <c r="F3" s="98"/>
-      <c r="G3" s="98"/>
-      <c r="H3" s="98"/>
-      <c r="I3" s="98"/>
-      <c r="J3" s="98"/>
-      <c r="K3" s="98"/>
-      <c r="L3" s="98"/>
-      <c r="M3" s="98"/>
-      <c r="N3" s="98"/>
-      <c r="O3" s="98"/>
-      <c r="P3" s="98"/>
+      <c r="C3" s="100"/>
+      <c r="D3" s="100"/>
+      <c r="E3" s="100"/>
+      <c r="F3" s="100"/>
+      <c r="G3" s="100"/>
+      <c r="H3" s="100"/>
+      <c r="I3" s="100"/>
+      <c r="J3" s="100"/>
+      <c r="K3" s="100"/>
+      <c r="L3" s="100"/>
+      <c r="M3" s="100"/>
+      <c r="N3" s="100"/>
+      <c r="O3" s="100"/>
+      <c r="P3" s="100"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="44" t="s">
@@ -6505,40 +6787,40 @@
       </c>
     </row>
     <row r="2" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="97"/>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="97"/>
-      <c r="J2" s="97"/>
-      <c r="K2" s="97"/>
-      <c r="L2" s="97"/>
-      <c r="M2" s="97"/>
-      <c r="N2" s="97"/>
-      <c r="O2" s="97"/>
-      <c r="P2" s="97"/>
+      <c r="B2" s="99"/>
+      <c r="C2" s="99"/>
+      <c r="D2" s="99"/>
+      <c r="E2" s="99"/>
+      <c r="F2" s="99"/>
+      <c r="G2" s="99"/>
+      <c r="H2" s="99"/>
+      <c r="I2" s="99"/>
+      <c r="J2" s="99"/>
+      <c r="K2" s="99"/>
+      <c r="L2" s="99"/>
+      <c r="M2" s="99"/>
+      <c r="N2" s="99"/>
+      <c r="O2" s="99"/>
+      <c r="P2" s="99"/>
     </row>
     <row r="3" spans="2:16" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="98" t="s">
+      <c r="B3" s="100" t="s">
         <v>64</v>
       </c>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="98"/>
-      <c r="F3" s="98"/>
-      <c r="G3" s="98"/>
-      <c r="H3" s="98"/>
-      <c r="I3" s="98"/>
-      <c r="J3" s="98"/>
-      <c r="K3" s="98"/>
-      <c r="L3" s="98"/>
-      <c r="M3" s="98"/>
-      <c r="N3" s="98"/>
-      <c r="O3" s="98"/>
-      <c r="P3" s="98"/>
+      <c r="C3" s="100"/>
+      <c r="D3" s="100"/>
+      <c r="E3" s="100"/>
+      <c r="F3" s="100"/>
+      <c r="G3" s="100"/>
+      <c r="H3" s="100"/>
+      <c r="I3" s="100"/>
+      <c r="J3" s="100"/>
+      <c r="K3" s="100"/>
+      <c r="L3" s="100"/>
+      <c r="M3" s="100"/>
+      <c r="N3" s="100"/>
+      <c r="O3" s="100"/>
+      <c r="P3" s="100"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="45" t="s">

</xml_diff>

<commit_message>
TRIEDA-1722 - Adicionando colunas salas e laboratórios nos relatórios de ambientes.
</commit_message>
<xml_diff>
--- a/code/client/web/src/main/resources/templateExport.xlsx
+++ b/code/client/web/src/main/resources/templateExport.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="17070" windowHeight="5370" tabRatio="964" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="17070" windowHeight="5370" tabRatio="976" firstSheet="35" activeTab="41"/>
   </bookViews>
   <sheets>
     <sheet name="Turnos" sheetId="49" r:id="rId1"/>
@@ -1420,7 +1420,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="245">
   <si>
     <t>Planilha de Unidades</t>
   </si>
@@ -2185,6 +2185,12 @@
   </si>
   <si>
     <t>É recomendavel preencher caso o deslocamento entre os prédios leve um tempo considerável</t>
+  </si>
+  <si>
+    <t>Salas</t>
+  </si>
+  <si>
+    <t>Laboratórios</t>
   </si>
 </sst>
 </file>
@@ -2948,15 +2954,18 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="28" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2983,9 +2992,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="28" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -6501,7 +6507,7 @@
   <dimension ref="B1:H6"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="T42" sqref="T42"/>
+      <selection activeCell="D5" sqref="D5:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6509,6 +6515,8 @@
     <col min="1" max="1" width="2.85546875" customWidth="1"/>
     <col min="2" max="2" width="38.7109375" customWidth="1"/>
     <col min="3" max="3" width="26.42578125" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
@@ -6543,10 +6551,18 @@
       <c r="C5" s="100" t="s">
         <v>222</v>
       </c>
+      <c r="D5" s="100" t="s">
+        <v>243</v>
+      </c>
+      <c r="E5" s="100" t="s">
+        <v>244</v>
+      </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -6561,8 +6577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H6"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6570,6 +6586,8 @@
     <col min="1" max="1" width="2.85546875" customWidth="1"/>
     <col min="2" max="2" width="38.7109375" customWidth="1"/>
     <col min="3" max="3" width="26.42578125" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
@@ -6604,10 +6622,18 @@
       <c r="C5" s="100" t="s">
         <v>222</v>
       </c>
+      <c r="D5" s="100" t="s">
+        <v>243</v>
+      </c>
+      <c r="E5" s="100" t="s">
+        <v>244</v>
+      </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -7384,70 +7410,70 @@
       <c r="R3" s="57"/>
     </row>
     <row r="5" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B5" s="116" t="s">
+      <c r="B5" s="117" t="s">
         <v>109</v>
       </c>
-      <c r="C5" s="117"/>
-      <c r="D5" s="117"/>
-      <c r="E5" s="117"/>
-      <c r="F5" s="117"/>
-      <c r="G5" s="117"/>
-      <c r="H5" s="117"/>
-      <c r="I5" s="117"/>
-      <c r="J5" s="117"/>
-      <c r="K5" s="117"/>
-      <c r="L5" s="118"/>
-      <c r="M5" s="116" t="s">
+      <c r="C5" s="118"/>
+      <c r="D5" s="118"/>
+      <c r="E5" s="118"/>
+      <c r="F5" s="118"/>
+      <c r="G5" s="118"/>
+      <c r="H5" s="118"/>
+      <c r="I5" s="118"/>
+      <c r="J5" s="118"/>
+      <c r="K5" s="118"/>
+      <c r="L5" s="119"/>
+      <c r="M5" s="117" t="s">
         <v>110</v>
       </c>
-      <c r="N5" s="117"/>
-      <c r="O5" s="117"/>
-      <c r="P5" s="117"/>
-      <c r="Q5" s="117"/>
-      <c r="R5" s="117"/>
-      <c r="S5" s="117"/>
-      <c r="T5" s="117"/>
-      <c r="U5" s="117"/>
-      <c r="V5" s="117"/>
-      <c r="W5" s="117"/>
-      <c r="X5" s="117"/>
-      <c r="Y5" s="118"/>
+      <c r="N5" s="118"/>
+      <c r="O5" s="118"/>
+      <c r="P5" s="118"/>
+      <c r="Q5" s="118"/>
+      <c r="R5" s="118"/>
+      <c r="S5" s="118"/>
+      <c r="T5" s="118"/>
+      <c r="U5" s="118"/>
+      <c r="V5" s="118"/>
+      <c r="W5" s="118"/>
+      <c r="X5" s="118"/>
+      <c r="Y5" s="119"/>
     </row>
     <row r="6" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B6" s="113"/>
-      <c r="C6" s="113"/>
-      <c r="D6" s="113"/>
-      <c r="E6" s="113"/>
-      <c r="F6" s="122" t="s">
+      <c r="B6" s="116"/>
+      <c r="C6" s="116"/>
+      <c r="D6" s="116"/>
+      <c r="E6" s="116"/>
+      <c r="F6" s="123" t="s">
         <v>26</v>
       </c>
-      <c r="G6" s="123"/>
-      <c r="H6" s="123"/>
-      <c r="I6" s="124"/>
-      <c r="J6" s="116" t="s">
+      <c r="G6" s="124"/>
+      <c r="H6" s="124"/>
+      <c r="I6" s="125"/>
+      <c r="J6" s="117" t="s">
         <v>29</v>
       </c>
-      <c r="K6" s="117"/>
-      <c r="L6" s="118"/>
+      <c r="K6" s="118"/>
+      <c r="L6" s="119"/>
       <c r="M6" s="87"/>
-      <c r="N6" s="114" t="s">
+      <c r="N6" s="113" t="s">
         <v>41</v>
       </c>
       <c r="O6" s="115"/>
-      <c r="P6" s="114" t="s">
+      <c r="P6" s="113" t="s">
         <v>103</v>
       </c>
-      <c r="Q6" s="125"/>
+      <c r="Q6" s="114"/>
       <c r="R6" s="115"/>
       <c r="S6" s="87"/>
-      <c r="T6" s="114" t="s">
+      <c r="T6" s="113" t="s">
         <v>120</v>
       </c>
       <c r="U6" s="115"/>
-      <c r="V6" s="119"/>
-      <c r="W6" s="120"/>
-      <c r="X6" s="120"/>
-      <c r="Y6" s="121"/>
+      <c r="V6" s="120"/>
+      <c r="W6" s="121"/>
+      <c r="X6" s="121"/>
+      <c r="Y6" s="122"/>
     </row>
     <row r="7" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B7" s="75" t="s">
@@ -7551,6 +7577,7 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="N6:O6"/>
     <mergeCell ref="P6:R6"/>
     <mergeCell ref="B6:E6"/>
     <mergeCell ref="T6:U6"/>
@@ -7561,7 +7588,6 @@
     <mergeCell ref="B5:L5"/>
     <mergeCell ref="J6:L6"/>
     <mergeCell ref="F6:I6"/>
-    <mergeCell ref="N6:O6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -7660,7 +7686,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:M7"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -8038,7 +8064,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:I6"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="C1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
TRIEDA-1723 - Criando exportações do resumo por campus e resumo por cenário. Alterando textos em alguns relatórios e adicionando novos campos. Criando novas telas para os histogramas nos relatórios.
</commit_message>
<xml_diff>
--- a/code/client/web/src/main/resources/templateExport.xlsx
+++ b/code/client/web/src/main/resources/templateExport.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="17070" windowHeight="5370" tabRatio="976" firstSheet="35" activeTab="41"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="17070" windowHeight="5370" tabRatio="976" firstSheet="25" activeTab="27"/>
   </bookViews>
   <sheets>
     <sheet name="Turnos" sheetId="49" r:id="rId1"/>
@@ -33,29 +33,31 @@
     <sheet name="Disponibilidades Professores" sheetId="28" r:id="rId24"/>
     <sheet name="Campi de Trabalho" sheetId="18" r:id="rId25"/>
     <sheet name="Habilitacao dos Professores" sheetId="13" r:id="rId26"/>
-    <sheet name="Resumo por curso" sheetId="14" r:id="rId27"/>
-    <sheet name="Resumo por disciplina" sheetId="15" r:id="rId28"/>
-    <sheet name="Atendimentos por Matricula" sheetId="30" r:id="rId29"/>
-    <sheet name="Atendimentos por Disciplina" sheetId="31" r:id="rId30"/>
-    <sheet name="Atendimentos Faixa de Demanda" sheetId="32" r:id="rId31"/>
-    <sheet name="Atendimentos Faixa de Credito" sheetId="40" r:id="rId32"/>
-    <sheet name="Atendimentos Faixa Disciplina" sheetId="41" r:id="rId33"/>
-    <sheet name="Atendimentos por Carga Horaria" sheetId="35" r:id="rId34"/>
-    <sheet name="Porcentagem Mestres e Doutores" sheetId="33" r:id="rId35"/>
-    <sheet name="Professores Quantidade Janelas" sheetId="42" r:id="rId36"/>
-    <sheet name="Professores Disc Habilitadas" sheetId="43" r:id="rId37"/>
-    <sheet name="Professores Disc Lecionadas" sheetId="44" r:id="rId38"/>
-    <sheet name="Professores Titulacoes" sheetId="45" r:id="rId39"/>
-    <sheet name="Professores Areas Conhecimento" sheetId="46" r:id="rId40"/>
-    <sheet name="Ambientes Faixa Utilizacao" sheetId="47" r:id="rId41"/>
-    <sheet name="Ambientes Faixa Ocupacao" sheetId="48" r:id="rId42"/>
-    <sheet name="Relatorio Visao Sala" sheetId="10" r:id="rId43"/>
-    <sheet name="Relatorio Visao Aluno" sheetId="25" r:id="rId44"/>
-    <sheet name="Relatorio Visao Professor" sheetId="21" r:id="rId45"/>
-    <sheet name="Relatorio Visao Curso" sheetId="20" r:id="rId46"/>
-    <sheet name="Atendimentos por Aluno" sheetId="23" r:id="rId47"/>
-    <sheet name="Aulas" sheetId="26" r:id="rId48"/>
-    <sheet name="PaletaCores" sheetId="11" r:id="rId49"/>
+    <sheet name="Resumo por Cenario" sheetId="54" r:id="rId27"/>
+    <sheet name="Resumo por Campus" sheetId="55" r:id="rId28"/>
+    <sheet name="Resumo por curso" sheetId="14" r:id="rId29"/>
+    <sheet name="Resumo por disciplina" sheetId="15" r:id="rId30"/>
+    <sheet name="Atendimentos por Matricula" sheetId="30" r:id="rId31"/>
+    <sheet name="Atendimentos por Disciplina" sheetId="31" r:id="rId32"/>
+    <sheet name="Atendimentos Faixa de Demanda" sheetId="32" r:id="rId33"/>
+    <sheet name="Atendimentos Faixa de Credito" sheetId="40" r:id="rId34"/>
+    <sheet name="Atendimentos Faixa Disciplina" sheetId="41" r:id="rId35"/>
+    <sheet name="Atendimentos por Carga Horaria" sheetId="35" r:id="rId36"/>
+    <sheet name="Porcentagem Mestres e Doutores" sheetId="33" r:id="rId37"/>
+    <sheet name="Professores Quantidade Janelas" sheetId="42" r:id="rId38"/>
+    <sheet name="Professores Disc Habilitadas" sheetId="43" r:id="rId39"/>
+    <sheet name="Professores Disc Lecionadas" sheetId="44" r:id="rId40"/>
+    <sheet name="Professores Titulacoes" sheetId="45" r:id="rId41"/>
+    <sheet name="Professores Areas Conhecimento" sheetId="46" r:id="rId42"/>
+    <sheet name="Ambientes Faixa Utilizacao" sheetId="47" r:id="rId43"/>
+    <sheet name="Ambientes Faixa Ocupacao" sheetId="48" r:id="rId44"/>
+    <sheet name="Relatorio Visao Sala" sheetId="10" r:id="rId45"/>
+    <sheet name="Relatorio Visao Aluno" sheetId="25" r:id="rId46"/>
+    <sheet name="Relatorio Visao Professor" sheetId="21" r:id="rId47"/>
+    <sheet name="Relatorio Visao Curso" sheetId="20" r:id="rId48"/>
+    <sheet name="Atendimentos por Aluno" sheetId="23" r:id="rId49"/>
+    <sheet name="Aulas" sheetId="26" r:id="rId50"/>
+    <sheet name="PaletaCores" sheetId="11" r:id="rId51"/>
   </sheets>
   <calcPr calcId="125725" concurrentCalc="0"/>
 </workbook>
@@ -1420,7 +1422,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="248">
   <si>
     <t>Planilha de Unidades</t>
   </si>
@@ -2191,6 +2193,15 @@
   </si>
   <si>
     <t>Laboratórios</t>
+  </si>
+  <si>
+    <t>Cenário</t>
+  </si>
+  <si>
+    <t>Planilha de Resumo por Cenário</t>
+  </si>
+  <si>
+    <t>Planilha de Resumo por Campus</t>
   </si>
 </sst>
 </file>
@@ -2632,7 +2643,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="126">
+  <cellXfs count="128">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2954,27 +2965,36 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="28" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="28" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="28" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="28" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2984,14 +3004,11 @@
     <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -5033,6 +5050,152 @@
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:P6"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:P3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.85546875" customWidth="1"/>
+    <col min="2" max="2" width="127.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:16" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B1" s="46" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="105"/>
+      <c r="C2" s="105"/>
+      <c r="D2" s="105"/>
+      <c r="E2" s="105"/>
+      <c r="F2" s="105"/>
+      <c r="G2" s="105"/>
+      <c r="H2" s="105"/>
+      <c r="I2" s="105"/>
+      <c r="J2" s="105"/>
+      <c r="K2" s="105"/>
+      <c r="L2" s="105"/>
+      <c r="M2" s="105"/>
+      <c r="N2" s="105"/>
+      <c r="O2" s="105"/>
+      <c r="P2" s="105"/>
+    </row>
+    <row r="3" spans="2:16" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B3" s="104" t="s">
+        <v>246</v>
+      </c>
+      <c r="C3" s="104"/>
+      <c r="D3" s="104"/>
+      <c r="E3" s="104"/>
+      <c r="F3" s="104"/>
+      <c r="G3" s="104"/>
+      <c r="H3" s="104"/>
+      <c r="I3" s="104"/>
+      <c r="J3" s="104"/>
+      <c r="K3" s="104"/>
+      <c r="L3" s="104"/>
+      <c r="M3" s="104"/>
+      <c r="N3" s="104"/>
+      <c r="O3" s="104"/>
+      <c r="P3" s="104"/>
+    </row>
+    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B5" s="126" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B6" s="127"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:P2"/>
+    <mergeCell ref="B3:P3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:P6"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.85546875" customWidth="1"/>
+    <col min="2" max="2" width="127.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:16" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B1" s="46" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="105"/>
+      <c r="C2" s="105"/>
+      <c r="D2" s="105"/>
+      <c r="E2" s="105"/>
+      <c r="F2" s="105"/>
+      <c r="G2" s="105"/>
+      <c r="H2" s="105"/>
+      <c r="I2" s="105"/>
+      <c r="J2" s="105"/>
+      <c r="K2" s="105"/>
+      <c r="L2" s="105"/>
+      <c r="M2" s="105"/>
+      <c r="N2" s="105"/>
+      <c r="O2" s="105"/>
+      <c r="P2" s="105"/>
+    </row>
+    <row r="3" spans="2:16" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B3" s="104" t="s">
+        <v>247</v>
+      </c>
+      <c r="C3" s="104"/>
+      <c r="D3" s="104"/>
+      <c r="E3" s="104"/>
+      <c r="F3" s="104"/>
+      <c r="G3" s="104"/>
+      <c r="H3" s="104"/>
+      <c r="I3" s="104"/>
+      <c r="J3" s="104"/>
+      <c r="K3" s="104"/>
+      <c r="L3" s="104"/>
+      <c r="M3" s="104"/>
+      <c r="N3" s="104"/>
+      <c r="O3" s="104"/>
+      <c r="P3" s="104"/>
+    </row>
+    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B5" s="126" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B6" s="127"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:P2"/>
+    <mergeCell ref="B3:P3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:R6"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
@@ -5184,7 +5347,81 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:M6"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.85546875" customWidth="1"/>
+    <col min="2" max="2" width="35.5703125" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:13" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B1" s="46" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="2:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="103" t="s">
+        <v>238</v>
+      </c>
+      <c r="C2" s="103"/>
+      <c r="D2" s="103"/>
+      <c r="E2" s="103"/>
+      <c r="F2" s="103"/>
+      <c r="G2" s="103"/>
+      <c r="H2" s="103"/>
+      <c r="I2" s="103"/>
+      <c r="J2" s="103"/>
+      <c r="K2" s="103"/>
+      <c r="L2" s="103"/>
+      <c r="M2" s="103"/>
+    </row>
+    <row r="3" spans="2:13" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="104" t="s">
+        <v>239</v>
+      </c>
+      <c r="C3" s="104"/>
+      <c r="D3" s="104"/>
+      <c r="E3" s="104"/>
+      <c r="F3" s="104"/>
+      <c r="G3" s="104"/>
+      <c r="H3" s="104"/>
+      <c r="I3" s="104"/>
+      <c r="J3" s="104"/>
+      <c r="K3" s="104"/>
+      <c r="L3" s="104"/>
+      <c r="M3" s="104"/>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B5" s="70" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B6" s="8"/>
+      <c r="C6" s="9"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B3:M3"/>
+    <mergeCell ref="B2:M2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:N6"/>
   <sheetViews>
@@ -5303,7 +5540,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:N6"/>
   <sheetViews>
@@ -5422,81 +5659,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:M6"/>
-  <sheetViews>
-    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="2.85546875" customWidth="1"/>
-    <col min="2" max="2" width="35.5703125" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:13" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="46" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="2" spans="2:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="103" t="s">
-        <v>238</v>
-      </c>
-      <c r="C2" s="103"/>
-      <c r="D2" s="103"/>
-      <c r="E2" s="103"/>
-      <c r="F2" s="103"/>
-      <c r="G2" s="103"/>
-      <c r="H2" s="103"/>
-      <c r="I2" s="103"/>
-      <c r="J2" s="103"/>
-      <c r="K2" s="103"/>
-      <c r="L2" s="103"/>
-      <c r="M2" s="103"/>
-    </row>
-    <row r="3" spans="2:13" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="104" t="s">
-        <v>239</v>
-      </c>
-      <c r="C3" s="104"/>
-      <c r="D3" s="104"/>
-      <c r="E3" s="104"/>
-      <c r="F3" s="104"/>
-      <c r="G3" s="104"/>
-      <c r="H3" s="104"/>
-      <c r="I3" s="104"/>
-      <c r="J3" s="104"/>
-      <c r="K3" s="104"/>
-      <c r="L3" s="104"/>
-      <c r="M3" s="104"/>
-    </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B5" s="70" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B6" s="8"/>
-      <c r="C6" s="9"/>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B3:M3"/>
-    <mergeCell ref="B2:M2"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J6"/>
   <sheetViews>
@@ -5592,7 +5755,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:T6"/>
   <sheetViews>
@@ -5746,7 +5909,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F6"/>
   <sheetViews>
@@ -5818,7 +5981,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:I6"/>
   <sheetViews>
@@ -5886,7 +6049,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:I6"/>
   <sheetViews>
@@ -5979,7 +6142,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K7"/>
   <sheetViews>
@@ -6110,7 +6273,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H6"/>
   <sheetViews>
@@ -6171,7 +6334,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H6"/>
   <sheetViews>
@@ -6214,128 +6377,6 @@
     <row r="5" spans="2:8" ht="27" x14ac:dyDescent="0.25">
       <c r="B5" s="100" t="s">
         <v>216</v>
-      </c>
-      <c r="C5" s="100" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="8"/>
-      <c r="C6" s="9"/>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B2:H3"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H6"/>
-  <sheetViews>
-    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="M40" sqref="M40"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="2.85546875" customWidth="1"/>
-    <col min="2" max="2" width="38.7109375" customWidth="1"/>
-    <col min="3" max="3" width="26.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:8" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="46" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="2" spans="2:8" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="104" t="s">
-        <v>217</v>
-      </c>
-      <c r="C2" s="104"/>
-      <c r="D2" s="104"/>
-      <c r="E2" s="104"/>
-      <c r="F2" s="104"/>
-      <c r="G2" s="104"/>
-      <c r="H2" s="104"/>
-    </row>
-    <row r="3" spans="2:8" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="104"/>
-      <c r="C3" s="104"/>
-      <c r="D3" s="104"/>
-      <c r="E3" s="104"/>
-      <c r="F3" s="104"/>
-      <c r="G3" s="104"/>
-      <c r="H3" s="104"/>
-    </row>
-    <row r="5" spans="2:8" ht="27" x14ac:dyDescent="0.25">
-      <c r="B5" s="100" t="s">
-        <v>218</v>
-      </c>
-      <c r="C5" s="100" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="8"/>
-      <c r="C6" s="9"/>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B2:H3"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H6"/>
-  <sheetViews>
-    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="P42" sqref="P42"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="2.85546875" customWidth="1"/>
-    <col min="2" max="2" width="38.7109375" customWidth="1"/>
-    <col min="3" max="3" width="26.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:8" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="46" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="2" spans="2:8" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="104" t="s">
-        <v>219</v>
-      </c>
-      <c r="C2" s="104"/>
-      <c r="D2" s="104"/>
-      <c r="E2" s="104"/>
-      <c r="F2" s="104"/>
-      <c r="G2" s="104"/>
-      <c r="H2" s="104"/>
-    </row>
-    <row r="3" spans="2:8" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="104"/>
-      <c r="C3" s="104"/>
-      <c r="D3" s="104"/>
-      <c r="E3" s="104"/>
-      <c r="F3" s="104"/>
-      <c r="G3" s="104"/>
-      <c r="H3" s="104"/>
-    </row>
-    <row r="5" spans="2:8" ht="27" x14ac:dyDescent="0.25">
-      <c r="B5" s="100" t="s">
-        <v>47</v>
       </c>
       <c r="C5" s="100" t="s">
         <v>212</v>
@@ -6446,6 +6487,128 @@
   <dimension ref="B1:H6"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="M40" sqref="M40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.85546875" customWidth="1"/>
+    <col min="2" max="2" width="38.7109375" customWidth="1"/>
+    <col min="3" max="3" width="26.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:8" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B1" s="46" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="2:8" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="104" t="s">
+        <v>217</v>
+      </c>
+      <c r="C2" s="104"/>
+      <c r="D2" s="104"/>
+      <c r="E2" s="104"/>
+      <c r="F2" s="104"/>
+      <c r="G2" s="104"/>
+      <c r="H2" s="104"/>
+    </row>
+    <row r="3" spans="2:8" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="104"/>
+      <c r="C3" s="104"/>
+      <c r="D3" s="104"/>
+      <c r="E3" s="104"/>
+      <c r="F3" s="104"/>
+      <c r="G3" s="104"/>
+      <c r="H3" s="104"/>
+    </row>
+    <row r="5" spans="2:8" ht="27" x14ac:dyDescent="0.25">
+      <c r="B5" s="100" t="s">
+        <v>218</v>
+      </c>
+      <c r="C5" s="100" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="8"/>
+      <c r="C6" s="9"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:H3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:H6"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="P42" sqref="P42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.85546875" customWidth="1"/>
+    <col min="2" max="2" width="38.7109375" customWidth="1"/>
+    <col min="3" max="3" width="26.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:8" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B1" s="46" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="2:8" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="104" t="s">
+        <v>219</v>
+      </c>
+      <c r="C2" s="104"/>
+      <c r="D2" s="104"/>
+      <c r="E2" s="104"/>
+      <c r="F2" s="104"/>
+      <c r="G2" s="104"/>
+      <c r="H2" s="104"/>
+    </row>
+    <row r="3" spans="2:8" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="104"/>
+      <c r="C3" s="104"/>
+      <c r="D3" s="104"/>
+      <c r="E3" s="104"/>
+      <c r="F3" s="104"/>
+      <c r="G3" s="104"/>
+      <c r="H3" s="104"/>
+    </row>
+    <row r="5" spans="2:8" ht="27" x14ac:dyDescent="0.25">
+      <c r="B5" s="100" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="100" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="8"/>
+      <c r="C6" s="9"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:H3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:H6"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
@@ -6502,7 +6665,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H6"/>
   <sheetViews>
@@ -6573,11 +6736,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H6"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -6644,7 +6807,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:Z8"/>
   <sheetViews>
@@ -6778,7 +6941,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:Z8"/>
   <sheetViews>
@@ -6907,7 +7070,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:Z8"/>
   <sheetViews>
@@ -7032,7 +7195,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:Z8"/>
   <sheetViews>
@@ -7162,7 +7325,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:Q7"/>
   <sheetViews>
@@ -7329,7 +7492,97 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:M7"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.85546875" customWidth="1"/>
+    <col min="2" max="2" width="35.5703125" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:13" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B1" s="46" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="2:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="103" t="s">
+        <v>242</v>
+      </c>
+      <c r="C2" s="103"/>
+      <c r="D2" s="103"/>
+      <c r="E2" s="103"/>
+      <c r="F2" s="103"/>
+      <c r="G2" s="103"/>
+      <c r="H2" s="103"/>
+      <c r="I2" s="103"/>
+      <c r="J2" s="103"/>
+      <c r="K2" s="103"/>
+      <c r="L2" s="103"/>
+    </row>
+    <row r="3" spans="2:13" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="104" t="s">
+        <v>241</v>
+      </c>
+      <c r="C3" s="104"/>
+      <c r="D3" s="104"/>
+      <c r="E3" s="104"/>
+      <c r="F3" s="104"/>
+      <c r="G3" s="104"/>
+      <c r="H3" s="104"/>
+      <c r="I3" s="104"/>
+      <c r="J3" s="104"/>
+      <c r="K3" s="104"/>
+      <c r="L3" s="104"/>
+      <c r="M3" s="104"/>
+    </row>
+    <row r="4" spans="2:13" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="102"/>
+      <c r="C4" s="102"/>
+      <c r="D4" s="102"/>
+      <c r="E4" s="102"/>
+      <c r="F4" s="102"/>
+      <c r="G4" s="102"/>
+      <c r="H4" s="102"/>
+      <c r="I4" s="102"/>
+      <c r="J4" s="102"/>
+      <c r="K4" s="102"/>
+      <c r="L4" s="102"/>
+      <c r="M4" s="102"/>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B5" s="70"/>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B6" s="70" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B7" s="8"/>
+      <c r="C7" s="9"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:L2"/>
+    <mergeCell ref="B3:M3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:Y8"/>
   <sheetViews>
@@ -7410,70 +7663,70 @@
       <c r="R3" s="57"/>
     </row>
     <row r="5" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B5" s="117" t="s">
+      <c r="B5" s="113" t="s">
         <v>109</v>
       </c>
-      <c r="C5" s="118"/>
-      <c r="D5" s="118"/>
-      <c r="E5" s="118"/>
-      <c r="F5" s="118"/>
-      <c r="G5" s="118"/>
-      <c r="H5" s="118"/>
-      <c r="I5" s="118"/>
-      <c r="J5" s="118"/>
-      <c r="K5" s="118"/>
-      <c r="L5" s="119"/>
-      <c r="M5" s="117" t="s">
+      <c r="C5" s="114"/>
+      <c r="D5" s="114"/>
+      <c r="E5" s="114"/>
+      <c r="F5" s="114"/>
+      <c r="G5" s="114"/>
+      <c r="H5" s="114"/>
+      <c r="I5" s="114"/>
+      <c r="J5" s="114"/>
+      <c r="K5" s="114"/>
+      <c r="L5" s="115"/>
+      <c r="M5" s="113" t="s">
         <v>110</v>
       </c>
-      <c r="N5" s="118"/>
-      <c r="O5" s="118"/>
-      <c r="P5" s="118"/>
-      <c r="Q5" s="118"/>
-      <c r="R5" s="118"/>
-      <c r="S5" s="118"/>
-      <c r="T5" s="118"/>
-      <c r="U5" s="118"/>
-      <c r="V5" s="118"/>
-      <c r="W5" s="118"/>
-      <c r="X5" s="118"/>
-      <c r="Y5" s="119"/>
+      <c r="N5" s="114"/>
+      <c r="O5" s="114"/>
+      <c r="P5" s="114"/>
+      <c r="Q5" s="114"/>
+      <c r="R5" s="114"/>
+      <c r="S5" s="114"/>
+      <c r="T5" s="114"/>
+      <c r="U5" s="114"/>
+      <c r="V5" s="114"/>
+      <c r="W5" s="114"/>
+      <c r="X5" s="114"/>
+      <c r="Y5" s="115"/>
     </row>
     <row r="6" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B6" s="116"/>
-      <c r="C6" s="116"/>
-      <c r="D6" s="116"/>
-      <c r="E6" s="116"/>
-      <c r="F6" s="123" t="s">
+      <c r="B6" s="122"/>
+      <c r="C6" s="122"/>
+      <c r="D6" s="122"/>
+      <c r="E6" s="122"/>
+      <c r="F6" s="116" t="s">
         <v>26</v>
       </c>
-      <c r="G6" s="124"/>
-      <c r="H6" s="124"/>
-      <c r="I6" s="125"/>
-      <c r="J6" s="117" t="s">
+      <c r="G6" s="117"/>
+      <c r="H6" s="117"/>
+      <c r="I6" s="118"/>
+      <c r="J6" s="113" t="s">
         <v>29</v>
       </c>
-      <c r="K6" s="118"/>
-      <c r="L6" s="119"/>
+      <c r="K6" s="114"/>
+      <c r="L6" s="115"/>
       <c r="M6" s="87"/>
-      <c r="N6" s="113" t="s">
+      <c r="N6" s="119" t="s">
         <v>41</v>
       </c>
-      <c r="O6" s="115"/>
-      <c r="P6" s="113" t="s">
+      <c r="O6" s="120"/>
+      <c r="P6" s="119" t="s">
         <v>103</v>
       </c>
-      <c r="Q6" s="114"/>
-      <c r="R6" s="115"/>
+      <c r="Q6" s="121"/>
+      <c r="R6" s="120"/>
       <c r="S6" s="87"/>
-      <c r="T6" s="113" t="s">
+      <c r="T6" s="119" t="s">
         <v>120</v>
       </c>
-      <c r="U6" s="115"/>
-      <c r="V6" s="120"/>
-      <c r="W6" s="121"/>
-      <c r="X6" s="121"/>
-      <c r="Y6" s="122"/>
+      <c r="U6" s="120"/>
+      <c r="V6" s="123"/>
+      <c r="W6" s="124"/>
+      <c r="X6" s="124"/>
+      <c r="Y6" s="125"/>
     </row>
     <row r="7" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B7" s="75" t="s">
@@ -7577,9 +7830,6 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="N6:O6"/>
-    <mergeCell ref="P6:R6"/>
-    <mergeCell ref="B6:E6"/>
     <mergeCell ref="T6:U6"/>
     <mergeCell ref="M5:Y5"/>
     <mergeCell ref="V6:Y6"/>
@@ -7588,13 +7838,16 @@
     <mergeCell ref="B5:L5"/>
     <mergeCell ref="J6:L6"/>
     <mergeCell ref="F6:I6"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="P6:R6"/>
+    <mergeCell ref="B6:E6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A24"/>
   <sheetViews>
@@ -7679,96 +7932,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:M7"/>
-  <sheetViews>
-    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="2.85546875" customWidth="1"/>
-    <col min="2" max="2" width="35.5703125" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:13" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="46" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="2" spans="2:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="103" t="s">
-        <v>242</v>
-      </c>
-      <c r="C2" s="103"/>
-      <c r="D2" s="103"/>
-      <c r="E2" s="103"/>
-      <c r="F2" s="103"/>
-      <c r="G2" s="103"/>
-      <c r="H2" s="103"/>
-      <c r="I2" s="103"/>
-      <c r="J2" s="103"/>
-      <c r="K2" s="103"/>
-      <c r="L2" s="103"/>
-    </row>
-    <row r="3" spans="2:13" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="104" t="s">
-        <v>241</v>
-      </c>
-      <c r="C3" s="104"/>
-      <c r="D3" s="104"/>
-      <c r="E3" s="104"/>
-      <c r="F3" s="104"/>
-      <c r="G3" s="104"/>
-      <c r="H3" s="104"/>
-      <c r="I3" s="104"/>
-      <c r="J3" s="104"/>
-      <c r="K3" s="104"/>
-      <c r="L3" s="104"/>
-      <c r="M3" s="104"/>
-    </row>
-    <row r="4" spans="2:13" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="102"/>
-      <c r="C4" s="102"/>
-      <c r="D4" s="102"/>
-      <c r="E4" s="102"/>
-      <c r="F4" s="102"/>
-      <c r="G4" s="102"/>
-      <c r="H4" s="102"/>
-      <c r="I4" s="102"/>
-      <c r="J4" s="102"/>
-      <c r="K4" s="102"/>
-      <c r="L4" s="102"/>
-      <c r="M4" s="102"/>
-    </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B5" s="70"/>
-    </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B6" s="70" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B7" s="8"/>
-      <c r="C7" s="9"/>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B2:L2"/>
-    <mergeCell ref="B3:M3"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
TRIEDA-1724 - Alterando template da exportação do resumo por campus
</commit_message>
<xml_diff>
--- a/code/client/web/src/main/resources/templateExport.xlsx
+++ b/code/client/web/src/main/resources/templateExport.xlsx
@@ -59,7 +59,7 @@
     <sheet name="Aulas" sheetId="26" r:id="rId50"/>
     <sheet name="PaletaCores" sheetId="11" r:id="rId51"/>
   </sheets>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -1422,7 +1422,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="255">
   <si>
     <t>Planilha de Unidades</t>
   </si>
@@ -2203,16 +2203,38 @@
   <si>
     <t>Planilha de Resumo por Campus</t>
   </si>
+  <si>
+    <t>Gerais</t>
+  </si>
+  <si>
+    <t>Eficiência de Alocação</t>
+  </si>
+  <si>
+    <t>Financeiro</t>
+  </si>
+  <si>
+    <t>Uso dos Ambientes</t>
+  </si>
+  <si>
+    <t>Uso dos Docentes</t>
+  </si>
+  <si>
+    <t>Da Instituição</t>
+  </si>
+  <si>
+    <t>Virtuais</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="3">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="&quot;R$&quot;\ #,##0.00"/>
     <numFmt numFmtId="178" formatCode="#,##0.0000"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2339,8 +2361,33 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="29">
+  <fills count="39">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2509,8 +2556,68 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -2611,6 +2718,15 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -2638,12 +2754,147 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="128">
+  <cellXfs count="191">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2799,7 +3050,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="10" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="10" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2864,7 +3115,7 @@
     <xf numFmtId="0" fontId="11" fillId="28" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="10" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="10" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2873,7 +3124,7 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -2899,13 +3150,13 @@
     <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="10" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="10" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="10" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="10" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="10" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="10" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2935,6 +3186,127 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="30" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="30" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="30" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="30" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="31" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="31" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="31" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="31" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="31" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2947,6 +3319,54 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="36" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="37" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="38" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="35" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="35" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2956,7 +3376,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2965,55 +3385,50 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="28" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="28" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -3023,6 +3438,66 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="71684" name=":0_674" descr="https://plus.google.com/u/0/_/focus/photos/private/AIbEiAIAAABDCK-Xzbi8pY7DeSILdmNhcmRfcGhvdG8qKDIxMGNjNTM3ZWQ4NjZjNTU4NTk4YjQ0ZDUwM2EwNmUxOGE4OTQyMTIwAdCjuGFdYwQCNlcR6WXw_rsQlR6Q?sz=32"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1371600" y="8401050"/>
+          <a:ext cx="457200" cy="295275"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3334,28 +3809,28 @@
       </c>
     </row>
     <row r="2" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="103"/>
-      <c r="C2" s="103"/>
-      <c r="D2" s="103"/>
-      <c r="E2" s="103"/>
-      <c r="F2" s="103"/>
-      <c r="G2" s="103"/>
-      <c r="H2" s="103"/>
-      <c r="I2" s="103"/>
+      <c r="B2" s="152"/>
+      <c r="C2" s="152"/>
+      <c r="D2" s="152"/>
+      <c r="E2" s="152"/>
+      <c r="F2" s="152"/>
+      <c r="G2" s="152"/>
+      <c r="H2" s="152"/>
+      <c r="I2" s="152"/>
     </row>
     <row r="3" spans="2:11" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="104" t="s">
+      <c r="B3" s="153" t="s">
         <v>227</v>
       </c>
-      <c r="C3" s="104"/>
-      <c r="D3" s="104"/>
-      <c r="E3" s="104"/>
-      <c r="F3" s="104"/>
-      <c r="G3" s="104"/>
-      <c r="H3" s="104"/>
-      <c r="I3" s="104"/>
-      <c r="J3" s="104"/>
-      <c r="K3" s="104"/>
+      <c r="C3" s="153"/>
+      <c r="D3" s="153"/>
+      <c r="E3" s="153"/>
+      <c r="F3" s="153"/>
+      <c r="G3" s="153"/>
+      <c r="H3" s="153"/>
+      <c r="I3" s="153"/>
+      <c r="J3" s="153"/>
+      <c r="K3" s="153"/>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" s="44" t="s">
@@ -3402,40 +3877,40 @@
       </c>
     </row>
     <row r="2" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="103"/>
-      <c r="C2" s="103"/>
-      <c r="D2" s="103"/>
-      <c r="E2" s="103"/>
-      <c r="F2" s="103"/>
-      <c r="G2" s="103"/>
-      <c r="H2" s="103"/>
-      <c r="I2" s="103"/>
-      <c r="J2" s="103"/>
-      <c r="K2" s="103"/>
-      <c r="L2" s="103"/>
-      <c r="M2" s="103"/>
-      <c r="N2" s="103"/>
-      <c r="O2" s="103"/>
-      <c r="P2" s="103"/>
+      <c r="B2" s="152"/>
+      <c r="C2" s="152"/>
+      <c r="D2" s="152"/>
+      <c r="E2" s="152"/>
+      <c r="F2" s="152"/>
+      <c r="G2" s="152"/>
+      <c r="H2" s="152"/>
+      <c r="I2" s="152"/>
+      <c r="J2" s="152"/>
+      <c r="K2" s="152"/>
+      <c r="L2" s="152"/>
+      <c r="M2" s="152"/>
+      <c r="N2" s="152"/>
+      <c r="O2" s="152"/>
+      <c r="P2" s="152"/>
     </row>
     <row r="3" spans="2:16" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="104" t="s">
+      <c r="B3" s="153" t="s">
         <v>67</v>
       </c>
-      <c r="C3" s="104"/>
-      <c r="D3" s="104"/>
-      <c r="E3" s="104"/>
-      <c r="F3" s="104"/>
-      <c r="G3" s="104"/>
-      <c r="H3" s="104"/>
-      <c r="I3" s="104"/>
-      <c r="J3" s="104"/>
-      <c r="K3" s="104"/>
-      <c r="L3" s="104"/>
-      <c r="M3" s="104"/>
-      <c r="N3" s="104"/>
-      <c r="O3" s="104"/>
-      <c r="P3" s="104"/>
+      <c r="C3" s="153"/>
+      <c r="D3" s="153"/>
+      <c r="E3" s="153"/>
+      <c r="F3" s="153"/>
+      <c r="G3" s="153"/>
+      <c r="H3" s="153"/>
+      <c r="I3" s="153"/>
+      <c r="J3" s="153"/>
+      <c r="K3" s="153"/>
+      <c r="L3" s="153"/>
+      <c r="M3" s="153"/>
+      <c r="N3" s="153"/>
+      <c r="O3" s="153"/>
+      <c r="P3" s="153"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
@@ -3484,40 +3959,40 @@
       </c>
     </row>
     <row r="2" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="103"/>
-      <c r="C2" s="103"/>
-      <c r="D2" s="103"/>
-      <c r="E2" s="103"/>
-      <c r="F2" s="103"/>
-      <c r="G2" s="103"/>
-      <c r="H2" s="103"/>
-      <c r="I2" s="103"/>
-      <c r="J2" s="103"/>
-      <c r="K2" s="103"/>
-      <c r="L2" s="103"/>
-      <c r="M2" s="103"/>
-      <c r="N2" s="103"/>
-      <c r="O2" s="103"/>
-      <c r="P2" s="103"/>
+      <c r="B2" s="152"/>
+      <c r="C2" s="152"/>
+      <c r="D2" s="152"/>
+      <c r="E2" s="152"/>
+      <c r="F2" s="152"/>
+      <c r="G2" s="152"/>
+      <c r="H2" s="152"/>
+      <c r="I2" s="152"/>
+      <c r="J2" s="152"/>
+      <c r="K2" s="152"/>
+      <c r="L2" s="152"/>
+      <c r="M2" s="152"/>
+      <c r="N2" s="152"/>
+      <c r="O2" s="152"/>
+      <c r="P2" s="152"/>
     </row>
     <row r="3" spans="2:16" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="104" t="s">
+      <c r="B3" s="153" t="s">
         <v>70</v>
       </c>
-      <c r="C3" s="104"/>
-      <c r="D3" s="104"/>
-      <c r="E3" s="104"/>
-      <c r="F3" s="104"/>
-      <c r="G3" s="104"/>
-      <c r="H3" s="104"/>
-      <c r="I3" s="104"/>
-      <c r="J3" s="104"/>
-      <c r="K3" s="104"/>
-      <c r="L3" s="104"/>
-      <c r="M3" s="104"/>
-      <c r="N3" s="104"/>
-      <c r="O3" s="104"/>
-      <c r="P3" s="104"/>
+      <c r="C3" s="153"/>
+      <c r="D3" s="153"/>
+      <c r="E3" s="153"/>
+      <c r="F3" s="153"/>
+      <c r="G3" s="153"/>
+      <c r="H3" s="153"/>
+      <c r="I3" s="153"/>
+      <c r="J3" s="153"/>
+      <c r="K3" s="153"/>
+      <c r="L3" s="153"/>
+      <c r="M3" s="153"/>
+      <c r="N3" s="153"/>
+      <c r="O3" s="153"/>
+      <c r="P3" s="153"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
@@ -3572,40 +4047,40 @@
       </c>
     </row>
     <row r="2" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="103"/>
-      <c r="C2" s="103"/>
-      <c r="D2" s="103"/>
-      <c r="E2" s="103"/>
-      <c r="F2" s="103"/>
-      <c r="G2" s="103"/>
-      <c r="H2" s="103"/>
-      <c r="I2" s="103"/>
-      <c r="J2" s="103"/>
-      <c r="K2" s="103"/>
-      <c r="L2" s="103"/>
-      <c r="M2" s="103"/>
-      <c r="N2" s="103"/>
-      <c r="O2" s="103"/>
-      <c r="P2" s="103"/>
+      <c r="B2" s="152"/>
+      <c r="C2" s="152"/>
+      <c r="D2" s="152"/>
+      <c r="E2" s="152"/>
+      <c r="F2" s="152"/>
+      <c r="G2" s="152"/>
+      <c r="H2" s="152"/>
+      <c r="I2" s="152"/>
+      <c r="J2" s="152"/>
+      <c r="K2" s="152"/>
+      <c r="L2" s="152"/>
+      <c r="M2" s="152"/>
+      <c r="N2" s="152"/>
+      <c r="O2" s="152"/>
+      <c r="P2" s="152"/>
     </row>
     <row r="3" spans="2:16" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="104" t="s">
+      <c r="B3" s="153" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="104"/>
-      <c r="D3" s="104"/>
-      <c r="E3" s="104"/>
-      <c r="F3" s="104"/>
-      <c r="G3" s="104"/>
-      <c r="H3" s="104"/>
-      <c r="I3" s="104"/>
-      <c r="J3" s="104"/>
-      <c r="K3" s="104"/>
-      <c r="L3" s="104"/>
-      <c r="M3" s="104"/>
-      <c r="N3" s="104"/>
-      <c r="O3" s="104"/>
-      <c r="P3" s="104"/>
+      <c r="C3" s="153"/>
+      <c r="D3" s="153"/>
+      <c r="E3" s="153"/>
+      <c r="F3" s="153"/>
+      <c r="G3" s="153"/>
+      <c r="H3" s="153"/>
+      <c r="I3" s="153"/>
+      <c r="J3" s="153"/>
+      <c r="K3" s="153"/>
+      <c r="L3" s="153"/>
+      <c r="M3" s="153"/>
+      <c r="N3" s="153"/>
+      <c r="O3" s="153"/>
+      <c r="P3" s="153"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="44" t="s">
@@ -3695,16 +4170,16 @@
       </c>
     </row>
     <row r="2" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="103"/>
-      <c r="C2" s="103"/>
-      <c r="D2" s="103"/>
-      <c r="E2" s="103"/>
-      <c r="F2" s="103"/>
-      <c r="G2" s="103"/>
-      <c r="H2" s="103"/>
-      <c r="I2" s="103"/>
-      <c r="J2" s="103"/>
-      <c r="K2" s="103"/>
+      <c r="B2" s="152"/>
+      <c r="C2" s="152"/>
+      <c r="D2" s="152"/>
+      <c r="E2" s="152"/>
+      <c r="F2" s="152"/>
+      <c r="G2" s="152"/>
+      <c r="H2" s="152"/>
+      <c r="I2" s="152"/>
+      <c r="J2" s="152"/>
+      <c r="K2" s="152"/>
     </row>
     <row r="3" spans="2:11" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="82" t="s">
@@ -3794,40 +4269,40 @@
       </c>
     </row>
     <row r="2" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="103"/>
-      <c r="C2" s="103"/>
-      <c r="D2" s="103"/>
-      <c r="E2" s="103"/>
-      <c r="F2" s="103"/>
-      <c r="G2" s="103"/>
-      <c r="H2" s="103"/>
-      <c r="I2" s="103"/>
-      <c r="J2" s="103"/>
-      <c r="K2" s="103"/>
-      <c r="L2" s="103"/>
-      <c r="M2" s="103"/>
-      <c r="N2" s="103"/>
-      <c r="O2" s="103"/>
-      <c r="P2" s="103"/>
+      <c r="B2" s="152"/>
+      <c r="C2" s="152"/>
+      <c r="D2" s="152"/>
+      <c r="E2" s="152"/>
+      <c r="F2" s="152"/>
+      <c r="G2" s="152"/>
+      <c r="H2" s="152"/>
+      <c r="I2" s="152"/>
+      <c r="J2" s="152"/>
+      <c r="K2" s="152"/>
+      <c r="L2" s="152"/>
+      <c r="M2" s="152"/>
+      <c r="N2" s="152"/>
+      <c r="O2" s="152"/>
+      <c r="P2" s="152"/>
     </row>
     <row r="3" spans="2:16" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="104" t="s">
+      <c r="B3" s="153" t="s">
         <v>64</v>
       </c>
-      <c r="C3" s="104"/>
-      <c r="D3" s="104"/>
-      <c r="E3" s="104"/>
-      <c r="F3" s="104"/>
-      <c r="G3" s="104"/>
-      <c r="H3" s="104"/>
-      <c r="I3" s="104"/>
-      <c r="J3" s="104"/>
-      <c r="K3" s="104"/>
-      <c r="L3" s="104"/>
-      <c r="M3" s="104"/>
-      <c r="N3" s="104"/>
-      <c r="O3" s="104"/>
-      <c r="P3" s="104"/>
+      <c r="C3" s="153"/>
+      <c r="D3" s="153"/>
+      <c r="E3" s="153"/>
+      <c r="F3" s="153"/>
+      <c r="G3" s="153"/>
+      <c r="H3" s="153"/>
+      <c r="I3" s="153"/>
+      <c r="J3" s="153"/>
+      <c r="K3" s="153"/>
+      <c r="L3" s="153"/>
+      <c r="M3" s="153"/>
+      <c r="N3" s="153"/>
+      <c r="O3" s="153"/>
+      <c r="P3" s="153"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="45" t="s">
@@ -3882,28 +4357,28 @@
       </c>
     </row>
     <row r="2" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="105"/>
-      <c r="C2" s="105"/>
-      <c r="D2" s="105"/>
-      <c r="E2" s="105"/>
-      <c r="F2" s="105"/>
-      <c r="G2" s="105"/>
-      <c r="H2" s="105"/>
-      <c r="I2" s="105"/>
+      <c r="B2" s="154"/>
+      <c r="C2" s="154"/>
+      <c r="D2" s="154"/>
+      <c r="E2" s="154"/>
+      <c r="F2" s="154"/>
+      <c r="G2" s="154"/>
+      <c r="H2" s="154"/>
+      <c r="I2" s="154"/>
       <c r="J2" s="83"/>
       <c r="K2" s="83"/>
     </row>
     <row r="3" spans="2:11" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="104" t="s">
+      <c r="B3" s="153" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="104"/>
-      <c r="D3" s="104"/>
-      <c r="E3" s="104"/>
-      <c r="F3" s="104"/>
-      <c r="G3" s="104"/>
-      <c r="H3" s="104"/>
-      <c r="I3" s="104"/>
+      <c r="C3" s="153"/>
+      <c r="D3" s="153"/>
+      <c r="E3" s="153"/>
+      <c r="F3" s="153"/>
+      <c r="G3" s="153"/>
+      <c r="H3" s="153"/>
+      <c r="I3" s="153"/>
       <c r="J3" s="82"/>
       <c r="K3" s="82"/>
     </row>
@@ -3958,36 +4433,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="103"/>
-      <c r="C2" s="103"/>
-      <c r="D2" s="103"/>
-      <c r="E2" s="103"/>
-      <c r="F2" s="103"/>
-      <c r="G2" s="103"/>
-      <c r="H2" s="103"/>
-      <c r="I2" s="103"/>
-      <c r="J2" s="103"/>
-      <c r="K2" s="103"/>
-      <c r="L2" s="103"/>
-      <c r="M2" s="103"/>
-      <c r="N2" s="103"/>
+      <c r="B2" s="152"/>
+      <c r="C2" s="152"/>
+      <c r="D2" s="152"/>
+      <c r="E2" s="152"/>
+      <c r="F2" s="152"/>
+      <c r="G2" s="152"/>
+      <c r="H2" s="152"/>
+      <c r="I2" s="152"/>
+      <c r="J2" s="152"/>
+      <c r="K2" s="152"/>
+      <c r="L2" s="152"/>
+      <c r="M2" s="152"/>
+      <c r="N2" s="152"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="104" t="s">
+      <c r="B3" s="153" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="104"/>
-      <c r="D3" s="104"/>
-      <c r="E3" s="104"/>
-      <c r="F3" s="104"/>
-      <c r="G3" s="104"/>
-      <c r="H3" s="104"/>
-      <c r="I3" s="104"/>
-      <c r="J3" s="104"/>
-      <c r="K3" s="104"/>
-      <c r="L3" s="104"/>
-      <c r="M3" s="104"/>
-      <c r="N3" s="104"/>
+      <c r="C3" s="153"/>
+      <c r="D3" s="153"/>
+      <c r="E3" s="153"/>
+      <c r="F3" s="153"/>
+      <c r="G3" s="153"/>
+      <c r="H3" s="153"/>
+      <c r="I3" s="153"/>
+      <c r="J3" s="153"/>
+      <c r="K3" s="153"/>
+      <c r="L3" s="153"/>
+      <c r="M3" s="153"/>
+      <c r="N3" s="153"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -4054,32 +4529,32 @@
       </c>
     </row>
     <row r="2" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="103"/>
-      <c r="C2" s="103"/>
-      <c r="D2" s="103"/>
-      <c r="E2" s="103"/>
-      <c r="F2" s="103"/>
-      <c r="G2" s="103"/>
-      <c r="H2" s="103"/>
-      <c r="I2" s="103"/>
-      <c r="J2" s="103"/>
-      <c r="K2" s="103"/>
-      <c r="L2" s="103"/>
+      <c r="B2" s="152"/>
+      <c r="C2" s="152"/>
+      <c r="D2" s="152"/>
+      <c r="E2" s="152"/>
+      <c r="F2" s="152"/>
+      <c r="G2" s="152"/>
+      <c r="H2" s="152"/>
+      <c r="I2" s="152"/>
+      <c r="J2" s="152"/>
+      <c r="K2" s="152"/>
+      <c r="L2" s="152"/>
     </row>
     <row r="3" spans="2:12" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="104" t="s">
+      <c r="B3" s="153" t="s">
         <v>198</v>
       </c>
-      <c r="C3" s="104"/>
-      <c r="D3" s="104"/>
-      <c r="E3" s="104"/>
-      <c r="F3" s="104"/>
-      <c r="G3" s="104"/>
-      <c r="H3" s="104"/>
-      <c r="I3" s="104"/>
-      <c r="J3" s="104"/>
-      <c r="K3" s="104"/>
-      <c r="L3" s="104"/>
+      <c r="C3" s="153"/>
+      <c r="D3" s="153"/>
+      <c r="E3" s="153"/>
+      <c r="F3" s="153"/>
+      <c r="G3" s="153"/>
+      <c r="H3" s="153"/>
+      <c r="I3" s="153"/>
+      <c r="J3" s="153"/>
+      <c r="K3" s="153"/>
+      <c r="L3" s="153"/>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B5" s="70" t="s">
@@ -4138,32 +4613,32 @@
       </c>
     </row>
     <row r="2" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="103"/>
-      <c r="C2" s="103"/>
-      <c r="D2" s="103"/>
-      <c r="E2" s="103"/>
-      <c r="F2" s="103"/>
-      <c r="G2" s="103"/>
-      <c r="H2" s="103"/>
-      <c r="I2" s="103"/>
-      <c r="J2" s="103"/>
-      <c r="K2" s="103"/>
-      <c r="L2" s="103"/>
+      <c r="B2" s="152"/>
+      <c r="C2" s="152"/>
+      <c r="D2" s="152"/>
+      <c r="E2" s="152"/>
+      <c r="F2" s="152"/>
+      <c r="G2" s="152"/>
+      <c r="H2" s="152"/>
+      <c r="I2" s="152"/>
+      <c r="J2" s="152"/>
+      <c r="K2" s="152"/>
+      <c r="L2" s="152"/>
     </row>
     <row r="3" spans="2:12" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="104" t="s">
+      <c r="B3" s="153" t="s">
         <v>201</v>
       </c>
-      <c r="C3" s="104"/>
-      <c r="D3" s="104"/>
-      <c r="E3" s="104"/>
-      <c r="F3" s="104"/>
-      <c r="G3" s="104"/>
-      <c r="H3" s="104"/>
-      <c r="I3" s="104"/>
-      <c r="J3" s="104"/>
-      <c r="K3" s="104"/>
-      <c r="L3" s="104"/>
+      <c r="C3" s="153"/>
+      <c r="D3" s="153"/>
+      <c r="E3" s="153"/>
+      <c r="F3" s="153"/>
+      <c r="G3" s="153"/>
+      <c r="H3" s="153"/>
+      <c r="I3" s="153"/>
+      <c r="J3" s="153"/>
+      <c r="K3" s="153"/>
+      <c r="L3" s="153"/>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B5" s="70" t="s">
@@ -4222,32 +4697,32 @@
       </c>
     </row>
     <row r="2" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="103"/>
-      <c r="C2" s="103"/>
-      <c r="D2" s="103"/>
-      <c r="E2" s="103"/>
-      <c r="F2" s="103"/>
-      <c r="G2" s="103"/>
-      <c r="H2" s="103"/>
-      <c r="I2" s="103"/>
-      <c r="J2" s="103"/>
-      <c r="K2" s="103"/>
-      <c r="L2" s="103"/>
+      <c r="B2" s="152"/>
+      <c r="C2" s="152"/>
+      <c r="D2" s="152"/>
+      <c r="E2" s="152"/>
+      <c r="F2" s="152"/>
+      <c r="G2" s="152"/>
+      <c r="H2" s="152"/>
+      <c r="I2" s="152"/>
+      <c r="J2" s="152"/>
+      <c r="K2" s="152"/>
+      <c r="L2" s="152"/>
     </row>
     <row r="3" spans="2:12" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="104" t="s">
+      <c r="B3" s="153" t="s">
         <v>202</v>
       </c>
-      <c r="C3" s="104"/>
-      <c r="D3" s="104"/>
-      <c r="E3" s="104"/>
-      <c r="F3" s="104"/>
-      <c r="G3" s="104"/>
-      <c r="H3" s="104"/>
-      <c r="I3" s="104"/>
-      <c r="J3" s="104"/>
-      <c r="K3" s="104"/>
-      <c r="L3" s="104"/>
+      <c r="C3" s="153"/>
+      <c r="D3" s="153"/>
+      <c r="E3" s="153"/>
+      <c r="F3" s="153"/>
+      <c r="G3" s="153"/>
+      <c r="H3" s="153"/>
+      <c r="I3" s="153"/>
+      <c r="J3" s="153"/>
+      <c r="K3" s="153"/>
+      <c r="L3" s="153"/>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B5" s="70" t="s">
@@ -4312,38 +4787,38 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="103" t="s">
+      <c r="B2" s="152" t="s">
         <v>93</v>
       </c>
-      <c r="C2" s="103"/>
-      <c r="D2" s="103"/>
-      <c r="E2" s="103"/>
-      <c r="F2" s="103"/>
-      <c r="G2" s="103"/>
-      <c r="H2" s="103"/>
-      <c r="I2" s="103"/>
-      <c r="J2" s="103"/>
-      <c r="K2" s="103"/>
-      <c r="L2" s="103"/>
-      <c r="M2" s="103"/>
-      <c r="N2" s="103"/>
+      <c r="C2" s="152"/>
+      <c r="D2" s="152"/>
+      <c r="E2" s="152"/>
+      <c r="F2" s="152"/>
+      <c r="G2" s="152"/>
+      <c r="H2" s="152"/>
+      <c r="I2" s="152"/>
+      <c r="J2" s="152"/>
+      <c r="K2" s="152"/>
+      <c r="L2" s="152"/>
+      <c r="M2" s="152"/>
+      <c r="N2" s="152"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="104" t="s">
+      <c r="B3" s="153" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="104"/>
-      <c r="D3" s="104"/>
-      <c r="E3" s="104"/>
-      <c r="F3" s="104"/>
-      <c r="G3" s="104"/>
-      <c r="H3" s="104"/>
-      <c r="I3" s="104"/>
-      <c r="J3" s="104"/>
-      <c r="K3" s="104"/>
-      <c r="L3" s="104"/>
-      <c r="M3" s="104"/>
-      <c r="N3" s="104"/>
+      <c r="C3" s="153"/>
+      <c r="D3" s="153"/>
+      <c r="E3" s="153"/>
+      <c r="F3" s="153"/>
+      <c r="G3" s="153"/>
+      <c r="H3" s="153"/>
+      <c r="I3" s="153"/>
+      <c r="J3" s="153"/>
+      <c r="K3" s="153"/>
+      <c r="L3" s="153"/>
+      <c r="M3" s="153"/>
+      <c r="N3" s="153"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="44" t="s">
@@ -4413,36 +4888,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="103"/>
-      <c r="C2" s="103"/>
-      <c r="D2" s="103"/>
-      <c r="E2" s="103"/>
-      <c r="F2" s="103"/>
-      <c r="G2" s="103"/>
-      <c r="H2" s="103"/>
-      <c r="I2" s="103"/>
-      <c r="J2" s="103"/>
-      <c r="K2" s="103"/>
-      <c r="L2" s="103"/>
-      <c r="M2" s="103"/>
-      <c r="N2" s="103"/>
+      <c r="B2" s="152"/>
+      <c r="C2" s="152"/>
+      <c r="D2" s="152"/>
+      <c r="E2" s="152"/>
+      <c r="F2" s="152"/>
+      <c r="G2" s="152"/>
+      <c r="H2" s="152"/>
+      <c r="I2" s="152"/>
+      <c r="J2" s="152"/>
+      <c r="K2" s="152"/>
+      <c r="L2" s="152"/>
+      <c r="M2" s="152"/>
+      <c r="N2" s="152"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="104" t="s">
+      <c r="B3" s="153" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="104"/>
-      <c r="D3" s="104"/>
-      <c r="E3" s="104"/>
-      <c r="F3" s="104"/>
-      <c r="G3" s="104"/>
-      <c r="H3" s="104"/>
-      <c r="I3" s="104"/>
-      <c r="J3" s="104"/>
-      <c r="K3" s="104"/>
-      <c r="L3" s="104"/>
-      <c r="M3" s="104"/>
-      <c r="N3" s="104"/>
+      <c r="C3" s="153"/>
+      <c r="D3" s="153"/>
+      <c r="E3" s="153"/>
+      <c r="F3" s="153"/>
+      <c r="G3" s="153"/>
+      <c r="H3" s="153"/>
+      <c r="I3" s="153"/>
+      <c r="J3" s="153"/>
+      <c r="K3" s="153"/>
+      <c r="L3" s="153"/>
+      <c r="M3" s="153"/>
+      <c r="N3" s="153"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -4527,18 +5002,18 @@
       </c>
     </row>
     <row r="2" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="103"/>
-      <c r="C2" s="103"/>
-      <c r="D2" s="103"/>
-      <c r="E2" s="103"/>
+      <c r="B2" s="152"/>
+      <c r="C2" s="152"/>
+      <c r="D2" s="152"/>
+      <c r="E2" s="152"/>
     </row>
     <row r="3" spans="2:5" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="104" t="s">
+      <c r="B3" s="153" t="s">
         <v>123</v>
       </c>
-      <c r="C3" s="104"/>
-      <c r="D3" s="104"/>
-      <c r="E3" s="104"/>
+      <c r="C3" s="153"/>
+      <c r="D3" s="153"/>
+      <c r="E3" s="153"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="60" t="s">
@@ -4591,36 +5066,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="103"/>
-      <c r="C2" s="103"/>
-      <c r="D2" s="103"/>
-      <c r="E2" s="103"/>
-      <c r="F2" s="103"/>
-      <c r="G2" s="103"/>
-      <c r="H2" s="103"/>
-      <c r="I2" s="103"/>
-      <c r="J2" s="103"/>
-      <c r="K2" s="103"/>
-      <c r="L2" s="103"/>
-      <c r="M2" s="103"/>
-      <c r="N2" s="103"/>
+      <c r="B2" s="152"/>
+      <c r="C2" s="152"/>
+      <c r="D2" s="152"/>
+      <c r="E2" s="152"/>
+      <c r="F2" s="152"/>
+      <c r="G2" s="152"/>
+      <c r="H2" s="152"/>
+      <c r="I2" s="152"/>
+      <c r="J2" s="152"/>
+      <c r="K2" s="152"/>
+      <c r="L2" s="152"/>
+      <c r="M2" s="152"/>
+      <c r="N2" s="152"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="104" t="s">
+      <c r="B3" s="153" t="s">
         <v>97</v>
       </c>
-      <c r="C3" s="104"/>
-      <c r="D3" s="104"/>
-      <c r="E3" s="104"/>
-      <c r="F3" s="104"/>
-      <c r="G3" s="104"/>
-      <c r="H3" s="104"/>
-      <c r="I3" s="104"/>
-      <c r="J3" s="104"/>
-      <c r="K3" s="104"/>
-      <c r="L3" s="104"/>
-      <c r="M3" s="104"/>
-      <c r="N3" s="104"/>
+      <c r="C3" s="153"/>
+      <c r="D3" s="153"/>
+      <c r="E3" s="153"/>
+      <c r="F3" s="153"/>
+      <c r="G3" s="153"/>
+      <c r="H3" s="153"/>
+      <c r="I3" s="153"/>
+      <c r="J3" s="153"/>
+      <c r="K3" s="153"/>
+      <c r="L3" s="153"/>
+      <c r="M3" s="153"/>
+      <c r="N3" s="153"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -4653,10 +5128,10 @@
       <c r="K5" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="L5" s="106" t="s">
+      <c r="L5" s="155" t="s">
         <v>107</v>
       </c>
-      <c r="M5" s="106"/>
+      <c r="M5" s="155"/>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
@@ -4711,38 +5186,38 @@
       </c>
     </row>
     <row r="2" spans="2:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="103"/>
-      <c r="C2" s="103"/>
-      <c r="D2" s="103"/>
-      <c r="E2" s="103"/>
-      <c r="F2" s="103"/>
-      <c r="G2" s="103"/>
-      <c r="H2" s="103"/>
-      <c r="I2" s="103"/>
-      <c r="J2" s="103"/>
-      <c r="K2" s="103"/>
-      <c r="L2" s="103"/>
-      <c r="M2" s="103"/>
-      <c r="N2" s="103"/>
-      <c r="O2" s="103"/>
+      <c r="B2" s="152"/>
+      <c r="C2" s="152"/>
+      <c r="D2" s="152"/>
+      <c r="E2" s="152"/>
+      <c r="F2" s="152"/>
+      <c r="G2" s="152"/>
+      <c r="H2" s="152"/>
+      <c r="I2" s="152"/>
+      <c r="J2" s="152"/>
+      <c r="K2" s="152"/>
+      <c r="L2" s="152"/>
+      <c r="M2" s="152"/>
+      <c r="N2" s="152"/>
+      <c r="O2" s="152"/>
     </row>
     <row r="3" spans="2:15" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="104" t="s">
+      <c r="B3" s="153" t="s">
         <v>72</v>
       </c>
-      <c r="C3" s="104"/>
-      <c r="D3" s="104"/>
-      <c r="E3" s="104"/>
-      <c r="F3" s="104"/>
-      <c r="G3" s="104"/>
-      <c r="H3" s="104"/>
-      <c r="I3" s="104"/>
-      <c r="J3" s="104"/>
-      <c r="K3" s="104"/>
-      <c r="L3" s="104"/>
-      <c r="M3" s="104"/>
-      <c r="N3" s="104"/>
-      <c r="O3" s="104"/>
+      <c r="C3" s="153"/>
+      <c r="D3" s="153"/>
+      <c r="E3" s="153"/>
+      <c r="F3" s="153"/>
+      <c r="G3" s="153"/>
+      <c r="H3" s="153"/>
+      <c r="I3" s="153"/>
+      <c r="J3" s="153"/>
+      <c r="K3" s="153"/>
+      <c r="L3" s="153"/>
+      <c r="M3" s="153"/>
+      <c r="N3" s="153"/>
+      <c r="O3" s="153"/>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -4829,18 +5304,18 @@
       </c>
     </row>
     <row r="2" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="103"/>
-      <c r="C2" s="103"/>
-      <c r="D2" s="103"/>
-      <c r="E2" s="103"/>
+      <c r="B2" s="152"/>
+      <c r="C2" s="152"/>
+      <c r="D2" s="152"/>
+      <c r="E2" s="152"/>
     </row>
     <row r="3" spans="2:5" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="104" t="s">
+      <c r="B3" s="153" t="s">
         <v>128</v>
       </c>
-      <c r="C3" s="104"/>
-      <c r="D3" s="104"/>
-      <c r="E3" s="104"/>
+      <c r="C3" s="153"/>
+      <c r="D3" s="153"/>
+      <c r="E3" s="153"/>
     </row>
     <row r="4" spans="2:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="64"/>
@@ -4902,36 +5377,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="103"/>
-      <c r="C2" s="103"/>
-      <c r="D2" s="103"/>
-      <c r="E2" s="103"/>
-      <c r="F2" s="103"/>
-      <c r="G2" s="103"/>
-      <c r="H2" s="103"/>
-      <c r="I2" s="103"/>
-      <c r="J2" s="103"/>
-      <c r="K2" s="103"/>
-      <c r="L2" s="103"/>
-      <c r="M2" s="103"/>
-      <c r="N2" s="103"/>
+      <c r="B2" s="152"/>
+      <c r="C2" s="152"/>
+      <c r="D2" s="152"/>
+      <c r="E2" s="152"/>
+      <c r="F2" s="152"/>
+      <c r="G2" s="152"/>
+      <c r="H2" s="152"/>
+      <c r="I2" s="152"/>
+      <c r="J2" s="152"/>
+      <c r="K2" s="152"/>
+      <c r="L2" s="152"/>
+      <c r="M2" s="152"/>
+      <c r="N2" s="152"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="104" t="s">
+      <c r="B3" s="153" t="s">
         <v>68</v>
       </c>
-      <c r="C3" s="104"/>
-      <c r="D3" s="104"/>
-      <c r="E3" s="104"/>
-      <c r="F3" s="104"/>
-      <c r="G3" s="104"/>
-      <c r="H3" s="104"/>
-      <c r="I3" s="104"/>
-      <c r="J3" s="104"/>
-      <c r="K3" s="104"/>
-      <c r="L3" s="104"/>
-      <c r="M3" s="104"/>
-      <c r="N3" s="104"/>
+      <c r="C3" s="153"/>
+      <c r="D3" s="153"/>
+      <c r="E3" s="153"/>
+      <c r="F3" s="153"/>
+      <c r="G3" s="153"/>
+      <c r="H3" s="153"/>
+      <c r="I3" s="153"/>
+      <c r="J3" s="153"/>
+      <c r="K3" s="153"/>
+      <c r="L3" s="153"/>
+      <c r="M3" s="153"/>
+      <c r="N3" s="153"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -4986,36 +5461,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="103"/>
-      <c r="C2" s="103"/>
-      <c r="D2" s="103"/>
-      <c r="E2" s="103"/>
-      <c r="F2" s="103"/>
-      <c r="G2" s="103"/>
-      <c r="H2" s="103"/>
-      <c r="I2" s="103"/>
-      <c r="J2" s="103"/>
-      <c r="K2" s="103"/>
-      <c r="L2" s="103"/>
-      <c r="M2" s="103"/>
-      <c r="N2" s="103"/>
+      <c r="B2" s="152"/>
+      <c r="C2" s="152"/>
+      <c r="D2" s="152"/>
+      <c r="E2" s="152"/>
+      <c r="F2" s="152"/>
+      <c r="G2" s="152"/>
+      <c r="H2" s="152"/>
+      <c r="I2" s="152"/>
+      <c r="J2" s="152"/>
+      <c r="K2" s="152"/>
+      <c r="L2" s="152"/>
+      <c r="M2" s="152"/>
+      <c r="N2" s="152"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="104" t="s">
+      <c r="B3" s="153" t="s">
         <v>73</v>
       </c>
-      <c r="C3" s="104"/>
-      <c r="D3" s="104"/>
-      <c r="E3" s="104"/>
-      <c r="F3" s="104"/>
-      <c r="G3" s="104"/>
-      <c r="H3" s="104"/>
-      <c r="I3" s="104"/>
-      <c r="J3" s="104"/>
-      <c r="K3" s="104"/>
-      <c r="L3" s="104"/>
-      <c r="M3" s="104"/>
-      <c r="N3" s="104"/>
+      <c r="C3" s="153"/>
+      <c r="D3" s="153"/>
+      <c r="E3" s="153"/>
+      <c r="F3" s="153"/>
+      <c r="G3" s="153"/>
+      <c r="H3" s="153"/>
+      <c r="I3" s="153"/>
+      <c r="J3" s="153"/>
+      <c r="K3" s="153"/>
+      <c r="L3" s="153"/>
+      <c r="M3" s="153"/>
+      <c r="N3" s="153"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -5068,48 +5543,48 @@
       </c>
     </row>
     <row r="2" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="105"/>
-      <c r="C2" s="105"/>
-      <c r="D2" s="105"/>
-      <c r="E2" s="105"/>
-      <c r="F2" s="105"/>
-      <c r="G2" s="105"/>
-      <c r="H2" s="105"/>
-      <c r="I2" s="105"/>
-      <c r="J2" s="105"/>
-      <c r="K2" s="105"/>
-      <c r="L2" s="105"/>
-      <c r="M2" s="105"/>
-      <c r="N2" s="105"/>
-      <c r="O2" s="105"/>
-      <c r="P2" s="105"/>
+      <c r="B2" s="154"/>
+      <c r="C2" s="154"/>
+      <c r="D2" s="154"/>
+      <c r="E2" s="154"/>
+      <c r="F2" s="154"/>
+      <c r="G2" s="154"/>
+      <c r="H2" s="154"/>
+      <c r="I2" s="154"/>
+      <c r="J2" s="154"/>
+      <c r="K2" s="154"/>
+      <c r="L2" s="154"/>
+      <c r="M2" s="154"/>
+      <c r="N2" s="154"/>
+      <c r="O2" s="154"/>
+      <c r="P2" s="154"/>
     </row>
     <row r="3" spans="2:16" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="104" t="s">
+      <c r="B3" s="153" t="s">
         <v>246</v>
       </c>
-      <c r="C3" s="104"/>
-      <c r="D3" s="104"/>
-      <c r="E3" s="104"/>
-      <c r="F3" s="104"/>
-      <c r="G3" s="104"/>
-      <c r="H3" s="104"/>
-      <c r="I3" s="104"/>
-      <c r="J3" s="104"/>
-      <c r="K3" s="104"/>
-      <c r="L3" s="104"/>
-      <c r="M3" s="104"/>
-      <c r="N3" s="104"/>
-      <c r="O3" s="104"/>
-      <c r="P3" s="104"/>
+      <c r="C3" s="153"/>
+      <c r="D3" s="153"/>
+      <c r="E3" s="153"/>
+      <c r="F3" s="153"/>
+      <c r="G3" s="153"/>
+      <c r="H3" s="153"/>
+      <c r="I3" s="153"/>
+      <c r="J3" s="153"/>
+      <c r="K3" s="153"/>
+      <c r="L3" s="153"/>
+      <c r="M3" s="153"/>
+      <c r="N3" s="153"/>
+      <c r="O3" s="153"/>
+      <c r="P3" s="153"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B5" s="126" t="s">
+      <c r="B5" s="104" t="s">
         <v>245</v>
       </c>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B6" s="127"/>
+      <c r="B6" s="105"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -5123,16 +5598,19 @@
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:P6"/>
+  <dimension ref="B1:P60"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A55" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="A70" sqref="A61:IV70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.85546875" customWidth="1"/>
-    <col min="2" max="2" width="127.42578125" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="60.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:16" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
@@ -5141,56 +5619,423 @@
       </c>
     </row>
     <row r="2" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="105"/>
-      <c r="C2" s="105"/>
-      <c r="D2" s="105"/>
-      <c r="E2" s="105"/>
-      <c r="F2" s="105"/>
-      <c r="G2" s="105"/>
-      <c r="H2" s="105"/>
-      <c r="I2" s="105"/>
-      <c r="J2" s="105"/>
-      <c r="K2" s="105"/>
-      <c r="L2" s="105"/>
-      <c r="M2" s="105"/>
-      <c r="N2" s="105"/>
-      <c r="O2" s="105"/>
-      <c r="P2" s="105"/>
+      <c r="B2" s="154"/>
+      <c r="C2" s="154"/>
+      <c r="D2" s="154"/>
+      <c r="E2" s="154"/>
+      <c r="F2" s="154"/>
+      <c r="G2" s="154"/>
+      <c r="H2" s="154"/>
+      <c r="I2" s="154"/>
+      <c r="J2" s="154"/>
+      <c r="K2" s="154"/>
+      <c r="L2" s="154"/>
+      <c r="M2" s="154"/>
+      <c r="N2" s="154"/>
+      <c r="O2" s="154"/>
+      <c r="P2" s="154"/>
     </row>
     <row r="3" spans="2:16" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="104" t="s">
+      <c r="B3" s="153" t="s">
         <v>247</v>
       </c>
-      <c r="C3" s="104"/>
-      <c r="D3" s="104"/>
-      <c r="E3" s="104"/>
-      <c r="F3" s="104"/>
-      <c r="G3" s="104"/>
-      <c r="H3" s="104"/>
-      <c r="I3" s="104"/>
-      <c r="J3" s="104"/>
-      <c r="K3" s="104"/>
-      <c r="L3" s="104"/>
-      <c r="M3" s="104"/>
-      <c r="N3" s="104"/>
-      <c r="O3" s="104"/>
-      <c r="P3" s="104"/>
-    </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B5" s="126" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B6" s="127"/>
+      <c r="C3" s="153"/>
+      <c r="D3" s="153"/>
+      <c r="E3" s="153"/>
+      <c r="F3" s="153"/>
+      <c r="G3" s="153"/>
+      <c r="H3" s="153"/>
+      <c r="I3" s="153"/>
+      <c r="J3" s="153"/>
+      <c r="K3" s="153"/>
+      <c r="L3" s="153"/>
+      <c r="M3" s="153"/>
+      <c r="N3" s="153"/>
+      <c r="O3" s="153"/>
+      <c r="P3" s="153"/>
+    </row>
+    <row r="4" spans="2:16" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B4" s="103"/>
+      <c r="C4" s="103"/>
+      <c r="D4" s="103"/>
+      <c r="E4" s="103"/>
+      <c r="F4" s="103"/>
+      <c r="G4" s="103"/>
+      <c r="H4" s="103"/>
+      <c r="I4" s="103"/>
+      <c r="J4" s="103"/>
+      <c r="K4" s="103"/>
+      <c r="L4" s="103"/>
+      <c r="M4" s="103"/>
+      <c r="N4" s="103"/>
+      <c r="O4" s="103"/>
+      <c r="P4" s="103"/>
+    </row>
+    <row r="5" spans="2:16" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E5" s="138"/>
+    </row>
+    <row r="6" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="156" t="s">
+        <v>248</v>
+      </c>
+      <c r="C6" s="106"/>
+      <c r="D6" s="107"/>
+      <c r="E6" s="139"/>
+    </row>
+    <row r="7" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="157"/>
+      <c r="C7" s="108"/>
+      <c r="D7" s="109"/>
+      <c r="E7" s="140"/>
+    </row>
+    <row r="8" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="157"/>
+      <c r="C8" s="108"/>
+      <c r="D8" s="109"/>
+      <c r="E8" s="141"/>
+    </row>
+    <row r="9" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="157"/>
+      <c r="C9" s="108"/>
+      <c r="D9" s="109"/>
+      <c r="E9" s="140"/>
+    </row>
+    <row r="10" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="157"/>
+      <c r="C10" s="108"/>
+      <c r="D10" s="109"/>
+      <c r="E10" s="140"/>
+    </row>
+    <row r="11" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B11" s="157"/>
+      <c r="C11" s="108"/>
+      <c r="D11" s="109"/>
+      <c r="E11" s="140"/>
+    </row>
+    <row r="12" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B12" s="157"/>
+      <c r="C12" s="108"/>
+      <c r="D12" s="109"/>
+      <c r="E12" s="140"/>
+    </row>
+    <row r="13" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B13" s="157"/>
+      <c r="C13" s="108"/>
+      <c r="D13" s="109"/>
+      <c r="E13" s="140"/>
+    </row>
+    <row r="14" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B14" s="157"/>
+      <c r="C14" s="108"/>
+      <c r="D14" s="109"/>
+      <c r="E14" s="140"/>
+    </row>
+    <row r="15" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B15" s="157"/>
+      <c r="C15" s="108"/>
+      <c r="D15" s="109"/>
+      <c r="E15" s="140"/>
+    </row>
+    <row r="16" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B16" s="157"/>
+      <c r="C16" s="108"/>
+      <c r="D16" s="109"/>
+      <c r="E16" s="140"/>
+    </row>
+    <row r="17" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B17" s="157"/>
+      <c r="C17" s="108"/>
+      <c r="D17" s="109"/>
+      <c r="E17" s="140"/>
+    </row>
+    <row r="18" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B18" s="157"/>
+      <c r="C18" s="108"/>
+      <c r="D18" s="109"/>
+      <c r="E18" s="140"/>
+    </row>
+    <row r="19" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B19" s="157"/>
+      <c r="C19" s="108"/>
+      <c r="D19" s="109"/>
+      <c r="E19" s="140"/>
+    </row>
+    <row r="20" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B20" s="157"/>
+      <c r="C20" s="108"/>
+      <c r="D20" s="109"/>
+      <c r="E20" s="140"/>
+    </row>
+    <row r="21" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B21" s="157"/>
+      <c r="C21" s="110"/>
+      <c r="D21" s="111"/>
+      <c r="E21" s="142"/>
+    </row>
+    <row r="22" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B22" s="112"/>
+      <c r="C22" s="112"/>
+      <c r="D22" s="113"/>
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B23" s="158" t="s">
+        <v>249</v>
+      </c>
+      <c r="C23" s="114"/>
+      <c r="D23" s="115"/>
+      <c r="E23" s="143"/>
+    </row>
+    <row r="24" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B24" s="159"/>
+      <c r="C24" s="116"/>
+      <c r="D24" s="117"/>
+      <c r="E24" s="141"/>
+    </row>
+    <row r="25" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B25" s="159"/>
+      <c r="C25" s="116"/>
+      <c r="D25" s="117"/>
+      <c r="E25" s="144"/>
+    </row>
+    <row r="26" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B26" s="159"/>
+      <c r="C26" s="118"/>
+      <c r="D26" s="117"/>
+      <c r="E26" s="144"/>
+    </row>
+    <row r="27" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B27" s="159"/>
+      <c r="C27" s="118"/>
+      <c r="D27" s="117"/>
+      <c r="E27" s="144"/>
+    </row>
+    <row r="28" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B28" s="159"/>
+      <c r="C28" s="119"/>
+      <c r="D28" s="120"/>
+      <c r="E28" s="145"/>
+    </row>
+    <row r="29" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B29" s="112"/>
+      <c r="C29" s="112"/>
+      <c r="D29" s="113"/>
+      <c r="E29" s="1"/>
+    </row>
+    <row r="30" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B30" s="160" t="s">
+        <v>250</v>
+      </c>
+      <c r="C30" s="121"/>
+      <c r="D30" s="122"/>
+      <c r="E30" s="146"/>
+    </row>
+    <row r="31" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B31" s="161"/>
+      <c r="C31" s="123"/>
+      <c r="D31" s="124"/>
+      <c r="E31" s="147"/>
+    </row>
+    <row r="32" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B32" s="161"/>
+      <c r="C32" s="123"/>
+      <c r="D32" s="124"/>
+      <c r="E32" s="147"/>
+    </row>
+    <row r="33" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B33" s="161"/>
+      <c r="C33" s="123"/>
+      <c r="D33" s="124"/>
+      <c r="E33" s="141"/>
+    </row>
+    <row r="34" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B34" s="161"/>
+      <c r="C34" s="123"/>
+      <c r="D34" s="124"/>
+      <c r="E34" s="144"/>
+    </row>
+    <row r="35" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B35" s="161"/>
+      <c r="C35" s="123"/>
+      <c r="D35" s="124"/>
+      <c r="E35" s="144"/>
+    </row>
+    <row r="36" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B36" s="161"/>
+      <c r="C36" s="123"/>
+      <c r="D36" s="124"/>
+      <c r="E36" s="140"/>
+    </row>
+    <row r="37" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B37" s="161"/>
+      <c r="C37" s="125"/>
+      <c r="D37" s="126"/>
+      <c r="E37" s="142"/>
+    </row>
+    <row r="38" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B38" s="112"/>
+      <c r="C38" s="112"/>
+      <c r="D38" s="113"/>
+      <c r="E38" s="1"/>
+    </row>
+    <row r="39" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B39" s="162" t="s">
+        <v>251</v>
+      </c>
+      <c r="C39" s="127"/>
+      <c r="D39" s="128"/>
+      <c r="E39" s="148"/>
+    </row>
+    <row r="40" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B40" s="163"/>
+      <c r="C40" s="129"/>
+      <c r="D40" s="130"/>
+      <c r="E40" s="141"/>
+    </row>
+    <row r="41" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B41" s="163"/>
+      <c r="C41" s="129"/>
+      <c r="D41" s="130"/>
+      <c r="E41" s="141"/>
+    </row>
+    <row r="42" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B42" s="163"/>
+      <c r="C42" s="129"/>
+      <c r="D42" s="130"/>
+      <c r="E42" s="141"/>
+    </row>
+    <row r="43" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B43" s="163"/>
+      <c r="C43" s="129"/>
+      <c r="D43" s="130"/>
+      <c r="E43" s="141"/>
+    </row>
+    <row r="44" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B44" s="163"/>
+      <c r="C44" s="131"/>
+      <c r="D44" s="132"/>
+      <c r="E44" s="149"/>
+    </row>
+    <row r="45" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B45" s="112"/>
+      <c r="C45" s="112"/>
+      <c r="D45" s="113"/>
+      <c r="E45" s="1"/>
+    </row>
+    <row r="46" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B46" s="164" t="s">
+        <v>252</v>
+      </c>
+      <c r="C46" s="167" t="s">
+        <v>113</v>
+      </c>
+      <c r="D46" s="133"/>
+      <c r="E46" s="139"/>
+    </row>
+    <row r="47" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B47" s="165"/>
+      <c r="C47" s="168"/>
+      <c r="D47" s="134"/>
+      <c r="E47" s="140"/>
+    </row>
+    <row r="48" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B48" s="165"/>
+      <c r="C48" s="168"/>
+      <c r="D48" s="134"/>
+      <c r="E48" s="140"/>
+    </row>
+    <row r="49" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B49" s="165"/>
+      <c r="C49" s="168"/>
+      <c r="D49" s="134"/>
+      <c r="E49" s="140"/>
+    </row>
+    <row r="50" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B50" s="165"/>
+      <c r="C50" s="168"/>
+      <c r="D50" s="134"/>
+      <c r="E50" s="140"/>
+    </row>
+    <row r="51" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B51" s="165"/>
+      <c r="C51" s="169" t="s">
+        <v>253</v>
+      </c>
+      <c r="D51" s="135"/>
+      <c r="E51" s="150"/>
+    </row>
+    <row r="52" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B52" s="165"/>
+      <c r="C52" s="168"/>
+      <c r="D52" s="134"/>
+      <c r="E52" s="140"/>
+    </row>
+    <row r="53" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B53" s="165"/>
+      <c r="C53" s="168"/>
+      <c r="D53" s="134"/>
+      <c r="E53" s="140"/>
+    </row>
+    <row r="54" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B54" s="165"/>
+      <c r="C54" s="168"/>
+      <c r="D54" s="134"/>
+      <c r="E54" s="140"/>
+    </row>
+    <row r="55" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B55" s="165"/>
+      <c r="C55" s="170"/>
+      <c r="D55" s="136"/>
+      <c r="E55" s="151"/>
+    </row>
+    <row r="56" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B56" s="165"/>
+      <c r="C56" s="168" t="s">
+        <v>254</v>
+      </c>
+      <c r="D56" s="134"/>
+      <c r="E56" s="140"/>
+    </row>
+    <row r="57" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B57" s="165"/>
+      <c r="C57" s="168"/>
+      <c r="D57" s="134"/>
+      <c r="E57" s="140"/>
+    </row>
+    <row r="58" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B58" s="165"/>
+      <c r="C58" s="168"/>
+      <c r="D58" s="134"/>
+      <c r="E58" s="140"/>
+    </row>
+    <row r="59" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B59" s="165"/>
+      <c r="C59" s="168"/>
+      <c r="D59" s="134"/>
+      <c r="E59" s="140"/>
+    </row>
+    <row r="60" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B60" s="166"/>
+      <c r="C60" s="171"/>
+      <c r="D60" s="137"/>
+      <c r="E60" s="142"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="10">
+    <mergeCell ref="B46:B60"/>
+    <mergeCell ref="C46:C50"/>
+    <mergeCell ref="C51:C55"/>
+    <mergeCell ref="C56:C60"/>
     <mergeCell ref="B2:P2"/>
     <mergeCell ref="B3:P3"/>
+    <mergeCell ref="B6:B21"/>
+    <mergeCell ref="B23:B28"/>
+    <mergeCell ref="B30:B37"/>
+    <mergeCell ref="B39:B44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -5230,40 +6075,40 @@
       </c>
     </row>
     <row r="2" spans="2:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="103"/>
-      <c r="C2" s="103"/>
-      <c r="D2" s="103"/>
-      <c r="E2" s="103"/>
-      <c r="F2" s="103"/>
-      <c r="G2" s="103"/>
-      <c r="H2" s="103"/>
-      <c r="I2" s="103"/>
-      <c r="J2" s="103"/>
-      <c r="K2" s="103"/>
-      <c r="L2" s="103"/>
-      <c r="M2" s="103"/>
-      <c r="N2" s="103"/>
-      <c r="O2" s="103"/>
-      <c r="P2" s="103"/>
+      <c r="B2" s="152"/>
+      <c r="C2" s="152"/>
+      <c r="D2" s="152"/>
+      <c r="E2" s="152"/>
+      <c r="F2" s="152"/>
+      <c r="G2" s="152"/>
+      <c r="H2" s="152"/>
+      <c r="I2" s="152"/>
+      <c r="J2" s="152"/>
+      <c r="K2" s="152"/>
+      <c r="L2" s="152"/>
+      <c r="M2" s="152"/>
+      <c r="N2" s="152"/>
+      <c r="O2" s="152"/>
+      <c r="P2" s="152"/>
     </row>
     <row r="3" spans="2:18" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="104" t="s">
+      <c r="B3" s="153" t="s">
         <v>62</v>
       </c>
-      <c r="C3" s="104"/>
-      <c r="D3" s="104"/>
-      <c r="E3" s="104"/>
-      <c r="F3" s="104"/>
-      <c r="G3" s="104"/>
-      <c r="H3" s="104"/>
-      <c r="I3" s="104"/>
-      <c r="J3" s="104"/>
-      <c r="K3" s="104"/>
-      <c r="L3" s="104"/>
-      <c r="M3" s="104"/>
-      <c r="N3" s="104"/>
-      <c r="O3" s="104"/>
-      <c r="P3" s="104"/>
+      <c r="C3" s="153"/>
+      <c r="D3" s="153"/>
+      <c r="E3" s="153"/>
+      <c r="F3" s="153"/>
+      <c r="G3" s="153"/>
+      <c r="H3" s="153"/>
+      <c r="I3" s="153"/>
+      <c r="J3" s="153"/>
+      <c r="K3" s="153"/>
+      <c r="L3" s="153"/>
+      <c r="M3" s="153"/>
+      <c r="N3" s="153"/>
+      <c r="O3" s="153"/>
+      <c r="P3" s="153"/>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
@@ -5371,36 +6216,36 @@
       </c>
     </row>
     <row r="2" spans="2:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="103" t="s">
+      <c r="B2" s="152" t="s">
         <v>238</v>
       </c>
-      <c r="C2" s="103"/>
-      <c r="D2" s="103"/>
-      <c r="E2" s="103"/>
-      <c r="F2" s="103"/>
-      <c r="G2" s="103"/>
-      <c r="H2" s="103"/>
-      <c r="I2" s="103"/>
-      <c r="J2" s="103"/>
-      <c r="K2" s="103"/>
-      <c r="L2" s="103"/>
-      <c r="M2" s="103"/>
+      <c r="C2" s="152"/>
+      <c r="D2" s="152"/>
+      <c r="E2" s="152"/>
+      <c r="F2" s="152"/>
+      <c r="G2" s="152"/>
+      <c r="H2" s="152"/>
+      <c r="I2" s="152"/>
+      <c r="J2" s="152"/>
+      <c r="K2" s="152"/>
+      <c r="L2" s="152"/>
+      <c r="M2" s="152"/>
     </row>
     <row r="3" spans="2:13" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="104" t="s">
+      <c r="B3" s="153" t="s">
         <v>239</v>
       </c>
-      <c r="C3" s="104"/>
-      <c r="D3" s="104"/>
-      <c r="E3" s="104"/>
-      <c r="F3" s="104"/>
-      <c r="G3" s="104"/>
-      <c r="H3" s="104"/>
-      <c r="I3" s="104"/>
-      <c r="J3" s="104"/>
-      <c r="K3" s="104"/>
-      <c r="L3" s="104"/>
-      <c r="M3" s="104"/>
+      <c r="C3" s="153"/>
+      <c r="D3" s="153"/>
+      <c r="E3" s="153"/>
+      <c r="F3" s="153"/>
+      <c r="G3" s="153"/>
+      <c r="H3" s="153"/>
+      <c r="I3" s="153"/>
+      <c r="J3" s="153"/>
+      <c r="K3" s="153"/>
+      <c r="L3" s="153"/>
+      <c r="M3" s="153"/>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B5" s="70" t="s">
@@ -5451,36 +6296,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="103"/>
-      <c r="C2" s="103"/>
-      <c r="D2" s="103"/>
-      <c r="E2" s="103"/>
-      <c r="F2" s="103"/>
-      <c r="G2" s="103"/>
-      <c r="H2" s="103"/>
-      <c r="I2" s="103"/>
-      <c r="J2" s="103"/>
-      <c r="K2" s="103"/>
-      <c r="L2" s="103"/>
-      <c r="M2" s="103"/>
-      <c r="N2" s="103"/>
+      <c r="B2" s="152"/>
+      <c r="C2" s="152"/>
+      <c r="D2" s="152"/>
+      <c r="E2" s="152"/>
+      <c r="F2" s="152"/>
+      <c r="G2" s="152"/>
+      <c r="H2" s="152"/>
+      <c r="I2" s="152"/>
+      <c r="J2" s="152"/>
+      <c r="K2" s="152"/>
+      <c r="L2" s="152"/>
+      <c r="M2" s="152"/>
+      <c r="N2" s="152"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="104" t="s">
+      <c r="B3" s="153" t="s">
         <v>63</v>
       </c>
-      <c r="C3" s="104"/>
-      <c r="D3" s="104"/>
-      <c r="E3" s="104"/>
-      <c r="F3" s="104"/>
-      <c r="G3" s="104"/>
-      <c r="H3" s="104"/>
-      <c r="I3" s="104"/>
-      <c r="J3" s="104"/>
-      <c r="K3" s="104"/>
-      <c r="L3" s="104"/>
-      <c r="M3" s="104"/>
-      <c r="N3" s="104"/>
+      <c r="C3" s="153"/>
+      <c r="D3" s="153"/>
+      <c r="E3" s="153"/>
+      <c r="F3" s="153"/>
+      <c r="G3" s="153"/>
+      <c r="H3" s="153"/>
+      <c r="I3" s="153"/>
+      <c r="J3" s="153"/>
+      <c r="K3" s="153"/>
+      <c r="L3" s="153"/>
+      <c r="M3" s="153"/>
+      <c r="N3" s="153"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="58" t="s">
@@ -5570,36 +6415,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="103"/>
-      <c r="C2" s="103"/>
-      <c r="D2" s="103"/>
-      <c r="E2" s="103"/>
-      <c r="F2" s="103"/>
-      <c r="G2" s="103"/>
-      <c r="H2" s="103"/>
-      <c r="I2" s="103"/>
-      <c r="J2" s="103"/>
-      <c r="K2" s="103"/>
-      <c r="L2" s="103"/>
-      <c r="M2" s="103"/>
-      <c r="N2" s="103"/>
+      <c r="B2" s="152"/>
+      <c r="C2" s="152"/>
+      <c r="D2" s="152"/>
+      <c r="E2" s="152"/>
+      <c r="F2" s="152"/>
+      <c r="G2" s="152"/>
+      <c r="H2" s="152"/>
+      <c r="I2" s="152"/>
+      <c r="J2" s="152"/>
+      <c r="K2" s="152"/>
+      <c r="L2" s="152"/>
+      <c r="M2" s="152"/>
+      <c r="N2" s="152"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="104" t="s">
+      <c r="B3" s="153" t="s">
         <v>149</v>
       </c>
-      <c r="C3" s="104"/>
-      <c r="D3" s="104"/>
-      <c r="E3" s="104"/>
-      <c r="F3" s="104"/>
-      <c r="G3" s="104"/>
-      <c r="H3" s="104"/>
-      <c r="I3" s="104"/>
-      <c r="J3" s="104"/>
-      <c r="K3" s="104"/>
-      <c r="L3" s="104"/>
-      <c r="M3" s="104"/>
-      <c r="N3" s="104"/>
+      <c r="C3" s="153"/>
+      <c r="D3" s="153"/>
+      <c r="E3" s="153"/>
+      <c r="F3" s="153"/>
+      <c r="G3" s="153"/>
+      <c r="H3" s="153"/>
+      <c r="I3" s="153"/>
+      <c r="J3" s="153"/>
+      <c r="K3" s="153"/>
+      <c r="L3" s="153"/>
+      <c r="M3" s="153"/>
+      <c r="N3" s="153"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="74" t="s">
@@ -5686,28 +6531,28 @@
       </c>
     </row>
     <row r="2" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="103"/>
-      <c r="C2" s="103"/>
-      <c r="D2" s="103"/>
-      <c r="E2" s="103"/>
-      <c r="F2" s="103"/>
-      <c r="G2" s="103"/>
-      <c r="H2" s="103"/>
-      <c r="I2" s="103"/>
-      <c r="J2" s="103"/>
+      <c r="B2" s="152"/>
+      <c r="C2" s="152"/>
+      <c r="D2" s="152"/>
+      <c r="E2" s="152"/>
+      <c r="F2" s="152"/>
+      <c r="G2" s="152"/>
+      <c r="H2" s="152"/>
+      <c r="I2" s="152"/>
+      <c r="J2" s="152"/>
     </row>
     <row r="3" spans="2:10" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="104" t="s">
+      <c r="B3" s="153" t="s">
         <v>152</v>
       </c>
-      <c r="C3" s="104"/>
-      <c r="D3" s="104"/>
-      <c r="E3" s="104"/>
-      <c r="F3" s="104"/>
-      <c r="G3" s="104"/>
-      <c r="H3" s="104"/>
-      <c r="I3" s="104"/>
-      <c r="J3" s="104"/>
+      <c r="C3" s="153"/>
+      <c r="D3" s="153"/>
+      <c r="E3" s="153"/>
+      <c r="F3" s="153"/>
+      <c r="G3" s="153"/>
+      <c r="H3" s="153"/>
+      <c r="I3" s="153"/>
+      <c r="J3" s="153"/>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" s="74" t="s">
@@ -5792,29 +6637,29 @@
       </c>
     </row>
     <row r="2" spans="2:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="105"/>
-      <c r="C2" s="105"/>
-      <c r="D2" s="105"/>
-      <c r="E2" s="105"/>
-      <c r="F2" s="105"/>
-      <c r="G2" s="105"/>
-      <c r="H2" s="105"/>
-      <c r="I2" s="105"/>
+      <c r="B2" s="154"/>
+      <c r="C2" s="154"/>
+      <c r="D2" s="154"/>
+      <c r="E2" s="154"/>
+      <c r="F2" s="154"/>
+      <c r="G2" s="154"/>
+      <c r="H2" s="154"/>
+      <c r="I2" s="154"/>
       <c r="L2" s="83"/>
       <c r="M2" s="83"/>
       <c r="N2" s="83"/>
     </row>
     <row r="3" spans="2:20" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="104" t="s">
+      <c r="B3" s="153" t="s">
         <v>153</v>
       </c>
-      <c r="C3" s="104"/>
-      <c r="D3" s="104"/>
-      <c r="E3" s="104"/>
-      <c r="F3" s="104"/>
-      <c r="G3" s="104"/>
-      <c r="H3" s="104"/>
-      <c r="I3" s="104"/>
+      <c r="C3" s="153"/>
+      <c r="D3" s="153"/>
+      <c r="E3" s="153"/>
+      <c r="F3" s="153"/>
+      <c r="G3" s="153"/>
+      <c r="H3" s="153"/>
+      <c r="I3" s="153"/>
       <c r="L3" s="82"/>
       <c r="M3" s="82"/>
       <c r="N3" s="82"/>
@@ -5933,20 +6778,20 @@
       </c>
     </row>
     <row r="2" spans="2:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="104" t="s">
+      <c r="B2" s="153" t="s">
         <v>203</v>
       </c>
-      <c r="C2" s="104"/>
-      <c r="D2" s="104"/>
-      <c r="E2" s="104"/>
-      <c r="F2" s="104"/>
+      <c r="C2" s="153"/>
+      <c r="D2" s="153"/>
+      <c r="E2" s="153"/>
+      <c r="F2" s="153"/>
     </row>
     <row r="3" spans="2:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="104"/>
-      <c r="C3" s="104"/>
-      <c r="D3" s="104"/>
-      <c r="E3" s="104"/>
-      <c r="F3" s="104"/>
+      <c r="B3" s="153"/>
+      <c r="C3" s="153"/>
+      <c r="D3" s="153"/>
+      <c r="E3" s="153"/>
+      <c r="F3" s="153"/>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="99" t="s">
@@ -6003,26 +6848,26 @@
       </c>
     </row>
     <row r="2" spans="2:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="104" t="s">
+      <c r="B2" s="153" t="s">
         <v>209</v>
       </c>
-      <c r="C2" s="104"/>
-      <c r="D2" s="104"/>
-      <c r="E2" s="104"/>
-      <c r="F2" s="104"/>
-      <c r="G2" s="104"/>
-      <c r="H2" s="104"/>
-      <c r="I2" s="104"/>
+      <c r="C2" s="153"/>
+      <c r="D2" s="153"/>
+      <c r="E2" s="153"/>
+      <c r="F2" s="153"/>
+      <c r="G2" s="153"/>
+      <c r="H2" s="153"/>
+      <c r="I2" s="153"/>
     </row>
     <row r="3" spans="2:9" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="104"/>
-      <c r="C3" s="104"/>
-      <c r="D3" s="104"/>
-      <c r="E3" s="104"/>
-      <c r="F3" s="104"/>
-      <c r="G3" s="104"/>
-      <c r="H3" s="104"/>
-      <c r="I3" s="104"/>
+      <c r="B3" s="153"/>
+      <c r="C3" s="153"/>
+      <c r="D3" s="153"/>
+      <c r="E3" s="153"/>
+      <c r="F3" s="153"/>
+      <c r="G3" s="153"/>
+      <c r="H3" s="153"/>
+      <c r="I3" s="153"/>
     </row>
     <row r="5" spans="2:9" ht="27" x14ac:dyDescent="0.25">
       <c r="B5" s="99" t="s">
@@ -6075,26 +6920,26 @@
       </c>
     </row>
     <row r="2" spans="2:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="103"/>
-      <c r="C2" s="103"/>
-      <c r="D2" s="103"/>
-      <c r="E2" s="103"/>
-      <c r="F2" s="103"/>
-      <c r="G2" s="103"/>
-      <c r="H2" s="103"/>
-      <c r="I2" s="103"/>
+      <c r="B2" s="152"/>
+      <c r="C2" s="152"/>
+      <c r="D2" s="152"/>
+      <c r="E2" s="152"/>
+      <c r="F2" s="152"/>
+      <c r="G2" s="152"/>
+      <c r="H2" s="152"/>
+      <c r="I2" s="152"/>
     </row>
     <row r="3" spans="2:9" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="104" t="s">
+      <c r="B3" s="153" t="s">
         <v>189</v>
       </c>
-      <c r="C3" s="104"/>
-      <c r="D3" s="104"/>
-      <c r="E3" s="104"/>
-      <c r="F3" s="104"/>
-      <c r="G3" s="104"/>
-      <c r="H3" s="104"/>
-      <c r="I3" s="104"/>
+      <c r="C3" s="153"/>
+      <c r="D3" s="153"/>
+      <c r="E3" s="153"/>
+      <c r="F3" s="153"/>
+      <c r="G3" s="153"/>
+      <c r="H3" s="153"/>
+      <c r="I3" s="153"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="88" t="s">
@@ -6170,30 +7015,30 @@
       </c>
     </row>
     <row r="2" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="103"/>
-      <c r="C2" s="103"/>
-      <c r="D2" s="103"/>
-      <c r="E2" s="103"/>
-      <c r="F2" s="103"/>
-      <c r="G2" s="103"/>
-      <c r="H2" s="103"/>
-      <c r="I2" s="103"/>
-      <c r="J2" s="103"/>
-      <c r="K2" s="103"/>
+      <c r="B2" s="152"/>
+      <c r="C2" s="152"/>
+      <c r="D2" s="152"/>
+      <c r="E2" s="152"/>
+      <c r="F2" s="152"/>
+      <c r="G2" s="152"/>
+      <c r="H2" s="152"/>
+      <c r="I2" s="152"/>
+      <c r="J2" s="152"/>
+      <c r="K2" s="152"/>
     </row>
     <row r="3" spans="2:11" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="104" t="s">
+      <c r="B3" s="153" t="s">
         <v>165</v>
       </c>
-      <c r="C3" s="104"/>
-      <c r="D3" s="104"/>
-      <c r="E3" s="104"/>
-      <c r="F3" s="104"/>
-      <c r="G3" s="104"/>
-      <c r="H3" s="104"/>
-      <c r="I3" s="104"/>
-      <c r="J3" s="104"/>
-      <c r="K3" s="104"/>
+      <c r="C3" s="153"/>
+      <c r="D3" s="153"/>
+      <c r="E3" s="153"/>
+      <c r="F3" s="153"/>
+      <c r="G3" s="153"/>
+      <c r="H3" s="153"/>
+      <c r="I3" s="153"/>
+      <c r="J3" s="153"/>
+      <c r="K3" s="153"/>
     </row>
     <row r="4" spans="2:11" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B4" s="84"/>
@@ -6208,14 +7053,14 @@
       <c r="K4" s="84"/>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="H5" s="107" t="s">
+      <c r="H5" s="172" t="s">
         <v>173</v>
       </c>
-      <c r="I5" s="108"/>
-      <c r="J5" s="107" t="s">
+      <c r="I5" s="173"/>
+      <c r="J5" s="172" t="s">
         <v>172</v>
       </c>
-      <c r="K5" s="108"/>
+      <c r="K5" s="173"/>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" s="85" t="s">
@@ -6294,24 +7139,24 @@
       </c>
     </row>
     <row r="2" spans="2:8" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="104" t="s">
+      <c r="B2" s="153" t="s">
         <v>214</v>
       </c>
-      <c r="C2" s="104"/>
-      <c r="D2" s="104"/>
-      <c r="E2" s="104"/>
-      <c r="F2" s="104"/>
-      <c r="G2" s="104"/>
-      <c r="H2" s="104"/>
+      <c r="C2" s="153"/>
+      <c r="D2" s="153"/>
+      <c r="E2" s="153"/>
+      <c r="F2" s="153"/>
+      <c r="G2" s="153"/>
+      <c r="H2" s="153"/>
     </row>
     <row r="3" spans="2:8" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="104"/>
-      <c r="C3" s="104"/>
-      <c r="D3" s="104"/>
-      <c r="E3" s="104"/>
-      <c r="F3" s="104"/>
-      <c r="G3" s="104"/>
-      <c r="H3" s="104"/>
+      <c r="B3" s="153"/>
+      <c r="C3" s="153"/>
+      <c r="D3" s="153"/>
+      <c r="E3" s="153"/>
+      <c r="F3" s="153"/>
+      <c r="G3" s="153"/>
+      <c r="H3" s="153"/>
     </row>
     <row r="5" spans="2:8" ht="27" x14ac:dyDescent="0.25">
       <c r="B5" s="100" t="s">
@@ -6355,24 +7200,24 @@
       </c>
     </row>
     <row r="2" spans="2:8" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="104" t="s">
+      <c r="B2" s="153" t="s">
         <v>215</v>
       </c>
-      <c r="C2" s="104"/>
-      <c r="D2" s="104"/>
-      <c r="E2" s="104"/>
-      <c r="F2" s="104"/>
-      <c r="G2" s="104"/>
-      <c r="H2" s="104"/>
+      <c r="C2" s="153"/>
+      <c r="D2" s="153"/>
+      <c r="E2" s="153"/>
+      <c r="F2" s="153"/>
+      <c r="G2" s="153"/>
+      <c r="H2" s="153"/>
     </row>
     <row r="3" spans="2:8" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="104"/>
-      <c r="C3" s="104"/>
-      <c r="D3" s="104"/>
-      <c r="E3" s="104"/>
-      <c r="F3" s="104"/>
-      <c r="G3" s="104"/>
-      <c r="H3" s="104"/>
+      <c r="B3" s="153"/>
+      <c r="C3" s="153"/>
+      <c r="D3" s="153"/>
+      <c r="E3" s="153"/>
+      <c r="F3" s="153"/>
+      <c r="G3" s="153"/>
+      <c r="H3" s="153"/>
     </row>
     <row r="5" spans="2:8" ht="27" x14ac:dyDescent="0.25">
       <c r="B5" s="100" t="s">
@@ -6422,38 +7267,38 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="103" t="s">
+      <c r="B2" s="152" t="s">
         <v>94</v>
       </c>
-      <c r="C2" s="103"/>
-      <c r="D2" s="103"/>
-      <c r="E2" s="103"/>
-      <c r="F2" s="103"/>
-      <c r="G2" s="103"/>
-      <c r="H2" s="103"/>
-      <c r="I2" s="103"/>
-      <c r="J2" s="103"/>
-      <c r="K2" s="103"/>
-      <c r="L2" s="103"/>
-      <c r="M2" s="103"/>
-      <c r="N2" s="103"/>
+      <c r="C2" s="152"/>
+      <c r="D2" s="152"/>
+      <c r="E2" s="152"/>
+      <c r="F2" s="152"/>
+      <c r="G2" s="152"/>
+      <c r="H2" s="152"/>
+      <c r="I2" s="152"/>
+      <c r="J2" s="152"/>
+      <c r="K2" s="152"/>
+      <c r="L2" s="152"/>
+      <c r="M2" s="152"/>
+      <c r="N2" s="152"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="104" t="s">
+      <c r="B3" s="153" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="104"/>
-      <c r="D3" s="104"/>
-      <c r="E3" s="104"/>
-      <c r="F3" s="104"/>
-      <c r="G3" s="104"/>
-      <c r="H3" s="104"/>
-      <c r="I3" s="104"/>
-      <c r="J3" s="104"/>
-      <c r="K3" s="104"/>
-      <c r="L3" s="104"/>
-      <c r="M3" s="104"/>
-      <c r="N3" s="104"/>
+      <c r="C3" s="153"/>
+      <c r="D3" s="153"/>
+      <c r="E3" s="153"/>
+      <c r="F3" s="153"/>
+      <c r="G3" s="153"/>
+      <c r="H3" s="153"/>
+      <c r="I3" s="153"/>
+      <c r="J3" s="153"/>
+      <c r="K3" s="153"/>
+      <c r="L3" s="153"/>
+      <c r="M3" s="153"/>
+      <c r="N3" s="153"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="44" t="s">
@@ -6503,24 +7348,24 @@
       </c>
     </row>
     <row r="2" spans="2:8" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="104" t="s">
+      <c r="B2" s="153" t="s">
         <v>217</v>
       </c>
-      <c r="C2" s="104"/>
-      <c r="D2" s="104"/>
-      <c r="E2" s="104"/>
-      <c r="F2" s="104"/>
-      <c r="G2" s="104"/>
-      <c r="H2" s="104"/>
+      <c r="C2" s="153"/>
+      <c r="D2" s="153"/>
+      <c r="E2" s="153"/>
+      <c r="F2" s="153"/>
+      <c r="G2" s="153"/>
+      <c r="H2" s="153"/>
     </row>
     <row r="3" spans="2:8" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="104"/>
-      <c r="C3" s="104"/>
-      <c r="D3" s="104"/>
-      <c r="E3" s="104"/>
-      <c r="F3" s="104"/>
-      <c r="G3" s="104"/>
-      <c r="H3" s="104"/>
+      <c r="B3" s="153"/>
+      <c r="C3" s="153"/>
+      <c r="D3" s="153"/>
+      <c r="E3" s="153"/>
+      <c r="F3" s="153"/>
+      <c r="G3" s="153"/>
+      <c r="H3" s="153"/>
     </row>
     <row r="5" spans="2:8" ht="27" x14ac:dyDescent="0.25">
       <c r="B5" s="100" t="s">
@@ -6564,24 +7409,24 @@
       </c>
     </row>
     <row r="2" spans="2:8" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="104" t="s">
+      <c r="B2" s="153" t="s">
         <v>219</v>
       </c>
-      <c r="C2" s="104"/>
-      <c r="D2" s="104"/>
-      <c r="E2" s="104"/>
-      <c r="F2" s="104"/>
-      <c r="G2" s="104"/>
-      <c r="H2" s="104"/>
+      <c r="C2" s="153"/>
+      <c r="D2" s="153"/>
+      <c r="E2" s="153"/>
+      <c r="F2" s="153"/>
+      <c r="G2" s="153"/>
+      <c r="H2" s="153"/>
     </row>
     <row r="3" spans="2:8" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="104"/>
-      <c r="C3" s="104"/>
-      <c r="D3" s="104"/>
-      <c r="E3" s="104"/>
-      <c r="F3" s="104"/>
-      <c r="G3" s="104"/>
-      <c r="H3" s="104"/>
+      <c r="B3" s="153"/>
+      <c r="C3" s="153"/>
+      <c r="D3" s="153"/>
+      <c r="E3" s="153"/>
+      <c r="F3" s="153"/>
+      <c r="G3" s="153"/>
+      <c r="H3" s="153"/>
     </row>
     <row r="5" spans="2:8" ht="27" x14ac:dyDescent="0.25">
       <c r="B5" s="100" t="s">
@@ -6625,24 +7470,24 @@
       </c>
     </row>
     <row r="2" spans="2:8" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="104" t="s">
+      <c r="B2" s="153" t="s">
         <v>220</v>
       </c>
-      <c r="C2" s="104"/>
-      <c r="D2" s="104"/>
-      <c r="E2" s="104"/>
-      <c r="F2" s="104"/>
-      <c r="G2" s="104"/>
-      <c r="H2" s="104"/>
+      <c r="C2" s="153"/>
+      <c r="D2" s="153"/>
+      <c r="E2" s="153"/>
+      <c r="F2" s="153"/>
+      <c r="G2" s="153"/>
+      <c r="H2" s="153"/>
     </row>
     <row r="3" spans="2:8" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="104"/>
-      <c r="C3" s="104"/>
-      <c r="D3" s="104"/>
-      <c r="E3" s="104"/>
-      <c r="F3" s="104"/>
-      <c r="G3" s="104"/>
-      <c r="H3" s="104"/>
+      <c r="B3" s="153"/>
+      <c r="C3" s="153"/>
+      <c r="D3" s="153"/>
+      <c r="E3" s="153"/>
+      <c r="F3" s="153"/>
+      <c r="G3" s="153"/>
+      <c r="H3" s="153"/>
     </row>
     <row r="5" spans="2:8" ht="27" x14ac:dyDescent="0.25">
       <c r="B5" s="100" t="s">
@@ -6688,24 +7533,24 @@
       </c>
     </row>
     <row r="2" spans="2:8" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="104" t="s">
+      <c r="B2" s="153" t="s">
         <v>223</v>
       </c>
-      <c r="C2" s="104"/>
-      <c r="D2" s="104"/>
-      <c r="E2" s="104"/>
-      <c r="F2" s="104"/>
-      <c r="G2" s="104"/>
-      <c r="H2" s="104"/>
+      <c r="C2" s="153"/>
+      <c r="D2" s="153"/>
+      <c r="E2" s="153"/>
+      <c r="F2" s="153"/>
+      <c r="G2" s="153"/>
+      <c r="H2" s="153"/>
     </row>
     <row r="3" spans="2:8" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="104"/>
-      <c r="C3" s="104"/>
-      <c r="D3" s="104"/>
-      <c r="E3" s="104"/>
-      <c r="F3" s="104"/>
-      <c r="G3" s="104"/>
-      <c r="H3" s="104"/>
+      <c r="B3" s="153"/>
+      <c r="C3" s="153"/>
+      <c r="D3" s="153"/>
+      <c r="E3" s="153"/>
+      <c r="F3" s="153"/>
+      <c r="G3" s="153"/>
+      <c r="H3" s="153"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" s="100" t="s">
@@ -6759,24 +7604,24 @@
       </c>
     </row>
     <row r="2" spans="2:8" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="104" t="s">
+      <c r="B2" s="153" t="s">
         <v>225</v>
       </c>
-      <c r="C2" s="104"/>
-      <c r="D2" s="104"/>
-      <c r="E2" s="104"/>
-      <c r="F2" s="104"/>
-      <c r="G2" s="104"/>
-      <c r="H2" s="104"/>
+      <c r="C2" s="153"/>
+      <c r="D2" s="153"/>
+      <c r="E2" s="153"/>
+      <c r="F2" s="153"/>
+      <c r="G2" s="153"/>
+      <c r="H2" s="153"/>
     </row>
     <row r="3" spans="2:8" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="104"/>
-      <c r="C3" s="104"/>
-      <c r="D3" s="104"/>
-      <c r="E3" s="104"/>
-      <c r="F3" s="104"/>
-      <c r="G3" s="104"/>
-      <c r="H3" s="104"/>
+      <c r="B3" s="153"/>
+      <c r="C3" s="153"/>
+      <c r="D3" s="153"/>
+      <c r="E3" s="153"/>
+      <c r="F3" s="153"/>
+      <c r="G3" s="153"/>
+      <c r="H3" s="153"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" s="100" t="s">
@@ -6831,37 +7676,37 @@
       <c r="Z1" s="38"/>
     </row>
     <row r="2" spans="2:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="103"/>
-      <c r="C2" s="103"/>
-      <c r="D2" s="103"/>
-      <c r="E2" s="103"/>
-      <c r="F2" s="103"/>
-      <c r="G2" s="103"/>
-      <c r="H2" s="103"/>
-      <c r="I2" s="103"/>
-      <c r="J2" s="103"/>
-      <c r="K2" s="103"/>
-      <c r="L2" s="103"/>
-      <c r="M2" s="103"/>
-      <c r="N2" s="103"/>
+      <c r="B2" s="152"/>
+      <c r="C2" s="152"/>
+      <c r="D2" s="152"/>
+      <c r="E2" s="152"/>
+      <c r="F2" s="152"/>
+      <c r="G2" s="152"/>
+      <c r="H2" s="152"/>
+      <c r="I2" s="152"/>
+      <c r="J2" s="152"/>
+      <c r="K2" s="152"/>
+      <c r="L2" s="152"/>
+      <c r="M2" s="152"/>
+      <c r="N2" s="152"/>
       <c r="Z2"/>
     </row>
     <row r="3" spans="2:26" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="104" t="s">
+      <c r="B3" s="153" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="104"/>
-      <c r="D3" s="104"/>
-      <c r="E3" s="104"/>
-      <c r="F3" s="104"/>
-      <c r="G3" s="104"/>
-      <c r="H3" s="104"/>
-      <c r="I3" s="104"/>
-      <c r="J3" s="104"/>
-      <c r="K3" s="104"/>
-      <c r="L3" s="104"/>
-      <c r="M3" s="104"/>
-      <c r="N3" s="104"/>
+      <c r="C3" s="153"/>
+      <c r="D3" s="153"/>
+      <c r="E3" s="153"/>
+      <c r="F3" s="153"/>
+      <c r="G3" s="153"/>
+      <c r="H3" s="153"/>
+      <c r="I3" s="153"/>
+      <c r="J3" s="153"/>
+      <c r="K3" s="153"/>
+      <c r="L3" s="153"/>
+      <c r="M3" s="153"/>
+      <c r="N3" s="153"/>
       <c r="Z3"/>
     </row>
     <row r="5" spans="2:26" x14ac:dyDescent="0.25">
@@ -6965,37 +7810,37 @@
       <c r="Z1" s="38"/>
     </row>
     <row r="2" spans="2:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="103"/>
-      <c r="C2" s="103"/>
-      <c r="D2" s="103"/>
-      <c r="E2" s="103"/>
-      <c r="F2" s="103"/>
-      <c r="G2" s="103"/>
-      <c r="H2" s="103"/>
-      <c r="I2" s="103"/>
-      <c r="J2" s="103"/>
-      <c r="K2" s="103"/>
-      <c r="L2" s="103"/>
-      <c r="M2" s="103"/>
-      <c r="N2" s="103"/>
+      <c r="B2" s="152"/>
+      <c r="C2" s="152"/>
+      <c r="D2" s="152"/>
+      <c r="E2" s="152"/>
+      <c r="F2" s="152"/>
+      <c r="G2" s="152"/>
+      <c r="H2" s="152"/>
+      <c r="I2" s="152"/>
+      <c r="J2" s="152"/>
+      <c r="K2" s="152"/>
+      <c r="L2" s="152"/>
+      <c r="M2" s="152"/>
+      <c r="N2" s="152"/>
       <c r="Z2"/>
     </row>
     <row r="3" spans="2:26" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="104" t="s">
+      <c r="B3" s="153" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="104"/>
-      <c r="D3" s="104"/>
-      <c r="E3" s="104"/>
-      <c r="F3" s="104"/>
-      <c r="G3" s="104"/>
-      <c r="H3" s="104"/>
-      <c r="I3" s="104"/>
-      <c r="J3" s="104"/>
-      <c r="K3" s="104"/>
-      <c r="L3" s="104"/>
-      <c r="M3" s="104"/>
-      <c r="N3" s="104"/>
+      <c r="C3" s="153"/>
+      <c r="D3" s="153"/>
+      <c r="E3" s="153"/>
+      <c r="F3" s="153"/>
+      <c r="G3" s="153"/>
+      <c r="H3" s="153"/>
+      <c r="I3" s="153"/>
+      <c r="J3" s="153"/>
+      <c r="K3" s="153"/>
+      <c r="L3" s="153"/>
+      <c r="M3" s="153"/>
+      <c r="N3" s="153"/>
       <c r="Z3"/>
     </row>
     <row r="5" spans="2:26" x14ac:dyDescent="0.25">
@@ -7014,9 +7859,9 @@
       <c r="C6" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="D6" s="109"/>
-      <c r="E6" s="110"/>
-      <c r="F6" s="111"/>
+      <c r="D6" s="174"/>
+      <c r="E6" s="175"/>
+      <c r="F6" s="176"/>
       <c r="G6" s="50"/>
       <c r="H6" s="50"/>
     </row>
@@ -7094,37 +7939,37 @@
       <c r="Z1" s="38"/>
     </row>
     <row r="2" spans="2:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="103"/>
-      <c r="C2" s="103"/>
-      <c r="D2" s="103"/>
-      <c r="E2" s="103"/>
-      <c r="F2" s="103"/>
-      <c r="G2" s="103"/>
-      <c r="H2" s="103"/>
-      <c r="I2" s="103"/>
-      <c r="J2" s="103"/>
-      <c r="K2" s="103"/>
-      <c r="L2" s="103"/>
-      <c r="M2" s="103"/>
-      <c r="N2" s="103"/>
+      <c r="B2" s="152"/>
+      <c r="C2" s="152"/>
+      <c r="D2" s="152"/>
+      <c r="E2" s="152"/>
+      <c r="F2" s="152"/>
+      <c r="G2" s="152"/>
+      <c r="H2" s="152"/>
+      <c r="I2" s="152"/>
+      <c r="J2" s="152"/>
+      <c r="K2" s="152"/>
+      <c r="L2" s="152"/>
+      <c r="M2" s="152"/>
+      <c r="N2" s="152"/>
       <c r="Z2"/>
     </row>
     <row r="3" spans="2:26" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="104" t="s">
+      <c r="B3" s="153" t="s">
         <v>90</v>
       </c>
-      <c r="C3" s="104"/>
-      <c r="D3" s="104"/>
-      <c r="E3" s="104"/>
-      <c r="F3" s="104"/>
-      <c r="G3" s="104"/>
-      <c r="H3" s="104"/>
-      <c r="I3" s="104"/>
-      <c r="J3" s="104"/>
-      <c r="K3" s="104"/>
-      <c r="L3" s="104"/>
-      <c r="M3" s="104"/>
-      <c r="N3" s="104"/>
+      <c r="C3" s="153"/>
+      <c r="D3" s="153"/>
+      <c r="E3" s="153"/>
+      <c r="F3" s="153"/>
+      <c r="G3" s="153"/>
+      <c r="H3" s="153"/>
+      <c r="I3" s="153"/>
+      <c r="J3" s="153"/>
+      <c r="K3" s="153"/>
+      <c r="L3" s="153"/>
+      <c r="M3" s="153"/>
+      <c r="N3" s="153"/>
       <c r="Z3"/>
     </row>
     <row r="5" spans="2:26" x14ac:dyDescent="0.25">
@@ -7217,37 +8062,37 @@
       <c r="Z1" s="38"/>
     </row>
     <row r="2" spans="2:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="103"/>
-      <c r="C2" s="103"/>
-      <c r="D2" s="103"/>
-      <c r="E2" s="103"/>
-      <c r="F2" s="103"/>
-      <c r="G2" s="103"/>
-      <c r="H2" s="103"/>
-      <c r="I2" s="103"/>
-      <c r="J2" s="103"/>
-      <c r="K2" s="103"/>
-      <c r="L2" s="103"/>
-      <c r="M2" s="103"/>
-      <c r="N2" s="103"/>
+      <c r="B2" s="152"/>
+      <c r="C2" s="152"/>
+      <c r="D2" s="152"/>
+      <c r="E2" s="152"/>
+      <c r="F2" s="152"/>
+      <c r="G2" s="152"/>
+      <c r="H2" s="152"/>
+      <c r="I2" s="152"/>
+      <c r="J2" s="152"/>
+      <c r="K2" s="152"/>
+      <c r="L2" s="152"/>
+      <c r="M2" s="152"/>
+      <c r="N2" s="152"/>
       <c r="Z2"/>
     </row>
     <row r="3" spans="2:26" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="104" t="s">
+      <c r="B3" s="153" t="s">
         <v>71</v>
       </c>
-      <c r="C3" s="104"/>
-      <c r="D3" s="104"/>
-      <c r="E3" s="104"/>
-      <c r="F3" s="104"/>
-      <c r="G3" s="104"/>
-      <c r="H3" s="104"/>
-      <c r="I3" s="104"/>
-      <c r="J3" s="104"/>
-      <c r="K3" s="104"/>
-      <c r="L3" s="104"/>
-      <c r="M3" s="104"/>
-      <c r="N3" s="104"/>
+      <c r="C3" s="153"/>
+      <c r="D3" s="153"/>
+      <c r="E3" s="153"/>
+      <c r="F3" s="153"/>
+      <c r="G3" s="153"/>
+      <c r="H3" s="153"/>
+      <c r="I3" s="153"/>
+      <c r="J3" s="153"/>
+      <c r="K3" s="153"/>
+      <c r="L3" s="153"/>
+      <c r="M3" s="153"/>
+      <c r="N3" s="153"/>
       <c r="Z3"/>
     </row>
     <row r="5" spans="2:26" x14ac:dyDescent="0.25">
@@ -7360,56 +8205,56 @@
       </c>
     </row>
     <row r="2" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="103"/>
-      <c r="C2" s="103"/>
-      <c r="D2" s="103"/>
-      <c r="E2" s="103"/>
-      <c r="F2" s="103"/>
-      <c r="G2" s="103"/>
-      <c r="H2" s="103"/>
-      <c r="I2" s="103"/>
-      <c r="J2" s="103"/>
-      <c r="K2" s="103"/>
-      <c r="L2" s="103"/>
+      <c r="B2" s="152"/>
+      <c r="C2" s="152"/>
+      <c r="D2" s="152"/>
+      <c r="E2" s="152"/>
+      <c r="F2" s="152"/>
+      <c r="G2" s="152"/>
+      <c r="H2" s="152"/>
+      <c r="I2" s="152"/>
+      <c r="J2" s="152"/>
+      <c r="K2" s="152"/>
+      <c r="L2" s="152"/>
     </row>
     <row r="3" spans="2:17" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="104" t="s">
+      <c r="B3" s="153" t="s">
         <v>105</v>
       </c>
-      <c r="C3" s="104"/>
-      <c r="D3" s="104"/>
-      <c r="E3" s="104"/>
-      <c r="F3" s="104"/>
-      <c r="G3" s="104"/>
-      <c r="H3" s="104"/>
-      <c r="I3" s="104"/>
-      <c r="J3" s="104"/>
-      <c r="K3" s="104"/>
-      <c r="L3" s="104"/>
+      <c r="C3" s="153"/>
+      <c r="D3" s="153"/>
+      <c r="E3" s="153"/>
+      <c r="F3" s="153"/>
+      <c r="G3" s="153"/>
+      <c r="H3" s="153"/>
+      <c r="I3" s="153"/>
+      <c r="J3" s="153"/>
+      <c r="K3" s="153"/>
+      <c r="L3" s="153"/>
     </row>
     <row r="5" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D5" s="112" t="s">
+      <c r="D5" s="177" t="s">
         <v>120</v>
       </c>
-      <c r="E5" s="112"/>
+      <c r="E5" s="177"/>
       <c r="F5" s="73"/>
       <c r="G5" s="73"/>
       <c r="H5" s="73"/>
       <c r="I5" s="73"/>
-      <c r="J5" s="112" t="s">
+      <c r="J5" s="177" t="s">
         <v>41</v>
       </c>
-      <c r="K5" s="112"/>
-      <c r="L5" s="112"/>
-      <c r="M5" s="112" t="s">
+      <c r="K5" s="177"/>
+      <c r="L5" s="177"/>
+      <c r="M5" s="177" t="s">
         <v>127</v>
       </c>
-      <c r="N5" s="112"/>
-      <c r="O5" s="112"/>
-      <c r="P5" s="106" t="s">
+      <c r="N5" s="177"/>
+      <c r="O5" s="177"/>
+      <c r="P5" s="155" t="s">
         <v>106</v>
       </c>
-      <c r="Q5" s="106"/>
+      <c r="Q5" s="155"/>
     </row>
     <row r="6" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="70" t="s">
@@ -7516,35 +8361,35 @@
       </c>
     </row>
     <row r="2" spans="2:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="103" t="s">
+      <c r="B2" s="152" t="s">
         <v>242</v>
       </c>
-      <c r="C2" s="103"/>
-      <c r="D2" s="103"/>
-      <c r="E2" s="103"/>
-      <c r="F2" s="103"/>
-      <c r="G2" s="103"/>
-      <c r="H2" s="103"/>
-      <c r="I2" s="103"/>
-      <c r="J2" s="103"/>
-      <c r="K2" s="103"/>
-      <c r="L2" s="103"/>
+      <c r="C2" s="152"/>
+      <c r="D2" s="152"/>
+      <c r="E2" s="152"/>
+      <c r="F2" s="152"/>
+      <c r="G2" s="152"/>
+      <c r="H2" s="152"/>
+      <c r="I2" s="152"/>
+      <c r="J2" s="152"/>
+      <c r="K2" s="152"/>
+      <c r="L2" s="152"/>
     </row>
     <row r="3" spans="2:13" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="104" t="s">
+      <c r="B3" s="153" t="s">
         <v>241</v>
       </c>
-      <c r="C3" s="104"/>
-      <c r="D3" s="104"/>
-      <c r="E3" s="104"/>
-      <c r="F3" s="104"/>
-      <c r="G3" s="104"/>
-      <c r="H3" s="104"/>
-      <c r="I3" s="104"/>
-      <c r="J3" s="104"/>
-      <c r="K3" s="104"/>
-      <c r="L3" s="104"/>
-      <c r="M3" s="104"/>
+      <c r="C3" s="153"/>
+      <c r="D3" s="153"/>
+      <c r="E3" s="153"/>
+      <c r="F3" s="153"/>
+      <c r="G3" s="153"/>
+      <c r="H3" s="153"/>
+      <c r="I3" s="153"/>
+      <c r="J3" s="153"/>
+      <c r="K3" s="153"/>
+      <c r="L3" s="153"/>
+      <c r="M3" s="153"/>
     </row>
     <row r="4" spans="2:13" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="102"/>
@@ -7623,110 +8468,110 @@
       </c>
     </row>
     <row r="2" spans="2:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="103"/>
-      <c r="C2" s="103"/>
-      <c r="D2" s="103"/>
-      <c r="E2" s="103"/>
-      <c r="F2" s="103"/>
-      <c r="G2" s="103"/>
-      <c r="H2" s="103"/>
-      <c r="I2" s="103"/>
-      <c r="J2" s="103"/>
-      <c r="K2" s="103"/>
-      <c r="L2" s="103"/>
-      <c r="M2" s="103"/>
-      <c r="N2" s="103"/>
-      <c r="O2" s="103"/>
-      <c r="P2" s="103"/>
+      <c r="B2" s="152"/>
+      <c r="C2" s="152"/>
+      <c r="D2" s="152"/>
+      <c r="E2" s="152"/>
+      <c r="F2" s="152"/>
+      <c r="G2" s="152"/>
+      <c r="H2" s="152"/>
+      <c r="I2" s="152"/>
+      <c r="J2" s="152"/>
+      <c r="K2" s="152"/>
+      <c r="L2" s="152"/>
+      <c r="M2" s="152"/>
+      <c r="N2" s="152"/>
+      <c r="O2" s="152"/>
+      <c r="P2" s="152"/>
       <c r="Q2" s="56"/>
       <c r="R2" s="56"/>
     </row>
     <row r="3" spans="2:25" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="104" t="s">
+      <c r="B3" s="153" t="s">
         <v>108</v>
       </c>
-      <c r="C3" s="104"/>
-      <c r="D3" s="104"/>
-      <c r="E3" s="104"/>
-      <c r="F3" s="104"/>
-      <c r="G3" s="104"/>
-      <c r="H3" s="104"/>
-      <c r="I3" s="104"/>
-      <c r="J3" s="104"/>
-      <c r="K3" s="104"/>
-      <c r="L3" s="104"/>
-      <c r="M3" s="104"/>
-      <c r="N3" s="104"/>
-      <c r="O3" s="104"/>
-      <c r="P3" s="104"/>
+      <c r="C3" s="153"/>
+      <c r="D3" s="153"/>
+      <c r="E3" s="153"/>
+      <c r="F3" s="153"/>
+      <c r="G3" s="153"/>
+      <c r="H3" s="153"/>
+      <c r="I3" s="153"/>
+      <c r="J3" s="153"/>
+      <c r="K3" s="153"/>
+      <c r="L3" s="153"/>
+      <c r="M3" s="153"/>
+      <c r="N3" s="153"/>
+      <c r="O3" s="153"/>
+      <c r="P3" s="153"/>
       <c r="Q3" s="57"/>
       <c r="R3" s="57"/>
     </row>
     <row r="5" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B5" s="113" t="s">
+      <c r="B5" s="182" t="s">
         <v>109</v>
       </c>
-      <c r="C5" s="114"/>
-      <c r="D5" s="114"/>
-      <c r="E5" s="114"/>
-      <c r="F5" s="114"/>
-      <c r="G5" s="114"/>
-      <c r="H5" s="114"/>
-      <c r="I5" s="114"/>
-      <c r="J5" s="114"/>
-      <c r="K5" s="114"/>
-      <c r="L5" s="115"/>
-      <c r="M5" s="113" t="s">
+      <c r="C5" s="183"/>
+      <c r="D5" s="183"/>
+      <c r="E5" s="183"/>
+      <c r="F5" s="183"/>
+      <c r="G5" s="183"/>
+      <c r="H5" s="183"/>
+      <c r="I5" s="183"/>
+      <c r="J5" s="183"/>
+      <c r="K5" s="183"/>
+      <c r="L5" s="184"/>
+      <c r="M5" s="182" t="s">
         <v>110</v>
       </c>
-      <c r="N5" s="114"/>
-      <c r="O5" s="114"/>
-      <c r="P5" s="114"/>
-      <c r="Q5" s="114"/>
-      <c r="R5" s="114"/>
-      <c r="S5" s="114"/>
-      <c r="T5" s="114"/>
-      <c r="U5" s="114"/>
-      <c r="V5" s="114"/>
-      <c r="W5" s="114"/>
-      <c r="X5" s="114"/>
-      <c r="Y5" s="115"/>
+      <c r="N5" s="183"/>
+      <c r="O5" s="183"/>
+      <c r="P5" s="183"/>
+      <c r="Q5" s="183"/>
+      <c r="R5" s="183"/>
+      <c r="S5" s="183"/>
+      <c r="T5" s="183"/>
+      <c r="U5" s="183"/>
+      <c r="V5" s="183"/>
+      <c r="W5" s="183"/>
+      <c r="X5" s="183"/>
+      <c r="Y5" s="184"/>
     </row>
     <row r="6" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B6" s="122"/>
-      <c r="C6" s="122"/>
-      <c r="D6" s="122"/>
-      <c r="E6" s="122"/>
-      <c r="F6" s="116" t="s">
+      <c r="B6" s="181"/>
+      <c r="C6" s="181"/>
+      <c r="D6" s="181"/>
+      <c r="E6" s="181"/>
+      <c r="F6" s="188" t="s">
         <v>26</v>
       </c>
-      <c r="G6" s="117"/>
-      <c r="H6" s="117"/>
-      <c r="I6" s="118"/>
-      <c r="J6" s="113" t="s">
+      <c r="G6" s="189"/>
+      <c r="H6" s="189"/>
+      <c r="I6" s="190"/>
+      <c r="J6" s="182" t="s">
         <v>29</v>
       </c>
-      <c r="K6" s="114"/>
-      <c r="L6" s="115"/>
+      <c r="K6" s="183"/>
+      <c r="L6" s="184"/>
       <c r="M6" s="87"/>
-      <c r="N6" s="119" t="s">
+      <c r="N6" s="178" t="s">
         <v>41</v>
       </c>
-      <c r="O6" s="120"/>
-      <c r="P6" s="119" t="s">
+      <c r="O6" s="179"/>
+      <c r="P6" s="178" t="s">
         <v>103</v>
       </c>
-      <c r="Q6" s="121"/>
-      <c r="R6" s="120"/>
+      <c r="Q6" s="180"/>
+      <c r="R6" s="179"/>
       <c r="S6" s="87"/>
-      <c r="T6" s="119" t="s">
+      <c r="T6" s="178" t="s">
         <v>120</v>
       </c>
-      <c r="U6" s="120"/>
-      <c r="V6" s="123"/>
-      <c r="W6" s="124"/>
-      <c r="X6" s="124"/>
-      <c r="Y6" s="125"/>
+      <c r="U6" s="179"/>
+      <c r="V6" s="185"/>
+      <c r="W6" s="186"/>
+      <c r="X6" s="186"/>
+      <c r="Y6" s="187"/>
     </row>
     <row r="7" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B7" s="75" t="s">
@@ -7830,9 +8675,6 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="T6:U6"/>
-    <mergeCell ref="M5:Y5"/>
-    <mergeCell ref="V6:Y6"/>
     <mergeCell ref="B2:P2"/>
     <mergeCell ref="B3:P3"/>
     <mergeCell ref="B5:L5"/>
@@ -7841,6 +8683,9 @@
     <mergeCell ref="N6:O6"/>
     <mergeCell ref="P6:R6"/>
     <mergeCell ref="B6:E6"/>
+    <mergeCell ref="T6:U6"/>
+    <mergeCell ref="M5:Y5"/>
+    <mergeCell ref="V6:Y6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -7963,36 +8808,36 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="103"/>
-      <c r="C2" s="103"/>
-      <c r="D2" s="103"/>
-      <c r="E2" s="103"/>
-      <c r="F2" s="103"/>
-      <c r="G2" s="103"/>
-      <c r="H2" s="103"/>
-      <c r="I2" s="103"/>
-      <c r="J2" s="103"/>
-      <c r="K2" s="103"/>
-      <c r="L2" s="103"/>
-      <c r="M2" s="103"/>
-      <c r="N2" s="103"/>
+      <c r="B2" s="152"/>
+      <c r="C2" s="152"/>
+      <c r="D2" s="152"/>
+      <c r="E2" s="152"/>
+      <c r="F2" s="152"/>
+      <c r="G2" s="152"/>
+      <c r="H2" s="152"/>
+      <c r="I2" s="152"/>
+      <c r="J2" s="152"/>
+      <c r="K2" s="152"/>
+      <c r="L2" s="152"/>
+      <c r="M2" s="152"/>
+      <c r="N2" s="152"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="104" t="s">
+      <c r="B3" s="153" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="104"/>
-      <c r="D3" s="104"/>
-      <c r="E3" s="104"/>
-      <c r="F3" s="104"/>
-      <c r="G3" s="104"/>
-      <c r="H3" s="104"/>
-      <c r="I3" s="104"/>
-      <c r="J3" s="104"/>
-      <c r="K3" s="104"/>
-      <c r="L3" s="104"/>
-      <c r="M3" s="104"/>
-      <c r="N3" s="104"/>
+      <c r="C3" s="153"/>
+      <c r="D3" s="153"/>
+      <c r="E3" s="153"/>
+      <c r="F3" s="153"/>
+      <c r="G3" s="153"/>
+      <c r="H3" s="153"/>
+      <c r="I3" s="153"/>
+      <c r="J3" s="153"/>
+      <c r="K3" s="153"/>
+      <c r="L3" s="153"/>
+      <c r="M3" s="153"/>
+      <c r="N3" s="153"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="44" t="s">
@@ -8065,18 +8910,18 @@
       </c>
     </row>
     <row r="2" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="103"/>
-      <c r="C2" s="103"/>
-      <c r="D2" s="103"/>
-      <c r="E2" s="103"/>
+      <c r="B2" s="152"/>
+      <c r="C2" s="152"/>
+      <c r="D2" s="152"/>
+      <c r="E2" s="152"/>
     </row>
     <row r="3" spans="2:5" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="104" t="s">
+      <c r="B3" s="153" t="s">
         <v>128</v>
       </c>
-      <c r="C3" s="104"/>
-      <c r="D3" s="104"/>
-      <c r="E3" s="104"/>
+      <c r="C3" s="153"/>
+      <c r="D3" s="153"/>
+      <c r="E3" s="153"/>
     </row>
     <row r="4" spans="2:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="64"/>
@@ -8137,40 +8982,40 @@
       </c>
     </row>
     <row r="2" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="103"/>
-      <c r="C2" s="103"/>
-      <c r="D2" s="103"/>
-      <c r="E2" s="103"/>
-      <c r="F2" s="103"/>
-      <c r="G2" s="103"/>
-      <c r="H2" s="103"/>
-      <c r="I2" s="103"/>
-      <c r="J2" s="103"/>
-      <c r="K2" s="103"/>
-      <c r="L2" s="103"/>
-      <c r="M2" s="103"/>
-      <c r="N2" s="103"/>
-      <c r="O2" s="103"/>
-      <c r="P2" s="103"/>
+      <c r="B2" s="152"/>
+      <c r="C2" s="152"/>
+      <c r="D2" s="152"/>
+      <c r="E2" s="152"/>
+      <c r="F2" s="152"/>
+      <c r="G2" s="152"/>
+      <c r="H2" s="152"/>
+      <c r="I2" s="152"/>
+      <c r="J2" s="152"/>
+      <c r="K2" s="152"/>
+      <c r="L2" s="152"/>
+      <c r="M2" s="152"/>
+      <c r="N2" s="152"/>
+      <c r="O2" s="152"/>
+      <c r="P2" s="152"/>
     </row>
     <row r="3" spans="2:16" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="104" t="s">
+      <c r="B3" s="153" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="104"/>
-      <c r="D3" s="104"/>
-      <c r="E3" s="104"/>
-      <c r="F3" s="104"/>
-      <c r="G3" s="104"/>
-      <c r="H3" s="104"/>
-      <c r="I3" s="104"/>
-      <c r="J3" s="104"/>
-      <c r="K3" s="104"/>
-      <c r="L3" s="104"/>
-      <c r="M3" s="104"/>
-      <c r="N3" s="104"/>
-      <c r="O3" s="104"/>
-      <c r="P3" s="104"/>
+      <c r="C3" s="153"/>
+      <c r="D3" s="153"/>
+      <c r="E3" s="153"/>
+      <c r="F3" s="153"/>
+      <c r="G3" s="153"/>
+      <c r="H3" s="153"/>
+      <c r="I3" s="153"/>
+      <c r="J3" s="153"/>
+      <c r="K3" s="153"/>
+      <c r="L3" s="153"/>
+      <c r="M3" s="153"/>
+      <c r="N3" s="153"/>
+      <c r="O3" s="153"/>
+      <c r="P3" s="153"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="44" t="s">
@@ -8244,14 +9089,14 @@
       </c>
     </row>
     <row r="2" spans="2:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="103"/>
-      <c r="C2" s="103"/>
-      <c r="D2" s="103"/>
-      <c r="E2" s="103"/>
-      <c r="F2" s="103"/>
-      <c r="G2" s="103"/>
-      <c r="H2" s="103"/>
-      <c r="I2" s="103"/>
+      <c r="B2" s="152"/>
+      <c r="C2" s="152"/>
+      <c r="D2" s="152"/>
+      <c r="E2" s="152"/>
+      <c r="F2" s="152"/>
+      <c r="G2" s="152"/>
+      <c r="H2" s="152"/>
+      <c r="I2" s="152"/>
     </row>
     <row r="3" spans="2:9" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="82" t="s">

</xml_diff>

<commit_message>
TRIEDA-1729 - Alterando textos "Área de Titulação" por "Área de Conhecimento"
</commit_message>
<xml_diff>
--- a/code/client/web/src/main/resources/templateExport.xlsx
+++ b/code/client/web/src/main/resources/templateExport.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="17070" windowHeight="5370" tabRatio="976" firstSheet="25" activeTab="27"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="17070" windowHeight="5370" tabRatio="976" firstSheet="12" activeTab="22"/>
   </bookViews>
   <sheets>
     <sheet name="Turnos" sheetId="49" r:id="rId1"/>
@@ -16,8 +16,8 @@
     <sheet name="Disponibilidades Salas" sheetId="36" r:id="rId7"/>
     <sheet name="Cursos" sheetId="5" r:id="rId8"/>
     <sheet name="Tipos de Curso" sheetId="50" r:id="rId9"/>
-    <sheet name="Areas de Titulacao" sheetId="16" r:id="rId10"/>
-    <sheet name="Curso - Area de Titulacao" sheetId="19" r:id="rId11"/>
+    <sheet name="Areas de Conhecimento" sheetId="16" r:id="rId10"/>
+    <sheet name="Curso - Area de Conhecimento" sheetId="19" r:id="rId11"/>
     <sheet name="Disciplinas" sheetId="6" r:id="rId12"/>
     <sheet name="Divisoes de Credito" sheetId="51" r:id="rId13"/>
     <sheet name="Equivalencias" sheetId="17" r:id="rId14"/>
@@ -1422,7 +1422,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="254">
   <si>
     <t>Planilha de Unidades</t>
   </si>
@@ -1568,9 +1568,6 @@
     <t>Titulação</t>
   </si>
   <si>
-    <t>Área de Titulação</t>
-  </si>
-  <si>
     <t>Tipo de Contrato</t>
   </si>
   <si>
@@ -1625,18 +1622,12 @@
     <t>Elimina</t>
   </si>
   <si>
-    <t>Planilha de Áreas de Titulação</t>
-  </si>
-  <si>
     <t>Campi de Trabalho</t>
   </si>
   <si>
     <t>Professor</t>
   </si>
   <si>
-    <t>Planilha de Curso - Área de Titulação</t>
-  </si>
-  <si>
     <t>Relatório Visão Curso</t>
   </si>
   <si>
@@ -1671,9 +1662,6 @@
   </si>
   <si>
     <t>Permite mais de uma Disciplina por Professor no Período</t>
-  </si>
-  <si>
-    <t>Código Área Titulação</t>
   </si>
   <si>
     <t>Código Disciplina</t>
@@ -2223,6 +2211,15 @@
   </si>
   <si>
     <t>Virtuais</t>
+  </si>
+  <si>
+    <t>Código Área Conhecimento</t>
+  </si>
+  <si>
+    <t>Planilha de Curso - Área de Conhecimento</t>
+  </si>
+  <si>
+    <t>Planilha de Áreas de Conhecimento</t>
   </si>
 </sst>
 </file>
@@ -2368,6 +2365,12 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="14"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -2376,12 +2379,6 @@
     <font>
       <b/>
       <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -2576,19 +2573,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="-0.249977111117893"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2613,6 +2604,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2808,6 +2805,24 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color theme="0" tint="-0.34998626667073579"/>
       </left>
@@ -2870,24 +2885,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="0" tint="-0.34998626667073579"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color theme="0" tint="-0.34998626667073579"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -3265,46 +3262,46 @@
     <xf numFmtId="0" fontId="18" fillId="31" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3319,53 +3316,53 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="36" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="35" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="37" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="36" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="38" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="37" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="38" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="35" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="35" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3385,44 +3382,44 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="28" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="28" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="28" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -3457,7 +3454,7 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="71684" name=":0_674" descr="https://plus.google.com/u/0/_/focus/photos/private/AIbEiAIAAABDCK-Xzbi8pY7DeSILdmNhcmRfcGhvdG8qKDIxMGNjNTM3ZWQ4NjZjNTU4NTk4YjQ0ZDUwM2EwNmUxOGE4OTQyMTIwAdCjuGFdYwQCNlcR6WXw_rsQlR6Q?sz=32"/>
+        <xdr:cNvPr id="71687" name=":0_674" descr="https://plus.google.com/u/0/_/focus/photos/private/AIbEiAIAAABDCK-Xzbi8pY7DeSILdmNhcmRfcGhvdG8qKDIxMGNjNTM3ZWQ4NjZjNTU4NTk4YjQ0ZDUwM2EwNmUxOGE4OTQyMTIwAdCjuGFdYwQCNlcR6WXw_rsQlR6Q?sz=32"/>
         <xdr:cNvSpPr>
           <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -3805,7 +3802,7 @@
   <sheetData>
     <row r="1" spans="2:11" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3820,7 +3817,7 @@
     </row>
     <row r="3" spans="2:11" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="153" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="C3" s="153"/>
       <c r="D3" s="153"/>
@@ -3855,12 +3852,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:P6"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.5703125" customWidth="1"/>
-    <col min="2" max="2" width="24.42578125" customWidth="1"/>
+    <col min="2" max="2" width="27.7109375" customWidth="1"/>
     <col min="3" max="3" width="69.5703125" customWidth="1"/>
     <col min="4" max="4" width="5.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
@@ -3873,7 +3872,7 @@
   <sheetData>
     <row r="1" spans="2:16" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3895,7 +3894,7 @@
     </row>
     <row r="3" spans="2:16" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="153" t="s">
-        <v>67</v>
+        <v>253</v>
       </c>
       <c r="C3" s="153"/>
       <c r="D3" s="153"/>
@@ -3914,7 +3913,7 @@
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
-        <v>83</v>
+        <v>251</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>23</v>
@@ -3938,7 +3937,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:P6"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3955,7 +3956,7 @@
   <sheetData>
     <row r="1" spans="2:16" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3977,7 +3978,7 @@
     </row>
     <row r="3" spans="2:16" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="153" t="s">
-        <v>70</v>
+        <v>252</v>
       </c>
       <c r="C3" s="153"/>
       <c r="D3" s="153"/>
@@ -3999,7 +4000,7 @@
         <v>24</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>48</v>
+        <v>217</v>
       </c>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
@@ -4043,7 +4044,7 @@
   <sheetData>
     <row r="1" spans="2:16" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -4084,10 +4085,10 @@
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="44" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>16</v>
@@ -4096,7 +4097,7 @@
         <v>17</v>
       </c>
       <c r="F5" s="45" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="G5" s="45" t="s">
         <v>8</v>
@@ -4111,16 +4112,16 @@
         <v>21</v>
       </c>
       <c r="K5" s="90" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="L5" s="90" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="M5" s="45" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="N5" s="45" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
@@ -4166,7 +4167,7 @@
   <sheetData>
     <row r="1" spans="2:11" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -4183,7 +4184,7 @@
     </row>
     <row r="3" spans="2:11" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="82" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="C3" s="82"/>
       <c r="D3" s="82"/>
@@ -4200,25 +4201,25 @@
         <v>41</v>
       </c>
       <c r="C5" s="101" t="s">
+        <v>227</v>
+      </c>
+      <c r="D5" s="101" t="s">
+        <v>228</v>
+      </c>
+      <c r="E5" s="101" t="s">
+        <v>229</v>
+      </c>
+      <c r="F5" s="101" t="s">
+        <v>230</v>
+      </c>
+      <c r="G5" s="101" t="s">
         <v>231</v>
       </c>
-      <c r="D5" s="101" t="s">
+      <c r="H5" s="101" t="s">
         <v>232</v>
       </c>
-      <c r="E5" s="101" t="s">
+      <c r="I5" s="101" t="s">
         <v>233</v>
-      </c>
-      <c r="F5" s="101" t="s">
-        <v>234</v>
-      </c>
-      <c r="G5" s="101" t="s">
-        <v>235</v>
-      </c>
-      <c r="H5" s="101" t="s">
-        <v>236</v>
-      </c>
-      <c r="I5" s="101" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
@@ -4265,7 +4266,7 @@
   <sheetData>
     <row r="1" spans="2:16" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -4287,7 +4288,7 @@
     </row>
     <row r="3" spans="2:16" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="153" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C3" s="153"/>
       <c r="D3" s="153"/>
@@ -4306,10 +4307,10 @@
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="C5" s="45" t="s">
         <v>65</v>
-      </c>
-      <c r="C5" s="45" t="s">
-        <v>66</v>
       </c>
       <c r="D5" s="90" t="s">
         <v>24</v>
@@ -4353,7 +4354,7 @@
   <sheetData>
     <row r="1" spans="2:11" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -4384,10 +4385,10 @@
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
@@ -4429,7 +4430,7 @@
   <sheetData>
     <row r="1" spans="2:14" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -4466,13 +4467,13 @@
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>25</v>
@@ -4481,7 +4482,7 @@
         <v>26</v>
       </c>
       <c r="G5" s="47" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
@@ -4525,7 +4526,7 @@
   <sheetData>
     <row r="1" spans="2:12" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -4543,7 +4544,7 @@
     </row>
     <row r="3" spans="2:12" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="153" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C3" s="153"/>
       <c r="D3" s="153"/>
@@ -4564,10 +4565,10 @@
         <v>25</v>
       </c>
       <c r="D5" s="97" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E5" s="97" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
@@ -4609,7 +4610,7 @@
   <sheetData>
     <row r="1" spans="2:12" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -4627,7 +4628,7 @@
     </row>
     <row r="3" spans="2:12" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="153" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C3" s="153"/>
       <c r="D3" s="153"/>
@@ -4648,10 +4649,10 @@
         <v>25</v>
       </c>
       <c r="D5" s="97" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E5" s="97" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
@@ -4693,7 +4694,7 @@
   <sheetData>
     <row r="1" spans="2:12" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -4711,7 +4712,7 @@
     </row>
     <row r="3" spans="2:12" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="153" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="C3" s="153"/>
       <c r="D3" s="153"/>
@@ -4726,10 +4727,10 @@
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B5" s="70" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C5" s="70" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D5" s="70" t="s">
         <v>28</v>
@@ -4738,7 +4739,7 @@
         <v>25</v>
       </c>
       <c r="F5" s="98" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
@@ -4783,12 +4784,12 @@
   <sheetData>
     <row r="1" spans="2:14" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="152" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C2" s="152"/>
       <c r="D2" s="152"/>
@@ -4822,7 +4823,7 @@
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="44" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>1</v>
@@ -4884,7 +4885,7 @@
   <sheetData>
     <row r="1" spans="2:14" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -4921,13 +4922,13 @@
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>28</v>
@@ -4936,25 +4937,25 @@
         <v>25</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="H5" s="4" t="s">
         <v>29</v>
       </c>
       <c r="I5" s="45" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J5" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="M5" s="4" t="s">
         <v>103</v>
-      </c>
-      <c r="K5" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="L5" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="M5" s="4" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
@@ -4998,7 +4999,7 @@
   <sheetData>
     <row r="1" spans="2:5" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -5009,7 +5010,7 @@
     </row>
     <row r="3" spans="2:5" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="153" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C3" s="153"/>
       <c r="D3" s="153"/>
@@ -5017,13 +5018,13 @@
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="60" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C5" s="59" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D5" s="59" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
@@ -5062,7 +5063,7 @@
   <sheetData>
     <row r="1" spans="2:14" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -5082,7 +5083,7 @@
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="153" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C3" s="153"/>
       <c r="D3" s="153"/>
@@ -5099,13 +5100,13 @@
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>28</v>
@@ -5114,22 +5115,22 @@
         <v>25</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="L5" s="155" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="M5" s="155"/>
     </row>
@@ -5159,8 +5160,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O6"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5182,7 +5183,7 @@
   <sheetData>
     <row r="1" spans="2:15" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="2:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -5203,7 +5204,7 @@
     </row>
     <row r="3" spans="2:15" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="153" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C3" s="153"/>
       <c r="D3" s="153"/>
@@ -5224,10 +5225,10 @@
         <v>44</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D5" s="45" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E5" s="45" t="s">
         <v>45</v>
@@ -5239,22 +5240,22 @@
         <v>47</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>48</v>
+        <v>217</v>
       </c>
       <c r="I5" s="45" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J5" s="45" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="K5" s="45" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="L5" s="94" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="M5" s="94" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.25">
@@ -5300,7 +5301,7 @@
   <sheetData>
     <row r="1" spans="2:5" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -5311,7 +5312,7 @@
     </row>
     <row r="3" spans="2:5" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="153" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C3" s="153"/>
       <c r="D3" s="153"/>
@@ -5325,13 +5326,13 @@
         <v>44</v>
       </c>
       <c r="C5" s="44" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="D5" s="61" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="E5" s="61" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6" spans="2:5" customFormat="1" x14ac:dyDescent="0.25">
@@ -5373,7 +5374,7 @@
   <sheetData>
     <row r="1" spans="2:14" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -5393,7 +5394,7 @@
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="153" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C3" s="153"/>
       <c r="D3" s="153"/>
@@ -5410,13 +5411,13 @@
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
@@ -5457,7 +5458,7 @@
   <sheetData>
     <row r="1" spans="2:14" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -5477,7 +5478,7 @@
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="153" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C3" s="153"/>
       <c r="D3" s="153"/>
@@ -5494,16 +5495,16 @@
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D5" s="45" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" s="45" t="s">
         <v>50</v>
-      </c>
-      <c r="E5" s="45" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
@@ -5539,7 +5540,7 @@
   <sheetData>
     <row r="1" spans="2:16" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -5561,7 +5562,7 @@
     </row>
     <row r="3" spans="2:16" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="153" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="C3" s="153"/>
       <c r="D3" s="153"/>
@@ -5580,7 +5581,7 @@
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="104" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
@@ -5600,7 +5601,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:P60"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A55" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A55" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="A70" sqref="A61:IV70"/>
     </sheetView>
   </sheetViews>
@@ -5615,7 +5616,7 @@
   <sheetData>
     <row r="1" spans="2:16" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -5637,7 +5638,7 @@
     </row>
     <row r="3" spans="2:16" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="153" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="C3" s="153"/>
       <c r="D3" s="153"/>
@@ -5675,99 +5676,99 @@
       <c r="E5" s="138"/>
     </row>
     <row r="6" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="156" t="s">
-        <v>248</v>
+      <c r="B6" s="164" t="s">
+        <v>244</v>
       </c>
       <c r="C6" s="106"/>
       <c r="D6" s="107"/>
       <c r="E6" s="139"/>
     </row>
     <row r="7" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="157"/>
+      <c r="B7" s="165"/>
       <c r="C7" s="108"/>
       <c r="D7" s="109"/>
       <c r="E7" s="140"/>
     </row>
     <row r="8" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="157"/>
+      <c r="B8" s="165"/>
       <c r="C8" s="108"/>
       <c r="D8" s="109"/>
       <c r="E8" s="141"/>
     </row>
     <row r="9" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="157"/>
+      <c r="B9" s="165"/>
       <c r="C9" s="108"/>
       <c r="D9" s="109"/>
       <c r="E9" s="140"/>
     </row>
     <row r="10" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="157"/>
+      <c r="B10" s="165"/>
       <c r="C10" s="108"/>
       <c r="D10" s="109"/>
       <c r="E10" s="140"/>
     </row>
     <row r="11" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B11" s="157"/>
+      <c r="B11" s="165"/>
       <c r="C11" s="108"/>
       <c r="D11" s="109"/>
       <c r="E11" s="140"/>
     </row>
     <row r="12" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="157"/>
+      <c r="B12" s="165"/>
       <c r="C12" s="108"/>
       <c r="D12" s="109"/>
       <c r="E12" s="140"/>
     </row>
     <row r="13" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B13" s="157"/>
+      <c r="B13" s="165"/>
       <c r="C13" s="108"/>
       <c r="D13" s="109"/>
       <c r="E13" s="140"/>
     </row>
     <row r="14" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="157"/>
+      <c r="B14" s="165"/>
       <c r="C14" s="108"/>
       <c r="D14" s="109"/>
       <c r="E14" s="140"/>
     </row>
     <row r="15" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B15" s="157"/>
+      <c r="B15" s="165"/>
       <c r="C15" s="108"/>
       <c r="D15" s="109"/>
       <c r="E15" s="140"/>
     </row>
     <row r="16" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="157"/>
+      <c r="B16" s="165"/>
       <c r="C16" s="108"/>
       <c r="D16" s="109"/>
       <c r="E16" s="140"/>
     </row>
     <row r="17" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B17" s="157"/>
+      <c r="B17" s="165"/>
       <c r="C17" s="108"/>
       <c r="D17" s="109"/>
       <c r="E17" s="140"/>
     </row>
     <row r="18" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B18" s="157"/>
+      <c r="B18" s="165"/>
       <c r="C18" s="108"/>
       <c r="D18" s="109"/>
       <c r="E18" s="140"/>
     </row>
     <row r="19" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B19" s="157"/>
+      <c r="B19" s="165"/>
       <c r="C19" s="108"/>
       <c r="D19" s="109"/>
       <c r="E19" s="140"/>
     </row>
     <row r="20" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B20" s="157"/>
+      <c r="B20" s="165"/>
       <c r="C20" s="108"/>
       <c r="D20" s="109"/>
       <c r="E20" s="140"/>
     </row>
     <row r="21" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B21" s="157"/>
+      <c r="B21" s="165"/>
       <c r="C21" s="110"/>
       <c r="D21" s="111"/>
       <c r="E21" s="142"/>
@@ -5779,39 +5780,39 @@
       <c r="E22" s="1"/>
     </row>
     <row r="23" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B23" s="158" t="s">
-        <v>249</v>
+      <c r="B23" s="166" t="s">
+        <v>245</v>
       </c>
       <c r="C23" s="114"/>
       <c r="D23" s="115"/>
       <c r="E23" s="143"/>
     </row>
     <row r="24" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B24" s="159"/>
+      <c r="B24" s="167"/>
       <c r="C24" s="116"/>
       <c r="D24" s="117"/>
       <c r="E24" s="141"/>
     </row>
     <row r="25" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B25" s="159"/>
+      <c r="B25" s="167"/>
       <c r="C25" s="116"/>
       <c r="D25" s="117"/>
       <c r="E25" s="144"/>
     </row>
     <row r="26" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B26" s="159"/>
+      <c r="B26" s="167"/>
       <c r="C26" s="118"/>
       <c r="D26" s="117"/>
       <c r="E26" s="144"/>
     </row>
     <row r="27" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B27" s="159"/>
+      <c r="B27" s="167"/>
       <c r="C27" s="118"/>
       <c r="D27" s="117"/>
       <c r="E27" s="144"/>
     </row>
     <row r="28" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B28" s="159"/>
+      <c r="B28" s="167"/>
       <c r="C28" s="119"/>
       <c r="D28" s="120"/>
       <c r="E28" s="145"/>
@@ -5823,51 +5824,51 @@
       <c r="E29" s="1"/>
     </row>
     <row r="30" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B30" s="160" t="s">
-        <v>250</v>
+      <c r="B30" s="168" t="s">
+        <v>246</v>
       </c>
       <c r="C30" s="121"/>
       <c r="D30" s="122"/>
       <c r="E30" s="146"/>
     </row>
     <row r="31" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B31" s="161"/>
+      <c r="B31" s="169"/>
       <c r="C31" s="123"/>
       <c r="D31" s="124"/>
       <c r="E31" s="147"/>
     </row>
     <row r="32" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B32" s="161"/>
+      <c r="B32" s="169"/>
       <c r="C32" s="123"/>
       <c r="D32" s="124"/>
       <c r="E32" s="147"/>
     </row>
     <row r="33" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B33" s="161"/>
+      <c r="B33" s="169"/>
       <c r="C33" s="123"/>
       <c r="D33" s="124"/>
       <c r="E33" s="141"/>
     </row>
     <row r="34" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B34" s="161"/>
+      <c r="B34" s="169"/>
       <c r="C34" s="123"/>
       <c r="D34" s="124"/>
       <c r="E34" s="144"/>
     </row>
     <row r="35" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B35" s="161"/>
+      <c r="B35" s="169"/>
       <c r="C35" s="123"/>
       <c r="D35" s="124"/>
       <c r="E35" s="144"/>
     </row>
     <row r="36" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B36" s="161"/>
+      <c r="B36" s="169"/>
       <c r="C36" s="123"/>
       <c r="D36" s="124"/>
       <c r="E36" s="140"/>
     </row>
     <row r="37" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B37" s="161"/>
+      <c r="B37" s="169"/>
       <c r="C37" s="125"/>
       <c r="D37" s="126"/>
       <c r="E37" s="142"/>
@@ -5879,39 +5880,39 @@
       <c r="E38" s="1"/>
     </row>
     <row r="39" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B39" s="162" t="s">
-        <v>251</v>
+      <c r="B39" s="170" t="s">
+        <v>247</v>
       </c>
       <c r="C39" s="127"/>
       <c r="D39" s="128"/>
       <c r="E39" s="148"/>
     </row>
     <row r="40" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="163"/>
+      <c r="B40" s="171"/>
       <c r="C40" s="129"/>
       <c r="D40" s="130"/>
       <c r="E40" s="141"/>
     </row>
     <row r="41" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B41" s="163"/>
+      <c r="B41" s="171"/>
       <c r="C41" s="129"/>
       <c r="D41" s="130"/>
       <c r="E41" s="141"/>
     </row>
     <row r="42" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B42" s="163"/>
+      <c r="B42" s="171"/>
       <c r="C42" s="129"/>
       <c r="D42" s="130"/>
       <c r="E42" s="141"/>
     </row>
     <row r="43" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B43" s="163"/>
+      <c r="B43" s="171"/>
       <c r="C43" s="129"/>
       <c r="D43" s="130"/>
       <c r="E43" s="141"/>
     </row>
     <row r="44" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B44" s="163"/>
+      <c r="B44" s="171"/>
       <c r="C44" s="131"/>
       <c r="D44" s="132"/>
       <c r="E44" s="149"/>
@@ -5923,100 +5924,100 @@
       <c r="E45" s="1"/>
     </row>
     <row r="46" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B46" s="164" t="s">
-        <v>252</v>
-      </c>
-      <c r="C46" s="167" t="s">
-        <v>113</v>
+      <c r="B46" s="156" t="s">
+        <v>248</v>
+      </c>
+      <c r="C46" s="159" t="s">
+        <v>109</v>
       </c>
       <c r="D46" s="133"/>
       <c r="E46" s="139"/>
     </row>
     <row r="47" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="165"/>
-      <c r="C47" s="168"/>
+      <c r="B47" s="157"/>
+      <c r="C47" s="160"/>
       <c r="D47" s="134"/>
       <c r="E47" s="140"/>
     </row>
     <row r="48" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B48" s="165"/>
-      <c r="C48" s="168"/>
+      <c r="B48" s="157"/>
+      <c r="C48" s="160"/>
       <c r="D48" s="134"/>
       <c r="E48" s="140"/>
     </row>
     <row r="49" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B49" s="165"/>
-      <c r="C49" s="168"/>
+      <c r="B49" s="157"/>
+      <c r="C49" s="160"/>
       <c r="D49" s="134"/>
       <c r="E49" s="140"/>
     </row>
     <row r="50" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B50" s="165"/>
-      <c r="C50" s="168"/>
+      <c r="B50" s="157"/>
+      <c r="C50" s="160"/>
       <c r="D50" s="134"/>
       <c r="E50" s="140"/>
     </row>
     <row r="51" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B51" s="165"/>
-      <c r="C51" s="169" t="s">
-        <v>253</v>
+      <c r="B51" s="157"/>
+      <c r="C51" s="161" t="s">
+        <v>249</v>
       </c>
       <c r="D51" s="135"/>
       <c r="E51" s="150"/>
     </row>
     <row r="52" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B52" s="165"/>
-      <c r="C52" s="168"/>
+      <c r="B52" s="157"/>
+      <c r="C52" s="160"/>
       <c r="D52" s="134"/>
       <c r="E52" s="140"/>
     </row>
     <row r="53" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B53" s="165"/>
-      <c r="C53" s="168"/>
+      <c r="B53" s="157"/>
+      <c r="C53" s="160"/>
       <c r="D53" s="134"/>
       <c r="E53" s="140"/>
     </row>
     <row r="54" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B54" s="165"/>
-      <c r="C54" s="168"/>
+      <c r="B54" s="157"/>
+      <c r="C54" s="160"/>
       <c r="D54" s="134"/>
       <c r="E54" s="140"/>
     </row>
     <row r="55" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B55" s="165"/>
-      <c r="C55" s="170"/>
+      <c r="B55" s="157"/>
+      <c r="C55" s="162"/>
       <c r="D55" s="136"/>
       <c r="E55" s="151"/>
     </row>
     <row r="56" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B56" s="165"/>
-      <c r="C56" s="168" t="s">
-        <v>254</v>
+      <c r="B56" s="157"/>
+      <c r="C56" s="160" t="s">
+        <v>250</v>
       </c>
       <c r="D56" s="134"/>
       <c r="E56" s="140"/>
     </row>
     <row r="57" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B57" s="165"/>
-      <c r="C57" s="168"/>
+      <c r="B57" s="157"/>
+      <c r="C57" s="160"/>
       <c r="D57" s="134"/>
       <c r="E57" s="140"/>
     </row>
     <row r="58" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B58" s="165"/>
-      <c r="C58" s="168"/>
+      <c r="B58" s="157"/>
+      <c r="C58" s="160"/>
       <c r="D58" s="134"/>
       <c r="E58" s="140"/>
     </row>
     <row r="59" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B59" s="165"/>
-      <c r="C59" s="168"/>
+      <c r="B59" s="157"/>
+      <c r="C59" s="160"/>
       <c r="D59" s="134"/>
       <c r="E59" s="140"/>
     </row>
     <row r="60" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B60" s="166"/>
-      <c r="C60" s="171"/>
+      <c r="B60" s="158"/>
+      <c r="C60" s="163"/>
       <c r="D60" s="137"/>
       <c r="E60" s="142"/>
     </row>
@@ -6071,7 +6072,7 @@
   <sheetData>
     <row r="1" spans="2:18" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="2:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -6093,7 +6094,7 @@
     </row>
     <row r="3" spans="2:18" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="153" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C3" s="153"/>
       <c r="D3" s="153"/>
@@ -6130,37 +6131,37 @@
         <v>26</v>
       </c>
       <c r="H5" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="I5" s="4" t="s">
         <v>52</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>53</v>
       </c>
       <c r="J5" s="4" t="s">
         <v>41</v>
       </c>
       <c r="K5" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="L5" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="L5" s="4" t="s">
+      <c r="M5" s="53" t="s">
+        <v>91</v>
+      </c>
+      <c r="N5" s="53" t="s">
+        <v>84</v>
+      </c>
+      <c r="O5" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="M5" s="53" t="s">
-        <v>95</v>
-      </c>
-      <c r="N5" s="53" t="s">
-        <v>88</v>
-      </c>
-      <c r="O5" s="4" t="s">
+      <c r="P5" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="P5" s="4" t="s">
+      <c r="Q5" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="Q5" s="4" t="s">
+      <c r="R5" s="4" t="s">
         <v>58</v>
-      </c>
-      <c r="R5" s="4" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.25">
@@ -6212,12 +6213,12 @@
   <sheetData>
     <row r="1" spans="2:13" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="2:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="152" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="C2" s="152"/>
       <c r="D2" s="152"/>
@@ -6233,7 +6234,7 @@
     </row>
     <row r="3" spans="2:13" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="153" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C3" s="153"/>
       <c r="D3" s="153"/>
@@ -6249,7 +6250,7 @@
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B5" s="70" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.25">
@@ -6292,7 +6293,7 @@
   <sheetData>
     <row r="1" spans="2:14" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -6312,7 +6313,7 @@
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="153" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C3" s="153"/>
       <c r="D3" s="153"/>
@@ -6335,31 +6336,31 @@
         <v>26</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>41</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I5" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="J5" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="J5" s="4" t="s">
+      <c r="K5" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="K5" s="4" t="s">
+      <c r="L5" s="4" t="s">
         <v>58</v>
-      </c>
-      <c r="L5" s="4" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
@@ -6411,7 +6412,7 @@
   <sheetData>
     <row r="1" spans="2:14" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -6431,7 +6432,7 @@
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="153" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C3" s="153"/>
       <c r="D3" s="153"/>
@@ -6451,34 +6452,34 @@
         <v>2</v>
       </c>
       <c r="C5" s="74" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D5" s="74" t="s">
+        <v>136</v>
+      </c>
+      <c r="E5" s="74" t="s">
+        <v>137</v>
+      </c>
+      <c r="F5" s="74" t="s">
+        <v>138</v>
+      </c>
+      <c r="G5" s="74" t="s">
+        <v>139</v>
+      </c>
+      <c r="H5" s="74" t="s">
         <v>140</v>
       </c>
-      <c r="E5" s="74" t="s">
+      <c r="I5" s="74" t="s">
         <v>141</v>
       </c>
-      <c r="F5" s="74" t="s">
+      <c r="J5" s="74" t="s">
         <v>142</v>
       </c>
-      <c r="G5" s="74" t="s">
+      <c r="K5" s="74" t="s">
         <v>143</v>
       </c>
-      <c r="H5" s="74" t="s">
+      <c r="L5" s="74" t="s">
         <v>144</v>
-      </c>
-      <c r="I5" s="74" t="s">
-        <v>145</v>
-      </c>
-      <c r="J5" s="74" t="s">
-        <v>146</v>
-      </c>
-      <c r="K5" s="74" t="s">
-        <v>147</v>
-      </c>
-      <c r="L5" s="74" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
@@ -6527,7 +6528,7 @@
   <sheetData>
     <row r="1" spans="2:10" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -6543,7 +6544,7 @@
     </row>
     <row r="3" spans="2:10" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="153" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C3" s="153"/>
       <c r="D3" s="153"/>
@@ -6562,22 +6563,22 @@
         <v>26</v>
       </c>
       <c r="D5" s="74" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E5" s="74" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="F5" s="74" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="G5" s="74" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="H5" s="74" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="I5" s="74" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
@@ -6633,7 +6634,7 @@
   <sheetData>
     <row r="1" spans="2:20" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="2:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -6651,7 +6652,7 @@
     </row>
     <row r="3" spans="2:20" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="153" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C3" s="153"/>
       <c r="D3" s="153"/>
@@ -6669,58 +6670,58 @@
         <v>2</v>
       </c>
       <c r="C5" s="79" t="s">
+        <v>150</v>
+      </c>
+      <c r="D5" s="79" t="s">
+        <v>136</v>
+      </c>
+      <c r="E5" s="79" t="s">
+        <v>151</v>
+      </c>
+      <c r="F5" s="79" t="s">
+        <v>152</v>
+      </c>
+      <c r="G5" s="79" t="s">
+        <v>153</v>
+      </c>
+      <c r="H5" s="79" t="s">
         <v>154</v>
       </c>
-      <c r="D5" s="79" t="s">
-        <v>140</v>
-      </c>
-      <c r="E5" s="79" t="s">
+      <c r="I5" s="79" t="s">
+        <v>158</v>
+      </c>
+      <c r="J5" s="79" t="s">
+        <v>159</v>
+      </c>
+      <c r="K5" s="79" t="s">
+        <v>160</v>
+      </c>
+      <c r="L5" s="79" t="s">
         <v>155</v>
       </c>
-      <c r="F5" s="79" t="s">
+      <c r="M5" s="79" t="s">
         <v>156</v>
       </c>
-      <c r="G5" s="79" t="s">
+      <c r="N5" s="79" t="s">
         <v>157</v>
       </c>
-      <c r="H5" s="79" t="s">
-        <v>158</v>
-      </c>
-      <c r="I5" s="79" t="s">
-        <v>162</v>
-      </c>
-      <c r="J5" s="79" t="s">
-        <v>163</v>
-      </c>
-      <c r="K5" s="79" t="s">
-        <v>164</v>
-      </c>
-      <c r="L5" s="79" t="s">
-        <v>159</v>
-      </c>
-      <c r="M5" s="79" t="s">
-        <v>160</v>
-      </c>
-      <c r="N5" s="79" t="s">
-        <v>161</v>
-      </c>
       <c r="O5" s="86" t="s">
+        <v>170</v>
+      </c>
+      <c r="P5" s="86" t="s">
+        <v>171</v>
+      </c>
+      <c r="Q5" s="86" t="s">
+        <v>175</v>
+      </c>
+      <c r="R5" s="86" t="s">
+        <v>172</v>
+      </c>
+      <c r="S5" s="86" t="s">
+        <v>173</v>
+      </c>
+      <c r="T5" s="86" t="s">
         <v>174</v>
-      </c>
-      <c r="P5" s="86" t="s">
-        <v>175</v>
-      </c>
-      <c r="Q5" s="86" t="s">
-        <v>179</v>
-      </c>
-      <c r="R5" s="86" t="s">
-        <v>176</v>
-      </c>
-      <c r="S5" s="86" t="s">
-        <v>177</v>
-      </c>
-      <c r="T5" s="86" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.25">
@@ -6774,12 +6775,12 @@
   <sheetData>
     <row r="1" spans="2:6" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="2:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="153" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="C2" s="153"/>
       <c r="D2" s="153"/>
@@ -6795,19 +6796,19 @@
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="99" t="s">
+        <v>200</v>
+      </c>
+      <c r="C5" s="63" t="s">
+        <v>201</v>
+      </c>
+      <c r="D5" s="63" t="s">
+        <v>202</v>
+      </c>
+      <c r="E5" s="63" t="s">
+        <v>203</v>
+      </c>
+      <c r="F5" s="63" t="s">
         <v>204</v>
-      </c>
-      <c r="C5" s="63" t="s">
-        <v>205</v>
-      </c>
-      <c r="D5" s="63" t="s">
-        <v>206</v>
-      </c>
-      <c r="E5" s="63" t="s">
-        <v>207</v>
-      </c>
-      <c r="F5" s="63" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
@@ -6844,12 +6845,12 @@
   <sheetData>
     <row r="1" spans="2:9" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="2:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="153" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="C2" s="153"/>
       <c r="D2" s="153"/>
@@ -6871,13 +6872,13 @@
     </row>
     <row r="5" spans="2:9" ht="27" x14ac:dyDescent="0.25">
       <c r="B5" s="99" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="C5" s="100" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="D5" s="100" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
@@ -6916,7 +6917,7 @@
   <sheetData>
     <row r="1" spans="2:9" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="2:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -6931,7 +6932,7 @@
     </row>
     <row r="3" spans="2:9" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="153" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C3" s="153"/>
       <c r="D3" s="153"/>
@@ -6943,28 +6944,28 @@
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="88" t="s">
+        <v>177</v>
+      </c>
+      <c r="C5" s="88" t="s">
+        <v>178</v>
+      </c>
+      <c r="D5" s="88" t="s">
+        <v>179</v>
+      </c>
+      <c r="E5" s="88" t="s">
+        <v>180</v>
+      </c>
+      <c r="F5" s="88" t="s">
         <v>181</v>
       </c>
-      <c r="C5" s="88" t="s">
+      <c r="G5" s="88" t="s">
         <v>182</v>
       </c>
-      <c r="D5" s="88" t="s">
+      <c r="H5" s="88" t="s">
         <v>183</v>
       </c>
-      <c r="E5" s="88" t="s">
+      <c r="I5" s="88" t="s">
         <v>184</v>
-      </c>
-      <c r="F5" s="88" t="s">
-        <v>185</v>
-      </c>
-      <c r="G5" s="88" t="s">
-        <v>186</v>
-      </c>
-      <c r="H5" s="88" t="s">
-        <v>187</v>
-      </c>
-      <c r="I5" s="88" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
@@ -7011,7 +7012,7 @@
   <sheetData>
     <row r="1" spans="2:11" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -7028,7 +7029,7 @@
     </row>
     <row r="3" spans="2:11" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="153" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C3" s="153"/>
       <c r="D3" s="153"/>
@@ -7054,11 +7055,11 @@
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="H5" s="172" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="I5" s="173"/>
       <c r="J5" s="172" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="K5" s="173"/>
     </row>
@@ -7070,28 +7071,28 @@
         <v>24</v>
       </c>
       <c r="D6" s="85" t="s">
+        <v>162</v>
+      </c>
+      <c r="E6" s="85" t="s">
+        <v>163</v>
+      </c>
+      <c r="F6" s="85" t="s">
+        <v>109</v>
+      </c>
+      <c r="G6" s="85" t="s">
+        <v>109</v>
+      </c>
+      <c r="H6" s="85" t="s">
+        <v>164</v>
+      </c>
+      <c r="I6" s="85" t="s">
+        <v>165</v>
+      </c>
+      <c r="J6" s="85" t="s">
         <v>166</v>
       </c>
-      <c r="E6" s="85" t="s">
+      <c r="K6" s="85" t="s">
         <v>167</v>
-      </c>
-      <c r="F6" s="85" t="s">
-        <v>113</v>
-      </c>
-      <c r="G6" s="85" t="s">
-        <v>113</v>
-      </c>
-      <c r="H6" s="85" t="s">
-        <v>168</v>
-      </c>
-      <c r="I6" s="85" t="s">
-        <v>169</v>
-      </c>
-      <c r="J6" s="85" t="s">
-        <v>170</v>
-      </c>
-      <c r="K6" s="85" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
@@ -7135,12 +7136,12 @@
   <sheetData>
     <row r="1" spans="2:8" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="2:8" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="153" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="C2" s="153"/>
       <c r="D2" s="153"/>
@@ -7160,10 +7161,10 @@
     </row>
     <row r="5" spans="2:8" ht="27" x14ac:dyDescent="0.25">
       <c r="B5" s="100" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C5" s="100" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
@@ -7196,12 +7197,12 @@
   <sheetData>
     <row r="1" spans="2:8" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="2:8" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="153" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="C2" s="153"/>
       <c r="D2" s="153"/>
@@ -7221,10 +7222,10 @@
     </row>
     <row r="5" spans="2:8" ht="27" x14ac:dyDescent="0.25">
       <c r="B5" s="100" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="C5" s="100" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
@@ -7263,12 +7264,12 @@
   <sheetData>
     <row r="1" spans="2:14" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="152" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C2" s="152"/>
       <c r="D2" s="152"/>
@@ -7302,13 +7303,13 @@
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="44" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
@@ -7344,12 +7345,12 @@
   <sheetData>
     <row r="1" spans="2:8" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="2:8" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="153" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="C2" s="153"/>
       <c r="D2" s="153"/>
@@ -7369,10 +7370,10 @@
     </row>
     <row r="5" spans="2:8" ht="27" x14ac:dyDescent="0.25">
       <c r="B5" s="100" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="C5" s="100" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
@@ -7405,12 +7406,12 @@
   <sheetData>
     <row r="1" spans="2:8" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="2:8" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="153" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="C2" s="153"/>
       <c r="D2" s="153"/>
@@ -7433,7 +7434,7 @@
         <v>47</v>
       </c>
       <c r="C5" s="100" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
@@ -7466,12 +7467,12 @@
   <sheetData>
     <row r="1" spans="2:8" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="2:8" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="153" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="C2" s="153"/>
       <c r="D2" s="153"/>
@@ -7491,10 +7492,10 @@
     </row>
     <row r="5" spans="2:8" ht="27" x14ac:dyDescent="0.25">
       <c r="B5" s="100" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="C5" s="100" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
@@ -7529,12 +7530,12 @@
   <sheetData>
     <row r="1" spans="2:8" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="2:8" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="153" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="C2" s="153"/>
       <c r="D2" s="153"/>
@@ -7554,16 +7555,16 @@
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" s="100" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="C5" s="100" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="D5" s="100" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="E5" s="100" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
@@ -7600,12 +7601,12 @@
   <sheetData>
     <row r="1" spans="2:8" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="2:8" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="153" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="C2" s="153"/>
       <c r="D2" s="153"/>
@@ -7625,16 +7626,16 @@
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" s="100" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="C5" s="100" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="D5" s="100" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="E5" s="100" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
@@ -7671,7 +7672,7 @@
   <sheetData>
     <row r="1" spans="2:26" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="Z1" s="38"/>
     </row>
@@ -7805,7 +7806,7 @@
   <sheetData>
     <row r="1" spans="2:26" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="Z1" s="38"/>
     </row>
@@ -7857,7 +7858,7 @@
     </row>
     <row r="6" spans="2:26" x14ac:dyDescent="0.25">
       <c r="C6" s="10" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D6" s="174"/>
       <c r="E6" s="175"/>
@@ -7934,7 +7935,7 @@
   <sheetData>
     <row r="1" spans="2:26" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="Z1" s="38"/>
     </row>
@@ -7956,7 +7957,7 @@
     </row>
     <row r="3" spans="2:26" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="153" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C3" s="153"/>
       <c r="D3" s="153"/>
@@ -7978,7 +7979,7 @@
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F5" s="13"/>
     </row>
@@ -7988,7 +7989,7 @@
       </c>
       <c r="D6" s="12"/>
       <c r="E6" s="10" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="F6" s="12"/>
     </row>
@@ -8057,7 +8058,7 @@
   <sheetData>
     <row r="1" spans="2:26" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="Z1" s="38"/>
     </row>
@@ -8079,7 +8080,7 @@
     </row>
     <row r="3" spans="2:26" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="153" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C3" s="153"/>
       <c r="D3" s="153"/>
@@ -8201,7 +8202,7 @@
   <sheetData>
     <row r="1" spans="2:17" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="2:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -8219,7 +8220,7 @@
     </row>
     <row r="3" spans="2:17" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="153" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C3" s="153"/>
       <c r="D3" s="153"/>
@@ -8234,7 +8235,7 @@
     </row>
     <row r="5" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D5" s="177" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="E5" s="177"/>
       <c r="F5" s="73"/>
@@ -8247,12 +8248,12 @@
       <c r="K5" s="177"/>
       <c r="L5" s="177"/>
       <c r="M5" s="177" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="N5" s="177"/>
       <c r="O5" s="177"/>
       <c r="P5" s="155" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="Q5" s="155"/>
     </row>
@@ -8261,49 +8262,49 @@
         <v>31</v>
       </c>
       <c r="C6" s="71" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="D6" s="63" t="s">
+        <v>117</v>
+      </c>
+      <c r="E6" s="63" t="s">
+        <v>118</v>
+      </c>
+      <c r="F6" s="71" t="s">
+        <v>132</v>
+      </c>
+      <c r="G6" s="71" t="s">
+        <v>133</v>
+      </c>
+      <c r="H6" s="72" t="s">
+        <v>51</v>
+      </c>
+      <c r="I6" s="70" t="s">
+        <v>67</v>
+      </c>
+      <c r="J6" s="63" t="s">
+        <v>122</v>
+      </c>
+      <c r="K6" s="63" t="s">
         <v>121</v>
       </c>
-      <c r="E6" s="63" t="s">
+      <c r="L6" s="69" t="s">
+        <v>109</v>
+      </c>
+      <c r="M6" s="63" t="s">
         <v>122</v>
       </c>
-      <c r="F6" s="71" t="s">
-        <v>136</v>
-      </c>
-      <c r="G6" s="71" t="s">
-        <v>137</v>
-      </c>
-      <c r="H6" s="72" t="s">
-        <v>52</v>
-      </c>
-      <c r="I6" s="70" t="s">
-        <v>69</v>
-      </c>
-      <c r="J6" s="63" t="s">
-        <v>126</v>
-      </c>
-      <c r="K6" s="63" t="s">
-        <v>125</v>
-      </c>
-      <c r="L6" s="69" t="s">
-        <v>113</v>
-      </c>
-      <c r="M6" s="63" t="s">
-        <v>126</v>
-      </c>
       <c r="N6" s="63" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="O6" s="69" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="P6" s="69" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="Q6" s="69" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.25">
@@ -8357,12 +8358,12 @@
   <sheetData>
     <row r="1" spans="2:13" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="2:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="152" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="C2" s="152"/>
       <c r="D2" s="152"/>
@@ -8377,7 +8378,7 @@
     </row>
     <row r="3" spans="2:13" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="153" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="C3" s="153"/>
       <c r="D3" s="153"/>
@@ -8410,7 +8411,7 @@
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B6" s="70" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.25">
@@ -8464,7 +8465,7 @@
   <sheetData>
     <row r="1" spans="2:25" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="2:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -8488,7 +8489,7 @@
     </row>
     <row r="3" spans="2:25" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="153" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C3" s="153"/>
       <c r="D3" s="153"/>
@@ -8508,70 +8509,70 @@
       <c r="R3" s="57"/>
     </row>
     <row r="5" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B5" s="182" t="s">
-        <v>109</v>
-      </c>
-      <c r="C5" s="183"/>
-      <c r="D5" s="183"/>
-      <c r="E5" s="183"/>
-      <c r="F5" s="183"/>
-      <c r="G5" s="183"/>
-      <c r="H5" s="183"/>
-      <c r="I5" s="183"/>
-      <c r="J5" s="183"/>
-      <c r="K5" s="183"/>
-      <c r="L5" s="184"/>
-      <c r="M5" s="182" t="s">
-        <v>110</v>
-      </c>
-      <c r="N5" s="183"/>
-      <c r="O5" s="183"/>
-      <c r="P5" s="183"/>
-      <c r="Q5" s="183"/>
-      <c r="R5" s="183"/>
-      <c r="S5" s="183"/>
-      <c r="T5" s="183"/>
-      <c r="U5" s="183"/>
-      <c r="V5" s="183"/>
-      <c r="W5" s="183"/>
-      <c r="X5" s="183"/>
-      <c r="Y5" s="184"/>
+      <c r="B5" s="181" t="s">
+        <v>105</v>
+      </c>
+      <c r="C5" s="182"/>
+      <c r="D5" s="182"/>
+      <c r="E5" s="182"/>
+      <c r="F5" s="182"/>
+      <c r="G5" s="182"/>
+      <c r="H5" s="182"/>
+      <c r="I5" s="182"/>
+      <c r="J5" s="182"/>
+      <c r="K5" s="182"/>
+      <c r="L5" s="183"/>
+      <c r="M5" s="181" t="s">
+        <v>106</v>
+      </c>
+      <c r="N5" s="182"/>
+      <c r="O5" s="182"/>
+      <c r="P5" s="182"/>
+      <c r="Q5" s="182"/>
+      <c r="R5" s="182"/>
+      <c r="S5" s="182"/>
+      <c r="T5" s="182"/>
+      <c r="U5" s="182"/>
+      <c r="V5" s="182"/>
+      <c r="W5" s="182"/>
+      <c r="X5" s="182"/>
+      <c r="Y5" s="183"/>
     </row>
     <row r="6" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B6" s="181"/>
-      <c r="C6" s="181"/>
-      <c r="D6" s="181"/>
-      <c r="E6" s="181"/>
-      <c r="F6" s="188" t="s">
+      <c r="B6" s="178"/>
+      <c r="C6" s="178"/>
+      <c r="D6" s="178"/>
+      <c r="E6" s="178"/>
+      <c r="F6" s="187" t="s">
         <v>26</v>
       </c>
-      <c r="G6" s="189"/>
-      <c r="H6" s="189"/>
-      <c r="I6" s="190"/>
-      <c r="J6" s="182" t="s">
+      <c r="G6" s="188"/>
+      <c r="H6" s="188"/>
+      <c r="I6" s="189"/>
+      <c r="J6" s="181" t="s">
         <v>29</v>
       </c>
-      <c r="K6" s="183"/>
-      <c r="L6" s="184"/>
+      <c r="K6" s="182"/>
+      <c r="L6" s="183"/>
       <c r="M6" s="87"/>
-      <c r="N6" s="178" t="s">
+      <c r="N6" s="179" t="s">
         <v>41</v>
       </c>
-      <c r="O6" s="179"/>
-      <c r="P6" s="178" t="s">
-        <v>103</v>
-      </c>
-      <c r="Q6" s="180"/>
-      <c r="R6" s="179"/>
+      <c r="O6" s="180"/>
+      <c r="P6" s="179" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q6" s="190"/>
+      <c r="R6" s="180"/>
       <c r="S6" s="87"/>
-      <c r="T6" s="178" t="s">
-        <v>120</v>
-      </c>
-      <c r="U6" s="179"/>
-      <c r="V6" s="185"/>
-      <c r="W6" s="186"/>
-      <c r="X6" s="186"/>
-      <c r="Y6" s="187"/>
+      <c r="T6" s="179" t="s">
+        <v>116</v>
+      </c>
+      <c r="U6" s="180"/>
+      <c r="V6" s="184"/>
+      <c r="W6" s="185"/>
+      <c r="X6" s="185"/>
+      <c r="Y6" s="186"/>
     </row>
     <row r="7" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B7" s="75" t="s">
@@ -8587,64 +8588,64 @@
         <v>28</v>
       </c>
       <c r="F7" s="77" t="s">
+        <v>110</v>
+      </c>
+      <c r="G7" s="77" t="s">
         <v>114</v>
       </c>
-      <c r="G7" s="77" t="s">
+      <c r="H7" s="77" t="s">
+        <v>115</v>
+      </c>
+      <c r="I7" s="77" t="s">
+        <v>111</v>
+      </c>
+      <c r="J7" s="77" t="s">
+        <v>107</v>
+      </c>
+      <c r="K7" s="77" t="s">
+        <v>108</v>
+      </c>
+      <c r="L7" s="77" t="s">
+        <v>109</v>
+      </c>
+      <c r="M7" s="76" t="s">
+        <v>51</v>
+      </c>
+      <c r="N7" s="77" t="s">
+        <v>112</v>
+      </c>
+      <c r="O7" s="77" t="s">
+        <v>113</v>
+      </c>
+      <c r="P7" s="77" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q7" s="77" t="s">
+        <v>108</v>
+      </c>
+      <c r="R7" s="77" t="s">
+        <v>109</v>
+      </c>
+      <c r="S7" s="75" t="s">
+        <v>134</v>
+      </c>
+      <c r="T7" s="77" t="s">
+        <v>117</v>
+      </c>
+      <c r="U7" s="77" t="s">
         <v>118</v>
       </c>
-      <c r="H7" s="77" t="s">
-        <v>119</v>
-      </c>
-      <c r="I7" s="77" t="s">
-        <v>115</v>
-      </c>
-      <c r="J7" s="77" t="s">
-        <v>111</v>
-      </c>
-      <c r="K7" s="77" t="s">
-        <v>112</v>
-      </c>
-      <c r="L7" s="77" t="s">
-        <v>113</v>
-      </c>
-      <c r="M7" s="76" t="s">
-        <v>52</v>
-      </c>
-      <c r="N7" s="77" t="s">
-        <v>116</v>
-      </c>
-      <c r="O7" s="77" t="s">
-        <v>117</v>
-      </c>
-      <c r="P7" s="77" t="s">
-        <v>111</v>
-      </c>
-      <c r="Q7" s="77" t="s">
-        <v>112</v>
-      </c>
-      <c r="R7" s="77" t="s">
-        <v>113</v>
-      </c>
-      <c r="S7" s="75" t="s">
-        <v>138</v>
-      </c>
-      <c r="T7" s="77" t="s">
-        <v>121</v>
-      </c>
-      <c r="U7" s="77" t="s">
-        <v>122</v>
-      </c>
       <c r="V7" s="76" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="W7" s="76" t="s">
         <v>31</v>
       </c>
       <c r="X7" s="75" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="Y7" s="75" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
     </row>
     <row r="8" spans="2:25" x14ac:dyDescent="0.25">
@@ -8675,17 +8676,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="P6:R6"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="T6:U6"/>
+    <mergeCell ref="M5:Y5"/>
+    <mergeCell ref="V6:Y6"/>
     <mergeCell ref="B2:P2"/>
     <mergeCell ref="B3:P3"/>
     <mergeCell ref="B5:L5"/>
     <mergeCell ref="J6:L6"/>
     <mergeCell ref="F6:I6"/>
     <mergeCell ref="N6:O6"/>
-    <mergeCell ref="P6:R6"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="T6:U6"/>
-    <mergeCell ref="M5:Y5"/>
-    <mergeCell ref="V6:Y6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -8804,7 +8805,7 @@
   <sheetData>
     <row r="1" spans="2:14" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -8841,13 +8842,13 @@
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="44" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C5" s="44" t="s">
         <v>8</v>
       </c>
       <c r="D5" s="45" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>10</v>
@@ -8856,13 +8857,13 @@
         <v>11</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="H5" s="95" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="I5" s="95" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
@@ -8906,7 +8907,7 @@
   <sheetData>
     <row r="1" spans="2:5" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -8917,7 +8918,7 @@
     </row>
     <row r="3" spans="2:5" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="153" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C3" s="153"/>
       <c r="D3" s="153"/>
@@ -8928,16 +8929,16 @@
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="70" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C5" s="44" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="D5" s="96" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="E5" s="96" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6" spans="2:5" customFormat="1" x14ac:dyDescent="0.25">
@@ -8978,7 +8979,7 @@
   <sheetData>
     <row r="1" spans="2:16" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -9019,19 +9020,19 @@
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="44" t="s">
+        <v>74</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D5" s="44" t="s">
+        <v>76</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="F5" s="4" t="s">
         <v>78</v>
-      </c>
-      <c r="D5" s="44" t="s">
-        <v>79</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>81</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>43</v>
@@ -9043,7 +9044,7 @@
         <v>15</v>
       </c>
       <c r="J5" s="45" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
@@ -9085,7 +9086,7 @@
   <sheetData>
     <row r="1" spans="2:9" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="46" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="2:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -9100,7 +9101,7 @@
     </row>
     <row r="3" spans="2:9" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="82" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="C3" s="82"/>
       <c r="D3" s="82"/>
@@ -9112,7 +9113,7 @@
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="44" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="C5" s="70" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
TRIEDA-1732 - Alterando e adicionando campos no resumo do cenário. Quebrando a exportação em 2 colunas.
</commit_message>
<xml_diff>
--- a/code/client/web/src/main/resources/templateExport.xlsx
+++ b/code/client/web/src/main/resources/templateExport.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="17070" windowHeight="5370" tabRatio="976" firstSheet="12" activeTab="22"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="17070" windowHeight="5370" tabRatio="976" firstSheet="19" activeTab="26"/>
   </bookViews>
   <sheets>
     <sheet name="Turnos" sheetId="49" r:id="rId1"/>
@@ -3382,15 +3382,18 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="28" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3417,9 +3420,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="28" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -3454,7 +3454,7 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="71687" name=":0_674" descr="https://plus.google.com/u/0/_/focus/photos/private/AIbEiAIAAABDCK-Xzbi8pY7DeSILdmNhcmRfcGhvdG8qKDIxMGNjNTM3ZWQ4NjZjNTU4NTk4YjQ0ZDUwM2EwNmUxOGE4OTQyMTIwAdCjuGFdYwQCNlcR6WXw_rsQlR6Q?sz=32"/>
+        <xdr:cNvPr id="71688" name=":0_674" descr="https://plus.google.com/u/0/_/focus/photos/private/AIbEiAIAAABDCK-Xzbi8pY7DeSILdmNhcmRfcGhvdG8qKDIxMGNjNTM3ZWQ4NjZjNTU4NTk4YjQ0ZDUwM2EwNmUxOGE4OTQyMTIwAdCjuGFdYwQCNlcR6WXw_rsQlR6Q?sz=32"/>
         <xdr:cNvSpPr>
           <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -5160,7 +5160,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O6"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
@@ -5287,7 +5287,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0"/>
+    <sheetView showGridLines="0" topLeftCell="C1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5528,14 +5528,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:P6"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:P3"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.85546875" customWidth="1"/>
-    <col min="2" max="2" width="127.42578125" customWidth="1"/>
+    <col min="2" max="2" width="72" customWidth="1"/>
+    <col min="3" max="3" width="29.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:16" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
@@ -5583,9 +5584,11 @@
       <c r="B5" s="104" t="s">
         <v>241</v>
       </c>
+      <c r="C5" s="104"/>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B6" s="105"/>
+      <c r="C6" s="105"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -5601,7 +5604,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:P60"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A55" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="A70" sqref="A61:IV70"/>
     </sheetView>
   </sheetViews>
@@ -8509,70 +8512,70 @@
       <c r="R3" s="57"/>
     </row>
     <row r="5" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B5" s="181" t="s">
+      <c r="B5" s="182" t="s">
         <v>105</v>
       </c>
-      <c r="C5" s="182"/>
-      <c r="D5" s="182"/>
-      <c r="E5" s="182"/>
-      <c r="F5" s="182"/>
-      <c r="G5" s="182"/>
-      <c r="H5" s="182"/>
-      <c r="I5" s="182"/>
-      <c r="J5" s="182"/>
-      <c r="K5" s="182"/>
-      <c r="L5" s="183"/>
-      <c r="M5" s="181" t="s">
+      <c r="C5" s="183"/>
+      <c r="D5" s="183"/>
+      <c r="E5" s="183"/>
+      <c r="F5" s="183"/>
+      <c r="G5" s="183"/>
+      <c r="H5" s="183"/>
+      <c r="I5" s="183"/>
+      <c r="J5" s="183"/>
+      <c r="K5" s="183"/>
+      <c r="L5" s="184"/>
+      <c r="M5" s="182" t="s">
         <v>106</v>
       </c>
-      <c r="N5" s="182"/>
-      <c r="O5" s="182"/>
-      <c r="P5" s="182"/>
-      <c r="Q5" s="182"/>
-      <c r="R5" s="182"/>
-      <c r="S5" s="182"/>
-      <c r="T5" s="182"/>
-      <c r="U5" s="182"/>
-      <c r="V5" s="182"/>
-      <c r="W5" s="182"/>
-      <c r="X5" s="182"/>
-      <c r="Y5" s="183"/>
+      <c r="N5" s="183"/>
+      <c r="O5" s="183"/>
+      <c r="P5" s="183"/>
+      <c r="Q5" s="183"/>
+      <c r="R5" s="183"/>
+      <c r="S5" s="183"/>
+      <c r="T5" s="183"/>
+      <c r="U5" s="183"/>
+      <c r="V5" s="183"/>
+      <c r="W5" s="183"/>
+      <c r="X5" s="183"/>
+      <c r="Y5" s="184"/>
     </row>
     <row r="6" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B6" s="178"/>
-      <c r="C6" s="178"/>
-      <c r="D6" s="178"/>
-      <c r="E6" s="178"/>
-      <c r="F6" s="187" t="s">
+      <c r="B6" s="181"/>
+      <c r="C6" s="181"/>
+      <c r="D6" s="181"/>
+      <c r="E6" s="181"/>
+      <c r="F6" s="188" t="s">
         <v>26</v>
       </c>
-      <c r="G6" s="188"/>
-      <c r="H6" s="188"/>
-      <c r="I6" s="189"/>
-      <c r="J6" s="181" t="s">
+      <c r="G6" s="189"/>
+      <c r="H6" s="189"/>
+      <c r="I6" s="190"/>
+      <c r="J6" s="182" t="s">
         <v>29</v>
       </c>
-      <c r="K6" s="182"/>
-      <c r="L6" s="183"/>
+      <c r="K6" s="183"/>
+      <c r="L6" s="184"/>
       <c r="M6" s="87"/>
-      <c r="N6" s="179" t="s">
+      <c r="N6" s="178" t="s">
         <v>41</v>
       </c>
       <c r="O6" s="180"/>
-      <c r="P6" s="179" t="s">
+      <c r="P6" s="178" t="s">
         <v>99</v>
       </c>
-      <c r="Q6" s="190"/>
+      <c r="Q6" s="179"/>
       <c r="R6" s="180"/>
       <c r="S6" s="87"/>
-      <c r="T6" s="179" t="s">
+      <c r="T6" s="178" t="s">
         <v>116</v>
       </c>
       <c r="U6" s="180"/>
-      <c r="V6" s="184"/>
-      <c r="W6" s="185"/>
-      <c r="X6" s="185"/>
-      <c r="Y6" s="186"/>
+      <c r="V6" s="185"/>
+      <c r="W6" s="186"/>
+      <c r="X6" s="186"/>
+      <c r="Y6" s="187"/>
     </row>
     <row r="7" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B7" s="75" t="s">
@@ -8676,6 +8679,7 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="N6:O6"/>
     <mergeCell ref="P6:R6"/>
     <mergeCell ref="B6:E6"/>
     <mergeCell ref="T6:U6"/>
@@ -8686,7 +8690,6 @@
     <mergeCell ref="B5:L5"/>
     <mergeCell ref="J6:L6"/>
     <mergeCell ref="F6:I6"/>
-    <mergeCell ref="N6:O6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
TRIEDA-1735 - Dividindo relatórios de docentes em professores da instituição e professores virtuais. Revisando calculo dos relatórios.
</commit_message>
<xml_diff>
--- a/code/client/web/src/main/resources/templateExport.xlsx
+++ b/code/client/web/src/main/resources/templateExport.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="17070" windowHeight="5370" tabRatio="976" firstSheet="19" activeTab="26"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="17070" windowHeight="5370" tabRatio="976" firstSheet="35" activeTab="37"/>
   </bookViews>
   <sheets>
     <sheet name="Turnos" sheetId="49" r:id="rId1"/>
@@ -1422,7 +1422,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="256">
   <si>
     <t>Planilha de Unidades</t>
   </si>
@@ -2220,6 +2220,36 @@
   </si>
   <si>
     <t>Planilha de Áreas de Conhecimento</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Professores Virtuais
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Qtde. Professores</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Professores da Instituição
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Qtde. Professores</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -3385,10 +3415,10 @@
     <xf numFmtId="0" fontId="11" fillId="28" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="28" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="28" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3454,7 +3484,7 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="71688" name=":0_674" descr="https://plus.google.com/u/0/_/focus/photos/private/AIbEiAIAAABDCK-Xzbi8pY7DeSILdmNhcmRfcGhvdG8qKDIxMGNjNTM3ZWQ4NjZjNTU4NTk4YjQ0ZDUwM2EwNmUxOGE4OTQyMTIwAdCjuGFdYwQCNlcR6WXw_rsQlR6Q?sz=32"/>
+        <xdr:cNvPr id="71689" name=":0_674" descr="https://plus.google.com/u/0/_/focus/photos/private/AIbEiAIAAABDCK-Xzbi8pY7DeSILdmNhcmRfcGhvdG8qKDIxMGNjNTM3ZWQ4NjZjNTU4NTk4YjQ0ZDUwM2EwNmUxOGE4OTQyMTIwAdCjuGFdYwQCNlcR6WXw_rsQlR6Q?sz=32"/>
         <xdr:cNvSpPr>
           <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -5528,8 +5558,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:P6"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7126,8 +7156,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H6"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:H3"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7135,6 +7165,7 @@
     <col min="1" max="1" width="2.85546875" customWidth="1"/>
     <col min="2" max="2" width="38.7109375" customWidth="1"/>
     <col min="3" max="3" width="26.42578125" customWidth="1"/>
+    <col min="4" max="4" width="28.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
@@ -7167,12 +7198,16 @@
         <v>209</v>
       </c>
       <c r="C5" s="100" t="s">
-        <v>208</v>
+        <v>254</v>
+      </c>
+      <c r="D5" s="100" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -7336,7 +7371,7 @@
   <dimension ref="B1:H6"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="M40" sqref="M40"/>
+      <selection activeCell="C5" sqref="C5:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7344,6 +7379,7 @@
     <col min="1" max="1" width="2.85546875" customWidth="1"/>
     <col min="2" max="2" width="38.7109375" customWidth="1"/>
     <col min="3" max="3" width="26.42578125" customWidth="1"/>
+    <col min="4" max="4" width="28.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
@@ -7376,12 +7412,16 @@
         <v>214</v>
       </c>
       <c r="C5" s="100" t="s">
-        <v>208</v>
+        <v>254</v>
+      </c>
+      <c r="D5" s="100" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -7397,7 +7437,7 @@
   <dimension ref="B1:H6"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="P42" sqref="P42"/>
+      <selection activeCell="C5" sqref="C5:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7405,6 +7445,7 @@
     <col min="1" max="1" width="2.85546875" customWidth="1"/>
     <col min="2" max="2" width="38.7109375" customWidth="1"/>
     <col min="3" max="3" width="26.42578125" customWidth="1"/>
+    <col min="4" max="4" width="28.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
@@ -7437,12 +7478,16 @@
         <v>47</v>
       </c>
       <c r="C5" s="100" t="s">
-        <v>208</v>
+        <v>254</v>
+      </c>
+      <c r="D5" s="100" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -8561,17 +8606,17 @@
       <c r="N6" s="178" t="s">
         <v>41</v>
       </c>
-      <c r="O6" s="180"/>
+      <c r="O6" s="179"/>
       <c r="P6" s="178" t="s">
         <v>99</v>
       </c>
-      <c r="Q6" s="179"/>
-      <c r="R6" s="180"/>
+      <c r="Q6" s="180"/>
+      <c r="R6" s="179"/>
       <c r="S6" s="87"/>
       <c r="T6" s="178" t="s">
         <v>116</v>
       </c>
-      <c r="U6" s="180"/>
+      <c r="U6" s="179"/>
       <c r="V6" s="185"/>
       <c r="W6" s="186"/>
       <c r="X6" s="186"/>
@@ -8679,17 +8724,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B2:P2"/>
+    <mergeCell ref="B3:P3"/>
+    <mergeCell ref="B5:L5"/>
+    <mergeCell ref="J6:L6"/>
+    <mergeCell ref="F6:I6"/>
     <mergeCell ref="N6:O6"/>
     <mergeCell ref="P6:R6"/>
     <mergeCell ref="B6:E6"/>
     <mergeCell ref="T6:U6"/>
     <mergeCell ref="M5:Y5"/>
     <mergeCell ref="V6:Y6"/>
-    <mergeCell ref="B2:P2"/>
-    <mergeCell ref="B3:P3"/>
-    <mergeCell ref="B5:L5"/>
-    <mergeCell ref="J6:L6"/>
-    <mergeCell ref="F6:I6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
TRIEDA-1774 - Diversas Melhorias em Textos e Inserção de Tool Tips
</commit_message>
<xml_diff>
--- a/code/client/web/src/main/resources/templateExport.xlsx
+++ b/code/client/web/src/main/resources/templateExport.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="17070" windowHeight="5370" tabRatio="826"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="17070" windowHeight="5370" tabRatio="826" firstSheet="35" activeTab="21"/>
   </bookViews>
   <sheets>
     <sheet name="Turnos" sheetId="49" r:id="rId1"/>
@@ -71,7 +71,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="E5" authorId="0" shapeId="0">
+    <comment ref="E5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -132,7 +132,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="B5" authorId="0" shapeId="0">
+    <comment ref="B5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -155,7 +155,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F5" authorId="0" shapeId="0">
+    <comment ref="F5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -194,7 +194,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G5" authorId="0" shapeId="0">
+    <comment ref="G5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -287,7 +287,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H5" authorId="0" shapeId="0">
+    <comment ref="H5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -399,7 +399,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I5" authorId="0" shapeId="0">
+    <comment ref="I5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -415,7 +415,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J5" authorId="0" shapeId="0">
+    <comment ref="J5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -431,7 +431,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K5" authorId="0" shapeId="0">
+    <comment ref="K5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -447,7 +447,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L5" authorId="0" shapeId="0">
+    <comment ref="L5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -463,7 +463,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M5" authorId="0" shapeId="0">
+    <comment ref="M5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -479,7 +479,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N5" authorId="0" shapeId="0">
+    <comment ref="N5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -505,7 +505,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="B5" authorId="0" shapeId="0">
+    <comment ref="B5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -538,7 +538,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="B5" authorId="0" shapeId="0">
+    <comment ref="B5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -552,7 +552,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C5" authorId="0" shapeId="0">
+    <comment ref="C5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -566,7 +566,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D5" authorId="0" shapeId="0">
+    <comment ref="D5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -599,7 +599,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="I5" authorId="0" shapeId="0">
+    <comment ref="I5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -623,7 +623,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="D5" authorId="0" shapeId="0">
+    <comment ref="D5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -648,7 +648,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="D5" authorId="0" shapeId="0">
+    <comment ref="D5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -722,7 +722,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E5" authorId="0" shapeId="0">
+    <comment ref="E5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -736,7 +736,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F5" authorId="0" shapeId="0">
+    <comment ref="F5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -750,7 +750,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G5" authorId="0" shapeId="0">
+    <comment ref="G5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -767,7 +767,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I5" authorId="0" shapeId="0">
+    <comment ref="I5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -794,7 +794,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J5" authorId="0" shapeId="0">
+    <comment ref="J5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -808,7 +808,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K5" authorId="0" shapeId="0">
+    <comment ref="K5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -850,7 +850,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="C5" authorId="0" shapeId="0">
+    <comment ref="C5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -899,7 +899,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="D5" authorId="0" shapeId="0">
+    <comment ref="D5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -926,7 +926,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E5" authorId="0" shapeId="0">
+    <comment ref="E5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -961,7 +961,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="Z1" authorId="0" shapeId="0">
+    <comment ref="Z1" authorId="0">
       <text/>
     </comment>
   </commentList>
@@ -974,7 +974,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="Z1" authorId="0" shapeId="0">
+    <comment ref="Z1" authorId="0">
       <text/>
     </comment>
   </commentList>
@@ -987,7 +987,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="E5" authorId="0" shapeId="0">
+    <comment ref="E5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1038,7 +1038,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F5" authorId="0" shapeId="0">
+    <comment ref="F5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1089,7 +1089,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G5" authorId="0" shapeId="0">
+    <comment ref="G5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1140,7 +1140,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H5" authorId="0" shapeId="0">
+    <comment ref="H5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1191,7 +1191,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I5" authorId="0" shapeId="0">
+    <comment ref="I5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1242,7 +1242,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J5" authorId="0" shapeId="0">
+    <comment ref="J5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1293,7 +1293,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K5" authorId="0" shapeId="0">
+    <comment ref="K5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1354,7 +1354,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="Z1" authorId="0" shapeId="0">
+    <comment ref="Z1" authorId="0">
       <text/>
     </comment>
   </commentList>
@@ -1367,7 +1367,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="Z1" authorId="0" shapeId="0">
+    <comment ref="Z1" authorId="0">
       <text/>
     </comment>
   </commentList>
@@ -1380,7 +1380,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="B5" authorId="0" shapeId="0">
+    <comment ref="B5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1403,7 +1403,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G5" authorId="0" shapeId="0">
+    <comment ref="G5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1436,7 +1436,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="B5" authorId="0" shapeId="0">
+    <comment ref="B5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1459,7 +1459,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D5" authorId="0" shapeId="0">
+    <comment ref="D5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1493,7 +1493,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="B5" authorId="0" shapeId="0">
+    <comment ref="B5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1516,7 +1516,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C5" authorId="0" shapeId="0">
+    <comment ref="C5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1589,7 +1589,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D5" authorId="0" shapeId="0">
+    <comment ref="D5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1631,7 +1631,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="C5" authorId="0" shapeId="0">
+    <comment ref="C5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1671,7 +1671,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="B5" authorId="0" shapeId="0">
+    <comment ref="B5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1694,7 +1694,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D5" authorId="0" shapeId="0">
+    <comment ref="D5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1804,7 +1804,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I5" authorId="0" shapeId="0">
+    <comment ref="I5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1827,7 +1827,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J5" authorId="0" shapeId="0">
+    <comment ref="J5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1869,7 +1869,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="B5" authorId="0" shapeId="0">
+    <comment ref="B5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1902,7 +1902,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="B5" authorId="0" shapeId="0">
+    <comment ref="B5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1921,7 +1921,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="264">
   <si>
     <t>Planilha de Unidades</t>
   </si>
@@ -2770,6 +2770,9 @@
   </si>
   <si>
     <t>É recomendavel preencher caso o deslocamento entre os prédios leve um tempo considerável.</t>
+  </si>
+  <si>
+    <t>Receita por Crédito (R$)</t>
   </si>
 </sst>
 </file>
@@ -2907,17 +2910,17 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -3128,6 +3131,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="3" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -3147,12 +3156,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3823,11 +3826,11 @@
     <xf numFmtId="0" fontId="13" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3849,52 +3852,52 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="35" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="36" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="37" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="38" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="38" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="31" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="31" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="31" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="31" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="31" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="35" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="36" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="37" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3965,9 +3968,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -3990,7 +3990,7 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="71740" name=":0_674" descr="https://plus.google.com/u/0/_/focus/photos/private/AIbEiAIAAABDCK-Xzbi8pY7DeSILdmNhcmRfcGhvdG8qKDIxMGNjNTM3ZWQ4NjZjNTU4NTk4YjQ0ZDUwM2EwNmUxOGE4OTQyMTIwAdCjuGFdYwQCNlcR6WXw_rsQlR6Q?sz=32"/>
+        <xdr:cNvPr id="71741" name=":0_674" descr="https://plus.google.com/u/0/_/focus/photos/private/AIbEiAIAAABDCK-Xzbi8pY7DeSILdmNhcmRfcGhvdG8qKDIxMGNjNTM3ZWQ4NjZjNTU4NTk4YjQ0ZDUwM2EwNmUxOGE4OTQyMTIwAdCjuGFdYwQCNlcR6WXw_rsQlR6Q?sz=32"/>
         <xdr:cNvSpPr>
           <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -4076,7 +4076,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4111,7 +4111,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4322,7 +4322,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K6"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -5402,8 +5402,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:M6"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5416,7 +5416,7 @@
     <col min="6" max="6" width="9.85546875" customWidth="1"/>
     <col min="7" max="7" width="19.28515625" customWidth="1"/>
     <col min="8" max="8" width="20.5703125" customWidth="1"/>
-    <col min="9" max="9" width="20.7109375" customWidth="1"/>
+    <col min="9" max="9" width="28" customWidth="1"/>
     <col min="10" max="10" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="33.140625" bestFit="1" customWidth="1"/>
@@ -5481,7 +5481,7 @@
         <v>28</v>
       </c>
       <c r="I5" s="45" t="s">
-        <v>52</v>
+        <v>263</v>
       </c>
       <c r="J5" s="45" t="s">
         <v>92</v>

</xml_diff>

<commit_message>
Com uma mudança na tooltip de dia da semana na aba Professores.
</commit_message>
<xml_diff>
--- a/code/client/web/src/main/resources/templateExport.xlsx
+++ b/code/client/web/src/main/resources/templateExport.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="17070" windowHeight="5370" tabRatio="826" firstSheet="35" activeTab="21"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="17070" windowHeight="5370" tabRatio="826" firstSheet="21" activeTab="25"/>
   </bookViews>
   <sheets>
     <sheet name="Turnos" sheetId="49" r:id="rId1"/>
@@ -71,7 +71,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="E5" authorId="0">
+    <comment ref="E5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -132,7 +132,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="B5" authorId="0">
+    <comment ref="B5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -155,7 +155,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F5" authorId="0">
+    <comment ref="F5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -194,7 +194,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G5" authorId="0">
+    <comment ref="G5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -287,7 +287,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H5" authorId="0">
+    <comment ref="H5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -399,7 +399,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I5" authorId="0">
+    <comment ref="I5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -415,7 +415,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J5" authorId="0">
+    <comment ref="J5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -431,7 +431,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K5" authorId="0">
+    <comment ref="K5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -447,7 +447,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L5" authorId="0">
+    <comment ref="L5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -463,7 +463,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M5" authorId="0">
+    <comment ref="M5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -479,7 +479,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N5" authorId="0">
+    <comment ref="N5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -505,7 +505,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="B5" authorId="0">
+    <comment ref="B5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -538,7 +538,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="B5" authorId="0">
+    <comment ref="B5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -552,7 +552,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C5" authorId="0">
+    <comment ref="C5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -566,7 +566,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D5" authorId="0">
+    <comment ref="D5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -599,7 +599,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="I5" authorId="0">
+    <comment ref="I5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -623,7 +623,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="D5" authorId="0">
+    <comment ref="D5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -648,7 +648,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="D5" authorId="0">
+    <comment ref="D5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -722,7 +722,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E5" authorId="0">
+    <comment ref="E5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -736,7 +736,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F5" authorId="0">
+    <comment ref="F5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -750,7 +750,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G5" authorId="0">
+    <comment ref="G5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -767,7 +767,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I5" authorId="0">
+    <comment ref="I5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -794,7 +794,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J5" authorId="0">
+    <comment ref="J5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -808,7 +808,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K5" authorId="0">
+    <comment ref="K5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -850,7 +850,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="C5" authorId="0">
+    <comment ref="C5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -869,23 +869,23 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>preenchido com números</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>, seguindo a lógica:
-1 = Domingo
-2 = Segunda-feira
-3 = Terça-feira
-4 = Quarta-feira
-5 = Quinta-feira
-6 = Sexta-feira
-7 = Sábado</t>
+          <t>preenchido com os seguintes códigos</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>:
+DOM = Domingo
+SEG = Segunda-feira
+TER = Terça-feira
+QUA = Quarta-feira
+QUI = Quinta-feira
+SEX = Sexta-feira
+SAB = Sábado</t>
         </r>
       </text>
     </comment>
@@ -899,7 +899,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="D5" authorId="0">
+    <comment ref="D5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -926,7 +926,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E5" authorId="0">
+    <comment ref="E5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -961,7 +961,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="Z1" authorId="0">
+    <comment ref="Z1" authorId="0" shapeId="0">
       <text/>
     </comment>
   </commentList>
@@ -974,7 +974,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="Z1" authorId="0">
+    <comment ref="Z1" authorId="0" shapeId="0">
       <text/>
     </comment>
   </commentList>
@@ -987,7 +987,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="E5" authorId="0">
+    <comment ref="E5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1038,7 +1038,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F5" authorId="0">
+    <comment ref="F5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1089,7 +1089,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G5" authorId="0">
+    <comment ref="G5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1140,7 +1140,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H5" authorId="0">
+    <comment ref="H5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1191,7 +1191,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I5" authorId="0">
+    <comment ref="I5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1242,7 +1242,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J5" authorId="0">
+    <comment ref="J5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1293,7 +1293,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K5" authorId="0">
+    <comment ref="K5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1354,7 +1354,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="Z1" authorId="0">
+    <comment ref="Z1" authorId="0" shapeId="0">
       <text/>
     </comment>
   </commentList>
@@ -1367,7 +1367,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="Z1" authorId="0">
+    <comment ref="Z1" authorId="0" shapeId="0">
       <text/>
     </comment>
   </commentList>
@@ -1380,7 +1380,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="B5" authorId="0">
+    <comment ref="B5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1403,7 +1403,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G5" authorId="0">
+    <comment ref="G5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1436,7 +1436,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="B5" authorId="0">
+    <comment ref="B5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1459,7 +1459,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D5" authorId="0">
+    <comment ref="D5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1493,7 +1493,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="B5" authorId="0">
+    <comment ref="B5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1516,7 +1516,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C5" authorId="0">
+    <comment ref="C5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1589,7 +1589,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D5" authorId="0">
+    <comment ref="D5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1631,7 +1631,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="C5" authorId="0">
+    <comment ref="C5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1671,7 +1671,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="B5" authorId="0">
+    <comment ref="B5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1694,7 +1694,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D5" authorId="0">
+    <comment ref="D5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1804,7 +1804,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I5" authorId="0">
+    <comment ref="I5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1827,7 +1827,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J5" authorId="0">
+    <comment ref="J5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1869,7 +1869,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="B5" authorId="0">
+    <comment ref="B5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1902,7 +1902,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="B5" authorId="0">
+    <comment ref="B5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -3969,6 +3969,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -3990,7 +3993,7 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="71741" name=":0_674" descr="https://plus.google.com/u/0/_/focus/photos/private/AIbEiAIAAABDCK-Xzbi8pY7DeSILdmNhcmRfcGhvdG8qKDIxMGNjNTM3ZWQ4NjZjNTU4NTk4YjQ0ZDUwM2EwNmUxOGE4OTQyMTIwAdCjuGFdYwQCNlcR6WXw_rsQlR6Q?sz=32"/>
+        <xdr:cNvPr id="71742" name=":0_674" descr="https://plus.google.com/u/0/_/focus/photos/private/AIbEiAIAAABDCK-Xzbi8pY7DeSILdmNhcmRfcGhvdG8qKDIxMGNjNTM3ZWQ4NjZjNTU4NTk4YjQ0ZDUwM2EwNmUxOGE4OTQyMTIwAdCjuGFdYwQCNlcR6WXw_rsQlR6Q?sz=32"/>
         <xdr:cNvSpPr>
           <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -4076,7 +4079,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4111,7 +4114,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -5402,7 +5405,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:M6"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
@@ -5827,8 +5830,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
TRIEDA-1777 - Adicionando colunas Virtual e Criado por Trieda. Adicionando tooltip para as respectivas colunas. Criando script de atualização do banco.
</commit_message>
<xml_diff>
--- a/code/client/web/src/main/resources/templateExport.xlsx
+++ b/code/client/web/src/main/resources/templateExport.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="17070" windowHeight="5370" tabRatio="826" firstSheet="21" activeTab="25"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="17070" windowHeight="5370" tabRatio="826" firstSheet="18" activeTab="25"/>
   </bookViews>
   <sheets>
     <sheet name="Turnos" sheetId="49" r:id="rId1"/>
@@ -71,7 +71,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="E5" authorId="0" shapeId="0">
+    <comment ref="E5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -132,7 +132,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="B5" authorId="0" shapeId="0">
+    <comment ref="B5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -155,7 +155,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F5" authorId="0" shapeId="0">
+    <comment ref="F5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -194,7 +194,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G5" authorId="0" shapeId="0">
+    <comment ref="G5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -287,7 +287,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H5" authorId="0" shapeId="0">
+    <comment ref="H5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -399,7 +399,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I5" authorId="0" shapeId="0">
+    <comment ref="I5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -415,7 +415,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J5" authorId="0" shapeId="0">
+    <comment ref="J5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -431,7 +431,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K5" authorId="0" shapeId="0">
+    <comment ref="K5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -447,7 +447,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L5" authorId="0" shapeId="0">
+    <comment ref="L5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -463,7 +463,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M5" authorId="0" shapeId="0">
+    <comment ref="M5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -479,7 +479,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N5" authorId="0" shapeId="0">
+    <comment ref="N5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -505,7 +505,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="B5" authorId="0" shapeId="0">
+    <comment ref="B5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -538,7 +538,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="B5" authorId="0" shapeId="0">
+    <comment ref="B5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -552,7 +552,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C5" authorId="0" shapeId="0">
+    <comment ref="C5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -566,7 +566,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D5" authorId="0" shapeId="0">
+    <comment ref="D5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -599,7 +599,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="I5" authorId="0" shapeId="0">
+    <comment ref="I5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -623,7 +623,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="D5" authorId="0" shapeId="0">
+    <comment ref="D5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -635,6 +635,34 @@
           </rPr>
           <t>Sim
 Não</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Alunos virtuais são aqueles ainda inexistentes, porém, que a Instituição de Ensino deseja simular a sua presenção, por exemplo, alunos entrantes. Além disso, estes alunos virtuais podem ser criados automaticamente pelo Trieda através do Módulo de Geração de Demanda da aba de Ofertas e Demandas. Mais especificamente, ao informar uma quantidade de alunos através da tela de Ofertas e Demandas o Trieda irá criar, automaticamente, a quantidade informada de alunos. Nestes casos, além do aluno ser considerado virtual o mesmo terá o campo Criado por Trieda? como marcado."</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Alunos virtuais são aqueles ainda inexistentes, porém, que a Instituição de Ensino deseja simular a sua presenção, por exemplo, alunos entrantes. Além disso, estes alunos virtuais podem ser criados automaticamente pelo Trieda através do Módulo de Geração de Demanda da aba de Ofertas e Demandas. Mais especificamente, ao informar uma quantidade de alunos através da tela de Ofertas e Demandas o Trieda irá criar, automaticamente, a quantidade informada de alunos. Nestes casos, além do aluno ser considerado virtual o mesmo terá o campo Criado por Trieda? como marcado."</t>
         </r>
       </text>
     </comment>
@@ -648,7 +676,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="D5" authorId="0" shapeId="0">
+    <comment ref="D5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -722,7 +750,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E5" authorId="0" shapeId="0">
+    <comment ref="E5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -736,7 +764,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F5" authorId="0" shapeId="0">
+    <comment ref="F5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -750,7 +778,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G5" authorId="0" shapeId="0">
+    <comment ref="G5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -767,7 +795,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I5" authorId="0" shapeId="0">
+    <comment ref="I5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -794,7 +822,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J5" authorId="0" shapeId="0">
+    <comment ref="J5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -808,7 +836,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K5" authorId="0" shapeId="0">
+    <comment ref="K5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -850,7 +878,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="C5" authorId="0" shapeId="0">
+    <comment ref="C5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -859,26 +887,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">A ser </t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>preenchido com os seguintes códigos</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>:
+          <t>A ser preenchido com os seguintes códigos:
 DOM = Domingo
 SEG = Segunda-feira
 TER = Terça-feira
@@ -899,7 +908,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="D5" authorId="0" shapeId="0">
+    <comment ref="D5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -926,7 +935,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E5" authorId="0" shapeId="0">
+    <comment ref="E5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -961,7 +970,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="Z1" authorId="0" shapeId="0">
+    <comment ref="Z1" authorId="0">
       <text/>
     </comment>
   </commentList>
@@ -974,7 +983,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="Z1" authorId="0" shapeId="0">
+    <comment ref="Z1" authorId="0">
       <text/>
     </comment>
   </commentList>
@@ -987,7 +996,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="E5" authorId="0" shapeId="0">
+    <comment ref="E5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1038,7 +1047,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F5" authorId="0" shapeId="0">
+    <comment ref="F5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1089,7 +1098,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G5" authorId="0" shapeId="0">
+    <comment ref="G5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1140,7 +1149,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H5" authorId="0" shapeId="0">
+    <comment ref="H5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1191,7 +1200,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I5" authorId="0" shapeId="0">
+    <comment ref="I5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1242,7 +1251,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J5" authorId="0" shapeId="0">
+    <comment ref="J5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1293,7 +1302,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K5" authorId="0" shapeId="0">
+    <comment ref="K5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1354,7 +1363,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="Z1" authorId="0" shapeId="0">
+    <comment ref="Z1" authorId="0">
       <text/>
     </comment>
   </commentList>
@@ -1367,7 +1376,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="Z1" authorId="0" shapeId="0">
+    <comment ref="Z1" authorId="0">
       <text/>
     </comment>
   </commentList>
@@ -1380,7 +1389,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="B5" authorId="0" shapeId="0">
+    <comment ref="B5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1403,7 +1412,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G5" authorId="0" shapeId="0">
+    <comment ref="G5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1436,7 +1445,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="B5" authorId="0" shapeId="0">
+    <comment ref="B5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1459,7 +1468,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D5" authorId="0" shapeId="0">
+    <comment ref="D5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1493,7 +1502,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="B5" authorId="0" shapeId="0">
+    <comment ref="B5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1516,7 +1525,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C5" authorId="0" shapeId="0">
+    <comment ref="C5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1589,7 +1598,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D5" authorId="0" shapeId="0">
+    <comment ref="D5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1631,7 +1640,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="C5" authorId="0" shapeId="0">
+    <comment ref="C5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1671,7 +1680,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="B5" authorId="0" shapeId="0">
+    <comment ref="B5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1694,7 +1703,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D5" authorId="0" shapeId="0">
+    <comment ref="D5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1804,7 +1813,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I5" authorId="0" shapeId="0">
+    <comment ref="I5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1827,7 +1836,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J5" authorId="0" shapeId="0">
+    <comment ref="J5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1869,7 +1878,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="B5" authorId="0" shapeId="0">
+    <comment ref="B5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1902,7 +1911,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="B5" authorId="0" shapeId="0">
+    <comment ref="B5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1921,7 +1930,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="266">
   <si>
     <t>Planilha de Unidades</t>
   </si>
@@ -2773,6 +2782,12 @@
   </si>
   <si>
     <t>Receita por Crédito (R$)</t>
+  </si>
+  <si>
+    <t>Virtual?</t>
+  </si>
+  <si>
+    <t>Criado por Trieda?</t>
   </si>
 </sst>
 </file>
@@ -3437,7 +3452,7 @@
     <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="189">
+  <cellXfs count="190">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -3838,6 +3853,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3968,9 +3986,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -3993,7 +4008,7 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="71742" name=":0_674" descr="https://plus.google.com/u/0/_/focus/photos/private/AIbEiAIAAABDCK-Xzbi8pY7DeSILdmNhcmRfcGhvdG8qKDIxMGNjNTM3ZWQ4NjZjNTU4NTk4YjQ0ZDUwM2EwNmUxOGE4OTQyMTIwAdCjuGFdYwQCNlcR6WXw_rsQlR6Q?sz=32"/>
+        <xdr:cNvPr id="71744" name=":0_674" descr="https://plus.google.com/u/0/_/focus/photos/private/AIbEiAIAAABDCK-Xzbi8pY7DeSILdmNhcmRfcGhvdG8qKDIxMGNjNTM3ZWQ4NjZjNTU4NTk4YjQ0ZDUwM2EwNmUxOGE4OTQyMTIwAdCjuGFdYwQCNlcR6WXw_rsQlR6Q?sz=32"/>
         <xdr:cNvSpPr>
           <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -4079,7 +4094,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4114,7 +4129,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4523,10 +4538,10 @@
       <c r="I2" s="78"/>
     </row>
     <row r="3" spans="2:9" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="150" t="s">
+      <c r="B3" s="151" t="s">
         <v>215</v>
       </c>
-      <c r="C3" s="150"/>
+      <c r="C3" s="151"/>
       <c r="D3" s="77"/>
       <c r="E3" s="77"/>
       <c r="F3" s="77"/>
@@ -4587,10 +4602,10 @@
       <c r="I2" s="78"/>
     </row>
     <row r="3" spans="2:9" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="150" t="s">
+      <c r="B3" s="151" t="s">
         <v>241</v>
       </c>
-      <c r="C3" s="150"/>
+      <c r="C3" s="151"/>
       <c r="D3" s="77"/>
       <c r="E3" s="77"/>
       <c r="F3" s="77"/>
@@ -4663,10 +4678,10 @@
       <c r="P2" s="78"/>
     </row>
     <row r="3" spans="2:16" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="150" t="s">
+      <c r="B3" s="151" t="s">
         <v>240</v>
       </c>
-      <c r="C3" s="150"/>
+      <c r="C3" s="151"/>
       <c r="D3" s="77"/>
       <c r="E3" s="77"/>
       <c r="F3" s="77"/>
@@ -4752,10 +4767,10 @@
       <c r="P2" s="78"/>
     </row>
     <row r="3" spans="2:16" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="150" t="s">
+      <c r="B3" s="151" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="150"/>
+      <c r="C3" s="151"/>
       <c r="D3" s="77"/>
       <c r="E3" s="77"/>
       <c r="F3" s="77"/>
@@ -4869,11 +4884,11 @@
       <c r="K2" s="78"/>
     </row>
     <row r="3" spans="2:11" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="150" t="s">
+      <c r="B3" s="151" t="s">
         <v>217</v>
       </c>
-      <c r="C3" s="150"/>
-      <c r="D3" s="150"/>
+      <c r="C3" s="151"/>
+      <c r="D3" s="151"/>
       <c r="E3" s="77"/>
       <c r="F3" s="77"/>
       <c r="G3" s="77"/>
@@ -4956,11 +4971,11 @@
       <c r="G2" s="78"/>
     </row>
     <row r="3" spans="2:7" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="150" t="s">
+      <c r="B3" s="151" t="s">
         <v>59</v>
       </c>
-      <c r="C3" s="150"/>
-      <c r="D3" s="150"/>
+      <c r="C3" s="151"/>
+      <c r="D3" s="151"/>
       <c r="E3" s="77"/>
       <c r="F3" s="77"/>
       <c r="G3" s="77"/>
@@ -5016,12 +5031,12 @@
       <c r="C2" s="78"/>
     </row>
     <row r="3" spans="2:5" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="150" t="s">
+      <c r="B3" s="151" t="s">
         <v>255</v>
       </c>
-      <c r="C3" s="150"/>
-      <c r="D3" s="150"/>
-      <c r="E3" s="150"/>
+      <c r="C3" s="151"/>
+      <c r="D3" s="151"/>
+      <c r="E3" s="151"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -5076,10 +5091,10 @@
       <c r="G2" s="78"/>
     </row>
     <row r="3" spans="2:7" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="150" t="s">
+      <c r="B3" s="151" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="150"/>
+      <c r="C3" s="151"/>
       <c r="D3" s="77"/>
       <c r="E3" s="77"/>
       <c r="F3" s="77"/>
@@ -5151,11 +5166,11 @@
       <c r="E2" s="78"/>
     </row>
     <row r="3" spans="2:5" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="150" t="s">
+      <c r="B3" s="151" t="s">
         <v>256</v>
       </c>
-      <c r="C3" s="150"/>
-      <c r="D3" s="150"/>
+      <c r="C3" s="151"/>
+      <c r="D3" s="151"/>
       <c r="E3" s="77"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
@@ -5221,10 +5236,10 @@
       <c r="I2" s="78"/>
     </row>
     <row r="3" spans="2:11" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="150" t="s">
+      <c r="B3" s="151" t="s">
         <v>244</v>
       </c>
-      <c r="C3" s="150"/>
+      <c r="C3" s="151"/>
       <c r="D3" s="77"/>
       <c r="E3" s="77"/>
       <c r="F3" s="77"/>
@@ -5293,11 +5308,11 @@
       <c r="E2" s="78"/>
     </row>
     <row r="3" spans="2:5" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="150" t="s">
+      <c r="B3" s="151" t="s">
         <v>257</v>
       </c>
-      <c r="C3" s="150"/>
-      <c r="D3" s="150"/>
+      <c r="C3" s="151"/>
+      <c r="D3" s="151"/>
       <c r="E3" s="77"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
@@ -5360,11 +5375,11 @@
       <c r="F2" s="78"/>
     </row>
     <row r="3" spans="2:6" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="150" t="s">
+      <c r="B3" s="151" t="s">
         <v>189</v>
       </c>
-      <c r="C3" s="150"/>
-      <c r="D3" s="150"/>
+      <c r="C3" s="151"/>
+      <c r="D3" s="151"/>
       <c r="E3" s="77"/>
       <c r="F3" s="77"/>
     </row>
@@ -5406,7 +5421,7 @@
   <dimension ref="B1:M6"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="Q42" sqref="Q42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5432,34 +5447,34 @@
       </c>
     </row>
     <row r="2" spans="2:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="151"/>
-      <c r="C2" s="151"/>
-      <c r="D2" s="151"/>
-      <c r="E2" s="151"/>
-      <c r="F2" s="151"/>
-      <c r="G2" s="151"/>
-      <c r="H2" s="151"/>
-      <c r="I2" s="151"/>
-      <c r="J2" s="151"/>
-      <c r="K2" s="151"/>
-      <c r="L2" s="151"/>
-      <c r="M2" s="151"/>
+      <c r="B2" s="152"/>
+      <c r="C2" s="152"/>
+      <c r="D2" s="152"/>
+      <c r="E2" s="152"/>
+      <c r="F2" s="152"/>
+      <c r="G2" s="152"/>
+      <c r="H2" s="152"/>
+      <c r="I2" s="152"/>
+      <c r="J2" s="152"/>
+      <c r="K2" s="152"/>
+      <c r="L2" s="152"/>
+      <c r="M2" s="152"/>
     </row>
     <row r="3" spans="2:13" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="150" t="s">
+      <c r="B3" s="151" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="150"/>
-      <c r="D3" s="150"/>
-      <c r="E3" s="150"/>
-      <c r="F3" s="150"/>
-      <c r="G3" s="150"/>
-      <c r="H3" s="150"/>
-      <c r="I3" s="150"/>
-      <c r="J3" s="150"/>
-      <c r="K3" s="150"/>
-      <c r="L3" s="150"/>
-      <c r="M3" s="150"/>
+      <c r="C3" s="151"/>
+      <c r="D3" s="151"/>
+      <c r="E3" s="151"/>
+      <c r="F3" s="151"/>
+      <c r="G3" s="151"/>
+      <c r="H3" s="151"/>
+      <c r="I3" s="151"/>
+      <c r="J3" s="151"/>
+      <c r="K3" s="151"/>
+      <c r="L3" s="151"/>
+      <c r="M3" s="151"/>
     </row>
     <row r="5" spans="2:13" s="144" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="143" t="s">
@@ -5526,10 +5541,10 @@
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:D6"/>
+  <dimension ref="B1:F6"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5537,27 +5552,28 @@
     <col min="1" max="1" width="2.85546875" customWidth="1"/>
     <col min="2" max="2" width="17.140625" customWidth="1"/>
     <col min="3" max="3" width="63" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:6" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="44" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="78"/>
       <c r="C2" s="78"/>
       <c r="D2" s="78"/>
     </row>
-    <row r="3" spans="2:4" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="150" t="s">
+    <row r="3" spans="2:6" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B3" s="151" t="s">
         <v>112</v>
       </c>
-      <c r="C3" s="150"/>
+      <c r="C3" s="151"/>
       <c r="D3" s="77"/>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="57" t="s">
         <v>87</v>
       </c>
@@ -5567,11 +5583,19 @@
       <c r="D5" s="56" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E5" s="150" t="s">
+        <v>264</v>
+      </c>
+      <c r="F5" s="150" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="9"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
+      <c r="E6" s="83"/>
+      <c r="F6" s="83"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -5672,10 +5696,10 @@
       <c r="K5" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="L5" s="152" t="s">
+      <c r="L5" s="153" t="s">
         <v>96</v>
       </c>
-      <c r="M5" s="152"/>
+      <c r="M5" s="153"/>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
@@ -5688,8 +5712,8 @@
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
-      <c r="L6" s="153"/>
-      <c r="M6" s="153"/>
+      <c r="L6" s="154"/>
+      <c r="M6" s="154"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -5747,10 +5771,10 @@
       <c r="O2" s="78"/>
     </row>
     <row r="3" spans="2:15" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="150" t="s">
+      <c r="B3" s="151" t="s">
         <v>65</v>
       </c>
-      <c r="C3" s="150"/>
+      <c r="C3" s="151"/>
       <c r="D3" s="77"/>
       <c r="E3" s="77"/>
       <c r="F3" s="77"/>
@@ -5831,7 +5855,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5855,11 +5879,11 @@
       <c r="E2" s="78"/>
     </row>
     <row r="3" spans="2:5" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="150" t="s">
+      <c r="B3" s="151" t="s">
         <v>117</v>
       </c>
-      <c r="C3" s="150"/>
-      <c r="D3" s="150"/>
+      <c r="C3" s="151"/>
+      <c r="D3" s="151"/>
       <c r="E3" s="77"/>
     </row>
     <row r="4" spans="2:5" customFormat="1" x14ac:dyDescent="0.25">
@@ -5921,10 +5945,10 @@
       <c r="D2" s="78"/>
     </row>
     <row r="3" spans="2:4" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="150" t="s">
+      <c r="B3" s="151" t="s">
         <v>62</v>
       </c>
-      <c r="C3" s="150"/>
+      <c r="C3" s="151"/>
       <c r="D3" s="77"/>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
@@ -5981,11 +6005,11 @@
       <c r="E2" s="78"/>
     </row>
     <row r="3" spans="2:5" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="150" t="s">
+      <c r="B3" s="151" t="s">
         <v>66</v>
       </c>
-      <c r="C3" s="150"/>
-      <c r="D3" s="150"/>
+      <c r="C3" s="151"/>
+      <c r="D3" s="151"/>
       <c r="E3" s="77"/>
     </row>
     <row r="5" spans="2:5" s="144" customFormat="1" x14ac:dyDescent="0.25">
@@ -6097,13 +6121,13 @@
       <c r="I2" s="78"/>
     </row>
     <row r="3" spans="2:11" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="150" t="s">
+      <c r="B3" s="151" t="s">
         <v>248</v>
       </c>
-      <c r="C3" s="150"/>
-      <c r="D3" s="150"/>
-      <c r="E3" s="150"/>
-      <c r="F3" s="150"/>
+      <c r="C3" s="151"/>
+      <c r="D3" s="151"/>
+      <c r="E3" s="151"/>
+      <c r="F3" s="151"/>
       <c r="G3" s="77"/>
       <c r="H3" s="77"/>
       <c r="I3" s="77"/>
@@ -6204,11 +6228,11 @@
       <c r="P2" s="78"/>
     </row>
     <row r="3" spans="2:16" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="150" t="s">
+      <c r="B3" s="151" t="s">
         <v>232</v>
       </c>
-      <c r="C3" s="150"/>
-      <c r="D3" s="150"/>
+      <c r="C3" s="151"/>
+      <c r="D3" s="151"/>
       <c r="E3" s="77"/>
       <c r="F3" s="77"/>
       <c r="G3" s="77"/>
@@ -6243,7 +6267,7 @@
       <c r="E5" s="129"/>
     </row>
     <row r="6" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="162" t="s">
+      <c r="B6" s="163" t="s">
         <v>233</v>
       </c>
       <c r="C6" s="97"/>
@@ -6251,91 +6275,91 @@
       <c r="E6" s="130"/>
     </row>
     <row r="7" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="163"/>
+      <c r="B7" s="164"/>
       <c r="C7" s="99"/>
       <c r="D7" s="100"/>
       <c r="E7" s="131"/>
     </row>
     <row r="8" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="163"/>
+      <c r="B8" s="164"/>
       <c r="C8" s="99"/>
       <c r="D8" s="100"/>
       <c r="E8" s="132"/>
     </row>
     <row r="9" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="163"/>
+      <c r="B9" s="164"/>
       <c r="C9" s="99"/>
       <c r="D9" s="100"/>
       <c r="E9" s="131"/>
     </row>
     <row r="10" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="163"/>
+      <c r="B10" s="164"/>
       <c r="C10" s="99"/>
       <c r="D10" s="100"/>
       <c r="E10" s="131"/>
     </row>
     <row r="11" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B11" s="163"/>
+      <c r="B11" s="164"/>
       <c r="C11" s="99"/>
       <c r="D11" s="100"/>
       <c r="E11" s="131"/>
     </row>
     <row r="12" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="163"/>
+      <c r="B12" s="164"/>
       <c r="C12" s="99"/>
       <c r="D12" s="100"/>
       <c r="E12" s="131"/>
     </row>
     <row r="13" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B13" s="163"/>
+      <c r="B13" s="164"/>
       <c r="C13" s="99"/>
       <c r="D13" s="100"/>
       <c r="E13" s="131"/>
     </row>
     <row r="14" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="163"/>
+      <c r="B14" s="164"/>
       <c r="C14" s="99"/>
       <c r="D14" s="100"/>
       <c r="E14" s="131"/>
     </row>
     <row r="15" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B15" s="163"/>
+      <c r="B15" s="164"/>
       <c r="C15" s="99"/>
       <c r="D15" s="100"/>
       <c r="E15" s="131"/>
     </row>
     <row r="16" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="163"/>
+      <c r="B16" s="164"/>
       <c r="C16" s="99"/>
       <c r="D16" s="100"/>
       <c r="E16" s="131"/>
     </row>
     <row r="17" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B17" s="163"/>
+      <c r="B17" s="164"/>
       <c r="C17" s="99"/>
       <c r="D17" s="100"/>
       <c r="E17" s="131"/>
     </row>
     <row r="18" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B18" s="163"/>
+      <c r="B18" s="164"/>
       <c r="C18" s="99"/>
       <c r="D18" s="100"/>
       <c r="E18" s="131"/>
     </row>
     <row r="19" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B19" s="163"/>
+      <c r="B19" s="164"/>
       <c r="C19" s="99"/>
       <c r="D19" s="100"/>
       <c r="E19" s="131"/>
     </row>
     <row r="20" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B20" s="163"/>
+      <c r="B20" s="164"/>
       <c r="C20" s="99"/>
       <c r="D20" s="100"/>
       <c r="E20" s="131"/>
     </row>
     <row r="21" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B21" s="163"/>
+      <c r="B21" s="164"/>
       <c r="C21" s="101"/>
       <c r="D21" s="102"/>
       <c r="E21" s="133"/>
@@ -6347,7 +6371,7 @@
       <c r="E22" s="1"/>
     </row>
     <row r="23" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B23" s="164" t="s">
+      <c r="B23" s="165" t="s">
         <v>234</v>
       </c>
       <c r="C23" s="105"/>
@@ -6355,31 +6379,31 @@
       <c r="E23" s="134"/>
     </row>
     <row r="24" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B24" s="165"/>
+      <c r="B24" s="166"/>
       <c r="C24" s="107"/>
       <c r="D24" s="108"/>
       <c r="E24" s="132"/>
     </row>
     <row r="25" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B25" s="165"/>
+      <c r="B25" s="166"/>
       <c r="C25" s="107"/>
       <c r="D25" s="108"/>
       <c r="E25" s="135"/>
     </row>
     <row r="26" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B26" s="165"/>
+      <c r="B26" s="166"/>
       <c r="C26" s="109"/>
       <c r="D26" s="108"/>
       <c r="E26" s="135"/>
     </row>
     <row r="27" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B27" s="165"/>
+      <c r="B27" s="166"/>
       <c r="C27" s="109"/>
       <c r="D27" s="108"/>
       <c r="E27" s="135"/>
     </row>
     <row r="28" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B28" s="165"/>
+      <c r="B28" s="166"/>
       <c r="C28" s="110"/>
       <c r="D28" s="111"/>
       <c r="E28" s="136"/>
@@ -6391,7 +6415,7 @@
       <c r="E29" s="1"/>
     </row>
     <row r="30" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B30" s="166" t="s">
+      <c r="B30" s="167" t="s">
         <v>235</v>
       </c>
       <c r="C30" s="112"/>
@@ -6399,43 +6423,43 @@
       <c r="E30" s="137"/>
     </row>
     <row r="31" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B31" s="167"/>
+      <c r="B31" s="168"/>
       <c r="C31" s="114"/>
       <c r="D31" s="115"/>
       <c r="E31" s="138"/>
     </row>
     <row r="32" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B32" s="167"/>
+      <c r="B32" s="168"/>
       <c r="C32" s="114"/>
       <c r="D32" s="115"/>
       <c r="E32" s="138"/>
     </row>
     <row r="33" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B33" s="167"/>
+      <c r="B33" s="168"/>
       <c r="C33" s="114"/>
       <c r="D33" s="115"/>
       <c r="E33" s="132"/>
     </row>
     <row r="34" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B34" s="167"/>
+      <c r="B34" s="168"/>
       <c r="C34" s="114"/>
       <c r="D34" s="115"/>
       <c r="E34" s="135"/>
     </row>
     <row r="35" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B35" s="167"/>
+      <c r="B35" s="168"/>
       <c r="C35" s="114"/>
       <c r="D35" s="115"/>
       <c r="E35" s="135"/>
     </row>
     <row r="36" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B36" s="167"/>
+      <c r="B36" s="168"/>
       <c r="C36" s="114"/>
       <c r="D36" s="115"/>
       <c r="E36" s="131"/>
     </row>
     <row r="37" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B37" s="167"/>
+      <c r="B37" s="168"/>
       <c r="C37" s="116"/>
       <c r="D37" s="117"/>
       <c r="E37" s="133"/>
@@ -6447,7 +6471,7 @@
       <c r="E38" s="1"/>
     </row>
     <row r="39" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B39" s="168" t="s">
+      <c r="B39" s="169" t="s">
         <v>236</v>
       </c>
       <c r="C39" s="118"/>
@@ -6455,31 +6479,31 @@
       <c r="E39" s="139"/>
     </row>
     <row r="40" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="169"/>
+      <c r="B40" s="170"/>
       <c r="C40" s="120"/>
       <c r="D40" s="121"/>
       <c r="E40" s="132"/>
     </row>
     <row r="41" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B41" s="169"/>
+      <c r="B41" s="170"/>
       <c r="C41" s="120"/>
       <c r="D41" s="121"/>
       <c r="E41" s="132"/>
     </row>
     <row r="42" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B42" s="169"/>
+      <c r="B42" s="170"/>
       <c r="C42" s="120"/>
       <c r="D42" s="121"/>
       <c r="E42" s="132"/>
     </row>
     <row r="43" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B43" s="169"/>
+      <c r="B43" s="170"/>
       <c r="C43" s="120"/>
       <c r="D43" s="121"/>
       <c r="E43" s="132"/>
     </row>
     <row r="44" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B44" s="169"/>
+      <c r="B44" s="170"/>
       <c r="C44" s="122"/>
       <c r="D44" s="123"/>
       <c r="E44" s="140"/>
@@ -6491,100 +6515,100 @@
       <c r="E45" s="1"/>
     </row>
     <row r="46" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B46" s="154" t="s">
+      <c r="B46" s="155" t="s">
         <v>237</v>
       </c>
-      <c r="C46" s="157" t="s">
+      <c r="C46" s="158" t="s">
         <v>102</v>
       </c>
       <c r="D46" s="124"/>
       <c r="E46" s="130"/>
     </row>
     <row r="47" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="155"/>
-      <c r="C47" s="158"/>
+      <c r="B47" s="156"/>
+      <c r="C47" s="159"/>
       <c r="D47" s="125"/>
       <c r="E47" s="131"/>
     </row>
     <row r="48" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B48" s="155"/>
-      <c r="C48" s="158"/>
+      <c r="B48" s="156"/>
+      <c r="C48" s="159"/>
       <c r="D48" s="125"/>
       <c r="E48" s="131"/>
     </row>
     <row r="49" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B49" s="155"/>
-      <c r="C49" s="158"/>
+      <c r="B49" s="156"/>
+      <c r="C49" s="159"/>
       <c r="D49" s="125"/>
       <c r="E49" s="131"/>
     </row>
     <row r="50" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B50" s="155"/>
-      <c r="C50" s="158"/>
+      <c r="B50" s="156"/>
+      <c r="C50" s="159"/>
       <c r="D50" s="125"/>
       <c r="E50" s="131"/>
     </row>
     <row r="51" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B51" s="155"/>
-      <c r="C51" s="159" t="s">
+      <c r="B51" s="156"/>
+      <c r="C51" s="160" t="s">
         <v>258</v>
       </c>
       <c r="D51" s="126"/>
       <c r="E51" s="141"/>
     </row>
     <row r="52" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B52" s="155"/>
-      <c r="C52" s="158"/>
+      <c r="B52" s="156"/>
+      <c r="C52" s="159"/>
       <c r="D52" s="125"/>
       <c r="E52" s="131"/>
     </row>
     <row r="53" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B53" s="155"/>
-      <c r="C53" s="158"/>
+      <c r="B53" s="156"/>
+      <c r="C53" s="159"/>
       <c r="D53" s="125"/>
       <c r="E53" s="131"/>
     </row>
     <row r="54" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B54" s="155"/>
-      <c r="C54" s="158"/>
+      <c r="B54" s="156"/>
+      <c r="C54" s="159"/>
       <c r="D54" s="125"/>
       <c r="E54" s="131"/>
     </row>
     <row r="55" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B55" s="155"/>
-      <c r="C55" s="160"/>
+      <c r="B55" s="156"/>
+      <c r="C55" s="161"/>
       <c r="D55" s="127"/>
       <c r="E55" s="142"/>
     </row>
     <row r="56" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B56" s="155"/>
-      <c r="C56" s="158" t="s">
+      <c r="B56" s="156"/>
+      <c r="C56" s="159" t="s">
         <v>238</v>
       </c>
       <c r="D56" s="125"/>
       <c r="E56" s="131"/>
     </row>
     <row r="57" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B57" s="155"/>
-      <c r="C57" s="158"/>
+      <c r="B57" s="156"/>
+      <c r="C57" s="159"/>
       <c r="D57" s="125"/>
       <c r="E57" s="131"/>
     </row>
     <row r="58" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B58" s="155"/>
-      <c r="C58" s="158"/>
+      <c r="B58" s="156"/>
+      <c r="C58" s="159"/>
       <c r="D58" s="125"/>
       <c r="E58" s="131"/>
     </row>
     <row r="59" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B59" s="155"/>
-      <c r="C59" s="158"/>
+      <c r="B59" s="156"/>
+      <c r="C59" s="159"/>
       <c r="D59" s="125"/>
       <c r="E59" s="131"/>
     </row>
     <row r="60" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B60" s="156"/>
-      <c r="C60" s="161"/>
+      <c r="B60" s="157"/>
+      <c r="C60" s="162"/>
       <c r="D60" s="128"/>
       <c r="E60" s="133"/>
     </row>
@@ -6655,12 +6679,12 @@
       <c r="P2" s="78"/>
     </row>
     <row r="3" spans="2:18" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="150" t="s">
+      <c r="B3" s="151" t="s">
         <v>57</v>
       </c>
-      <c r="C3" s="150"/>
-      <c r="D3" s="150"/>
-      <c r="E3" s="150"/>
+      <c r="C3" s="151"/>
+      <c r="D3" s="151"/>
+      <c r="E3" s="151"/>
       <c r="F3" s="77"/>
       <c r="G3" s="77"/>
       <c r="H3" s="77"/>
@@ -6912,12 +6936,12 @@
       <c r="N2" s="78"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="150" t="s">
+      <c r="B3" s="151" t="s">
         <v>138</v>
       </c>
-      <c r="C3" s="150"/>
-      <c r="D3" s="150"/>
-      <c r="E3" s="150"/>
+      <c r="C3" s="151"/>
+      <c r="D3" s="151"/>
+      <c r="E3" s="151"/>
       <c r="F3" s="77"/>
       <c r="G3" s="77"/>
       <c r="H3" s="77"/>
@@ -7012,28 +7036,28 @@
       </c>
     </row>
     <row r="2" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="151"/>
-      <c r="C2" s="151"/>
-      <c r="D2" s="151"/>
-      <c r="E2" s="151"/>
-      <c r="F2" s="151"/>
-      <c r="G2" s="151"/>
-      <c r="H2" s="151"/>
-      <c r="I2" s="151"/>
-      <c r="J2" s="151"/>
+      <c r="B2" s="152"/>
+      <c r="C2" s="152"/>
+      <c r="D2" s="152"/>
+      <c r="E2" s="152"/>
+      <c r="F2" s="152"/>
+      <c r="G2" s="152"/>
+      <c r="H2" s="152"/>
+      <c r="I2" s="152"/>
+      <c r="J2" s="152"/>
     </row>
     <row r="3" spans="2:10" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="150" t="s">
+      <c r="B3" s="151" t="s">
         <v>141</v>
       </c>
-      <c r="C3" s="150"/>
-      <c r="D3" s="150"/>
-      <c r="E3" s="150"/>
-      <c r="F3" s="150"/>
-      <c r="G3" s="150"/>
-      <c r="H3" s="150"/>
-      <c r="I3" s="150"/>
-      <c r="J3" s="150"/>
+      <c r="C3" s="151"/>
+      <c r="D3" s="151"/>
+      <c r="E3" s="151"/>
+      <c r="F3" s="151"/>
+      <c r="G3" s="151"/>
+      <c r="H3" s="151"/>
+      <c r="I3" s="151"/>
+      <c r="J3" s="151"/>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" s="71" t="s">
@@ -7127,13 +7151,13 @@
       <c r="N2" s="78"/>
     </row>
     <row r="3" spans="2:20" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="150" t="s">
+      <c r="B3" s="151" t="s">
         <v>142</v>
       </c>
-      <c r="C3" s="150"/>
-      <c r="D3" s="150"/>
-      <c r="E3" s="150"/>
-      <c r="F3" s="150"/>
+      <c r="C3" s="151"/>
+      <c r="D3" s="151"/>
+      <c r="E3" s="151"/>
+      <c r="F3" s="151"/>
       <c r="G3" s="77"/>
       <c r="H3" s="77"/>
       <c r="I3" s="77"/>
@@ -7259,10 +7283,10 @@
       <c r="F2" s="77"/>
     </row>
     <row r="3" spans="2:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="150" t="s">
+      <c r="B3" s="151" t="s">
         <v>190</v>
       </c>
-      <c r="C3" s="150"/>
+      <c r="C3" s="151"/>
       <c r="D3" s="77"/>
       <c r="E3" s="77"/>
       <c r="F3" s="77"/>
@@ -7325,10 +7349,10 @@
       <c r="D2" s="77"/>
     </row>
     <row r="3" spans="2:4" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="150" t="s">
+      <c r="B3" s="151" t="s">
         <v>196</v>
       </c>
-      <c r="C3" s="150"/>
+      <c r="C3" s="151"/>
       <c r="D3" s="77"/>
     </row>
     <row r="5" spans="2:4" ht="27" x14ac:dyDescent="0.25">
@@ -7387,12 +7411,12 @@
       <c r="I2" s="78"/>
     </row>
     <row r="3" spans="2:9" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="150" t="s">
+      <c r="B3" s="151" t="s">
         <v>178</v>
       </c>
-      <c r="C3" s="150"/>
-      <c r="D3" s="150"/>
-      <c r="E3" s="150"/>
+      <c r="C3" s="151"/>
+      <c r="D3" s="151"/>
+      <c r="E3" s="151"/>
       <c r="F3" s="77"/>
       <c r="G3" s="77"/>
       <c r="H3" s="77"/>
@@ -7480,10 +7504,10 @@
       <c r="K2" s="78"/>
     </row>
     <row r="3" spans="2:11" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="150" t="s">
+      <c r="B3" s="151" t="s">
         <v>154</v>
       </c>
-      <c r="C3" s="150"/>
+      <c r="C3" s="151"/>
       <c r="D3" s="77"/>
       <c r="E3" s="77"/>
       <c r="F3" s="77"/>
@@ -7506,14 +7530,14 @@
       <c r="K4" s="79"/>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="H5" s="170" t="s">
+      <c r="H5" s="171" t="s">
         <v>162</v>
       </c>
-      <c r="I5" s="171"/>
-      <c r="J5" s="170" t="s">
+      <c r="I5" s="172"/>
+      <c r="J5" s="171" t="s">
         <v>161</v>
       </c>
-      <c r="K5" s="171"/>
+      <c r="K5" s="172"/>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" s="80" t="s">
@@ -7599,10 +7623,10 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="151" t="s">
+      <c r="B2" s="152" t="s">
         <v>82</v>
       </c>
-      <c r="C2" s="151"/>
+      <c r="C2" s="152"/>
       <c r="D2" s="78"/>
       <c r="E2" s="78"/>
       <c r="F2" s="78"/>
@@ -7700,11 +7724,11 @@
       <c r="H2" s="77"/>
     </row>
     <row r="3" spans="2:8" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="150" t="s">
+      <c r="B3" s="151" t="s">
         <v>201</v>
       </c>
-      <c r="C3" s="150"/>
-      <c r="D3" s="150"/>
+      <c r="C3" s="151"/>
+      <c r="D3" s="151"/>
       <c r="E3" s="77"/>
       <c r="F3" s="77"/>
       <c r="G3" s="77"/>
@@ -7759,13 +7783,13 @@
       <c r="C2" s="77"/>
     </row>
     <row r="3" spans="2:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="150" t="s">
+      <c r="B3" s="151" t="s">
         <v>202</v>
       </c>
-      <c r="C3" s="150"/>
-      <c r="D3" s="150"/>
-      <c r="E3" s="150"/>
-      <c r="F3" s="150"/>
+      <c r="C3" s="151"/>
+      <c r="D3" s="151"/>
+      <c r="E3" s="151"/>
+      <c r="F3" s="151"/>
     </row>
     <row r="5" spans="2:6" ht="27" x14ac:dyDescent="0.25">
       <c r="B5" s="91" t="s">
@@ -7818,11 +7842,11 @@
       <c r="H2" s="77"/>
     </row>
     <row r="3" spans="2:8" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="150" t="s">
+      <c r="B3" s="151" t="s">
         <v>204</v>
       </c>
-      <c r="C3" s="150"/>
-      <c r="D3" s="150"/>
+      <c r="C3" s="151"/>
+      <c r="D3" s="151"/>
       <c r="E3" s="77"/>
       <c r="F3" s="77"/>
       <c r="G3" s="77"/>
@@ -7944,11 +7968,11 @@
       <c r="H2" s="77"/>
     </row>
     <row r="3" spans="2:8" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="150" t="s">
+      <c r="B3" s="151" t="s">
         <v>207</v>
       </c>
-      <c r="C3" s="150"/>
-      <c r="D3" s="150"/>
+      <c r="C3" s="151"/>
+      <c r="D3" s="151"/>
       <c r="E3" s="77"/>
       <c r="F3" s="77"/>
       <c r="G3" s="77"/>
@@ -8004,12 +8028,12 @@
       <c r="H2" s="77"/>
     </row>
     <row r="3" spans="2:8" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="150" t="s">
+      <c r="B3" s="151" t="s">
         <v>210</v>
       </c>
-      <c r="C3" s="150"/>
-      <c r="D3" s="150"/>
-      <c r="E3" s="150"/>
+      <c r="C3" s="151"/>
+      <c r="D3" s="151"/>
+      <c r="E3" s="151"/>
       <c r="F3" s="77"/>
       <c r="G3" s="77"/>
       <c r="H3" s="77"/>
@@ -8148,10 +8172,10 @@
       <c r="Z2"/>
     </row>
     <row r="3" spans="2:26" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="150" t="s">
+      <c r="B3" s="151" t="s">
         <v>253</v>
       </c>
-      <c r="C3" s="150"/>
+      <c r="C3" s="151"/>
       <c r="D3" s="77"/>
       <c r="E3" s="77"/>
       <c r="F3" s="77"/>
@@ -8281,10 +8305,10 @@
       <c r="Z2"/>
     </row>
     <row r="3" spans="2:26" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="150" t="s">
+      <c r="B3" s="151" t="s">
         <v>260</v>
       </c>
-      <c r="C3" s="150"/>
+      <c r="C3" s="151"/>
       <c r="D3" s="77"/>
       <c r="E3" s="77"/>
       <c r="F3" s="77"/>
@@ -8314,9 +8338,9 @@
       <c r="C6" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="D6" s="172"/>
-      <c r="E6" s="173"/>
-      <c r="F6" s="174"/>
+      <c r="D6" s="173"/>
+      <c r="E6" s="174"/>
+      <c r="F6" s="175"/>
       <c r="G6" s="48"/>
       <c r="H6" s="48"/>
     </row>
@@ -8409,10 +8433,10 @@
       <c r="Z2"/>
     </row>
     <row r="3" spans="2:26" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="150" t="s">
+      <c r="B3" s="151" t="s">
         <v>79</v>
       </c>
-      <c r="C3" s="150"/>
+      <c r="C3" s="151"/>
       <c r="D3" s="77"/>
       <c r="E3" s="77"/>
       <c r="F3" s="77"/>
@@ -8531,10 +8555,10 @@
       <c r="M2" s="78"/>
     </row>
     <row r="3" spans="2:13" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="150" t="s">
+      <c r="B3" s="151" t="s">
         <v>225</v>
       </c>
-      <c r="C3" s="150"/>
+      <c r="C3" s="151"/>
       <c r="D3" s="77"/>
       <c r="E3" s="77"/>
       <c r="F3" s="77"/>
@@ -8604,10 +8628,10 @@
       <c r="Z2"/>
     </row>
     <row r="3" spans="2:26" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="150" t="s">
+      <c r="B3" s="151" t="s">
         <v>64</v>
       </c>
-      <c r="C3" s="150"/>
+      <c r="C3" s="151"/>
       <c r="D3" s="77"/>
       <c r="E3" s="77"/>
       <c r="F3" s="77"/>
@@ -8737,12 +8761,12 @@
       <c r="L2" s="78"/>
     </row>
     <row r="3" spans="2:17" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="150" t="s">
+      <c r="B3" s="151" t="s">
         <v>94</v>
       </c>
-      <c r="C3" s="150"/>
-      <c r="D3" s="150"/>
-      <c r="E3" s="150"/>
+      <c r="C3" s="151"/>
+      <c r="D3" s="151"/>
+      <c r="E3" s="151"/>
       <c r="F3" s="77"/>
       <c r="G3" s="77"/>
       <c r="H3" s="77"/>
@@ -8752,28 +8776,28 @@
       <c r="L3" s="77"/>
     </row>
     <row r="5" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D5" s="175" t="s">
+      <c r="D5" s="176" t="s">
         <v>109</v>
       </c>
-      <c r="E5" s="175"/>
+      <c r="E5" s="176"/>
       <c r="F5" s="70"/>
       <c r="G5" s="70"/>
       <c r="H5" s="70"/>
       <c r="I5" s="70"/>
-      <c r="J5" s="175" t="s">
+      <c r="J5" s="176" t="s">
         <v>37</v>
       </c>
-      <c r="K5" s="175"/>
-      <c r="L5" s="175"/>
-      <c r="M5" s="175" t="s">
+      <c r="K5" s="176"/>
+      <c r="L5" s="176"/>
+      <c r="M5" s="176" t="s">
         <v>116</v>
       </c>
-      <c r="N5" s="175"/>
-      <c r="O5" s="175"/>
-      <c r="P5" s="152" t="s">
+      <c r="N5" s="176"/>
+      <c r="O5" s="176"/>
+      <c r="P5" s="153" t="s">
         <v>95</v>
       </c>
-      <c r="Q5" s="152"/>
+      <c r="Q5" s="153"/>
     </row>
     <row r="6" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="67" t="s">
@@ -8912,11 +8936,11 @@
       <c r="R2" s="53"/>
     </row>
     <row r="3" spans="2:25" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="150" t="s">
+      <c r="B3" s="151" t="s">
         <v>97</v>
       </c>
-      <c r="C3" s="150"/>
-      <c r="D3" s="150"/>
+      <c r="C3" s="151"/>
+      <c r="D3" s="151"/>
       <c r="E3" s="77"/>
       <c r="F3" s="77"/>
       <c r="G3" s="77"/>
@@ -8933,70 +8957,70 @@
       <c r="R3" s="54"/>
     </row>
     <row r="5" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B5" s="178" t="s">
+      <c r="B5" s="179" t="s">
         <v>98</v>
       </c>
-      <c r="C5" s="179"/>
-      <c r="D5" s="179"/>
-      <c r="E5" s="179"/>
-      <c r="F5" s="179"/>
-      <c r="G5" s="179"/>
-      <c r="H5" s="179"/>
-      <c r="I5" s="179"/>
-      <c r="J5" s="179"/>
-      <c r="K5" s="179"/>
-      <c r="L5" s="180"/>
-      <c r="M5" s="178" t="s">
+      <c r="C5" s="180"/>
+      <c r="D5" s="180"/>
+      <c r="E5" s="180"/>
+      <c r="F5" s="180"/>
+      <c r="G5" s="180"/>
+      <c r="H5" s="180"/>
+      <c r="I5" s="180"/>
+      <c r="J5" s="180"/>
+      <c r="K5" s="180"/>
+      <c r="L5" s="181"/>
+      <c r="M5" s="179" t="s">
         <v>99</v>
       </c>
-      <c r="N5" s="179"/>
-      <c r="O5" s="179"/>
-      <c r="P5" s="179"/>
-      <c r="Q5" s="179"/>
-      <c r="R5" s="179"/>
-      <c r="S5" s="179"/>
-      <c r="T5" s="179"/>
-      <c r="U5" s="179"/>
-      <c r="V5" s="179"/>
-      <c r="W5" s="179"/>
-      <c r="X5" s="179"/>
-      <c r="Y5" s="180"/>
+      <c r="N5" s="180"/>
+      <c r="O5" s="180"/>
+      <c r="P5" s="180"/>
+      <c r="Q5" s="180"/>
+      <c r="R5" s="180"/>
+      <c r="S5" s="180"/>
+      <c r="T5" s="180"/>
+      <c r="U5" s="180"/>
+      <c r="V5" s="180"/>
+      <c r="W5" s="180"/>
+      <c r="X5" s="180"/>
+      <c r="Y5" s="181"/>
     </row>
     <row r="6" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B6" s="188"/>
-      <c r="C6" s="188"/>
-      <c r="D6" s="188"/>
-      <c r="E6" s="188"/>
-      <c r="F6" s="184" t="s">
+      <c r="B6" s="189"/>
+      <c r="C6" s="189"/>
+      <c r="D6" s="189"/>
+      <c r="E6" s="189"/>
+      <c r="F6" s="185" t="s">
         <v>25</v>
       </c>
-      <c r="G6" s="185"/>
-      <c r="H6" s="185"/>
-      <c r="I6" s="186"/>
-      <c r="J6" s="178" t="s">
+      <c r="G6" s="186"/>
+      <c r="H6" s="186"/>
+      <c r="I6" s="187"/>
+      <c r="J6" s="179" t="s">
         <v>28</v>
       </c>
-      <c r="K6" s="179"/>
-      <c r="L6" s="180"/>
+      <c r="K6" s="180"/>
+      <c r="L6" s="181"/>
       <c r="M6" s="81"/>
-      <c r="N6" s="176" t="s">
+      <c r="N6" s="177" t="s">
         <v>37</v>
       </c>
-      <c r="O6" s="177"/>
-      <c r="P6" s="176" t="s">
+      <c r="O6" s="178"/>
+      <c r="P6" s="177" t="s">
         <v>92</v>
       </c>
-      <c r="Q6" s="187"/>
-      <c r="R6" s="177"/>
+      <c r="Q6" s="188"/>
+      <c r="R6" s="178"/>
       <c r="S6" s="81"/>
-      <c r="T6" s="176" t="s">
+      <c r="T6" s="177" t="s">
         <v>109</v>
       </c>
-      <c r="U6" s="177"/>
-      <c r="V6" s="181"/>
-      <c r="W6" s="182"/>
-      <c r="X6" s="182"/>
-      <c r="Y6" s="183"/>
+      <c r="U6" s="178"/>
+      <c r="V6" s="182"/>
+      <c r="W6" s="183"/>
+      <c r="X6" s="183"/>
+      <c r="Y6" s="184"/>
     </row>
     <row r="7" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B7" s="72" t="s">
@@ -9226,14 +9250,14 @@
       </c>
     </row>
     <row r="2" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="151" t="s">
+      <c r="B2" s="152" t="s">
         <v>83</v>
       </c>
-      <c r="C2" s="151"/>
-      <c r="D2" s="151"/>
-      <c r="E2" s="151"/>
-      <c r="F2" s="151"/>
-      <c r="G2" s="151"/>
+      <c r="C2" s="152"/>
+      <c r="D2" s="152"/>
+      <c r="E2" s="152"/>
+      <c r="F2" s="152"/>
+      <c r="G2" s="152"/>
     </row>
     <row r="3" spans="2:7" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="77" t="s">
@@ -9289,20 +9313,20 @@
       </c>
     </row>
     <row r="2" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="151" t="s">
+      <c r="B2" s="152" t="s">
         <v>262</v>
       </c>
-      <c r="C2" s="151"/>
-      <c r="D2" s="151"/>
-      <c r="E2" s="151"/>
-      <c r="F2" s="151"/>
-      <c r="G2" s="151"/>
+      <c r="C2" s="152"/>
+      <c r="D2" s="152"/>
+      <c r="E2" s="152"/>
+      <c r="F2" s="152"/>
+      <c r="G2" s="152"/>
     </row>
     <row r="3" spans="2:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="150" t="s">
+      <c r="B3" s="151" t="s">
         <v>227</v>
       </c>
-      <c r="C3" s="150"/>
+      <c r="C3" s="151"/>
     </row>
     <row r="4" spans="2:7" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="93"/>
@@ -9369,10 +9393,10 @@
     </row>
     <row r="3" spans="1:10" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="145"/>
-      <c r="B3" s="150" t="s">
+      <c r="B3" s="151" t="s">
         <v>254</v>
       </c>
-      <c r="C3" s="150"/>
+      <c r="C3" s="151"/>
       <c r="D3" s="77"/>
       <c r="E3" s="77"/>
       <c r="F3" s="77"/>
@@ -9461,11 +9485,11 @@
       <c r="E2" s="78"/>
     </row>
     <row r="3" spans="2:5" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="150" t="s">
+      <c r="B3" s="151" t="s">
         <v>117</v>
       </c>
-      <c r="C3" s="150"/>
-      <c r="D3" s="150"/>
+      <c r="C3" s="151"/>
+      <c r="D3" s="151"/>
       <c r="E3" s="77"/>
     </row>
     <row r="4" spans="2:5" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
TRIEDA-1776 - Alterando tela de Ofertas e Demandas e criação de demandas. Criando algoritmo para gerar demandas de alunos virtuais. Criando algoritmo de criar demandas na importação. Alterando BD para remover a coluna de quantidade da tabela demandas.
</commit_message>
<xml_diff>
--- a/code/client/web/src/main/resources/templateExport.xlsx
+++ b/code/client/web/src/main/resources/templateExport.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="17070" windowHeight="5370" tabRatio="826"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="17070" windowHeight="5370" tabRatio="919" firstSheet="18" activeTab="21"/>
   </bookViews>
   <sheets>
     <sheet name="Turnos" sheetId="49" r:id="rId1"/>
@@ -71,7 +71,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="E5" authorId="0" shapeId="0">
+    <comment ref="E5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -132,7 +132,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="B5" authorId="0" shapeId="0">
+    <comment ref="B5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -155,7 +155,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F5" authorId="0" shapeId="0">
+    <comment ref="F5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -194,7 +194,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G5" authorId="0" shapeId="0">
+    <comment ref="G5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -267,7 +267,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H5" authorId="0" shapeId="0">
+    <comment ref="H5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -379,7 +379,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I5" authorId="0" shapeId="0">
+    <comment ref="I5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -405,7 +405,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J5" authorId="0" shapeId="0">
+    <comment ref="J5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -431,7 +431,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K5" authorId="0" shapeId="0">
+    <comment ref="K5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -447,7 +447,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L5" authorId="0" shapeId="0">
+    <comment ref="L5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -463,7 +463,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M5" authorId="0" shapeId="0">
+    <comment ref="M5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -479,7 +479,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N5" authorId="0" shapeId="0">
+    <comment ref="N5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -505,7 +505,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="B5" authorId="0" shapeId="0">
+    <comment ref="B5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -538,7 +538,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="B5" authorId="0" shapeId="0">
+    <comment ref="B5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -552,7 +552,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C5" authorId="0" shapeId="0">
+    <comment ref="C5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -566,7 +566,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D5" authorId="0" shapeId="0">
+    <comment ref="D5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -599,7 +599,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="I5" authorId="0" shapeId="0">
+    <comment ref="K5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -623,7 +623,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="D5" authorId="0" shapeId="0">
+    <comment ref="D5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -638,7 +638,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E5" authorId="0" shapeId="0">
+    <comment ref="E5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -663,7 +663,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F5" authorId="0" shapeId="0">
+    <comment ref="F5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -717,7 +717,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="D5" authorId="0" shapeId="0">
+    <comment ref="D5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -791,7 +791,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E5" authorId="0" shapeId="0">
+    <comment ref="E5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -805,7 +805,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F5" authorId="0" shapeId="0">
+    <comment ref="F5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -819,7 +819,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G5" authorId="0" shapeId="0">
+    <comment ref="G5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -836,7 +836,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I5" authorId="0" shapeId="0">
+    <comment ref="I5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -863,7 +863,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J5" authorId="0" shapeId="0">
+    <comment ref="J5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -877,7 +877,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K5" authorId="0" shapeId="0">
+    <comment ref="K5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -919,7 +919,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="C5" authorId="0" shapeId="0">
+    <comment ref="C5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -949,7 +949,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="D5" authorId="0" shapeId="0">
+    <comment ref="D5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -976,7 +976,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E5" authorId="0" shapeId="0">
+    <comment ref="E5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1011,7 +1011,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="Z1" authorId="0" shapeId="0">
+    <comment ref="Z1" authorId="0">
       <text/>
     </comment>
   </commentList>
@@ -1024,7 +1024,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="Z1" authorId="0" shapeId="0">
+    <comment ref="Z1" authorId="0">
       <text/>
     </comment>
   </commentList>
@@ -1037,7 +1037,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="E5" authorId="0" shapeId="0">
+    <comment ref="E5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1088,7 +1088,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F5" authorId="0" shapeId="0">
+    <comment ref="F5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1139,7 +1139,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G5" authorId="0" shapeId="0">
+    <comment ref="G5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1190,7 +1190,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H5" authorId="0" shapeId="0">
+    <comment ref="H5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1241,7 +1241,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I5" authorId="0" shapeId="0">
+    <comment ref="I5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1292,7 +1292,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J5" authorId="0" shapeId="0">
+    <comment ref="J5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1343,7 +1343,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K5" authorId="0" shapeId="0">
+    <comment ref="K5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1404,7 +1404,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="Z1" authorId="0" shapeId="0">
+    <comment ref="Z1" authorId="0">
       <text/>
     </comment>
   </commentList>
@@ -1417,7 +1417,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="Z1" authorId="0" shapeId="0">
+    <comment ref="Z1" authorId="0">
       <text/>
     </comment>
   </commentList>
@@ -1430,7 +1430,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="B5" authorId="0" shapeId="0">
+    <comment ref="B5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1453,7 +1453,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G5" authorId="0" shapeId="0">
+    <comment ref="G5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1486,7 +1486,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="B5" authorId="0" shapeId="0">
+    <comment ref="B5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1509,7 +1509,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D5" authorId="0" shapeId="0">
+    <comment ref="D5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1542,7 +1542,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="B5" authorId="0" shapeId="0">
+    <comment ref="B5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1565,7 +1565,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C5" authorId="0" shapeId="0">
+    <comment ref="C5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1638,7 +1638,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D5" authorId="0" shapeId="0">
+    <comment ref="D5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1680,7 +1680,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="C5" authorId="0" shapeId="0">
+    <comment ref="C5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1710,7 +1710,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="B5" authorId="0" shapeId="0">
+    <comment ref="B5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1733,7 +1733,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D5" authorId="0" shapeId="0">
+    <comment ref="D5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1843,7 +1843,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I5" authorId="0" shapeId="0">
+    <comment ref="I5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1866,7 +1866,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J5" authorId="0" shapeId="0">
+    <comment ref="J5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1908,7 +1908,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="B5" authorId="0" shapeId="0">
+    <comment ref="B5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1941,7 +1941,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="B5" authorId="0" shapeId="0">
+    <comment ref="B5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1960,7 +1960,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="269">
   <si>
     <t>Planilha de Unidades</t>
   </si>
@@ -2818,6 +2818,15 @@
   </si>
   <si>
     <t>Planilha de Número de Ambientes por Faixa de Utilização Média dos Horários</t>
+  </si>
+  <si>
+    <t>Demanda de Alunos (Real)</t>
+  </si>
+  <si>
+    <t>Demanda de Alunos (Virtual)</t>
+  </si>
+  <si>
+    <t>Demanda de Alunos (Total)</t>
   </si>
 </sst>
 </file>
@@ -4017,9 +4026,6 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -4041,7 +4047,7 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="71745" name=":0_674" descr="https://plus.google.com/u/0/_/focus/photos/private/AIbEiAIAAABDCK-Xzbi8pY7DeSILdmNhcmRfcGhvdG8qKDIxMGNjNTM3ZWQ4NjZjNTU4NTk4YjQ0ZDUwM2EwNmUxOGE4OTQyMTIwAdCjuGFdYwQCNlcR6WXw_rsQlR6Q?sz=32"/>
+        <xdr:cNvPr id="71749" name=":0_674" descr="https://plus.google.com/u/0/_/focus/photos/private/AIbEiAIAAABDCK-Xzbi8pY7DeSILdmNhcmRfcGhvdG8qKDIxMGNjNTM3ZWQ4NjZjNTU4NTk4YjQ0ZDUwM2EwNmUxOGE4OTQyMTIwAdCjuGFdYwQCNlcR6WXw_rsQlR6Q?sz=32"/>
         <xdr:cNvSpPr>
           <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -4127,7 +4133,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4162,7 +4168,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4373,7 +4379,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K6"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -5451,10 +5457,10 @@
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:M6"/>
+  <dimension ref="B1:O6"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="Q42" sqref="Q42"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5466,20 +5472,22 @@
     <col min="5" max="5" width="20.140625" customWidth="1"/>
     <col min="6" max="6" width="9.85546875" customWidth="1"/>
     <col min="7" max="7" width="19.28515625" customWidth="1"/>
-    <col min="8" max="8" width="20.5703125" customWidth="1"/>
-    <col min="9" max="9" width="28" customWidth="1"/>
-    <col min="10" max="10" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="33.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="27.7109375" customWidth="1"/>
+    <col min="8" max="8" width="29.140625" customWidth="1"/>
+    <col min="9" max="9" width="29.7109375" customWidth="1"/>
+    <col min="10" max="10" width="31.42578125" customWidth="1"/>
+    <col min="11" max="11" width="28" customWidth="1"/>
+    <col min="12" max="12" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="33.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="27.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:15" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="44" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="2:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="152"/>
       <c r="C2" s="152"/>
       <c r="D2" s="152"/>
@@ -5492,8 +5500,10 @@
       <c r="K2" s="152"/>
       <c r="L2" s="152"/>
       <c r="M2" s="152"/>
-    </row>
-    <row r="3" spans="2:13" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="N2" s="152"/>
+      <c r="O2" s="152"/>
+    </row>
+    <row r="3" spans="2:15" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="151" t="s">
         <v>29</v>
       </c>
@@ -5508,8 +5518,10 @@
       <c r="K3" s="151"/>
       <c r="L3" s="151"/>
       <c r="M3" s="151"/>
-    </row>
-    <row r="5" spans="2:13" s="144" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="N3" s="151"/>
+      <c r="O3" s="151"/>
+    </row>
+    <row r="5" spans="2:15" s="144" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="143" t="s">
         <v>67</v>
       </c>
@@ -5529,25 +5541,31 @@
         <v>75</v>
       </c>
       <c r="H5" s="45" t="s">
-        <v>28</v>
+        <v>266</v>
       </c>
       <c r="I5" s="45" t="s">
+        <v>267</v>
+      </c>
+      <c r="J5" s="45" t="s">
+        <v>268</v>
+      </c>
+      <c r="K5" s="45" t="s">
         <v>262</v>
       </c>
-      <c r="J5" s="45" t="s">
+      <c r="L5" s="45" t="s">
         <v>92</v>
       </c>
-      <c r="K5" s="45" t="s">
+      <c r="M5" s="45" t="s">
         <v>93</v>
       </c>
-      <c r="L5" s="45" t="s">
+      <c r="N5" s="45" t="s">
         <v>123</v>
       </c>
-      <c r="M5" s="45" t="s">
+      <c r="O5" s="45" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
@@ -5555,16 +5573,18 @@
       <c r="F6" s="9"/>
       <c r="G6" s="2"/>
       <c r="H6" s="9"/>
-      <c r="I6" s="7"/>
+      <c r="I6" s="9"/>
       <c r="J6" s="9"/>
-      <c r="K6" s="9"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="83"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="83"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B2:M2"/>
-    <mergeCell ref="B3:M3"/>
+    <mergeCell ref="B2:O2"/>
+    <mergeCell ref="B3:O3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
TRIEDA-1786 - Adicionando motivos de nao atendimentos no output. Criando modal para mostrar motivo de nao atendimento. Alterando export para mostrar motivos de nao atendimento. Criando script para atualizar BD
</commit_message>
<xml_diff>
--- a/code/client/web/src/main/resources/templateExport.xlsx
+++ b/code/client/web/src/main/resources/templateExport.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="17070" windowHeight="5370" tabRatio="919" firstSheet="18" activeTab="21"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="17070" windowHeight="5370" tabRatio="919" firstSheet="18" activeTab="23"/>
   </bookViews>
   <sheets>
     <sheet name="Turnos" sheetId="49" r:id="rId1"/>
@@ -1960,7 +1960,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="270">
   <si>
     <t>Planilha de Unidades</t>
   </si>
@@ -2827,6 +2827,9 @@
   </si>
   <si>
     <t>Demanda de Alunos (Total)</t>
+  </si>
+  <si>
+    <t>Motivos Não Atendimento</t>
   </si>
 </sst>
 </file>
@@ -3491,7 +3494,7 @@
     <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="190">
+  <cellXfs count="191">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -3892,6 +3895,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4047,7 +4053,7 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="71749" name=":0_674" descr="https://plus.google.com/u/0/_/focus/photos/private/AIbEiAIAAABDCK-Xzbi8pY7DeSILdmNhcmRfcGhvdG8qKDIxMGNjNTM3ZWQ4NjZjNTU4NTk4YjQ0ZDUwM2EwNmUxOGE4OTQyMTIwAdCjuGFdYwQCNlcR6WXw_rsQlR6Q?sz=32"/>
+        <xdr:cNvPr id="71752" name=":0_674" descr="https://plus.google.com/u/0/_/focus/photos/private/AIbEiAIAAABDCK-Xzbi8pY7DeSILdmNhcmRfcGhvdG8qKDIxMGNjNTM3ZWQ4NjZjNTU4NTk4YjQ0ZDUwM2EwNmUxOGE4OTQyMTIwAdCjuGFdYwQCNlcR6WXw_rsQlR6Q?sz=32"/>
         <xdr:cNvSpPr>
           <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -4577,10 +4583,10 @@
       <c r="I2" s="78"/>
     </row>
     <row r="3" spans="2:9" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="151" t="s">
+      <c r="B3" s="152" t="s">
         <v>214</v>
       </c>
-      <c r="C3" s="151"/>
+      <c r="C3" s="152"/>
       <c r="D3" s="77"/>
       <c r="E3" s="77"/>
       <c r="F3" s="77"/>
@@ -4641,10 +4647,10 @@
       <c r="I2" s="78"/>
     </row>
     <row r="3" spans="2:9" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="151" t="s">
+      <c r="B3" s="152" t="s">
         <v>240</v>
       </c>
-      <c r="C3" s="151"/>
+      <c r="C3" s="152"/>
       <c r="D3" s="77"/>
       <c r="E3" s="77"/>
       <c r="F3" s="77"/>
@@ -4717,10 +4723,10 @@
       <c r="P2" s="78"/>
     </row>
     <row r="3" spans="2:16" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="151" t="s">
+      <c r="B3" s="152" t="s">
         <v>239</v>
       </c>
-      <c r="C3" s="151"/>
+      <c r="C3" s="152"/>
       <c r="D3" s="77"/>
       <c r="E3" s="77"/>
       <c r="F3" s="77"/>
@@ -4806,10 +4812,10 @@
       <c r="P2" s="78"/>
     </row>
     <row r="3" spans="2:16" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="151" t="s">
+      <c r="B3" s="152" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="151"/>
+      <c r="C3" s="152"/>
       <c r="D3" s="77"/>
       <c r="E3" s="77"/>
       <c r="F3" s="77"/>
@@ -4923,11 +4929,11 @@
       <c r="K2" s="78"/>
     </row>
     <row r="3" spans="2:11" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="151" t="s">
+      <c r="B3" s="152" t="s">
         <v>216</v>
       </c>
-      <c r="C3" s="151"/>
-      <c r="D3" s="151"/>
+      <c r="C3" s="152"/>
+      <c r="D3" s="152"/>
       <c r="E3" s="77"/>
       <c r="F3" s="77"/>
       <c r="G3" s="77"/>
@@ -5010,11 +5016,11 @@
       <c r="G2" s="78"/>
     </row>
     <row r="3" spans="2:7" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="151" t="s">
+      <c r="B3" s="152" t="s">
         <v>59</v>
       </c>
-      <c r="C3" s="151"/>
-      <c r="D3" s="151"/>
+      <c r="C3" s="152"/>
+      <c r="D3" s="152"/>
       <c r="E3" s="77"/>
       <c r="F3" s="77"/>
       <c r="G3" s="77"/>
@@ -5070,12 +5076,12 @@
       <c r="C2" s="78"/>
     </row>
     <row r="3" spans="2:5" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="151" t="s">
+      <c r="B3" s="152" t="s">
         <v>254</v>
       </c>
-      <c r="C3" s="151"/>
-      <c r="D3" s="151"/>
-      <c r="E3" s="151"/>
+      <c r="C3" s="152"/>
+      <c r="D3" s="152"/>
+      <c r="E3" s="152"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -5130,10 +5136,10 @@
       <c r="G2" s="78"/>
     </row>
     <row r="3" spans="2:7" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="151" t="s">
+      <c r="B3" s="152" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="151"/>
+      <c r="C3" s="152"/>
       <c r="D3" s="77"/>
       <c r="E3" s="77"/>
       <c r="F3" s="77"/>
@@ -5205,11 +5211,11 @@
       <c r="E2" s="78"/>
     </row>
     <row r="3" spans="2:5" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="151" t="s">
+      <c r="B3" s="152" t="s">
         <v>255</v>
       </c>
-      <c r="C3" s="151"/>
-      <c r="D3" s="151"/>
+      <c r="C3" s="152"/>
+      <c r="D3" s="152"/>
       <c r="E3" s="77"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
@@ -5275,10 +5281,10 @@
       <c r="I2" s="78"/>
     </row>
     <row r="3" spans="2:11" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="151" t="s">
+      <c r="B3" s="152" t="s">
         <v>243</v>
       </c>
-      <c r="C3" s="151"/>
+      <c r="C3" s="152"/>
       <c r="D3" s="77"/>
       <c r="E3" s="77"/>
       <c r="F3" s="77"/>
@@ -5347,11 +5353,11 @@
       <c r="E2" s="78"/>
     </row>
     <row r="3" spans="2:5" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="151" t="s">
+      <c r="B3" s="152" t="s">
         <v>256</v>
       </c>
-      <c r="C3" s="151"/>
-      <c r="D3" s="151"/>
+      <c r="C3" s="152"/>
+      <c r="D3" s="152"/>
       <c r="E3" s="77"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
@@ -5414,11 +5420,11 @@
       <c r="F2" s="78"/>
     </row>
     <row r="3" spans="2:6" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="151" t="s">
+      <c r="B3" s="152" t="s">
         <v>189</v>
       </c>
-      <c r="C3" s="151"/>
-      <c r="D3" s="151"/>
+      <c r="C3" s="152"/>
+      <c r="D3" s="152"/>
       <c r="E3" s="77"/>
       <c r="F3" s="77"/>
     </row>
@@ -5459,7 +5465,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O6"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
@@ -5488,38 +5494,38 @@
       </c>
     </row>
     <row r="2" spans="2:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="152"/>
-      <c r="C2" s="152"/>
-      <c r="D2" s="152"/>
-      <c r="E2" s="152"/>
-      <c r="F2" s="152"/>
-      <c r="G2" s="152"/>
-      <c r="H2" s="152"/>
-      <c r="I2" s="152"/>
-      <c r="J2" s="152"/>
-      <c r="K2" s="152"/>
-      <c r="L2" s="152"/>
-      <c r="M2" s="152"/>
-      <c r="N2" s="152"/>
-      <c r="O2" s="152"/>
+      <c r="B2" s="153"/>
+      <c r="C2" s="153"/>
+      <c r="D2" s="153"/>
+      <c r="E2" s="153"/>
+      <c r="F2" s="153"/>
+      <c r="G2" s="153"/>
+      <c r="H2" s="153"/>
+      <c r="I2" s="153"/>
+      <c r="J2" s="153"/>
+      <c r="K2" s="153"/>
+      <c r="L2" s="153"/>
+      <c r="M2" s="153"/>
+      <c r="N2" s="153"/>
+      <c r="O2" s="153"/>
     </row>
     <row r="3" spans="2:15" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="151" t="s">
+      <c r="B3" s="152" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="151"/>
-      <c r="D3" s="151"/>
-      <c r="E3" s="151"/>
-      <c r="F3" s="151"/>
-      <c r="G3" s="151"/>
-      <c r="H3" s="151"/>
-      <c r="I3" s="151"/>
-      <c r="J3" s="151"/>
-      <c r="K3" s="151"/>
-      <c r="L3" s="151"/>
-      <c r="M3" s="151"/>
-      <c r="N3" s="151"/>
-      <c r="O3" s="151"/>
+      <c r="C3" s="152"/>
+      <c r="D3" s="152"/>
+      <c r="E3" s="152"/>
+      <c r="F3" s="152"/>
+      <c r="G3" s="152"/>
+      <c r="H3" s="152"/>
+      <c r="I3" s="152"/>
+      <c r="J3" s="152"/>
+      <c r="K3" s="152"/>
+      <c r="L3" s="152"/>
+      <c r="M3" s="152"/>
+      <c r="N3" s="152"/>
+      <c r="O3" s="152"/>
     </row>
     <row r="5" spans="2:15" s="144" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="143" t="s">
@@ -5620,10 +5626,10 @@
       <c r="D2" s="78"/>
     </row>
     <row r="3" spans="2:6" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="151" t="s">
+      <c r="B3" s="152" t="s">
         <v>112</v>
       </c>
-      <c r="C3" s="151"/>
+      <c r="C3" s="152"/>
       <c r="D3" s="77"/>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
@@ -5661,10 +5667,10 @@
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:N6"/>
+  <dimension ref="B1:O6"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5679,14 +5685,15 @@
     <col min="9" max="9" width="56.42578125" customWidth="1"/>
     <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15" customWidth="1"/>
+    <col min="12" max="12" width="34.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:15" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="44" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="78"/>
       <c r="C2" s="78"/>
       <c r="D2" s="78"/>
@@ -5700,8 +5707,9 @@
       <c r="L2" s="78"/>
       <c r="M2" s="78"/>
       <c r="N2" s="78"/>
-    </row>
-    <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="O2" s="78"/>
+    </row>
+    <row r="3" spans="2:15" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="77" t="s">
         <v>86</v>
       </c>
@@ -5717,8 +5725,9 @@
       <c r="L3" s="77"/>
       <c r="M3" s="77"/>
       <c r="N3" s="77"/>
-    </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="O3" s="77"/>
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>67</v>
       </c>
@@ -5749,12 +5758,15 @@
       <c r="K5" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="L5" s="153" t="s">
+      <c r="L5" s="151" t="s">
+        <v>269</v>
+      </c>
+      <c r="M5" s="154" t="s">
         <v>96</v>
       </c>
-      <c r="M5" s="153"/>
-    </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="N5" s="154"/>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
@@ -5765,13 +5777,14 @@
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
-      <c r="L6" s="154"/>
-      <c r="M6" s="154"/>
+      <c r="L6" s="83"/>
+      <c r="M6" s="155"/>
+      <c r="N6" s="155"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="M6:N6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5824,10 +5837,10 @@
       <c r="O2" s="78"/>
     </row>
     <row r="3" spans="2:15" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="151" t="s">
+      <c r="B3" s="152" t="s">
         <v>65</v>
       </c>
-      <c r="C3" s="151"/>
+      <c r="C3" s="152"/>
       <c r="D3" s="77"/>
       <c r="E3" s="77"/>
       <c r="F3" s="77"/>
@@ -5932,11 +5945,11 @@
       <c r="E2" s="78"/>
     </row>
     <row r="3" spans="2:5" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="151" t="s">
+      <c r="B3" s="152" t="s">
         <v>117</v>
       </c>
-      <c r="C3" s="151"/>
-      <c r="D3" s="151"/>
+      <c r="C3" s="152"/>
+      <c r="D3" s="152"/>
       <c r="E3" s="77"/>
     </row>
     <row r="4" spans="2:5" customFormat="1" x14ac:dyDescent="0.25">
@@ -5998,10 +6011,10 @@
       <c r="D2" s="78"/>
     </row>
     <row r="3" spans="2:4" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="151" t="s">
+      <c r="B3" s="152" t="s">
         <v>62</v>
       </c>
-      <c r="C3" s="151"/>
+      <c r="C3" s="152"/>
       <c r="D3" s="77"/>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
@@ -6058,11 +6071,11 @@
       <c r="E2" s="78"/>
     </row>
     <row r="3" spans="2:5" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="151" t="s">
+      <c r="B3" s="152" t="s">
         <v>66</v>
       </c>
-      <c r="C3" s="151"/>
-      <c r="D3" s="151"/>
+      <c r="C3" s="152"/>
+      <c r="D3" s="152"/>
       <c r="E3" s="77"/>
     </row>
     <row r="5" spans="2:5" s="144" customFormat="1" x14ac:dyDescent="0.25">
@@ -6174,13 +6187,13 @@
       <c r="I2" s="78"/>
     </row>
     <row r="3" spans="2:11" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="151" t="s">
+      <c r="B3" s="152" t="s">
         <v>247</v>
       </c>
-      <c r="C3" s="151"/>
-      <c r="D3" s="151"/>
-      <c r="E3" s="151"/>
-      <c r="F3" s="151"/>
+      <c r="C3" s="152"/>
+      <c r="D3" s="152"/>
+      <c r="E3" s="152"/>
+      <c r="F3" s="152"/>
       <c r="G3" s="77"/>
       <c r="H3" s="77"/>
       <c r="I3" s="77"/>
@@ -6281,11 +6294,11 @@
       <c r="P2" s="78"/>
     </row>
     <row r="3" spans="2:16" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="151" t="s">
+      <c r="B3" s="152" t="s">
         <v>231</v>
       </c>
-      <c r="C3" s="151"/>
-      <c r="D3" s="151"/>
+      <c r="C3" s="152"/>
+      <c r="D3" s="152"/>
       <c r="E3" s="77"/>
       <c r="F3" s="77"/>
       <c r="G3" s="77"/>
@@ -6320,7 +6333,7 @@
       <c r="E5" s="129"/>
     </row>
     <row r="6" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="163" t="s">
+      <c r="B6" s="164" t="s">
         <v>232</v>
       </c>
       <c r="C6" s="97"/>
@@ -6328,91 +6341,91 @@
       <c r="E6" s="130"/>
     </row>
     <row r="7" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="164"/>
+      <c r="B7" s="165"/>
       <c r="C7" s="99"/>
       <c r="D7" s="100"/>
       <c r="E7" s="131"/>
     </row>
     <row r="8" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="164"/>
+      <c r="B8" s="165"/>
       <c r="C8" s="99"/>
       <c r="D8" s="100"/>
       <c r="E8" s="132"/>
     </row>
     <row r="9" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="164"/>
+      <c r="B9" s="165"/>
       <c r="C9" s="99"/>
       <c r="D9" s="100"/>
       <c r="E9" s="131"/>
     </row>
     <row r="10" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="164"/>
+      <c r="B10" s="165"/>
       <c r="C10" s="99"/>
       <c r="D10" s="100"/>
       <c r="E10" s="131"/>
     </row>
     <row r="11" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B11" s="164"/>
+      <c r="B11" s="165"/>
       <c r="C11" s="99"/>
       <c r="D11" s="100"/>
       <c r="E11" s="131"/>
     </row>
     <row r="12" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="164"/>
+      <c r="B12" s="165"/>
       <c r="C12" s="99"/>
       <c r="D12" s="100"/>
       <c r="E12" s="131"/>
     </row>
     <row r="13" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B13" s="164"/>
+      <c r="B13" s="165"/>
       <c r="C13" s="99"/>
       <c r="D13" s="100"/>
       <c r="E13" s="131"/>
     </row>
     <row r="14" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="164"/>
+      <c r="B14" s="165"/>
       <c r="C14" s="99"/>
       <c r="D14" s="100"/>
       <c r="E14" s="131"/>
     </row>
     <row r="15" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B15" s="164"/>
+      <c r="B15" s="165"/>
       <c r="C15" s="99"/>
       <c r="D15" s="100"/>
       <c r="E15" s="131"/>
     </row>
     <row r="16" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="164"/>
+      <c r="B16" s="165"/>
       <c r="C16" s="99"/>
       <c r="D16" s="100"/>
       <c r="E16" s="131"/>
     </row>
     <row r="17" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B17" s="164"/>
+      <c r="B17" s="165"/>
       <c r="C17" s="99"/>
       <c r="D17" s="100"/>
       <c r="E17" s="131"/>
     </row>
     <row r="18" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B18" s="164"/>
+      <c r="B18" s="165"/>
       <c r="C18" s="99"/>
       <c r="D18" s="100"/>
       <c r="E18" s="131"/>
     </row>
     <row r="19" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B19" s="164"/>
+      <c r="B19" s="165"/>
       <c r="C19" s="99"/>
       <c r="D19" s="100"/>
       <c r="E19" s="131"/>
     </row>
     <row r="20" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B20" s="164"/>
+      <c r="B20" s="165"/>
       <c r="C20" s="99"/>
       <c r="D20" s="100"/>
       <c r="E20" s="131"/>
     </row>
     <row r="21" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B21" s="164"/>
+      <c r="B21" s="165"/>
       <c r="C21" s="101"/>
       <c r="D21" s="102"/>
       <c r="E21" s="133"/>
@@ -6424,7 +6437,7 @@
       <c r="E22" s="1"/>
     </row>
     <row r="23" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B23" s="165" t="s">
+      <c r="B23" s="166" t="s">
         <v>233</v>
       </c>
       <c r="C23" s="105"/>
@@ -6432,31 +6445,31 @@
       <c r="E23" s="134"/>
     </row>
     <row r="24" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B24" s="166"/>
+      <c r="B24" s="167"/>
       <c r="C24" s="107"/>
       <c r="D24" s="108"/>
       <c r="E24" s="132"/>
     </row>
     <row r="25" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B25" s="166"/>
+      <c r="B25" s="167"/>
       <c r="C25" s="107"/>
       <c r="D25" s="108"/>
       <c r="E25" s="135"/>
     </row>
     <row r="26" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B26" s="166"/>
+      <c r="B26" s="167"/>
       <c r="C26" s="109"/>
       <c r="D26" s="108"/>
       <c r="E26" s="135"/>
     </row>
     <row r="27" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B27" s="166"/>
+      <c r="B27" s="167"/>
       <c r="C27" s="109"/>
       <c r="D27" s="108"/>
       <c r="E27" s="135"/>
     </row>
     <row r="28" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B28" s="166"/>
+      <c r="B28" s="167"/>
       <c r="C28" s="110"/>
       <c r="D28" s="111"/>
       <c r="E28" s="136"/>
@@ -6468,7 +6481,7 @@
       <c r="E29" s="1"/>
     </row>
     <row r="30" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B30" s="167" t="s">
+      <c r="B30" s="168" t="s">
         <v>234</v>
       </c>
       <c r="C30" s="112"/>
@@ -6476,43 +6489,43 @@
       <c r="E30" s="137"/>
     </row>
     <row r="31" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B31" s="168"/>
+      <c r="B31" s="169"/>
       <c r="C31" s="114"/>
       <c r="D31" s="115"/>
       <c r="E31" s="138"/>
     </row>
     <row r="32" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B32" s="168"/>
+      <c r="B32" s="169"/>
       <c r="C32" s="114"/>
       <c r="D32" s="115"/>
       <c r="E32" s="138"/>
     </row>
     <row r="33" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B33" s="168"/>
+      <c r="B33" s="169"/>
       <c r="C33" s="114"/>
       <c r="D33" s="115"/>
       <c r="E33" s="132"/>
     </row>
     <row r="34" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B34" s="168"/>
+      <c r="B34" s="169"/>
       <c r="C34" s="114"/>
       <c r="D34" s="115"/>
       <c r="E34" s="135"/>
     </row>
     <row r="35" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B35" s="168"/>
+      <c r="B35" s="169"/>
       <c r="C35" s="114"/>
       <c r="D35" s="115"/>
       <c r="E35" s="135"/>
     </row>
     <row r="36" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B36" s="168"/>
+      <c r="B36" s="169"/>
       <c r="C36" s="114"/>
       <c r="D36" s="115"/>
       <c r="E36" s="131"/>
     </row>
     <row r="37" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B37" s="168"/>
+      <c r="B37" s="169"/>
       <c r="C37" s="116"/>
       <c r="D37" s="117"/>
       <c r="E37" s="133"/>
@@ -6524,7 +6537,7 @@
       <c r="E38" s="1"/>
     </row>
     <row r="39" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B39" s="169" t="s">
+      <c r="B39" s="170" t="s">
         <v>235</v>
       </c>
       <c r="C39" s="118"/>
@@ -6532,31 +6545,31 @@
       <c r="E39" s="139"/>
     </row>
     <row r="40" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="170"/>
+      <c r="B40" s="171"/>
       <c r="C40" s="120"/>
       <c r="D40" s="121"/>
       <c r="E40" s="132"/>
     </row>
     <row r="41" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B41" s="170"/>
+      <c r="B41" s="171"/>
       <c r="C41" s="120"/>
       <c r="D41" s="121"/>
       <c r="E41" s="132"/>
     </row>
     <row r="42" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B42" s="170"/>
+      <c r="B42" s="171"/>
       <c r="C42" s="120"/>
       <c r="D42" s="121"/>
       <c r="E42" s="132"/>
     </row>
     <row r="43" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B43" s="170"/>
+      <c r="B43" s="171"/>
       <c r="C43" s="120"/>
       <c r="D43" s="121"/>
       <c r="E43" s="132"/>
     </row>
     <row r="44" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B44" s="170"/>
+      <c r="B44" s="171"/>
       <c r="C44" s="122"/>
       <c r="D44" s="123"/>
       <c r="E44" s="140"/>
@@ -6568,100 +6581,100 @@
       <c r="E45" s="1"/>
     </row>
     <row r="46" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B46" s="155" t="s">
+      <c r="B46" s="156" t="s">
         <v>236</v>
       </c>
-      <c r="C46" s="158" t="s">
+      <c r="C46" s="159" t="s">
         <v>102</v>
       </c>
       <c r="D46" s="124"/>
       <c r="E46" s="130"/>
     </row>
     <row r="47" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="156"/>
-      <c r="C47" s="159"/>
+      <c r="B47" s="157"/>
+      <c r="C47" s="160"/>
       <c r="D47" s="125"/>
       <c r="E47" s="131"/>
     </row>
     <row r="48" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B48" s="156"/>
-      <c r="C48" s="159"/>
+      <c r="B48" s="157"/>
+      <c r="C48" s="160"/>
       <c r="D48" s="125"/>
       <c r="E48" s="131"/>
     </row>
     <row r="49" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B49" s="156"/>
-      <c r="C49" s="159"/>
+      <c r="B49" s="157"/>
+      <c r="C49" s="160"/>
       <c r="D49" s="125"/>
       <c r="E49" s="131"/>
     </row>
     <row r="50" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B50" s="156"/>
-      <c r="C50" s="159"/>
+      <c r="B50" s="157"/>
+      <c r="C50" s="160"/>
       <c r="D50" s="125"/>
       <c r="E50" s="131"/>
     </row>
     <row r="51" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B51" s="156"/>
-      <c r="C51" s="160" t="s">
+      <c r="B51" s="157"/>
+      <c r="C51" s="161" t="s">
         <v>257</v>
       </c>
       <c r="D51" s="126"/>
       <c r="E51" s="141"/>
     </row>
     <row r="52" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B52" s="156"/>
-      <c r="C52" s="159"/>
+      <c r="B52" s="157"/>
+      <c r="C52" s="160"/>
       <c r="D52" s="125"/>
       <c r="E52" s="131"/>
     </row>
     <row r="53" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B53" s="156"/>
-      <c r="C53" s="159"/>
+      <c r="B53" s="157"/>
+      <c r="C53" s="160"/>
       <c r="D53" s="125"/>
       <c r="E53" s="131"/>
     </row>
     <row r="54" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B54" s="156"/>
-      <c r="C54" s="159"/>
+      <c r="B54" s="157"/>
+      <c r="C54" s="160"/>
       <c r="D54" s="125"/>
       <c r="E54" s="131"/>
     </row>
     <row r="55" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B55" s="156"/>
-      <c r="C55" s="161"/>
+      <c r="B55" s="157"/>
+      <c r="C55" s="162"/>
       <c r="D55" s="127"/>
       <c r="E55" s="142"/>
     </row>
     <row r="56" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B56" s="156"/>
-      <c r="C56" s="159" t="s">
+      <c r="B56" s="157"/>
+      <c r="C56" s="160" t="s">
         <v>237</v>
       </c>
       <c r="D56" s="125"/>
       <c r="E56" s="131"/>
     </row>
     <row r="57" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B57" s="156"/>
-      <c r="C57" s="159"/>
+      <c r="B57" s="157"/>
+      <c r="C57" s="160"/>
       <c r="D57" s="125"/>
       <c r="E57" s="131"/>
     </row>
     <row r="58" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B58" s="156"/>
-      <c r="C58" s="159"/>
+      <c r="B58" s="157"/>
+      <c r="C58" s="160"/>
       <c r="D58" s="125"/>
       <c r="E58" s="131"/>
     </row>
     <row r="59" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B59" s="156"/>
-      <c r="C59" s="159"/>
+      <c r="B59" s="157"/>
+      <c r="C59" s="160"/>
       <c r="D59" s="125"/>
       <c r="E59" s="131"/>
     </row>
     <row r="60" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B60" s="157"/>
-      <c r="C60" s="162"/>
+      <c r="B60" s="158"/>
+      <c r="C60" s="163"/>
       <c r="D60" s="128"/>
       <c r="E60" s="133"/>
     </row>
@@ -6732,12 +6745,12 @@
       <c r="P2" s="78"/>
     </row>
     <row r="3" spans="2:18" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="151" t="s">
+      <c r="B3" s="152" t="s">
         <v>57</v>
       </c>
-      <c r="C3" s="151"/>
-      <c r="D3" s="151"/>
-      <c r="E3" s="151"/>
+      <c r="C3" s="152"/>
+      <c r="D3" s="152"/>
+      <c r="E3" s="152"/>
       <c r="F3" s="77"/>
       <c r="G3" s="77"/>
       <c r="H3" s="77"/>
@@ -6989,12 +7002,12 @@
       <c r="N2" s="78"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="151" t="s">
+      <c r="B3" s="152" t="s">
         <v>138</v>
       </c>
-      <c r="C3" s="151"/>
-      <c r="D3" s="151"/>
-      <c r="E3" s="151"/>
+      <c r="C3" s="152"/>
+      <c r="D3" s="152"/>
+      <c r="E3" s="152"/>
       <c r="F3" s="77"/>
       <c r="G3" s="77"/>
       <c r="H3" s="77"/>
@@ -7089,28 +7102,28 @@
       </c>
     </row>
     <row r="2" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="152"/>
-      <c r="C2" s="152"/>
-      <c r="D2" s="152"/>
-      <c r="E2" s="152"/>
-      <c r="F2" s="152"/>
-      <c r="G2" s="152"/>
-      <c r="H2" s="152"/>
-      <c r="I2" s="152"/>
-      <c r="J2" s="152"/>
+      <c r="B2" s="153"/>
+      <c r="C2" s="153"/>
+      <c r="D2" s="153"/>
+      <c r="E2" s="153"/>
+      <c r="F2" s="153"/>
+      <c r="G2" s="153"/>
+      <c r="H2" s="153"/>
+      <c r="I2" s="153"/>
+      <c r="J2" s="153"/>
     </row>
     <row r="3" spans="2:10" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="151" t="s">
+      <c r="B3" s="152" t="s">
         <v>141</v>
       </c>
-      <c r="C3" s="151"/>
-      <c r="D3" s="151"/>
-      <c r="E3" s="151"/>
-      <c r="F3" s="151"/>
-      <c r="G3" s="151"/>
-      <c r="H3" s="151"/>
-      <c r="I3" s="151"/>
-      <c r="J3" s="151"/>
+      <c r="C3" s="152"/>
+      <c r="D3" s="152"/>
+      <c r="E3" s="152"/>
+      <c r="F3" s="152"/>
+      <c r="G3" s="152"/>
+      <c r="H3" s="152"/>
+      <c r="I3" s="152"/>
+      <c r="J3" s="152"/>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" s="71" t="s">
@@ -7204,13 +7217,13 @@
       <c r="N2" s="78"/>
     </row>
     <row r="3" spans="2:20" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="151" t="s">
+      <c r="B3" s="152" t="s">
         <v>142</v>
       </c>
-      <c r="C3" s="151"/>
-      <c r="D3" s="151"/>
-      <c r="E3" s="151"/>
-      <c r="F3" s="151"/>
+      <c r="C3" s="152"/>
+      <c r="D3" s="152"/>
+      <c r="E3" s="152"/>
+      <c r="F3" s="152"/>
       <c r="G3" s="77"/>
       <c r="H3" s="77"/>
       <c r="I3" s="77"/>
@@ -7336,10 +7349,10 @@
       <c r="F2" s="77"/>
     </row>
     <row r="3" spans="2:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="151" t="s">
+      <c r="B3" s="152" t="s">
         <v>190</v>
       </c>
-      <c r="C3" s="151"/>
+      <c r="C3" s="152"/>
       <c r="D3" s="77"/>
       <c r="E3" s="77"/>
       <c r="F3" s="77"/>
@@ -7402,10 +7415,10 @@
       <c r="D2" s="77"/>
     </row>
     <row r="3" spans="2:4" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="151" t="s">
+      <c r="B3" s="152" t="s">
         <v>196</v>
       </c>
-      <c r="C3" s="151"/>
+      <c r="C3" s="152"/>
       <c r="D3" s="77"/>
     </row>
     <row r="5" spans="2:4" ht="27" x14ac:dyDescent="0.25">
@@ -7464,12 +7477,12 @@
       <c r="I2" s="78"/>
     </row>
     <row r="3" spans="2:9" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="151" t="s">
+      <c r="B3" s="152" t="s">
         <v>178</v>
       </c>
-      <c r="C3" s="151"/>
-      <c r="D3" s="151"/>
-      <c r="E3" s="151"/>
+      <c r="C3" s="152"/>
+      <c r="D3" s="152"/>
+      <c r="E3" s="152"/>
       <c r="F3" s="77"/>
       <c r="G3" s="77"/>
       <c r="H3" s="77"/>
@@ -7557,10 +7570,10 @@
       <c r="K2" s="78"/>
     </row>
     <row r="3" spans="2:11" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="151" t="s">
+      <c r="B3" s="152" t="s">
         <v>154</v>
       </c>
-      <c r="C3" s="151"/>
+      <c r="C3" s="152"/>
       <c r="D3" s="77"/>
       <c r="E3" s="77"/>
       <c r="F3" s="77"/>
@@ -7583,14 +7596,14 @@
       <c r="K4" s="79"/>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="H5" s="171" t="s">
+      <c r="H5" s="172" t="s">
         <v>162</v>
       </c>
-      <c r="I5" s="172"/>
-      <c r="J5" s="171" t="s">
+      <c r="I5" s="173"/>
+      <c r="J5" s="172" t="s">
         <v>161</v>
       </c>
-      <c r="K5" s="172"/>
+      <c r="K5" s="173"/>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" s="80" t="s">
@@ -7676,10 +7689,10 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="152" t="s">
+      <c r="B2" s="153" t="s">
         <v>82</v>
       </c>
-      <c r="C2" s="152"/>
+      <c r="C2" s="153"/>
       <c r="D2" s="78"/>
       <c r="E2" s="78"/>
       <c r="F2" s="78"/>
@@ -7777,11 +7790,11 @@
       <c r="H2" s="77"/>
     </row>
     <row r="3" spans="2:8" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="151" t="s">
+      <c r="B3" s="152" t="s">
         <v>201</v>
       </c>
-      <c r="C3" s="151"/>
-      <c r="D3" s="151"/>
+      <c r="C3" s="152"/>
+      <c r="D3" s="152"/>
       <c r="E3" s="77"/>
       <c r="F3" s="77"/>
       <c r="G3" s="77"/>
@@ -7836,13 +7849,13 @@
       <c r="C2" s="77"/>
     </row>
     <row r="3" spans="2:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="151" t="s">
+      <c r="B3" s="152" t="s">
         <v>202</v>
       </c>
-      <c r="C3" s="151"/>
-      <c r="D3" s="151"/>
-      <c r="E3" s="151"/>
-      <c r="F3" s="151"/>
+      <c r="C3" s="152"/>
+      <c r="D3" s="152"/>
+      <c r="E3" s="152"/>
+      <c r="F3" s="152"/>
     </row>
     <row r="5" spans="2:6" ht="27" x14ac:dyDescent="0.25">
       <c r="B5" s="91" t="s">
@@ -7895,11 +7908,11 @@
       <c r="H2" s="77"/>
     </row>
     <row r="3" spans="2:8" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="151" t="s">
+      <c r="B3" s="152" t="s">
         <v>204</v>
       </c>
-      <c r="C3" s="151"/>
-      <c r="D3" s="151"/>
+      <c r="C3" s="152"/>
+      <c r="D3" s="152"/>
       <c r="E3" s="77"/>
       <c r="F3" s="77"/>
       <c r="G3" s="77"/>
@@ -8021,11 +8034,11 @@
       <c r="H2" s="77"/>
     </row>
     <row r="3" spans="2:8" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="151" t="s">
+      <c r="B3" s="152" t="s">
         <v>207</v>
       </c>
-      <c r="C3" s="151"/>
-      <c r="D3" s="151"/>
+      <c r="C3" s="152"/>
+      <c r="D3" s="152"/>
       <c r="E3" s="77"/>
       <c r="F3" s="77"/>
       <c r="G3" s="77"/>
@@ -8081,12 +8094,12 @@
       <c r="H2" s="77"/>
     </row>
     <row r="3" spans="2:8" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="151" t="s">
+      <c r="B3" s="152" t="s">
         <v>265</v>
       </c>
-      <c r="C3" s="151"/>
-      <c r="D3" s="151"/>
-      <c r="E3" s="151"/>
+      <c r="C3" s="152"/>
+      <c r="D3" s="152"/>
+      <c r="E3" s="152"/>
       <c r="F3" s="77"/>
       <c r="G3" s="77"/>
       <c r="H3" s="77"/>
@@ -8225,10 +8238,10 @@
       <c r="Z2"/>
     </row>
     <row r="3" spans="2:26" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="151" t="s">
+      <c r="B3" s="152" t="s">
         <v>252</v>
       </c>
-      <c r="C3" s="151"/>
+      <c r="C3" s="152"/>
       <c r="D3" s="77"/>
       <c r="E3" s="77"/>
       <c r="F3" s="77"/>
@@ -8358,10 +8371,10 @@
       <c r="Z2"/>
     </row>
     <row r="3" spans="2:26" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="151" t="s">
+      <c r="B3" s="152" t="s">
         <v>259</v>
       </c>
-      <c r="C3" s="151"/>
+      <c r="C3" s="152"/>
       <c r="D3" s="77"/>
       <c r="E3" s="77"/>
       <c r="F3" s="77"/>
@@ -8391,9 +8404,9 @@
       <c r="C6" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="D6" s="173"/>
-      <c r="E6" s="174"/>
-      <c r="F6" s="175"/>
+      <c r="D6" s="174"/>
+      <c r="E6" s="175"/>
+      <c r="F6" s="176"/>
       <c r="G6" s="48"/>
       <c r="H6" s="48"/>
     </row>
@@ -8486,10 +8499,10 @@
       <c r="Z2"/>
     </row>
     <row r="3" spans="2:26" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="151" t="s">
+      <c r="B3" s="152" t="s">
         <v>79</v>
       </c>
-      <c r="C3" s="151"/>
+      <c r="C3" s="152"/>
       <c r="D3" s="77"/>
       <c r="E3" s="77"/>
       <c r="F3" s="77"/>
@@ -8608,10 +8621,10 @@
       <c r="M2" s="78"/>
     </row>
     <row r="3" spans="2:13" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="151" t="s">
+      <c r="B3" s="152" t="s">
         <v>224</v>
       </c>
-      <c r="C3" s="151"/>
+      <c r="C3" s="152"/>
       <c r="D3" s="77"/>
       <c r="E3" s="77"/>
       <c r="F3" s="77"/>
@@ -8681,10 +8694,10 @@
       <c r="Z2"/>
     </row>
     <row r="3" spans="2:26" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="151" t="s">
+      <c r="B3" s="152" t="s">
         <v>64</v>
       </c>
-      <c r="C3" s="151"/>
+      <c r="C3" s="152"/>
       <c r="D3" s="77"/>
       <c r="E3" s="77"/>
       <c r="F3" s="77"/>
@@ -8814,12 +8827,12 @@
       <c r="L2" s="78"/>
     </row>
     <row r="3" spans="2:17" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="151" t="s">
+      <c r="B3" s="152" t="s">
         <v>94</v>
       </c>
-      <c r="C3" s="151"/>
-      <c r="D3" s="151"/>
-      <c r="E3" s="151"/>
+      <c r="C3" s="152"/>
+      <c r="D3" s="152"/>
+      <c r="E3" s="152"/>
       <c r="F3" s="77"/>
       <c r="G3" s="77"/>
       <c r="H3" s="77"/>
@@ -8829,28 +8842,28 @@
       <c r="L3" s="77"/>
     </row>
     <row r="5" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D5" s="176" t="s">
+      <c r="D5" s="177" t="s">
         <v>109</v>
       </c>
-      <c r="E5" s="176"/>
+      <c r="E5" s="177"/>
       <c r="F5" s="70"/>
       <c r="G5" s="70"/>
       <c r="H5" s="70"/>
       <c r="I5" s="70"/>
-      <c r="J5" s="176" t="s">
+      <c r="J5" s="177" t="s">
         <v>37</v>
       </c>
-      <c r="K5" s="176"/>
-      <c r="L5" s="176"/>
-      <c r="M5" s="176" t="s">
+      <c r="K5" s="177"/>
+      <c r="L5" s="177"/>
+      <c r="M5" s="177" t="s">
         <v>116</v>
       </c>
-      <c r="N5" s="176"/>
-      <c r="O5" s="176"/>
-      <c r="P5" s="153" t="s">
+      <c r="N5" s="177"/>
+      <c r="O5" s="177"/>
+      <c r="P5" s="154" t="s">
         <v>95</v>
       </c>
-      <c r="Q5" s="153"/>
+      <c r="Q5" s="154"/>
     </row>
     <row r="6" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="67" t="s">
@@ -8989,11 +9002,11 @@
       <c r="R2" s="53"/>
     </row>
     <row r="3" spans="2:25" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="151" t="s">
+      <c r="B3" s="152" t="s">
         <v>97</v>
       </c>
-      <c r="C3" s="151"/>
-      <c r="D3" s="151"/>
+      <c r="C3" s="152"/>
+      <c r="D3" s="152"/>
       <c r="E3" s="77"/>
       <c r="F3" s="77"/>
       <c r="G3" s="77"/>
@@ -9010,70 +9023,70 @@
       <c r="R3" s="54"/>
     </row>
     <row r="5" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B5" s="179" t="s">
+      <c r="B5" s="180" t="s">
         <v>98</v>
       </c>
-      <c r="C5" s="180"/>
-      <c r="D5" s="180"/>
-      <c r="E5" s="180"/>
-      <c r="F5" s="180"/>
-      <c r="G5" s="180"/>
-      <c r="H5" s="180"/>
-      <c r="I5" s="180"/>
-      <c r="J5" s="180"/>
-      <c r="K5" s="180"/>
-      <c r="L5" s="181"/>
-      <c r="M5" s="179" t="s">
+      <c r="C5" s="181"/>
+      <c r="D5" s="181"/>
+      <c r="E5" s="181"/>
+      <c r="F5" s="181"/>
+      <c r="G5" s="181"/>
+      <c r="H5" s="181"/>
+      <c r="I5" s="181"/>
+      <c r="J5" s="181"/>
+      <c r="K5" s="181"/>
+      <c r="L5" s="182"/>
+      <c r="M5" s="180" t="s">
         <v>99</v>
       </c>
-      <c r="N5" s="180"/>
-      <c r="O5" s="180"/>
-      <c r="P5" s="180"/>
-      <c r="Q5" s="180"/>
-      <c r="R5" s="180"/>
-      <c r="S5" s="180"/>
-      <c r="T5" s="180"/>
-      <c r="U5" s="180"/>
-      <c r="V5" s="180"/>
-      <c r="W5" s="180"/>
-      <c r="X5" s="180"/>
-      <c r="Y5" s="181"/>
+      <c r="N5" s="181"/>
+      <c r="O5" s="181"/>
+      <c r="P5" s="181"/>
+      <c r="Q5" s="181"/>
+      <c r="R5" s="181"/>
+      <c r="S5" s="181"/>
+      <c r="T5" s="181"/>
+      <c r="U5" s="181"/>
+      <c r="V5" s="181"/>
+      <c r="W5" s="181"/>
+      <c r="X5" s="181"/>
+      <c r="Y5" s="182"/>
     </row>
     <row r="6" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B6" s="189"/>
-      <c r="C6" s="189"/>
-      <c r="D6" s="189"/>
-      <c r="E6" s="189"/>
-      <c r="F6" s="185" t="s">
+      <c r="B6" s="190"/>
+      <c r="C6" s="190"/>
+      <c r="D6" s="190"/>
+      <c r="E6" s="190"/>
+      <c r="F6" s="186" t="s">
         <v>25</v>
       </c>
-      <c r="G6" s="186"/>
-      <c r="H6" s="186"/>
-      <c r="I6" s="187"/>
-      <c r="J6" s="179" t="s">
+      <c r="G6" s="187"/>
+      <c r="H6" s="187"/>
+      <c r="I6" s="188"/>
+      <c r="J6" s="180" t="s">
         <v>28</v>
       </c>
-      <c r="K6" s="180"/>
-      <c r="L6" s="181"/>
+      <c r="K6" s="181"/>
+      <c r="L6" s="182"/>
       <c r="M6" s="81"/>
-      <c r="N6" s="177" t="s">
+      <c r="N6" s="178" t="s">
         <v>37</v>
       </c>
-      <c r="O6" s="178"/>
-      <c r="P6" s="177" t="s">
+      <c r="O6" s="179"/>
+      <c r="P6" s="178" t="s">
         <v>92</v>
       </c>
-      <c r="Q6" s="188"/>
-      <c r="R6" s="178"/>
+      <c r="Q6" s="189"/>
+      <c r="R6" s="179"/>
       <c r="S6" s="81"/>
-      <c r="T6" s="177" t="s">
+      <c r="T6" s="178" t="s">
         <v>109</v>
       </c>
-      <c r="U6" s="178"/>
-      <c r="V6" s="182"/>
-      <c r="W6" s="183"/>
-      <c r="X6" s="183"/>
-      <c r="Y6" s="184"/>
+      <c r="U6" s="179"/>
+      <c r="V6" s="183"/>
+      <c r="W6" s="184"/>
+      <c r="X6" s="184"/>
+      <c r="Y6" s="185"/>
     </row>
     <row r="7" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B7" s="72" t="s">
@@ -9301,14 +9314,14 @@
       </c>
     </row>
     <row r="2" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="152" t="s">
+      <c r="B2" s="153" t="s">
         <v>83</v>
       </c>
-      <c r="C2" s="152"/>
-      <c r="D2" s="152"/>
-      <c r="E2" s="152"/>
-      <c r="F2" s="152"/>
-      <c r="G2" s="152"/>
+      <c r="C2" s="153"/>
+      <c r="D2" s="153"/>
+      <c r="E2" s="153"/>
+      <c r="F2" s="153"/>
+      <c r="G2" s="153"/>
     </row>
     <row r="3" spans="2:7" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="77" t="s">
@@ -9364,20 +9377,20 @@
       </c>
     </row>
     <row r="2" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="152" t="s">
+      <c r="B2" s="153" t="s">
         <v>261</v>
       </c>
-      <c r="C2" s="152"/>
-      <c r="D2" s="152"/>
-      <c r="E2" s="152"/>
-      <c r="F2" s="152"/>
-      <c r="G2" s="152"/>
+      <c r="C2" s="153"/>
+      <c r="D2" s="153"/>
+      <c r="E2" s="153"/>
+      <c r="F2" s="153"/>
+      <c r="G2" s="153"/>
     </row>
     <row r="3" spans="2:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="151" t="s">
+      <c r="B3" s="152" t="s">
         <v>226</v>
       </c>
-      <c r="C3" s="151"/>
+      <c r="C3" s="152"/>
     </row>
     <row r="4" spans="2:7" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="93"/>
@@ -9444,10 +9457,10 @@
     </row>
     <row r="3" spans="1:10" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="145"/>
-      <c r="B3" s="151" t="s">
+      <c r="B3" s="152" t="s">
         <v>253</v>
       </c>
-      <c r="C3" s="151"/>
+      <c r="C3" s="152"/>
       <c r="D3" s="77"/>
       <c r="E3" s="77"/>
       <c r="F3" s="77"/>
@@ -9536,11 +9549,11 @@
       <c r="E2" s="78"/>
     </row>
     <row r="3" spans="2:5" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="151" t="s">
+      <c r="B3" s="152" t="s">
         <v>117</v>
       </c>
-      <c r="C3" s="151"/>
-      <c r="D3" s="151"/>
+      <c r="C3" s="152"/>
+      <c r="D3" s="152"/>
       <c r="E3" s="77"/>
     </row>
     <row r="4" spans="2:5" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
TRIEDA-1866: Correção na importação de Ambientes TRIEDA-1867: Correção na exportação de Disciplinas TRIEDA-1868: Criação da tabela de importação e exportação da tela de Ofertas de Cursos em Campi
</commit_message>
<xml_diff>
--- a/code/client/web/src/main/resources/templateExport.xlsx
+++ b/code/client/web/src/main/resources/templateExport.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="17070" windowHeight="5370" tabRatio="919" firstSheet="18" activeTab="23"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="17070" windowHeight="5370" tabRatio="919" firstSheet="18" activeTab="21"/>
   </bookViews>
   <sheets>
     <sheet name="Turnos" sheetId="49" r:id="rId1"/>
@@ -28,38 +28,39 @@
     <sheet name="Disciplinas Pre-Requisitos" sheetId="37" r:id="rId19"/>
     <sheet name="Disciplinas Co-Requisitos" sheetId="38" r:id="rId20"/>
     <sheet name="Disciplinas Cursadas por Aluno" sheetId="39" r:id="rId21"/>
-    <sheet name="Ofertas e Demandas" sheetId="8" r:id="rId22"/>
-    <sheet name="Alunos" sheetId="27" r:id="rId23"/>
-    <sheet name="Demanda por Aluno" sheetId="22" r:id="rId24"/>
-    <sheet name="Professores" sheetId="12" r:id="rId25"/>
-    <sheet name="Disponibilidades Professores" sheetId="28" r:id="rId26"/>
-    <sheet name="Campi de Trabalho" sheetId="18" r:id="rId27"/>
-    <sheet name="Habilitacao dos Professores" sheetId="13" r:id="rId28"/>
-    <sheet name="Resumo por Cenario" sheetId="54" r:id="rId29"/>
-    <sheet name="Resumo por Campus" sheetId="55" r:id="rId30"/>
-    <sheet name="Resumo por curso" sheetId="14" r:id="rId31"/>
-    <sheet name="Resumo por disciplina" sheetId="15" r:id="rId32"/>
-    <sheet name="Atendimentos por Matricula" sheetId="30" r:id="rId33"/>
-    <sheet name="Atendimentos por Disciplina" sheetId="31" r:id="rId34"/>
-    <sheet name="Atendimentos Faixa de Demanda" sheetId="32" r:id="rId35"/>
-    <sheet name="Atendimentos Faixa de Credito" sheetId="40" r:id="rId36"/>
-    <sheet name="Atendimentos Faixa Disciplina" sheetId="41" r:id="rId37"/>
-    <sheet name="Atendimentos por Carga Horaria" sheetId="35" r:id="rId38"/>
-    <sheet name="Porcentagem Mestres e Doutores" sheetId="33" r:id="rId39"/>
-    <sheet name="Professores Quantidade Janelas" sheetId="42" r:id="rId40"/>
-    <sheet name="Professores Disc Habilitadas" sheetId="43" r:id="rId41"/>
-    <sheet name="Professores Disc Lecionadas" sheetId="44" r:id="rId42"/>
-    <sheet name="Professores Titulacoes" sheetId="45" r:id="rId43"/>
-    <sheet name="Professores Areas Conhecimento" sheetId="46" r:id="rId44"/>
-    <sheet name="Ambientes Faixa Utilizacao" sheetId="47" r:id="rId45"/>
-    <sheet name="Ambientes Faixa Ocupacao" sheetId="48" r:id="rId46"/>
-    <sheet name="Relatorio Visao Ambiente" sheetId="10" r:id="rId47"/>
-    <sheet name="Relatorio Visao Aluno" sheetId="25" r:id="rId48"/>
-    <sheet name="Relatorio Visao Professor" sheetId="21" r:id="rId49"/>
-    <sheet name="Relatorio Visao Curso" sheetId="20" r:id="rId50"/>
-    <sheet name="Atendimentos por Aluno" sheetId="23" r:id="rId51"/>
-    <sheet name="Aulas" sheetId="26" r:id="rId52"/>
-    <sheet name="PaletaCores" sheetId="11" r:id="rId53"/>
+    <sheet name="Ofertas de Cursos em Campi" sheetId="58" r:id="rId22"/>
+    <sheet name="Ofertas e Demandas" sheetId="8" r:id="rId23"/>
+    <sheet name="Alunos" sheetId="27" r:id="rId24"/>
+    <sheet name="Demanda por Aluno" sheetId="22" r:id="rId25"/>
+    <sheet name="Professores" sheetId="12" r:id="rId26"/>
+    <sheet name="Disponibilidades Professores" sheetId="28" r:id="rId27"/>
+    <sheet name="Campi de Trabalho" sheetId="18" r:id="rId28"/>
+    <sheet name="Habilitacao dos Professores" sheetId="13" r:id="rId29"/>
+    <sheet name="Resumo por Cenario" sheetId="54" r:id="rId30"/>
+    <sheet name="Resumo por Campus" sheetId="55" r:id="rId31"/>
+    <sheet name="Resumo por curso" sheetId="14" r:id="rId32"/>
+    <sheet name="Resumo por disciplina" sheetId="15" r:id="rId33"/>
+    <sheet name="Atendimentos por Matricula" sheetId="30" r:id="rId34"/>
+    <sheet name="Atendimentos por Disciplina" sheetId="31" r:id="rId35"/>
+    <sheet name="Atendimentos Faixa de Demanda" sheetId="32" r:id="rId36"/>
+    <sheet name="Atendimentos Faixa de Credito" sheetId="40" r:id="rId37"/>
+    <sheet name="Atendimentos Faixa Disciplina" sheetId="41" r:id="rId38"/>
+    <sheet name="Atendimentos por Carga Horaria" sheetId="35" r:id="rId39"/>
+    <sheet name="Porcentagem Mestres e Doutores" sheetId="33" r:id="rId40"/>
+    <sheet name="Professores Quantidade Janelas" sheetId="42" r:id="rId41"/>
+    <sheet name="Professores Disc Habilitadas" sheetId="43" r:id="rId42"/>
+    <sheet name="Professores Disc Lecionadas" sheetId="44" r:id="rId43"/>
+    <sheet name="Professores Titulacoes" sheetId="45" r:id="rId44"/>
+    <sheet name="Professores Areas Conhecimento" sheetId="46" r:id="rId45"/>
+    <sheet name="Ambientes Faixa Utilizacao" sheetId="47" r:id="rId46"/>
+    <sheet name="Ambientes Faixa Ocupacao" sheetId="48" r:id="rId47"/>
+    <sheet name="Relatorio Visao Ambiente" sheetId="10" r:id="rId48"/>
+    <sheet name="Relatorio Visao Aluno" sheetId="25" r:id="rId49"/>
+    <sheet name="Relatorio Visao Professor" sheetId="21" r:id="rId50"/>
+    <sheet name="Relatorio Visao Curso" sheetId="20" r:id="rId51"/>
+    <sheet name="Atendimentos por Aluno" sheetId="23" r:id="rId52"/>
+    <sheet name="Aulas" sheetId="26" r:id="rId53"/>
+    <sheet name="PaletaCores" sheetId="11" r:id="rId54"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
@@ -68,7 +69,7 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Author</author>
+    <author>Autor</author>
   </authors>
   <commentList>
     <comment ref="E5" authorId="0">
@@ -129,7 +130,7 @@
 <file path=xl/comments10.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Author</author>
+    <author>Autor</author>
   </authors>
   <commentList>
     <comment ref="B5" authorId="0">
@@ -502,7 +503,7 @@
 <file path=xl/comments11.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Author</author>
+    <author>Autor</author>
   </authors>
   <commentList>
     <comment ref="B5" authorId="0">
@@ -535,7 +536,7 @@
 <file path=xl/comments12.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Author</author>
+    <author>Autor</author>
   </authors>
   <commentList>
     <comment ref="B5" authorId="0">
@@ -596,10 +597,10 @@
 <file path=xl/comments13.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Author</author>
+    <author>Autor</author>
   </authors>
   <commentList>
-    <comment ref="K5" authorId="0">
+    <comment ref="F5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -620,90 +621,20 @@
 <file path=xl/comments14.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Author</author>
+    <author>Autor</author>
   </authors>
   <commentList>
-    <comment ref="D5" authorId="0">
+    <comment ref="K5" authorId="0">
       <text>
         <r>
           <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Sim
-Não</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E5" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Alunos virtuais são aqueles ainda inexistentes, porém, que a Instituição de Ensino deseja simular a sua presenção, por exemplo, alunos entrantes. </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Além disso, estes alunos virtuais podem ser criados automaticamente pelo Trieda através do Módulo de Geração de Demanda da aba de Ofertas e Demandas. Mais especificamente, ao informar uma quantidade de alunos através da tela de Ofertas e Demandas o Trieda irá criar, automaticamente, a quantidade informada de alunos. 
-Nestes casos, além do aluno ser considerado virtual o mesmo terá o campo Criado por Trieda? como marcado."</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F5" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Alunos virtuais são aqueles ainda inexistentes, porém, que a Instituição de Ensino deseja simular a sua presenção, por exemplo, alunos entrantes.
-Além disso, estes alunos virtuais podem ser criados automaticamente pelo Trieda através do Módulo de Geração de Demanda da aba de Ofertas e Demandas. Mais especificamente, </t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">ao informar uma quantidade de alunos através da tela de Ofertas e Demandas o Trieda irá criar, automaticamente, a quantidade informada de alunos. </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Receita Semanal por Crédito e Aluno (em Reais)
 </t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Nestes casos, além do aluno ser considerado virtual o mesmo terá o campo Criado por Trieda? como marcado."</t>
         </r>
       </text>
     </comment>
@@ -714,80 +645,21 @@
 <file path=xl/comments15.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Author</author>
+    <author>Autor</author>
   </authors>
   <commentList>
     <comment ref="D5" authorId="0">
       <text>
         <r>
           <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Neste campo é necessário inserir o </t>
-        </r>
-        <r>
-          <rPr>
             <b/>
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Tipo de Contrato do Professor</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">. Os valores permitidos são: 
-- </t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Tempo</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> </t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Integral
-- Tempo Parcial
-- Horista</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-obs: qualquer valor diferente dos valores permitidos impossibiltará a importação dos dados pelo Trieda Web e disponibilizará uma mensagem de erro para o usuário.</t>
+          <t>Sim
+Não</t>
         </r>
       </text>
     </comment>
@@ -801,7 +673,18 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Em créditos semanais</t>
+          <t xml:space="preserve">Alunos virtuais são aqueles ainda inexistentes, porém, que a Instituição de Ensino deseja simular a sua presenção, por exemplo, alunos entrantes. </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Além disso, estes alunos virtuais podem ser criados automaticamente pelo Trieda através do Módulo de Geração de Demanda da aba de Ofertas e Demandas. Mais especificamente, ao informar uma quantidade de alunos através da tela de Ofertas e Demandas o Trieda irá criar, automaticamente, a quantidade informada de alunos. 
+Nestes casos, além do aluno ser considerado virtual o mesmo terá o campo Criado por Trieda? como marcado."</t>
         </r>
       </text>
     </comment>
@@ -809,18 +692,34 @@
       <text>
         <r>
           <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Alunos virtuais são aqueles ainda inexistentes, porém, que a Instituição de Ensino deseja simular a sua presenção, por exemplo, alunos entrantes.
+Além disso, estes alunos virtuais podem ser criados automaticamente pelo Trieda através do Módulo de Geração de Demanda da aba de Ofertas e Demandas. Mais especificamente, </t>
+        </r>
+        <r>
+          <rPr>
             <b/>
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Em créditos semanais</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G5" authorId="0">
-      <text>
+          <t xml:space="preserve">ao informar uma quantidade de alunos através da tela de Ofertas e Demandas o Trieda irá criar, automaticamente, a quantidade informada de alunos. </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
         <r>
           <rPr>
             <b/>
@@ -829,83 +728,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Bacharel
-Especialista
-Mestre
-Doutor</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I5" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">OPCIONAL:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Nota consolidada da avaliação de desempenho do professor.
-Melhor desempenho = 10
-Pior desempenho = 1
-Para desconsiderar este critério, manter todas as notas iguais a 1.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="J5" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Em créditos semanais.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="K5" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Apenas o custo do professor </t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>em sala de aula</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>.</t>
+          <t>Nestes casos, além do aluno ser considerado virtual o mesmo terá o campo Criado por Trieda? como marcado."</t>
         </r>
       </text>
     </comment>
@@ -916,10 +739,10 @@
 <file path=xl/comments16.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Author</author>
+    <author>Autor</author>
   </authors>
   <commentList>
-    <comment ref="C5" authorId="0">
+    <comment ref="D5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -928,14 +751,186 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>A ser preenchido com os seguintes códigos:
-DOM = Domingo
-SEG = Segunda-feira
-TER = Terça-feira
-QUA = Quarta-feira
-QUI = Quinta-feira
-SEX = Sexta-feira
-SAB = Sábado</t>
+          <t xml:space="preserve">Neste campo é necessário inserir o </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Tipo de Contrato do Professor</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">. Os valores permitidos são: 
+- </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Tempo</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Integral
+- Tempo Parcial
+- Horista</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+obs: qualquer valor diferente dos valores permitidos impossibiltará a importação dos dados pelo Trieda Web e disponibilizará uma mensagem de erro para o usuário.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Em créditos semanais</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Em créditos semanais</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Bacharel
+Especialista
+Mestre
+Doutor</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">OPCIONAL:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Nota consolidada da avaliação de desempenho do professor.
+Melhor desempenho = 10
+Pior desempenho = 1
+Para desconsiderar este critério, manter todas as notas iguais a 1.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Em créditos semanais.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Apenas o custo do professor </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>em sala de aula</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>.</t>
         </r>
       </text>
     </comment>
@@ -946,58 +941,26 @@
 <file path=xl/comments17.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Author</author>
+    <author>Autor</author>
   </authors>
   <commentList>
-    <comment ref="D5" authorId="0">
+    <comment ref="C5" authorId="0">
       <text>
         <r>
           <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>OPCIONAL:
-Preferência do professor em ministrar a disciplina.</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Maior Preferência = 10
-Menor preferência = 1
-Para desconsiderar este critério, manter todas as preferências iguais a 1.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E5" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>OPCIONAL:
-Nota da avaliação de desempenho do professor na disciplina, em períodos passados.</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Para desconsiderar este critério, manter todas as notas iguais a 1.</t>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>A ser preenchido com os seguintes códigos:
+DOM = Domingo
+SEG = Segunda-feira
+TER = Terça-feira
+QUA = Quarta-feira
+QUI = Quinta-feira
+SEX = Sexta-feira
+SAB = Sábado</t>
         </r>
       </text>
     </comment>
@@ -1008,11 +971,60 @@
 <file path=xl/comments18.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Author</author>
+    <author>Autor</author>
   </authors>
   <commentList>
-    <comment ref="Z1" authorId="0">
-      <text/>
+    <comment ref="D5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>OPCIONAL:
+Preferência do professor em ministrar a disciplina.</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Maior Preferência = 10
+Menor preferência = 1
+Para desconsiderar este critério, manter todas as preferências iguais a 1.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>OPCIONAL:
+Nota da avaliação de desempenho do professor na disciplina, em períodos passados.</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Para desconsiderar este critério, manter todas as notas iguais a 1.</t>
+        </r>
+      </text>
     </comment>
   </commentList>
 </comments>
@@ -1021,7 +1033,7 @@
 <file path=xl/comments19.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Author</author>
+    <author>Autor</author>
   </authors>
   <commentList>
     <comment ref="Z1" authorId="0">
@@ -1034,7 +1046,7 @@
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Author</author>
+    <author>Autor</author>
   </authors>
   <commentList>
     <comment ref="E5" authorId="0">
@@ -1401,7 +1413,7 @@
 <file path=xl/comments20.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Author</author>
+    <author>Autor</author>
   </authors>
   <commentList>
     <comment ref="Z1" authorId="0">
@@ -1414,7 +1426,20 @@
 <file path=xl/comments21.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Author</author>
+    <author>Autor</author>
+  </authors>
+  <commentList>
+    <comment ref="Z1" authorId="0">
+      <text/>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments22.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Autor</author>
   </authors>
   <commentList>
     <comment ref="Z1" authorId="0">
@@ -1427,7 +1452,7 @@
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Author</author>
+    <author>Autor</author>
   </authors>
   <commentList>
     <comment ref="B5" authorId="0">
@@ -1483,7 +1508,7 @@
 <file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Author</author>
+    <author>Autor</author>
   </authors>
   <commentList>
     <comment ref="B5" authorId="0">
@@ -1539,7 +1564,7 @@
 <file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Author</author>
+    <author>Autor</author>
   </authors>
   <commentList>
     <comment ref="B5" authorId="0">
@@ -1677,7 +1702,7 @@
 <file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Author</author>
+    <author>Autor</author>
   </authors>
   <commentList>
     <comment ref="C5" authorId="0">
@@ -1707,7 +1732,7 @@
 <file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Author</author>
+    <author>Autor</author>
   </authors>
   <commentList>
     <comment ref="B5" authorId="0">
@@ -1905,7 +1930,7 @@
 <file path=xl/comments8.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Author</author>
+    <author>Autor</author>
   </authors>
   <commentList>
     <comment ref="B5" authorId="0">
@@ -1938,7 +1963,7 @@
 <file path=xl/comments9.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Author</author>
+    <author>Autor</author>
   </authors>
   <commentList>
     <comment ref="B5" authorId="0">
@@ -1960,7 +1985,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="270">
   <si>
     <t>Planilha de Unidades</t>
   </si>
@@ -2838,10 +2863,10 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="&quot;R$&quot;\ #,##0.00"/>
-    <numFmt numFmtId="178" formatCode="#,##0.0000"/>
+    <numFmt numFmtId="164" formatCode="&quot;R$&quot;\ #,##0.00"/>
+    <numFmt numFmtId="165" formatCode="#,##0.0000"/>
   </numFmts>
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2863,36 +2888,10 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
       <family val="2"/>
     </font>
     <font>
@@ -3491,8 +3490,8 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="191">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -3500,13 +3499,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -3521,16 +3520,16 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3612,61 +3611,61 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="27" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="9" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="5" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -3679,216 +3678,216 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="9" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="28" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="9" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="9" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="5" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="9" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="29" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="29" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="29" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="29" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="30" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="30" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="30" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="30" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="31" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="31" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="31" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="31" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="31" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="32" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="33" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="33" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="33" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="33" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="33" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="33" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="33" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="33" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="33" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="33" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="33" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -3897,76 +3896,76 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="31" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="31" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="31" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="31" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="31" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="35" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="35" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="36" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="36" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="37" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="37" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="38" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="38" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -3978,22 +3977,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="28" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4005,16 +4004,16 @@
     <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="28" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4022,9 +4021,9 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="2" builtinId="5"/>
+    <cellStyle name="Porcentagem" xfId="2" builtinId="5"/>
+    <cellStyle name="Vírgula" xfId="1" builtinId="3"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -4097,9 +4096,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Escritório">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -4137,7 +4136,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Escritório">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -4209,7 +4208,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Escritório">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -5463,6 +5462,80 @@
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:F6"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:J1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.85546875" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.140625" customWidth="1"/>
+    <col min="6" max="6" width="28" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:6" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B1" s="44" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="2:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="153"/>
+      <c r="C2" s="153"/>
+      <c r="D2" s="153"/>
+      <c r="E2" s="153"/>
+      <c r="F2" s="153"/>
+    </row>
+    <row r="3" spans="2:6" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B3" s="152" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="152"/>
+      <c r="D3" s="152"/>
+      <c r="E3" s="152"/>
+      <c r="F3" s="152"/>
+    </row>
+    <row r="5" spans="2:6" s="144" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="143" t="s">
+        <v>67</v>
+      </c>
+      <c r="C5" s="143" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="45" t="s">
+        <v>69</v>
+      </c>
+      <c r="E5" s="45" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="45" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="83"/>
+      <c r="C6" s="83"/>
+      <c r="D6" s="83"/>
+      <c r="E6" s="83"/>
+      <c r="F6" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B3:F3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O6"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
@@ -5598,7 +5671,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F6"/>
   <sheetViews>
@@ -5665,11 +5738,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O6"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
@@ -5790,7 +5863,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O6"/>
   <sheetViews>
@@ -5916,7 +5989,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
@@ -5984,7 +6057,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D6"/>
   <sheetViews>
@@ -6042,7 +6115,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E6"/>
   <sheetViews>
@@ -6105,52 +6178,6 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:C6"/>
-  <sheetViews>
-    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="2.85546875" customWidth="1"/>
-    <col min="2" max="2" width="72" customWidth="1"/>
-    <col min="3" max="3" width="29.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:3" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="44" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="2" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="78"/>
-      <c r="C2" s="78"/>
-    </row>
-    <row r="3" spans="2:3" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="77" t="s">
-        <v>230</v>
-      </c>
-      <c r="C3" s="77"/>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B5" s="95" t="s">
-        <v>229</v>
-      </c>
-      <c r="C5" s="95"/>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B6" s="96"/>
-      <c r="C6" s="96"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -6256,6 +6283,52 @@
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:C6"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.85546875" customWidth="1"/>
+    <col min="2" max="2" width="72" customWidth="1"/>
+    <col min="3" max="3" width="29.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:3" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B1" s="44" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="78"/>
+      <c r="C2" s="78"/>
+    </row>
+    <row r="3" spans="2:3" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B3" s="77" t="s">
+        <v>230</v>
+      </c>
+      <c r="C3" s="77"/>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="95" t="s">
+        <v>229</v>
+      </c>
+      <c r="C5" s="95"/>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" s="96"/>
+      <c r="C6" s="96"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:P60"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
@@ -6696,7 +6769,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:R6"/>
   <sheetViews>
@@ -6844,7 +6917,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:N6"/>
   <sheetViews>
@@ -6957,7 +7030,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:N6"/>
   <sheetViews>
@@ -7075,7 +7148,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J6"/>
   <sheetViews>
@@ -7171,7 +7244,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:T6"/>
   <sheetViews>
@@ -7320,7 +7393,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F6"/>
   <sheetViews>
@@ -7390,7 +7463,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D6"/>
   <sheetViews>
@@ -7446,7 +7519,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:I6"/>
   <sheetViews>
@@ -7527,133 +7600,6 @@
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B3:E3"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:K7"/>
-  <sheetViews>
-    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="2.85546875" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" customWidth="1"/>
-    <col min="3" max="3" width="53.7109375" customWidth="1"/>
-    <col min="4" max="4" width="12" customWidth="1"/>
-    <col min="5" max="6" width="11.5703125" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" customWidth="1"/>
-    <col min="8" max="11" width="31.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:11" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="44" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="2" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="78"/>
-      <c r="C2" s="78"/>
-      <c r="D2" s="78"/>
-      <c r="E2" s="78"/>
-      <c r="F2" s="78"/>
-      <c r="G2" s="78"/>
-      <c r="H2" s="78"/>
-      <c r="I2" s="78"/>
-      <c r="J2" s="78"/>
-      <c r="K2" s="78"/>
-    </row>
-    <row r="3" spans="2:11" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="152" t="s">
-        <v>154</v>
-      </c>
-      <c r="C3" s="152"/>
-      <c r="D3" s="77"/>
-      <c r="E3" s="77"/>
-      <c r="F3" s="77"/>
-      <c r="G3" s="77"/>
-      <c r="H3" s="77"/>
-      <c r="I3" s="77"/>
-      <c r="J3" s="77"/>
-      <c r="K3" s="77"/>
-    </row>
-    <row r="4" spans="2:11" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B4" s="79"/>
-      <c r="C4" s="79"/>
-      <c r="D4" s="79"/>
-      <c r="E4" s="79"/>
-      <c r="F4" s="79"/>
-      <c r="G4" s="79"/>
-      <c r="H4" s="79"/>
-      <c r="I4" s="79"/>
-      <c r="J4" s="79"/>
-      <c r="K4" s="79"/>
-    </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="H5" s="172" t="s">
-        <v>162</v>
-      </c>
-      <c r="I5" s="173"/>
-      <c r="J5" s="172" t="s">
-        <v>161</v>
-      </c>
-      <c r="K5" s="173"/>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="80" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="80" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="80" t="s">
-        <v>155</v>
-      </c>
-      <c r="E6" s="80" t="s">
-        <v>156</v>
-      </c>
-      <c r="F6" s="80" t="s">
-        <v>258</v>
-      </c>
-      <c r="G6" s="80" t="s">
-        <v>102</v>
-      </c>
-      <c r="H6" s="80" t="s">
-        <v>157</v>
-      </c>
-      <c r="I6" s="80" t="s">
-        <v>158</v>
-      </c>
-      <c r="J6" s="80" t="s">
-        <v>159</v>
-      </c>
-      <c r="K6" s="80" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="76"/>
-      <c r="J7" s="76"/>
-      <c r="K7" s="76"/>
-    </row>
-  </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="B3:C3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -7762,7 +7708,7 @@
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H6"/>
+  <dimension ref="B1:K7"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
@@ -7771,54 +7717,116 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.85546875" customWidth="1"/>
-    <col min="2" max="2" width="38.7109375" customWidth="1"/>
-    <col min="3" max="3" width="26.42578125" customWidth="1"/>
-    <col min="4" max="4" width="28.7109375" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="3" max="3" width="53.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12" customWidth="1"/>
+    <col min="5" max="6" width="11.5703125" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" customWidth="1"/>
+    <col min="8" max="11" width="31.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:11" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="44" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="2:8" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="77"/>
-      <c r="D2" s="77"/>
-      <c r="E2" s="77"/>
-      <c r="F2" s="77"/>
-      <c r="G2" s="77"/>
-      <c r="H2" s="77"/>
-    </row>
-    <row r="3" spans="2:8" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="78"/>
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="78"/>
+      <c r="G2" s="78"/>
+      <c r="H2" s="78"/>
+      <c r="I2" s="78"/>
+      <c r="J2" s="78"/>
+      <c r="K2" s="78"/>
+    </row>
+    <row r="3" spans="2:11" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="152" t="s">
-        <v>201</v>
+        <v>154</v>
       </c>
       <c r="C3" s="152"/>
-      <c r="D3" s="152"/>
+      <c r="D3" s="77"/>
       <c r="E3" s="77"/>
       <c r="F3" s="77"/>
       <c r="G3" s="77"/>
       <c r="H3" s="77"/>
-    </row>
-    <row r="5" spans="2:8" ht="27" x14ac:dyDescent="0.25">
-      <c r="B5" s="91" t="s">
-        <v>200</v>
-      </c>
-      <c r="C5" s="91" t="s">
-        <v>241</v>
-      </c>
-      <c r="D5" s="91" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="8"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
+      <c r="I3" s="77"/>
+      <c r="J3" s="77"/>
+      <c r="K3" s="77"/>
+    </row>
+    <row r="4" spans="2:11" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B4" s="79"/>
+      <c r="C4" s="79"/>
+      <c r="D4" s="79"/>
+      <c r="E4" s="79"/>
+      <c r="F4" s="79"/>
+      <c r="G4" s="79"/>
+      <c r="H4" s="79"/>
+      <c r="I4" s="79"/>
+      <c r="J4" s="79"/>
+      <c r="K4" s="79"/>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="H5" s="172" t="s">
+        <v>162</v>
+      </c>
+      <c r="I5" s="173"/>
+      <c r="J5" s="172" t="s">
+        <v>161</v>
+      </c>
+      <c r="K5" s="173"/>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B6" s="80" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="80" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="80" t="s">
+        <v>155</v>
+      </c>
+      <c r="E6" s="80" t="s">
+        <v>156</v>
+      </c>
+      <c r="F6" s="80" t="s">
+        <v>258</v>
+      </c>
+      <c r="G6" s="80" t="s">
+        <v>102</v>
+      </c>
+      <c r="H6" s="80" t="s">
+        <v>157</v>
+      </c>
+      <c r="I6" s="80" t="s">
+        <v>158</v>
+      </c>
+      <c r="J6" s="80" t="s">
+        <v>159</v>
+      </c>
+      <c r="K6" s="80" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="76"/>
+      <c r="J7" s="76"/>
+      <c r="K7" s="76"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B3:D3"/>
+  <mergeCells count="3">
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="B3:C3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -7826,59 +7834,6 @@
 </file>
 
 <file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:F6"/>
-  <sheetViews>
-    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="2.85546875" customWidth="1"/>
-    <col min="2" max="2" width="38.7109375" customWidth="1"/>
-    <col min="3" max="3" width="26.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:6" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="44" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="2" spans="2:6" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="77"/>
-    </row>
-    <row r="3" spans="2:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="152" t="s">
-        <v>202</v>
-      </c>
-      <c r="C3" s="152"/>
-      <c r="D3" s="152"/>
-      <c r="E3" s="152"/>
-      <c r="F3" s="152"/>
-    </row>
-    <row r="5" spans="2:6" ht="27" x14ac:dyDescent="0.25">
-      <c r="B5" s="91" t="s">
-        <v>203</v>
-      </c>
-      <c r="C5" s="91" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="8"/>
-      <c r="C6" s="9"/>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B3:F3"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H6"/>
   <sheetViews>
@@ -7909,7 +7864,7 @@
     </row>
     <row r="3" spans="2:8" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="152" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C3" s="152"/>
       <c r="D3" s="152"/>
@@ -7920,7 +7875,7 @@
     </row>
     <row r="5" spans="2:8" ht="27" x14ac:dyDescent="0.25">
       <c r="B5" s="91" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="C5" s="91" t="s">
         <v>241</v>
@@ -7937,6 +7892,59 @@
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B3:D3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:F6"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.85546875" customWidth="1"/>
+    <col min="2" max="2" width="38.7109375" customWidth="1"/>
+    <col min="3" max="3" width="26.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:6" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B1" s="44" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="2:6" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="77"/>
+    </row>
+    <row r="3" spans="2:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="152" t="s">
+        <v>202</v>
+      </c>
+      <c r="C3" s="152"/>
+      <c r="D3" s="152"/>
+      <c r="E3" s="152"/>
+      <c r="F3" s="152"/>
+    </row>
+    <row r="5" spans="2:6" ht="27" x14ac:dyDescent="0.25">
+      <c r="B5" s="91" t="s">
+        <v>203</v>
+      </c>
+      <c r="C5" s="91" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="8"/>
+      <c r="C6" s="9"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B3:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -7973,11 +7981,11 @@
       <c r="H2" s="77"/>
     </row>
     <row r="3" spans="2:8" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="77" t="s">
-        <v>206</v>
-      </c>
-      <c r="C3" s="77"/>
-      <c r="D3" s="77"/>
+      <c r="B3" s="152" t="s">
+        <v>204</v>
+      </c>
+      <c r="C3" s="152"/>
+      <c r="D3" s="152"/>
       <c r="E3" s="77"/>
       <c r="F3" s="77"/>
       <c r="G3" s="77"/>
@@ -7985,7 +7993,7 @@
     </row>
     <row r="5" spans="2:8" ht="27" x14ac:dyDescent="0.25">
       <c r="B5" s="91" t="s">
-        <v>43</v>
+        <v>205</v>
       </c>
       <c r="C5" s="91" t="s">
         <v>241</v>
@@ -8000,6 +8008,9 @@
       <c r="D6" s="9"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B3:D3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
@@ -8018,6 +8029,7 @@
     <col min="1" max="1" width="2.85546875" customWidth="1"/>
     <col min="2" max="2" width="38.7109375" customWidth="1"/>
     <col min="3" max="3" width="26.42578125" customWidth="1"/>
+    <col min="4" max="4" width="28.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
@@ -8034,11 +8046,11 @@
       <c r="H2" s="77"/>
     </row>
     <row r="3" spans="2:8" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="152" t="s">
-        <v>207</v>
-      </c>
-      <c r="C3" s="152"/>
-      <c r="D3" s="152"/>
+      <c r="B3" s="77" t="s">
+        <v>206</v>
+      </c>
+      <c r="C3" s="77"/>
+      <c r="D3" s="77"/>
       <c r="E3" s="77"/>
       <c r="F3" s="77"/>
       <c r="G3" s="77"/>
@@ -8046,20 +8058,21 @@
     </row>
     <row r="5" spans="2:8" ht="27" x14ac:dyDescent="0.25">
       <c r="B5" s="91" t="s">
-        <v>208</v>
+        <v>43</v>
       </c>
       <c r="C5" s="91" t="s">
-        <v>199</v>
+        <v>241</v>
+      </c>
+      <c r="D5" s="91" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B3:D3"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
@@ -8077,7 +8090,7 @@
   <cols>
     <col min="1" max="1" width="2.85546875" customWidth="1"/>
     <col min="2" max="2" width="38.7109375" customWidth="1"/>
-    <col min="3" max="5" width="17.140625" customWidth="1"/>
+    <col min="3" max="3" width="26.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
@@ -8095,38 +8108,30 @@
     </row>
     <row r="3" spans="2:8" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="152" t="s">
-        <v>265</v>
+        <v>207</v>
       </c>
       <c r="C3" s="152"/>
       <c r="D3" s="152"/>
-      <c r="E3" s="152"/>
+      <c r="E3" s="77"/>
       <c r="F3" s="77"/>
       <c r="G3" s="77"/>
       <c r="H3" s="77"/>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:8" ht="27" x14ac:dyDescent="0.25">
       <c r="B5" s="91" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C5" s="91" t="s">
-        <v>209</v>
-      </c>
-      <c r="D5" s="91" t="s">
-        <v>227</v>
-      </c>
-      <c r="E5" s="91" t="s">
-        <v>228</v>
+        <v>199</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B3:D3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -8145,7 +8150,7 @@
   <cols>
     <col min="1" max="1" width="2.85546875" customWidth="1"/>
     <col min="2" max="2" width="38.7109375" customWidth="1"/>
-    <col min="3" max="5" width="17" customWidth="1"/>
+    <col min="3" max="5" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
@@ -8162,19 +8167,19 @@
       <c r="H2" s="77"/>
     </row>
     <row r="3" spans="2:8" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="77" t="s">
-        <v>211</v>
-      </c>
-      <c r="C3" s="77"/>
-      <c r="D3" s="77"/>
-      <c r="E3" s="77"/>
+      <c r="B3" s="152" t="s">
+        <v>265</v>
+      </c>
+      <c r="C3" s="152"/>
+      <c r="D3" s="152"/>
+      <c r="E3" s="152"/>
       <c r="F3" s="77"/>
       <c r="G3" s="77"/>
       <c r="H3" s="77"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" s="91" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C5" s="91" t="s">
         <v>209</v>
@@ -8193,14 +8198,17 @@
       <c r="E6" s="9"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B3:E3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:Z8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:H6"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
@@ -8209,125 +8217,57 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.85546875" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="9" width="22.7109375" customWidth="1"/>
-    <col min="10" max="10" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.7109375" customWidth="1"/>
+    <col min="3" max="5" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:26" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:8" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="44" t="s">
         <v>81</v>
       </c>
-      <c r="Z1" s="38"/>
-    </row>
-    <row r="2" spans="2:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="78"/>
-      <c r="C2" s="78"/>
-      <c r="D2" s="78"/>
-      <c r="E2" s="78"/>
-      <c r="F2" s="78"/>
-      <c r="G2" s="78"/>
-      <c r="H2" s="78"/>
-      <c r="I2" s="78"/>
-      <c r="J2" s="78"/>
-      <c r="K2" s="78"/>
-      <c r="L2" s="78"/>
-      <c r="M2" s="78"/>
-      <c r="N2" s="78"/>
-      <c r="Z2"/>
-    </row>
-    <row r="3" spans="2:26" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="152" t="s">
-        <v>252</v>
-      </c>
-      <c r="C3" s="152"/>
+    </row>
+    <row r="2" spans="2:8" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="77"/>
+      <c r="D2" s="77"/>
+      <c r="E2" s="77"/>
+      <c r="F2" s="77"/>
+      <c r="G2" s="77"/>
+      <c r="H2" s="77"/>
+    </row>
+    <row r="3" spans="2:8" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="77" t="s">
+        <v>211</v>
+      </c>
+      <c r="C3" s="77"/>
       <c r="D3" s="77"/>
       <c r="E3" s="77"/>
       <c r="F3" s="77"/>
       <c r="G3" s="77"/>
       <c r="H3" s="77"/>
-      <c r="I3" s="77"/>
-      <c r="J3" s="77"/>
-      <c r="K3" s="77"/>
-      <c r="L3" s="77"/>
-      <c r="M3" s="77"/>
-      <c r="N3" s="77"/>
-      <c r="Z3"/>
-    </row>
-    <row r="5" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="C5" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="11" t="s">
-        <v>249</v>
-      </c>
-      <c r="F5" s="13"/>
-      <c r="G5" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="H5" s="2"/>
-    </row>
-    <row r="6" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="C6" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="12"/>
-      <c r="E6" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="F6" s="12"/>
-      <c r="G6" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="H6" s="12"/>
-    </row>
-    <row r="7" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B7" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B8" s="2">
-        <v>1</v>
-      </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5" s="91" t="s">
+        <v>212</v>
+      </c>
+      <c r="C5" s="91" t="s">
+        <v>209</v>
+      </c>
+      <c r="D5" s="91" t="s">
+        <v>227</v>
+      </c>
+      <c r="E5" s="91" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="8"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B3:C3"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -8372,7 +8312,7 @@
     </row>
     <row r="3" spans="2:26" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="152" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="C3" s="152"/>
       <c r="D3" s="77"/>
@@ -8393,22 +8333,28 @@
         <v>2</v>
       </c>
       <c r="D5" s="2"/>
-      <c r="E5" s="49" t="s">
-        <v>26</v>
+      <c r="E5" s="11" t="s">
+        <v>249</v>
       </c>
       <c r="F5" s="13"/>
-      <c r="G5" s="46"/>
-      <c r="H5" s="47"/>
+      <c r="G5" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="2"/>
     </row>
     <row r="6" spans="2:26" x14ac:dyDescent="0.25">
       <c r="C6" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="D6" s="174"/>
-      <c r="E6" s="175"/>
-      <c r="F6" s="176"/>
-      <c r="G6" s="48"/>
-      <c r="H6" s="48"/>
+        <v>8</v>
+      </c>
+      <c r="D6" s="12"/>
+      <c r="E6" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" s="12"/>
+      <c r="G6" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="H6" s="12"/>
     </row>
     <row r="7" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
@@ -8429,7 +8375,7 @@
       <c r="G7" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="H7" s="41" t="s">
+      <c r="H7" s="4" t="s">
         <v>35</v>
       </c>
       <c r="I7" s="4" t="s">
@@ -8449,8 +8395,7 @@
       <c r="I8" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="D6:F6"/>
+  <mergeCells count="1">
     <mergeCell ref="B3:C3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8500,7 +8445,7 @@
     </row>
     <row r="3" spans="2:26" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="152" t="s">
-        <v>79</v>
+        <v>259</v>
       </c>
       <c r="C3" s="152"/>
       <c r="D3" s="77"/>
@@ -8521,20 +8466,22 @@
         <v>2</v>
       </c>
       <c r="D5" s="2"/>
-      <c r="E5" s="11" t="s">
-        <v>63</v>
+      <c r="E5" s="49" t="s">
+        <v>26</v>
       </c>
       <c r="F5" s="13"/>
+      <c r="G5" s="46"/>
+      <c r="H5" s="47"/>
     </row>
     <row r="6" spans="2:26" x14ac:dyDescent="0.25">
       <c r="C6" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" s="12"/>
-      <c r="E6" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="F6" s="12"/>
+        <v>95</v>
+      </c>
+      <c r="D6" s="174"/>
+      <c r="E6" s="175"/>
+      <c r="F6" s="176"/>
+      <c r="G6" s="48"/>
+      <c r="H6" s="48"/>
     </row>
     <row r="7" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
@@ -8555,7 +8502,7 @@
       <c r="G7" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="H7" s="41" t="s">
         <v>35</v>
       </c>
       <c r="I7" s="4" t="s">
@@ -8575,11 +8522,13 @@
       <c r="I8" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
+    <mergeCell ref="D6:F6"/>
     <mergeCell ref="B3:C3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -8695,7 +8644,7 @@
     </row>
     <row r="3" spans="2:26" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="152" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
       <c r="C3" s="152"/>
       <c r="D3" s="77"/>
@@ -8713,6 +8662,130 @@
     </row>
     <row r="5" spans="2:26" x14ac:dyDescent="0.25">
       <c r="C5" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="F5" s="13"/>
+    </row>
+    <row r="6" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="C6" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="12"/>
+      <c r="E6" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="F6" s="12"/>
+    </row>
+    <row r="7" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B7" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B8" s="2">
+        <v>1</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B3:C3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:Z8"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.85546875" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="9" width="22.7109375" customWidth="1"/>
+    <col min="10" max="10" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:26" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B1" s="44" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z1" s="38"/>
+    </row>
+    <row r="2" spans="2:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="78"/>
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="78"/>
+      <c r="G2" s="78"/>
+      <c r="H2" s="78"/>
+      <c r="I2" s="78"/>
+      <c r="J2" s="78"/>
+      <c r="K2" s="78"/>
+      <c r="L2" s="78"/>
+      <c r="M2" s="78"/>
+      <c r="N2" s="78"/>
+      <c r="Z2"/>
+    </row>
+    <row r="3" spans="2:26" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B3" s="152" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" s="152"/>
+      <c r="D3" s="77"/>
+      <c r="E3" s="77"/>
+      <c r="F3" s="77"/>
+      <c r="G3" s="77"/>
+      <c r="H3" s="77"/>
+      <c r="I3" s="77"/>
+      <c r="J3" s="77"/>
+      <c r="K3" s="77"/>
+      <c r="L3" s="77"/>
+      <c r="M3" s="77"/>
+      <c r="N3" s="77"/>
+      <c r="Z3"/>
+    </row>
+    <row r="5" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="C5" s="10" t="s">
         <v>23</v>
       </c>
       <c r="D5" s="2"/>
@@ -8785,7 +8858,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:Q7"/>
   <sheetViews>
@@ -8945,7 +9018,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:Y8"/>
   <sheetViews>
@@ -9206,7 +9279,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A24"/>
   <sheetViews>

</xml_diff>

<commit_message>
TRIEDA-1869: Retirada da coluna Receita Por Crédito(R$) da planilha importacao/exportacao de Ofertas e Demandas
</commit_message>
<xml_diff>
--- a/code/client/web/src/main/resources/templateExport.xlsx
+++ b/code/client/web/src/main/resources/templateExport.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="17070" windowHeight="5370" tabRatio="919" firstSheet="18" activeTab="21"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="17070" windowHeight="5370" tabRatio="919" firstSheet="18" activeTab="22"/>
   </bookViews>
   <sheets>
     <sheet name="Turnos" sheetId="49" r:id="rId1"/>
@@ -624,17 +624,87 @@
     <author>Autor</author>
   </authors>
   <commentList>
-    <comment ref="K5" authorId="0">
+    <comment ref="D5" authorId="0">
       <text>
         <r>
           <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Receita Semanal por Crédito e Aluno (em Reais)
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sim
+Não</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+ 